<commit_message>
Copy Excel Columns feature
</commit_message>
<xml_diff>
--- a/output/layerCoordinates_left.xlsx
+++ b/output/layerCoordinates_left.xlsx
@@ -727,7 +727,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>[(-0.3, 30.0), (-0.3, 29.86), (-5.672, 30.0), (-5.672, 29.86), (-0.3, 29.86), (-0.3, 29.74), (-5.672, 29.86), (-5.672, 29.74)]</t>
+          <t>[(0.0, 30.0), (0.0, 29.86), (-5.672, 30.0), (-5.672, 29.86), (0.0, 29.86), (0.0, 29.74), (-5.672, 29.86), (-5.672, 29.74)]</t>
         </is>
       </c>
     </row>
@@ -737,7 +737,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>[(-0.3, 31.0), (-0.3, 30.85), (-5.585, 31.0), (-5.585, 30.85), (-0.3, 30.85), (-0.3, 30.73), (-5.585, 30.85), (-5.585, 30.72)]</t>
+          <t>[(0.0, 31.0), (0.0, 30.85), (-5.585, 31.0), (-5.585, 30.85), (0.0, 30.85), (0.0, 30.73), (-5.585, 30.85), (-5.585, 30.72)]</t>
         </is>
       </c>
     </row>
@@ -747,7 +747,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>[(-0.3, 32.0), (-0.3, 31.8), (-5.304, 32.0), (-5.304, 31.8), (-0.3, 31.8), (-0.3, 31.68), (-5.304, 31.8), (-5.304, 31.61)]</t>
+          <t>[(0.0, 32.0), (0.0, 31.8), (-5.304, 32.0), (-5.304, 31.8), (0.0, 31.8), (0.0, 31.68), (-5.304, 31.8), (-5.304, 31.61)]</t>
         </is>
       </c>
     </row>
@@ -757,7 +757,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>[(-0.3, 33.0), (-0.3, 32.78), (-4.806, 33.0), (-4.806, 32.78), (-0.3, 32.78), (-0.3, 32.63), (-4.806, 32.78), (-4.806, 32.57)]</t>
+          <t>[(0.0, 33.0), (0.0, 32.78), (-4.806, 33.0), (-4.806, 32.78), (0.0, 32.78), (0.0, 32.63), (-4.806, 32.78), (-4.806, 32.57)]</t>
         </is>
       </c>
     </row>
@@ -767,7 +767,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>[(-0.3, 34.0), (-0.3, 33.8), (-3.873, 34.0), (-3.873, 33.8), (-0.3, 33.8), (-0.3, 33.62), (-3.873, 33.8), (-3.873, 33.61)]</t>
+          <t>[(0.0, 34.0), (0.0, 33.8), (-3.873, 34.0), (-3.873, 33.8), (0.0, 33.8), (0.0, 33.62), (-3.873, 33.8), (-3.873, 33.61)]</t>
         </is>
       </c>
     </row>
@@ -777,7 +777,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>[(-0.3, 35.0), (-0.3, 34.85), (-2.676, 35.0), (-2.676, 34.85), (-0.3, 34.85), (-0.3, 34.7), (-2.676, 34.85), (-2.676, 34.7), (-0.3, 34.7), (-0.3, 34.57), (-2.676, 34.7), (-2.676, 34.57)]</t>
+          <t>[(0.0, 35.0), (0.0, 34.85), (-2.676, 35.0), (-2.676, 34.85), (0.0, 34.85), (0.0, 34.7), (-2.676, 34.85), (-2.676, 34.7), (0.0, 34.7), (0.0, 34.57), (-2.676, 34.7), (-2.676, 34.57)]</t>
         </is>
       </c>
     </row>
@@ -1837,7 +1837,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>[(-0.3, 141.0), (-0.3, 140.74), (-2.69, 141.0), (-2.69, 140.74), (-0.3, 140.74), (-0.3, 140.54), (-2.69, 140.74), (-2.69, 140.48)]</t>
+          <t>[(0.0, 141.0), (0.0, 140.74), (-2.69, 141.0), (-2.69, 140.74), (0.0, 140.74), (0.0, 140.54), (-2.69, 140.74), (-2.69, 140.48)]</t>
         </is>
       </c>
     </row>
@@ -1847,7 +1847,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>[(-0.3, 142.0), (-0.3, 141.73), (-3.261, 142.0), (-3.261, 141.73), (-0.3, 141.73), (-0.3, 141.54), (-3.261, 141.73), (-3.261, 141.46)]</t>
+          <t>[(0.0, 142.0), (0.0, 141.73), (-3.261, 142.0), (-3.261, 141.73), (0.0, 141.73), (0.0, 141.54), (-3.261, 141.73), (-3.261, 141.46)]</t>
         </is>
       </c>
     </row>
@@ -1857,7 +1857,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>[(-0.3, 143.0), (-0.3, 142.74), (-3.659, 143.0), (-3.659, 142.74), (-0.3, 142.74), (-0.3, 142.55), (-3.659, 142.74), (-3.659, 142.48)]</t>
+          <t>[(0.0, 143.0), (0.0, 142.74), (-3.659, 143.0), (-3.659, 142.74), (0.0, 142.74), (0.0, 142.55), (-3.659, 142.74), (-3.659, 142.48)]</t>
         </is>
       </c>
     </row>
@@ -1867,7 +1867,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>[(-0.3, 144.0), (-0.3, 143.85), (-4.017, 144.0), (-4.017, 143.85), (-0.3, 143.85), (-0.3, 143.7), (-4.017, 143.85), (-4.017, 143.7), (-0.3, 143.7), (-0.3, 143.59), (-4.017, 143.7), (-4.017, 143.57)]</t>
+          <t>[(0.0, 144.0), (0.0, 143.85), (-4.017, 144.0), (-4.017, 143.85), (0.0, 143.85), (0.0, 143.7), (-4.017, 143.85), (-4.017, 143.7), (0.0, 143.7), (0.0, 143.59), (-4.017, 143.7), (-4.017, 143.57)]</t>
         </is>
       </c>
     </row>
@@ -1877,7 +1877,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>[(-0.3, 145.0), (-0.3, 144.81), (-4.438, 145.0), (-4.438, 144.81), (-0.3, 144.81), (-0.3, 144.64), (-4.438, 144.81), (-4.438, 144.62)]</t>
+          <t>[(0.0, 145.0), (0.0, 144.81), (-4.438, 145.0), (-4.438, 144.81), (0.0, 144.81), (0.0, 144.64), (-4.438, 144.81), (-4.438, 144.62)]</t>
         </is>
       </c>
     </row>
@@ -1887,7 +1887,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>[(-0.3, 146.0), (-0.3, 145.81), (-4.773, 146.0), (-4.773, 145.81), (-0.3, 145.81), (-0.3, 145.65), (-4.773, 145.81), (-4.773, 145.62)]</t>
+          <t>[(0.0, 146.0), (0.0, 145.81), (-4.773, 146.0), (-4.773, 145.81), (0.0, 145.81), (0.0, 145.65), (-4.773, 145.81), (-4.773, 145.62)]</t>
         </is>
       </c>
     </row>
@@ -1897,7 +1897,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>[(-0.3, 147.0), (-0.3, 146.79), (-5.091, 147.0), (-5.091, 146.79), (-0.3, 146.79), (-0.3, 146.61), (-5.091, 146.79), (-5.091, 146.58)]</t>
+          <t>[(0.0, 147.0), (0.0, 146.79), (-5.091, 147.0), (-5.091, 146.79), (0.0, 146.79), (0.0, 146.61), (-5.091, 146.79), (-5.091, 146.58)]</t>
         </is>
       </c>
     </row>
@@ -1907,7 +1907,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>[(-0.3, 148.0), (-0.3, 147.85), (-5.595, 148.0), (-5.595, 147.85), (-0.3, 147.85), (-0.3, 147.7), (-5.595, 147.85), (-5.595, 147.7), (-0.3, 147.7), (-0.3, 147.58), (-5.595, 147.7), (-5.595, 147.56)]</t>
+          <t>[(0.0, 148.0), (0.0, 147.85), (-5.595, 148.0), (-5.595, 147.85), (0.0, 147.85), (0.0, 147.7), (-5.595, 147.85), (-5.595, 147.7), (0.0, 147.7), (0.0, 147.58), (-5.595, 147.7), (-5.595, 147.56)]</t>
         </is>
       </c>
     </row>
@@ -1917,7 +1917,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>[(-0.3, 149.0), (-0.3, 148.85), (-6.265, 149.0), (-6.265, 148.85), (-0.3, 148.85), (-0.3, 148.7), (-6.265, 148.85), (-6.265, 148.7), (-0.3, 148.7), (-0.3, 148.57), (-6.265, 148.7), (-6.265, 148.55)]</t>
+          <t>[(0.0, 149.0), (0.0, 148.85), (-6.265, 149.0), (-6.265, 148.85), (0.0, 148.85), (0.0, 148.7), (-6.265, 148.85), (-6.265, 148.7), (0.0, 148.7), (0.0, 148.57), (-6.265, 148.7), (-6.265, 148.55)]</t>
         </is>
       </c>
     </row>
@@ -1927,7 +1927,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>[(-0.3, 150.0), (-0.3, 149.85), (-7.035, 150.0), (-7.035, 149.85), (-0.3, 149.85), (-0.3, 149.7), (-7.035, 149.85), (-7.035, 149.7), (-0.3, 149.7), (-0.3, 149.59), (-7.035, 149.7), (-7.035, 149.56)]</t>
+          <t>[(0.0, 150.0), (0.0, 149.85), (-7.035, 150.0), (-7.035, 149.85), (0.0, 149.85), (0.0, 149.7), (-7.035, 149.85), (-7.035, 149.7), (0.0, 149.7), (0.0, 149.59), (-7.035, 149.7), (-7.035, 149.56)]</t>
         </is>
       </c>
     </row>
@@ -1937,7 +1937,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>[(-0.3, 151.0), (-0.3, 150.79), (-7.802, 151.0), (-7.802, 150.79), (-0.3, 150.79), (-0.3, 150.61), (-7.802, 150.79), (-7.802, 150.58)]</t>
+          <t>[(0.0, 151.0), (0.0, 150.79), (-7.802, 151.0), (-7.802, 150.79), (0.0, 150.79), (0.0, 150.61), (-7.802, 150.79), (-7.802, 150.58)]</t>
         </is>
       </c>
     </row>
@@ -1947,7 +1947,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>[(-0.3, 152.0), (-0.3, 151.82), (-8.397, 152.0), (-8.397, 151.82), (-0.3, 151.82), (-0.3, 151.65), (-8.397, 151.82), (-8.397, 151.67)]</t>
+          <t>[(0.0, 152.0), (0.0, 151.82), (-8.397, 152.0), (-8.397, 151.82), (0.0, 151.82), (0.0, 151.65), (-8.397, 151.82), (-8.397, 151.67)]</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>[(-0.3, 160.0), (-0.3, 159.88), (-4.255, 160.0), (-4.255, 159.88), (-4.255, 160.0), (-4.255, 159.86), (-15.746, 160.0), (-15.746, 159.86), (-0.3, 159.88), (-0.3, 159.58), (-4.255, 159.88), (-4.255, 159.74), (-4.255, 159.86), (-4.255, 159.74), (-15.746, 159.86), (-15.746, 159.74)]</t>
+          <t>[(0.0, 160.0), (0.0, 159.88), (0.0, 160.0), (0.0, 159.88), (-4.255, 160.0), (-4.255, 159.86), (-15.746, 160.0), (-15.746, 159.86), (0.0, 159.88), (0.0, 159.58), (0.0, 159.88), (0.0, 159.74), (-4.255, 159.86), (-4.255, 159.74), (-15.746, 159.86), (-15.746, 159.74)]</t>
         </is>
       </c>
     </row>
@@ -2317,7 +2317,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>[(-0.3, 189.0), (-0.3, 188.81), (-3.637, 189.0), (-3.637, 188.81), (-0.3, 188.81), (-0.3, 188.62), (-3.637, 188.81), (-3.637, 188.69)]</t>
+          <t>[(0.0, 189.0), (0.0, 188.81), (-3.637, 189.0), (-3.637, 188.81), (0.0, 188.81), (0.0, 188.62), (-3.637, 188.81), (-3.637, 188.69)]</t>
         </is>
       </c>
     </row>
@@ -2327,7 +2327,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>[(-0.3, 190.0), (-0.3, 189.89), (-3.053, 190.0), (-3.053, 189.89), (-0.3, 189.89), (-0.3, 189.67), (-3.053, 189.89), (-3.053, 189.75)]</t>
+          <t>[(0.0, 190.0), (0.0, 189.89), (-3.053, 190.0), (-3.053, 189.89), (0.0, 189.89), (0.0, 189.67), (-3.053, 189.89), (-3.053, 189.75)]</t>
         </is>
       </c>
     </row>
@@ -2337,7 +2337,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>[(-0.3, 191.0), (-0.3, 190.82), (-2.361, 191.0), (-2.361, 190.82), (-0.3, 190.82), (-0.3, 190.64), (-2.361, 190.82), (-2.361, 190.68)]</t>
+          <t>[(0.0, 191.0), (0.0, 190.82), (-2.361, 191.0), (-2.361, 190.82), (0.0, 190.82), (0.0, 190.64), (-2.361, 190.82), (-2.361, 190.68)]</t>
         </is>
       </c>
     </row>
@@ -2607,7 +2607,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>[(-0.3, 218.0), (-0.3, 217.89), (-6.083, 218.0), (-6.083, 217.89), (-6.083, 218.0), (-6.083, 217.75), (-9.456, 218.0), (-9.456, 217.75), (-0.3, 217.89), (-0.3, 217.73), (-6.083, 217.89), (-6.083, 217.64), (-6.083, 217.75), (-6.083, 217.64), (-9.456, 217.75), (-9.456, 217.51)]</t>
+          <t>[(0.0, 218.0), (0.0, 217.89), (0.0, 218.0), (0.0, 217.89), (-6.083, 218.0), (-6.083, 217.75), (-9.456, 218.0), (-9.456, 217.75), (0.0, 217.89), (0.0, 217.73), (0.0, 217.89), (0.0, 217.64), (-6.083, 217.75), (-6.083, 217.64), (-9.456, 217.75), (-9.456, 217.51)]</t>
         </is>
       </c>
     </row>
@@ -2617,7 +2617,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>[(-0.3, 219.0), (-0.3, 218.89), (-7.801, 219.0), (-7.801, 218.89), (-7.801, 219.0), (-7.801, 218.72), (-11.196, 219.0), (-11.196, 218.72), (-0.3, 218.89), (-0.3, 218.72), (-7.801, 218.89), (-7.801, 218.59), (-7.801, 218.72), (-7.801, 218.59), (-11.196, 218.72), (-11.196, 218.44)]</t>
+          <t>[(0.0, 219.0), (0.0, 218.89), (0.0, 219.0), (0.0, 218.89), (-7.801, 219.0), (-7.801, 218.72), (-11.196, 219.0), (-11.196, 218.72), (0.0, 218.89), (0.0, 218.72), (0.0, 218.89), (0.0, 218.59), (-7.801, 218.72), (-7.801, 218.59), (-11.196, 218.72), (-11.196, 218.44)]</t>
         </is>
       </c>
     </row>
@@ -2627,7 +2627,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>[(-0.3, 220.0), (-0.3, 219.86), (-9.188, 220.0), (-9.188, 219.86), (-9.188, 220.0), (-9.188, 219.71), (-12.555, 220.0), (-12.555, 219.71), (-0.3, 219.86), (-0.3, 219.69), (-9.188, 219.86), (-9.188, 219.56), (-9.188, 219.71), (-9.188, 219.56), (-12.555, 219.71), (-12.555, 219.42)]</t>
+          <t>[(0.0, 220.0), (0.0, 219.86), (0.0, 220.0), (0.0, 219.86), (-9.188, 220.0), (-9.188, 219.71), (-12.555, 220.0), (-12.555, 219.71), (0.0, 219.86), (0.0, 219.69), (0.0, 219.86), (0.0, 219.56), (-9.188, 219.71), (-9.188, 219.56), (-12.555, 219.71), (-12.555, 219.42)]</t>
         </is>
       </c>
     </row>
@@ -2637,7 +2637,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>[(-0.3, 221.0), (-0.3, 220.76), (-10.073, 221.0), (-10.073, 220.76), (-10.073, 221.0), (-10.073, 220.76), (-13.47, 221.0), (-13.47, 220.76), (-0.3, 220.76), (-0.3, 220.53), (-10.073, 220.76), (-10.073, 220.64), (-10.073, 220.76), (-10.073, 220.64), (-13.47, 220.76), (-13.47, 220.53)]</t>
+          <t>[(0.0, 221.0), (0.0, 220.76), (0.0, 221.0), (0.0, 220.76), (-10.073, 221.0), (-10.073, 220.76), (-13.47, 221.0), (-13.47, 220.76), (0.0, 220.76), (0.0, 220.53), (0.0, 220.76), (0.0, 220.64), (-10.073, 220.76), (-10.073, 220.64), (-13.47, 220.76), (-13.47, 220.53)]</t>
         </is>
       </c>
     </row>
@@ -2857,7 +2857,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>[(-0.3, 243.0), (-0.3, 242.85), (-3.224, 243.0), (-3.224, 242.85), (-3.224, 243.0), (-3.224, 242.83), (-9.022, 243.0), (-9.022, 242.83), (-0.3, 242.85), (-0.3, 242.71), (-3.224, 242.85), (-3.224, 242.7), (-3.224, 242.83), (-3.224, 242.7), (-9.022, 242.83), (-9.022, 242.66)]</t>
+          <t>[(0.0, 243.0), (0.0, 242.85), (0.0, 243.0), (0.0, 242.85), (-3.224, 243.0), (-3.224, 242.83), (-9.022, 243.0), (-9.022, 242.83), (0.0, 242.85), (0.0, 242.71), (0.0, 242.85), (0.0, 242.7), (-3.224, 242.83), (-3.224, 242.7), (-9.022, 242.83), (-9.022, 242.66)]</t>
         </is>
       </c>
     </row>
@@ -2867,7 +2867,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>[(-0.3, 244.0), (-0.3, 243.83), (-3.053, 244.0), (-3.053, 243.83), (-3.053, 244.0), (-3.053, 243.77), (-9.943, 244.0), (-9.943, 243.77), (-0.3, 243.83), (-0.3, 243.67), (-3.053, 243.83), (-3.053, 243.66), (-3.053, 243.77), (-3.053, 243.66), (-9.943, 243.77), (-9.943, 243.47)]</t>
+          <t>[(0.0, 244.0), (0.0, 243.83), (0.0, 244.0), (0.0, 243.83), (-3.053, 244.0), (-3.053, 243.77), (-9.943, 244.0), (-9.943, 243.77), (0.0, 243.83), (0.0, 243.67), (0.0, 243.83), (0.0, 243.66), (-3.053, 243.77), (-3.053, 243.66), (-9.943, 243.77), (-9.943, 243.47)]</t>
         </is>
       </c>
     </row>
@@ -2877,7 +2877,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>[(-0.3, 245.0), (-0.3, 244.83), (-2.817, 245.0), (-2.817, 244.83), (-2.817, 245.0), (-2.817, 244.83), (-9.696, 245.0), (-9.696, 244.73), (-0.3, 244.83), (-0.3, 244.69), (-2.817, 244.83), (-2.817, 244.66), (-2.817, 244.83), (-2.817, 244.66), (-9.696, 244.73), (-9.696, 244.46)]</t>
+          <t>[(0.0, 245.0), (0.0, 244.83), (0.0, 245.0), (0.0, 244.83), (-2.817, 245.0), (-2.817, 244.83), (-9.696, 245.0), (-9.696, 244.73), (0.0, 244.83), (0.0, 244.69), (0.0, 244.83), (0.0, 244.66), (-2.817, 244.83), (-2.817, 244.66), (-9.696, 244.73), (-9.696, 244.46)]</t>
         </is>
       </c>
     </row>
@@ -2887,7 +2887,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>[(-0.3, 246.0), (-0.3, 245.84), (-2.868, 246.0), (-2.868, 245.84), (-2.868, 246.0), (-2.868, 245.81), (-9.652, 246.0), (-9.652, 245.81), (-0.3, 245.84), (-0.3, 245.73), (-2.868, 245.84), (-2.868, 245.68), (-2.868, 245.81), (-2.868, 245.68), (-9.652, 245.81), (-9.652, 245.51)]</t>
+          <t>[(0.0, 246.0), (0.0, 245.84), (0.0, 246.0), (0.0, 245.84), (-2.868, 246.0), (-2.868, 245.81), (-9.652, 246.0), (-9.652, 245.81), (0.0, 245.84), (0.0, 245.73), (0.0, 245.84), (0.0, 245.68), (-2.868, 245.81), (-2.868, 245.68), (-9.652, 245.81), (-9.652, 245.51)]</t>
         </is>
       </c>
     </row>
@@ -2927,7 +2927,7 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>[(-0.3, 250.0), (-0.3, 249.89), (-3.599, 250.0), (-3.599, 249.89), (-3.599, 250.0), (-3.599, 249.79), (-7.357, 250.0), (-7.357, 249.79), (-0.3, 249.89), (-0.3, 249.74), (-3.599, 249.89), (-3.599, 249.67), (-3.599, 249.79), (-3.599, 249.67), (-7.357, 249.79), (-7.357, 249.59)]</t>
+          <t>[(0.0, 250.0), (0.0, 249.89), (0.0, 250.0), (0.0, 249.89), (-3.599, 250.0), (-3.599, 249.79), (-7.357, 250.0), (-7.357, 249.79), (0.0, 249.89), (0.0, 249.74), (0.0, 249.89), (0.0, 249.67), (-3.599, 249.79), (-3.599, 249.67), (-7.357, 249.79), (-7.357, 249.59)]</t>
         </is>
       </c>
     </row>
@@ -2937,7 +2937,7 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>[(-0.3, 251.0), (-0.3, 250.79), (-3.931, 251.0), (-3.931, 250.79), (-3.931, 251.0), (-3.931, 250.71), (-11.377, 251.0), (-11.377, 250.71), (-0.3, 250.79), (-0.3, 250.63), (-3.931, 250.79), (-3.931, 250.58), (-3.931, 250.71), (-3.931, 250.58), (-11.377, 250.71), (-11.377, 250.42)]</t>
+          <t>[(0.0, 251.0), (0.0, 250.79), (0.0, 251.0), (0.0, 250.79), (-3.931, 251.0), (-3.931, 250.71), (-11.377, 251.0), (-11.377, 250.71), (0.0, 250.79), (0.0, 250.63), (0.0, 250.79), (0.0, 250.58), (-3.931, 250.71), (-3.931, 250.58), (-11.377, 250.71), (-11.377, 250.42)]</t>
         </is>
       </c>
     </row>
@@ -2947,7 +2947,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>[(-0.3, 252.0), (-0.3, 251.85), (-4.19, 252.0), (-4.19, 251.85), (-4.19, 252.0), (-4.19, 251.85), (-7.959, 252.0), (-7.959, 251.85), (-0.3, 251.85), (-0.3, 251.7), (-4.19, 251.85), (-4.19, 251.7), (-4.19, 251.85), (-4.19, 251.7), (-7.959, 251.85), (-7.959, 251.7), (-0.3, 251.7), (-0.3, 251.55), (-4.19, 251.7), (-4.19, 251.56), (-4.19, 251.7), (-4.19, 251.56), (-7.959, 251.7), (-7.959, 251.56)]</t>
+          <t>[(0.0, 252.0), (0.0, 251.85), (0.0, 252.0), (0.0, 251.85), (-4.19, 252.0), (-4.19, 251.85), (-7.959, 252.0), (-7.959, 251.85), (0.0, 251.85), (0.0, 251.7), (0.0, 251.85), (0.0, 251.7), (-4.19, 251.85), (-4.19, 251.7), (-7.959, 251.85), (-7.959, 251.7), (0.0, 251.7), (0.0, 251.55), (0.0, 251.7), (0.0, 251.56), (-4.19, 251.7), (-4.19, 251.56), (-7.959, 251.7), (-7.959, 251.56)]</t>
         </is>
       </c>
     </row>
@@ -2957,7 +2957,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>[(-0.3, 253.0), (-0.3, 252.83), (-5.084, 253.0), (-5.084, 252.83), (-5.084, 253.0), (-5.084, 252.85), (-8.801, 253.0), (-8.801, 252.85), (-0.3, 252.83), (-0.3, 252.66), (-5.084, 252.83), (-5.084, 252.66), (-5.084, 252.85), (-5.084, 252.7), (-8.801, 252.85), (-8.801, 252.7), (-0.3, 252.66), (-0.3, 252.51), (-5.084, 252.66), (-5.084, 252.55), (-5.084, 252.7), (-5.084, 252.55), (-8.801, 252.7), (-8.801, 252.56)]</t>
+          <t>[(0.0, 253.0), (0.0, 252.83), (0.0, 253.0), (0.0, 252.83), (-5.084, 253.0), (-5.084, 252.85), (-8.801, 253.0), (-8.801, 252.85), (0.0, 252.83), (0.0, 252.66), (0.0, 252.83), (0.0, 252.66), (-5.084, 252.85), (-5.084, 252.7), (-8.801, 252.85), (-8.801, 252.7), (0.0, 252.66), (0.0, 252.51), (0.0, 252.66), (0.0, 252.55), (-5.084, 252.7), (-5.084, 252.55), (-8.801, 252.7), (-8.801, 252.56)]</t>
         </is>
       </c>
     </row>
@@ -2967,7 +2967,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>[(-0.3, 254.0), (-0.3, 253.79), (-5.837, 254.0), (-5.837, 253.79), (-5.837, 254.0), (-5.837, 253.82), (-9.608, 254.0), (-9.608, 253.82), (-0.3, 253.79), (-0.3, 253.59), (-5.837, 253.79), (-5.837, 253.64), (-5.837, 253.82), (-5.837, 253.64), (-9.608, 253.82), (-9.608, 253.65)]</t>
+          <t>[(0.0, 254.0), (0.0, 253.79), (0.0, 254.0), (0.0, 253.79), (-5.837, 254.0), (-5.837, 253.82), (-9.608, 254.0), (-9.608, 253.82), (0.0, 253.79), (0.0, 253.59), (0.0, 253.79), (0.0, 253.64), (-5.837, 253.82), (-5.837, 253.64), (-9.608, 253.82), (-9.608, 253.65)]</t>
         </is>
       </c>
     </row>
@@ -2977,7 +2977,7 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>[(-0.3, 255.0), (-0.3, 254.84), (-6.327, 255.0), (-6.327, 254.84), (-6.327, 255.0), (-6.327, 254.85), (-10.119, 255.0), (-10.119, 254.85), (-0.3, 254.84), (-0.3, 254.69), (-6.327, 254.84), (-6.327, 254.72), (-6.327, 254.85), (-6.327, 254.72), (-10.119, 254.85), (-10.119, 254.74)]</t>
+          <t>[(0.0, 255.0), (0.0, 254.84), (0.0, 255.0), (0.0, 254.84), (-6.327, 255.0), (-6.327, 254.85), (-10.119, 255.0), (-10.119, 254.85), (0.0, 254.84), (0.0, 254.69), (0.0, 254.84), (0.0, 254.72), (-6.327, 254.85), (-6.327, 254.72), (-10.119, 254.85), (-10.119, 254.74)]</t>
         </is>
       </c>
     </row>
@@ -2987,7 +2987,7 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>[(-0.3, 256.0), (-0.3, 255.84), (-6.895, 256.0), (-6.895, 255.84), (-6.895, 256.0), (-6.895, 255.84), (-10.601, 256.0), (-10.601, 255.84), (-0.3, 255.84), (-0.3, 255.69), (-6.895, 255.84), (-6.895, 255.7), (-6.895, 255.84), (-6.895, 255.7), (-10.601, 255.84), (-10.601, 255.69)]</t>
+          <t>[(0.0, 256.0), (0.0, 255.84), (0.0, 256.0), (0.0, 255.84), (-6.895, 256.0), (-6.895, 255.84), (-10.601, 256.0), (-10.601, 255.84), (0.0, 255.84), (0.0, 255.69), (0.0, 255.84), (0.0, 255.7), (-6.895, 255.84), (-6.895, 255.7), (-10.601, 255.84), (-10.601, 255.69)]</t>
         </is>
       </c>
     </row>
@@ -2997,7 +2997,7 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>[(-0.3, 257.0), (-0.3, 256.79), (-7.551, 257.0), (-7.551, 256.79), (-7.551, 257.0), (-7.551, 256.79), (-11.175, 257.0), (-11.175, 256.79), (-0.3, 256.79), (-0.3, 256.59), (-7.551, 256.79), (-7.551, 256.62), (-7.551, 256.79), (-7.551, 256.62), (-11.175, 256.79), (-11.175, 256.59)]</t>
+          <t>[(0.0, 257.0), (0.0, 256.79), (0.0, 257.0), (0.0, 256.79), (-7.551, 257.0), (-7.551, 256.79), (-11.175, 257.0), (-11.175, 256.79), (0.0, 256.79), (0.0, 256.59), (0.0, 256.79), (0.0, 256.62), (-7.551, 256.79), (-7.551, 256.62), (-11.175, 256.79), (-11.175, 256.59)]</t>
         </is>
       </c>
     </row>
@@ -3007,7 +3007,7 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>[(-0.3, 258.0), (-0.3, 257.78), (-8.147, 258.0), (-8.147, 257.78), (-8.147, 258.0), (-8.147, 257.82), (-11.826, 258.0), (-11.826, 257.82), (-0.3, 257.78), (-0.3, 257.57), (-8.147, 257.78), (-8.147, 257.65), (-8.147, 257.82), (-8.147, 257.65), (-11.826, 257.82), (-11.826, 257.69)]</t>
+          <t>[(0.0, 258.0), (0.0, 257.78), (0.0, 258.0), (0.0, 257.78), (-8.147, 258.0), (-8.147, 257.82), (-11.826, 258.0), (-11.826, 257.82), (0.0, 257.78), (0.0, 257.57), (0.0, 257.78), (0.0, 257.65), (-8.147, 257.82), (-8.147, 257.65), (-11.826, 257.82), (-11.826, 257.69)]</t>
         </is>
       </c>
     </row>
@@ -3017,7 +3017,7 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>[(-0.3, 259.0), (-0.3, 258.8), (-8.681, 259.0), (-8.681, 258.8), (-8.681, 259.0), (-8.681, 258.89), (-12.316, 259.0), (-12.316, 258.89), (-0.3, 258.8), (-0.3, 258.6), (-8.681, 258.8), (-8.681, 258.69), (-8.681, 258.89), (-8.681, 258.69), (-12.316, 258.89), (-12.316, 258.75)]</t>
+          <t>[(0.0, 259.0), (0.0, 258.8), (0.0, 259.0), (0.0, 258.8), (-8.681, 259.0), (-8.681, 258.89), (-12.316, 259.0), (-12.316, 258.89), (0.0, 258.8), (0.0, 258.6), (0.0, 258.8), (0.0, 258.69), (-8.681, 258.89), (-8.681, 258.69), (-12.316, 258.89), (-12.316, 258.75)]</t>
         </is>
       </c>
     </row>
@@ -3027,7 +3027,7 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>[(-0.3, 260.0), (-0.3, 259.76), (-8.606, 260.0), (-8.606, 259.76), (-8.606, 260.0), (-8.606, 259.82), (-12.32, 260.0), (-12.32, 259.82), (-0.3, 259.76), (-0.3, 259.53), (-8.606, 259.76), (-8.606, 259.65), (-8.606, 259.82), (-8.606, 259.65), (-12.32, 259.82), (-12.32, 259.71)]</t>
+          <t>[(0.0, 260.0), (0.0, 259.76), (0.0, 260.0), (0.0, 259.76), (-8.606, 260.0), (-8.606, 259.82), (-12.32, 260.0), (-12.32, 259.82), (0.0, 259.76), (0.0, 259.53), (0.0, 259.76), (0.0, 259.65), (-8.606, 259.82), (-8.606, 259.65), (-12.32, 259.82), (-12.32, 259.71)]</t>
         </is>
       </c>
     </row>
@@ -3037,7 +3037,7 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>[(-0.3, 261.0), (-0.3, 260.71), (-8.556, 261.0), (-8.556, 260.71), (-8.556, 261.0), (-8.556, 260.8), (-12.298, 261.0), (-12.298, 260.8), (-0.3, 260.71), (-0.3, 260.42), (-8.556, 260.71), (-8.556, 260.6), (-8.556, 260.8), (-8.556, 260.6), (-12.298, 260.8), (-12.298, 260.65)]</t>
+          <t>[(0.0, 261.0), (0.0, 260.71), (0.0, 261.0), (0.0, 260.71), (-8.556, 261.0), (-8.556, 260.8), (-12.298, 261.0), (-12.298, 260.8), (0.0, 260.71), (0.0, 260.42), (0.0, 260.71), (0.0, 260.6), (-8.556, 260.8), (-8.556, 260.6), (-12.298, 260.8), (-12.298, 260.65)]</t>
         </is>
       </c>
     </row>
@@ -3047,7 +3047,7 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>[(-0.3, 262.0), (-0.3, 261.67), (-8.125, 262.0), (-8.125, 261.74), (-8.125, 262.0), (-8.125, 261.83), (-12.034, 262.0), (-12.034, 261.83), (-0.3, 261.67), (-0.3, 261.34), (-8.125, 261.74), (-8.125, 261.48), (-8.125, 261.83), (-8.125, 261.66), (-12.034, 261.83), (-12.034, 261.66)]</t>
+          <t>[(0.0, 262.0), (0.0, 261.67), (0.0, 262.0), (0.0, 261.74), (-8.125, 262.0), (-8.125, 261.83), (-12.034, 262.0), (-12.034, 261.83), (0.0, 261.67), (0.0, 261.34), (0.0, 261.74), (0.0, 261.48), (-8.125, 261.83), (-8.125, 261.66), (-12.034, 261.83), (-12.034, 261.66)]</t>
         </is>
       </c>
     </row>
@@ -3057,7 +3057,7 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>[(-0.3, 263.0), (-0.3, 262.66), (-7.604, 263.0), (-7.604, 262.72), (-7.604, 263.0), (-7.604, 262.81), (-11.496, 263.0), (-11.496, 262.81), (-0.3, 262.66), (-0.3, 262.32), (-7.604, 262.72), (-7.604, 262.44), (-7.604, 262.81), (-7.604, 262.62), (-11.496, 262.81), (-11.496, 262.62)]</t>
+          <t>[(0.0, 263.0), (0.0, 262.66), (0.0, 263.0), (0.0, 262.72), (-7.604, 263.0), (-7.604, 262.81), (-11.496, 263.0), (-11.496, 262.81), (0.0, 262.66), (0.0, 262.32), (0.0, 262.72), (0.0, 262.44), (-7.604, 262.81), (-7.604, 262.62), (-11.496, 262.81), (-11.496, 262.62)]</t>
         </is>
       </c>
     </row>
@@ -3067,7 +3067,7 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>[(-0.3, 264.0), (-0.3, 263.7), (-6.979, 264.0), (-6.979, 263.7), (-6.979, 264.0), (-6.979, 263.84), (-10.837, 264.0), (-10.837, 263.84), (-0.3, 263.7), (-0.3, 263.41), (-6.979, 263.7), (-6.979, 263.52), (-6.979, 263.84), (-6.979, 263.68), (-10.837, 263.84), (-10.837, 263.68)]</t>
+          <t>[(0.0, 264.0), (0.0, 263.7), (0.0, 264.0), (0.0, 263.7), (-6.979, 264.0), (-6.979, 263.84), (-10.837, 264.0), (-10.837, 263.84), (0.0, 263.7), (0.0, 263.41), (0.0, 263.7), (0.0, 263.52), (-6.979, 263.84), (-6.979, 263.68), (-10.837, 263.84), (-10.837, 263.68)]</t>
         </is>
       </c>
     </row>
@@ -3087,7 +3087,7 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>[(-0.3, 266.0), (-0.3, 265.75), (-6.725, 266.0), (-6.725, 265.75), (-6.725, 266.0), (-6.725, 265.82), (-10.403, 266.0), (-10.403, 265.82), (-0.3, 265.75), (-0.3, 265.5), (-6.725, 265.75), (-6.725, 265.64), (-6.725, 265.82), (-6.725, 265.64), (-10.403, 265.82), (-10.403, 265.7)]</t>
+          <t>[(0.0, 266.0), (0.0, 265.75), (0.0, 266.0), (0.0, 265.75), (-6.725, 266.0), (-6.725, 265.82), (-10.403, 266.0), (-10.403, 265.82), (0.0, 265.75), (0.0, 265.5), (0.0, 265.75), (0.0, 265.64), (-6.725, 265.82), (-6.725, 265.64), (-10.403, 265.82), (-10.403, 265.7)]</t>
         </is>
       </c>
     </row>
@@ -3097,7 +3097,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>[(-0.3, 267.0), (-0.3, 266.71), (-6.746, 267.0), (-6.746, 266.71), (-6.746, 267.0), (-6.746, 266.75), (-10.553, 267.0), (-10.553, 266.75), (-0.3, 266.71), (-0.3, 266.42), (-6.746, 266.71), (-6.746, 266.5), (-6.746, 266.75), (-6.746, 266.5), (-10.553, 266.75), (-10.553, 266.56)]</t>
+          <t>[(0.0, 267.0), (0.0, 266.71), (0.0, 267.0), (0.0, 266.71), (-6.746, 267.0), (-6.746, 266.75), (-10.553, 267.0), (-10.553, 266.75), (0.0, 266.71), (0.0, 266.42), (0.0, 266.71), (0.0, 266.5), (-6.746, 266.75), (-6.746, 266.5), (-10.553, 266.75), (-10.553, 266.56)]</t>
         </is>
       </c>
     </row>
@@ -3107,7 +3107,7 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>[(-0.3, 268.0), (-0.3, 267.8), (-6.694, 268.0), (-6.694, 267.8), (-6.694, 268.0), (-6.694, 267.83), (-10.486, 268.0), (-10.486, 267.83), (-0.3, 267.8), (-0.3, 267.6), (-6.694, 267.8), (-6.694, 267.6), (-6.694, 267.83), (-6.694, 267.66), (-10.486, 267.83), (-10.486, 267.66), (-0.3, 267.6), (-0.3, 267.4), (-6.694, 267.6), (-6.694, 267.49), (-6.694, 267.66), (-6.694, 267.49), (-10.486, 267.66), (-10.486, 267.54)]</t>
+          <t>[(0.0, 268.0), (0.0, 267.8), (0.0, 268.0), (0.0, 267.8), (-6.694, 268.0), (-6.694, 267.83), (-10.486, 268.0), (-10.486, 267.83), (0.0, 267.8), (0.0, 267.6), (0.0, 267.8), (0.0, 267.6), (-6.694, 267.83), (-6.694, 267.66), (-10.486, 267.83), (-10.486, 267.66), (0.0, 267.6), (0.0, 267.4), (0.0, 267.6), (0.0, 267.49), (-6.694, 267.66), (-6.694, 267.49), (-10.486, 267.66), (-10.486, 267.54)]</t>
         </is>
       </c>
     </row>
@@ -3117,7 +3117,7 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>[(-0.3, 269.0), (-0.3, 268.82), (-6.61, 269.0), (-6.61, 268.82), (-6.61, 269.0), (-6.61, 268.76), (-10.361, 269.0), (-10.361, 268.76), (-0.3, 268.82), (-0.3, 268.64), (-6.61, 268.82), (-6.61, 268.64), (-6.61, 268.76), (-6.61, 268.52), (-10.361, 268.76), (-10.361, 268.58), (-0.3, 268.64), (-0.3, 268.46), (-6.61, 268.64), (-6.61, 268.52), (-6.61, 268.52), (-6.61, 268.52), (-10.361, 268.58), (-10.361, 268.58)]</t>
+          <t>[(0.0, 269.0), (0.0, 268.82), (0.0, 269.0), (0.0, 268.82), (-6.61, 269.0), (-6.61, 268.76), (-10.361, 269.0), (-10.361, 268.76), (0.0, 268.82), (0.0, 268.64), (0.0, 268.82), (0.0, 268.64), (-6.61, 268.76), (-6.61, 268.52), (-10.361, 268.76), (-10.361, 268.58), (0.0, 268.64), (0.0, 268.46), (0.0, 268.64), (0.0, 268.52), (-6.61, 268.52), (-6.61, 268.52), (-10.361, 268.58), (-10.361, 268.58)]</t>
         </is>
       </c>
     </row>
@@ -3127,7 +3127,7 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>[(-0.3, 270.0), (-0.3, 269.77), (-5.972, 270.0), (-5.972, 269.77), (-5.972, 270.0), (-5.972, 269.8), (-9.945, 270.0), (-9.945, 269.8), (-0.3, 269.77), (-0.3, 269.55), (-5.972, 269.77), (-5.972, 269.61), (-5.972, 269.8), (-5.972, 269.61), (-9.945, 269.8), (-9.945, 269.67)]</t>
+          <t>[(0.0, 270.0), (0.0, 269.77), (0.0, 270.0), (0.0, 269.77), (-5.972, 270.0), (-5.972, 269.8), (-9.945, 270.0), (-9.945, 269.8), (0.0, 269.77), (0.0, 269.55), (0.0, 269.77), (0.0, 269.61), (-5.972, 269.8), (-5.972, 269.61), (-9.945, 269.8), (-9.945, 269.67)]</t>
         </is>
       </c>
     </row>
@@ -3137,7 +3137,7 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>[(-0.3, 271.0), (-0.3, 270.8), (-5.101, 271.0), (-5.101, 270.8), (-5.101, 271.0), (-5.101, 270.82), (-8.92, 271.0), (-8.92, 270.82), (-0.3, 270.8), (-0.3, 270.6), (-5.101, 270.8), (-5.101, 270.65), (-5.101, 270.82), (-5.101, 270.65), (-8.92, 270.82), (-8.92, 270.71)]</t>
+          <t>[(0.0, 271.0), (0.0, 270.8), (0.0, 271.0), (0.0, 270.8), (-5.101, 271.0), (-5.101, 270.82), (-8.92, 271.0), (-8.92, 270.82), (0.0, 270.8), (0.0, 270.6), (0.0, 270.8), (0.0, 270.65), (-5.101, 270.82), (-5.101, 270.65), (-8.92, 270.82), (-8.92, 270.71)]</t>
         </is>
       </c>
     </row>
@@ -3147,7 +3147,7 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>[(-0.3, 272.0), (-0.3, 271.8), (-4.282, 272.0), (-4.282, 271.8), (-4.282, 272.0), (-4.282, 271.89), (-7.976, 272.0), (-7.976, 271.89), (-0.3, 271.8), (-0.3, 271.61), (-4.282, 271.8), (-4.282, 271.68), (-4.282, 271.89), (-4.282, 271.68), (-7.976, 271.89), (-7.976, 271.74)]</t>
+          <t>[(0.0, 272.0), (0.0, 271.8), (0.0, 272.0), (0.0, 271.8), (-4.282, 272.0), (-4.282, 271.89), (-7.976, 272.0), (-7.976, 271.89), (0.0, 271.8), (0.0, 271.61), (0.0, 271.8), (0.0, 271.68), (-4.282, 271.89), (-4.282, 271.68), (-7.976, 271.89), (-7.976, 271.74)]</t>
         </is>
       </c>
     </row>
@@ -3157,7 +3157,7 @@
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>[(-0.3, 273.0), (-0.3, 272.83), (-3.183, 273.0), (-3.183, 272.83), (-3.183, 273.0), (-3.183, 272.85), (-6.948, 273.0), (-6.948, 272.85), (-0.3, 272.83), (-0.3, 272.66), (-3.183, 272.83), (-3.183, 272.7), (-3.183, 272.85), (-3.183, 272.7), (-6.948, 272.85), (-6.948, 272.73)]</t>
+          <t>[(0.0, 273.0), (0.0, 272.83), (0.0, 273.0), (0.0, 272.83), (-3.183, 273.0), (-3.183, 272.85), (-6.948, 273.0), (-6.948, 272.85), (0.0, 272.83), (0.0, 272.66), (0.0, 272.83), (0.0, 272.7), (-3.183, 272.85), (-3.183, 272.7), (-6.948, 272.85), (-6.948, 272.73)]</t>
         </is>
       </c>
     </row>
@@ -3177,7 +3177,7 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>[(-0.3, 275.0), (-0.3, 274.87), (-4.864, 275.0), (-4.864, 274.87), (-0.3, 274.87), (-0.3, 274.74), (-4.864, 274.87), (-4.864, 274.74), (-0.3, 274.74), (-0.3, 274.63), (-4.864, 274.74), (-4.864, 274.63)]</t>
+          <t>[(0.0, 275.0), (0.0, 274.87), (-4.864, 275.0), (-4.864, 274.87), (0.0, 274.87), (0.0, 274.74), (-4.864, 274.87), (-4.864, 274.74), (0.0, 274.74), (0.0, 274.63), (-4.864, 274.74), (-4.864, 274.63)]</t>
         </is>
       </c>
     </row>
@@ -3187,7 +3187,7 @@
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>[(-0.3, 276.0), (-0.3, 275.8), (-4.198, 276.0), (-4.198, 275.8), (-0.3, 275.8), (-0.3, 275.62), (-4.198, 275.8), (-4.198, 275.6)]</t>
+          <t>[(0.0, 276.0), (0.0, 275.8), (-4.198, 276.0), (-4.198, 275.8), (0.0, 275.8), (0.0, 275.62), (-4.198, 275.8), (-4.198, 275.6)]</t>
         </is>
       </c>
     </row>
@@ -3197,7 +3197,7 @@
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>[(-0.3, 277.0), (-0.3, 276.84), (-3.617, 277.0), (-3.617, 276.84), (-0.3, 276.84), (-0.3, 276.68), (-3.617, 276.84), (-3.617, 276.68), (-0.3, 276.68), (-0.3, 276.55), (-3.617, 276.68), (-3.617, 276.53)]</t>
+          <t>[(0.0, 277.0), (0.0, 276.84), (-3.617, 277.0), (-3.617, 276.84), (0.0, 276.84), (0.0, 276.68), (-3.617, 276.84), (-3.617, 276.68), (0.0, 276.68), (0.0, 276.55), (-3.617, 276.68), (-3.617, 276.53)]</t>
         </is>
       </c>
     </row>
@@ -3207,7 +3207,7 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>[(-0.3, 278.0), (-0.3, 277.82), (-3.264, 278.0), (-3.264, 277.82), (-0.3, 277.82), (-0.3, 277.64), (-3.264, 277.82), (-3.264, 277.64), (-0.3, 277.64), (-0.3, 277.5), (-3.264, 277.64), (-3.264, 277.46)]</t>
+          <t>[(0.0, 278.0), (0.0, 277.82), (-3.264, 278.0), (-3.264, 277.82), (0.0, 277.82), (0.0, 277.64), (-3.264, 277.82), (-3.264, 277.64), (0.0, 277.64), (0.0, 277.5), (-3.264, 277.64), (-3.264, 277.46)]</t>
         </is>
       </c>
     </row>
@@ -3217,7 +3217,7 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>[(-0.3, 279.0), (-0.3, 278.79), (-3.209, 279.0), (-3.209, 278.79), (-0.3, 278.79), (-0.3, 278.58), (-3.209, 278.79), (-3.209, 278.58), (-0.3, 278.58), (-0.3, 278.43), (-3.209, 278.58), (-3.209, 278.39)]</t>
+          <t>[(0.0, 279.0), (0.0, 278.79), (-3.209, 279.0), (-3.209, 278.79), (0.0, 278.79), (0.0, 278.58), (-3.209, 278.79), (-3.209, 278.58), (0.0, 278.58), (0.0, 278.43), (-3.209, 278.58), (-3.209, 278.39)]</t>
         </is>
       </c>
     </row>
@@ -3227,7 +3227,7 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>[(-0.3, 280.0), (-0.3, 279.76), (-3.332, 280.0), (-3.332, 279.76), (-0.3, 279.76), (-0.3, 279.52), (-3.332, 279.76), (-3.332, 279.52), (-0.3, 279.52), (-0.3, 279.36), (-3.332, 279.52), (-3.332, 279.29)]</t>
+          <t>[(0.0, 280.0), (0.0, 279.76), (-3.332, 280.0), (-3.332, 279.76), (0.0, 279.76), (0.0, 279.52), (-3.332, 279.76), (-3.332, 279.52), (0.0, 279.52), (0.0, 279.36), (-3.332, 279.52), (-3.332, 279.29)]</t>
         </is>
       </c>
     </row>
@@ -3237,7 +3237,7 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>[(-0.3, 281.0), (-0.3, 280.75), (-3.387, 281.0), (-3.387, 280.75), (-0.3, 280.75), (-0.3, 280.5), (-3.387, 280.75), (-3.387, 280.5), (-0.3, 280.5), (-0.3, 280.34), (-3.387, 280.5), (-3.387, 280.26)]</t>
+          <t>[(0.0, 281.0), (0.0, 280.75), (-3.387, 281.0), (-3.387, 280.75), (0.0, 280.75), (0.0, 280.5), (-3.387, 280.75), (-3.387, 280.5), (0.0, 280.5), (0.0, 280.34), (-3.387, 280.5), (-3.387, 280.26)]</t>
         </is>
       </c>
     </row>
@@ -3247,7 +3247,7 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>[(-0.3, 282.0), (-0.3, 281.75), (-3.34, 282.0), (-3.34, 281.75), (-0.3, 281.75), (-0.3, 281.5), (-3.34, 281.75), (-3.34, 281.5), (-0.3, 281.5), (-0.3, 281.36), (-3.34, 281.5), (-3.34, 281.27)]</t>
+          <t>[(0.0, 282.0), (0.0, 281.75), (-3.34, 282.0), (-3.34, 281.75), (0.0, 281.75), (0.0, 281.5), (-3.34, 281.75), (-3.34, 281.5), (0.0, 281.5), (0.0, 281.36), (-3.34, 281.5), (-3.34, 281.27)]</t>
         </is>
       </c>
     </row>
@@ -3257,7 +3257,7 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>[(-0.3, 283.0), (-0.3, 282.8), (-3.153, 283.0), (-3.153, 282.8), (-0.3, 282.8), (-0.3, 282.6), (-3.153, 282.8), (-3.153, 282.6), (-0.3, 282.6), (-0.3, 282.4), (-3.153, 282.6), (-3.153, 282.4), (-0.3, 282.4), (-0.3, 282.29), (-3.153, 282.4), (-3.153, 282.23)]</t>
+          <t>[(0.0, 283.0), (0.0, 282.8), (-3.153, 283.0), (-3.153, 282.8), (0.0, 282.8), (0.0, 282.6), (-3.153, 282.8), (-3.153, 282.6), (0.0, 282.6), (0.0, 282.4), (-3.153, 282.6), (-3.153, 282.4), (0.0, 282.4), (0.0, 282.29), (-3.153, 282.4), (-3.153, 282.23)]</t>
         </is>
       </c>
     </row>
@@ -3267,7 +3267,7 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>[(-0.3, 284.0), (-0.3, 283.75), (-2.809, 284.0), (-2.809, 283.75), (-0.3, 283.75), (-0.3, 283.5), (-2.809, 283.75), (-2.809, 283.5), (-0.3, 283.5), (-0.3, 283.36), (-2.809, 283.5), (-2.809, 283.27)]</t>
+          <t>[(0.0, 284.0), (0.0, 283.75), (-2.809, 284.0), (-2.809, 283.75), (0.0, 283.75), (0.0, 283.5), (-2.809, 283.75), (-2.809, 283.5), (0.0, 283.5), (0.0, 283.36), (-2.809, 283.5), (-2.809, 283.27)]</t>
         </is>
       </c>
     </row>
@@ -3277,7 +3277,7 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>[(-0.3, 285.0), (-0.3, 284.77), (-2.587, 285.0), (-2.587, 284.77), (-0.3, 284.77), (-0.3, 284.54), (-2.587, 284.77), (-2.587, 284.54), (-0.3, 284.54), (-0.3, 284.4), (-2.587, 284.54), (-2.587, 284.33)]</t>
+          <t>[(0.0, 285.0), (0.0, 284.77), (-2.587, 285.0), (-2.587, 284.77), (0.0, 284.77), (0.0, 284.54), (-2.587, 284.77), (-2.587, 284.54), (0.0, 284.54), (0.0, 284.4), (-2.587, 284.54), (-2.587, 284.33)]</t>
         </is>
       </c>
     </row>
@@ -3287,7 +3287,7 @@
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>[(-0.3, 286.0), (-0.3, 285.77), (-2.332, 286.0), (-2.332, 285.77), (-0.3, 285.77), (-0.3, 285.54), (-2.332, 285.77), (-2.332, 285.54), (-0.3, 285.54), (-0.3, 285.4), (-2.332, 285.54), (-2.332, 285.33)]</t>
+          <t>[(0.0, 286.0), (0.0, 285.77), (-2.332, 286.0), (-2.332, 285.77), (0.0, 285.77), (0.0, 285.54), (-2.332, 285.77), (-2.332, 285.54), (0.0, 285.54), (0.0, 285.4), (-2.332, 285.54), (-2.332, 285.33)]</t>
         </is>
       </c>
     </row>
@@ -3337,7 +3337,7 @@
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>[(-0.3, 291.0), (-0.3, 290.8), (-2.383, 291.0), (-2.383, 290.8), (-0.3, 290.8), (-0.3, 290.61), (-2.383, 290.8), (-2.383, 290.66)]</t>
+          <t>[(0.0, 291.0), (0.0, 290.8), (-2.383, 291.0), (-2.383, 290.8), (0.0, 290.8), (0.0, 290.61), (-2.383, 290.8), (-2.383, 290.66)]</t>
         </is>
       </c>
     </row>
@@ -3357,7 +3357,7 @@
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>[(-0.3, 293.0), (-0.3, 292.84), (-2.637, 293.0), (-2.637, 292.84), (-0.3, 292.84), (-0.3, 292.69), (-2.637, 292.84), (-2.637, 292.71)]</t>
+          <t>[(0.0, 293.0), (0.0, 292.84), (-2.637, 293.0), (-2.637, 292.84), (0.0, 292.84), (0.0, 292.69), (-2.637, 292.84), (-2.637, 292.71)]</t>
         </is>
       </c>
     </row>
@@ -3367,7 +3367,7 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>[(-0.3, 294.0), (-0.3, 293.84), (-2.775, 294.0), (-2.775, 293.84), (-0.3, 293.84), (-0.3, 293.68), (-2.775, 293.84), (-2.775, 293.71)]</t>
+          <t>[(0.0, 294.0), (0.0, 293.84), (-2.775, 294.0), (-2.775, 293.84), (0.0, 293.84), (0.0, 293.68), (-2.775, 293.84), (-2.775, 293.71)]</t>
         </is>
       </c>
     </row>
@@ -3377,7 +3377,7 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>[(-0.3, 295.0), (-0.3, 294.82), (-2.84, 295.0), (-2.84, 294.82), (-0.3, 294.82), (-0.3, 294.65), (-2.84, 294.82), (-2.84, 294.67)]</t>
+          <t>[(0.0, 295.0), (0.0, 294.82), (-2.84, 295.0), (-2.84, 294.82), (0.0, 294.82), (0.0, 294.65), (-2.84, 294.82), (-2.84, 294.67)]</t>
         </is>
       </c>
     </row>
@@ -3387,7 +3387,7 @@
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>[(-0.3, 296.0), (-0.3, 295.8), (-2.912, 296.0), (-2.912, 295.8), (-0.3, 295.8), (-0.3, 295.6), (-2.912, 295.8), (-2.912, 295.64)]</t>
+          <t>[(0.0, 296.0), (0.0, 295.8), (-2.912, 296.0), (-2.912, 295.8), (0.0, 295.8), (0.0, 295.6), (-2.912, 295.8), (-2.912, 295.64)]</t>
         </is>
       </c>
     </row>
@@ -3397,7 +3397,7 @@
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>[(-0.3, 297.0), (-0.3, 296.85), (-3.01, 297.0), (-3.01, 296.85), (-0.3, 296.85), (-0.3, 296.7), (-3.01, 296.85), (-3.01, 296.7), (-0.3, 296.7), (-0.3, 296.57), (-3.01, 296.7), (-3.01, 296.58)]</t>
+          <t>[(0.0, 297.0), (0.0, 296.85), (-3.01, 297.0), (-3.01, 296.85), (0.0, 296.85), (0.0, 296.7), (-3.01, 296.85), (-3.01, 296.7), (0.0, 296.7), (0.0, 296.57), (-3.01, 296.7), (-3.01, 296.58)]</t>
         </is>
       </c>
     </row>
@@ -3407,7 +3407,7 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>[(-0.3, 298.0), (-0.3, 297.82), (-2.908, 298.0), (-2.908, 297.82), (-0.3, 297.82), (-0.3, 297.64), (-2.908, 297.82), (-2.908, 297.64), (-0.3, 297.64), (-0.3, 297.5), (-2.908, 297.64), (-2.908, 297.48)]</t>
+          <t>[(0.0, 298.0), (0.0, 297.82), (-2.908, 298.0), (-2.908, 297.82), (0.0, 297.82), (0.0, 297.64), (-2.908, 297.82), (-2.908, 297.64), (0.0, 297.64), (0.0, 297.5), (-2.908, 297.64), (-2.908, 297.48)]</t>
         </is>
       </c>
     </row>
@@ -3417,7 +3417,7 @@
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>[(-0.3, 299.0), (-0.3, 298.83), (-2.859, 299.0), (-2.859, 298.83), (-0.3, 298.83), (-0.3, 298.66), (-2.859, 298.83), (-2.859, 298.66), (-0.3, 298.66), (-0.3, 298.53), (-2.859, 298.66), (-2.859, 298.5)]</t>
+          <t>[(0.0, 299.0), (0.0, 298.83), (-2.859, 299.0), (-2.859, 298.83), (0.0, 298.83), (0.0, 298.66), (-2.859, 298.83), (-2.859, 298.66), (0.0, 298.66), (0.0, 298.53), (-2.859, 298.66), (-2.859, 298.5)]</t>
         </is>
       </c>
     </row>
@@ -3427,7 +3427,7 @@
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>[(-0.3, 300.0), (-0.3, 299.82), (-2.716, 300.0), (-2.716, 299.82), (-0.3, 299.82), (-0.3, 299.64), (-2.716, 299.82), (-2.716, 299.64), (-0.3, 299.64), (-0.3, 299.51), (-2.716, 299.64), (-2.716, 299.46)]</t>
+          <t>[(0.0, 300.0), (0.0, 299.82), (-2.716, 300.0), (-2.716, 299.82), (0.0, 299.82), (0.0, 299.64), (-2.716, 299.82), (-2.716, 299.64), (0.0, 299.64), (0.0, 299.51), (-2.716, 299.64), (-2.716, 299.46)]</t>
         </is>
       </c>
     </row>
@@ -3437,7 +3437,7 @@
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>[(-0.3, 301.0), (-0.3, 300.82), (-2.574, 301.0), (-2.574, 300.82), (-0.3, 300.82), (-0.3, 300.64), (-2.574, 300.82), (-2.574, 300.64), (-0.3, 300.64), (-0.3, 300.5), (-2.574, 300.64), (-2.574, 300.46)]</t>
+          <t>[(0.0, 301.0), (0.0, 300.82), (-2.574, 301.0), (-2.574, 300.82), (0.0, 300.82), (0.0, 300.64), (-2.574, 300.82), (-2.574, 300.64), (0.0, 300.64), (0.0, 300.5), (-2.574, 300.64), (-2.574, 300.46)]</t>
         </is>
       </c>
     </row>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>[(-0.3, 302.0), (-0.3, 301.78), (-2.465, 302.0), (-2.465, 301.78), (-0.3, 301.78), (-0.3, 301.56), (-2.465, 301.78), (-2.465, 301.56), (-0.3, 301.56), (-0.3, 301.42), (-2.465, 301.56), (-2.465, 301.36)]</t>
+          <t>[(0.0, 302.0), (0.0, 301.78), (-2.465, 302.0), (-2.465, 301.78), (0.0, 301.78), (0.0, 301.56), (-2.465, 301.78), (-2.465, 301.56), (0.0, 301.56), (0.0, 301.42), (-2.465, 301.56), (-2.465, 301.36)]</t>
         </is>
       </c>
     </row>
@@ -4247,7 +4247,7 @@
       </c>
       <c r="B383" t="inlineStr">
         <is>
-          <t>[(-0.3, 382.0), (-0.3, 381.88), (-2.403, 382.0), (-2.403, 381.88), (-0.3, 381.88), (-0.3, 381.76), (-2.403, 381.88), (-2.403, 381.76), (-0.3, 381.76), (-0.3, 381.65), (-2.403, 381.76), (-2.403, 381.65)]</t>
+          <t>[(0.0, 382.0), (0.0, 381.88), (-2.403, 382.0), (-2.403, 381.88), (0.0, 381.88), (0.0, 381.76), (-2.403, 381.88), (-2.403, 381.76), (0.0, 381.76), (0.0, 381.65), (-2.403, 381.76), (-2.403, 381.65)]</t>
         </is>
       </c>
     </row>
@@ -4257,7 +4257,7 @@
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>[(-0.3, 383.0), (-0.3, 382.86), (-2.438, 383.0), (-2.438, 382.86), (-0.3, 382.86), (-0.3, 382.72), (-2.438, 382.86), (-2.438, 382.72), (-0.3, 382.72), (-0.3, 382.61), (-2.438, 382.72), (-2.438, 382.61)]</t>
+          <t>[(0.0, 383.0), (0.0, 382.86), (-2.438, 383.0), (-2.438, 382.86), (0.0, 382.86), (0.0, 382.72), (-2.438, 382.86), (-2.438, 382.72), (0.0, 382.72), (0.0, 382.61), (-2.438, 382.72), (-2.438, 382.61)]</t>
         </is>
       </c>
     </row>
@@ -4817,7 +4817,7 @@
       </c>
       <c r="B440" t="inlineStr">
         <is>
-          <t>[(-0.3, 439.0), (-0.3, 438.83), (-4.836, 439.0), (-4.836, 438.83), (-0.3, 438.83), (-0.3, 438.69), (-4.836, 438.83), (-4.836, 438.66)]</t>
+          <t>[(0.0, 439.0), (0.0, 438.83), (-4.836, 439.0), (-4.836, 438.83), (0.0, 438.83), (0.0, 438.69), (-4.836, 438.83), (-4.836, 438.66)]</t>
         </is>
       </c>
     </row>
@@ -4827,7 +4827,7 @@
       </c>
       <c r="B441" t="inlineStr">
         <is>
-          <t>[(-0.3, 440.0), (-0.3, 439.83), (-2.75, 440.0), (-2.75, 439.83), (-0.3, 439.83), (-0.3, 439.68), (-2.75, 439.83), (-2.75, 439.66)]</t>
+          <t>[(0.0, 440.0), (0.0, 439.83), (-2.75, 440.0), (-2.75, 439.83), (0.0, 439.83), (0.0, 439.68), (-2.75, 439.83), (-2.75, 439.66)]</t>
         </is>
       </c>
     </row>
@@ -4837,7 +4837,7 @@
       </c>
       <c r="B442" t="inlineStr">
         <is>
-          <t>[(-0.3, 441.0), (-0.3, 440.83), (-4.523, 441.0), (-4.523, 440.83), (-0.3, 440.83), (-0.3, 440.69), (-4.523, 440.83), (-4.523, 440.67)]</t>
+          <t>[(0.0, 441.0), (0.0, 440.83), (-4.523, 441.0), (-4.523, 440.83), (0.0, 440.83), (0.0, 440.69), (-4.523, 440.83), (-4.523, 440.67)]</t>
         </is>
       </c>
     </row>
@@ -4847,7 +4847,7 @@
       </c>
       <c r="B443" t="inlineStr">
         <is>
-          <t>[(-0.3, 442.0), (-0.3, 441.83), (-5.604, 442.0), (-5.604, 441.83), (-0.3, 441.83), (-0.3, 441.67), (-5.604, 441.83), (-5.604, 441.67)]</t>
+          <t>[(0.0, 442.0), (0.0, 441.83), (-5.604, 442.0), (-5.604, 441.83), (0.0, 441.83), (0.0, 441.67), (-5.604, 441.83), (-5.604, 441.67)]</t>
         </is>
       </c>
     </row>
@@ -4857,7 +4857,7 @@
       </c>
       <c r="B444" t="inlineStr">
         <is>
-          <t>[(-0.3, 443.0), (-0.3, 442.81), (-6.634, 443.0), (-6.634, 442.81), (-0.3, 442.81), (-0.3, 442.64), (-6.634, 442.81), (-6.634, 442.63)]</t>
+          <t>[(0.0, 443.0), (0.0, 442.81), (-6.634, 443.0), (-6.634, 442.81), (0.0, 442.81), (0.0, 442.64), (-6.634, 442.81), (-6.634, 442.63)]</t>
         </is>
       </c>
     </row>
@@ -4867,7 +4867,7 @@
       </c>
       <c r="B445" t="inlineStr">
         <is>
-          <t>[(-0.3, 444.0), (-0.3, 443.86), (-2.622, 444.0), (-2.622, 443.86), (-0.3, 443.86), (-0.3, 443.72), (-2.622, 443.86), (-2.622, 443.72), (-0.3, 443.72), (-0.3, 443.61), (-2.622, 443.72), (-2.622, 443.61)]</t>
+          <t>[(0.0, 444.0), (0.0, 443.86), (-2.622, 444.0), (-2.622, 443.86), (0.0, 443.86), (0.0, 443.72), (-2.622, 443.86), (-2.622, 443.72), (0.0, 443.72), (0.0, 443.61), (-2.622, 443.72), (-2.622, 443.61)]</t>
         </is>
       </c>
     </row>
@@ -4877,7 +4877,7 @@
       </c>
       <c r="B446" t="inlineStr">
         <is>
-          <t>[(-0.3, 445.0), (-0.3, 444.87), (-3.713, 445.0), (-3.713, 444.87), (-0.3, 444.87), (-0.3, 444.74), (-3.713, 444.87), (-3.713, 444.74), (-0.3, 444.74), (-0.3, 444.63), (-3.713, 444.74), (-3.713, 444.62)]</t>
+          <t>[(0.0, 445.0), (0.0, 444.87), (-3.713, 445.0), (-3.713, 444.87), (0.0, 444.87), (0.0, 444.74), (-3.713, 444.87), (-3.713, 444.74), (0.0, 444.74), (0.0, 444.63), (-3.713, 444.74), (-3.713, 444.62)]</t>
         </is>
       </c>
     </row>
@@ -4887,7 +4887,7 @@
       </c>
       <c r="B447" t="inlineStr">
         <is>
-          <t>[(-0.3, 446.0), (-0.3, 445.83), (-5.03, 446.0), (-5.03, 445.83), (-0.3, 445.83), (-0.3, 445.66), (-5.03, 445.83), (-5.03, 445.66)]</t>
+          <t>[(0.0, 446.0), (0.0, 445.83), (-5.03, 446.0), (-5.03, 445.83), (0.0, 445.83), (0.0, 445.66), (-5.03, 445.83), (-5.03, 445.66)]</t>
         </is>
       </c>
     </row>
@@ -4897,7 +4897,7 @@
       </c>
       <c r="B448" t="inlineStr">
         <is>
-          <t>[(-0.3, 447.0), (-0.3, 446.8), (-5.47, 447.0), (-5.47, 446.8), (-0.3, 446.8), (-0.3, 446.61), (-5.47, 446.8), (-5.47, 446.63)]</t>
+          <t>[(0.0, 447.0), (0.0, 446.8), (-5.47, 447.0), (-5.47, 446.8), (0.0, 446.8), (0.0, 446.61), (-5.47, 446.8), (-5.47, 446.63)]</t>
         </is>
       </c>
     </row>
@@ -4907,7 +4907,7 @@
       </c>
       <c r="B449" t="inlineStr">
         <is>
-          <t>[(-0.3, 448.0), (-0.3, 447.86), (-5.501, 448.0), (-5.501, 447.86), (-0.3, 447.86), (-0.3, 447.56), (-5.501, 447.86), (-5.501, 447.7)]</t>
+          <t>[(0.0, 448.0), (0.0, 447.86), (-5.501, 448.0), (-5.501, 447.86), (0.0, 447.86), (0.0, 447.56), (-5.501, 447.86), (-5.501, 447.7)]</t>
         </is>
       </c>
     </row>
@@ -4917,7 +4917,7 @@
       </c>
       <c r="B450" t="inlineStr">
         <is>
-          <t>[(-0.3, 449.0), (-0.3, 448.85), (-8.746, 449.0), (-8.746, 448.85), (-0.3, 448.85), (-0.3, 448.7), (-8.746, 448.85), (-8.746, 448.7), (-0.3, 448.7), (-0.3, 448.55), (-8.746, 448.7), (-8.746, 448.56)]</t>
+          <t>[(0.0, 449.0), (0.0, 448.85), (-8.746, 449.0), (-8.746, 448.85), (0.0, 448.85), (0.0, 448.7), (-8.746, 448.85), (-8.746, 448.7), (0.0, 448.7), (0.0, 448.55), (-8.746, 448.7), (-8.746, 448.56)]</t>
         </is>
       </c>
     </row>
@@ -4927,7 +4927,7 @@
       </c>
       <c r="B451" t="inlineStr">
         <is>
-          <t>[(-0.3, 450.0), (-0.3, 449.79), (-7.23, 450.0), (-7.23, 449.79), (-0.3, 449.79), (-0.3, 449.58), (-7.23, 449.79), (-7.23, 449.64)]</t>
+          <t>[(0.0, 450.0), (0.0, 449.79), (-7.23, 450.0), (-7.23, 449.79), (0.0, 449.79), (0.0, 449.58), (-7.23, 449.79), (-7.23, 449.64)]</t>
         </is>
       </c>
     </row>
@@ -4937,7 +4937,7 @@
       </c>
       <c r="B452" t="inlineStr">
         <is>
-          <t>[(-0.3, 451.0), (-0.3, 450.81), (-6.067, 451.0), (-6.067, 450.81), (-0.3, 450.81), (-0.3, 450.62), (-6.067, 450.81), (-6.067, 450.65)]</t>
+          <t>[(0.0, 451.0), (0.0, 450.81), (-6.067, 451.0), (-6.067, 450.81), (0.0, 450.81), (0.0, 450.62), (-6.067, 450.81), (-6.067, 450.65)]</t>
         </is>
       </c>
     </row>
@@ -4947,7 +4947,7 @@
       </c>
       <c r="B453" t="inlineStr">
         <is>
-          <t>[(-0.3, 452.0), (-0.3, 451.82), (-6.353, 452.0), (-6.353, 451.82), (-0.3, 451.82), (-0.3, 451.65), (-6.353, 451.82), (-6.353, 451.69)]</t>
+          <t>[(0.0, 452.0), (0.0, 451.82), (-6.353, 452.0), (-6.353, 451.82), (0.0, 451.82), (0.0, 451.65), (-6.353, 451.82), (-6.353, 451.69)]</t>
         </is>
       </c>
     </row>
@@ -4957,7 +4957,7 @@
       </c>
       <c r="B454" t="inlineStr">
         <is>
-          <t>[(-0.3, 453.0), (-0.3, 452.84), (-6.671, 453.0), (-6.671, 452.84), (-0.3, 452.84), (-0.3, 452.68), (-6.671, 452.84), (-6.671, 452.71)]</t>
+          <t>[(0.0, 453.0), (0.0, 452.84), (-6.671, 453.0), (-6.671, 452.84), (0.0, 452.84), (0.0, 452.68), (-6.671, 452.84), (-6.671, 452.71)]</t>
         </is>
       </c>
     </row>
@@ -4967,7 +4967,7 @@
       </c>
       <c r="B455" t="inlineStr">
         <is>
-          <t>[(-0.3, 454.0), (-0.3, 453.84), (-6.993, 454.0), (-6.993, 453.84), (-0.3, 453.84), (-0.3, 453.68), (-6.993, 453.84), (-6.993, 453.71)]</t>
+          <t>[(0.0, 454.0), (0.0, 453.84), (-6.993, 454.0), (-6.993, 453.84), (0.0, 453.84), (0.0, 453.68), (-6.993, 453.84), (-6.993, 453.71)]</t>
         </is>
       </c>
     </row>
@@ -4977,7 +4977,7 @@
       </c>
       <c r="B456" t="inlineStr">
         <is>
-          <t>[(-0.3, 455.0), (-0.3, 454.82), (-7.248, 455.0), (-7.248, 454.82), (-0.3, 454.82), (-0.3, 454.64), (-7.248, 454.82), (-7.248, 454.68)]</t>
+          <t>[(0.0, 455.0), (0.0, 454.82), (-7.248, 455.0), (-7.248, 454.82), (0.0, 454.82), (0.0, 454.64), (-7.248, 454.82), (-7.248, 454.68)]</t>
         </is>
       </c>
     </row>
@@ -4987,7 +4987,7 @@
       </c>
       <c r="B457" t="inlineStr">
         <is>
-          <t>[(-0.3, 456.0), (-0.3, 455.83), (-7.525, 456.0), (-7.525, 455.83), (-0.3, 455.83), (-0.3, 455.66), (-7.525, 455.83), (-7.525, 455.71)]</t>
+          <t>[(0.0, 456.0), (0.0, 455.83), (-7.525, 456.0), (-7.525, 455.83), (0.0, 455.83), (0.0, 455.66), (-7.525, 455.83), (-7.525, 455.71)]</t>
         </is>
       </c>
     </row>
@@ -4997,7 +4997,7 @@
       </c>
       <c r="B458" t="inlineStr">
         <is>
-          <t>[(-0.3, 457.0), (-0.3, 456.8), (-7.834, 457.0), (-7.834, 456.8), (-0.3, 456.8), (-0.3, 456.6), (-7.834, 456.8), (-7.834, 456.67)]</t>
+          <t>[(0.0, 457.0), (0.0, 456.8), (-7.834, 457.0), (-7.834, 456.8), (0.0, 456.8), (0.0, 456.6), (-7.834, 456.8), (-7.834, 456.67)]</t>
         </is>
       </c>
     </row>
@@ -5007,7 +5007,7 @@
       </c>
       <c r="B459" t="inlineStr">
         <is>
-          <t>[(-0.3, 458.0), (-0.3, 457.89), (-8.13, 458.0), (-8.13, 457.89), (-0.3, 457.89), (-0.3, 457.62), (-8.13, 457.89), (-8.13, 457.71)]</t>
+          <t>[(0.0, 458.0), (0.0, 457.89), (-8.13, 458.0), (-8.13, 457.89), (0.0, 457.89), (0.0, 457.62), (-8.13, 457.89), (-8.13, 457.71)]</t>
         </is>
       </c>
     </row>
@@ -5027,7 +5027,7 @@
       </c>
       <c r="B461" t="inlineStr">
         <is>
-          <t>[(-0.3, 460.0), (-0.3, 459.84), (-8.559, 460.0), (-8.559, 459.84), (-0.3, 459.84), (-0.3, 459.68), (-8.559, 459.84), (-8.559, 459.71)]</t>
+          <t>[(0.0, 460.0), (0.0, 459.84), (-8.559, 460.0), (-8.559, 459.84), (0.0, 459.84), (0.0, 459.68), (-8.559, 459.84), (-8.559, 459.71)]</t>
         </is>
       </c>
     </row>
@@ -5037,7 +5037,7 @@
       </c>
       <c r="B462" t="inlineStr">
         <is>
-          <t>[(-0.3, 461.0), (-0.3, 460.81), (-8.777, 461.0), (-8.777, 460.81), (-0.3, 460.81), (-0.3, 460.67), (-8.777, 460.81), (-8.777, 460.63)]</t>
+          <t>[(0.0, 461.0), (0.0, 460.81), (-8.777, 461.0), (-8.777, 460.81), (0.0, 460.81), (0.0, 460.67), (-8.777, 460.81), (-8.777, 460.63)]</t>
         </is>
       </c>
     </row>
@@ -5067,7 +5067,7 @@
       </c>
       <c r="B465" t="inlineStr">
         <is>
-          <t>[(-0.3, 464.0), (-0.3, 463.85), (-2.353, 464.0), (-2.353, 463.85), (-2.353, 464.0), (-2.353, 463.89), (-9.118, 464.0), (-9.118, 463.89), (-0.3, 463.85), (-0.3, 463.74), (-2.353, 463.85), (-2.353, 463.72), (-2.353, 463.89), (-2.353, 463.72), (-9.118, 463.89), (-9.118, 463.62)]</t>
+          <t>[(0.0, 464.0), (0.0, 463.85), (0.0, 464.0), (0.0, 463.85), (-2.353, 464.0), (-2.353, 463.89), (-9.118, 464.0), (-9.118, 463.89), (0.0, 463.85), (0.0, 463.74), (0.0, 463.85), (0.0, 463.72), (-2.353, 463.89), (-2.353, 463.72), (-9.118, 463.89), (-9.118, 463.62)]</t>
         </is>
       </c>
     </row>
@@ -5077,7 +5077,7 @@
       </c>
       <c r="B466" t="inlineStr">
         <is>
-          <t>[(-0.3, 465.0), (-0.3, 464.85), (-2.525, 465.0), (-2.525, 464.85), (-2.525, 465.0), (-2.525, 464.87), (-9.207, 465.0), (-9.207, 464.87), (-0.3, 464.85), (-0.3, 464.74), (-2.525, 464.85), (-2.525, 464.72), (-2.525, 464.87), (-2.525, 464.72), (-9.207, 464.87), (-9.207, 464.57)]</t>
+          <t>[(0.0, 465.0), (0.0, 464.85), (0.0, 465.0), (0.0, 464.85), (-2.525, 465.0), (-2.525, 464.87), (-9.207, 465.0), (-9.207, 464.87), (0.0, 464.85), (0.0, 464.74), (0.0, 464.85), (0.0, 464.72), (-2.525, 464.87), (-2.525, 464.72), (-9.207, 464.87), (-9.207, 464.57)]</t>
         </is>
       </c>
     </row>
@@ -5117,7 +5117,7 @@
       </c>
       <c r="B470" t="inlineStr">
         <is>
-          <t>[(-0.3, 469.0), (-0.3, 468.84), (-3.597, 469.0), (-3.597, 468.84), (-3.597, 469.0), (-3.597, 468.86), (-10.382, 469.0), (-10.382, 468.86), (-0.3, 468.84), (-0.3, 468.72), (-3.597, 468.84), (-3.597, 468.68), (-3.597, 468.86), (-3.597, 468.68), (-10.382, 468.86), (-10.382, 468.56)]</t>
+          <t>[(0.0, 469.0), (0.0, 468.84), (0.0, 469.0), (0.0, 468.84), (-3.597, 469.0), (-3.597, 468.86), (-10.382, 469.0), (-10.382, 468.86), (0.0, 468.84), (0.0, 468.72), (0.0, 468.84), (0.0, 468.68), (-3.597, 468.86), (-3.597, 468.68), (-10.382, 468.86), (-10.382, 468.56)]</t>
         </is>
       </c>
     </row>
@@ -5137,7 +5137,7 @@
       </c>
       <c r="B472" t="inlineStr">
         <is>
-          <t>[(-0.3, 471.0), (-0.3, 470.84), (-4.191, 471.0), (-4.191, 470.84), (-4.191, 471.0), (-4.191, 470.85), (-10.943, 471.0), (-10.943, 470.85), (-0.3, 470.84), (-0.3, 470.72), (-4.191, 470.84), (-4.191, 470.69), (-4.191, 470.85), (-4.191, 470.69), (-10.943, 470.85), (-10.943, 470.55)]</t>
+          <t>[(0.0, 471.0), (0.0, 470.84), (0.0, 471.0), (0.0, 470.84), (-4.191, 471.0), (-4.191, 470.85), (-10.943, 471.0), (-10.943, 470.85), (0.0, 470.84), (0.0, 470.72), (0.0, 470.84), (0.0, 470.69), (-4.191, 470.85), (-4.191, 470.69), (-10.943, 470.85), (-10.943, 470.55)]</t>
         </is>
       </c>
     </row>
@@ -5147,7 +5147,7 @@
       </c>
       <c r="B473" t="inlineStr">
         <is>
-          <t>[(-0.3, 472.0), (-0.3, 471.86), (-4.416, 472.0), (-4.416, 471.86), (-4.416, 472.0), (-4.416, 471.85), (-11.157, 472.0), (-11.157, 471.85), (-0.3, 471.86), (-0.3, 471.74), (-4.416, 471.86), (-4.416, 471.73), (-4.416, 471.85), (-4.416, 471.73), (-11.157, 471.85), (-11.157, 471.55)]</t>
+          <t>[(0.0, 472.0), (0.0, 471.86), (0.0, 472.0), (0.0, 471.86), (-4.416, 472.0), (-4.416, 471.85), (-11.157, 472.0), (-11.157, 471.85), (0.0, 471.86), (0.0, 471.74), (0.0, 471.86), (0.0, 471.73), (-4.416, 471.85), (-4.416, 471.73), (-11.157, 471.85), (-11.157, 471.55)]</t>
         </is>
       </c>
     </row>
@@ -5177,7 +5177,7 @@
       </c>
       <c r="B476" t="inlineStr">
         <is>
-          <t>[(-0.3, 475.0), (-0.3, 474.85), (-4.821, 475.0), (-4.821, 474.85), (-4.821, 475.0), (-4.821, 474.86), (-11.595, 475.0), (-11.595, 474.86), (-0.3, 474.85), (-0.3, 474.74), (-4.821, 474.85), (-4.821, 474.71), (-4.821, 474.86), (-4.821, 474.71), (-11.595, 474.86), (-11.595, 474.56)]</t>
+          <t>[(0.0, 475.0), (0.0, 474.85), (0.0, 475.0), (0.0, 474.85), (-4.821, 475.0), (-4.821, 474.86), (-11.595, 475.0), (-11.595, 474.86), (0.0, 474.85), (0.0, 474.74), (0.0, 474.85), (0.0, 474.71), (-4.821, 474.86), (-4.821, 474.71), (-11.595, 474.86), (-11.595, 474.56)]</t>
         </is>
       </c>
     </row>
@@ -5187,7 +5187,7 @@
       </c>
       <c r="B477" t="inlineStr">
         <is>
-          <t>[(-0.3, 476.0), (-0.3, 475.85), (-4.916, 476.0), (-4.916, 475.85), (-4.916, 476.0), (-4.916, 475.89), (-11.628, 476.0), (-11.628, 475.89), (-0.3, 475.85), (-0.3, 475.74), (-4.916, 475.85), (-4.916, 475.71), (-4.916, 475.89), (-4.916, 475.71), (-11.628, 475.89), (-11.628, 475.59)]</t>
+          <t>[(0.0, 476.0), (0.0, 475.85), (0.0, 476.0), (0.0, 475.85), (-4.916, 476.0), (-4.916, 475.89), (-11.628, 476.0), (-11.628, 475.89), (0.0, 475.85), (0.0, 475.74), (0.0, 475.85), (0.0, 475.71), (-4.916, 475.89), (-4.916, 475.71), (-11.628, 475.89), (-11.628, 475.59)]</t>
         </is>
       </c>
     </row>
@@ -5247,7 +5247,7 @@
       </c>
       <c r="B483" t="inlineStr">
         <is>
-          <t>[(-0.3, 482.0), (-0.3, 481.84), (-4.711, 482.0), (-4.711, 481.84), (-4.711, 482.0), (-4.711, 481.81), (-11.456, 482.0), (-11.456, 481.81), (-0.3, 481.84), (-0.3, 481.73), (-4.711, 481.84), (-4.711, 481.69), (-4.711, 481.81), (-4.711, 481.69), (-11.456, 481.81), (-11.456, 481.51)]</t>
+          <t>[(0.0, 482.0), (0.0, 481.84), (0.0, 482.0), (0.0, 481.84), (-4.711, 482.0), (-4.711, 481.81), (-11.456, 482.0), (-11.456, 481.81), (0.0, 481.84), (0.0, 481.73), (0.0, 481.84), (0.0, 481.69), (-4.711, 481.81), (-4.711, 481.69), (-11.456, 481.81), (-11.456, 481.51)]</t>
         </is>
       </c>
     </row>
@@ -5257,7 +5257,7 @@
       </c>
       <c r="B484" t="inlineStr">
         <is>
-          <t>[(-0.3, 483.0), (-0.3, 482.83), (-4.708, 483.0), (-4.708, 482.83), (-4.708, 483.0), (-4.708, 482.81), (-11.451, 483.0), (-11.451, 482.81), (-0.3, 482.83), (-0.3, 482.71), (-4.708, 482.83), (-4.708, 482.67), (-4.708, 482.81), (-4.708, 482.67), (-11.451, 482.81), (-11.451, 482.51)]</t>
+          <t>[(0.0, 483.0), (0.0, 482.83), (0.0, 483.0), (0.0, 482.83), (-4.708, 483.0), (-4.708, 482.81), (-11.451, 483.0), (-11.451, 482.81), (0.0, 482.83), (0.0, 482.71), (0.0, 482.83), (0.0, 482.67), (-4.708, 482.81), (-4.708, 482.67), (-11.451, 482.81), (-11.451, 482.51)]</t>
         </is>
       </c>
     </row>
@@ -5267,7 +5267,7 @@
       </c>
       <c r="B485" t="inlineStr">
         <is>
-          <t>[(-0.3, 484.0), (-0.3, 483.82), (-4.827, 484.0), (-4.827, 483.82), (-4.827, 484.0), (-4.827, 483.75), (-11.636, 484.0), (-11.636, 483.75), (-0.3, 483.82), (-0.3, 483.69), (-4.827, 483.82), (-4.827, 483.64), (-4.827, 483.75), (-4.827, 483.64), (-11.636, 483.75), (-11.636, 483.51)]</t>
+          <t>[(0.0, 484.0), (0.0, 483.82), (0.0, 484.0), (0.0, 483.82), (-4.827, 484.0), (-4.827, 483.75), (-11.636, 484.0), (-11.636, 483.75), (0.0, 483.82), (0.0, 483.69), (0.0, 483.82), (0.0, 483.64), (-4.827, 483.75), (-4.827, 483.64), (-11.636, 483.75), (-11.636, 483.51)]</t>
         </is>
       </c>
     </row>
@@ -5277,7 +5277,7 @@
       </c>
       <c r="B486" t="inlineStr">
         <is>
-          <t>[(-0.3, 485.0), (-0.3, 484.82), (-5.008, 485.0), (-5.008, 484.82), (-5.008, 485.0), (-5.008, 484.78), (-11.805, 485.0), (-11.805, 484.78), (-0.3, 484.82), (-0.3, 484.67), (-5.008, 484.82), (-5.008, 484.65), (-5.008, 484.78), (-5.008, 484.65), (-11.805, 484.78), (-11.805, 484.57)]</t>
+          <t>[(0.0, 485.0), (0.0, 484.82), (0.0, 485.0), (0.0, 484.82), (-5.008, 485.0), (-5.008, 484.78), (-11.805, 485.0), (-11.805, 484.78), (0.0, 484.82), (0.0, 484.67), (0.0, 484.82), (0.0, 484.65), (-5.008, 484.78), (-5.008, 484.65), (-11.805, 484.78), (-11.805, 484.57)]</t>
         </is>
       </c>
     </row>
@@ -5287,7 +5287,7 @@
       </c>
       <c r="B487" t="inlineStr">
         <is>
-          <t>[(-0.3, 486.0), (-0.3, 485.85), (-5.129, 486.0), (-5.129, 485.85), (-5.129, 486.0), (-5.129, 485.73), (-12.005, 486.0), (-12.005, 485.73), (-0.3, 485.85), (-0.3, 485.7), (-5.129, 485.85), (-5.129, 485.7), (-5.129, 485.73), (-5.129, 485.58), (-12.005, 485.73), (-12.005, 485.46), (-0.3, 485.7), (-0.3, 485.58), (-5.129, 485.7), (-5.129, 485.58), (-5.129, 485.58), (-5.129, 485.58), (-12.005, 485.46), (-12.005, 485.46)]</t>
+          <t>[(0.0, 486.0), (0.0, 485.85), (0.0, 486.0), (0.0, 485.85), (-5.129, 486.0), (-5.129, 485.73), (-12.005, 486.0), (-12.005, 485.73), (0.0, 485.85), (0.0, 485.7), (0.0, 485.85), (0.0, 485.7), (-5.129, 485.73), (-5.129, 485.58), (-12.005, 485.73), (-12.005, 485.46), (0.0, 485.7), (0.0, 485.58), (0.0, 485.7), (0.0, 485.58), (-5.129, 485.58), (-5.129, 485.58), (-12.005, 485.46), (-12.005, 485.46)]</t>
         </is>
       </c>
     </row>
@@ -5297,7 +5297,7 @@
       </c>
       <c r="B488" t="inlineStr">
         <is>
-          <t>[(-0.3, 487.0), (-0.3, 486.82), (-5.221, 487.0), (-5.221, 486.82), (-5.221, 487.0), (-5.221, 486.81), (-11.995, 487.0), (-11.995, 486.81), (-0.3, 486.82), (-0.3, 486.64), (-5.221, 486.82), (-5.221, 486.64), (-5.221, 486.81), (-5.221, 486.62), (-11.995, 486.81), (-11.995, 486.62), (-0.3, 486.64), (-0.3, 486.48), (-5.221, 486.64), (-5.221, 486.5), (-5.221, 486.62), (-5.221, 486.5), (-11.995, 486.62), (-11.995, 486.45)]</t>
+          <t>[(0.0, 487.0), (0.0, 486.82), (0.0, 487.0), (0.0, 486.82), (-5.221, 487.0), (-5.221, 486.81), (-11.995, 487.0), (-11.995, 486.81), (0.0, 486.82), (0.0, 486.64), (0.0, 486.82), (0.0, 486.64), (-5.221, 486.81), (-5.221, 486.62), (-11.995, 486.81), (-11.995, 486.62), (0.0, 486.64), (0.0, 486.48), (0.0, 486.64), (0.0, 486.5), (-5.221, 486.62), (-5.221, 486.5), (-11.995, 486.62), (-11.995, 486.45)]</t>
         </is>
       </c>
     </row>
@@ -5307,7 +5307,7 @@
       </c>
       <c r="B489" t="inlineStr">
         <is>
-          <t>[(-0.3, 488.0), (-0.3, 487.7), (-5.246, 488.0), (-5.246, 487.7), (-5.246, 488.0), (-5.246, 487.83), (-12.042, 488.0), (-12.042, 487.83), (-0.3, 487.7), (-0.3, 487.41), (-5.246, 487.7), (-5.246, 487.52), (-5.246, 487.83), (-5.246, 487.66), (-12.042, 487.83), (-12.042, 487.66)]</t>
+          <t>[(0.0, 488.0), (0.0, 487.7), (0.0, 488.0), (0.0, 487.7), (-5.246, 488.0), (-5.246, 487.83), (-12.042, 488.0), (-12.042, 487.83), (0.0, 487.7), (0.0, 487.41), (0.0, 487.7), (0.0, 487.52), (-5.246, 487.83), (-5.246, 487.66), (-12.042, 487.83), (-12.042, 487.66)]</t>
         </is>
       </c>
     </row>
@@ -5317,7 +5317,7 @@
       </c>
       <c r="B490" t="inlineStr">
         <is>
-          <t>[(-0.3, 489.0), (-0.3, 488.73), (-5.258, 489.0), (-5.258, 488.73), (-5.258, 489.0), (-5.258, 488.89), (-12.017, 489.0), (-12.017, 488.89), (-0.3, 488.73), (-0.3, 488.43), (-5.258, 488.73), (-5.258, 488.61), (-5.258, 488.89), (-5.258, 488.61), (-12.017, 488.89), (-12.017, 488.74)]</t>
+          <t>[(0.0, 489.0), (0.0, 488.73), (0.0, 489.0), (0.0, 488.73), (-5.258, 489.0), (-5.258, 488.89), (-12.017, 489.0), (-12.017, 488.89), (0.0, 488.73), (0.0, 488.43), (0.0, 488.73), (0.0, 488.61), (-5.258, 488.89), (-5.258, 488.61), (-12.017, 488.89), (-12.017, 488.74)]</t>
         </is>
       </c>
     </row>
@@ -5337,7 +5337,7 @@
       </c>
       <c r="B492" t="inlineStr">
         <is>
-          <t>[(-0.3, 491.0), (-0.3, 490.66), (-5.197, 491.0), (-5.197, 490.78), (-5.197, 491.0), (-5.197, 490.85), (-12.024, 491.0), (-12.024, 490.85), (-0.3, 490.66), (-0.3, 490.32), (-5.197, 490.78), (-5.197, 490.56), (-5.197, 490.85), (-5.197, 490.55), (-12.024, 490.85), (-12.024, 490.68)]</t>
+          <t>[(0.0, 491.0), (0.0, 490.66), (0.0, 491.0), (0.0, 490.78), (-5.197, 491.0), (-5.197, 490.85), (-12.024, 491.0), (-12.024, 490.85), (0.0, 490.66), (0.0, 490.32), (0.0, 490.78), (0.0, 490.56), (-5.197, 490.85), (-5.197, 490.55), (-12.024, 490.85), (-12.024, 490.68)]</t>
         </is>
       </c>
     </row>
@@ -5347,7 +5347,7 @@
       </c>
       <c r="B493" t="inlineStr">
         <is>
-          <t>[(-0.3, 492.0), (-0.3, 491.61), (-5.221, 492.0), (-5.221, 491.72), (-5.221, 492.0), (-5.221, 491.72), (-12.004, 492.0), (-12.004, 491.72), (-0.3, 491.61), (-0.3, 491.22), (-5.221, 491.72), (-5.221, 491.44), (-5.221, 491.72), (-5.221, 491.45), (-12.004, 491.72), (-12.004, 491.56)]</t>
+          <t>[(0.0, 492.0), (0.0, 491.61), (0.0, 492.0), (0.0, 491.72), (-5.221, 492.0), (-5.221, 491.72), (-12.004, 492.0), (-12.004, 491.72), (0.0, 491.61), (0.0, 491.22), (0.0, 491.72), (0.0, 491.44), (-5.221, 491.72), (-5.221, 491.45), (-12.004, 491.72), (-12.004, 491.56)]</t>
         </is>
       </c>
     </row>
@@ -5357,7 +5357,7 @@
       </c>
       <c r="B494" t="inlineStr">
         <is>
-          <t>[(-0.3, 493.0), (-0.3, 492.55), (-5.159, 493.0), (-5.159, 492.68), (-5.159, 493.0), (-5.159, 492.79), (-11.984, 493.0), (-11.984, 492.79), (-0.3, 492.55), (-0.3, 492.1), (-5.159, 492.68), (-5.159, 492.36), (-5.159, 492.79), (-5.159, 492.58), (-11.984, 492.79), (-11.984, 492.58)]</t>
+          <t>[(0.0, 493.0), (0.0, 492.55), (0.0, 493.0), (0.0, 492.68), (-5.159, 493.0), (-5.159, 492.79), (-11.984, 493.0), (-11.984, 492.79), (0.0, 492.55), (0.0, 492.1), (0.0, 492.68), (0.0, 492.36), (-5.159, 492.79), (-5.159, 492.58), (-11.984, 492.79), (-11.984, 492.58)]</t>
         </is>
       </c>
     </row>
@@ -5367,7 +5367,7 @@
       </c>
       <c r="B495" t="inlineStr">
         <is>
-          <t>[(-0.3, 494.0), (-0.3, 493.5), (-5.114, 494.0), (-5.114, 493.6), (-5.114, 494.0), (-5.114, 493.73), (-11.935, 494.0), (-11.935, 493.73), (-0.3, 493.5), (-0.3, 493.0), (-5.114, 493.6), (-5.114, 493.2), (-5.114, 493.73), (-5.114, 493.46), (-11.935, 493.73), (-11.935, 493.46)]</t>
+          <t>[(0.0, 494.0), (0.0, 493.5), (0.0, 494.0), (0.0, 493.6), (-5.114, 494.0), (-5.114, 493.73), (-11.935, 494.0), (-11.935, 493.73), (0.0, 493.5), (0.0, 493.0), (0.0, 493.6), (0.0, 493.2), (-5.114, 493.73), (-5.114, 493.46), (-11.935, 493.73), (-11.935, 493.46)]</t>
         </is>
       </c>
     </row>
@@ -5377,7 +5377,7 @@
       </c>
       <c r="B496" t="inlineStr">
         <is>
-          <t>[(-0.3, 495.0), (-0.3, 494.5), (-5.078, 495.0), (-5.078, 494.58), (-5.078, 495.0), (-5.078, 494.79), (-11.886, 495.0), (-11.886, 494.79), (-0.3, 494.5), (-0.3, 494.0), (-5.078, 494.58), (-5.078, 494.16), (-5.078, 494.79), (-5.078, 494.58), (-11.886, 494.79), (-11.886, 494.58)]</t>
+          <t>[(0.0, 495.0), (0.0, 494.5), (0.0, 495.0), (0.0, 494.58), (-5.078, 495.0), (-5.078, 494.79), (-11.886, 495.0), (-11.886, 494.79), (0.0, 494.5), (0.0, 494.0), (0.0, 494.58), (0.0, 494.16), (-5.078, 494.79), (-5.078, 494.58), (-11.886, 494.79), (-11.886, 494.58)]</t>
         </is>
       </c>
     </row>
@@ -5417,7 +5417,7 @@
       </c>
       <c r="B500" t="inlineStr">
         <is>
-          <t>[(-0.3, 499.0), (-0.3, 498.71), (-5.357, 499.0), (-5.357, 498.71), (-5.357, 499.0), (-5.357, 498.76), (-12.301, 499.0), (-12.301, 498.76), (-0.3, 498.71), (-0.3, 498.42), (-5.357, 498.71), (-5.357, 498.42), (-5.357, 498.76), (-5.357, 498.52), (-12.301, 498.76), (-12.301, 498.52), (-0.3, 498.42), (-0.3, 498.14), (-5.357, 498.42), (-5.357, 498.28), (-5.357, 498.52), (-5.357, 498.28), (-12.301, 498.52), (-12.301, 498.39)]</t>
+          <t>[(0.0, 499.0), (0.0, 498.71), (0.0, 499.0), (0.0, 498.71), (-5.357, 499.0), (-5.357, 498.76), (-12.301, 499.0), (-12.301, 498.76), (0.0, 498.71), (0.0, 498.42), (0.0, 498.71), (0.0, 498.42), (-5.357, 498.76), (-5.357, 498.52), (-12.301, 498.76), (-12.301, 498.52), (0.0, 498.42), (0.0, 498.14), (0.0, 498.42), (0.0, 498.28), (-5.357, 498.52), (-5.357, 498.28), (-12.301, 498.52), (-12.301, 498.39)]</t>
         </is>
       </c>
     </row>
@@ -5427,7 +5427,7 @@
       </c>
       <c r="B501" t="inlineStr">
         <is>
-          <t>[(-0.3, 500.0), (-0.3, 499.72), (-5.533, 500.0), (-5.533, 499.72), (-5.533, 500.0), (-5.533, 499.66), (-12.507, 500.0), (-12.507, 499.76), (-0.3, 499.72), (-0.3, 499.44), (-5.533, 499.72), (-5.533, 499.44), (-5.533, 499.66), (-5.533, 499.32), (-12.507, 499.76), (-12.507, 499.52), (-0.3, 499.44), (-0.3, 499.17), (-5.533, 499.44), (-5.533, 499.33), (-5.533, 499.32), (-5.533, 499.32), (-12.507, 499.52), (-12.507, 499.52)]</t>
+          <t>[(0.0, 500.0), (0.0, 499.72), (0.0, 500.0), (0.0, 499.72), (-5.533, 500.0), (-5.533, 499.66), (-12.507, 500.0), (-12.507, 499.76), (0.0, 499.72), (0.0, 499.44), (0.0, 499.72), (0.0, 499.44), (-5.533, 499.66), (-5.533, 499.32), (-12.507, 499.76), (-12.507, 499.52), (0.0, 499.44), (0.0, 499.17), (0.0, 499.44), (0.0, 499.33), (-5.533, 499.32), (-5.533, 499.32), (-12.507, 499.52), (-12.507, 499.52)]</t>
         </is>
       </c>
     </row>
@@ -5437,7 +5437,7 @@
       </c>
       <c r="B502" t="inlineStr">
         <is>
-          <t>[(-0.3, 501.0), (-0.3, 500.6), (-5.774, 501.0), (-5.774, 500.7), (-5.774, 501.0), (-5.774, 500.7), (-12.784, 501.0), (-12.784, 500.7), (-0.3, 500.6), (-0.3, 500.2), (-5.774, 500.7), (-5.774, 500.4), (-5.774, 500.7), (-5.774, 500.41), (-12.784, 500.7), (-12.784, 500.59)]</t>
+          <t>[(0.0, 501.0), (0.0, 500.6), (0.0, 501.0), (0.0, 500.7), (-5.774, 501.0), (-5.774, 500.7), (-12.784, 501.0), (-12.784, 500.7), (0.0, 500.6), (0.0, 500.2), (0.0, 500.7), (0.0, 500.4), (-5.774, 500.7), (-5.774, 500.41), (-12.784, 500.7), (-12.784, 500.59)]</t>
         </is>
       </c>
     </row>
@@ -5447,7 +5447,7 @@
       </c>
       <c r="B503" t="inlineStr">
         <is>
-          <t>[(-0.3, 502.0), (-0.3, 501.65), (-5.857, 502.0), (-5.857, 501.77), (-5.857, 502.0), (-5.857, 501.77), (-12.779, 502.0), (-12.779, 501.87), (-0.3, 501.65), (-0.3, 501.3), (-5.857, 501.77), (-5.857, 501.54), (-5.857, 501.77), (-5.857, 501.54), (-12.779, 501.87), (-12.779, 501.74)]</t>
+          <t>[(0.0, 502.0), (0.0, 501.65), (0.0, 502.0), (0.0, 501.77), (-5.857, 502.0), (-5.857, 501.77), (-12.779, 502.0), (-12.779, 501.87), (0.0, 501.65), (0.0, 501.3), (0.0, 501.77), (0.0, 501.54), (-5.857, 501.77), (-5.857, 501.54), (-12.779, 501.87), (-12.779, 501.74)]</t>
         </is>
       </c>
     </row>
@@ -5457,7 +5457,7 @@
       </c>
       <c r="B504" t="inlineStr">
         <is>
-          <t>[(-0.3, 503.0), (-0.3, 502.68), (-5.904, 503.0), (-5.904, 502.77), (-5.904, 503.0), (-5.904, 502.77), (-12.805, 503.0), (-12.805, 502.87), (-0.3, 502.68), (-0.3, 502.36), (-5.904, 502.77), (-5.904, 502.54), (-5.904, 502.77), (-5.904, 502.54), (-12.805, 502.87), (-12.805, 502.74)]</t>
+          <t>[(0.0, 503.0), (0.0, 502.68), (0.0, 503.0), (0.0, 502.77), (-5.904, 503.0), (-5.904, 502.77), (-12.805, 503.0), (-12.805, 502.87), (0.0, 502.68), (0.0, 502.36), (0.0, 502.77), (0.0, 502.54), (-5.904, 502.77), (-5.904, 502.54), (-12.805, 502.87), (-12.805, 502.74)]</t>
         </is>
       </c>
     </row>
@@ -5467,7 +5467,7 @@
       </c>
       <c r="B505" t="inlineStr">
         <is>
-          <t>[(-0.3, 504.0), (-0.3, 503.64), (-5.981, 504.0), (-5.981, 503.76), (-5.981, 504.0), (-5.981, 503.81), (-12.864, 504.0), (-12.864, 503.81), (-0.3, 503.64), (-0.3, 503.28), (-5.981, 503.76), (-5.981, 503.52), (-5.981, 503.81), (-5.981, 503.51), (-12.864, 503.81), (-12.864, 503.65)]</t>
+          <t>[(0.0, 504.0), (0.0, 503.64), (0.0, 504.0), (0.0, 503.76), (-5.981, 504.0), (-5.981, 503.81), (-12.864, 504.0), (-12.864, 503.81), (0.0, 503.64), (0.0, 503.28), (0.0, 503.76), (0.0, 503.52), (-5.981, 503.81), (-5.981, 503.51), (-12.864, 503.81), (-12.864, 503.65)]</t>
         </is>
       </c>
     </row>
@@ -5477,7 +5477,7 @@
       </c>
       <c r="B506" t="inlineStr">
         <is>
-          <t>[(-0.3, 505.0), (-0.3, 504.66), (-5.857, 505.0), (-5.857, 504.74), (-5.857, 505.0), (-5.857, 504.74), (-12.727, 505.0), (-12.727, 504.84), (-0.3, 504.66), (-0.3, 504.32), (-5.857, 504.74), (-5.857, 504.48), (-5.857, 504.74), (-5.857, 504.48), (-12.727, 504.84), (-12.727, 504.68)]</t>
+          <t>[(0.0, 505.0), (0.0, 504.66), (0.0, 505.0), (0.0, 504.74), (-5.857, 505.0), (-5.857, 504.74), (-12.727, 505.0), (-12.727, 504.84), (0.0, 504.66), (0.0, 504.32), (0.0, 504.74), (0.0, 504.48), (-5.857, 504.74), (-5.857, 504.48), (-12.727, 504.84), (-12.727, 504.68)]</t>
         </is>
       </c>
     </row>
@@ -5547,7 +5547,7 @@
       </c>
       <c r="B513" t="inlineStr">
         <is>
-          <t>[(-0.3, 512.0), (-0.3, 511.89), (-4.393, 512.0), (-4.393, 511.89), (-4.393, 512.0), (-4.393, 511.85), (-11.313, 512.0), (-11.313, 511.85), (-0.3, 511.89), (-0.3, 511.63), (-4.393, 511.89), (-4.393, 511.72), (-4.393, 511.85), (-4.393, 511.72), (-11.313, 511.85), (-11.313, 511.55)]</t>
+          <t>[(0.0, 512.0), (0.0, 511.89), (0.0, 512.0), (0.0, 511.89), (-4.393, 512.0), (-4.393, 511.85), (-11.313, 512.0), (-11.313, 511.85), (0.0, 511.89), (0.0, 511.63), (0.0, 511.89), (0.0, 511.72), (-4.393, 511.85), (-4.393, 511.72), (-11.313, 511.85), (-11.313, 511.55)]</t>
         </is>
       </c>
     </row>
@@ -5557,7 +5557,7 @@
       </c>
       <c r="B514" t="inlineStr">
         <is>
-          <t>[(-0.3, 513.0), (-0.3, 512.76), (-4.237, 513.0), (-4.237, 512.76), (-4.237, 513.0), (-4.237, 512.79), (-11.169, 513.0), (-11.169, 512.69), (-0.3, 512.76), (-0.3, 512.52), (-4.237, 512.76), (-4.237, 512.58), (-4.237, 512.79), (-4.237, 512.58), (-11.169, 512.69), (-11.169, 512.38)]</t>
+          <t>[(0.0, 513.0), (0.0, 512.76), (0.0, 513.0), (0.0, 512.76), (-4.237, 513.0), (-4.237, 512.79), (-11.169, 513.0), (-11.169, 512.69), (0.0, 512.76), (0.0, 512.52), (0.0, 512.76), (0.0, 512.58), (-4.237, 512.79), (-4.237, 512.58), (-11.169, 512.69), (-11.169, 512.38)]</t>
         </is>
       </c>
     </row>
@@ -5567,7 +5567,7 @@
       </c>
       <c r="B515" t="inlineStr">
         <is>
-          <t>[(-0.3, 514.0), (-0.3, 513.73), (-4.16, 514.0), (-4.16, 513.73), (-4.16, 514.0), (-4.16, 513.77), (-11.078, 514.0), (-11.078, 513.68), (-0.3, 513.73), (-0.3, 513.47), (-4.16, 513.73), (-4.16, 513.54), (-4.16, 513.77), (-4.16, 513.54), (-11.078, 513.68), (-11.078, 513.36)]</t>
+          <t>[(0.0, 514.0), (0.0, 513.73), (0.0, 514.0), (0.0, 513.73), (-4.16, 514.0), (-4.16, 513.77), (-11.078, 514.0), (-11.078, 513.68), (0.0, 513.73), (0.0, 513.47), (0.0, 513.73), (0.0, 513.54), (-4.16, 513.77), (-4.16, 513.54), (-11.078, 513.68), (-11.078, 513.36)]</t>
         </is>
       </c>
     </row>
@@ -5577,7 +5577,7 @@
       </c>
       <c r="B516" t="inlineStr">
         <is>
-          <t>[(-0.3, 515.0), (-0.3, 514.85), (-4.027, 515.0), (-4.027, 514.85), (-4.027, 515.0), (-4.027, 514.72), (-10.92, 515.0), (-10.92, 514.72), (-0.3, 514.85), (-0.3, 514.7), (-4.027, 514.85), (-4.027, 514.7), (-4.027, 514.72), (-4.027, 514.57), (-10.92, 514.72), (-10.92, 514.45), (-0.3, 514.7), (-0.3, 514.58), (-4.027, 514.7), (-4.027, 514.57), (-4.027, 514.57), (-4.027, 514.57), (-10.92, 514.45), (-10.92, 514.45)]</t>
+          <t>[(0.0, 515.0), (0.0, 514.85), (0.0, 515.0), (0.0, 514.85), (-4.027, 515.0), (-4.027, 514.72), (-10.92, 515.0), (-10.92, 514.72), (0.0, 514.85), (0.0, 514.7), (0.0, 514.85), (0.0, 514.7), (-4.027, 514.72), (-4.027, 514.57), (-10.92, 514.72), (-10.92, 514.45), (0.0, 514.7), (0.0, 514.58), (0.0, 514.7), (0.0, 514.57), (-4.027, 514.57), (-4.027, 514.57), (-10.92, 514.45), (-10.92, 514.45)]</t>
         </is>
       </c>
     </row>
@@ -5587,7 +5587,7 @@
       </c>
       <c r="B517" t="inlineStr">
         <is>
-          <t>[(-0.3, 516.0), (-0.3, 515.86), (-3.916, 516.0), (-3.916, 515.86), (-3.916, 516.0), (-3.916, 515.74), (-10.782, 516.0), (-10.782, 515.74), (-0.3, 515.86), (-0.3, 515.72), (-3.916, 515.86), (-3.916, 515.72), (-3.916, 515.74), (-3.916, 515.6), (-10.782, 515.74), (-10.782, 515.48), (-0.3, 515.72), (-0.3, 515.6), (-3.916, 515.72), (-3.916, 515.6), (-3.916, 515.6), (-3.916, 515.6), (-10.782, 515.48), (-10.782, 515.48)]</t>
+          <t>[(0.0, 516.0), (0.0, 515.86), (0.0, 516.0), (0.0, 515.86), (-3.916, 516.0), (-3.916, 515.74), (-10.782, 516.0), (-10.782, 515.74), (0.0, 515.86), (0.0, 515.72), (0.0, 515.86), (0.0, 515.72), (-3.916, 515.74), (-3.916, 515.6), (-10.782, 515.74), (-10.782, 515.48), (0.0, 515.72), (0.0, 515.6), (0.0, 515.72), (0.0, 515.6), (-3.916, 515.6), (-3.916, 515.6), (-10.782, 515.48), (-10.782, 515.48)]</t>
         </is>
       </c>
     </row>
@@ -5597,7 +5597,7 @@
       </c>
       <c r="B518" t="inlineStr">
         <is>
-          <t>[(-0.3, 517.0), (-0.3, 516.79), (-4.131, 517.0), (-4.131, 516.79), (-4.131, 517.0), (-4.131, 516.75), (-10.953, 517.0), (-10.953, 516.75), (-0.3, 516.79), (-0.3, 516.59), (-4.131, 516.79), (-4.131, 516.63), (-4.131, 516.75), (-4.131, 516.63), (-10.953, 516.75), (-10.953, 516.5)]</t>
+          <t>[(0.0, 517.0), (0.0, 516.79), (0.0, 517.0), (0.0, 516.79), (-4.131, 517.0), (-4.131, 516.75), (-10.953, 517.0), (-10.953, 516.75), (0.0, 516.79), (0.0, 516.59), (0.0, 516.79), (0.0, 516.63), (-4.131, 516.75), (-4.131, 516.63), (-10.953, 516.75), (-10.953, 516.5)]</t>
         </is>
       </c>
     </row>
@@ -5607,7 +5607,7 @@
       </c>
       <c r="B519" t="inlineStr">
         <is>
-          <t>[(-0.3, 518.0), (-0.3, 517.77), (-4.733, 518.0), (-4.733, 517.77), (-4.733, 518.0), (-4.733, 517.77), (-11.574, 518.0), (-11.574, 517.68), (-0.3, 517.77), (-0.3, 517.59), (-4.733, 517.77), (-4.733, 517.54), (-4.733, 517.77), (-4.733, 517.54), (-11.574, 517.68), (-11.574, 517.36)]</t>
+          <t>[(0.0, 518.0), (0.0, 517.77), (0.0, 518.0), (0.0, 517.77), (-4.733, 518.0), (-4.733, 517.77), (-11.574, 518.0), (-11.574, 517.68), (0.0, 517.77), (0.0, 517.59), (0.0, 517.77), (0.0, 517.54), (-4.733, 517.77), (-4.733, 517.54), (-11.574, 517.68), (-11.574, 517.36)]</t>
         </is>
       </c>
     </row>
@@ -5617,7 +5617,7 @@
       </c>
       <c r="B520" t="inlineStr">
         <is>
-          <t>[(-0.3, 519.0), (-0.3, 518.75), (-5.234, 519.0), (-5.234, 518.75), (-5.234, 519.0), (-5.234, 518.75), (-12.18, 519.0), (-12.18, 518.66), (-0.3, 518.75), (-0.3, 518.6), (-5.234, 518.75), (-5.234, 518.5), (-5.234, 518.75), (-5.234, 518.5), (-12.18, 518.66), (-12.18, 518.32)]</t>
+          <t>[(0.0, 519.0), (0.0, 518.75), (0.0, 519.0), (0.0, 518.75), (-5.234, 519.0), (-5.234, 518.75), (-12.18, 519.0), (-12.18, 518.66), (0.0, 518.75), (0.0, 518.6), (0.0, 518.75), (0.0, 518.5), (-5.234, 518.75), (-5.234, 518.5), (-12.18, 518.66), (-12.18, 518.32)]</t>
         </is>
       </c>
     </row>
@@ -5627,7 +5627,7 @@
       </c>
       <c r="B521" t="inlineStr">
         <is>
-          <t>[(-0.3, 520.0), (-0.3, 519.73), (-5.555, 520.0), (-5.555, 519.73), (-5.555, 520.0), (-5.555, 519.74), (-12.458, 520.0), (-12.458, 519.66), (-0.3, 519.73), (-0.3, 519.55), (-5.555, 519.73), (-5.555, 519.47), (-5.555, 519.74), (-5.555, 519.48), (-12.458, 519.66), (-12.458, 519.32)]</t>
+          <t>[(0.0, 520.0), (0.0, 519.73), (0.0, 520.0), (0.0, 519.73), (-5.555, 520.0), (-5.555, 519.74), (-12.458, 520.0), (-12.458, 519.66), (0.0, 519.73), (0.0, 519.55), (0.0, 519.73), (0.0, 519.47), (-5.555, 519.74), (-5.555, 519.48), (-12.458, 519.66), (-12.458, 519.32)]</t>
         </is>
       </c>
     </row>
@@ -5637,7 +5637,7 @@
       </c>
       <c r="B522" t="inlineStr">
         <is>
-          <t>[(-0.3, 521.0), (-0.3, 520.75), (-5.537, 521.0), (-5.537, 520.75), (-5.537, 521.0), (-5.537, 520.75), (-12.466, 521.0), (-12.466, 520.67), (-0.3, 520.75), (-0.3, 520.6), (-5.537, 520.75), (-5.537, 520.5), (-5.537, 520.75), (-5.537, 520.5), (-12.466, 520.67), (-12.466, 520.34)]</t>
+          <t>[(0.0, 521.0), (0.0, 520.75), (0.0, 521.0), (0.0, 520.75), (-5.537, 521.0), (-5.537, 520.75), (-12.466, 521.0), (-12.466, 520.67), (0.0, 520.75), (0.0, 520.6), (0.0, 520.75), (0.0, 520.5), (-5.537, 520.75), (-5.537, 520.5), (-12.466, 520.67), (-12.466, 520.34)]</t>
         </is>
       </c>
     </row>
@@ -5647,7 +5647,7 @@
       </c>
       <c r="B523" t="inlineStr">
         <is>
-          <t>[(-0.3, 522.0), (-0.3, 521.77), (-5.217, 522.0), (-5.217, 521.77), (-5.217, 522.0), (-5.217, 521.77), (-12.168, 522.0), (-12.168, 521.67), (-0.3, 521.77), (-0.3, 521.61), (-5.217, 521.77), (-5.217, 521.54), (-5.217, 521.77), (-5.217, 521.54), (-12.168, 521.67), (-12.168, 521.34)]</t>
+          <t>[(0.0, 522.0), (0.0, 521.77), (0.0, 522.0), (0.0, 521.77), (-5.217, 522.0), (-5.217, 521.77), (-12.168, 522.0), (-12.168, 521.67), (0.0, 521.77), (0.0, 521.61), (0.0, 521.77), (0.0, 521.54), (-5.217, 521.77), (-5.217, 521.54), (-12.168, 521.67), (-12.168, 521.34)]</t>
         </is>
       </c>
     </row>
@@ -5657,7 +5657,7 @@
       </c>
       <c r="B524" t="inlineStr">
         <is>
-          <t>[(-0.3, 523.0), (-0.3, 522.81), (-4.758, 523.0), (-4.758, 522.81), (-4.758, 523.0), (-4.758, 522.81), (-11.678, 523.0), (-11.678, 522.71), (-0.3, 522.81), (-0.3, 522.66), (-4.758, 522.81), (-4.758, 522.62), (-4.758, 522.81), (-4.758, 522.62), (-11.678, 522.71), (-11.678, 522.42)]</t>
+          <t>[(0.0, 523.0), (0.0, 522.81), (0.0, 523.0), (0.0, 522.81), (-4.758, 523.0), (-4.758, 522.81), (-11.678, 523.0), (-11.678, 522.71), (0.0, 522.81), (0.0, 522.66), (0.0, 522.81), (0.0, 522.62), (-4.758, 522.81), (-4.758, 522.62), (-11.678, 522.71), (-11.678, 522.42)]</t>
         </is>
       </c>
     </row>
@@ -5667,7 +5667,7 @@
       </c>
       <c r="B525" t="inlineStr">
         <is>
-          <t>[(-0.3, 524.0), (-0.3, 523.83), (-3.886, 524.0), (-3.886, 523.83), (-3.886, 524.0), (-3.886, 523.84), (-10.769, 524.0), (-10.769, 523.56), (-0.3, 523.83), (-0.3, 523.7), (-3.886, 523.83), (-3.886, 523.67), (-3.886, 523.84), (-3.886, 523.68), (-10.769, 523.56), (-10.769, 523.12)]</t>
+          <t>[(0.0, 524.0), (0.0, 523.83), (0.0, 524.0), (0.0, 523.83), (-3.886, 524.0), (-3.886, 523.84), (-10.769, 524.0), (-10.769, 523.56), (0.0, 523.83), (0.0, 523.7), (0.0, 523.83), (0.0, 523.67), (-3.886, 523.84), (-3.886, 523.68), (-10.769, 523.56), (-10.769, 523.12)]</t>
         </is>
       </c>
     </row>
@@ -5677,7 +5677,7 @@
       </c>
       <c r="B526" t="inlineStr">
         <is>
-          <t>[(-0.3, 525.0), (-0.3, 524.82), (-2.604, 525.0), (-2.604, 524.82), (-2.604, 525.0), (-2.604, 524.84), (-9.407, 525.0), (-9.407, 524.55), (-0.3, 524.82), (-0.3, 524.64), (-2.604, 524.82), (-2.604, 524.67), (-2.604, 524.84), (-2.604, 524.68), (-9.407, 524.55), (-9.407, 524.1)]</t>
+          <t>[(0.0, 525.0), (0.0, 524.82), (0.0, 525.0), (0.0, 524.82), (-2.604, 525.0), (-2.604, 524.84), (-9.407, 525.0), (-9.407, 524.55), (0.0, 524.82), (0.0, 524.64), (0.0, 524.82), (0.0, 524.67), (-2.604, 524.84), (-2.604, 524.68), (-9.407, 524.55), (-9.407, 524.1)]</t>
         </is>
       </c>
     </row>
@@ -5687,7 +5687,7 @@
       </c>
       <c r="B527" t="inlineStr">
         <is>
-          <t>[(-0.3, 526.0), (-0.3, 525.82), (-8.305, 526.0), (-8.305, 525.56), (-0.3, 525.82), (-0.3, 525.64), (-8.305, 525.56), (-8.305, 525.12)]</t>
+          <t>[(0.0, 526.0), (0.0, 525.82), (-8.305, 526.0), (-8.305, 525.56), (0.0, 525.82), (0.0, 525.64), (-8.305, 525.56), (-8.305, 525.12)]</t>
         </is>
       </c>
     </row>
@@ -5697,7 +5697,7 @@
       </c>
       <c r="B528" t="inlineStr">
         <is>
-          <t>[(-0.3, 527.0), (-0.3, 526.82), (-7.338, 527.0), (-7.338, 526.71), (-0.3, 526.82), (-0.3, 526.64), (-7.338, 526.71), (-7.338, 526.42)]</t>
+          <t>[(0.0, 527.0), (0.0, 526.82), (-7.338, 527.0), (-7.338, 526.71), (0.0, 526.82), (0.0, 526.64), (-7.338, 526.71), (-7.338, 526.42)]</t>
         </is>
       </c>
     </row>
@@ -5707,7 +5707,7 @@
       </c>
       <c r="B529" t="inlineStr">
         <is>
-          <t>[(-0.3, 528.0), (-0.3, 527.81), (-6.61, 528.0), (-6.61, 527.81), (-0.3, 527.81), (-0.3, 527.67), (-6.61, 527.81), (-6.61, 527.51)]</t>
+          <t>[(0.0, 528.0), (0.0, 527.81), (-6.61, 528.0), (-6.61, 527.81), (0.0, 527.81), (0.0, 527.67), (-6.61, 527.81), (-6.61, 527.51)]</t>
         </is>
       </c>
     </row>
@@ -5717,7 +5717,7 @@
       </c>
       <c r="B530" t="inlineStr">
         <is>
-          <t>[(-0.3, 529.0), (-0.3, 528.89), (-6.439, 529.0), (-6.439, 528.89), (-0.3, 528.89), (-0.3, 528.69), (-6.439, 528.89), (-6.439, 528.59)]</t>
+          <t>[(0.0, 529.0), (0.0, 528.89), (-6.439, 529.0), (-6.439, 528.89), (0.0, 528.89), (0.0, 528.69), (-6.439, 528.89), (-6.439, 528.59)]</t>
         </is>
       </c>
     </row>
@@ -5727,7 +5727,7 @@
       </c>
       <c r="B531" t="inlineStr">
         <is>
-          <t>[(-0.3, 530.0), (-0.3, 529.78), (-6.65, 530.0), (-6.65, 529.78), (-0.3, 529.78), (-0.3, 529.61), (-6.65, 529.78), (-6.65, 529.57)]</t>
+          <t>[(0.0, 530.0), (0.0, 529.78), (-6.65, 530.0), (-6.65, 529.78), (0.0, 529.78), (0.0, 529.61), (-6.65, 529.78), (-6.65, 529.57)]</t>
         </is>
       </c>
     </row>
@@ -5737,7 +5737,7 @@
       </c>
       <c r="B532" t="inlineStr">
         <is>
-          <t>[(-0.3, 531.0), (-0.3, 530.8), (-6.883, 531.0), (-6.883, 530.8), (-0.3, 530.8), (-0.3, 530.6), (-6.883, 530.8), (-6.883, 530.68)]</t>
+          <t>[(0.0, 531.0), (0.0, 530.8), (-6.883, 531.0), (-6.883, 530.8), (0.0, 530.8), (0.0, 530.6), (-6.883, 530.8), (-6.883, 530.68)]</t>
         </is>
       </c>
     </row>
@@ -5757,7 +5757,7 @@
       </c>
       <c r="B534" t="inlineStr">
         <is>
-          <t>[(-0.3, 533.0), (-0.3, 532.84), (-8.053, 533.0), (-8.053, 532.84), (-0.3, 532.84), (-0.3, 532.68), (-8.053, 532.84), (-8.053, 532.72)]</t>
+          <t>[(0.0, 533.0), (0.0, 532.84), (-8.053, 533.0), (-8.053, 532.84), (0.0, 532.84), (0.0, 532.68), (-8.053, 532.84), (-8.053, 532.72)]</t>
         </is>
       </c>
     </row>
@@ -5767,7 +5767,7 @@
       </c>
       <c r="B535" t="inlineStr">
         <is>
-          <t>[(-0.3, 534.0), (-0.3, 533.85), (-8.848, 534.0), (-8.848, 533.85), (-0.3, 533.85), (-0.3, 533.73), (-8.848, 533.85), (-8.848, 533.72)]</t>
+          <t>[(0.0, 534.0), (0.0, 533.85), (-8.848, 534.0), (-8.848, 533.85), (0.0, 533.85), (0.0, 533.73), (-8.848, 533.85), (-8.848, 533.72)]</t>
         </is>
       </c>
     </row>
@@ -5777,7 +5777,7 @@
       </c>
       <c r="B536" t="inlineStr">
         <is>
-          <t>[(-0.3, 535.0), (-0.3, 534.85), (-9.776, 535.0), (-9.776, 534.85), (-0.3, 534.85), (-0.3, 534.74), (-9.776, 534.85), (-9.776, 534.7)]</t>
+          <t>[(0.0, 535.0), (0.0, 534.85), (-9.776, 535.0), (-9.776, 534.85), (0.0, 534.85), (0.0, 534.74), (-9.776, 534.85), (-9.776, 534.7)]</t>
         </is>
       </c>
     </row>
@@ -5797,7 +5797,7 @@
       </c>
       <c r="B538" t="inlineStr">
         <is>
-          <t>[(-0.3, 537.0), (-0.3, 536.86), (-7.109, 537.0), (-7.109, 536.86), (-0.3, 536.86), (-0.3, 536.74), (-7.109, 536.86), (-7.109, 536.73)]</t>
+          <t>[(0.0, 537.0), (0.0, 536.86), (-7.109, 537.0), (-7.109, 536.86), (0.0, 536.86), (0.0, 536.74), (-7.109, 536.86), (-7.109, 536.73)]</t>
         </is>
       </c>
     </row>
@@ -5817,7 +5817,7 @@
       </c>
       <c r="B540" t="inlineStr">
         <is>
-          <t>[(-0.3, 539.0), (-0.3, 538.85), (-6.982, 539.0), (-6.982, 538.85), (-0.3, 538.85), (-0.3, 538.71), (-6.982, 538.85), (-6.982, 538.7)]</t>
+          <t>[(0.0, 539.0), (0.0, 538.85), (-6.982, 539.0), (-6.982, 538.85), (0.0, 538.85), (0.0, 538.71), (-6.982, 538.85), (-6.982, 538.7)]</t>
         </is>
       </c>
     </row>
@@ -5827,7 +5827,7 @@
       </c>
       <c r="B541" t="inlineStr">
         <is>
-          <t>[(-0.3, 540.0), (-0.3, 539.85), (-6.919, 540.0), (-6.919, 539.85), (-0.3, 539.85), (-0.3, 539.74), (-6.919, 539.85), (-6.919, 539.7)]</t>
+          <t>[(0.0, 540.0), (0.0, 539.85), (-6.919, 540.0), (-6.919, 539.85), (0.0, 539.85), (0.0, 539.74), (-6.919, 539.85), (-6.919, 539.7)]</t>
         </is>
       </c>
     </row>
@@ -6017,7 +6017,7 @@
       </c>
       <c r="B560" t="inlineStr">
         <is>
-          <t>[(-0.3, 559.0), (-0.3, 558.86), (-7.618, 559.0), (-7.618, 558.86), (-0.3, 558.86), (-0.3, 558.73), (-7.618, 558.86), (-7.618, 558.75)]</t>
+          <t>[(0.0, 559.0), (0.0, 558.86), (-7.618, 559.0), (-7.618, 558.86), (0.0, 558.86), (0.0, 558.73), (-7.618, 558.86), (-7.618, 558.75)]</t>
         </is>
       </c>
     </row>
@@ -6027,7 +6027,7 @@
       </c>
       <c r="B561" t="inlineStr">
         <is>
-          <t>[(-0.3, 560.0), (-0.3, 559.82), (-7.298, 560.0), (-7.298, 559.82), (-0.3, 559.82), (-0.3, 559.64), (-7.298, 559.82), (-7.298, 559.69)]</t>
+          <t>[(0.0, 560.0), (0.0, 559.82), (-7.298, 560.0), (-7.298, 559.82), (0.0, 559.82), (0.0, 559.64), (-7.298, 559.82), (-7.298, 559.69)]</t>
         </is>
       </c>
     </row>
@@ -6037,7 +6037,7 @@
       </c>
       <c r="B562" t="inlineStr">
         <is>
-          <t>[(-0.3, 561.0), (-0.3, 560.82), (-7.039, 561.0), (-7.039, 560.82), (-0.3, 560.82), (-0.3, 560.65), (-7.039, 560.82), (-7.039, 560.69)]</t>
+          <t>[(0.0, 561.0), (0.0, 560.82), (-7.039, 561.0), (-7.039, 560.82), (0.0, 560.82), (0.0, 560.65), (-7.039, 560.82), (-7.039, 560.69)]</t>
         </is>
       </c>
     </row>
@@ -6047,7 +6047,7 @@
       </c>
       <c r="B563" t="inlineStr">
         <is>
-          <t>[(-0.3, 562.0), (-0.3, 561.89), (-6.683, 562.0), (-6.683, 561.89), (-0.3, 561.89), (-0.3, 561.61), (-6.683, 561.89), (-6.683, 561.72)]</t>
+          <t>[(0.0, 562.0), (0.0, 561.89), (-6.683, 562.0), (-6.683, 561.89), (0.0, 561.89), (0.0, 561.61), (-6.683, 561.89), (-6.683, 561.72)]</t>
         </is>
       </c>
     </row>
@@ -6067,7 +6067,7 @@
       </c>
       <c r="B565" t="inlineStr">
         <is>
-          <t>[(-0.3, 564.0), (-0.3, 563.84), (-6.054, 564.0), (-6.054, 563.84), (-0.3, 563.84), (-0.3, 563.68), (-6.054, 563.84), (-6.054, 563.73)]</t>
+          <t>[(0.0, 564.0), (0.0, 563.84), (-6.054, 564.0), (-6.054, 563.84), (0.0, 563.84), (0.0, 563.68), (-6.054, 563.84), (-6.054, 563.73)]</t>
         </is>
       </c>
     </row>
@@ -6077,7 +6077,7 @@
       </c>
       <c r="B566" t="inlineStr">
         <is>
-          <t>[(-0.3, 565.0), (-0.3, 564.83), (-5.826, 565.0), (-5.826, 564.83), (-0.3, 564.83), (-0.3, 564.67), (-5.826, 564.83), (-5.826, 564.68)]</t>
+          <t>[(0.0, 565.0), (0.0, 564.83), (-5.826, 565.0), (-5.826, 564.83), (0.0, 564.83), (0.0, 564.67), (-5.826, 564.83), (-5.826, 564.68)]</t>
         </is>
       </c>
     </row>
@@ -6087,7 +6087,7 @@
       </c>
       <c r="B567" t="inlineStr">
         <is>
-          <t>[(-0.3, 566.0), (-0.3, 565.84), (-5.72, 566.0), (-5.72, 565.84), (-0.3, 565.84), (-0.3, 565.73), (-5.72, 565.84), (-5.72, 565.69)]</t>
+          <t>[(0.0, 566.0), (0.0, 565.84), (-5.72, 566.0), (-5.72, 565.84), (0.0, 565.84), (0.0, 565.73), (-5.72, 565.84), (-5.72, 565.69)]</t>
         </is>
       </c>
     </row>
@@ -6097,7 +6097,7 @@
       </c>
       <c r="B568" t="inlineStr">
         <is>
-          <t>[(-0.3, 567.0), (-0.3, 566.89), (-5.575, 567.0), (-5.575, 566.89), (-0.3, 566.89), (-0.3, 566.72), (-5.575, 566.89), (-5.575, 566.65)]</t>
+          <t>[(0.0, 567.0), (0.0, 566.89), (-5.575, 567.0), (-5.575, 566.89), (0.0, 566.89), (0.0, 566.72), (-5.575, 566.89), (-5.575, 566.65)]</t>
         </is>
       </c>
     </row>
@@ -6107,7 +6107,7 @@
       </c>
       <c r="B569" t="inlineStr">
         <is>
-          <t>[(-0.3, 568.0), (-0.3, 567.89), (-5.352, 568.0), (-5.352, 567.89), (-0.3, 567.89), (-0.3, 567.72), (-5.352, 567.89), (-5.352, 567.65)]</t>
+          <t>[(0.0, 568.0), (0.0, 567.89), (-5.352, 568.0), (-5.352, 567.89), (0.0, 567.89), (0.0, 567.72), (-5.352, 567.89), (-5.352, 567.65)]</t>
         </is>
       </c>
     </row>
@@ -6117,7 +6117,7 @@
       </c>
       <c r="B570" t="inlineStr">
         <is>
-          <t>[(-0.3, 569.0), (-0.3, 568.89), (-5.076, 569.0), (-5.076, 568.89), (-0.3, 568.89), (-0.3, 568.75), (-5.076, 568.89), (-5.076, 568.62)]</t>
+          <t>[(0.0, 569.0), (0.0, 568.89), (-5.076, 569.0), (-5.076, 568.89), (0.0, 568.89), (0.0, 568.75), (-5.076, 568.89), (-5.076, 568.62)]</t>
         </is>
       </c>
     </row>
@@ -6127,7 +6127,7 @@
       </c>
       <c r="B571" t="inlineStr">
         <is>
-          <t>[(-0.3, 570.0), (-0.3, 569.88), (-4.808, 570.0), (-4.808, 569.88), (-0.3, 569.88), (-0.3, 569.75), (-4.808, 569.88), (-4.808, 569.58)]</t>
+          <t>[(0.0, 570.0), (0.0, 569.88), (-4.808, 570.0), (-4.808, 569.88), (0.0, 569.88), (0.0, 569.75), (-4.808, 569.88), (-4.808, 569.58)]</t>
         </is>
       </c>
     </row>
@@ -6137,7 +6137,7 @@
       </c>
       <c r="B572" t="inlineStr">
         <is>
-          <t>[(-0.3, 571.0), (-0.3, 570.87), (-4.475, 571.0), (-4.475, 570.87), (-0.3, 570.87), (-0.3, 570.73), (-4.475, 570.87), (-4.475, 570.57)]</t>
+          <t>[(0.0, 571.0), (0.0, 570.87), (-4.475, 571.0), (-4.475, 570.87), (0.0, 570.87), (0.0, 570.73), (-4.475, 570.87), (-4.475, 570.57)]</t>
         </is>
       </c>
     </row>
@@ -6147,7 +6147,7 @@
       </c>
       <c r="B573" t="inlineStr">
         <is>
-          <t>[(-0.3, 572.0), (-0.3, 571.82), (-4.178, 572.0), (-4.178, 571.82), (-0.3, 571.82), (-0.3, 571.68), (-4.178, 571.82), (-4.178, 571.52)]</t>
+          <t>[(0.0, 572.0), (0.0, 571.82), (-4.178, 572.0), (-4.178, 571.82), (0.0, 571.82), (0.0, 571.68), (-4.178, 571.82), (-4.178, 571.52)]</t>
         </is>
       </c>
     </row>
@@ -6157,7 +6157,7 @@
       </c>
       <c r="B574" t="inlineStr">
         <is>
-          <t>[(-0.3, 573.0), (-0.3, 572.88), (-3.883, 573.0), (-3.883, 572.88), (-0.3, 572.88), (-0.3, 572.69), (-3.883, 572.88), (-3.883, 572.58)]</t>
+          <t>[(0.0, 573.0), (0.0, 572.88), (-3.883, 573.0), (-3.883, 572.88), (0.0, 572.88), (0.0, 572.69), (-3.883, 572.88), (-3.883, 572.58)]</t>
         </is>
       </c>
     </row>
@@ -6167,7 +6167,7 @@
       </c>
       <c r="B575" t="inlineStr">
         <is>
-          <t>[(-0.3, 574.0), (-0.3, 573.89), (-3.535, 574.0), (-3.535, 573.89), (-0.3, 573.89), (-0.3, 573.71), (-3.535, 573.89), (-3.535, 573.62)]</t>
+          <t>[(0.0, 574.0), (0.0, 573.89), (-3.535, 574.0), (-3.535, 573.89), (0.0, 573.89), (0.0, 573.71), (-3.535, 573.89), (-3.535, 573.62)]</t>
         </is>
       </c>
     </row>
@@ -6177,7 +6177,7 @@
       </c>
       <c r="B576" t="inlineStr">
         <is>
-          <t>[(-0.3, 575.0), (-0.3, 574.89), (-3.088, 575.0), (-3.088, 574.89), (-0.3, 574.89), (-0.3, 574.74), (-3.088, 574.89), (-3.088, 574.69)]</t>
+          <t>[(0.0, 575.0), (0.0, 574.89), (-3.088, 575.0), (-3.088, 574.89), (0.0, 574.89), (0.0, 574.74), (-3.088, 574.89), (-3.088, 574.69)]</t>
         </is>
       </c>
     </row>
@@ -6187,7 +6187,7 @@
       </c>
       <c r="B577" t="inlineStr">
         <is>
-          <t>[(-0.3, 576.0), (-0.3, 575.89), (-2.856, 576.0), (-2.856, 575.89), (-0.3, 575.89), (-0.3, 575.73), (-2.856, 575.89), (-2.856, 575.63)]</t>
+          <t>[(0.0, 576.0), (0.0, 575.89), (-2.856, 576.0), (-2.856, 575.89), (0.0, 575.89), (0.0, 575.73), (-2.856, 575.89), (-2.856, 575.63)]</t>
         </is>
       </c>
     </row>
@@ -6197,7 +6197,7 @@
       </c>
       <c r="B578" t="inlineStr">
         <is>
-          <t>[(-0.3, 577.0), (-0.3, 576.79), (-2.574, 577.0), (-2.574, 576.79), (-0.3, 576.79), (-0.3, 576.65), (-2.574, 576.79), (-2.574, 576.59)]</t>
+          <t>[(0.0, 577.0), (0.0, 576.79), (-2.574, 577.0), (-2.574, 576.79), (0.0, 576.79), (0.0, 576.65), (-2.574, 576.79), (-2.574, 576.59)]</t>
         </is>
       </c>
     </row>
@@ -6257,7 +6257,7 @@
       </c>
       <c r="B584" t="inlineStr">
         <is>
-          <t>[(-0.3, 583.0), (-0.3, 582.82), (-2.817, 583.0), (-2.817, 582.82), (-0.3, 582.82), (-0.3, 582.64), (-2.817, 582.82), (-2.817, 582.64), (-0.3, 582.64), (-0.3, 582.51), (-2.817, 582.64), (-2.817, 582.47)]</t>
+          <t>[(0.0, 583.0), (0.0, 582.82), (-2.817, 583.0), (-2.817, 582.82), (0.0, 582.82), (0.0, 582.64), (-2.817, 582.82), (-2.817, 582.64), (0.0, 582.64), (0.0, 582.51), (-2.817, 582.64), (-2.817, 582.47)]</t>
         </is>
       </c>
     </row>
@@ -6267,7 +6267,7 @@
       </c>
       <c r="B585" t="inlineStr">
         <is>
-          <t>[(-0.3, 584.0), (-0.3, 583.8), (-3.503, 584.0), (-3.503, 583.8), (-0.3, 583.8), (-0.3, 583.6), (-3.503, 583.8), (-3.503, 583.6), (-0.3, 583.6), (-0.3, 583.48), (-3.503, 583.6), (-3.503, 583.42)]</t>
+          <t>[(0.0, 584.0), (0.0, 583.8), (-3.503, 584.0), (-3.503, 583.8), (0.0, 583.8), (0.0, 583.6), (-3.503, 583.8), (-3.503, 583.6), (0.0, 583.6), (0.0, 583.48), (-3.503, 583.6), (-3.503, 583.42)]</t>
         </is>
       </c>
     </row>
@@ -6277,7 +6277,7 @@
       </c>
       <c r="B586" t="inlineStr">
         <is>
-          <t>[(-0.3, 585.0), (-0.3, 584.81), (-4.21, 585.0), (-4.21, 584.81), (-0.3, 584.81), (-0.3, 584.62), (-4.21, 584.81), (-4.21, 584.62), (-0.3, 584.62), (-0.3, 584.49), (-4.21, 584.62), (-4.21, 584.44)]</t>
+          <t>[(0.0, 585.0), (0.0, 584.81), (-4.21, 585.0), (-4.21, 584.81), (0.0, 584.81), (0.0, 584.62), (-4.21, 584.81), (-4.21, 584.62), (0.0, 584.62), (0.0, 584.49), (-4.21, 584.62), (-4.21, 584.44)]</t>
         </is>
       </c>
     </row>
@@ -6287,7 +6287,7 @@
       </c>
       <c r="B587" t="inlineStr">
         <is>
-          <t>[(-0.3, 586.0), (-0.3, 585.86), (-4.773, 586.0), (-4.773, 585.86), (-0.3, 585.86), (-0.3, 585.72), (-4.773, 585.86), (-4.773, 585.72), (-0.3, 585.72), (-0.3, 585.58), (-4.773, 585.72), (-4.773, 585.58), (-0.3, 585.58), (-0.3, 585.45), (-4.773, 585.58), (-4.773, 585.45)]</t>
+          <t>[(0.0, 586.0), (0.0, 585.86), (-4.773, 586.0), (-4.773, 585.86), (0.0, 585.86), (0.0, 585.72), (-4.773, 585.86), (-4.773, 585.72), (0.0, 585.72), (0.0, 585.58), (-4.773, 585.72), (-4.773, 585.58), (0.0, 585.58), (0.0, 585.45), (-4.773, 585.58), (-4.773, 585.45)]</t>
         </is>
       </c>
     </row>
@@ -6297,7 +6297,7 @@
       </c>
       <c r="B588" t="inlineStr">
         <is>
-          <t>[(-0.3, 587.0), (-0.3, 586.81), (-5.262, 587.0), (-5.262, 586.81), (-0.3, 586.81), (-0.3, 586.62), (-5.262, 586.81), (-5.262, 586.62), (-0.3, 586.62), (-0.3, 586.46), (-5.262, 586.62), (-5.262, 586.44)]</t>
+          <t>[(0.0, 587.0), (0.0, 586.81), (-5.262, 587.0), (-5.262, 586.81), (0.0, 586.81), (0.0, 586.62), (-5.262, 586.81), (-5.262, 586.62), (0.0, 586.62), (0.0, 586.46), (-5.262, 586.62), (-5.262, 586.44)]</t>
         </is>
       </c>
     </row>
@@ -6307,7 +6307,7 @@
       </c>
       <c r="B589" t="inlineStr">
         <is>
-          <t>[(-0.3, 588.0), (-0.3, 587.83), (-5.703, 588.0), (-5.703, 587.83), (-0.3, 587.83), (-0.3, 587.66), (-5.703, 587.83), (-5.703, 587.66), (-0.3, 587.66), (-0.3, 587.52), (-5.703, 587.66), (-5.703, 587.5)]</t>
+          <t>[(0.0, 588.0), (0.0, 587.83), (-5.703, 588.0), (-5.703, 587.83), (0.0, 587.83), (0.0, 587.66), (-5.703, 587.83), (-5.703, 587.66), (0.0, 587.66), (0.0, 587.52), (-5.703, 587.66), (-5.703, 587.5)]</t>
         </is>
       </c>
     </row>
@@ -6317,7 +6317,7 @@
       </c>
       <c r="B590" t="inlineStr">
         <is>
-          <t>[(-0.3, 589.0), (-0.3, 588.84), (-6.002, 589.0), (-6.002, 588.84), (-0.3, 588.84), (-0.3, 588.68), (-6.002, 588.84), (-6.002, 588.68), (-0.3, 588.68), (-0.3, 588.57), (-6.002, 588.68), (-6.002, 588.53)]</t>
+          <t>[(0.0, 589.0), (0.0, 588.84), (-6.002, 589.0), (-6.002, 588.84), (0.0, 588.84), (0.0, 588.68), (-6.002, 588.84), (-6.002, 588.68), (0.0, 588.68), (0.0, 588.57), (-6.002, 588.68), (-6.002, 588.53)]</t>
         </is>
       </c>
     </row>
@@ -6327,7 +6327,7 @@
       </c>
       <c r="B591" t="inlineStr">
         <is>
-          <t>[(-0.3, 590.0), (-0.3, 589.85), (-6.096, 590.0), (-6.096, 589.85), (-0.3, 589.85), (-0.3, 589.7), (-6.096, 589.85), (-6.096, 589.7), (-0.3, 589.7), (-0.3, 589.56), (-6.096, 589.7), (-6.096, 589.57)]</t>
+          <t>[(0.0, 590.0), (0.0, 589.85), (-6.096, 590.0), (-6.096, 589.85), (0.0, 589.85), (0.0, 589.7), (-6.096, 589.85), (-6.096, 589.7), (0.0, 589.7), (0.0, 589.56), (-6.096, 589.7), (-6.096, 589.57)]</t>
         </is>
       </c>
     </row>
@@ -6337,7 +6337,7 @@
       </c>
       <c r="B592" t="inlineStr">
         <is>
-          <t>[(-0.3, 591.0), (-0.3, 590.8), (-6.187, 591.0), (-6.187, 590.8), (-0.3, 590.8), (-0.3, 590.61), (-6.187, 590.8), (-6.187, 590.63)]</t>
+          <t>[(0.0, 591.0), (0.0, 590.8), (-6.187, 591.0), (-6.187, 590.8), (0.0, 590.8), (0.0, 590.61), (-6.187, 590.8), (-6.187, 590.63)]</t>
         </is>
       </c>
     </row>
@@ -6347,7 +6347,7 @@
       </c>
       <c r="B593" t="inlineStr">
         <is>
-          <t>[(-0.3, 592.0), (-0.3, 591.8), (-6.289, 592.0), (-6.289, 591.8), (-0.3, 591.8), (-0.3, 591.62), (-6.289, 591.8), (-6.289, 591.61)]</t>
+          <t>[(0.0, 592.0), (0.0, 591.8), (-6.289, 592.0), (-6.289, 591.8), (0.0, 591.8), (0.0, 591.62), (-6.289, 591.8), (-6.289, 591.61)]</t>
         </is>
       </c>
     </row>
@@ -6357,7 +6357,7 @@
       </c>
       <c r="B594" t="inlineStr">
         <is>
-          <t>[(-0.3, 593.0), (-0.3, 592.85), (-6.402, 593.0), (-6.402, 592.85), (-0.3, 592.85), (-0.3, 592.7), (-6.402, 592.85), (-6.402, 592.7), (-0.3, 592.7), (-0.3, 592.56), (-6.402, 592.7), (-6.402, 592.55)]</t>
+          <t>[(0.0, 593.0), (0.0, 592.85), (-6.402, 593.0), (-6.402, 592.85), (0.0, 592.85), (0.0, 592.7), (-6.402, 592.85), (-6.402, 592.7), (0.0, 592.7), (0.0, 592.56), (-6.402, 592.7), (-6.402, 592.55)]</t>
         </is>
       </c>
     </row>
@@ -6367,7 +6367,7 @@
       </c>
       <c r="B595" t="inlineStr">
         <is>
-          <t>[(-0.3, 594.0), (-0.3, 593.84), (-6.422, 594.0), (-6.422, 593.84), (-0.3, 593.84), (-0.3, 593.68), (-6.422, 593.84), (-6.422, 593.68), (-0.3, 593.68), (-0.3, 593.54), (-6.422, 593.68), (-6.422, 593.52)]</t>
+          <t>[(0.0, 594.0), (0.0, 593.84), (-6.422, 594.0), (-6.422, 593.84), (0.0, 593.84), (0.0, 593.68), (-6.422, 593.84), (-6.422, 593.68), (0.0, 593.68), (0.0, 593.54), (-6.422, 593.68), (-6.422, 593.52)]</t>
         </is>
       </c>
     </row>
@@ -6377,7 +6377,7 @@
       </c>
       <c r="B596" t="inlineStr">
         <is>
-          <t>[(-0.3, 595.0), (-0.3, 594.83), (-6.296, 595.0), (-6.296, 594.83), (-0.3, 594.83), (-0.3, 594.66), (-6.296, 594.83), (-6.296, 594.66), (-0.3, 594.66), (-0.3, 594.51), (-6.296, 594.66), (-6.296, 594.49)]</t>
+          <t>[(0.0, 595.0), (0.0, 594.83), (-6.296, 595.0), (-6.296, 594.83), (0.0, 594.83), (0.0, 594.66), (-6.296, 594.83), (-6.296, 594.66), (0.0, 594.66), (0.0, 594.51), (-6.296, 594.66), (-6.296, 594.49)]</t>
         </is>
       </c>
     </row>
@@ -6387,7 +6387,7 @@
       </c>
       <c r="B597" t="inlineStr">
         <is>
-          <t>[(-0.3, 596.0), (-0.3, 595.78), (-6.131, 596.0), (-6.131, 595.78), (-0.3, 595.78), (-0.3, 595.61), (-6.131, 595.78), (-6.131, 595.56)]</t>
+          <t>[(0.0, 596.0), (0.0, 595.78), (-6.131, 596.0), (-6.131, 595.78), (0.0, 595.78), (0.0, 595.61), (-6.131, 595.78), (-6.131, 595.56)]</t>
         </is>
       </c>
     </row>
@@ -6397,7 +6397,7 @@
       </c>
       <c r="B598" t="inlineStr">
         <is>
-          <t>[(-0.3, 597.0), (-0.3, 596.8), (-6.058, 597.0), (-6.058, 596.8), (-0.3, 596.8), (-0.3, 596.61), (-6.058, 596.8), (-6.058, 596.64)]</t>
+          <t>[(0.0, 597.0), (0.0, 596.8), (-6.058, 597.0), (-6.058, 596.8), (0.0, 596.8), (0.0, 596.61), (-6.058, 596.8), (-6.058, 596.64)]</t>
         </is>
       </c>
     </row>
@@ -6407,7 +6407,7 @@
       </c>
       <c r="B599" t="inlineStr">
         <is>
-          <t>[(-0.3, 598.0), (-0.3, 597.83), (-6.146, 598.0), (-6.146, 597.83), (-0.3, 597.83), (-0.3, 597.53), (-6.146, 597.83), (-6.146, 597.71)]</t>
+          <t>[(0.0, 598.0), (0.0, 597.83), (-6.146, 598.0), (-6.146, 597.83), (0.0, 597.83), (0.0, 597.53), (-6.146, 597.83), (-6.146, 597.71)]</t>
         </is>
       </c>
     </row>
@@ -6417,7 +6417,7 @@
       </c>
       <c r="B600" t="inlineStr">
         <is>
-          <t>[(-0.3, 599.0), (-0.3, 598.82), (-6.221, 599.0), (-6.221, 598.82), (-0.3, 598.82), (-0.3, 598.64), (-6.221, 598.82), (-6.221, 598.64), (-0.3, 598.64), (-0.3, 598.48), (-6.221, 598.64), (-6.221, 598.53)]</t>
+          <t>[(0.0, 599.0), (0.0, 598.82), (-6.221, 599.0), (-6.221, 598.82), (0.0, 598.82), (0.0, 598.64), (-6.221, 598.82), (-6.221, 598.64), (0.0, 598.64), (0.0, 598.48), (-6.221, 598.64), (-6.221, 598.53)]</t>
         </is>
       </c>
     </row>
@@ -6427,7 +6427,7 @@
       </c>
       <c r="B601" t="inlineStr">
         <is>
-          <t>[(-0.3, 600.0), (-0.3, 599.72), (-6.222, 600.0), (-6.222, 599.72), (-0.3, 599.72), (-0.3, 599.45), (-6.222, 599.72), (-6.222, 599.57)]</t>
+          <t>[(0.0, 600.0), (0.0, 599.72), (-6.222, 600.0), (-6.222, 599.72), (0.0, 599.72), (0.0, 599.45), (-6.222, 599.72), (-6.222, 599.57)]</t>
         </is>
       </c>
     </row>
@@ -6437,7 +6437,7 @@
       </c>
       <c r="B602" t="inlineStr">
         <is>
-          <t>[(-0.3, 601.0), (-0.3, 600.76), (-6.155, 601.0), (-6.155, 600.76), (-0.3, 600.76), (-0.3, 600.46), (-6.155, 600.76), (-6.155, 600.63)]</t>
+          <t>[(0.0, 601.0), (0.0, 600.76), (-6.155, 601.0), (-6.155, 600.76), (0.0, 600.76), (0.0, 600.46), (-6.155, 600.76), (-6.155, 600.63)]</t>
         </is>
       </c>
     </row>
@@ -6447,7 +6447,7 @@
       </c>
       <c r="B603" t="inlineStr">
         <is>
-          <t>[(-0.3, 602.0), (-0.3, 601.74), (-6.006, 602.0), (-6.006, 601.86), (-0.3, 601.74), (-0.3, 601.48), (-6.006, 601.86), (-6.006, 601.72)]</t>
+          <t>[(0.0, 602.0), (0.0, 601.74), (-6.006, 602.0), (-6.006, 601.86), (0.0, 601.74), (0.0, 601.48), (-6.006, 601.86), (-6.006, 601.72)]</t>
         </is>
       </c>
     </row>
@@ -6457,7 +6457,7 @@
       </c>
       <c r="B604" t="inlineStr">
         <is>
-          <t>[(-0.3, 603.0), (-0.3, 602.76), (-5.889, 603.0), (-5.889, 602.88), (-0.3, 602.76), (-0.3, 602.52), (-5.889, 602.88), (-5.889, 602.76)]</t>
+          <t>[(0.0, 603.0), (0.0, 602.76), (-5.889, 603.0), (-5.889, 602.88), (0.0, 602.76), (0.0, 602.52), (-5.889, 602.88), (-5.889, 602.76)]</t>
         </is>
       </c>
     </row>
@@ -6477,7 +6477,7 @@
       </c>
       <c r="B606" t="inlineStr">
         <is>
-          <t>[(-0.3, 605.0), (-0.3, 604.76), (-5.663, 605.0), (-5.663, 604.87), (-0.3, 604.76), (-0.3, 604.52), (-5.663, 604.87), (-5.663, 604.74)]</t>
+          <t>[(0.0, 605.0), (0.0, 604.76), (-5.663, 605.0), (-5.663, 604.87), (0.0, 604.76), (0.0, 604.52), (-5.663, 604.87), (-5.663, 604.74)]</t>
         </is>
       </c>
     </row>
@@ -6487,7 +6487,7 @@
       </c>
       <c r="B607" t="inlineStr">
         <is>
-          <t>[(-0.3, 606.0), (-0.3, 605.74), (-5.511, 606.0), (-5.511, 605.85), (-0.3, 605.74), (-0.3, 605.48), (-5.511, 605.85), (-5.511, 605.7)]</t>
+          <t>[(0.0, 606.0), (0.0, 605.74), (-5.511, 606.0), (-5.511, 605.85), (0.0, 605.74), (0.0, 605.48), (-5.511, 605.85), (-5.511, 605.7)]</t>
         </is>
       </c>
     </row>
@@ -6497,7 +6497,7 @@
       </c>
       <c r="B608" t="inlineStr">
         <is>
-          <t>[(-0.3, 607.0), (-0.3, 606.74), (-5.47, 607.0), (-5.47, 606.85), (-0.3, 606.74), (-0.3, 606.48), (-5.47, 606.85), (-5.47, 606.7)]</t>
+          <t>[(0.0, 607.0), (0.0, 606.74), (-5.47, 607.0), (-5.47, 606.85), (0.0, 606.74), (0.0, 606.48), (-5.47, 606.85), (-5.47, 606.7)]</t>
         </is>
       </c>
     </row>
@@ -6507,7 +6507,7 @@
       </c>
       <c r="B609" t="inlineStr">
         <is>
-          <t>[(-0.3, 608.0), (-0.3, 607.77), (-5.416, 608.0), (-5.416, 607.77), (-0.3, 607.77), (-0.3, 607.47), (-5.416, 607.77), (-5.416, 607.66)]</t>
+          <t>[(0.0, 608.0), (0.0, 607.77), (-5.416, 608.0), (-5.416, 607.77), (0.0, 607.77), (0.0, 607.47), (-5.416, 607.77), (-5.416, 607.66)]</t>
         </is>
       </c>
     </row>
@@ -6517,7 +6517,7 @@
       </c>
       <c r="B610" t="inlineStr">
         <is>
-          <t>[(-0.3, 609.0), (-0.3, 608.81), (-5.474, 609.0), (-5.474, 608.81), (-0.3, 608.81), (-0.3, 608.51), (-5.474, 608.81), (-5.474, 608.67)]</t>
+          <t>[(0.0, 609.0), (0.0, 608.81), (-5.474, 609.0), (-5.474, 608.81), (0.0, 608.81), (0.0, 608.51), (-5.474, 608.81), (-5.474, 608.67)]</t>
         </is>
       </c>
     </row>
@@ -6527,7 +6527,7 @@
       </c>
       <c r="B611" t="inlineStr">
         <is>
-          <t>[(-0.3, 610.0), (-0.3, 609.82), (-5.528, 610.0), (-5.528, 609.82), (-0.3, 609.82), (-0.3, 609.52), (-5.528, 609.82), (-5.528, 609.68)]</t>
+          <t>[(0.0, 610.0), (0.0, 609.82), (-5.528, 610.0), (-5.528, 609.82), (0.0, 609.82), (0.0, 609.52), (-5.528, 609.82), (-5.528, 609.68)]</t>
         </is>
       </c>
     </row>
@@ -6537,7 +6537,7 @@
       </c>
       <c r="B612" t="inlineStr">
         <is>
-          <t>[(-0.3, 611.0), (-0.3, 610.78), (-5.578, 611.0), (-5.578, 610.78), (-0.3, 610.78), (-0.3, 610.56), (-5.578, 610.78), (-5.578, 610.65)]</t>
+          <t>[(0.0, 611.0), (0.0, 610.78), (-5.578, 611.0), (-5.578, 610.78), (0.0, 610.78), (0.0, 610.56), (-5.578, 610.78), (-5.578, 610.65)]</t>
         </is>
       </c>
     </row>
@@ -6547,7 +6547,7 @@
       </c>
       <c r="B613" t="inlineStr">
         <is>
-          <t>[(-0.3, 612.0), (-0.3, 611.84), (-5.642, 612.0), (-5.642, 611.84), (-0.3, 611.84), (-0.3, 611.68), (-5.642, 611.84), (-5.642, 611.68), (-0.3, 611.68), (-0.3, 611.55), (-5.642, 611.68), (-5.642, 611.52)]</t>
+          <t>[(0.0, 612.0), (0.0, 611.84), (-5.642, 612.0), (-5.642, 611.84), (0.0, 611.84), (0.0, 611.68), (-5.642, 611.84), (-5.642, 611.68), (0.0, 611.68), (0.0, 611.55), (-5.642, 611.68), (-5.642, 611.52)]</t>
         </is>
       </c>
     </row>
@@ -6557,7 +6557,7 @@
       </c>
       <c r="B614" t="inlineStr">
         <is>
-          <t>[(-0.3, 613.0), (-0.3, 612.76), (-5.707, 613.0), (-5.707, 612.76), (-0.3, 612.76), (-0.3, 612.59), (-5.707, 612.76), (-5.707, 612.53)]</t>
+          <t>[(0.0, 613.0), (0.0, 612.76), (-5.707, 613.0), (-5.707, 612.76), (0.0, 612.76), (0.0, 612.59), (-5.707, 612.76), (-5.707, 612.53)]</t>
         </is>
       </c>
     </row>
@@ -6567,7 +6567,7 @@
       </c>
       <c r="B615" t="inlineStr">
         <is>
-          <t>[(-0.3, 614.0), (-0.3, 613.78), (-5.693, 614.0), (-5.693, 613.78), (-0.3, 613.78), (-0.3, 613.61), (-5.693, 613.78), (-5.693, 613.57)]</t>
+          <t>[(0.0, 614.0), (0.0, 613.78), (-5.693, 614.0), (-5.693, 613.78), (0.0, 613.78), (0.0, 613.61), (-5.693, 613.78), (-5.693, 613.57)]</t>
         </is>
       </c>
     </row>
@@ -6577,7 +6577,7 @@
       </c>
       <c r="B616" t="inlineStr">
         <is>
-          <t>[(-0.3, 615.0), (-0.3, 614.82), (-5.737, 615.0), (-5.737, 614.82), (-0.3, 614.82), (-0.3, 614.65), (-5.737, 614.82), (-5.737, 614.64)]</t>
+          <t>[(0.0, 615.0), (0.0, 614.82), (-5.737, 615.0), (-5.737, 614.82), (0.0, 614.82), (0.0, 614.65), (-5.737, 614.82), (-5.737, 614.64)]</t>
         </is>
       </c>
     </row>
@@ -6587,7 +6587,7 @@
       </c>
       <c r="B617" t="inlineStr">
         <is>
-          <t>[(-0.3, 616.0), (-0.3, 615.83), (-5.754, 616.0), (-5.754, 615.83), (-0.3, 615.83), (-0.3, 615.72), (-5.754, 615.83), (-5.754, 615.67)]</t>
+          <t>[(0.0, 616.0), (0.0, 615.83), (-5.754, 616.0), (-5.754, 615.83), (0.0, 615.83), (0.0, 615.72), (-5.754, 615.83), (-5.754, 615.67)]</t>
         </is>
       </c>
     </row>
@@ -6597,7 +6597,7 @@
       </c>
       <c r="B618" t="inlineStr">
         <is>
-          <t>[(-0.3, 617.0), (-0.3, 616.82), (-5.745, 617.0), (-5.745, 616.82), (-0.3, 616.82), (-0.3, 616.69), (-5.745, 616.82), (-5.745, 616.64)]</t>
+          <t>[(0.0, 617.0), (0.0, 616.82), (-5.745, 617.0), (-5.745, 616.82), (0.0, 616.82), (0.0, 616.69), (-5.745, 616.82), (-5.745, 616.64)]</t>
         </is>
       </c>
     </row>
@@ -6607,7 +6607,7 @@
       </c>
       <c r="B619" t="inlineStr">
         <is>
-          <t>[(-0.3, 618.0), (-0.3, 617.85), (-5.566, 618.0), (-5.566, 617.85), (-0.3, 617.85), (-0.3, 617.72), (-5.566, 617.85), (-5.566, 617.7)]</t>
+          <t>[(0.0, 618.0), (0.0, 617.85), (-5.566, 618.0), (-5.566, 617.85), (0.0, 617.85), (0.0, 617.72), (-5.566, 617.85), (-5.566, 617.7)]</t>
         </is>
       </c>
     </row>
@@ -6627,7 +6627,7 @@
       </c>
       <c r="B621" t="inlineStr">
         <is>
-          <t>[(-0.3, 620.0), (-0.3, 619.85), (-5.379, 620.0), (-5.379, 619.85), (-0.3, 619.85), (-0.3, 619.72), (-5.379, 619.85), (-5.379, 619.72)]</t>
+          <t>[(0.0, 620.0), (0.0, 619.85), (-5.379, 620.0), (-5.379, 619.85), (0.0, 619.85), (0.0, 619.72), (-5.379, 619.85), (-5.379, 619.72)]</t>
         </is>
       </c>
     </row>
@@ -6647,7 +6647,7 @@
       </c>
       <c r="B623" t="inlineStr">
         <is>
-          <t>[(-0.3, 622.0), (-0.3, 621.84), (-5.574, 622.0), (-5.574, 621.84), (-0.3, 621.84), (-0.3, 621.68), (-5.574, 621.84), (-5.574, 621.73)]</t>
+          <t>[(0.0, 622.0), (0.0, 621.84), (-5.574, 622.0), (-5.574, 621.84), (0.0, 621.84), (0.0, 621.68), (-5.574, 621.84), (-5.574, 621.73)]</t>
         </is>
       </c>
     </row>
@@ -6657,7 +6657,7 @@
       </c>
       <c r="B624" t="inlineStr">
         <is>
-          <t>[(-0.3, 623.0), (-0.3, 622.89), (-5.733, 623.0), (-5.733, 622.89), (-0.3, 622.89), (-0.3, 622.67), (-5.733, 622.89), (-5.733, 622.73)]</t>
+          <t>[(0.0, 623.0), (0.0, 622.89), (-5.733, 623.0), (-5.733, 622.89), (0.0, 622.89), (0.0, 622.67), (-5.733, 622.89), (-5.733, 622.73)]</t>
         </is>
       </c>
     </row>
@@ -6667,7 +6667,7 @@
       </c>
       <c r="B625" t="inlineStr">
         <is>
-          <t>[(-0.3, 624.0), (-0.3, 623.82), (-5.937, 624.0), (-5.937, 623.82), (-0.3, 623.82), (-0.3, 623.65), (-5.937, 623.82), (-5.937, 623.68)]</t>
+          <t>[(0.0, 624.0), (0.0, 623.82), (-5.937, 624.0), (-5.937, 623.82), (0.0, 623.82), (0.0, 623.65), (-5.937, 623.82), (-5.937, 623.68)]</t>
         </is>
       </c>
     </row>
@@ -6677,7 +6677,7 @@
       </c>
       <c r="B626" t="inlineStr">
         <is>
-          <t>[(-0.3, 625.0), (-0.3, 624.8), (-6.034, 625.0), (-6.034, 624.8), (-0.3, 624.8), (-0.3, 624.61), (-6.034, 624.8), (-6.034, 624.64)]</t>
+          <t>[(0.0, 625.0), (0.0, 624.8), (-6.034, 625.0), (-6.034, 624.8), (0.0, 624.8), (0.0, 624.61), (-6.034, 624.8), (-6.034, 624.64)]</t>
         </is>
       </c>
     </row>
@@ -6687,7 +6687,7 @@
       </c>
       <c r="B627" t="inlineStr">
         <is>
-          <t>[(-0.3, 626.0), (-0.3, 625.78), (-6.25, 626.0), (-6.25, 625.78), (-0.3, 625.78), (-0.3, 625.57), (-6.25, 625.78), (-6.25, 625.6)]</t>
+          <t>[(0.0, 626.0), (0.0, 625.78), (-6.25, 626.0), (-6.25, 625.78), (0.0, 625.78), (0.0, 625.57), (-6.25, 625.78), (-6.25, 625.6)]</t>
         </is>
       </c>
     </row>
@@ -6697,7 +6697,7 @@
       </c>
       <c r="B628" t="inlineStr">
         <is>
-          <t>[(-0.3, 627.0), (-0.3, 626.78), (-6.434, 627.0), (-6.434, 626.78), (-0.3, 626.78), (-0.3, 626.56), (-6.434, 626.78), (-6.434, 626.6)]</t>
+          <t>[(0.0, 627.0), (0.0, 626.78), (-6.434, 627.0), (-6.434, 626.78), (0.0, 626.78), (0.0, 626.56), (-6.434, 626.78), (-6.434, 626.6)]</t>
         </is>
       </c>
     </row>
@@ -6707,7 +6707,7 @@
       </c>
       <c r="B629" t="inlineStr">
         <is>
-          <t>[(-0.3, 628.0), (-0.3, 627.78), (-6.611, 628.0), (-6.611, 627.78), (-0.3, 627.78), (-0.3, 627.57), (-6.611, 627.78), (-6.611, 627.61)]</t>
+          <t>[(0.0, 628.0), (0.0, 627.78), (-6.611, 628.0), (-6.611, 627.78), (0.0, 627.78), (0.0, 627.57), (-6.611, 627.78), (-6.611, 627.61)]</t>
         </is>
       </c>
     </row>
@@ -6717,7 +6717,7 @@
       </c>
       <c r="B630" t="inlineStr">
         <is>
-          <t>[(-0.3, 629.0), (-0.3, 628.79), (-6.849, 629.0), (-6.849, 628.79), (-0.3, 628.79), (-0.3, 628.58), (-6.849, 628.79), (-6.849, 628.64)]</t>
+          <t>[(0.0, 629.0), (0.0, 628.79), (-6.849, 629.0), (-6.849, 628.79), (0.0, 628.79), (0.0, 628.58), (-6.849, 628.79), (-6.849, 628.64)]</t>
         </is>
       </c>
     </row>
@@ -6727,7 +6727,7 @@
       </c>
       <c r="B631" t="inlineStr">
         <is>
-          <t>[(-0.3, 630.0), (-0.3, 629.77), (-7.077, 630.0), (-7.077, 629.77), (-0.3, 629.77), (-0.3, 629.54), (-7.077, 629.77), (-7.077, 629.6)]</t>
+          <t>[(0.0, 630.0), (0.0, 629.77), (-7.077, 630.0), (-7.077, 629.77), (0.0, 629.77), (0.0, 629.54), (-7.077, 629.77), (-7.077, 629.6)]</t>
         </is>
       </c>
     </row>
@@ -6737,7 +6737,7 @@
       </c>
       <c r="B632" t="inlineStr">
         <is>
-          <t>[(-0.3, 631.0), (-0.3, 630.81), (-7.33, 631.0), (-7.33, 630.81), (-0.3, 630.81), (-0.3, 630.62), (-7.33, 630.81), (-7.33, 630.64)]</t>
+          <t>[(0.0, 631.0), (0.0, 630.81), (-7.33, 631.0), (-7.33, 630.81), (0.0, 630.81), (0.0, 630.62), (-7.33, 630.81), (-7.33, 630.64)]</t>
         </is>
       </c>
     </row>
@@ -6747,7 +6747,7 @@
       </c>
       <c r="B633" t="inlineStr">
         <is>
-          <t>[(-0.3, 632.0), (-0.3, 631.83), (-7.345, 632.0), (-7.345, 631.83), (-0.3, 631.83), (-0.3, 631.67), (-7.345, 631.83), (-7.345, 631.72)]</t>
+          <t>[(0.0, 632.0), (0.0, 631.83), (-7.345, 632.0), (-7.345, 631.83), (0.0, 631.83), (0.0, 631.67), (-7.345, 631.83), (-7.345, 631.72)]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Superelevation data. Coordinates.py review
</commit_message>
<xml_diff>
--- a/output/layerCoordinates_left.xlsx
+++ b/output/layerCoordinates_left.xlsx
@@ -727,7 +727,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>[(-0.3, 30.0), (-0.3, 29.86), (-5.672, 30.0), (-5.672, 29.86), (-0.3, 29.86), (-0.3, 29.74), (-5.672, 29.86), (-5.672, 29.74)]</t>
+          <t>[(-0.3, 30.0), (-0.3, 29.86), (-5.672, 29.6593978429311), (-5.672, 29.5193978429311), (-0.3, 29.86), (-0.3, 29.74), (-5.672, 29.5193978429311), (-5.672, 29.399397842931098)]</t>
         </is>
       </c>
     </row>
@@ -737,7 +737,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>[(-0.3, 31.0), (-0.3, 30.85), (-5.585, 31.0), (-5.585, 30.85), (-0.3, 30.85), (-0.3, 30.73), (-5.585, 30.85), (-5.585, 30.72)]</t>
+          <t>[(-0.3, 31.0), (-0.3, 30.85), (-5.585, 30.6999841400797), (-5.585, 30.5499841400797), (-0.3, 30.85), (-0.3, 30.73), (-5.585, 30.5499841400797), (-5.585, 30.4199841400797)]</t>
         </is>
       </c>
     </row>
@@ -747,7 +747,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>[(-0.3, 32.0), (-0.3, 31.8), (-5.304, 32.0), (-5.304, 31.8), (-0.3, 31.8), (-0.3, 31.68), (-5.304, 31.8), (-5.304, 31.61)]</t>
+          <t>[(-0.3, 32.0), (-0.3, 31.8), (-5.304, 31.7491413430596), (-5.304, 31.5491413430596), (-0.3, 31.8), (-0.3, 31.68), (-5.304, 31.5491413430596), (-5.304, 31.359141343059598)]</t>
         </is>
       </c>
     </row>
@@ -757,7 +757,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>[(-0.3, 33.0), (-0.3, 32.78), (-4.806, 33.0), (-4.806, 32.78), (-0.3, 32.78), (-0.3, 32.63), (-4.806, 32.78), (-4.806, 32.57)]</t>
+          <t>[(-0.3, 33.0), (-0.3, 32.78), (-4.806, 32.80400781877695), (-4.806, 32.58400781877695), (-0.3, 32.78), (-0.3, 32.63), (-4.806, 32.58400781877695), (-4.806, 32.37400781877695)]</t>
         </is>
       </c>
     </row>
@@ -767,7 +767,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>[(-0.3, 34.0), (-0.3, 33.8), (-3.873, 34.0), (-3.873, 33.8), (-0.3, 33.8), (-0.3, 33.62), (-3.873, 33.8), (-3.873, 33.61)]</t>
+          <t>[(-0.3, 34.0), (-0.3, 33.8), (-3.873, 33.868299144434836), (-3.873, 33.66829914443483), (-0.3, 33.8), (-0.3, 33.62), (-3.873, 33.66829914443483), (-3.873, 33.478299144434835)]</t>
         </is>
       </c>
     </row>
@@ -777,7 +777,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>[(-0.3, 35.0), (-0.3, 34.85), (-2.676, 35.0), (-2.676, 34.85), (-0.3, 34.85), (-0.3, 34.7), (-2.676, 34.85), (-2.676, 34.7), (-0.3, 34.7), (-0.3, 34.57), (-2.676, 34.7), (-2.676, 34.57)]</t>
+          <t>[(-0.3, 35.0), (-0.3, 34.85), (-2.676, 34.928187256416784), (-2.676, 34.778187256416786), (-0.3, 34.85), (-0.3, 34.7), (-2.676, 34.778187256416786), (-2.676, 34.62818725641679), (-0.3, 34.7), (-0.3, 34.57), (-2.676, 34.62818725641679), (-2.676, 34.498187256416784)]</t>
         </is>
       </c>
     </row>
@@ -1837,7 +1837,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>[(-0.3, 141.0), (-0.3, 140.74), (-2.69, 141.0), (-2.69, 140.74), (-0.3, 140.74), (-0.3, 140.54), (-2.69, 140.74), (-2.69, 140.48)]</t>
+          <t>[(-0.3, 141.0), (-0.3, 140.74), (-2.69, 141.15639433372263), (-2.69, 140.89639433372264), (-0.3, 140.74), (-0.3, 140.54), (-2.69, 140.89639433372264), (-2.69, 140.63639433372262)]</t>
         </is>
       </c>
     </row>
@@ -1847,7 +1847,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>[(-0.3, 142.0), (-0.3, 141.73), (-3.261, 142.0), (-3.261, 141.73), (-0.3, 141.73), (-0.3, 141.54), (-3.261, 141.73), (-3.261, 141.46)]</t>
+          <t>[(-0.3, 142.0), (-0.3, 141.73), (-3.261, 142.18157941193954), (-3.261, 141.91157941193953), (-0.3, 141.73), (-0.3, 141.54), (-3.261, 141.91157941193953), (-3.261, 141.64157941193955)]</t>
         </is>
       </c>
     </row>
@@ -1857,7 +1857,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>[(-0.3, 143.0), (-0.3, 142.74), (-3.659, 143.0), (-3.659, 142.74), (-0.3, 142.74), (-0.3, 142.55), (-3.659, 142.74), (-3.659, 142.48)]</t>
+          <t>[(-0.3, 143.0), (-0.3, 142.74), (-3.659, 143.1921697242505), (-3.659, 142.9321697242505), (-0.3, 142.74), (-0.3, 142.55), (-3.659, 142.9321697242505), (-3.659, 142.6721697242505)]</t>
         </is>
       </c>
     </row>
@@ -1867,7 +1867,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>[(-0.3, 144.0), (-0.3, 143.85), (-4.017, 144.0), (-4.017, 143.85), (-0.3, 143.85), (-0.3, 143.7), (-4.017, 143.85), (-4.017, 143.7), (-0.3, 143.7), (-0.3, 143.59), (-4.017, 143.7), (-4.017, 143.57)]</t>
+          <t>[(-0.3, 144.0), (-0.3, 143.85), (-4.017, 144.1973619800478), (-4.017, 144.04736198004778), (-0.3, 143.85), (-0.3, 143.7), (-4.017, 144.04736198004778), (-4.017, 143.89736198004778), (-0.3, 143.7), (-0.3, 143.59), (-4.017, 143.89736198004778), (-4.017, 143.76736198004778)]</t>
         </is>
       </c>
     </row>
@@ -1877,7 +1877,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>[(-0.3, 145.0), (-0.3, 144.81), (-4.438, 145.0), (-4.438, 144.81), (-0.3, 144.81), (-0.3, 144.64), (-4.438, 144.81), (-4.438, 144.62)]</t>
+          <t>[(-0.3, 145.0), (-0.3, 144.81), (-4.438, 145.2026951080572), (-4.438, 145.01269510805722), (-0.3, 144.81), (-0.3, 144.64), (-4.438, 145.01269510805722), (-4.438, 144.82269510805722)]</t>
         </is>
       </c>
     </row>
@@ -1887,7 +1887,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>[(-0.3, 146.0), (-0.3, 145.81), (-4.773, 146.0), (-4.773, 145.81), (-0.3, 145.81), (-0.3, 145.65), (-4.773, 145.81), (-4.773, 145.62)]</t>
+          <t>[(-0.3, 146.0), (-0.3, 145.81), (-4.773, 146.20070598565601), (-4.773, 146.01070598565602), (-0.3, 145.81), (-0.3, 145.65), (-4.773, 146.01070598565602), (-4.773, 145.82070598565602)]</t>
         </is>
       </c>
     </row>
@@ -1897,7 +1897,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>[(-0.3, 147.0), (-0.3, 146.79), (-5.091, 147.0), (-5.091, 146.79), (-0.3, 146.79), (-0.3, 146.61), (-5.091, 146.79), (-5.091, 146.58)]</t>
+          <t>[(-0.3, 147.0), (-0.3, 146.79), (-5.091, 147.19526809118963), (-5.091, 146.98526809118962), (-0.3, 146.79), (-0.3, 146.61), (-5.091, 146.98526809118962), (-5.091, 146.77526809118964)]</t>
         </is>
       </c>
     </row>
@@ -1907,7 +1907,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>[(-0.3, 148.0), (-0.3, 147.85), (-5.595, 148.0), (-5.595, 147.85), (-0.3, 147.85), (-0.3, 147.7), (-5.595, 147.85), (-5.595, 147.7), (-0.3, 147.7), (-0.3, 147.58), (-5.595, 147.7), (-5.595, 147.56)]</t>
+          <t>[(-0.3, 148.0), (-0.3, 147.85), (-5.595, 148.19402993216804), (-5.595, 148.04402993216803), (-0.3, 147.85), (-0.3, 147.7), (-5.595, 148.04402993216803), (-5.595, 147.89402993216802), (-0.3, 147.7), (-0.3, 147.58), (-5.595, 147.89402993216802), (-5.595, 147.75402993216804)]</t>
         </is>
       </c>
     </row>
@@ -1917,7 +1917,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>[(-0.3, 149.0), (-0.3, 148.85), (-6.265, 149.0), (-6.265, 148.85), (-0.3, 148.85), (-0.3, 148.7), (-6.265, 148.85), (-6.265, 148.7), (-0.3, 148.7), (-0.3, 148.57), (-6.265, 148.7), (-6.265, 148.55)]</t>
+          <t>[(-0.3, 149.0), (-0.3, 148.85), (-6.265, 149.1940456834594), (-6.265, 149.0440456834594), (-0.3, 148.85), (-0.3, 148.7), (-6.265, 149.0440456834594), (-6.265, 148.89404568345938), (-0.3, 148.7), (-0.3, 148.57), (-6.265, 148.89404568345938), (-6.265, 148.7440456834594)]</t>
         </is>
       </c>
     </row>
@@ -1927,7 +1927,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>[(-0.3, 150.0), (-0.3, 149.85), (-7.035, 150.0), (-7.035, 149.85), (-0.3, 149.85), (-0.3, 149.7), (-7.035, 149.85), (-7.035, 149.7), (-0.3, 149.7), (-0.3, 149.59), (-7.035, 149.7), (-7.035, 149.56)]</t>
+          <t>[(-0.3, 150.0), (-0.3, 149.85), (-7.035, 150.19139138072242), (-7.035, 150.04139138072242), (-0.3, 149.85), (-0.3, 149.7), (-7.035, 150.04139138072242), (-7.035, 149.8913913807224), (-0.3, 149.7), (-0.3, 149.59), (-7.035, 149.8913913807224), (-7.035, 149.75139138072242)]</t>
         </is>
       </c>
     </row>
@@ -1937,7 +1937,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>[(-0.3, 151.0), (-0.3, 150.79), (-7.802, 151.0), (-7.802, 150.79), (-0.3, 150.79), (-0.3, 150.61), (-7.802, 150.79), (-7.802, 150.58)]</t>
+          <t>[(-0.3, 151.0), (-0.3, 150.79), (-7.802, 151.15582175639148), (-7.802, 150.94582175639147), (-0.3, 150.79), (-0.3, 150.61), (-7.802, 150.94582175639147), (-7.802, 150.7358217563915)]</t>
         </is>
       </c>
     </row>
@@ -1947,7 +1947,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>[(-0.3, 152.0), (-0.3, 151.82), (-8.397, 152.0), (-8.397, 151.82), (-0.3, 151.82), (-0.3, 151.65), (-8.397, 151.82), (-8.397, 151.67)]</t>
+          <t>[(-0.3, 152.0), (-0.3, 151.82), (-8.397, 151.96575532011482), (-8.397, 151.78575532011482), (-0.3, 151.82), (-0.3, 151.65), (-8.397, 151.78575532011482), (-8.397, 151.6357553201148)]</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>[(-0.3, 160.0), (-0.3, 159.88), (-4.255, 160.0), (-4.255, 159.88), (-4.255, 160.0), (-4.255, 159.86), (-15.746, 160.0), (-15.746, 159.86), (-0.3, 159.88), (-0.3, 159.58), (-4.255, 159.88), (-4.255, 159.74), (-4.255, 159.86), (-4.255, 159.74), (-15.746, 159.86), (-15.746, 159.74)]</t>
+          <t>[(-0.3, 160.0), (-0.3, 159.88), (-4.255, 159.901125), (-4.255, 159.781125), (-4.255, 159.901125), (-4.255, 159.76112500000002), (-15.746, 159.61385), (-15.746, 159.47385000000003), (-0.3, 159.88), (-0.3, 159.58), (-4.255, 159.781125), (-4.255, 159.64112500000002), (-4.255, 159.76112500000002), (-4.255, 159.64112500000002), (-15.746, 159.47385000000003), (-15.746, 159.35385000000002)]</t>
         </is>
       </c>
     </row>
@@ -2317,7 +2317,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>[(-0.3, 189.0), (-0.3, 188.81), (-3.637, 189.0), (-3.637, 188.81), (-0.3, 188.81), (-0.3, 188.62), (-3.637, 188.81), (-3.637, 188.69)]</t>
+          <t>[(-0.3, 189.0), (-0.3, 188.81), (-3.637, 188.79978), (-3.637, 188.60978), (-0.3, 188.81), (-0.3, 188.62), (-3.637, 188.60978), (-3.637, 188.48978)]</t>
         </is>
       </c>
     </row>
@@ -2327,7 +2327,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>[(-0.3, 190.0), (-0.3, 189.89), (-3.053, 190.0), (-3.053, 189.89), (-0.3, 189.89), (-0.3, 189.67), (-3.053, 189.89), (-3.053, 189.75)]</t>
+          <t>[(-0.3, 190.0), (-0.3, 189.89), (-3.053, 189.83482), (-3.053, 189.72482), (-0.3, 189.89), (-0.3, 189.67), (-3.053, 189.72482), (-3.053, 189.58482)]</t>
         </is>
       </c>
     </row>
@@ -2337,7 +2337,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>[(-0.3, 191.0), (-0.3, 190.82), (-2.361, 191.0), (-2.361, 190.82), (-0.3, 190.82), (-0.3, 190.64), (-2.361, 190.82), (-2.361, 190.68)]</t>
+          <t>[(-0.3, 191.0), (-0.3, 190.82), (-2.361, 190.8818044998697), (-2.361, 190.7018044998697), (-0.3, 190.82), (-0.3, 190.64), (-2.361, 190.7018044998697), (-2.361, 190.5618044998697)]</t>
         </is>
       </c>
     </row>
@@ -2607,7 +2607,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>[(-0.3, 218.0), (-0.3, 217.89), (-6.083, 218.0), (-6.083, 217.89), (-6.083, 218.0), (-6.083, 217.75), (-9.456, 218.0), (-9.456, 217.75), (-0.3, 217.89), (-0.3, 217.73), (-6.083, 217.89), (-6.083, 217.64), (-6.083, 217.75), (-6.083, 217.64), (-9.456, 217.75), (-9.456, 217.51)]</t>
+          <t>[(-0.3, 218.0), (-0.3, 217.89), (-6.083, 218.40481), (-6.083, 218.29480999999998), (-6.083, 218.40481), (-6.083, 218.15481), (-9.456, 218.64092), (-9.456, 218.39092), (-0.3, 217.89), (-0.3, 217.73), (-6.083, 218.29480999999998), (-6.083, 218.04480999999998), (-6.083, 218.15481), (-6.083, 218.04480999999998), (-9.456, 218.39092), (-9.456, 218.15091999999999)]</t>
         </is>
       </c>
     </row>
@@ -2617,7 +2617,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>[(-0.3, 219.0), (-0.3, 218.89), (-7.801, 219.0), (-7.801, 218.89), (-7.801, 219.0), (-7.801, 218.72), (-11.196, 219.0), (-11.196, 218.72), (-0.3, 218.89), (-0.3, 218.72), (-7.801, 218.89), (-7.801, 218.59), (-7.801, 218.72), (-7.801, 218.59), (-11.196, 218.72), (-11.196, 218.44)]</t>
+          <t>[(-0.3, 219.0), (-0.3, 218.89), (-7.801, 219.52507), (-7.801, 219.41507), (-7.801, 219.52507), (-7.801, 219.24507), (-11.196, 219.76272), (-11.196, 219.48272), (-0.3, 218.89), (-0.3, 218.72), (-7.801, 219.41507), (-7.801, 219.11507), (-7.801, 219.24507), (-7.801, 219.11507), (-11.196, 219.48272), (-11.196, 219.20272)]</t>
         </is>
       </c>
     </row>
@@ -2627,7 +2627,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>[(-0.3, 220.0), (-0.3, 219.86), (-9.188, 220.0), (-9.188, 219.86), (-9.188, 220.0), (-9.188, 219.71), (-12.555, 220.0), (-12.555, 219.71), (-0.3, 219.86), (-0.3, 219.69), (-9.188, 219.86), (-9.188, 219.56), (-9.188, 219.71), (-9.188, 219.56), (-12.555, 219.71), (-12.555, 219.42)]</t>
+          <t>[(-0.3, 220.0), (-0.3, 219.86), (-9.188, 220.62216), (-9.188, 220.48216000000002), (-9.188, 220.62216), (-9.188, 220.33216000000002), (-12.555, 220.85785), (-12.555, 220.56785000000002), (-0.3, 219.86), (-0.3, 219.69), (-9.188, 220.48216000000002), (-9.188, 220.18216), (-9.188, 220.33216000000002), (-9.188, 220.18216), (-12.555, 220.56785000000002), (-12.555, 220.27785)]</t>
         </is>
       </c>
     </row>
@@ -2637,7 +2637,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>[(-0.3, 221.0), (-0.3, 220.76), (-10.073, 221.0), (-10.073, 220.76), (-10.073, 221.0), (-10.073, 220.76), (-13.47, 221.0), (-13.47, 220.76), (-0.3, 220.76), (-0.3, 220.53), (-10.073, 220.76), (-10.073, 220.64), (-10.073, 220.76), (-10.073, 220.64), (-13.47, 220.76), (-13.47, 220.53)]</t>
+          <t>[(-0.3, 221.0), (-0.3, 220.76), (-10.073, 221.68411), (-10.073, 221.44411), (-10.073, 221.68411), (-10.073, 221.44411), (-13.47, 221.9219), (-13.47, 221.68189999999998), (-0.3, 220.76), (-0.3, 220.53), (-10.073, 221.44411), (-10.073, 221.32411), (-10.073, 221.44411), (-10.073, 221.32411), (-13.47, 221.68189999999998), (-13.47, 221.4519)]</t>
         </is>
       </c>
     </row>
@@ -2857,7 +2857,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>[(-0.3, 243.0), (-0.3, 242.85), (-3.224, 243.0), (-3.224, 242.85), (-3.224, 243.0), (-3.224, 242.83), (-9.022, 243.0), (-9.022, 242.83), (-0.3, 242.85), (-0.3, 242.71), (-3.224, 242.85), (-3.224, 242.7), (-3.224, 242.83), (-3.224, 242.7), (-9.022, 242.83), (-9.022, 242.66)]</t>
+          <t>[(-0.3, 243.0), (-0.3, 242.85), (-3.224, 242.97603312978836), (-3.224, 242.82603312978836), (-3.224, 242.97603312978836), (-3.224, 242.80603312978837), (-9.022, 242.92850921956708), (-9.022, 242.7585092195671), (-0.3, 242.85), (-0.3, 242.71), (-3.224, 242.82603312978836), (-3.224, 242.67603312978835), (-3.224, 242.80603312978837), (-3.224, 242.67603312978835), (-9.022, 242.7585092195671), (-9.022, 242.58850921956707)]</t>
         </is>
       </c>
     </row>
@@ -2867,7 +2867,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>[(-0.3, 244.0), (-0.3, 243.83), (-3.053, 244.0), (-3.053, 243.83), (-3.053, 244.0), (-3.053, 243.77), (-9.943, 244.0), (-9.943, 243.77), (-0.3, 243.83), (-0.3, 243.67), (-3.053, 243.83), (-3.053, 243.66), (-3.053, 243.77), (-3.053, 243.66), (-9.943, 243.77), (-9.943, 243.47)]</t>
+          <t>[(-0.3, 244.0), (-0.3, 243.83), (-3.053, 244.0344342511686), (-3.053, 243.8644342511686), (-3.053, 244.0344342511686), (-3.053, 243.8044342511686), (-9.943, 244.12061368834682), (-9.943, 243.89061368834683), (-0.3, 243.83), (-0.3, 243.67), (-3.053, 243.8644342511686), (-3.053, 243.6944342511686), (-3.053, 243.8044342511686), (-3.053, 243.6944342511686), (-9.943, 243.89061368834683), (-9.943, 243.59061368834682)]</t>
         </is>
       </c>
     </row>
@@ -2877,7 +2877,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>[(-0.3, 245.0), (-0.3, 244.83), (-2.817, 245.0), (-2.817, 244.83), (-2.817, 245.0), (-2.817, 244.83), (-9.696, 245.0), (-9.696, 244.73), (-0.3, 244.83), (-0.3, 244.69), (-2.817, 244.83), (-2.817, 244.66), (-2.817, 244.83), (-2.817, 244.66), (-9.696, 244.73), (-9.696, 244.46)]</t>
+          <t>[(-0.3, 245.0), (-0.3, 244.83), (-2.817, 245.0778240497055), (-2.817, 244.9078240497055), (-2.817, 245.0778240497055), (-2.817, 244.9078240497055), (-9.696, 245.290518383406), (-9.696, 245.020518383406), (-0.3, 244.83), (-0.3, 244.69), (-2.817, 244.9078240497055), (-2.817, 244.7378240497055), (-2.817, 244.9078240497055), (-2.817, 244.7378240497055), (-9.696, 245.020518383406), (-9.696, 244.75051838340602)]</t>
         </is>
       </c>
     </row>
@@ -2887,7 +2887,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>[(-0.3, 246.0), (-0.3, 245.84), (-2.868, 246.0), (-2.868, 245.84), (-2.868, 246.0), (-2.868, 245.81), (-9.652, 246.0), (-9.652, 245.81), (-0.3, 245.84), (-0.3, 245.73), (-2.868, 245.84), (-2.868, 245.68), (-2.868, 245.81), (-2.868, 245.68), (-9.652, 245.81), (-9.652, 245.51)]</t>
+          <t>[(-0.3, 246.0), (-0.3, 245.84), (-2.868, 246.1177244070659), (-2.868, 245.9577244070659), (-2.868, 246.1177244070659), (-2.868, 245.9277244070659), (-9.652, 246.4287222176325), (-9.652, 246.2387222176325), (-0.3, 245.84), (-0.3, 245.73), (-2.868, 245.9577244070659), (-2.868, 245.7977244070659), (-2.868, 245.9277244070659), (-2.868, 245.7977244070659), (-9.652, 246.2387222176325), (-9.652, 245.9387222176325)]</t>
         </is>
       </c>
     </row>
@@ -2927,7 +2927,7 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>[(-0.3, 250.0), (-0.3, 249.89), (-3.599, 250.0), (-3.599, 249.89), (-3.599, 250.0), (-3.599, 249.79), (-7.357, 250.0), (-7.357, 249.79), (-0.3, 249.89), (-0.3, 249.74), (-3.599, 249.89), (-3.599, 249.67), (-3.599, 249.79), (-3.599, 249.67), (-7.357, 249.79), (-7.357, 249.59)]</t>
+          <t>[(-0.3, 250.0), (-0.3, 249.89), (-3.599, 250.23093), (-3.599, 250.12093), (-3.599, 250.23093), (-3.599, 250.02093), (-7.357, 250.49399), (-7.357, 250.28399), (-0.3, 249.89), (-0.3, 249.74), (-3.599, 250.12093), (-3.599, 249.90093), (-3.599, 250.02093), (-3.599, 249.90093), (-7.357, 250.28399), (-7.357, 250.08399)]</t>
         </is>
       </c>
     </row>
@@ -2937,7 +2937,7 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>[(-0.3, 251.0), (-0.3, 250.79), (-3.931, 251.0), (-3.931, 250.79), (-3.931, 251.0), (-3.931, 250.71), (-11.377, 251.0), (-11.377, 250.71), (-0.3, 250.79), (-0.3, 250.63), (-3.931, 250.79), (-3.931, 250.58), (-3.931, 250.71), (-3.931, 250.58), (-11.377, 250.71), (-11.377, 250.42)]</t>
+          <t>[(-0.3, 251.0), (-0.3, 250.79), (-3.931, 251.25417), (-3.931, 251.04416999999998), (-3.931, 251.25417), (-3.931, 250.96417), (-11.377, 251.77539), (-11.377, 251.48539), (-0.3, 250.79), (-0.3, 250.63), (-3.931, 251.04416999999998), (-3.931, 250.83417), (-3.931, 250.96417), (-3.931, 250.83417), (-11.377, 251.48539), (-11.377, 251.19538999999997)]</t>
         </is>
       </c>
     </row>
@@ -2947,7 +2947,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>[(-0.3, 252.0), (-0.3, 251.85), (-4.19, 252.0), (-4.19, 251.85), (-4.19, 252.0), (-4.19, 251.85), (-7.959, 252.0), (-7.959, 251.85), (-0.3, 251.85), (-0.3, 251.7), (-4.19, 251.85), (-4.19, 251.7), (-4.19, 251.85), (-4.19, 251.7), (-7.959, 251.85), (-7.959, 251.7), (-0.3, 251.7), (-0.3, 251.55), (-4.19, 251.7), (-4.19, 251.56), (-4.19, 251.7), (-4.19, 251.56), (-7.959, 251.7), (-7.959, 251.56)]</t>
+          <t>[(-0.3, 252.0), (-0.3, 251.85), (-4.19, 252.2017708578057), (-4.19, 252.0517708578057), (-4.19, 252.2017708578057), (-4.19, 252.0517708578057), (-7.959, 252.39726555268226), (-7.959, 252.24726555268225), (-0.3, 251.85), (-0.3, 251.7), (-4.19, 252.0517708578057), (-4.19, 251.9017708578057), (-4.19, 252.0517708578057), (-4.19, 251.9017708578057), (-7.959, 252.24726555268225), (-7.959, 252.09726555268225), (-0.3, 251.7), (-0.3, 251.55), (-4.19, 251.9017708578057), (-4.19, 251.76177085780571), (-4.19, 251.9017708578057), (-4.19, 251.76177085780571), (-7.959, 252.09726555268225), (-7.959, 251.95726555268226)]</t>
         </is>
       </c>
     </row>
@@ -2957,7 +2957,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>[(-0.3, 253.0), (-0.3, 252.83), (-5.084, 253.0), (-5.084, 252.83), (-5.084, 253.0), (-5.084, 252.85), (-8.801, 253.0), (-8.801, 252.85), (-0.3, 252.83), (-0.3, 252.66), (-5.084, 252.83), (-5.084, 252.66), (-5.084, 252.85), (-5.084, 252.7), (-8.801, 252.85), (-8.801, 252.7), (-0.3, 252.66), (-0.3, 252.51), (-5.084, 252.66), (-5.084, 252.55), (-5.084, 252.7), (-5.084, 252.55), (-8.801, 252.7), (-8.801, 252.56)]</t>
+          <t>[(-0.3, 253.0), (-0.3, 252.83), (-5.084, 253.15003449126203), (-5.084, 252.98003449126205), (-5.084, 253.15003449126203), (-5.084, 253.00003449126203), (-8.801, 253.26660602220286), (-8.801, 253.11660602220286), (-0.3, 252.83), (-0.3, 252.66), (-5.084, 252.98003449126205), (-5.084, 252.81003449126203), (-5.084, 253.00003449126203), (-5.084, 252.85003449126202), (-8.801, 253.11660602220286), (-8.801, 252.96660602220285), (-0.3, 252.66), (-0.3, 252.51), (-5.084, 252.81003449126203), (-5.084, 252.70003449126204), (-5.084, 252.85003449126202), (-5.084, 252.70003449126204), (-8.801, 252.96660602220285), (-8.801, 252.82660602220287)]</t>
         </is>
       </c>
     </row>
@@ -2967,7 +2967,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>[(-0.3, 254.0), (-0.3, 253.79), (-5.837, 254.0), (-5.837, 253.79), (-5.837, 254.0), (-5.837, 253.82), (-9.608, 254.0), (-9.608, 253.82), (-0.3, 253.79), (-0.3, 253.59), (-5.837, 253.79), (-5.837, 253.64), (-5.837, 253.82), (-5.837, 253.64), (-9.608, 253.82), (-9.608, 253.65)]</t>
+          <t>[(-0.3, 254.0), (-0.3, 253.79), (-5.837, 254.06010044961215), (-5.837, 253.85010044961214), (-5.837, 254.06010044961215), (-5.837, 253.88010044961214), (-9.608, 254.10103214466136), (-9.608, 253.92103214466135), (-0.3, 253.79), (-0.3, 253.59), (-5.837, 253.85010044961214), (-5.837, 253.70010044961214), (-5.837, 253.88010044961214), (-5.837, 253.70010044961214), (-9.608, 253.92103214466135), (-9.608, 253.75103214466137)]</t>
         </is>
       </c>
     </row>
@@ -2977,7 +2977,7 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>[(-0.3, 255.0), (-0.3, 254.84), (-6.327, 255.0), (-6.327, 254.84), (-6.327, 255.0), (-6.327, 254.85), (-10.119, 255.0), (-10.119, 254.85), (-0.3, 254.84), (-0.3, 254.69), (-6.327, 254.84), (-6.327, 254.72), (-6.327, 254.85), (-6.327, 254.72), (-10.119, 254.85), (-10.119, 254.74)]</t>
+          <t>[(-0.3, 255.0), (-0.3, 254.84), (-6.327, 254.97155252502202), (-6.327, 254.81155252502202), (-6.327, 254.97155252502202), (-6.327, 254.821552525022), (-10.119, 254.95365426301495), (-10.119, 254.80365426301495), (-0.3, 254.84), (-0.3, 254.69), (-6.327, 254.81155252502202), (-6.327, 254.69155252502202), (-6.327, 254.821552525022), (-6.327, 254.69155252502202), (-10.119, 254.80365426301495), (-10.119, 254.69365426301496)]</t>
         </is>
       </c>
     </row>
@@ -2987,7 +2987,7 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>[(-0.3, 256.0), (-0.3, 255.84), (-6.895, 256.0), (-6.895, 255.84), (-6.895, 256.0), (-6.895, 255.84), (-10.601, 256.0), (-10.601, 255.84), (-0.3, 255.84), (-0.3, 255.69), (-6.895, 255.84), (-6.895, 255.7), (-6.895, 255.84), (-6.895, 255.7), (-10.601, 255.84), (-10.601, 255.69)]</t>
+          <t>[(-0.3, 256.0), (-0.3, 255.84), (-6.895, 255.90274089406148), (-6.895, 255.74274089406148), (-6.895, 255.90274089406148), (-6.895, 255.74274089406148), (-10.601, 255.8480870280102), (-10.601, 255.68808702801022), (-0.3, 255.84), (-0.3, 255.69), (-6.895, 255.74274089406148), (-6.895, 255.60274089406147), (-6.895, 255.74274089406148), (-6.895, 255.60274089406147), (-10.601, 255.68808702801022), (-10.601, 255.5380870280102)]</t>
         </is>
       </c>
     </row>
@@ -2997,7 +2997,7 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>[(-0.3, 257.0), (-0.3, 256.79), (-7.551, 257.0), (-7.551, 256.79), (-7.551, 257.0), (-7.551, 256.79), (-11.175, 257.0), (-11.175, 256.79), (-0.3, 256.79), (-0.3, 256.59), (-7.551, 256.79), (-7.551, 256.62), (-7.551, 256.79), (-7.551, 256.62), (-11.175, 256.79), (-11.175, 256.59)]</t>
+          <t>[(-0.3, 257.0), (-0.3, 256.79), (-7.551, 256.8203579608199), (-7.551, 256.6103579608199), (-7.551, 256.8203579608199), (-7.551, 256.6103579608199), (-11.175, 256.73057410342244), (-11.175, 256.52057410342246), (-0.3, 256.79), (-0.3, 256.59), (-7.551, 256.6103579608199), (-7.551, 256.4403579608199), (-7.551, 256.6103579608199), (-7.551, 256.4403579608199), (-11.175, 256.52057410342246), (-11.175, 256.3205741034224)]</t>
         </is>
       </c>
     </row>
@@ -3007,7 +3007,7 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>[(-0.3, 258.0), (-0.3, 257.78), (-8.147, 258.0), (-8.147, 257.78), (-8.147, 258.0), (-8.147, 257.82), (-11.826, 258.0), (-11.826, 257.82), (-0.3, 257.78), (-0.3, 257.57), (-8.147, 257.78), (-8.147, 257.65), (-8.147, 257.82), (-8.147, 257.65), (-11.826, 257.82), (-11.826, 257.69)]</t>
+          <t>[(-0.3, 258.0), (-0.3, 257.78), (-8.147, 257.7269072171917), (-8.147, 257.50690721719167), (-8.147, 257.7269072171917), (-8.147, 257.5469072171917), (-11.826, 257.5988699611765), (-11.826, 257.4188699611765), (-0.3, 257.78), (-0.3, 257.57), (-8.147, 257.50690721719167), (-8.147, 257.3769072171917), (-8.147, 257.5469072171917), (-8.147, 257.3769072171917), (-11.826, 257.4188699611765), (-11.826, 257.2888699611765)]</t>
         </is>
       </c>
     </row>
@@ -3017,7 +3017,7 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>[(-0.3, 259.0), (-0.3, 258.8), (-8.681, 259.0), (-8.681, 258.8), (-8.681, 259.0), (-8.681, 258.89), (-12.316, 259.0), (-12.316, 258.89), (-0.3, 258.8), (-0.3, 258.6), (-8.681, 258.8), (-8.681, 258.69), (-8.681, 258.89), (-8.681, 258.69), (-12.316, 258.89), (-12.316, 258.75)]</t>
+          <t>[(-0.3, 259.0), (-0.3, 258.8), (-8.681, 258.62428325338135), (-8.681, 258.42428325338136), (-8.681, 258.62428325338135), (-8.681, 258.51428325338134), (-12.316, 258.4613277141905), (-12.316, 258.35132771419046), (-0.3, 258.8), (-0.3, 258.6), (-8.681, 258.42428325338136), (-8.681, 258.31428325338135), (-8.681, 258.51428325338134), (-8.681, 258.31428325338135), (-12.316, 258.35132771419046), (-12.316, 258.2113277141905)]</t>
         </is>
       </c>
     </row>
@@ -3027,7 +3027,7 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>[(-0.3, 260.0), (-0.3, 259.76), (-8.606, 260.0), (-8.606, 259.76), (-8.606, 260.0), (-8.606, 259.82), (-12.32, 260.0), (-12.32, 259.82), (-0.3, 259.76), (-0.3, 259.53), (-8.606, 259.76), (-8.606, 259.65), (-8.606, 259.82), (-8.606, 259.65), (-12.32, 259.82), (-12.32, 259.71)]</t>
+          <t>[(-0.3, 260.0), (-0.3, 259.76), (-8.606, 259.54435793231255), (-8.606, 259.30435793231254), (-8.606, 259.54435793231255), (-8.606, 259.36435793231254), (-12.32, 259.34061911225587), (-12.32, 259.16061911225586), (-0.3, 259.76), (-0.3, 259.53), (-8.606, 259.30435793231254), (-8.606, 259.1943579323125), (-8.606, 259.36435793231254), (-8.606, 259.1943579323125), (-12.32, 259.16061911225586), (-12.32, 259.05061911225584)]</t>
         </is>
       </c>
     </row>
@@ -3037,7 +3037,7 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>[(-0.3, 261.0), (-0.3, 260.71), (-8.556, 261.0), (-8.556, 260.71), (-8.556, 261.0), (-8.556, 260.8), (-12.298, 261.0), (-12.298, 260.8), (-0.3, 260.71), (-0.3, 260.42), (-8.556, 260.71), (-8.556, 260.6), (-8.556, 260.8), (-8.556, 260.6), (-12.298, 260.8), (-12.298, 260.65)]</t>
+          <t>[(-0.3, 261.0), (-0.3, 260.71), (-8.556, 260.4643146110987), (-8.556, 260.1743146110987), (-8.556, 260.4643146110987), (-8.556, 260.2643146110987), (-12.298, 260.22151728487916), (-12.298, 260.02151728487917), (-0.3, 260.71), (-0.3, 260.42), (-8.556, 260.1743146110987), (-8.556, 260.0643146110987), (-8.556, 260.2643146110987), (-8.556, 260.0643146110987), (-12.298, 260.02151728487917), (-12.298, 259.87151728487913)]</t>
         </is>
       </c>
     </row>
@@ -3047,7 +3047,7 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>[(-0.3, 262.0), (-0.3, 261.67), (-8.125, 262.0), (-8.125, 261.74), (-8.125, 262.0), (-8.125, 261.83), (-12.034, 262.0), (-12.034, 261.83), (-0.3, 261.67), (-0.3, 261.34), (-8.125, 261.74), (-8.125, 261.48), (-8.125, 261.83), (-8.125, 261.66), (-12.034, 261.83), (-12.034, 261.66)]</t>
+          <t>[(-0.3, 262.0), (-0.3, 261.67), (-8.125, 261.45225), (-8.125, 261.19225), (-8.125, 261.45225), (-8.125, 261.28225), (-12.034, 261.17862), (-12.034, 261.00862), (-0.3, 261.67), (-0.3, 261.34), (-8.125, 261.19225), (-8.125, 260.93225), (-8.125, 261.28225), (-8.125, 261.11225), (-12.034, 261.00862), (-12.034, 260.83862000000005)]</t>
         </is>
       </c>
     </row>
@@ -3057,7 +3057,7 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>[(-0.3, 263.0), (-0.3, 262.66), (-7.604, 263.0), (-7.604, 262.72), (-7.604, 263.0), (-7.604, 262.81), (-11.496, 263.0), (-11.496, 262.81), (-0.3, 262.66), (-0.3, 262.32), (-7.604, 262.72), (-7.604, 262.44), (-7.604, 262.81), (-7.604, 262.62), (-11.496, 262.81), (-11.496, 262.62)]</t>
+          <t>[(-0.3, 263.0), (-0.3, 262.66), (-7.604, 262.48872), (-7.604, 262.20872), (-7.604, 262.48872), (-7.604, 262.29872), (-11.496, 262.21628), (-11.496, 262.02628), (-0.3, 262.66), (-0.3, 262.32), (-7.604, 262.20872), (-7.604, 261.92872), (-7.604, 262.29872), (-7.604, 262.10872), (-11.496, 262.02628), (-11.496, 261.83628)]</t>
         </is>
       </c>
     </row>
@@ -3067,7 +3067,7 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>[(-0.3, 264.0), (-0.3, 263.7), (-6.979, 264.0), (-6.979, 263.7), (-6.979, 264.0), (-6.979, 263.84), (-10.837, 264.0), (-10.837, 263.84), (-0.3, 263.7), (-0.3, 263.41), (-6.979, 263.7), (-6.979, 263.52), (-6.979, 263.84), (-6.979, 263.68), (-10.837, 263.84), (-10.837, 263.68)]</t>
+          <t>[(-0.3, 264.0), (-0.3, 263.7), (-6.979, 263.53247), (-6.979, 263.23247), (-6.979, 263.53247), (-6.979, 263.37246999999996), (-10.837, 263.26241), (-10.837, 263.10240999999996), (-0.3, 263.7), (-0.3, 263.41), (-6.979, 263.23247), (-6.979, 263.05246999999997), (-6.979, 263.37246999999996), (-6.979, 263.21247), (-10.837, 263.10240999999996), (-10.837, 262.94241)]</t>
         </is>
       </c>
     </row>
@@ -3087,7 +3087,7 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>[(-0.3, 266.0), (-0.3, 265.75), (-6.725, 266.0), (-6.725, 265.75), (-6.725, 266.0), (-6.725, 265.82), (-10.403, 266.0), (-10.403, 265.82), (-0.3, 265.75), (-0.3, 265.5), (-6.725, 265.75), (-6.725, 265.64), (-6.725, 265.82), (-6.725, 265.64), (-10.403, 265.82), (-10.403, 265.7)]</t>
+          <t>[(-0.3, 266.0), (-0.3, 265.75), (-6.725, 265.55025), (-6.725, 265.30025), (-6.725, 265.55025), (-6.725, 265.37025), (-10.403, 265.29279), (-10.403, 265.11279), (-0.3, 265.75), (-0.3, 265.5), (-6.725, 265.30025), (-6.725, 265.19025), (-6.725, 265.37025), (-6.725, 265.19025), (-10.403, 265.11279), (-10.403, 264.99279)]</t>
         </is>
       </c>
     </row>
@@ -3097,7 +3097,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>[(-0.3, 267.0), (-0.3, 266.71), (-6.746, 267.0), (-6.746, 266.71), (-6.746, 267.0), (-6.746, 266.75), (-10.553, 267.0), (-10.553, 266.75), (-0.3, 266.71), (-0.3, 266.42), (-6.746, 266.71), (-6.746, 266.5), (-6.746, 266.75), (-6.746, 266.5), (-10.553, 266.75), (-10.553, 266.56)]</t>
+          <t>[(-0.3, 267.0), (-0.3, 266.71), (-6.746, 266.54878), (-6.746, 266.25878), (-6.746, 266.54878), (-6.746, 266.29878), (-10.553, 266.28229), (-10.553, 266.03229), (-0.3, 266.71), (-0.3, 266.42), (-6.746, 266.25878), (-6.746, 266.04878), (-6.746, 266.29878), (-6.746, 266.04878), (-10.553, 266.03229), (-10.553, 265.84229)]</t>
         </is>
       </c>
     </row>
@@ -3107,7 +3107,7 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>[(-0.3, 268.0), (-0.3, 267.8), (-6.694, 268.0), (-6.694, 267.8), (-6.694, 268.0), (-6.694, 267.83), (-10.486, 268.0), (-10.486, 267.83), (-0.3, 267.8), (-0.3, 267.6), (-6.694, 267.8), (-6.694, 267.6), (-6.694, 267.83), (-6.694, 267.66), (-10.486, 267.83), (-10.486, 267.66), (-0.3, 267.6), (-0.3, 267.4), (-6.694, 267.6), (-6.694, 267.49), (-6.694, 267.66), (-6.694, 267.49), (-10.486, 267.66), (-10.486, 267.54)]</t>
+          <t>[(-0.3, 268.0), (-0.3, 267.8), (-6.694, 267.55242), (-6.694, 267.35242), (-6.694, 267.55242), (-6.694, 267.38241999999997), (-10.486, 267.28698), (-10.486, 267.11698), (-0.3, 267.8), (-0.3, 267.6), (-6.694, 267.35242), (-6.694, 267.15242), (-6.694, 267.38241999999997), (-6.694, 267.21242), (-10.486, 267.11698), (-10.486, 266.94698000000005), (-0.3, 267.6), (-0.3, 267.4), (-6.694, 267.15242), (-6.694, 267.04242), (-6.694, 267.21242), (-6.694, 267.04242), (-10.486, 266.94698000000005), (-10.486, 266.82698000000005)]</t>
         </is>
       </c>
     </row>
@@ -3117,7 +3117,7 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>[(-0.3, 269.0), (-0.3, 268.82), (-6.61, 269.0), (-6.61, 268.82), (-6.61, 269.0), (-6.61, 268.76), (-10.361, 269.0), (-10.361, 268.76), (-0.3, 268.82), (-0.3, 268.64), (-6.61, 268.82), (-6.61, 268.64), (-6.61, 268.76), (-6.61, 268.52), (-10.361, 268.76), (-10.361, 268.58), (-0.3, 268.64), (-0.3, 268.46), (-6.61, 268.64), (-6.61, 268.52), (-6.61, 268.52), (-6.61, 268.52), (-10.361, 268.58), (-10.361, 268.58)]</t>
+          <t>[(-0.3, 269.0), (-0.3, 268.82), (-6.61, 268.5583), (-6.61, 268.37829999999997), (-6.61, 268.5583), (-6.61, 268.31829999999997), (-10.361, 268.29573), (-10.361, 268.05573), (-0.3, 268.82), (-0.3, 268.64), (-6.61, 268.37829999999997), (-6.61, 268.19829999999996), (-6.61, 268.31829999999997), (-6.61, 268.07829999999996), (-10.361, 268.05573), (-10.361, 267.87573), (-0.3, 268.64), (-0.3, 268.46), (-6.61, 268.19829999999996), (-6.61, 268.07829999999996), (-6.61, 268.07829999999996), (-6.61, 268.07829999999996), (-10.361, 267.87573), (-10.361, 267.87573)]</t>
         </is>
       </c>
     </row>
@@ -3127,7 +3127,7 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>[(-0.3, 270.0), (-0.3, 269.77), (-5.972, 270.0), (-5.972, 269.77), (-5.972, 270.0), (-5.972, 269.8), (-9.945, 270.0), (-9.945, 269.8), (-0.3, 269.77), (-0.3, 269.55), (-5.972, 269.77), (-5.972, 269.61), (-5.972, 269.8), (-5.972, 269.61), (-9.945, 269.8), (-9.945, 269.67)]</t>
+          <t>[(-0.3, 270.0), (-0.3, 269.77), (-5.972, 269.60296), (-5.972, 269.37296), (-5.972, 269.60296), (-5.972, 269.40296), (-9.945, 269.32485), (-9.945, 269.12485000000004), (-0.3, 269.77), (-0.3, 269.55), (-5.972, 269.37296), (-5.972, 269.21296), (-5.972, 269.40296), (-5.972, 269.21296), (-9.945, 269.12485000000004), (-9.945, 268.99485000000004)]</t>
         </is>
       </c>
     </row>
@@ -3137,7 +3137,7 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>[(-0.3, 271.0), (-0.3, 270.8), (-5.101, 271.0), (-5.101, 270.8), (-5.101, 271.0), (-5.101, 270.82), (-8.92, 271.0), (-8.92, 270.82), (-0.3, 270.8), (-0.3, 270.6), (-5.101, 270.8), (-5.101, 270.65), (-5.101, 270.82), (-5.101, 270.65), (-8.92, 270.82), (-8.92, 270.71)]</t>
+          <t>[(-0.3, 271.0), (-0.3, 270.8), (-5.101, 270.66393), (-5.101, 270.46393), (-5.101, 270.66393), (-5.101, 270.48393), (-8.92, 270.3966), (-8.92, 270.21659999999997), (-0.3, 270.8), (-0.3, 270.6), (-5.101, 270.46393), (-5.101, 270.31392999999997), (-5.101, 270.48393), (-5.101, 270.31392999999997), (-8.92, 270.21659999999997), (-8.92, 270.10659999999996)]</t>
         </is>
       </c>
     </row>
@@ -3147,7 +3147,7 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>[(-0.3, 272.0), (-0.3, 271.8), (-4.282, 272.0), (-4.282, 271.8), (-4.282, 272.0), (-4.282, 271.89), (-7.976, 272.0), (-7.976, 271.89), (-0.3, 271.8), (-0.3, 271.61), (-4.282, 271.8), (-4.282, 271.68), (-4.282, 271.89), (-4.282, 271.68), (-7.976, 271.89), (-7.976, 271.74)]</t>
+          <t>[(-0.3, 272.0), (-0.3, 271.8), (-4.282, 271.72126), (-4.282, 271.52126), (-4.282, 271.72126), (-4.282, 271.61125999999996), (-7.976, 271.46268), (-7.976, 271.35267999999996), (-0.3, 271.8), (-0.3, 271.61), (-4.282, 271.52126), (-4.282, 271.40126), (-4.282, 271.61125999999996), (-4.282, 271.40126), (-7.976, 271.35267999999996), (-7.976, 271.20268)]</t>
         </is>
       </c>
     </row>
@@ -3157,7 +3157,7 @@
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>[(-0.3, 273.0), (-0.3, 272.83), (-3.183, 273.0), (-3.183, 272.83), (-3.183, 273.0), (-3.183, 272.85), (-6.948, 273.0), (-6.948, 272.85), (-0.3, 272.83), (-0.3, 272.66), (-3.183, 272.83), (-3.183, 272.7), (-3.183, 272.85), (-3.183, 272.7), (-6.948, 272.85), (-6.948, 272.73)]</t>
+          <t>[(-0.3, 273.0), (-0.3, 272.83), (-3.183, 272.8088881494139), (-3.183, 272.6388881494139), (-3.183, 272.8088881494139), (-3.183, 272.65888814941394), (-6.948, 272.55930919781605), (-6.948, 272.40930919781607), (-0.3, 272.83), (-0.3, 272.66), (-3.183, 272.6388881494139), (-3.183, 272.5088881494139), (-3.183, 272.65888814941394), (-3.183, 272.5088881494139), (-6.948, 272.40930919781607), (-6.948, 272.28930919781607)]</t>
         </is>
       </c>
     </row>
@@ -3177,7 +3177,7 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>[(-0.3, 275.0), (-0.3, 274.87), (-4.864, 275.0), (-4.864, 274.87), (-0.3, 274.87), (-0.3, 274.74), (-4.864, 274.87), (-4.864, 274.74), (-0.3, 274.74), (-0.3, 274.63), (-4.864, 274.74), (-4.864, 274.63)]</t>
+          <t>[(-0.3, 275.0), (-0.3, 274.87), (-4.864, 274.75985439099463), (-4.864, 274.62985439099464), (-0.3, 274.87), (-0.3, 274.74), (-4.864, 274.62985439099464), (-4.864, 274.49985439099464), (-0.3, 274.74), (-0.3, 274.63), (-4.864, 274.49985439099464), (-4.864, 274.3898543909946)]</t>
         </is>
       </c>
     </row>
@@ -3187,7 +3187,7 @@
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>[(-0.3, 276.0), (-0.3, 275.8), (-4.198, 276.0), (-4.198, 275.8), (-0.3, 275.8), (-0.3, 275.62), (-4.198, 275.8), (-4.198, 275.6)]</t>
+          <t>[(-0.3, 276.0), (-0.3, 275.8), (-4.198, 275.8215440339142), (-4.198, 275.62154403391423), (-0.3, 275.8), (-0.3, 275.62), (-4.198, 275.62154403391423), (-4.198, 275.42154403391424)]</t>
         </is>
       </c>
     </row>
@@ -3197,7 +3197,7 @@
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>[(-0.3, 277.0), (-0.3, 276.84), (-3.617, 277.0), (-3.617, 276.84), (-0.3, 276.84), (-0.3, 276.68), (-3.617, 276.84), (-3.617, 276.68), (-0.3, 276.68), (-0.3, 276.55), (-3.617, 276.68), (-3.617, 276.53)]</t>
+          <t>[(-0.3, 277.0), (-0.3, 276.84), (-3.617, 276.8708178422692), (-3.617, 276.7108178422692), (-0.3, 276.84), (-0.3, 276.68), (-3.617, 276.7108178422692), (-3.617, 276.5508178422692), (-0.3, 276.68), (-0.3, 276.55), (-3.617, 276.5508178422692), (-3.617, 276.4008178422692)]</t>
         </is>
       </c>
     </row>
@@ -3207,7 +3207,7 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>[(-0.3, 278.0), (-0.3, 277.82), (-3.264, 278.0), (-3.264, 277.82), (-0.3, 277.82), (-0.3, 277.64), (-3.264, 277.82), (-3.264, 277.64), (-0.3, 277.64), (-0.3, 277.5), (-3.264, 277.64), (-3.264, 277.46)]</t>
+          <t>[(-0.3, 278.0), (-0.3, 277.82), (-3.264, 277.90482731552), (-3.264, 277.72482731552), (-0.3, 277.82), (-0.3, 277.64), (-3.264, 277.72482731552), (-3.264, 277.54482731551997), (-0.3, 277.64), (-0.3, 277.5), (-3.264, 277.54482731551997), (-3.264, 277.36482731551996)]</t>
         </is>
       </c>
     </row>
@@ -3217,7 +3217,7 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>[(-0.3, 279.0), (-0.3, 278.79), (-3.209, 279.0), (-3.209, 278.79), (-0.3, 278.79), (-0.3, 278.58), (-3.209, 278.79), (-3.209, 278.58), (-0.3, 278.58), (-0.3, 278.43), (-3.209, 278.58), (-3.209, 278.39)]</t>
+          <t>[(-0.3, 279.0), (-0.3, 278.79), (-3.209, 278.9264790825544), (-3.209, 278.71647908255443), (-0.3, 278.79), (-0.3, 278.58), (-3.209, 278.71647908255443), (-3.209, 278.5064790825544), (-0.3, 278.58), (-0.3, 278.43), (-3.209, 278.5064790825544), (-3.209, 278.3164790825544)]</t>
         </is>
       </c>
     </row>
@@ -3227,7 +3227,7 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>[(-0.3, 280.0), (-0.3, 279.76), (-3.332, 280.0), (-3.332, 279.76), (-0.3, 279.76), (-0.3, 279.52), (-3.332, 279.76), (-3.332, 279.52), (-0.3, 279.52), (-0.3, 279.36), (-3.332, 279.52), (-3.332, 279.29)]</t>
+          <t>[(-0.3, 280.0), (-0.3, 279.76), (-3.332, 279.97557525354165), (-3.332, 279.73557525354164), (-0.3, 279.76), (-0.3, 279.52), (-3.332, 279.73557525354164), (-3.332, 279.49557525354163), (-0.3, 279.52), (-0.3, 279.36), (-3.332, 279.49557525354163), (-3.332, 279.26557525354167)]</t>
         </is>
       </c>
     </row>
@@ -3237,7 +3237,7 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>[(-0.3, 281.0), (-0.3, 280.75), (-3.387, 281.0), (-3.387, 280.75), (-0.3, 280.75), (-0.3, 280.5), (-3.387, 280.75), (-3.387, 280.5), (-0.3, 280.5), (-0.3, 280.34), (-3.387, 280.5), (-3.387, 280.26)]</t>
+          <t>[(-0.3, 281.0), (-0.3, 280.75), (-3.387, 281.02962024354105), (-3.387, 280.77962024354105), (-0.3, 280.75), (-0.3, 280.5), (-3.387, 280.77962024354105), (-3.387, 280.52962024354105), (-0.3, 280.5), (-0.3, 280.34), (-3.387, 280.52962024354105), (-3.387, 280.28962024354104)]</t>
         </is>
       </c>
     </row>
@@ -3247,7 +3247,7 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>[(-0.3, 282.0), (-0.3, 281.75), (-3.34, 282.0), (-3.34, 281.75), (-0.3, 281.75), (-0.3, 281.5), (-3.34, 281.75), (-3.34, 281.5), (-0.3, 281.5), (-0.3, 281.36), (-3.34, 281.5), (-3.34, 281.27)]</t>
+          <t>[(-0.3, 282.0), (-0.3, 281.75), (-3.34, 282.0867889340757), (-3.34, 281.8367889340757), (-0.3, 281.75), (-0.3, 281.5), (-3.34, 281.8367889340757), (-3.34, 281.5867889340757), (-0.3, 281.5), (-0.3, 281.36), (-3.34, 281.5867889340757), (-3.34, 281.35678893407567)]</t>
         </is>
       </c>
     </row>
@@ -3257,7 +3257,7 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>[(-0.3, 283.0), (-0.3, 282.8), (-3.153, 283.0), (-3.153, 282.8), (-0.3, 282.8), (-0.3, 282.6), (-3.153, 282.8), (-3.153, 282.6), (-0.3, 282.6), (-0.3, 282.4), (-3.153, 282.6), (-3.153, 282.4), (-0.3, 282.4), (-0.3, 282.29), (-3.153, 282.4), (-3.153, 282.23)]</t>
+          <t>[(-0.3, 283.0), (-0.3, 282.8), (-3.153, 283.1610237522136), (-3.153, 282.96102375221363), (-0.3, 282.8), (-0.3, 282.6), (-3.153, 282.96102375221363), (-3.153, 282.76102375221365), (-0.3, 282.6), (-0.3, 282.4), (-3.153, 282.76102375221365), (-3.153, 282.5610237522136), (-0.3, 282.4), (-0.3, 282.29), (-3.153, 282.5610237522136), (-3.153, 282.39102375221364)]</t>
         </is>
       </c>
     </row>
@@ -3267,7 +3267,7 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>[(-0.3, 284.0), (-0.3, 283.75), (-2.809, 284.0), (-2.809, 283.75), (-0.3, 283.75), (-0.3, 283.5), (-2.809, 283.75), (-2.809, 283.5), (-0.3, 283.5), (-0.3, 283.36), (-2.809, 283.5), (-2.809, 283.27)]</t>
+          <t>[(-0.3, 284.0), (-0.3, 283.75), (-2.809, 284.17563), (-2.809, 283.92563), (-0.3, 283.75), (-0.3, 283.5), (-2.809, 283.92563), (-2.809, 283.67563), (-0.3, 283.5), (-0.3, 283.36), (-2.809, 283.67563), (-2.809, 283.44563)]</t>
         </is>
       </c>
     </row>
@@ -3277,7 +3277,7 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>[(-0.3, 285.0), (-0.3, 284.77), (-2.587, 285.0), (-2.587, 284.77), (-0.3, 284.77), (-0.3, 284.54), (-2.587, 284.77), (-2.587, 284.54), (-0.3, 284.54), (-0.3, 284.4), (-2.587, 284.54), (-2.587, 284.33)]</t>
+          <t>[(-0.3, 285.0), (-0.3, 284.77), (-2.587, 285.16009), (-2.587, 284.93009), (-0.3, 284.77), (-0.3, 284.54), (-2.587, 284.93009), (-2.587, 284.70009000000005), (-0.3, 284.54), (-0.3, 284.4), (-2.587, 284.70009000000005), (-2.587, 284.49009)]</t>
         </is>
       </c>
     </row>
@@ -3287,7 +3287,7 @@
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>[(-0.3, 286.0), (-0.3, 285.77), (-2.332, 286.0), (-2.332, 285.77), (-0.3, 285.77), (-0.3, 285.54), (-2.332, 285.77), (-2.332, 285.54), (-0.3, 285.54), (-0.3, 285.4), (-2.332, 285.54), (-2.332, 285.33)]</t>
+          <t>[(-0.3, 286.0), (-0.3, 285.77), (-2.332, 286.14224), (-2.332, 285.91224), (-0.3, 285.77), (-0.3, 285.54), (-2.332, 285.91224), (-2.332, 285.68224000000004), (-0.3, 285.54), (-0.3, 285.4), (-2.332, 285.68224000000004), (-2.332, 285.47224)]</t>
         </is>
       </c>
     </row>
@@ -3337,7 +3337,7 @@
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>[(-0.3, 291.0), (-0.3, 290.8), (-2.383, 291.0), (-2.383, 290.8), (-0.3, 290.8), (-0.3, 290.61), (-2.383, 290.8), (-2.383, 290.66)]</t>
+          <t>[(-0.3, 291.0), (-0.3, 290.8), (-2.383, 290.8686552714), (-2.383, 290.6686552714), (-0.3, 290.8), (-0.3, 290.61), (-2.383, 290.6686552714), (-2.383, 290.5286552714)]</t>
         </is>
       </c>
     </row>
@@ -3357,7 +3357,7 @@
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>[(-0.3, 293.0), (-0.3, 292.84), (-2.637, 293.0), (-2.637, 292.84), (-0.3, 292.84), (-0.3, 292.69), (-2.637, 292.84), (-2.637, 292.71)]</t>
+          <t>[(-0.3, 293.0), (-0.3, 292.84), (-2.637, 292.83641), (-2.637, 292.67641), (-0.3, 292.84), (-0.3, 292.69), (-2.637, 292.67641), (-2.637, 292.54641)]</t>
         </is>
       </c>
     </row>
@@ -3367,7 +3367,7 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>[(-0.3, 294.0), (-0.3, 293.84), (-2.775, 294.0), (-2.775, 293.84), (-0.3, 293.84), (-0.3, 293.68), (-2.775, 293.84), (-2.775, 293.71)]</t>
+          <t>[(-0.3, 294.0), (-0.3, 293.84), (-2.775, 293.82675), (-2.775, 293.66675), (-0.3, 293.84), (-0.3, 293.68), (-2.775, 293.66675), (-2.775, 293.53675)]</t>
         </is>
       </c>
     </row>
@@ -3377,7 +3377,7 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>[(-0.3, 295.0), (-0.3, 294.82), (-2.84, 295.0), (-2.84, 294.82), (-0.3, 294.82), (-0.3, 294.65), (-2.84, 294.82), (-2.84, 294.67)]</t>
+          <t>[(-0.3, 295.0), (-0.3, 294.82), (-2.84, 294.8222), (-2.84, 294.6422), (-0.3, 294.82), (-0.3, 294.65), (-2.84, 294.6422), (-2.84, 294.4922)]</t>
         </is>
       </c>
     </row>
@@ -3387,7 +3387,7 @@
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>[(-0.3, 296.0), (-0.3, 295.8), (-2.912, 296.0), (-2.912, 295.8), (-0.3, 295.8), (-0.3, 295.6), (-2.912, 295.8), (-2.912, 295.64)]</t>
+          <t>[(-0.3, 296.0), (-0.3, 295.8), (-2.912, 295.8424308753054), (-2.912, 295.6424308753054), (-0.3, 295.8), (-0.3, 295.6), (-2.912, 295.6424308753054), (-2.912, 295.4824308753054)]</t>
         </is>
       </c>
     </row>
@@ -3397,7 +3397,7 @@
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>[(-0.3, 297.0), (-0.3, 296.85), (-3.01, 297.0), (-3.01, 296.85), (-0.3, 296.85), (-0.3, 296.7), (-3.01, 296.85), (-3.01, 296.7), (-0.3, 296.7), (-0.3, 296.57), (-3.01, 296.7), (-3.01, 296.58)]</t>
+          <t>[(-0.3, 297.0), (-0.3, 296.85), (-3.01, 296.9053266548737), (-3.01, 296.7553266548737), (-0.3, 296.85), (-0.3, 296.7), (-3.01, 296.7553266548737), (-3.01, 296.6053266548737), (-0.3, 296.7), (-0.3, 296.57), (-3.01, 296.6053266548737), (-3.01, 296.4853266548737)]</t>
         </is>
       </c>
     </row>
@@ -3407,7 +3407,7 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>[(-0.3, 298.0), (-0.3, 297.82), (-2.908, 298.0), (-2.908, 297.82), (-0.3, 297.82), (-0.3, 297.64), (-2.908, 297.82), (-2.908, 297.64), (-0.3, 297.64), (-0.3, 297.5), (-2.908, 297.64), (-2.908, 297.48)]</t>
+          <t>[(-0.3, 298.0), (-0.3, 297.82), (-2.908, 297.97510783609266), (-2.908, 297.79510783609265), (-0.3, 297.82), (-0.3, 297.64), (-2.908, 297.79510783609265), (-2.908, 297.61510783609265), (-0.3, 297.64), (-0.3, 297.5), (-2.908, 297.61510783609265), (-2.908, 297.4551078360927)]</t>
         </is>
       </c>
     </row>
@@ -3417,7 +3417,7 @@
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>[(-0.3, 299.0), (-0.3, 298.83), (-2.859, 299.0), (-2.859, 298.83), (-0.3, 298.83), (-0.3, 298.66), (-2.859, 298.83), (-2.859, 298.66), (-0.3, 298.66), (-0.3, 298.53), (-2.859, 298.66), (-2.859, 298.5)]</t>
+          <t>[(-0.3, 299.0), (-0.3, 298.83), (-2.859, 299.02169509896345), (-2.859, 298.85169509896343), (-0.3, 298.83), (-0.3, 298.66), (-2.859, 298.85169509896343), (-2.859, 298.6816950989635), (-0.3, 298.66), (-0.3, 298.53), (-2.859, 298.6816950989635), (-2.859, 298.52169509896345)]</t>
         </is>
       </c>
     </row>
@@ -3427,7 +3427,7 @@
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>[(-0.3, 300.0), (-0.3, 299.82), (-2.716, 300.0), (-2.716, 299.82), (-0.3, 299.82), (-0.3, 299.64), (-2.716, 299.82), (-2.716, 299.64), (-0.3, 299.64), (-0.3, 299.51), (-2.716, 299.64), (-2.716, 299.46)]</t>
+          <t>[(-0.3, 300.0), (-0.3, 299.82), (-2.716, 300.0533031122713), (-2.716, 299.8733031122713), (-0.3, 299.82), (-0.3, 299.64), (-2.716, 299.8733031122713), (-2.716, 299.6933031122713), (-0.3, 299.64), (-0.3, 299.51), (-2.716, 299.6933031122713), (-2.716, 299.5133031122713)]</t>
         </is>
       </c>
     </row>
@@ -3437,7 +3437,7 @@
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>[(-0.3, 301.0), (-0.3, 300.82), (-2.574, 301.0), (-2.574, 300.82), (-0.3, 300.82), (-0.3, 300.64), (-2.574, 300.82), (-2.574, 300.64), (-0.3, 300.64), (-0.3, 300.5), (-2.574, 300.64), (-2.574, 300.46)]</t>
+          <t>[(-0.3, 301.0), (-0.3, 300.82), (-2.574, 301.08106158090635), (-2.574, 300.90106158090634), (-0.3, 300.82), (-0.3, 300.64), (-2.574, 300.90106158090634), (-2.574, 300.72106158090634), (-0.3, 300.64), (-0.3, 300.5), (-2.574, 300.72106158090634), (-2.574, 300.54106158090633)]</t>
         </is>
       </c>
     </row>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>[(-0.3, 302.0), (-0.3, 301.78), (-2.465, 302.0), (-2.465, 301.78), (-0.3, 301.78), (-0.3, 301.56), (-2.465, 301.78), (-2.465, 301.56), (-0.3, 301.56), (-0.3, 301.42), (-2.465, 301.56), (-2.465, 301.36)]</t>
+          <t>[(-0.3, 302.0), (-0.3, 301.78), (-2.465, 302.10658667366687), (-2.465, 301.88658667366684), (-0.3, 301.78), (-0.3, 301.56), (-2.465, 301.88658667366684), (-2.465, 301.66658667366687), (-0.3, 301.56), (-0.3, 301.42), (-2.465, 301.66658667366687), (-2.465, 301.4665866736669)]</t>
         </is>
       </c>
     </row>
@@ -4247,7 +4247,7 @@
       </c>
       <c r="B383" t="inlineStr">
         <is>
-          <t>[(-0.3, 382.0), (-0.3, 381.88), (-2.403, 382.0), (-2.403, 381.88), (-0.3, 381.88), (-0.3, 381.76), (-2.403, 381.88), (-2.403, 381.76), (-0.3, 381.76), (-0.3, 381.65), (-2.403, 381.76), (-2.403, 381.65)]</t>
+          <t>[(-0.3, 382.0), (-0.3, 381.88), (-2.403, 381.85827593933175), (-2.403, 381.73827593933174), (-0.3, 381.88), (-0.3, 381.76), (-2.403, 381.73827593933174), (-2.403, 381.61827593933174), (-0.3, 381.76), (-0.3, 381.65), (-2.403, 381.61827593933174), (-2.403, 381.5082759393317)]</t>
         </is>
       </c>
     </row>
@@ -4257,7 +4257,7 @@
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>[(-0.3, 383.0), (-0.3, 382.86), (-2.438, 383.0), (-2.438, 382.86), (-0.3, 382.86), (-0.3, 382.72), (-2.438, 382.86), (-2.438, 382.72), (-0.3, 382.72), (-0.3, 382.61), (-2.438, 382.72), (-2.438, 382.61)]</t>
+          <t>[(-0.3, 383.0), (-0.3, 382.86), (-2.438, 382.8770834411549), (-2.438, 382.73708344115494), (-0.3, 382.86), (-0.3, 382.72), (-2.438, 382.73708344115494), (-2.438, 382.59708344115495), (-0.3, 382.72), (-0.3, 382.61), (-2.438, 382.59708344115495), (-2.438, 382.48708344115494)]</t>
         </is>
       </c>
     </row>
@@ -4817,7 +4817,7 @@
       </c>
       <c r="B440" t="inlineStr">
         <is>
-          <t>[(-0.3, 439.0), (-0.3, 438.83), (-4.836, 439.0), (-4.836, 438.83), (-0.3, 438.83), (-0.3, 438.69), (-4.836, 438.83), (-4.836, 438.66)]</t>
+          <t>[(-0.3, 439.0), (-0.3, 438.83), (-4.836, 438.8098424565933), (-4.836, 438.63984245659327), (-0.3, 438.83), (-0.3, 438.69), (-4.836, 438.63984245659327), (-4.836, 438.4698424565933)]</t>
         </is>
       </c>
     </row>
@@ -4827,7 +4827,7 @@
       </c>
       <c r="B441" t="inlineStr">
         <is>
-          <t>[(-0.3, 440.0), (-0.3, 439.83), (-2.75, 440.0), (-2.75, 439.83), (-0.3, 439.83), (-0.3, 439.68), (-2.75, 439.83), (-2.75, 439.66)]</t>
+          <t>[(-0.3, 440.0), (-0.3, 439.83), (-2.75, 439.91079145032046), (-2.75, 439.74079145032044), (-0.3, 439.83), (-0.3, 439.68), (-2.75, 439.74079145032044), (-2.75, 439.5707914503205)]</t>
         </is>
       </c>
     </row>
@@ -4837,7 +4837,7 @@
       </c>
       <c r="B442" t="inlineStr">
         <is>
-          <t>[(-0.3, 441.0), (-0.3, 440.83), (-4.523, 441.0), (-4.523, 440.83), (-0.3, 440.83), (-0.3, 440.69), (-4.523, 440.83), (-4.523, 440.67)]</t>
+          <t>[(-0.3, 441.0), (-0.3, 440.83), (-4.523, 440.8695031815115), (-4.523, 440.6995031815115), (-0.3, 440.83), (-0.3, 440.69), (-4.523, 440.6995031815115), (-4.523, 440.5395031815115)]</t>
         </is>
       </c>
     </row>
@@ -4847,7 +4847,7 @@
       </c>
       <c r="B443" t="inlineStr">
         <is>
-          <t>[(-0.3, 442.0), (-0.3, 441.83), (-5.604, 442.0), (-5.604, 441.83), (-0.3, 441.83), (-0.3, 441.67), (-5.604, 441.83), (-5.604, 441.67)]</t>
+          <t>[(-0.3, 442.0), (-0.3, 441.83), (-5.604, 441.865324837755), (-5.604, 441.695324837755), (-0.3, 441.83), (-0.3, 441.67), (-5.604, 441.695324837755), (-5.604, 441.535324837755)]</t>
         </is>
       </c>
     </row>
@@ -4857,7 +4857,7 @@
       </c>
       <c r="B444" t="inlineStr">
         <is>
-          <t>[(-0.3, 443.0), (-0.3, 442.81), (-6.634, 443.0), (-6.634, 442.81), (-0.3, 442.81), (-0.3, 442.64), (-6.634, 442.81), (-6.634, 442.63)]</t>
+          <t>[(-0.3, 443.0), (-0.3, 442.81), (-6.634, 442.84165), (-6.634, 442.65165), (-0.3, 442.81), (-0.3, 442.64), (-6.634, 442.65165), (-6.634, 442.47165)]</t>
         </is>
       </c>
     </row>
@@ -4867,7 +4867,7 @@
       </c>
       <c r="B445" t="inlineStr">
         <is>
-          <t>[(-0.3, 444.0), (-0.3, 443.86), (-2.622, 444.0), (-2.622, 443.86), (-0.3, 443.86), (-0.3, 443.72), (-2.622, 443.86), (-2.622, 443.72), (-0.3, 443.72), (-0.3, 443.61), (-2.622, 443.72), (-2.622, 443.61)]</t>
+          <t>[(-0.3, 444.0), (-0.3, 443.86), (-2.622, 443.94195), (-2.622, 443.80195000000003), (-0.3, 443.86), (-0.3, 443.72), (-2.622, 443.80195000000003), (-2.622, 443.66195000000005), (-0.3, 443.72), (-0.3, 443.61), (-2.622, 443.66195000000005), (-2.622, 443.55195000000003)]</t>
         </is>
       </c>
     </row>
@@ -4877,7 +4877,7 @@
       </c>
       <c r="B446" t="inlineStr">
         <is>
-          <t>[(-0.3, 445.0), (-0.3, 444.87), (-3.713, 445.0), (-3.713, 444.87), (-0.3, 444.87), (-0.3, 444.74), (-3.713, 444.87), (-3.713, 444.74), (-0.3, 444.74), (-0.3, 444.63), (-3.713, 444.74), (-3.713, 444.62)]</t>
+          <t>[(-0.3, 445.0), (-0.3, 444.87), (-3.713, 444.914675), (-3.713, 444.784675), (-0.3, 444.87), (-0.3, 444.74), (-3.713, 444.784675), (-3.713, 444.654675), (-0.3, 444.74), (-0.3, 444.63), (-3.713, 444.654675), (-3.713, 444.534675)]</t>
         </is>
       </c>
     </row>
@@ -4887,7 +4887,7 @@
       </c>
       <c r="B447" t="inlineStr">
         <is>
-          <t>[(-0.3, 446.0), (-0.3, 445.83), (-5.03, 446.0), (-5.03, 445.83), (-0.3, 445.83), (-0.3, 445.66), (-5.03, 445.83), (-5.03, 445.66)]</t>
+          <t>[(-0.3, 446.0), (-0.3, 445.83), (-5.03, 445.88175), (-5.03, 445.71175), (-0.3, 445.83), (-0.3, 445.66), (-5.03, 445.71175), (-5.03, 445.54175000000004)]</t>
         </is>
       </c>
     </row>
@@ -4897,7 +4897,7 @@
       </c>
       <c r="B448" t="inlineStr">
         <is>
-          <t>[(-0.3, 447.0), (-0.3, 446.8), (-5.47, 447.0), (-5.47, 446.8), (-0.3, 446.8), (-0.3, 446.61), (-5.47, 446.8), (-5.47, 446.63)]</t>
+          <t>[(-0.3, 447.0), (-0.3, 446.8), (-5.47, 446.87075), (-5.47, 446.67075), (-0.3, 446.8), (-0.3, 446.61), (-5.47, 446.67075), (-5.47, 446.50075)]</t>
         </is>
       </c>
     </row>
@@ -4907,7 +4907,7 @@
       </c>
       <c r="B449" t="inlineStr">
         <is>
-          <t>[(-0.3, 448.0), (-0.3, 447.86), (-5.501, 448.0), (-5.501, 447.86), (-0.3, 447.86), (-0.3, 447.56), (-5.501, 447.86), (-5.501, 447.7)]</t>
+          <t>[(-0.3, 448.0), (-0.3, 447.86), (-5.501, 447.869975), (-5.501, 447.729975), (-0.3, 447.86), (-0.3, 447.56), (-5.501, 447.729975), (-5.501, 447.569975)]</t>
         </is>
       </c>
     </row>
@@ -4917,7 +4917,7 @@
       </c>
       <c r="B450" t="inlineStr">
         <is>
-          <t>[(-0.3, 449.0), (-0.3, 448.85), (-8.746, 449.0), (-8.746, 448.85), (-0.3, 448.85), (-0.3, 448.7), (-8.746, 448.85), (-8.746, 448.7), (-0.3, 448.7), (-0.3, 448.55), (-8.746, 448.7), (-8.746, 448.56)]</t>
+          <t>[(-0.3, 449.0), (-0.3, 448.85), (-8.746, 448.78885), (-8.746, 448.63885000000005), (-0.3, 448.85), (-0.3, 448.7), (-8.746, 448.63885000000005), (-8.746, 448.48885), (-0.3, 448.7), (-0.3, 448.55), (-8.746, 448.48885), (-8.746, 448.34885)]</t>
         </is>
       </c>
     </row>
@@ -4927,7 +4927,7 @@
       </c>
       <c r="B451" t="inlineStr">
         <is>
-          <t>[(-0.3, 450.0), (-0.3, 449.79), (-7.23, 450.0), (-7.23, 449.79), (-0.3, 449.79), (-0.3, 449.58), (-7.23, 449.79), (-7.23, 449.64)]</t>
+          <t>[(-0.3, 450.0), (-0.3, 449.79), (-7.23, 449.82675), (-7.23, 449.61675), (-0.3, 449.79), (-0.3, 449.58), (-7.23, 449.61675), (-7.23, 449.46675)]</t>
         </is>
       </c>
     </row>
@@ -4937,7 +4937,7 @@
       </c>
       <c r="B452" t="inlineStr">
         <is>
-          <t>[(-0.3, 451.0), (-0.3, 450.81), (-6.067, 451.0), (-6.067, 450.81), (-0.3, 450.81), (-0.3, 450.62), (-6.067, 450.81), (-6.067, 450.65)]</t>
+          <t>[(-0.3, 451.0), (-0.3, 450.81), (-6.067, 450.855825), (-6.067, 450.665825), (-0.3, 450.81), (-0.3, 450.62), (-6.067, 450.665825), (-6.067, 450.50582499999996)]</t>
         </is>
       </c>
     </row>
@@ -4947,7 +4947,7 @@
       </c>
       <c r="B453" t="inlineStr">
         <is>
-          <t>[(-0.3, 452.0), (-0.3, 451.82), (-6.353, 452.0), (-6.353, 451.82), (-0.3, 451.82), (-0.3, 451.65), (-6.353, 451.82), (-6.353, 451.69)]</t>
+          <t>[(-0.3, 452.0), (-0.3, 451.82), (-6.353, 451.848675), (-6.353, 451.668675), (-0.3, 451.82), (-0.3, 451.65), (-6.353, 451.668675), (-6.353, 451.538675)]</t>
         </is>
       </c>
     </row>
@@ -4957,7 +4957,7 @@
       </c>
       <c r="B454" t="inlineStr">
         <is>
-          <t>[(-0.3, 453.0), (-0.3, 452.84), (-6.671, 453.0), (-6.671, 452.84), (-0.3, 452.84), (-0.3, 452.68), (-6.671, 452.84), (-6.671, 452.71)]</t>
+          <t>[(-0.3, 453.0), (-0.3, 452.84), (-6.671, 452.840725), (-6.671, 452.680725), (-0.3, 452.84), (-0.3, 452.68), (-6.671, 452.680725), (-6.671, 452.550725)]</t>
         </is>
       </c>
     </row>
@@ -4967,7 +4967,7 @@
       </c>
       <c r="B455" t="inlineStr">
         <is>
-          <t>[(-0.3, 454.0), (-0.3, 453.84), (-6.993, 454.0), (-6.993, 453.84), (-0.3, 453.84), (-0.3, 453.68), (-6.993, 453.84), (-6.993, 453.71)]</t>
+          <t>[(-0.3, 454.0), (-0.3, 453.84), (-6.993, 453.832675), (-6.993, 453.67267499999997), (-0.3, 453.84), (-0.3, 453.68), (-6.993, 453.67267499999997), (-6.993, 453.542675)]</t>
         </is>
       </c>
     </row>
@@ -4977,7 +4977,7 @@
       </c>
       <c r="B456" t="inlineStr">
         <is>
-          <t>[(-0.3, 455.0), (-0.3, 454.82), (-7.248, 455.0), (-7.248, 454.82), (-0.3, 454.82), (-0.3, 454.64), (-7.248, 454.82), (-7.248, 454.68)]</t>
+          <t>[(-0.3, 455.0), (-0.3, 454.82), (-7.248, 454.8263), (-7.248, 454.6463), (-0.3, 454.82), (-0.3, 454.64), (-7.248, 454.6463), (-7.248, 454.5063)]</t>
         </is>
       </c>
     </row>
@@ -4987,7 +4987,7 @@
       </c>
       <c r="B457" t="inlineStr">
         <is>
-          <t>[(-0.3, 456.0), (-0.3, 455.83), (-7.525, 456.0), (-7.525, 455.83), (-0.3, 455.83), (-0.3, 455.66), (-7.525, 455.83), (-7.525, 455.71)]</t>
+          <t>[(-0.3, 456.0), (-0.3, 455.83), (-7.525, 455.819375), (-7.525, 455.64937499999996), (-0.3, 455.83), (-0.3, 455.66), (-7.525, 455.64937499999996), (-7.525, 455.52937499999996)]</t>
         </is>
       </c>
     </row>
@@ -4997,7 +4997,7 @@
       </c>
       <c r="B458" t="inlineStr">
         <is>
-          <t>[(-0.3, 457.0), (-0.3, 456.8), (-7.834, 457.0), (-7.834, 456.8), (-0.3, 456.8), (-0.3, 456.6), (-7.834, 456.8), (-7.834, 456.67)]</t>
+          <t>[(-0.3, 457.0), (-0.3, 456.8), (-7.834, 456.81165), (-7.834, 456.61165), (-0.3, 456.8), (-0.3, 456.6), (-7.834, 456.61165), (-7.834, 456.48165)]</t>
         </is>
       </c>
     </row>
@@ -5007,7 +5007,7 @@
       </c>
       <c r="B459" t="inlineStr">
         <is>
-          <t>[(-0.3, 458.0), (-0.3, 457.89), (-8.13, 458.0), (-8.13, 457.89), (-0.3, 457.89), (-0.3, 457.62), (-8.13, 457.89), (-8.13, 457.71)]</t>
+          <t>[(-0.3, 458.0), (-0.3, 457.89), (-8.13, 457.80425), (-8.13, 457.69425), (-0.3, 457.89), (-0.3, 457.62), (-8.13, 457.69425), (-8.13, 457.51425)]</t>
         </is>
       </c>
     </row>
@@ -5027,7 +5027,7 @@
       </c>
       <c r="B461" t="inlineStr">
         <is>
-          <t>[(-0.3, 460.0), (-0.3, 459.84), (-8.559, 460.0), (-8.559, 459.84), (-0.3, 459.84), (-0.3, 459.68), (-8.559, 459.84), (-8.559, 459.71)]</t>
+          <t>[(-0.3, 460.0), (-0.3, 459.84), (-8.559, 460.1209384210791), (-8.559, 459.96093842107905), (-0.3, 459.84), (-0.3, 459.68), (-8.559, 459.96093842107905), (-8.559, 459.83093842107905)]</t>
         </is>
       </c>
     </row>
@@ -5037,7 +5037,7 @@
       </c>
       <c r="B462" t="inlineStr">
         <is>
-          <t>[(-0.3, 461.0), (-0.3, 460.81), (-8.777, 461.0), (-8.777, 460.81), (-0.3, 460.81), (-0.3, 460.67), (-8.777, 460.81), (-8.777, 460.63)]</t>
+          <t>[(-0.3, 461.0), (-0.3, 460.81), (-8.777, 461.2525008251755), (-8.777, 461.0625008251755), (-0.3, 460.81), (-0.3, 460.67), (-8.777, 461.0625008251755), (-8.777, 460.8825008251755)]</t>
         </is>
       </c>
     </row>
@@ -5067,7 +5067,7 @@
       </c>
       <c r="B465" t="inlineStr">
         <is>
-          <t>[(-0.3, 464.0), (-0.3, 463.85), (-2.353, 464.0), (-2.353, 463.85), (-2.353, 464.0), (-2.353, 463.89), (-9.118, 464.0), (-9.118, 463.89), (-0.3, 463.85), (-0.3, 463.74), (-2.353, 463.85), (-2.353, 463.72), (-2.353, 463.89), (-2.353, 463.72), (-9.118, 463.89), (-9.118, 463.62)]</t>
+          <t>[(-0.3, 464.0), (-0.3, 463.85), (-2.353, 464.11148319347427), (-2.353, 463.9614831934743), (-2.353, 464.11148319347427), (-2.353, 464.00148319347426), (-9.118, 464.4788401364131), (-9.118, 464.3688401364131), (-0.3, 463.85), (-0.3, 463.74), (-2.353, 463.9614831934743), (-2.353, 463.8314831934743), (-2.353, 464.00148319347426), (-2.353, 463.8314831934743), (-9.118, 464.3688401364131), (-9.118, 464.0988401364131)]</t>
         </is>
       </c>
     </row>
@@ -5077,7 +5077,7 @@
       </c>
       <c r="B466" t="inlineStr">
         <is>
-          <t>[(-0.3, 465.0), (-0.3, 464.85), (-2.525, 465.0), (-2.525, 464.85), (-2.525, 465.0), (-2.525, 464.87), (-9.207, 465.0), (-9.207, 464.87), (-0.3, 464.85), (-0.3, 464.74), (-2.525, 464.85), (-2.525, 464.72), (-2.525, 464.87), (-2.525, 464.72), (-9.207, 464.87), (-9.207, 464.57)]</t>
+          <t>[(-0.3, 465.0), (-0.3, 464.85), (-2.525, 465.13900593696064), (-2.525, 464.98900593696067), (-2.525, 465.13900593696064), (-2.525, 465.00900593696065), (-9.207, 465.5564610698915), (-9.207, 465.4264610698915), (-0.3, 464.85), (-0.3, 464.74), (-2.525, 464.98900593696067), (-2.525, 464.85900593696067), (-2.525, 465.00900593696065), (-2.525, 464.85900593696067), (-9.207, 465.4264610698915), (-9.207, 465.1264610698915)]</t>
         </is>
       </c>
     </row>
@@ -5117,7 +5117,7 @@
       </c>
       <c r="B470" t="inlineStr">
         <is>
-          <t>[(-0.3, 469.0), (-0.3, 468.84), (-3.597, 469.0), (-3.597, 468.84), (-3.597, 469.0), (-3.597, 468.86), (-10.382, 469.0), (-10.382, 468.86), (-0.3, 468.84), (-0.3, 468.72), (-3.597, 468.84), (-3.597, 468.68), (-3.597, 468.86), (-3.597, 468.68), (-10.382, 468.86), (-10.382, 468.56)]</t>
+          <t>[(-0.3, 469.0), (-0.3, 468.84), (-3.597, 469.23079), (-3.597, 469.07079), (-3.597, 469.23079), (-3.597, 469.09079), (-10.382, 469.70574), (-10.382, 469.56574), (-0.3, 468.84), (-0.3, 468.72), (-3.597, 469.07079), (-3.597, 468.91079), (-3.597, 469.09079), (-3.597, 468.91079), (-10.382, 469.56574), (-10.382, 469.26574)]</t>
         </is>
       </c>
     </row>
@@ -5137,7 +5137,7 @@
       </c>
       <c r="B472" t="inlineStr">
         <is>
-          <t>[(-0.3, 471.0), (-0.3, 470.84), (-4.191, 471.0), (-4.191, 470.84), (-4.191, 471.0), (-4.191, 470.85), (-10.943, 471.0), (-10.943, 470.85), (-0.3, 470.84), (-0.3, 470.72), (-4.191, 470.84), (-4.191, 470.69), (-4.191, 470.85), (-4.191, 470.69), (-10.943, 470.85), (-10.943, 470.55)]</t>
+          <t>[(-0.3, 471.0), (-0.3, 470.84), (-4.191, 471.27237), (-4.191, 471.11237), (-4.191, 471.27237), (-4.191, 471.12237000000005), (-10.943, 471.74501), (-10.943, 471.59501), (-0.3, 470.84), (-0.3, 470.72), (-4.191, 471.11237), (-4.191, 470.96237), (-4.191, 471.12237000000005), (-4.191, 470.96237), (-10.943, 471.59501), (-10.943, 471.29501)]</t>
         </is>
       </c>
     </row>
@@ -5147,7 +5147,7 @@
       </c>
       <c r="B473" t="inlineStr">
         <is>
-          <t>[(-0.3, 472.0), (-0.3, 471.86), (-4.416, 472.0), (-4.416, 471.86), (-4.416, 472.0), (-4.416, 471.85), (-11.157, 472.0), (-11.157, 471.85), (-0.3, 471.86), (-0.3, 471.74), (-4.416, 471.86), (-4.416, 471.73), (-4.416, 471.85), (-4.416, 471.73), (-11.157, 471.85), (-11.157, 471.55)]</t>
+          <t>[(-0.3, 472.0), (-0.3, 471.86), (-4.416, 472.28812), (-4.416, 472.14812), (-4.416, 472.28812), (-4.416, 472.13812), (-11.157, 472.75999), (-11.157, 472.60999000000004), (-0.3, 471.86), (-0.3, 471.74), (-4.416, 472.14812), (-4.416, 472.01812), (-4.416, 472.13812), (-4.416, 472.01812), (-11.157, 472.60999000000004), (-11.157, 472.30999)]</t>
         </is>
       </c>
     </row>
@@ -5177,7 +5177,7 @@
       </c>
       <c r="B476" t="inlineStr">
         <is>
-          <t>[(-0.3, 475.0), (-0.3, 474.85), (-4.821, 475.0), (-4.821, 474.85), (-4.821, 475.0), (-4.821, 474.86), (-11.595, 475.0), (-11.595, 474.86), (-0.3, 474.85), (-0.3, 474.74), (-4.821, 474.85), (-4.821, 474.71), (-4.821, 474.86), (-4.821, 474.71), (-11.595, 474.86), (-11.595, 474.56)]</t>
+          <t>[(-0.3, 475.0), (-0.3, 474.85), (-4.821, 475.31647), (-4.821, 475.16647), (-4.821, 475.31647), (-4.821, 475.17647), (-11.595, 475.79065), (-11.595, 475.65065000000004), (-0.3, 474.85), (-0.3, 474.74), (-4.821, 475.16647), (-4.821, 475.02646999999996), (-4.821, 475.17647), (-4.821, 475.02646999999996), (-11.595, 475.65065000000004), (-11.595, 475.35065000000003)]</t>
         </is>
       </c>
     </row>
@@ -5187,7 +5187,7 @@
       </c>
       <c r="B477" t="inlineStr">
         <is>
-          <t>[(-0.3, 476.0), (-0.3, 475.85), (-4.916, 476.0), (-4.916, 475.85), (-4.916, 476.0), (-4.916, 475.89), (-11.628, 476.0), (-11.628, 475.89), (-0.3, 475.85), (-0.3, 475.74), (-4.916, 475.85), (-4.916, 475.71), (-4.916, 475.89), (-4.916, 475.71), (-11.628, 475.89), (-11.628, 475.59)]</t>
+          <t>[(-0.3, 476.0), (-0.3, 475.85), (-4.916, 476.32312), (-4.916, 476.17312000000004), (-4.916, 476.32312), (-4.916, 476.21312), (-11.628, 476.79296), (-11.628, 476.68296), (-0.3, 475.85), (-0.3, 475.74), (-4.916, 476.17312000000004), (-4.916, 476.03312), (-4.916, 476.21312), (-4.916, 476.03312), (-11.628, 476.68296), (-11.628, 476.38295999999997)]</t>
         </is>
       </c>
     </row>
@@ -5247,7 +5247,7 @@
       </c>
       <c r="B483" t="inlineStr">
         <is>
-          <t>[(-0.3, 482.0), (-0.3, 481.84), (-4.711, 482.0), (-4.711, 481.84), (-4.711, 482.0), (-4.711, 481.81), (-11.456, 482.0), (-11.456, 481.81), (-0.3, 481.84), (-0.3, 481.73), (-4.711, 481.84), (-4.711, 481.69), (-4.711, 481.81), (-4.711, 481.69), (-11.456, 481.81), (-11.456, 481.51)]</t>
+          <t>[(-0.3, 482.0), (-0.3, 481.84), (-4.711, 482.30175702402823), (-4.711, 482.1417570240282), (-4.711, 482.30175702402823), (-4.711, 482.11175702402824), (-11.456, 482.76318326004514), (-11.456, 482.57318326004514), (-0.3, 481.84), (-0.3, 481.73), (-4.711, 482.1417570240282), (-4.711, 481.99175702402823), (-4.711, 482.11175702402824), (-4.711, 481.99175702402823), (-11.456, 482.57318326004514), (-11.456, 482.27318326004513)]</t>
         </is>
       </c>
     </row>
@@ -5257,7 +5257,7 @@
       </c>
       <c r="B484" t="inlineStr">
         <is>
-          <t>[(-0.3, 483.0), (-0.3, 482.83), (-4.708, 483.0), (-4.708, 482.83), (-4.708, 483.0), (-4.708, 482.81), (-11.451, 483.0), (-11.451, 482.81), (-0.3, 482.83), (-0.3, 482.71), (-4.708, 482.83), (-4.708, 482.67), (-4.708, 482.81), (-4.708, 482.67), (-11.451, 482.81), (-11.451, 482.51)]</t>
+          <t>[(-0.3, 483.0), (-0.3, 482.83), (-4.708, 483.2655296176786), (-4.708, 483.0955296176786), (-4.708, 483.2655296176786), (-4.708, 483.0755296176786), (-11.451, 483.6717152374625), (-11.451, 483.4817152374625), (-0.3, 482.83), (-0.3, 482.71), (-4.708, 483.0955296176786), (-4.708, 482.93552961767864), (-4.708, 483.0755296176786), (-4.708, 482.93552961767864), (-11.451, 483.4817152374625), (-11.451, 483.18171523746247)]</t>
         </is>
       </c>
     </row>
@@ -5267,7 +5267,7 @@
       </c>
       <c r="B485" t="inlineStr">
         <is>
-          <t>[(-0.3, 484.0), (-0.3, 483.82), (-4.827, 484.0), (-4.827, 483.82), (-4.827, 484.0), (-4.827, 483.75), (-11.636, 484.0), (-11.636, 483.75), (-0.3, 483.82), (-0.3, 483.69), (-4.827, 483.82), (-4.827, 483.64), (-4.827, 483.75), (-4.827, 483.64), (-11.636, 483.75), (-11.636, 483.51)]</t>
+          <t>[(-0.3, 484.0), (-0.3, 483.82), (-4.827, 484.2357033095461), (-4.827, 484.0557033095461), (-4.827, 484.2357033095461), (-4.827, 483.9857033095461), (-11.636, 484.5902214970211), (-11.636, 484.3402214970211), (-0.3, 483.82), (-0.3, 483.69), (-4.827, 484.0557033095461), (-4.827, 483.8757033095461), (-4.827, 483.9857033095461), (-4.827, 483.8757033095461), (-11.636, 484.3402214970211), (-11.636, 484.1002214970211)]</t>
         </is>
       </c>
     </row>
@@ -5277,7 +5277,7 @@
       </c>
       <c r="B486" t="inlineStr">
         <is>
-          <t>[(-0.3, 485.0), (-0.3, 484.82), (-5.008, 485.0), (-5.008, 484.82), (-5.008, 485.0), (-5.008, 484.78), (-11.805, 485.0), (-11.805, 484.78), (-0.3, 484.82), (-0.3, 484.67), (-5.008, 484.82), (-5.008, 484.65), (-5.008, 484.78), (-5.008, 484.65), (-11.805, 484.78), (-11.805, 484.57)]</t>
+          <t>[(-0.3, 485.0), (-0.3, 484.82), (-5.008, 485.2066535006386), (-5.008, 485.0266535006386), (-5.008, 485.2066535006386), (-5.008, 484.98665350063857), (-11.805, 485.5050018107152), (-11.805, 485.2850018107152), (-0.3, 484.82), (-0.3, 484.67), (-5.008, 485.0266535006386), (-5.008, 484.8566535006386), (-5.008, 484.98665350063857), (-5.008, 484.8566535006386), (-11.805, 485.2850018107152), (-11.805, 485.0750018107152)]</t>
         </is>
       </c>
     </row>
@@ -5287,7 +5287,7 @@
       </c>
       <c r="B487" t="inlineStr">
         <is>
-          <t>[(-0.3, 486.0), (-0.3, 485.85), (-5.129, 486.0), (-5.129, 485.85), (-5.129, 486.0), (-5.129, 485.73), (-12.005, 486.0), (-12.005, 485.73), (-0.3, 485.85), (-0.3, 485.7), (-5.129, 485.85), (-5.129, 485.7), (-5.129, 485.73), (-5.129, 485.58), (-12.005, 485.73), (-12.005, 485.46), (-0.3, 485.7), (-0.3, 485.58), (-5.129, 485.7), (-5.129, 485.58), (-5.129, 485.58), (-5.129, 485.58), (-12.005, 485.46), (-12.005, 485.46)]</t>
+          <t>[(-0.3, 486.0), (-0.3, 485.85), (-5.129, 486.17250210073917), (-5.129, 486.0225021007392), (-5.129, 486.17250210073917), (-5.129, 485.9025021007392), (-12.005, 486.4181273740219), (-12.005, 486.1481273740219), (-0.3, 485.85), (-0.3, 485.7), (-5.129, 486.0225021007392), (-5.129, 485.87250210073915), (-5.129, 485.9025021007392), (-5.129, 485.75250210073915), (-12.005, 486.1481273740219), (-12.005, 485.87812737402186), (-0.3, 485.7), (-0.3, 485.58), (-5.129, 485.87250210073915), (-5.129, 485.75250210073915), (-5.129, 485.75250210073915), (-5.129, 485.75250210073915), (-12.005, 485.87812737402186), (-12.005, 485.87812737402186)]</t>
         </is>
       </c>
     </row>
@@ -5297,7 +5297,7 @@
       </c>
       <c r="B488" t="inlineStr">
         <is>
-          <t>[(-0.3, 487.0), (-0.3, 486.82), (-5.221, 487.0), (-5.221, 486.82), (-5.221, 487.0), (-5.221, 486.81), (-11.995, 487.0), (-11.995, 486.81), (-0.3, 486.82), (-0.3, 486.64), (-5.221, 486.82), (-5.221, 486.64), (-5.221, 486.81), (-5.221, 486.62), (-11.995, 486.81), (-11.995, 486.62), (-0.3, 486.64), (-0.3, 486.48), (-5.221, 486.64), (-5.221, 486.5), (-5.221, 486.62), (-5.221, 486.5), (-11.995, 486.62), (-11.995, 486.45)]</t>
+          <t>[(-0.3, 487.0), (-0.3, 486.82), (-5.221, 487.13557412346023), (-5.221, 486.9555741234602), (-5.221, 487.13557412346023), (-5.221, 486.94557412346023), (-11.995, 487.32219861285654), (-11.995, 487.13219861285654), (-0.3, 486.82), (-0.3, 486.64), (-5.221, 486.9555741234602), (-5.221, 486.7755741234602), (-5.221, 486.94557412346023), (-5.221, 486.75557412346024), (-11.995, 487.13219861285654), (-11.995, 486.94219861285654), (-0.3, 486.64), (-0.3, 486.48), (-5.221, 486.7755741234602), (-5.221, 486.63557412346023), (-5.221, 486.75557412346024), (-5.221, 486.63557412346023), (-11.995, 486.94219861285654), (-11.995, 486.7721986128565)]</t>
         </is>
       </c>
     </row>
@@ -5307,7 +5307,7 @@
       </c>
       <c r="B489" t="inlineStr">
         <is>
-          <t>[(-0.3, 488.0), (-0.3, 487.7), (-5.246, 488.0), (-5.246, 487.7), (-5.246, 488.0), (-5.246, 487.83), (-12.042, 488.0), (-12.042, 487.83), (-0.3, 487.7), (-0.3, 487.41), (-5.246, 487.7), (-5.246, 487.52), (-5.246, 487.83), (-5.246, 487.66), (-12.042, 487.83), (-12.042, 487.66)]</t>
+          <t>[(-0.3, 488.0), (-0.3, 487.7), (-5.246, 488.03858564725135), (-5.246, 487.73858564725134), (-5.246, 488.03858564725135), (-5.246, 487.86858564725134), (-12.042, 488.09160385564604), (-12.042, 487.921603855646), (-0.3, 487.7), (-0.3, 487.41), (-5.246, 487.73858564725134), (-5.246, 487.55858564725133), (-5.246, 487.86858564725134), (-5.246, 487.6985856472514), (-12.042, 487.921603855646), (-12.042, 487.75160385564607)]</t>
         </is>
       </c>
     </row>
@@ -5317,7 +5317,7 @@
       </c>
       <c r="B490" t="inlineStr">
         <is>
-          <t>[(-0.3, 489.0), (-0.3, 488.73), (-5.258, 489.0), (-5.258, 488.73), (-5.258, 489.0), (-5.258, 488.89), (-12.017, 489.0), (-12.017, 488.89), (-0.3, 488.73), (-0.3, 488.43), (-5.258, 488.73), (-5.258, 488.61), (-5.258, 488.89), (-5.258, 488.61), (-12.017, 488.89), (-12.017, 488.74)]</t>
+          <t>[(-0.3, 489.0), (-0.3, 488.73), (-5.258, 488.91472926386416), (-5.258, 488.6447292638642), (-5.258, 488.91472926386416), (-5.258, 488.80472926386415), (-12.017, 488.79848382103603), (-12.017, 488.688483821036), (-0.3, 488.73), (-0.3, 488.43), (-5.258, 488.6447292638642), (-5.258, 488.5247292638642), (-5.258, 488.80472926386415), (-5.258, 488.5247292638642), (-12.017, 488.688483821036), (-12.017, 488.53848382103604)]</t>
         </is>
       </c>
     </row>
@@ -5337,7 +5337,7 @@
       </c>
       <c r="B492" t="inlineStr">
         <is>
-          <t>[(-0.3, 491.0), (-0.3, 490.66), (-5.197, 491.0), (-5.197, 490.78), (-5.197, 491.0), (-5.197, 490.85), (-12.024, 491.0), (-12.024, 490.85), (-0.3, 490.66), (-0.3, 490.32), (-5.197, 490.78), (-5.197, 490.56), (-5.197, 490.85), (-5.197, 490.55), (-12.024, 490.85), (-12.024, 490.68)]</t>
+          <t>[(-0.3, 491.0), (-0.3, 490.66), (-5.197, 490.877575), (-5.197, 490.65757499999995), (-5.197, 490.877575), (-5.197, 490.727575), (-12.024, 490.7069), (-12.024, 490.55690000000004), (-0.3, 490.66), (-0.3, 490.32), (-5.197, 490.65757499999995), (-5.197, 490.437575), (-5.197, 490.727575), (-5.197, 490.427575), (-12.024, 490.55690000000004), (-12.024, 490.3869)]</t>
         </is>
       </c>
     </row>
@@ -5347,7 +5347,7 @@
       </c>
       <c r="B493" t="inlineStr">
         <is>
-          <t>[(-0.3, 492.0), (-0.3, 491.61), (-5.221, 492.0), (-5.221, 491.72), (-5.221, 492.0), (-5.221, 491.72), (-12.004, 492.0), (-12.004, 491.72), (-0.3, 491.61), (-0.3, 491.22), (-5.221, 491.72), (-5.221, 491.44), (-5.221, 491.72), (-5.221, 491.45), (-12.004, 491.72), (-12.004, 491.56)]</t>
+          <t>[(-0.3, 492.0), (-0.3, 491.61), (-5.221, 491.876975), (-5.221, 491.59697500000004), (-5.221, 491.876975), (-5.221, 491.59697500000004), (-12.004, 491.7074), (-12.004, 491.42740000000003), (-0.3, 491.61), (-0.3, 491.22), (-5.221, 491.59697500000004), (-5.221, 491.316975), (-5.221, 491.59697500000004), (-5.221, 491.326975), (-12.004, 491.42740000000003), (-12.004, 491.2674)]</t>
         </is>
       </c>
     </row>
@@ -5357,7 +5357,7 @@
       </c>
       <c r="B494" t="inlineStr">
         <is>
-          <t>[(-0.3, 493.0), (-0.3, 492.55), (-5.159, 493.0), (-5.159, 492.68), (-5.159, 493.0), (-5.159, 492.79), (-11.984, 493.0), (-11.984, 492.79), (-0.3, 492.55), (-0.3, 492.1), (-5.159, 492.68), (-5.159, 492.36), (-5.159, 492.79), (-5.159, 492.58), (-11.984, 492.79), (-11.984, 492.58)]</t>
+          <t>[(-0.3, 493.0), (-0.3, 492.55), (-5.159, 492.878525), (-5.159, 492.55852500000003), (-5.159, 492.878525), (-5.159, 492.66852500000005), (-11.984, 492.7079), (-11.984, 492.4979), (-0.3, 492.55), (-0.3, 492.1), (-5.159, 492.55852500000003), (-5.159, 492.23852500000004), (-5.159, 492.66852500000005), (-5.159, 492.458525), (-11.984, 492.4979), (-11.984, 492.2879)]</t>
         </is>
       </c>
     </row>
@@ -5367,7 +5367,7 @@
       </c>
       <c r="B495" t="inlineStr">
         <is>
-          <t>[(-0.3, 494.0), (-0.3, 493.5), (-5.114, 494.0), (-5.114, 493.6), (-5.114, 494.0), (-5.114, 493.73), (-11.935, 494.0), (-11.935, 493.73), (-0.3, 493.5), (-0.3, 493.0), (-5.114, 493.6), (-5.114, 493.2), (-5.114, 493.73), (-5.114, 493.46), (-11.935, 493.73), (-11.935, 493.46)]</t>
+          <t>[(-0.3, 494.0), (-0.3, 493.5), (-5.114, 493.87965), (-5.114, 493.47965000000005), (-5.114, 493.87965), (-5.114, 493.60965000000004), (-11.935, 493.709125), (-11.935, 493.439125), (-0.3, 493.5), (-0.3, 493.0), (-5.114, 493.47965000000005), (-5.114, 493.07965), (-5.114, 493.60965000000004), (-5.114, 493.33965), (-11.935, 493.439125), (-11.935, 493.16912499999995)]</t>
         </is>
       </c>
     </row>
@@ -5377,7 +5377,7 @@
       </c>
       <c r="B496" t="inlineStr">
         <is>
-          <t>[(-0.3, 495.0), (-0.3, 494.5), (-5.078, 495.0), (-5.078, 494.58), (-5.078, 495.0), (-5.078, 494.79), (-11.886, 495.0), (-11.886, 494.79), (-0.3, 494.5), (-0.3, 494.0), (-5.078, 494.58), (-5.078, 494.16), (-5.078, 494.79), (-5.078, 494.58), (-11.886, 494.79), (-11.886, 494.58)]</t>
+          <t>[(-0.3, 495.0), (-0.3, 494.5), (-5.078, 494.88055), (-5.078, 494.46055), (-5.078, 494.88055), (-5.078, 494.67055000000005), (-11.886, 494.71035), (-11.886, 494.50035), (-0.3, 494.5), (-0.3, 494.0), (-5.078, 494.46055), (-5.078, 494.04055000000005), (-5.078, 494.67055000000005), (-5.078, 494.46055), (-11.886, 494.50035), (-11.886, 494.29035)]</t>
         </is>
       </c>
     </row>
@@ -5417,7 +5417,7 @@
       </c>
       <c r="B500" t="inlineStr">
         <is>
-          <t>[(-0.3, 499.0), (-0.3, 498.71), (-5.357, 499.0), (-5.357, 498.71), (-5.357, 499.0), (-5.357, 498.76), (-12.301, 499.0), (-12.301, 498.76), (-0.3, 498.71), (-0.3, 498.42), (-5.357, 498.71), (-5.357, 498.42), (-5.357, 498.76), (-5.357, 498.52), (-12.301, 498.76), (-12.301, 498.52), (-0.3, 498.42), (-0.3, 498.14), (-5.357, 498.42), (-5.357, 498.28), (-5.357, 498.52), (-5.357, 498.28), (-12.301, 498.52), (-12.301, 498.39)]</t>
+          <t>[(-0.3, 499.0), (-0.3, 498.71), (-5.357, 498.74285700980244), (-5.357, 498.4528570098024), (-5.357, 498.74285700980244), (-5.357, 498.5028570098024), (-12.301, 498.389762106909), (-12.301, 498.149762106909), (-0.3, 498.71), (-0.3, 498.42), (-5.357, 498.4528570098024), (-5.357, 498.16285700980245), (-5.357, 498.5028570098024), (-5.357, 498.2628570098024), (-12.301, 498.149762106909), (-12.301, 497.909762106909), (-0.3, 498.42), (-0.3, 498.14), (-5.357, 498.16285700980245), (-5.357, 498.0228570098024), (-5.357, 498.2628570098024), (-5.357, 498.0228570098024), (-12.301, 497.909762106909), (-12.301, 497.779762106909)]</t>
         </is>
       </c>
     </row>
@@ -5427,7 +5427,7 @@
       </c>
       <c r="B501" t="inlineStr">
         <is>
-          <t>[(-0.3, 500.0), (-0.3, 499.72), (-5.533, 500.0), (-5.533, 499.72), (-5.533, 500.0), (-5.533, 499.66), (-12.507, 500.0), (-12.507, 499.76), (-0.3, 499.72), (-0.3, 499.44), (-5.533, 499.72), (-5.533, 499.44), (-5.533, 499.66), (-5.533, 499.32), (-12.507, 499.76), (-12.507, 499.52), (-0.3, 499.44), (-0.3, 499.17), (-5.533, 499.44), (-5.533, 499.33), (-5.533, 499.32), (-5.533, 499.32), (-12.507, 499.52), (-12.507, 499.52)]</t>
+          <t>[(-0.3, 500.0), (-0.3, 499.72), (-5.533, 499.68160462999606), (-5.533, 499.4016046299961), (-5.533, 499.68160462999606), (-5.533, 499.3416046299961), (-12.507, 499.2572802825075), (-12.507, 499.0172802825075), (-0.3, 499.72), (-0.3, 499.44), (-5.533, 499.4016046299961), (-5.533, 499.12160462999606), (-5.533, 499.3416046299961), (-5.533, 499.00160462999605), (-12.507, 499.0172802825075), (-12.507, 498.7772802825075), (-0.3, 499.44), (-0.3, 499.17), (-5.533, 499.12160462999606), (-5.533, 499.01160462999604), (-5.533, 499.00160462999605), (-5.533, 499.00160462999605), (-12.507, 498.7772802825075), (-12.507, 498.7772802825075)]</t>
         </is>
       </c>
     </row>
@@ -5437,7 +5437,7 @@
       </c>
       <c r="B502" t="inlineStr">
         <is>
-          <t>[(-0.3, 501.0), (-0.3, 500.6), (-5.774, 501.0), (-5.774, 500.7), (-5.774, 501.0), (-5.774, 500.7), (-12.784, 501.0), (-12.784, 500.7), (-0.3, 500.6), (-0.3, 500.2), (-5.774, 500.7), (-5.774, 500.4), (-5.774, 500.7), (-5.774, 500.41), (-12.784, 500.7), (-12.784, 500.59)]</t>
+          <t>[(-0.3, 501.0), (-0.3, 500.6), (-5.774, 500.61682), (-5.774, 500.31682), (-5.774, 500.61682), (-5.774, 500.31682), (-12.784, 500.12612), (-12.784, 499.82612), (-0.3, 500.6), (-0.3, 500.2), (-5.774, 500.31682), (-5.774, 500.01682), (-5.774, 500.31682), (-5.774, 500.02682000000004), (-12.784, 499.82612), (-12.784, 499.71612)]</t>
         </is>
       </c>
     </row>
@@ -5447,7 +5447,7 @@
       </c>
       <c r="B503" t="inlineStr">
         <is>
-          <t>[(-0.3, 502.0), (-0.3, 501.65), (-5.857, 502.0), (-5.857, 501.77), (-5.857, 502.0), (-5.857, 501.77), (-12.779, 502.0), (-12.779, 501.87), (-0.3, 501.65), (-0.3, 501.3), (-5.857, 501.77), (-5.857, 501.54), (-5.857, 501.77), (-5.857, 501.54), (-12.779, 501.87), (-12.779, 501.74)]</t>
+          <t>[(-0.3, 502.0), (-0.3, 501.65), (-5.857, 501.61101), (-5.857, 501.38101), (-5.857, 501.61101), (-5.857, 501.38101), (-12.779, 501.12647), (-12.779, 500.99647), (-0.3, 501.65), (-0.3, 501.3), (-5.857, 501.38101), (-5.857, 501.15101000000004), (-5.857, 501.38101), (-5.857, 501.15101000000004), (-12.779, 500.99647), (-12.779, 500.86647)]</t>
         </is>
       </c>
     </row>
@@ -5457,7 +5457,7 @@
       </c>
       <c r="B504" t="inlineStr">
         <is>
-          <t>[(-0.3, 503.0), (-0.3, 502.68), (-5.904, 503.0), (-5.904, 502.77), (-5.904, 503.0), (-5.904, 502.77), (-12.805, 503.0), (-12.805, 502.87), (-0.3, 502.68), (-0.3, 502.36), (-5.904, 502.77), (-5.904, 502.54), (-5.904, 502.77), (-5.904, 502.54), (-12.805, 502.87), (-12.805, 502.74)]</t>
+          <t>[(-0.3, 503.0), (-0.3, 502.68), (-5.904, 502.60772), (-5.904, 502.37771999999995), (-5.904, 502.60772), (-5.904, 502.37771999999995), (-12.805, 502.12465), (-12.805, 501.99465), (-0.3, 502.68), (-0.3, 502.36), (-5.904, 502.37771999999995), (-5.904, 502.14772), (-5.904, 502.37771999999995), (-5.904, 502.14772), (-12.805, 501.99465), (-12.805, 501.86465)]</t>
         </is>
       </c>
     </row>
@@ -5467,7 +5467,7 @@
       </c>
       <c r="B505" t="inlineStr">
         <is>
-          <t>[(-0.3, 504.0), (-0.3, 503.64), (-5.981, 504.0), (-5.981, 503.76), (-5.981, 504.0), (-5.981, 503.81), (-12.864, 504.0), (-12.864, 503.81), (-0.3, 503.64), (-0.3, 503.28), (-5.981, 503.76), (-5.981, 503.52), (-5.981, 503.81), (-5.981, 503.51), (-12.864, 503.81), (-12.864, 503.65)]</t>
+          <t>[(-0.3, 504.0), (-0.3, 503.64), (-5.981, 503.60233), (-5.981, 503.36233), (-5.981, 503.60233), (-5.981, 503.41233), (-12.864, 503.12052), (-12.864, 502.93052), (-0.3, 503.64), (-0.3, 503.28), (-5.981, 503.36233), (-5.981, 503.12233), (-5.981, 503.41233), (-5.981, 503.11233), (-12.864, 502.93052), (-12.864, 502.77052)]</t>
         </is>
       </c>
     </row>
@@ -5477,7 +5477,7 @@
       </c>
       <c r="B506" t="inlineStr">
         <is>
-          <t>[(-0.3, 505.0), (-0.3, 504.66), (-5.857, 505.0), (-5.857, 504.74), (-5.857, 505.0), (-5.857, 504.74), (-12.727, 505.0), (-12.727, 504.84), (-0.3, 504.66), (-0.3, 504.32), (-5.857, 504.74), (-5.857, 504.48), (-5.857, 504.74), (-5.857, 504.48), (-12.727, 504.84), (-12.727, 504.68)]</t>
+          <t>[(-0.3, 505.0), (-0.3, 504.66), (-5.857, 504.61101), (-5.857, 504.35101000000003), (-5.857, 504.61101), (-5.857, 504.35101000000003), (-12.727, 504.13011), (-12.727, 503.97011), (-0.3, 504.66), (-0.3, 504.32), (-5.857, 504.35101000000003), (-5.857, 504.09101000000004), (-5.857, 504.35101000000003), (-5.857, 504.09101000000004), (-12.727, 503.97011), (-12.727, 503.81011)]</t>
         </is>
       </c>
     </row>
@@ -5547,7 +5547,7 @@
       </c>
       <c r="B513" t="inlineStr">
         <is>
-          <t>[(-0.3, 512.0), (-0.3, 511.89), (-4.393, 512.0), (-4.393, 511.89), (-4.393, 512.0), (-4.393, 511.85), (-11.313, 512.0), (-11.313, 511.85), (-0.3, 511.89), (-0.3, 511.63), (-4.393, 511.89), (-4.393, 511.72), (-4.393, 511.85), (-4.393, 511.72), (-11.313, 511.85), (-11.313, 511.55)]</t>
+          <t>[(-0.3, 512.0), (-0.3, 511.89), (-4.393, 511.9270935479339), (-4.393, 511.8170935479339), (-4.393, 511.9270935479339), (-4.393, 511.77709354793393), (-11.313, 511.80383123464367), (-11.313, 511.6538312346437), (-0.3, 511.89), (-0.3, 511.63), (-4.393, 511.8170935479339), (-4.393, 511.64709354793393), (-4.393, 511.77709354793393), (-4.393, 511.64709354793393), (-11.313, 511.6538312346437), (-11.313, 511.3538312346437)]</t>
         </is>
       </c>
     </row>
@@ -5557,7 +5557,7 @@
       </c>
       <c r="B514" t="inlineStr">
         <is>
-          <t>[(-0.3, 513.0), (-0.3, 512.76), (-4.237, 513.0), (-4.237, 512.76), (-4.237, 513.0), (-4.237, 512.79), (-11.169, 513.0), (-11.169, 512.69), (-0.3, 512.76), (-0.3, 512.52), (-4.237, 512.76), (-4.237, 512.58), (-4.237, 512.79), (-4.237, 512.58), (-11.169, 512.69), (-11.169, 512.38)]</t>
+          <t>[(-0.3, 513.0), (-0.3, 512.76), (-4.237, 512.9865706123701), (-4.237, 512.7465706123701), (-4.237, 512.9865706123701), (-4.237, 512.77657061237), (-11.169, 512.962925066256), (-11.169, 512.6529250662561), (-0.3, 512.76), (-0.3, 512.52), (-4.237, 512.7465706123701), (-4.237, 512.5665706123701), (-4.237, 512.77657061237), (-4.237, 512.5665706123701), (-11.169, 512.6529250662561), (-11.169, 512.342925066256)]</t>
         </is>
       </c>
     </row>
@@ -5567,7 +5567,7 @@
       </c>
       <c r="B515" t="inlineStr">
         <is>
-          <t>[(-0.3, 514.0), (-0.3, 513.73), (-4.16, 514.0), (-4.16, 513.73), (-4.16, 514.0), (-4.16, 513.77), (-11.078, 514.0), (-11.078, 513.68), (-0.3, 513.73), (-0.3, 513.47), (-4.16, 513.73), (-4.16, 513.54), (-4.16, 513.77), (-4.16, 513.54), (-11.078, 513.68), (-11.078, 513.36)]</t>
+          <t>[(-0.3, 514.0), (-0.3, 513.73), (-4.16, 514.0424226755699), (-4.16, 513.7724226755699), (-4.16, 514.0424226755699), (-4.16, 513.8124226755699), (-11.078, 514.1184537816821), (-11.078, 513.798453781682), (-0.3, 513.73), (-0.3, 513.47), (-4.16, 513.7724226755699), (-4.16, 513.5824226755699), (-4.16, 513.8124226755699), (-4.16, 513.5824226755699), (-11.078, 513.798453781682), (-11.078, 513.4784537816821)]</t>
         </is>
       </c>
     </row>
@@ -5577,7 +5577,7 @@
       </c>
       <c r="B516" t="inlineStr">
         <is>
-          <t>[(-0.3, 515.0), (-0.3, 514.85), (-4.027, 515.0), (-4.027, 514.85), (-4.027, 515.0), (-4.027, 514.72), (-10.92, 515.0), (-10.92, 514.72), (-0.3, 514.85), (-0.3, 514.7), (-4.027, 514.85), (-4.027, 514.7), (-4.027, 514.72), (-4.027, 514.57), (-10.92, 514.72), (-10.92, 514.45), (-0.3, 514.7), (-0.3, 514.58), (-4.027, 514.7), (-4.027, 514.57), (-4.027, 514.57), (-4.027, 514.57), (-10.92, 514.45), (-10.92, 514.45)]</t>
+          <t>[(-0.3, 515.0), (-0.3, 514.85), (-4.027, 515.0942611932987), (-4.027, 514.9442611932988), (-4.027, 515.0942611932987), (-4.027, 514.8142611932988), (-10.92, 515.2685950825953), (-10.92, 514.9885950825953), (-0.3, 514.85), (-0.3, 514.7), (-4.027, 514.9442611932988), (-4.027, 514.7942611932988), (-4.027, 514.8142611932988), (-4.027, 514.6642611932988), (-10.92, 514.9885950825953), (-10.92, 514.7185950825954), (-0.3, 514.7), (-0.3, 514.58), (-4.027, 514.7942611932988), (-4.027, 514.6642611932988), (-4.027, 514.6642611932988), (-4.027, 514.6642611932988), (-10.92, 514.7185950825954), (-10.92, 514.7185950825954)]</t>
         </is>
       </c>
     </row>
@@ -5587,7 +5587,7 @@
       </c>
       <c r="B517" t="inlineStr">
         <is>
-          <t>[(-0.3, 516.0), (-0.3, 515.86), (-3.916, 516.0), (-3.916, 515.86), (-3.916, 516.0), (-3.916, 515.74), (-10.782, 516.0), (-10.782, 515.74), (-0.3, 515.86), (-0.3, 515.72), (-3.916, 515.86), (-3.916, 515.72), (-3.916, 515.74), (-3.916, 515.6), (-10.782, 515.74), (-10.782, 515.48), (-0.3, 515.72), (-0.3, 515.6), (-3.916, 515.72), (-3.916, 515.6), (-3.916, 515.6), (-3.916, 515.6), (-10.782, 515.48), (-10.782, 515.48)]</t>
+          <t>[(-0.3, 516.0), (-0.3, 515.86), (-3.916, 516.1301967007082), (-3.916, 515.9901967007082), (-3.916, 516.1301967007082), (-3.916, 515.8701967007082), (-10.782, 516.377412006865), (-10.782, 516.117412006865), (-0.3, 515.86), (-0.3, 515.72), (-3.916, 515.9901967007082), (-3.916, 515.8501967007082), (-3.916, 515.8701967007082), (-3.916, 515.7301967007082), (-10.782, 516.117412006865), (-10.782, 515.857412006865), (-0.3, 515.72), (-0.3, 515.6), (-3.916, 515.8501967007082), (-3.916, 515.7301967007082), (-3.916, 515.7301967007082), (-3.916, 515.7301967007082), (-10.782, 515.857412006865), (-10.782, 515.857412006865)]</t>
         </is>
       </c>
     </row>
@@ -5597,7 +5597,7 @@
       </c>
       <c r="B518" t="inlineStr">
         <is>
-          <t>[(-0.3, 517.0), (-0.3, 516.79), (-4.131, 517.0), (-4.131, 516.79), (-4.131, 517.0), (-4.131, 516.75), (-10.953, 517.0), (-10.953, 516.75), (-0.3, 516.79), (-0.3, 516.59), (-4.131, 516.79), (-4.131, 516.63), (-4.131, 516.75), (-4.131, 516.63), (-10.953, 516.75), (-10.953, 516.5)]</t>
+          <t>[(-0.3, 517.0), (-0.3, 516.79), (-4.131, 517.1789843601017), (-4.131, 516.9689843601017), (-4.131, 517.1789843601017), (-4.131, 516.9289843601017), (-10.953, 517.4977082715121), (-10.953, 517.2477082715121), (-0.3, 516.79), (-0.3, 516.59), (-4.131, 516.9689843601017), (-4.131, 516.8089843601017), (-4.131, 516.9289843601017), (-4.131, 516.8089843601017), (-10.953, 517.2477082715121), (-10.953, 516.9977082715121)]</t>
         </is>
       </c>
     </row>
@@ -5607,7 +5607,7 @@
       </c>
       <c r="B519" t="inlineStr">
         <is>
-          <t>[(-0.3, 518.0), (-0.3, 517.77), (-4.733, 518.0), (-4.733, 517.77), (-4.733, 518.0), (-4.733, 517.77), (-11.574, 518.0), (-11.574, 517.68), (-0.3, 517.77), (-0.3, 517.59), (-4.733, 517.77), (-4.733, 517.54), (-4.733, 517.77), (-4.733, 517.54), (-11.574, 517.68), (-11.574, 517.36)]</t>
+          <t>[(-0.3, 518.0), (-0.3, 517.77), (-4.733, 518.2546062349746), (-4.733, 518.0246062349746), (-4.733, 518.2546062349746), (-4.733, 518.0246062349746), (-11.574, 518.6475142551554), (-11.574, 518.3275142551554), (-0.3, 517.77), (-0.3, 517.59), (-4.733, 518.0246062349746), (-4.733, 517.7946062349746), (-4.733, 518.0246062349746), (-4.733, 517.7946062349746), (-11.574, 518.3275142551554), (-11.574, 518.0075142551555)]</t>
         </is>
       </c>
     </row>
@@ -5617,7 +5617,7 @@
       </c>
       <c r="B520" t="inlineStr">
         <is>
-          <t>[(-0.3, 519.0), (-0.3, 518.75), (-5.234, 519.0), (-5.234, 518.75), (-5.234, 519.0), (-5.234, 518.75), (-12.18, 519.0), (-12.18, 518.66), (-0.3, 518.75), (-0.3, 518.6), (-5.234, 518.75), (-5.234, 518.5), (-5.234, 518.75), (-5.234, 518.5), (-12.18, 518.66), (-12.18, 518.32)]</t>
+          <t>[(-0.3, 519.0), (-0.3, 518.75), (-5.234, 519.3362451030761), (-5.234, 519.0862451030761), (-5.234, 519.3362451030761), (-5.234, 519.0862451030761), (-12.18, 519.8096051529274), (-12.18, 519.4696051529273), (-0.3, 518.75), (-0.3, 518.6), (-5.234, 519.0862451030761), (-5.234, 518.8362451030761), (-5.234, 519.0862451030761), (-5.234, 518.8362451030761), (-12.18, 519.4696051529273), (-12.18, 519.1296051529274)]</t>
         </is>
       </c>
     </row>
@@ -5627,7 +5627,7 @@
       </c>
       <c r="B521" t="inlineStr">
         <is>
-          <t>[(-0.3, 520.0), (-0.3, 519.73), (-5.555, 520.0), (-5.555, 519.73), (-5.555, 520.0), (-5.555, 519.74), (-12.458, 520.0), (-12.458, 519.66), (-0.3, 519.73), (-0.3, 519.55), (-5.555, 519.73), (-5.555, 519.47), (-5.555, 519.74), (-5.555, 519.48), (-12.458, 519.66), (-12.458, 519.32)]</t>
+          <t>[(-0.3, 520.0), (-0.3, 519.73), (-5.555, 520.36785), (-5.555, 520.09785), (-5.555, 520.36785), (-5.555, 520.10785), (-12.458, 520.85106), (-12.458, 520.5110599999999), (-0.3, 519.73), (-0.3, 519.55), (-5.555, 520.09785), (-5.555, 519.83785), (-5.555, 520.10785), (-5.555, 519.84785), (-12.458, 520.5110599999999), (-12.458, 520.17106)]</t>
         </is>
       </c>
     </row>
@@ -5637,7 +5637,7 @@
       </c>
       <c r="B522" t="inlineStr">
         <is>
-          <t>[(-0.3, 521.0), (-0.3, 520.75), (-5.537, 521.0), (-5.537, 520.75), (-5.537, 521.0), (-5.537, 520.75), (-12.466, 521.0), (-12.466, 520.67), (-0.3, 520.75), (-0.3, 520.6), (-5.537, 520.75), (-5.537, 520.5), (-5.537, 520.75), (-5.537, 520.5), (-12.466, 520.67), (-12.466, 520.34)]</t>
+          <t>[(-0.3, 521.0), (-0.3, 520.75), (-5.537, 521.36659), (-5.537, 521.11659), (-5.537, 521.36659), (-5.537, 521.11659), (-12.466, 521.85162), (-12.466, 521.52162), (-0.3, 520.75), (-0.3, 520.6), (-5.537, 521.11659), (-5.537, 520.86659), (-5.537, 521.11659), (-5.537, 520.86659), (-12.466, 521.52162), (-12.466, 521.1916200000001)]</t>
         </is>
       </c>
     </row>
@@ -5647,7 +5647,7 @@
       </c>
       <c r="B523" t="inlineStr">
         <is>
-          <t>[(-0.3, 522.0), (-0.3, 521.77), (-5.217, 522.0), (-5.217, 521.77), (-5.217, 522.0), (-5.217, 521.77), (-12.168, 522.0), (-12.168, 521.67), (-0.3, 521.77), (-0.3, 521.61), (-5.217, 521.77), (-5.217, 521.54), (-5.217, 521.77), (-5.217, 521.54), (-12.168, 521.67), (-12.168, 521.34)]</t>
+          <t>[(-0.3, 522.0), (-0.3, 521.77), (-5.217, 522.34419), (-5.217, 522.11419), (-5.217, 522.34419), (-5.217, 522.11419), (-12.168, 522.83076), (-12.168, 522.50076), (-0.3, 521.77), (-0.3, 521.61), (-5.217, 522.11419), (-5.217, 521.88419), (-5.217, 522.11419), (-5.217, 521.88419), (-12.168, 522.50076), (-12.168, 522.1707600000001)]</t>
         </is>
       </c>
     </row>
@@ -5657,7 +5657,7 @@
       </c>
       <c r="B524" t="inlineStr">
         <is>
-          <t>[(-0.3, 523.0), (-0.3, 522.81), (-4.758, 523.0), (-4.758, 522.81), (-4.758, 523.0), (-4.758, 522.81), (-11.678, 523.0), (-11.678, 522.71), (-0.3, 522.81), (-0.3, 522.66), (-4.758, 522.81), (-4.758, 522.62), (-4.758, 522.81), (-4.758, 522.62), (-11.678, 522.71), (-11.678, 522.42)]</t>
+          <t>[(-0.3, 523.0), (-0.3, 522.81), (-4.758, 523.31206), (-4.758, 523.1220599999999), (-4.758, 523.31206), (-4.758, 523.1220599999999), (-11.678, 523.79646), (-11.678, 523.5064600000001), (-0.3, 522.81), (-0.3, 522.66), (-4.758, 523.1220599999999), (-4.758, 522.93206), (-4.758, 523.1220599999999), (-4.758, 522.93206), (-11.678, 523.5064600000001), (-11.678, 523.21646)]</t>
         </is>
       </c>
     </row>
@@ -5667,7 +5667,7 @@
       </c>
       <c r="B525" t="inlineStr">
         <is>
-          <t>[(-0.3, 524.0), (-0.3, 523.83), (-3.886, 524.0), (-3.886, 523.83), (-3.886, 524.0), (-3.886, 523.84), (-10.769, 524.0), (-10.769, 523.56), (-0.3, 523.83), (-0.3, 523.7), (-3.886, 523.83), (-3.886, 523.67), (-3.886, 523.84), (-3.886, 523.68), (-10.769, 523.56), (-10.769, 523.12)]</t>
+          <t>[(-0.3, 524.0), (-0.3, 523.83), (-3.886, 524.25102), (-3.886, 524.0810200000001), (-3.886, 524.25102), (-3.886, 524.0910200000001), (-10.769, 524.73283), (-10.769, 524.29283), (-0.3, 523.83), (-0.3, 523.7), (-3.886, 524.0810200000001), (-3.886, 523.92102), (-3.886, 524.0910200000001), (-3.886, 523.93102), (-10.769, 524.29283), (-10.769, 523.85283)]</t>
         </is>
       </c>
     </row>
@@ -5677,7 +5677,7 @@
       </c>
       <c r="B526" t="inlineStr">
         <is>
-          <t>[(-0.3, 525.0), (-0.3, 524.82), (-2.604, 525.0), (-2.604, 524.82), (-2.604, 525.0), (-2.604, 524.84), (-9.407, 525.0), (-9.407, 524.55), (-0.3, 524.82), (-0.3, 524.64), (-2.604, 524.82), (-2.604, 524.67), (-2.604, 524.84), (-2.604, 524.68), (-9.407, 524.55), (-9.407, 524.1)]</t>
+          <t>[(-0.3, 525.0), (-0.3, 524.82), (-2.604, 525.16128), (-2.604, 524.9812800000001), (-2.604, 525.16128), (-2.604, 525.0012800000001), (-9.407, 525.63749), (-9.407, 525.1874899999999), (-0.3, 524.82), (-0.3, 524.64), (-2.604, 524.9812800000001), (-2.604, 524.83128), (-2.604, 525.0012800000001), (-2.604, 524.84128), (-9.407, 525.1874899999999), (-9.407, 524.73749)]</t>
         </is>
       </c>
     </row>
@@ -5687,7 +5687,7 @@
       </c>
       <c r="B527" t="inlineStr">
         <is>
-          <t>[(-0.3, 526.0), (-0.3, 525.82), (-8.305, 526.0), (-8.305, 525.56), (-0.3, 525.82), (-0.3, 525.64), (-8.305, 525.56), (-8.305, 525.12)]</t>
+          <t>[(-0.3, 526.0), (-0.3, 525.82), (-8.305, 526.5478867924375), (-8.305, 526.1078867924374), (-0.3, 525.82), (-0.3, 525.64), (-8.305, 526.1078867924374), (-8.305, 525.6678867924375)]</t>
         </is>
       </c>
     </row>
@@ -5697,7 +5697,7 @@
       </c>
       <c r="B528" t="inlineStr">
         <is>
-          <t>[(-0.3, 527.0), (-0.3, 526.82), (-7.338, 527.0), (-7.338, 526.71), (-0.3, 526.82), (-0.3, 526.64), (-7.338, 526.71), (-7.338, 526.42)]</t>
+          <t>[(-0.3, 527.0), (-0.3, 526.82), (-7.338, 527.4062951988262), (-7.338, 527.1162951988263), (-0.3, 526.82), (-0.3, 526.64), (-7.338, 527.1162951988263), (-7.338, 526.8262951988262)]</t>
         </is>
       </c>
     </row>
@@ -5707,7 +5707,7 @@
       </c>
       <c r="B529" t="inlineStr">
         <is>
-          <t>[(-0.3, 528.0), (-0.3, 527.81), (-6.61, 528.0), (-6.61, 527.81), (-0.3, 527.81), (-0.3, 527.67), (-6.61, 527.81), (-6.61, 527.51)]</t>
+          <t>[(-0.3, 528.0), (-0.3, 527.81), (-6.61, 528.296661499455), (-6.61, 528.106661499455), (-0.3, 527.81), (-0.3, 527.67), (-6.61, 528.106661499455), (-6.61, 527.806661499455)]</t>
         </is>
       </c>
     </row>
@@ -5717,7 +5717,7 @@
       </c>
       <c r="B530" t="inlineStr">
         <is>
-          <t>[(-0.3, 529.0), (-0.3, 528.89), (-6.439, 529.0), (-6.439, 528.89), (-0.3, 528.89), (-0.3, 528.69), (-6.439, 528.89), (-6.439, 528.59)]</t>
+          <t>[(-0.3, 529.0), (-0.3, 528.89), (-6.439, 529.2228470198344), (-6.439, 529.1128470198344), (-0.3, 528.89), (-0.3, 528.69), (-6.439, 529.1128470198344), (-6.439, 528.8128470198344)]</t>
         </is>
       </c>
     </row>
@@ -5727,7 +5727,7 @@
       </c>
       <c r="B531" t="inlineStr">
         <is>
-          <t>[(-0.3, 530.0), (-0.3, 529.78), (-6.65, 530.0), (-6.65, 529.78), (-0.3, 529.78), (-0.3, 529.61), (-6.65, 529.78), (-6.65, 529.57)]</t>
+          <t>[(-0.3, 530.0), (-0.3, 529.78), (-6.65, 530.1624706509119), (-6.65, 529.9424706509119), (-0.3, 529.78), (-0.3, 529.61), (-6.65, 529.9424706509119), (-6.65, 529.732470650912)]</t>
         </is>
       </c>
     </row>
@@ -5737,7 +5737,7 @@
       </c>
       <c r="B532" t="inlineStr">
         <is>
-          <t>[(-0.3, 531.0), (-0.3, 530.8), (-6.883, 531.0), (-6.883, 530.8), (-0.3, 530.8), (-0.3, 530.6), (-6.883, 530.8), (-6.883, 530.68)]</t>
+          <t>[(-0.3, 531.0), (-0.3, 530.8), (-6.883, 531.0090000690116), (-6.883, 530.8090000690115), (-0.3, 530.8), (-0.3, 530.6), (-6.883, 530.8090000690115), (-6.883, 530.6890000690115)]</t>
         </is>
       </c>
     </row>
@@ -5757,7 +5757,7 @@
       </c>
       <c r="B534" t="inlineStr">
         <is>
-          <t>[(-0.3, 533.0), (-0.3, 532.84), (-8.053, 533.0), (-8.053, 532.84), (-0.3, 532.84), (-0.3, 532.68), (-8.053, 532.84), (-8.053, 532.72)]</t>
+          <t>[(-0.3, 533.0), (-0.3, 532.84), (-8.053, 532.806175), (-8.053, 532.6461750000001), (-0.3, 532.84), (-0.3, 532.68), (-8.053, 532.6461750000001), (-8.053, 532.5261750000001)]</t>
         </is>
       </c>
     </row>
@@ -5767,7 +5767,7 @@
       </c>
       <c r="B535" t="inlineStr">
         <is>
-          <t>[(-0.3, 534.0), (-0.3, 533.85), (-8.848, 534.0), (-8.848, 533.85), (-0.3, 533.85), (-0.3, 533.73), (-8.848, 533.85), (-8.848, 533.72)]</t>
+          <t>[(-0.3, 534.0), (-0.3, 533.85), (-8.848, 533.7863), (-8.848, 533.6363), (-0.3, 533.85), (-0.3, 533.73), (-8.848, 533.6363), (-8.848, 533.5063)]</t>
         </is>
       </c>
     </row>
@@ -5777,7 +5777,7 @@
       </c>
       <c r="B536" t="inlineStr">
         <is>
-          <t>[(-0.3, 535.0), (-0.3, 534.85), (-9.776, 535.0), (-9.776, 534.85), (-0.3, 534.85), (-0.3, 534.74), (-9.776, 534.85), (-9.776, 534.7)]</t>
+          <t>[(-0.3, 535.0), (-0.3, 534.85), (-9.776, 534.7631), (-9.776, 534.6131), (-0.3, 534.85), (-0.3, 534.74), (-9.776, 534.6131), (-9.776, 534.4631)]</t>
         </is>
       </c>
     </row>
@@ -5797,7 +5797,7 @@
       </c>
       <c r="B538" t="inlineStr">
         <is>
-          <t>[(-0.3, 537.0), (-0.3, 536.86), (-7.109, 537.0), (-7.109, 536.86), (-0.3, 536.86), (-0.3, 536.74), (-7.109, 536.86), (-7.109, 536.73)]</t>
+          <t>[(-0.3, 537.0), (-0.3, 536.86), (-7.109, 536.829775), (-7.109, 536.689775), (-0.3, 536.86), (-0.3, 536.74), (-7.109, 536.689775), (-7.109, 536.5597750000001)]</t>
         </is>
       </c>
     </row>
@@ -5817,7 +5817,7 @@
       </c>
       <c r="B540" t="inlineStr">
         <is>
-          <t>[(-0.3, 539.0), (-0.3, 538.85), (-6.982, 539.0), (-6.982, 538.85), (-0.3, 538.85), (-0.3, 538.71), (-6.982, 538.85), (-6.982, 538.7)]</t>
+          <t>[(-0.3, 539.0), (-0.3, 538.85), (-6.982, 538.83295), (-6.982, 538.68295), (-0.3, 538.85), (-0.3, 538.71), (-6.982, 538.68295), (-6.982, 538.53295)]</t>
         </is>
       </c>
     </row>
@@ -5827,7 +5827,7 @@
       </c>
       <c r="B541" t="inlineStr">
         <is>
-          <t>[(-0.3, 540.0), (-0.3, 539.85), (-6.919, 540.0), (-6.919, 539.85), (-0.3, 539.85), (-0.3, 539.74), (-6.919, 539.85), (-6.919, 539.7)]</t>
+          <t>[(-0.3, 540.0), (-0.3, 539.85), (-6.919, 539.834525), (-6.919, 539.684525), (-0.3, 539.85), (-0.3, 539.74), (-6.919, 539.684525), (-6.919, 539.534525)]</t>
         </is>
       </c>
     </row>
@@ -6017,7 +6017,7 @@
       </c>
       <c r="B560" t="inlineStr">
         <is>
-          <t>[(-0.3, 559.0), (-0.3, 558.86), (-7.618, 559.0), (-7.618, 558.86), (-0.3, 558.86), (-0.3, 558.73), (-7.618, 558.86), (-7.618, 558.75)]</t>
+          <t>[(-0.3, 559.0), (-0.3, 558.86), (-7.618, 558.81705), (-7.618, 558.67705), (-0.3, 558.86), (-0.3, 558.73), (-7.618, 558.67705), (-7.618, 558.56705)]</t>
         </is>
       </c>
     </row>
@@ -6027,7 +6027,7 @@
       </c>
       <c r="B561" t="inlineStr">
         <is>
-          <t>[(-0.3, 560.0), (-0.3, 559.82), (-7.298, 560.0), (-7.298, 559.82), (-0.3, 559.82), (-0.3, 559.64), (-7.298, 559.82), (-7.298, 559.69)]</t>
+          <t>[(-0.3, 560.0), (-0.3, 559.82), (-7.298, 559.82505), (-7.298, 559.6450500000001), (-0.3, 559.82), (-0.3, 559.64), (-7.298, 559.6450500000001), (-7.298, 559.5150500000001)]</t>
         </is>
       </c>
     </row>
@@ -6037,7 +6037,7 @@
       </c>
       <c r="B562" t="inlineStr">
         <is>
-          <t>[(-0.3, 561.0), (-0.3, 560.82), (-7.039, 561.0), (-7.039, 560.82), (-0.3, 560.82), (-0.3, 560.65), (-7.039, 560.82), (-7.039, 560.69)]</t>
+          <t>[(-0.3, 561.0), (-0.3, 560.82), (-7.039, 560.831525), (-7.039, 560.6515250000001), (-0.3, 560.82), (-0.3, 560.65), (-7.039, 560.6515250000001), (-7.039, 560.5215250000001)]</t>
         </is>
       </c>
     </row>
@@ -6047,7 +6047,7 @@
       </c>
       <c r="B563" t="inlineStr">
         <is>
-          <t>[(-0.3, 562.0), (-0.3, 561.89), (-6.683, 562.0), (-6.683, 561.89), (-0.3, 561.89), (-0.3, 561.61), (-6.683, 561.89), (-6.683, 561.72)]</t>
+          <t>[(-0.3, 562.0), (-0.3, 561.89), (-6.683, 561.840425), (-6.683, 561.730425), (-0.3, 561.89), (-0.3, 561.61), (-6.683, 561.730425), (-6.683, 561.560425)]</t>
         </is>
       </c>
     </row>
@@ -6067,7 +6067,7 @@
       </c>
       <c r="B565" t="inlineStr">
         <is>
-          <t>[(-0.3, 564.0), (-0.3, 563.84), (-6.054, 564.0), (-6.054, 563.84), (-0.3, 563.84), (-0.3, 563.68), (-6.054, 563.84), (-6.054, 563.73)]</t>
+          <t>[(-0.3, 564.0), (-0.3, 563.84), (-6.054, 564.0040787350335), (-6.054, 563.8440787350336), (-0.3, 563.84), (-0.3, 563.68), (-6.054, 563.8440787350336), (-6.054, 563.7340787350336)]</t>
         </is>
       </c>
     </row>
@@ -6077,7 +6077,7 @@
       </c>
       <c r="B566" t="inlineStr">
         <is>
-          <t>[(-0.3, 565.0), (-0.3, 564.83), (-5.826, 565.0), (-5.826, 564.83), (-0.3, 564.83), (-0.3, 564.67), (-5.826, 564.83), (-5.826, 564.68)]</t>
+          <t>[(-0.3, 565.0), (-0.3, 564.83), (-5.826, 565.1394990070415), (-5.826, 564.9694990070416), (-0.3, 564.83), (-0.3, 564.67), (-5.826, 564.9694990070416), (-5.826, 564.8194990070415)]</t>
         </is>
       </c>
     </row>
@@ -6087,7 +6087,7 @@
       </c>
       <c r="B567" t="inlineStr">
         <is>
-          <t>[(-0.3, 566.0), (-0.3, 565.84), (-5.72, 566.0), (-5.72, 565.84), (-0.3, 565.84), (-0.3, 565.73), (-5.72, 565.84), (-5.72, 565.69)]</t>
+          <t>[(-0.3, 566.0), (-0.3, 565.84), (-5.72, 566.1834876710203), (-5.72, 566.0234876710203), (-0.3, 565.84), (-0.3, 565.73), (-5.72, 566.0234876710203), (-5.72, 565.8734876710204)]</t>
         </is>
       </c>
     </row>
@@ -6097,7 +6097,7 @@
       </c>
       <c r="B568" t="inlineStr">
         <is>
-          <t>[(-0.3, 567.0), (-0.3, 566.89), (-5.575, 567.0), (-5.575, 566.89), (-0.3, 566.89), (-0.3, 566.72), (-5.575, 566.89), (-5.575, 566.65)]</t>
+          <t>[(-0.3, 567.0), (-0.3, 566.89), (-5.575, 567.2239950031015), (-5.575, 567.1139950031015), (-0.3, 566.89), (-0.3, 566.72), (-5.575, 567.1139950031015), (-5.575, 566.8739950031015)]</t>
         </is>
       </c>
     </row>
@@ -6107,7 +6107,7 @@
       </c>
       <c r="B569" t="inlineStr">
         <is>
-          <t>[(-0.3, 568.0), (-0.3, 567.89), (-5.352, 568.0), (-5.352, 567.89), (-0.3, 567.89), (-0.3, 567.72), (-5.352, 567.89), (-5.352, 567.65)]</t>
+          <t>[(-0.3, 568.0), (-0.3, 567.89), (-5.352, 568.2580218142435), (-5.352, 568.1480218142435), (-0.3, 567.89), (-0.3, 567.72), (-5.352, 568.1480218142435), (-5.352, 567.9080218142435)]</t>
         </is>
       </c>
     </row>
@@ -6117,7 +6117,7 @@
       </c>
       <c r="B570" t="inlineStr">
         <is>
-          <t>[(-0.3, 569.0), (-0.3, 568.89), (-5.076, 569.0), (-5.076, 568.89), (-0.3, 568.89), (-0.3, 568.75), (-5.076, 568.89), (-5.076, 568.62)]</t>
+          <t>[(-0.3, 569.0), (-0.3, 568.89), (-5.076, 569.2850455084694), (-5.076, 569.1750455084693), (-0.3, 568.89), (-0.3, 568.75), (-5.076, 569.1750455084693), (-5.076, 568.9050455084694)]</t>
         </is>
       </c>
     </row>
@@ -6127,7 +6127,7 @@
       </c>
       <c r="B571" t="inlineStr">
         <is>
-          <t>[(-0.3, 570.0), (-0.3, 569.88), (-4.808, 570.0), (-4.808, 569.88), (-0.3, 569.88), (-0.3, 569.75), (-4.808, 569.88), (-4.808, 569.58)]</t>
+          <t>[(-0.3, 570.0), (-0.3, 569.88), (-4.808, 570.3078629924009), (-4.808, 570.1878629924009), (-0.3, 569.88), (-0.3, 569.75), (-4.808, 570.1878629924009), (-4.808, 569.887862992401)]</t>
         </is>
       </c>
     </row>
@@ -6137,7 +6137,7 @@
       </c>
       <c r="B572" t="inlineStr">
         <is>
-          <t>[(-0.3, 571.0), (-0.3, 570.87), (-4.475, 571.0), (-4.475, 570.87), (-0.3, 570.87), (-0.3, 570.73), (-4.475, 570.87), (-4.475, 570.57)]</t>
+          <t>[(-0.3, 571.0), (-0.3, 570.87), (-4.475, 571.29225), (-4.475, 571.16225), (-0.3, 570.87), (-0.3, 570.73), (-4.475, 571.16225), (-4.475, 570.86225)]</t>
         </is>
       </c>
     </row>
@@ -6147,7 +6147,7 @@
       </c>
       <c r="B573" t="inlineStr">
         <is>
-          <t>[(-0.3, 572.0), (-0.3, 571.82), (-4.178, 572.0), (-4.178, 571.82), (-0.3, 571.82), (-0.3, 571.68), (-4.178, 571.82), (-4.178, 571.52)]</t>
+          <t>[(-0.3, 572.0), (-0.3, 571.82), (-4.178, 572.27146), (-4.178, 572.0914600000001), (-0.3, 571.82), (-0.3, 571.68), (-4.178, 572.0914600000001), (-4.178, 571.79146)]</t>
         </is>
       </c>
     </row>
@@ -6157,7 +6157,7 @@
       </c>
       <c r="B574" t="inlineStr">
         <is>
-          <t>[(-0.3, 573.0), (-0.3, 572.88), (-3.883, 573.0), (-3.883, 572.88), (-0.3, 572.88), (-0.3, 572.69), (-3.883, 572.88), (-3.883, 572.58)]</t>
+          <t>[(-0.3, 573.0), (-0.3, 572.88), (-3.883, 573.25081), (-3.883, 573.13081), (-0.3, 572.88), (-0.3, 572.69), (-3.883, 573.13081), (-3.883, 572.83081)]</t>
         </is>
       </c>
     </row>
@@ -6167,7 +6167,7 @@
       </c>
       <c r="B575" t="inlineStr">
         <is>
-          <t>[(-0.3, 574.0), (-0.3, 573.89), (-3.535, 574.0), (-3.535, 573.89), (-0.3, 573.89), (-0.3, 573.71), (-3.535, 573.89), (-3.535, 573.62)]</t>
+          <t>[(-0.3, 574.0), (-0.3, 573.89), (-3.535, 574.22645), (-3.535, 574.11645), (-0.3, 573.89), (-0.3, 573.71), (-3.535, 574.11645), (-3.535, 573.84645)]</t>
         </is>
       </c>
     </row>
@@ -6177,7 +6177,7 @@
       </c>
       <c r="B576" t="inlineStr">
         <is>
-          <t>[(-0.3, 575.0), (-0.3, 574.89), (-3.088, 575.0), (-3.088, 574.89), (-0.3, 574.89), (-0.3, 574.74), (-3.088, 574.89), (-3.088, 574.69)]</t>
+          <t>[(-0.3, 575.0), (-0.3, 574.89), (-3.088, 575.19516), (-3.088, 575.08516), (-0.3, 574.89), (-0.3, 574.74), (-3.088, 575.08516), (-3.088, 574.88516)]</t>
         </is>
       </c>
     </row>
@@ -6187,7 +6187,7 @@
       </c>
       <c r="B577" t="inlineStr">
         <is>
-          <t>[(-0.3, 576.0), (-0.3, 575.89), (-2.856, 576.0), (-2.856, 575.89), (-0.3, 575.89), (-0.3, 575.73), (-2.856, 575.89), (-2.856, 575.63)]</t>
+          <t>[(-0.3, 576.0), (-0.3, 575.89), (-2.856, 576.17892), (-2.856, 576.0689199999999), (-0.3, 575.89), (-0.3, 575.73), (-2.856, 576.0689199999999), (-2.856, 575.80892)]</t>
         </is>
       </c>
     </row>
@@ -6197,7 +6197,7 @@
       </c>
       <c r="B578" t="inlineStr">
         <is>
-          <t>[(-0.3, 577.0), (-0.3, 576.79), (-2.574, 577.0), (-2.574, 576.79), (-0.3, 576.79), (-0.3, 576.65), (-2.574, 576.79), (-2.574, 576.59)]</t>
+          <t>[(-0.3, 577.0), (-0.3, 576.79), (-2.574, 577.15918), (-2.574, 576.94918), (-0.3, 576.79), (-0.3, 576.65), (-2.574, 576.94918), (-2.574, 576.74918)]</t>
         </is>
       </c>
     </row>
@@ -6257,7 +6257,7 @@
       </c>
       <c r="B584" t="inlineStr">
         <is>
-          <t>[(-0.3, 583.0), (-0.3, 582.82), (-2.817, 583.0), (-2.817, 582.82), (-0.3, 582.82), (-0.3, 582.64), (-2.817, 582.82), (-2.817, 582.64), (-0.3, 582.64), (-0.3, 582.51), (-2.817, 582.64), (-2.817, 582.47)]</t>
+          <t>[(-0.3, 583.0), (-0.3, 582.82), (-2.817, 583.0832250563483), (-2.817, 582.9032250563483), (-0.3, 582.82), (-0.3, 582.64), (-2.817, 582.9032250563483), (-2.817, 582.7232250563483), (-0.3, 582.64), (-0.3, 582.51), (-2.817, 582.7232250563483), (-2.817, 582.5532250563483)]</t>
         </is>
       </c>
     </row>
@@ -6267,7 +6267,7 @@
       </c>
       <c r="B585" t="inlineStr">
         <is>
-          <t>[(-0.3, 584.0), (-0.3, 583.8), (-3.503, 584.0), (-3.503, 583.8), (-0.3, 583.8), (-0.3, 583.6), (-3.503, 583.8), (-3.503, 583.6), (-0.3, 583.6), (-0.3, 583.48), (-3.503, 583.6), (-3.503, 583.42)]</t>
+          <t>[(-0.3, 584.0), (-0.3, 583.8), (-3.503, 584.0750107082639), (-3.503, 583.8750107082639), (-0.3, 583.8), (-0.3, 583.6), (-3.503, 583.8750107082639), (-3.503, 583.6750107082639), (-0.3, 583.6), (-0.3, 583.48), (-3.503, 583.6750107082639), (-3.503, 583.4950107082639)]</t>
         </is>
       </c>
     </row>
@@ -6277,7 +6277,7 @@
       </c>
       <c r="B586" t="inlineStr">
         <is>
-          <t>[(-0.3, 585.0), (-0.3, 584.81), (-4.21, 585.0), (-4.21, 584.81), (-0.3, 584.81), (-0.3, 584.62), (-4.21, 584.81), (-4.21, 584.62), (-0.3, 584.62), (-0.3, 584.49), (-4.21, 584.62), (-4.21, 584.44)]</t>
+          <t>[(-0.3, 585.0), (-0.3, 584.81), (-4.21, 584.9938178642872), (-4.21, 584.8038178642871), (-0.3, 584.81), (-0.3, 584.62), (-4.21, 584.8038178642871), (-4.21, 584.6138178642872), (-0.3, 584.62), (-0.3, 584.49), (-4.21, 584.6138178642872), (-4.21, 584.4338178642872)]</t>
         </is>
       </c>
     </row>
@@ -6287,7 +6287,7 @@
       </c>
       <c r="B587" t="inlineStr">
         <is>
-          <t>[(-0.3, 586.0), (-0.3, 585.86), (-4.773, 586.0), (-4.773, 585.86), (-0.3, 585.86), (-0.3, 585.72), (-4.773, 585.86), (-4.773, 585.72), (-0.3, 585.72), (-0.3, 585.58), (-4.773, 585.72), (-4.773, 585.58), (-0.3, 585.58), (-0.3, 585.45), (-4.773, 585.58), (-4.773, 585.45)]</t>
+          <t>[(-0.3, 586.0), (-0.3, 585.86), (-4.773, 585.888175), (-4.773, 585.7481750000001), (-0.3, 585.86), (-0.3, 585.72), (-4.773, 585.7481750000001), (-4.773, 585.6081750000001), (-0.3, 585.72), (-0.3, 585.58), (-4.773, 585.6081750000001), (-4.773, 585.4681750000001), (-0.3, 585.58), (-0.3, 585.45), (-4.773, 585.4681750000001), (-4.773, 585.3381750000001)]</t>
         </is>
       </c>
     </row>
@@ -6297,7 +6297,7 @@
       </c>
       <c r="B588" t="inlineStr">
         <is>
-          <t>[(-0.3, 587.0), (-0.3, 586.81), (-5.262, 587.0), (-5.262, 586.81), (-0.3, 586.81), (-0.3, 586.62), (-5.262, 586.81), (-5.262, 586.62), (-0.3, 586.62), (-0.3, 586.46), (-5.262, 586.62), (-5.262, 586.44)]</t>
+          <t>[(-0.3, 587.0), (-0.3, 586.81), (-5.262, 586.87595), (-5.262, 586.6859499999999), (-0.3, 586.81), (-0.3, 586.62), (-5.262, 586.6859499999999), (-5.262, 586.49595), (-0.3, 586.62), (-0.3, 586.46), (-5.262, 586.49595), (-5.262, 586.31595)]</t>
         </is>
       </c>
     </row>
@@ -6307,7 +6307,7 @@
       </c>
       <c r="B589" t="inlineStr">
         <is>
-          <t>[(-0.3, 588.0), (-0.3, 587.83), (-5.703, 588.0), (-5.703, 587.83), (-0.3, 587.83), (-0.3, 587.66), (-5.703, 587.83), (-5.703, 587.66), (-0.3, 587.66), (-0.3, 587.52), (-5.703, 587.66), (-5.703, 587.5)]</t>
+          <t>[(-0.3, 588.0), (-0.3, 587.83), (-5.703, 587.864925), (-5.703, 587.694925), (-0.3, 587.83), (-0.3, 587.66), (-5.703, 587.694925), (-5.703, 587.5249249999999), (-0.3, 587.66), (-0.3, 587.52), (-5.703, 587.5249249999999), (-5.703, 587.364925)]</t>
         </is>
       </c>
     </row>
@@ -6317,7 +6317,7 @@
       </c>
       <c r="B590" t="inlineStr">
         <is>
-          <t>[(-0.3, 589.0), (-0.3, 588.84), (-6.002, 589.0), (-6.002, 588.84), (-0.3, 588.84), (-0.3, 588.68), (-6.002, 588.84), (-6.002, 588.68), (-0.3, 588.68), (-0.3, 588.57), (-6.002, 588.68), (-6.002, 588.53)]</t>
+          <t>[(-0.3, 589.0), (-0.3, 588.84), (-6.002, 588.85745), (-6.002, 588.69745), (-0.3, 588.84), (-0.3, 588.68), (-6.002, 588.69745), (-6.002, 588.5374499999999), (-0.3, 588.68), (-0.3, 588.57), (-6.002, 588.5374499999999), (-6.002, 588.38745)]</t>
         </is>
       </c>
     </row>
@@ -6327,7 +6327,7 @@
       </c>
       <c r="B591" t="inlineStr">
         <is>
-          <t>[(-0.3, 590.0), (-0.3, 589.85), (-6.096, 590.0), (-6.096, 589.85), (-0.3, 589.85), (-0.3, 589.7), (-6.096, 589.85), (-6.096, 589.7), (-0.3, 589.7), (-0.3, 589.56), (-6.096, 589.7), (-6.096, 589.57)]</t>
+          <t>[(-0.3, 590.0), (-0.3, 589.85), (-6.096, 589.8551), (-6.096, 589.7051), (-0.3, 589.85), (-0.3, 589.7), (-6.096, 589.7051), (-6.096, 589.5551), (-0.3, 589.7), (-0.3, 589.56), (-6.096, 589.5551), (-6.096, 589.4251)]</t>
         </is>
       </c>
     </row>
@@ -6337,7 +6337,7 @@
       </c>
       <c r="B592" t="inlineStr">
         <is>
-          <t>[(-0.3, 591.0), (-0.3, 590.8), (-6.187, 591.0), (-6.187, 590.8), (-0.3, 590.8), (-0.3, 590.61), (-6.187, 590.8), (-6.187, 590.63)]</t>
+          <t>[(-0.3, 591.0), (-0.3, 590.8), (-6.187, 590.852825), (-6.187, 590.652825), (-0.3, 590.8), (-0.3, 590.61), (-6.187, 590.652825), (-6.187, 590.482825)]</t>
         </is>
       </c>
     </row>
@@ -6347,7 +6347,7 @@
       </c>
       <c r="B593" t="inlineStr">
         <is>
-          <t>[(-0.3, 592.0), (-0.3, 591.8), (-6.289, 592.0), (-6.289, 591.8), (-0.3, 591.8), (-0.3, 591.62), (-6.289, 591.8), (-6.289, 591.61)]</t>
+          <t>[(-0.3, 592.0), (-0.3, 591.8), (-6.289, 591.850275), (-6.289, 591.650275), (-0.3, 591.8), (-0.3, 591.62), (-6.289, 591.650275), (-6.289, 591.460275)]</t>
         </is>
       </c>
     </row>
@@ -6357,7 +6357,7 @@
       </c>
       <c r="B594" t="inlineStr">
         <is>
-          <t>[(-0.3, 593.0), (-0.3, 592.85), (-6.402, 593.0), (-6.402, 592.85), (-0.3, 592.85), (-0.3, 592.7), (-6.402, 592.85), (-6.402, 592.7), (-0.3, 592.7), (-0.3, 592.56), (-6.402, 592.7), (-6.402, 592.55)]</t>
+          <t>[(-0.3, 593.0), (-0.3, 592.85), (-6.402, 592.84745), (-6.402, 592.69745), (-0.3, 592.85), (-0.3, 592.7), (-6.402, 592.69745), (-6.402, 592.54745), (-0.3, 592.7), (-0.3, 592.56), (-6.402, 592.54745), (-6.402, 592.3974499999999)]</t>
         </is>
       </c>
     </row>
@@ -6367,7 +6367,7 @@
       </c>
       <c r="B595" t="inlineStr">
         <is>
-          <t>[(-0.3, 594.0), (-0.3, 593.84), (-6.422, 594.0), (-6.422, 593.84), (-0.3, 593.84), (-0.3, 593.68), (-6.422, 593.84), (-6.422, 593.68), (-0.3, 593.68), (-0.3, 593.54), (-6.422, 593.68), (-6.422, 593.52)]</t>
+          <t>[(-0.3, 594.0), (-0.3, 593.84), (-6.422, 593.84695), (-6.422, 593.68695), (-0.3, 593.84), (-0.3, 593.68), (-6.422, 593.68695), (-6.422, 593.5269499999999), (-0.3, 593.68), (-0.3, 593.54), (-6.422, 593.5269499999999), (-6.422, 593.36695)]</t>
         </is>
       </c>
     </row>
@@ -6377,7 +6377,7 @@
       </c>
       <c r="B596" t="inlineStr">
         <is>
-          <t>[(-0.3, 595.0), (-0.3, 594.83), (-6.296, 595.0), (-6.296, 594.83), (-0.3, 594.83), (-0.3, 594.66), (-6.296, 594.83), (-6.296, 594.66), (-0.3, 594.66), (-0.3, 594.51), (-6.296, 594.66), (-6.296, 594.49)]</t>
+          <t>[(-0.3, 595.0), (-0.3, 594.83), (-6.296, 594.8501), (-6.296, 594.6801), (-0.3, 594.83), (-0.3, 594.66), (-6.296, 594.6801), (-6.296, 594.5101), (-0.3, 594.66), (-0.3, 594.51), (-6.296, 594.5101), (-6.296, 594.3401)]</t>
         </is>
       </c>
     </row>
@@ -6387,7 +6387,7 @@
       </c>
       <c r="B597" t="inlineStr">
         <is>
-          <t>[(-0.3, 596.0), (-0.3, 595.78), (-6.131, 596.0), (-6.131, 595.78), (-0.3, 595.78), (-0.3, 595.61), (-6.131, 595.78), (-6.131, 595.56)]</t>
+          <t>[(-0.3, 596.0), (-0.3, 595.78), (-6.131, 595.854225), (-6.131, 595.634225), (-0.3, 595.78), (-0.3, 595.61), (-6.131, 595.634225), (-6.131, 595.414225)]</t>
         </is>
       </c>
     </row>
@@ -6397,7 +6397,7 @@
       </c>
       <c r="B598" t="inlineStr">
         <is>
-          <t>[(-0.3, 597.0), (-0.3, 596.8), (-6.058, 597.0), (-6.058, 596.8), (-0.3, 596.8), (-0.3, 596.61), (-6.058, 596.8), (-6.058, 596.64)]</t>
+          <t>[(-0.3, 597.0), (-0.3, 596.8), (-6.058, 596.85605), (-6.058, 596.6560499999999), (-0.3, 596.8), (-0.3, 596.61), (-6.058, 596.6560499999999), (-6.058, 596.49605)]</t>
         </is>
       </c>
     </row>
@@ -6407,7 +6407,7 @@
       </c>
       <c r="B599" t="inlineStr">
         <is>
-          <t>[(-0.3, 598.0), (-0.3, 597.83), (-6.146, 598.0), (-6.146, 597.83), (-0.3, 597.83), (-0.3, 597.53), (-6.146, 597.83), (-6.146, 597.71)]</t>
+          <t>[(-0.3, 598.0), (-0.3, 597.83), (-6.146, 597.85385), (-6.146, 597.68385), (-0.3, 597.83), (-0.3, 597.53), (-6.146, 597.68385), (-6.146, 597.56385)]</t>
         </is>
       </c>
     </row>
@@ -6417,7 +6417,7 @@
       </c>
       <c r="B600" t="inlineStr">
         <is>
-          <t>[(-0.3, 599.0), (-0.3, 598.82), (-6.221, 599.0), (-6.221, 598.82), (-0.3, 598.82), (-0.3, 598.64), (-6.221, 598.82), (-6.221, 598.64), (-0.3, 598.64), (-0.3, 598.48), (-6.221, 598.64), (-6.221, 598.53)]</t>
+          <t>[(-0.3, 599.0), (-0.3, 598.82), (-6.221, 598.851975), (-6.221, 598.6719750000001), (-0.3, 598.82), (-0.3, 598.64), (-6.221, 598.6719750000001), (-6.221, 598.491975), (-0.3, 598.64), (-0.3, 598.48), (-6.221, 598.491975), (-6.221, 598.381975)]</t>
         </is>
       </c>
     </row>
@@ -6427,7 +6427,7 @@
       </c>
       <c r="B601" t="inlineStr">
         <is>
-          <t>[(-0.3, 600.0), (-0.3, 599.72), (-6.222, 600.0), (-6.222, 599.72), (-0.3, 599.72), (-0.3, 599.45), (-6.222, 599.72), (-6.222, 599.57)]</t>
+          <t>[(-0.3, 600.0), (-0.3, 599.72), (-6.222, 599.85195), (-6.222, 599.57195), (-0.3, 599.72), (-0.3, 599.45), (-6.222, 599.57195), (-6.222, 599.42195)]</t>
         </is>
       </c>
     </row>
@@ -6437,7 +6437,7 @@
       </c>
       <c r="B602" t="inlineStr">
         <is>
-          <t>[(-0.3, 601.0), (-0.3, 600.76), (-6.155, 601.0), (-6.155, 600.76), (-0.3, 600.76), (-0.3, 600.46), (-6.155, 600.76), (-6.155, 600.63)]</t>
+          <t>[(-0.3, 601.0), (-0.3, 600.76), (-6.155, 600.853625), (-6.155, 600.613625), (-0.3, 600.76), (-0.3, 600.46), (-6.155, 600.613625), (-6.155, 600.483625)]</t>
         </is>
       </c>
     </row>
@@ -6447,7 +6447,7 @@
       </c>
       <c r="B603" t="inlineStr">
         <is>
-          <t>[(-0.3, 602.0), (-0.3, 601.74), (-6.006, 602.0), (-6.006, 601.86), (-0.3, 601.74), (-0.3, 601.48), (-6.006, 601.86), (-6.006, 601.72)]</t>
+          <t>[(-0.3, 602.0), (-0.3, 601.74), (-6.006, 601.85735), (-6.006, 601.71735), (-0.3, 601.74), (-0.3, 601.48), (-6.006, 601.71735), (-6.006, 601.57735)]</t>
         </is>
       </c>
     </row>
@@ -6457,7 +6457,7 @@
       </c>
       <c r="B604" t="inlineStr">
         <is>
-          <t>[(-0.3, 603.0), (-0.3, 602.76), (-5.889, 603.0), (-5.889, 602.88), (-0.3, 602.76), (-0.3, 602.52), (-5.889, 602.88), (-5.889, 602.76)]</t>
+          <t>[(-0.3, 603.0), (-0.3, 602.76), (-5.889, 602.860275), (-5.889, 602.740275), (-0.3, 602.76), (-0.3, 602.52), (-5.889, 602.740275), (-5.889, 602.620275)]</t>
         </is>
       </c>
     </row>
@@ -6477,7 +6477,7 @@
       </c>
       <c r="B606" t="inlineStr">
         <is>
-          <t>[(-0.3, 605.0), (-0.3, 604.76), (-5.663, 605.0), (-5.663, 604.87), (-0.3, 604.76), (-0.3, 604.52), (-5.663, 604.87), (-5.663, 604.74)]</t>
+          <t>[(-0.3, 605.0), (-0.3, 604.76), (-5.663, 604.865925), (-5.663, 604.735925), (-0.3, 604.76), (-0.3, 604.52), (-5.663, 604.735925), (-5.663, 604.605925)]</t>
         </is>
       </c>
     </row>
@@ -6487,7 +6487,7 @@
       </c>
       <c r="B607" t="inlineStr">
         <is>
-          <t>[(-0.3, 606.0), (-0.3, 605.74), (-5.511, 606.0), (-5.511, 605.85), (-0.3, 605.74), (-0.3, 605.48), (-5.511, 605.85), (-5.511, 605.7)]</t>
+          <t>[(-0.3, 606.0), (-0.3, 605.74), (-5.511, 605.869725), (-5.511, 605.719725), (-0.3, 605.74), (-0.3, 605.48), (-5.511, 605.719725), (-5.511, 605.5697250000001)]</t>
         </is>
       </c>
     </row>
@@ -6497,7 +6497,7 @@
       </c>
       <c r="B608" t="inlineStr">
         <is>
-          <t>[(-0.3, 607.0), (-0.3, 606.74), (-5.47, 607.0), (-5.47, 606.85), (-0.3, 606.74), (-0.3, 606.48), (-5.47, 606.85), (-5.47, 606.7)]</t>
+          <t>[(-0.3, 607.0), (-0.3, 606.74), (-5.47, 606.87075), (-5.47, 606.7207500000001), (-0.3, 606.74), (-0.3, 606.48), (-5.47, 606.7207500000001), (-5.47, 606.5707500000001)]</t>
         </is>
       </c>
     </row>
@@ -6507,7 +6507,7 @@
       </c>
       <c r="B609" t="inlineStr">
         <is>
-          <t>[(-0.3, 608.0), (-0.3, 607.77), (-5.416, 608.0), (-5.416, 607.77), (-0.3, 607.77), (-0.3, 607.47), (-5.416, 607.77), (-5.416, 607.66)]</t>
+          <t>[(-0.3, 608.0), (-0.3, 607.77), (-5.416, 607.8721), (-5.416, 607.6421), (-0.3, 607.77), (-0.3, 607.47), (-5.416, 607.6421), (-5.416, 607.5321)]</t>
         </is>
       </c>
     </row>
@@ -6517,7 +6517,7 @@
       </c>
       <c r="B610" t="inlineStr">
         <is>
-          <t>[(-0.3, 609.0), (-0.3, 608.81), (-5.474, 609.0), (-5.474, 608.81), (-0.3, 608.81), (-0.3, 608.51), (-5.474, 608.81), (-5.474, 608.67)]</t>
+          <t>[(-0.3, 609.0), (-0.3, 608.81), (-5.474, 608.87065), (-5.474, 608.6806499999999), (-0.3, 608.81), (-0.3, 608.51), (-5.474, 608.6806499999999), (-5.474, 608.5406499999999)]</t>
         </is>
       </c>
     </row>
@@ -6527,7 +6527,7 @@
       </c>
       <c r="B611" t="inlineStr">
         <is>
-          <t>[(-0.3, 610.0), (-0.3, 609.82), (-5.528, 610.0), (-5.528, 609.82), (-0.3, 609.82), (-0.3, 609.52), (-5.528, 609.82), (-5.528, 609.68)]</t>
+          <t>[(-0.3, 610.0), (-0.3, 609.82), (-5.528, 609.8693), (-5.528, 609.6893), (-0.3, 609.82), (-0.3, 609.52), (-5.528, 609.6893), (-5.528, 609.5492999999999)]</t>
         </is>
       </c>
     </row>
@@ -6537,7 +6537,7 @@
       </c>
       <c r="B612" t="inlineStr">
         <is>
-          <t>[(-0.3, 611.0), (-0.3, 610.78), (-5.578, 611.0), (-5.578, 610.78), (-0.3, 610.78), (-0.3, 610.56), (-5.578, 610.78), (-5.578, 610.65)]</t>
+          <t>[(-0.3, 611.0), (-0.3, 610.78), (-5.578, 610.86805), (-5.578, 610.64805), (-0.3, 610.78), (-0.3, 610.56), (-5.578, 610.64805), (-5.578, 610.51805)]</t>
         </is>
       </c>
     </row>
@@ -6547,7 +6547,7 @@
       </c>
       <c r="B613" t="inlineStr">
         <is>
-          <t>[(-0.3, 612.0), (-0.3, 611.84), (-5.642, 612.0), (-5.642, 611.84), (-0.3, 611.84), (-0.3, 611.68), (-5.642, 611.84), (-5.642, 611.68), (-0.3, 611.68), (-0.3, 611.55), (-5.642, 611.68), (-5.642, 611.52)]</t>
+          <t>[(-0.3, 612.0), (-0.3, 611.84), (-5.642, 611.86645), (-5.642, 611.70645), (-0.3, 611.84), (-0.3, 611.68), (-5.642, 611.70645), (-5.642, 611.5464499999999), (-0.3, 611.68), (-0.3, 611.55), (-5.642, 611.5464499999999), (-5.642, 611.38645)]</t>
         </is>
       </c>
     </row>
@@ -6557,7 +6557,7 @@
       </c>
       <c r="B614" t="inlineStr">
         <is>
-          <t>[(-0.3, 613.0), (-0.3, 612.76), (-5.707, 613.0), (-5.707, 612.76), (-0.3, 612.76), (-0.3, 612.59), (-5.707, 612.76), (-5.707, 612.53)]</t>
+          <t>[(-0.3, 613.0), (-0.3, 612.76), (-5.707, 612.864825), (-5.707, 612.624825), (-0.3, 612.76), (-0.3, 612.59), (-5.707, 612.624825), (-5.707, 612.394825)]</t>
         </is>
       </c>
     </row>
@@ -6567,7 +6567,7 @@
       </c>
       <c r="B615" t="inlineStr">
         <is>
-          <t>[(-0.3, 614.0), (-0.3, 613.78), (-5.693, 614.0), (-5.693, 613.78), (-0.3, 613.78), (-0.3, 613.61), (-5.693, 613.78), (-5.693, 613.57)]</t>
+          <t>[(-0.3, 614.0), (-0.3, 613.78), (-5.693, 613.865175), (-5.693, 613.645175), (-0.3, 613.78), (-0.3, 613.61), (-5.693, 613.645175), (-5.693, 613.4351750000001)]</t>
         </is>
       </c>
     </row>
@@ -6577,7 +6577,7 @@
       </c>
       <c r="B616" t="inlineStr">
         <is>
-          <t>[(-0.3, 615.0), (-0.3, 614.82), (-5.737, 615.0), (-5.737, 614.82), (-0.3, 614.82), (-0.3, 614.65), (-5.737, 614.82), (-5.737, 614.64)]</t>
+          <t>[(-0.3, 615.0), (-0.3, 614.82), (-5.737, 614.864075), (-5.737, 614.684075), (-0.3, 614.82), (-0.3, 614.65), (-5.737, 614.684075), (-5.737, 614.504075)]</t>
         </is>
       </c>
     </row>
@@ -6587,7 +6587,7 @@
       </c>
       <c r="B617" t="inlineStr">
         <is>
-          <t>[(-0.3, 616.0), (-0.3, 615.83), (-5.754, 616.0), (-5.754, 615.83), (-0.3, 615.83), (-0.3, 615.72), (-5.754, 615.83), (-5.754, 615.67)]</t>
+          <t>[(-0.3, 616.0), (-0.3, 615.83), (-5.754, 615.86365), (-5.754, 615.69365), (-0.3, 615.83), (-0.3, 615.72), (-5.754, 615.69365), (-5.754, 615.53365)]</t>
         </is>
       </c>
     </row>
@@ -6597,7 +6597,7 @@
       </c>
       <c r="B618" t="inlineStr">
         <is>
-          <t>[(-0.3, 617.0), (-0.3, 616.82), (-5.745, 617.0), (-5.745, 616.82), (-0.3, 616.82), (-0.3, 616.69), (-5.745, 616.82), (-5.745, 616.64)]</t>
+          <t>[(-0.3, 617.0), (-0.3, 616.82), (-5.745, 616.8564821347211), (-5.745, 616.6764821347211), (-0.3, 616.82), (-0.3, 616.69), (-5.745, 616.6764821347211), (-5.745, 616.4964821347211)]</t>
         </is>
       </c>
     </row>
@@ -6607,7 +6607,7 @@
       </c>
       <c r="B619" t="inlineStr">
         <is>
-          <t>[(-0.3, 618.0), (-0.3, 617.85), (-5.566, 618.0), (-5.566, 617.85), (-0.3, 617.85), (-0.3, 617.72), (-5.566, 617.85), (-5.566, 617.7)]</t>
+          <t>[(-0.3, 618.0), (-0.3, 617.85), (-5.566, 617.8504776380835), (-5.566, 617.7004776380835), (-0.3, 617.85), (-0.3, 617.72), (-5.566, 617.7004776380835), (-5.566, 617.5504776380835)]</t>
         </is>
       </c>
     </row>
@@ -6627,7 +6627,7 @@
       </c>
       <c r="B621" t="inlineStr">
         <is>
-          <t>[(-0.3, 620.0), (-0.3, 619.85), (-5.379, 620.0), (-5.379, 619.85), (-0.3, 619.85), (-0.3, 619.72), (-5.379, 619.85), (-5.379, 619.72)]</t>
+          <t>[(-0.3, 620.0), (-0.3, 619.85), (-5.379, 619.8351037699337), (-5.379, 619.6851037699337), (-0.3, 619.85), (-0.3, 619.72), (-5.379, 619.6851037699337), (-5.379, 619.5551037699337)]</t>
         </is>
       </c>
     </row>
@@ -6647,7 +6647,7 @@
       </c>
       <c r="B623" t="inlineStr">
         <is>
-          <t>[(-0.3, 622.0), (-0.3, 621.84), (-5.574, 622.0), (-5.574, 621.84), (-0.3, 621.84), (-0.3, 621.68), (-5.574, 621.84), (-5.574, 621.73)]</t>
+          <t>[(-0.3, 622.0), (-0.3, 621.84), (-5.574, 621.81541), (-5.574, 621.6554100000001), (-0.3, 621.84), (-0.3, 621.68), (-5.574, 621.6554100000001), (-5.574, 621.5454100000001)]</t>
         </is>
       </c>
     </row>
@@ -6657,7 +6657,7 @@
       </c>
       <c r="B624" t="inlineStr">
         <is>
-          <t>[(-0.3, 623.0), (-0.3, 622.89), (-5.733, 623.0), (-5.733, 622.89), (-0.3, 622.89), (-0.3, 622.67), (-5.733, 622.89), (-5.733, 622.73)]</t>
+          <t>[(-0.3, 623.0), (-0.3, 622.89), (-5.733, 622.809845), (-5.733, 622.699845), (-0.3, 622.89), (-0.3, 622.67), (-5.733, 622.699845), (-5.733, 622.539845)]</t>
         </is>
       </c>
     </row>
@@ -6667,7 +6667,7 @@
       </c>
       <c r="B625" t="inlineStr">
         <is>
-          <t>[(-0.3, 624.0), (-0.3, 623.82), (-5.937, 624.0), (-5.937, 623.82), (-0.3, 623.82), (-0.3, 623.65), (-5.937, 623.82), (-5.937, 623.68)]</t>
+          <t>[(-0.3, 624.0), (-0.3, 623.82), (-5.937, 623.802705), (-5.937, 623.622705), (-0.3, 623.82), (-0.3, 623.65), (-5.937, 623.622705), (-5.937, 623.4827049999999)]</t>
         </is>
       </c>
     </row>
@@ -6677,7 +6677,7 @@
       </c>
       <c r="B626" t="inlineStr">
         <is>
-          <t>[(-0.3, 625.0), (-0.3, 624.8), (-6.034, 625.0), (-6.034, 624.8), (-0.3, 624.8), (-0.3, 624.61), (-6.034, 624.8), (-6.034, 624.64)]</t>
+          <t>[(-0.3, 625.0), (-0.3, 624.8), (-6.034, 624.79931), (-6.034, 624.59931), (-0.3, 624.8), (-0.3, 624.61), (-6.034, 624.59931), (-6.034, 624.43931)]</t>
         </is>
       </c>
     </row>
@@ -6687,7 +6687,7 @@
       </c>
       <c r="B627" t="inlineStr">
         <is>
-          <t>[(-0.3, 626.0), (-0.3, 625.78), (-6.25, 626.0), (-6.25, 625.78), (-0.3, 625.78), (-0.3, 625.57), (-6.25, 625.78), (-6.25, 625.6)]</t>
+          <t>[(-0.3, 626.0), (-0.3, 625.78), (-6.25, 625.79175), (-6.25, 625.57175), (-0.3, 625.78), (-0.3, 625.57), (-6.25, 625.57175), (-6.25, 625.39175)]</t>
         </is>
       </c>
     </row>
@@ -6697,7 +6697,7 @@
       </c>
       <c r="B628" t="inlineStr">
         <is>
-          <t>[(-0.3, 627.0), (-0.3, 626.78), (-6.434, 627.0), (-6.434, 626.78), (-0.3, 626.78), (-0.3, 626.56), (-6.434, 626.78), (-6.434, 626.6)]</t>
+          <t>[(-0.3, 627.0), (-0.3, 626.78), (-6.434, 626.78531), (-6.434, 626.56531), (-0.3, 626.78), (-0.3, 626.56), (-6.434, 626.56531), (-6.434, 626.38531)]</t>
         </is>
       </c>
     </row>
@@ -6707,7 +6707,7 @@
       </c>
       <c r="B629" t="inlineStr">
         <is>
-          <t>[(-0.3, 628.0), (-0.3, 627.78), (-6.611, 628.0), (-6.611, 627.78), (-0.3, 627.78), (-0.3, 627.57), (-6.611, 627.78), (-6.611, 627.61)]</t>
+          <t>[(-0.3, 628.0), (-0.3, 627.78), (-6.611, 627.779115), (-6.611, 627.559115), (-0.3, 627.78), (-0.3, 627.57), (-6.611, 627.559115), (-6.611, 627.3891150000001)]</t>
         </is>
       </c>
     </row>
@@ -6717,7 +6717,7 @@
       </c>
       <c r="B630" t="inlineStr">
         <is>
-          <t>[(-0.3, 629.0), (-0.3, 628.79), (-6.849, 629.0), (-6.849, 628.79), (-0.3, 628.79), (-0.3, 628.58), (-6.849, 628.79), (-6.849, 628.64)]</t>
+          <t>[(-0.3, 629.0), (-0.3, 628.79), (-6.849, 628.770785), (-6.849, 628.560785), (-0.3, 628.79), (-0.3, 628.58), (-6.849, 628.560785), (-6.849, 628.410785)]</t>
         </is>
       </c>
     </row>
@@ -6727,7 +6727,7 @@
       </c>
       <c r="B631" t="inlineStr">
         <is>
-          <t>[(-0.3, 630.0), (-0.3, 629.77), (-7.077, 630.0), (-7.077, 629.77), (-0.3, 629.77), (-0.3, 629.54), (-7.077, 629.77), (-7.077, 629.6)]</t>
+          <t>[(-0.3, 630.0), (-0.3, 629.77), (-7.077, 629.762805), (-7.077, 629.5328049999999), (-0.3, 629.77), (-0.3, 629.54), (-7.077, 629.5328049999999), (-7.077, 629.362805)]</t>
         </is>
       </c>
     </row>
@@ -6737,7 +6737,7 @@
       </c>
       <c r="B632" t="inlineStr">
         <is>
-          <t>[(-0.3, 631.0), (-0.3, 630.81), (-7.33, 631.0), (-7.33, 630.81), (-0.3, 630.81), (-0.3, 630.62), (-7.33, 630.81), (-7.33, 630.64)]</t>
+          <t>[(-0.3, 631.0), (-0.3, 630.81), (-7.33, 630.75395), (-7.33, 630.56395), (-0.3, 630.81), (-0.3, 630.62), (-7.33, 630.56395), (-7.33, 630.39395)]</t>
         </is>
       </c>
     </row>
@@ -6747,7 +6747,7 @@
       </c>
       <c r="B633" t="inlineStr">
         <is>
-          <t>[(-0.3, 632.0), (-0.3, 631.83), (-7.345, 632.0), (-7.345, 631.83), (-0.3, 631.83), (-0.3, 631.67), (-7.345, 631.83), (-7.345, 631.72)]</t>
+          <t>[(-0.3, 632.0), (-0.3, 631.83), (-7.345, 631.753425), (-7.345, 631.583425), (-0.3, 631.83), (-0.3, 631.67), (-7.345, 631.583425), (-7.345, 631.473425)]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Layers to CAD file addded
</commit_message>
<xml_diff>
--- a/output/layerCoordinates_left.xlsx
+++ b/output/layerCoordinates_left.xlsx
@@ -427,7 +427,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-2.0, 0.0), (-2.0, -0.13), (-13.452, -0.2724750527055538), (-13.452, -0.4024750527055538), (-2.0, -0.13), (-2.0, -0.25), (-13.452, -0.4024750527055538), (-13.452, -0.5224750527055537)]</t>
         </is>
       </c>
     </row>
@@ -437,7 +437,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-2.0, 1.0), (-2.0, 0.87), (-14.169, 0.7650108327053524), (-14.169, 0.6350108327053523), (-2.0, 0.87), (-2.0, 0.75), (-14.169, 0.6350108327053523), (-14.169, 0.5150108327053524)]</t>
         </is>
       </c>
     </row>
@@ -447,7 +447,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-2.0, 2.0), (-2.0, 1.87), (-13.64, 1.7366317044100097), (-13.64, 1.6066317044100098), (-2.0, 1.87), (-2.0, 1.75), (-13.64, 1.6066317044100098), (-13.64, 1.4866317044100097)]</t>
         </is>
       </c>
     </row>
@@ -457,7 +457,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-2.0, 3.0), (-2.0, 2.87), (-13.653, 2.7765873638344267), (-13.653, 2.646587363834427), (-2.0, 2.87), (-2.0, 2.75), (-13.653, 2.646587363834427), (-13.653, 2.5265873638344267)]</t>
         </is>
       </c>
     </row>
@@ -467,7 +467,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-2.0, 4.0), (-2.0, 3.87), (-13.605, 3.743245028480061), (-13.605, 3.613245028480061), (-2.0, 3.87), (-2.0, 3.75), (-13.605, 3.613245028480061), (-13.605, 3.493245028480061)]</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-2.0, 5.0), (-2.0, 4.87), (-14.207, 4.733979528301885), (-14.207, 4.603979528301885), (-2.0, 4.87), (-2.0, 4.75), (-14.207, 4.603979528301885), (-14.207, 4.483979528301885)]</t>
         </is>
       </c>
     </row>
@@ -487,7 +487,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-2.0, 6.0), (-2.0, 5.87), (-10.541, 5.844206061042327), (-10.541, 5.7142060610423275), (-2.0, 5.87), (-2.0, 5.75), (-10.541, 5.7142060610423275), (-10.541, 5.594206061042327)]</t>
         </is>
       </c>
     </row>
@@ -497,7 +497,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-2.0, 7.0), (-2.0, 6.87), (-10.654, 6.890557444984277), (-10.654, 6.760557444984277), (-2.0, 6.87), (-2.0, 6.75), (-10.654, 6.760557444984277), (-10.654, 6.640557444984277)]</t>
         </is>
       </c>
     </row>
@@ -507,7 +507,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-2.0, 8.0), (-2.0, 7.87), (-10.673, 7.862074598814507), (-10.673, 7.732074598814507), (-2.0, 7.87), (-2.0, 7.75), (-10.673, 7.732074598814507), (-10.673, 7.612074598814507)]</t>
         </is>
       </c>
     </row>
@@ -517,7 +517,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-2.0, 9.0), (-2.0, 8.87), (-10.704, 8.906585699841107), (-10.704, 8.776585699841107), (-2.0, 8.87), (-2.0, 8.75), (-10.704, 8.776585699841107), (-10.704, 8.656585699841107)]</t>
         </is>
       </c>
     </row>
@@ -527,7 +527,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-2.0, 10.0), (-2.0, 9.87), (-10.767, 9.874775122021248), (-10.767, 9.744775122021247), (-2.0, 9.87), (-2.0, 9.75), (-10.767, 9.744775122021247), (-10.767, 9.624775122021248)]</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-2.0, 11.0), (-2.0, 10.87), (-10.728, 10.87606615936827), (-10.728, 10.746066159368269), (-2.0, 10.87), (-2.0, 10.75), (-10.728, 10.746066159368269), (-10.728, 10.62606615936827)]</t>
         </is>
       </c>
     </row>
@@ -547,7 +547,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-2.0, 12.0), (-2.0, 11.87), (-10.747, 11.869367069138994), (-10.747, 11.739367069138993), (-2.0, 11.87), (-2.0, 11.75), (-10.747, 11.739367069138993), (-10.747, 11.619367069138994)]</t>
         </is>
       </c>
     </row>
@@ -557,7 +557,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-2.0, 13.0), (-2.0, 12.87), (-10.712, 12.859261918437683), (-10.712, 12.729261918437683), (-2.0, 12.87), (-2.0, 12.75), (-10.712, 12.729261918437683), (-10.712, 12.609261918437683)]</t>
         </is>
       </c>
     </row>
@@ -567,7 +567,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-2.0, 14.0), (-2.0, 13.87), (-10.721, 13.842581227436822), (-10.721, 13.712581227436822), (-2.0, 13.87), (-2.0, 13.75), (-10.721, 13.712581227436822), (-10.721, 13.592581227436822)]</t>
         </is>
       </c>
     </row>
@@ -577,7 +577,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-2.0, 15.0), (-2.0, 14.87), (-10.711, 14.783197349848766), (-10.711, 14.653197349848766), (-2.0, 14.87), (-2.0, 14.75), (-10.711, 14.653197349848766), (-10.711, 14.533197349848766)]</t>
         </is>
       </c>
     </row>
@@ -587,7 +587,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-2.00011, 16.0), (-2.00011, 15.87), (-10.664, 15.83059988423468), (-10.664, 15.700599884234679), (-2.00011, 15.87), (-2.00011, 15.75), (-10.664, 15.700599884234679), (-10.664, 15.58059988423468)]</t>
         </is>
       </c>
     </row>
@@ -597,7 +597,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-1.99961, 17.0), (-1.99961, 16.87), (-10.548, 16.720150002575476), (-10.548, 16.590150002575477), (-1.99961, 16.87), (-1.99961, 16.75), (-10.548, 16.590150002575477), (-10.548, 16.470150002575476)]</t>
         </is>
       </c>
     </row>
@@ -607,7 +607,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-1.99935, 18.0), (-1.99935, 17.87), (-10.299, 17.69027787646722), (-10.299, 17.56027787646722), (-1.99935, 17.87), (-1.99935, 17.75), (-10.299, 17.56027787646722), (-10.299, 17.44027787646722)]</t>
         </is>
       </c>
     </row>
@@ -617,7 +617,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-1.99929, 19.0), (-1.99929, 18.87), (-10.014, 18.636504566666662), (-10.014, 18.506504566666663), (-1.99929, 18.87), (-1.99929, 18.75), (-10.014, 18.506504566666663), (-10.014, 18.386504566666662)]</t>
         </is>
       </c>
     </row>
@@ -627,7 +627,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-1.99955, 20.0), (-1.99955, 19.87), (-9.792, 19.616670637574384), (-9.792, 19.486670637574385), (-1.99955, 19.87), (-1.99955, 19.75), (-9.792, 19.486670637574385), (-9.792, 19.366670637574384)]</t>
         </is>
       </c>
     </row>
@@ -637,7 +637,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-2.0, 21.0), (-2.0, 20.87), (-9.625, 20.581407364284676), (-9.625, 20.451407364284677), (-2.0, 20.87), (-2.0, 20.75), (-9.625, 20.451407364284677), (-9.625, 20.331407364284676)]</t>
         </is>
       </c>
     </row>
@@ -647,7 +647,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-1.717, 22.0), (-1.717, 21.87), (-9.685, 21.5227168), (-9.685, 21.392716800000002), (-1.717, 21.87), (-1.717, 21.75), (-9.685, 21.392716800000002), (-9.685, 21.2727168)]</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-1.4335, 23.0), (-1.4335, 22.87), (-12.241, 22.2975125), (-12.241, 22.1675125), (-1.4335, 22.87), (-1.4335, 22.75), (-12.241, 22.1675125), (-12.241, 22.0475125)]</t>
         </is>
       </c>
     </row>
@@ -667,7 +667,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-1.15, 24.0), (-1.15, 23.87), (-10.958, 23.31344), (-10.958, 23.18344), (-1.15, 23.87), (-1.15, 23.75), (-10.958, 23.18344), (-10.958, 23.06344)]</t>
         </is>
       </c>
     </row>
@@ -677,7 +677,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.8665, 25.0), (-0.8665, 24.87), (-9.651, 24.385085), (-9.651, 24.255085), (-0.8665, 24.87), (-0.8665, 24.75), (-9.651, 24.255085), (-9.651, 24.135085)]</t>
         </is>
       </c>
     </row>
@@ -687,7 +687,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.5835, 26.0), (-0.5835, 25.87), (-8.446, 25.449625), (-8.446, 25.319625000000002), (-0.5835, 25.87), (-0.5835, 25.75), (-8.446, 25.319625000000002), (-8.446, 25.199625)]</t>
         </is>
       </c>
     </row>
@@ -697,7 +697,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 27.0), (-0.3, 26.87), (-6.71, 26.5513), (-6.71, 26.421300000000002), (-0.3, 26.87), (-0.3, 26.75), (-6.71, 26.421300000000002), (-6.71, 26.3013)]</t>
         </is>
       </c>
     </row>
@@ -707,7 +707,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 28.0), (-0.3, 27.87), (-6.105, 27.59365), (-6.105, 27.46365), (-0.3, 27.87), (-0.3, 27.75), (-6.105, 27.46365), (-6.105, 27.34365)]</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 29.0), (-0.3, 28.87), (-5.902, 28.60786), (-5.902, 28.47786), (-0.3, 28.87), (-0.3, 28.75), (-5.902, 28.47786), (-5.902, 28.35786)]</t>
         </is>
       </c>
     </row>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 95.0), (-0.3, 94.87), (-2.48, 94.8692), (-2.48, 94.73920000000001), (-0.3, 94.87), (-0.3, 94.75), (-2.48, 94.73920000000001), (-2.48, 94.6192)]</t>
         </is>
       </c>
     </row>
@@ -1977,7 +1977,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 155.0), (-0.3, 154.86), (-2.846, 154.93635), (-2.846, 154.79635000000002), (-2.846, 154.93635), (-2.846, 154.80635), (-10.83, 154.73675), (-10.83, 154.60675), (-0.3, 154.86), (-0.3, 154.73), (-2.846, 154.79635000000002), (-2.846, 154.68635), (-2.846, 154.80635), (-2.846, 154.68635), (-10.83, 154.60675), (-10.83, 154.48675)]</t>
         </is>
       </c>
     </row>
@@ -2007,7 +2007,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 158.0), (-0.3, 157.87), (-3.906, 157.90985), (-3.906, 157.77985), (-3.906, 157.90985), (-3.906, 157.77985), (-13.443, 157.671425), (-13.443, 157.541425), (-0.3, 157.87), (-0.3, 157.75), (-3.906, 157.77985), (-3.906, 157.65985), (-3.906, 157.77985), (-3.906, 157.65985), (-13.443, 157.541425), (-13.443, 157.421425)]</t>
         </is>
       </c>
     </row>
@@ -2017,7 +2017,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 159.0), (-0.3, 158.89), (-4.157, 158.903575), (-4.157, 158.79357499999998), (-4.157, 158.903575), (-4.157, 158.773575), (-14.083, 158.655425), (-14.083, 158.525425), (-0.3, 158.89), (-0.3, 158.68), (-4.157, 158.79357499999998), (-4.157, 158.653575), (-4.157, 158.773575), (-4.157, 158.653575), (-14.083, 158.525425), (-14.083, 158.405425)]</t>
         </is>
       </c>
     </row>
@@ -2047,7 +2047,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 162.0), (-0.3, 161.89), (-4.481, 161.895475), (-4.481, 161.785475), (-4.481, 161.895475), (-4.481, 161.765475), (-11.438, 161.72155), (-11.438, 161.59155), (-0.3, 161.89), (-0.3, 161.62), (-4.481, 161.785475), (-4.481, 161.645475), (-4.481, 161.765475), (-4.481, 161.645475), (-11.438, 161.59155), (-11.438, 161.47155)]</t>
         </is>
       </c>
     </row>
@@ -2057,7 +2057,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 163.0), (-0.3, 162.89), (-4.635, 162.891625), (-4.635, 162.781625), (-4.635, 162.891625), (-4.635, 162.761625), (-11.526, 162.71935), (-11.526, 162.58935), (-0.3, 162.89), (-0.3, 162.62), (-4.635, 162.781625), (-4.635, 162.641625), (-4.635, 162.761625), (-4.635, 162.641625), (-11.526, 162.58935), (-11.526, 162.46935)]</t>
         </is>
       </c>
     </row>
@@ -2067,7 +2067,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 164.0), (-0.3, 163.88), (-4.568, 163.8933), (-4.568, 163.7733), (-4.568, 163.8933), (-4.568, 163.76330000000002), (-11.542, 163.71895), (-11.542, 163.58895), (-0.3, 163.88), (-0.3, 163.58), (-4.568, 163.7733), (-4.568, 163.6433), (-4.568, 163.76330000000002), (-4.568, 163.6433), (-11.542, 163.58895), (-11.542, 163.46895)]</t>
         </is>
       </c>
     </row>
@@ -2077,7 +2077,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 165.0), (-0.3, 164.88), (-4.461, 164.895975), (-4.461, 164.775975), (-4.461, 164.895975), (-4.461, 164.765975), (-11.467, 164.720825), (-11.467, 164.590825), (-0.3, 164.88), (-0.3, 164.58), (-4.461, 164.775975), (-4.461, 164.645975), (-4.461, 164.765975), (-4.461, 164.645975), (-11.467, 164.590825), (-11.467, 164.470825)]</t>
         </is>
       </c>
     </row>
@@ -2087,7 +2087,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 166.0), (-0.3, 165.89), (-4.253, 165.901175), (-4.253, 165.79117499999998), (-4.253, 165.901175), (-4.253, 165.771175), (-11.362, 165.72345), (-11.362, 165.59345000000002), (-0.3, 165.89), (-0.3, 165.68), (-4.253, 165.79117499999998), (-4.253, 165.651175), (-4.253, 165.771175), (-4.253, 165.651175), (-11.362, 165.59345000000002), (-11.362, 165.47345)]</t>
         </is>
       </c>
     </row>
@@ -2097,7 +2097,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 167.0), (-0.3, 166.87), (-4.252, 166.9012), (-4.252, 166.7712), (-4.252, 166.9012), (-4.252, 166.7712), (-11.259, 166.726025), (-11.259, 166.596025), (-0.3, 166.87), (-0.3, 166.75), (-4.252, 166.7712), (-4.252, 166.6512), (-4.252, 166.7712), (-4.252, 166.6512), (-11.259, 166.596025), (-11.259, 166.476025)]</t>
         </is>
       </c>
     </row>
@@ -2107,7 +2107,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 168.0), (-0.3, 167.86), (-4.164, 167.9034), (-4.164, 167.76340000000002), (-4.164, 167.9034), (-4.164, 167.7734), (-11.148, 167.7288), (-11.148, 167.5988), (-0.3, 167.86), (-0.3, 167.74), (-4.164, 167.76340000000002), (-4.164, 167.6534), (-4.164, 167.7734), (-4.164, 167.6534), (-11.148, 167.5988), (-11.148, 167.4788)]</t>
         </is>
       </c>
     </row>
@@ -2117,7 +2117,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 169.0), (-0.3, 168.87), (-4.036, 168.9066), (-4.036, 168.7766), (-4.036, 168.9066), (-4.036, 168.7766), (-13.582, 168.66795), (-13.582, 168.53795), (-0.3, 168.87), (-0.3, 168.75), (-4.036, 168.7766), (-4.036, 168.6566), (-4.036, 168.7766), (-4.036, 168.6566), (-13.582, 168.53795), (-13.582, 168.41795)]</t>
         </is>
       </c>
     </row>
@@ -2127,7 +2127,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 170.0), (-0.3, 169.87), (-4.007, 169.907325), (-4.007, 169.777325), (-4.007, 169.907325), (-4.007, 169.777325), (-13.19, 169.67775), (-13.19, 169.54775), (-0.3, 169.87), (-0.3, 169.75), (-4.007, 169.777325), (-4.007, 169.657325), (-4.007, 169.777325), (-4.007, 169.657325), (-13.19, 169.54775), (-13.19, 169.42775)]</t>
         </is>
       </c>
     </row>
@@ -2137,7 +2137,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 171.0), (-0.3, 170.89), (-3.944, 170.9089), (-3.944, 170.79889999999997), (-3.944, 170.9089), (-3.944, 170.7789), (-12.833, 170.686675), (-12.833, 170.556675), (-0.3, 170.89), (-0.3, 170.67), (-3.944, 170.79889999999997), (-3.944, 170.6589), (-3.944, 170.7789), (-3.944, 170.6589), (-12.833, 170.556675), (-12.833, 170.436675)]</t>
         </is>
       </c>
     </row>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 172.0), (-0.3, 171.89), (-3.841, 171.911475), (-3.841, 171.80147499999998), (-3.841, 171.911475), (-3.841, 171.781475), (-12.411, 171.697225), (-12.411, 171.567225), (-0.3, 171.89), (-0.3, 171.66), (-3.841, 171.80147499999998), (-3.841, 171.661475), (-3.841, 171.781475), (-3.841, 171.661475), (-12.411, 171.567225), (-12.411, 171.447225)]</t>
         </is>
       </c>
     </row>
@@ -2167,7 +2167,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 174.0), (-0.3, 173.86), (-4.002, 173.88920942046707), (-4.002, 173.74920942046708), (-4.002, 173.88920942046707), (-4.002, 173.75920942046707), (-11.644, 173.66050558232808), (-11.644, 173.5305055823281), (-0.3, 173.86), (-0.3, 173.73), (-4.002, 173.74920942046708), (-4.002, 173.63920942046707), (-4.002, 173.75920942046707), (-4.002, 173.63920942046707), (-11.644, 173.5305055823281), (-11.644, 173.41050558232808)]</t>
         </is>
       </c>
     </row>
@@ -2177,7 +2177,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 175.0), (-0.3, 174.87), (-4.157, 174.86302894558347), (-4.157, 174.73302894558347), (-4.157, 174.86302894558347), (-4.157, 174.73302894558347), (-11.37, 174.60687851376954), (-11.37, 174.47687851376955), (-0.3, 174.87), (-0.3, 174.75), (-4.157, 174.73302894558347), (-4.157, 174.61302894558347), (-4.157, 174.73302894558347), (-4.157, 174.61302894558347), (-11.37, 174.47687851376955), (-11.37, 174.35687851376954)]</t>
         </is>
       </c>
     </row>
@@ -2217,7 +2217,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 179.0), (-0.3, 178.89), (-3.955, 178.78854818079898), (-3.955, 178.67854818079897), (-3.955, 178.78854818079898), (-3.955, 178.658548180799), (-10.974, 178.38247969407612), (-10.974, 178.25247969407613), (-0.3, 178.89), (-0.3, 178.67), (-3.955, 178.67854818079897), (-3.955, 178.53854818079898), (-3.955, 178.658548180799), (-3.955, 178.53854818079898), (-10.974, 178.25247969407613), (-10.974, 178.13247969407612)]</t>
         </is>
       </c>
     </row>
@@ -2227,7 +2227,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 180.0), (-0.3, 179.89), (-3.483, 179.80902), (-3.483, 179.69902), (-3.483, 179.80902), (-3.483, 179.67902), (-10.493, 179.38842), (-10.493, 179.25842), (-0.3, 179.89), (-0.3, 179.69), (-3.483, 179.69902), (-3.483, 179.55902), (-3.483, 179.67902), (-3.483, 179.55902), (-10.493, 179.25842), (-10.493, 179.13842)]</t>
         </is>
       </c>
     </row>
@@ -2237,7 +2237,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 181.0), (-0.3, 180.89), (-2.824, 180.84856), (-2.824, 180.73855999999998), (-2.824, 180.84856), (-2.824, 180.71856), (-9.811, 180.42934), (-9.811, 180.29934), (-0.3, 180.89), (-0.3, 180.66), (-2.824, 180.73855999999998), (-2.824, 180.59856), (-2.824, 180.71856), (-2.824, 180.59856), (-9.811, 180.29934), (-9.811, 180.17934)]</t>
         </is>
       </c>
     </row>
@@ -2247,7 +2247,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 182.0), (-0.3, 181.89), (-9.17, 181.4678), (-9.17, 181.3578), (-0.3, 181.89), (-0.3, 181.67), (-9.17, 181.3578), (-9.17, 181.2178)]</t>
         </is>
       </c>
     </row>
@@ -2257,7 +2257,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 183.0), (-0.3, 182.89), (-8.644, 182.49936), (-8.644, 182.38935999999998), (-0.3, 182.89), (-0.3, 182.63), (-8.644, 182.38935999999998), (-8.644, 182.24936)]</t>
         </is>
       </c>
     </row>
@@ -2267,7 +2267,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 184.0), (-0.3, 183.89), (-7.857, 183.54658), (-7.857, 183.43658), (-0.3, 183.89), (-0.3, 183.61), (-7.857, 183.43658), (-7.857, 183.29658)]</t>
         </is>
       </c>
     </row>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 185.0), (-0.3, 184.89), (-6.888, 184.60472), (-6.888, 184.49471999999997), (-0.3, 184.89), (-0.3, 184.63), (-6.888, 184.49471999999997), (-6.888, 184.35472)]</t>
         </is>
       </c>
     </row>
@@ -2287,7 +2287,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 186.0), (-0.3, 185.89), (-5.892, 185.66448), (-5.892, 185.55447999999998), (-0.3, 185.89), (-0.3, 185.68), (-5.892, 185.55447999999998), (-5.892, 185.41448)]</t>
         </is>
       </c>
     </row>
@@ -2297,7 +2297,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 187.0), (-0.3, 186.89), (-4.905, 186.7237), (-4.905, 186.6137), (-0.3, 186.89), (-0.3, 186.68), (-4.905, 186.6137), (-4.905, 186.4737)]</t>
         </is>
       </c>
     </row>
@@ -2307,7 +2307,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 188.0), (-0.3, 187.89), (-4.146, 187.76924), (-4.146, 187.65923999999998), (-0.3, 187.89), (-0.3, 187.67), (-4.146, 187.65923999999998), (-4.146, 187.51924)]</t>
         </is>
       </c>
     </row>
@@ -2557,7 +2557,7 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 213.0), (-0.3, 212.89), (-2.761, 213.07269782605752), (-2.761, 212.9626978260575), (-0.3, 212.89), (-0.3, 212.75), (-2.761, 212.9626978260575), (-2.761, 212.75269782605753)]</t>
         </is>
       </c>
     </row>
@@ -2567,7 +2567,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 214.0), (-0.3, 213.87), (-3.359, 214.09941811729925), (-3.359, 213.96941811729926), (-0.3, 213.87), (-0.3, 213.75), (-3.359, 213.96941811729926), (-3.359, 213.84941811729925)]</t>
         </is>
       </c>
     </row>
@@ -2577,7 +2577,7 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 215.0), (-0.3, 214.87), (-4.285, 215.14130989283044), (-4.285, 215.01130989283044), (-0.3, 214.87), (-0.3, 214.75), (-4.285, 215.01130989283044), (-4.285, 214.89130989283044)]</t>
         </is>
       </c>
     </row>
@@ -2587,7 +2587,7 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 216.0), (-0.3, 215.87), (-2.315, 216.0764202606724), (-2.315, 215.9464202606724), (-2.315, 216.0764202606724), (-2.315, 215.9464202606724), (-5.644, 216.20267487495445), (-5.644, 216.07267487495446), (-0.3, 215.87), (-0.3, 215.75), (-2.315, 215.9464202606724), (-2.315, 215.8264202606724), (-2.315, 215.9464202606724), (-2.315, 215.8264202606724), (-5.644, 216.07267487495446), (-5.644, 215.95267487495445)]</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 217.0), (-0.3, 216.87), (-4.206, 217.23903990672179), (-4.206, 217.1090399067218), (-4.206, 217.23903990672179), (-4.206, 217.12903990672177), (-7.515, 217.4415445281612), (-7.515, 217.33154452816117), (-0.3, 216.87), (-0.3, 216.75), (-4.206, 217.1090399067218), (-4.206, 216.98903990672179), (-4.206, 217.12903990672177), (-4.206, 216.98903990672179), (-7.515, 217.33154452816117), (-7.515, 217.11154452816118)]</t>
         </is>
       </c>
     </row>
@@ -2647,7 +2647,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 222.0), (-0.3, 221.89), (-10.766, 222.73262), (-10.766, 222.62261999999998), (-10.766, 222.73262), (-10.766, 222.62261999999998), (-14.023, 222.96061), (-14.023, 222.85061), (-0.3, 221.89), (-0.3, 221.75), (-10.766, 222.62261999999998), (-10.766, 222.42262), (-10.766, 222.62261999999998), (-10.766, 222.42262), (-14.023, 222.85061), (-14.023, 222.55061)]</t>
         </is>
       </c>
     </row>
@@ -2657,7 +2657,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 223.0), (-0.3, 222.89), (-11.007, 223.74949), (-11.007, 223.63949), (-11.007, 223.74949), (-11.007, 223.58949), (-14.317, 223.98119), (-14.317, 223.82119), (-0.3, 222.89), (-0.3, 222.75), (-11.007, 223.63949), (-11.007, 223.41949), (-11.007, 223.58949), (-11.007, 223.41949), (-14.317, 223.82119), (-14.317, 223.52119)]</t>
         </is>
       </c>
     </row>
@@ -2667,7 +2667,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 224.0), (-0.3, 223.88), (-11.092, 224.75544), (-11.092, 224.51543999999998), (-11.092, 224.75544), (-11.092, 224.51543999999998), (-14.44, 224.9898), (-14.44, 224.6598), (-0.3, 223.88), (-0.3, 223.76), (-11.092, 224.51543999999998), (-11.092, 224.27544), (-11.092, 224.51543999999998), (-11.092, 224.27544), (-14.44, 224.6598), (-14.44, 224.3298)]</t>
         </is>
       </c>
     </row>
@@ -2677,7 +2677,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 225.0), (-0.3, 224.88), (-10.831, 225.73717), (-10.831, 225.47717), (-10.831, 225.73717), (-10.831, 225.47717), (-14.2, 225.973), (-14.2, 225.633), (-0.3, 224.88), (-0.3, 224.76), (-10.831, 225.47717), (-10.831, 225.21716999999998), (-10.831, 225.47717), (-10.831, 225.21716999999998), (-14.2, 225.633), (-14.2, 225.293)]</t>
         </is>
       </c>
     </row>
@@ -2687,7 +2687,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 226.0), (-0.3, 225.88), (-10.166, 226.69062), (-10.166, 226.43062), (-10.166, 226.69062), (-10.166, 226.43062), (-13.518, 226.92526), (-13.518, 226.59526), (-0.3, 225.88), (-0.3, 225.76), (-10.166, 226.43062), (-10.166, 226.17061999999999), (-10.166, 226.43062), (-10.166, 226.17061999999999), (-13.518, 226.59526), (-13.518, 226.26526)]</t>
         </is>
       </c>
     </row>
@@ -2697,7 +2697,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 227.0), (-0.3, 226.88), (-9.205, 227.62335), (-9.205, 227.38334999999998), (-9.205, 227.62335), (-9.205, 227.38334999999998), (-12.504, 227.85428), (-12.504, 227.51427999999999), (-0.3, 226.88), (-0.3, 226.76), (-9.205, 227.38334999999998), (-9.205, 227.14335), (-9.205, 227.38334999999998), (-9.205, 227.14335), (-12.504, 227.51427999999999), (-12.504, 227.17427999999998)]</t>
         </is>
       </c>
     </row>
@@ -2707,7 +2707,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 228.0), (-0.3, 227.89), (-8.19, 228.4920039533576), (-8.19, 228.38200395335758), (-8.19, 228.4920039533576), (-8.19, 228.3120039533576), (-11.646, 228.70751290935303), (-11.646, 228.52751290935302), (-0.3, 227.89), (-0.3, 227.75), (-8.19, 228.38200395335758), (-8.19, 228.1820039533576), (-8.19, 228.3120039533576), (-8.19, 228.1820039533576), (-11.646, 228.52751290935302), (-11.646, 228.22751290935304)]</t>
         </is>
       </c>
     </row>
@@ -2717,7 +2717,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 229.0), (-0.3, 228.87), (-7.184, 229.37280157785662), (-7.184, 229.24280157785662), (-7.184, 229.37280157785662), (-7.184, 229.23280157785663), (-10.707, 229.56358890481607), (-10.707, 229.42358890481609), (-0.3, 228.87), (-0.3, 228.75), (-7.184, 229.24280157785662), (-7.184, 229.12280157785662), (-7.184, 229.23280157785663), (-7.184, 229.12280157785662), (-10.707, 229.42358890481609), (-10.707, 229.12358890481607)]</t>
         </is>
       </c>
     </row>
@@ -2747,7 +2747,7 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 232.0), (-0.3, 231.87), (-6.473, 232.1823838499305), (-6.473, 232.0523838499305), (-6.473, 232.1823838499305), (-6.473, 232.0423838499305), (-9.977, 232.2859109858703), (-9.977, 232.1459109858703), (-0.3, 231.87), (-0.3, 231.75), (-6.473, 232.0523838499305), (-6.473, 231.9323838499305), (-6.473, 232.0423838499305), (-6.473, 231.9323838499305), (-9.977, 232.1459109858703), (-9.977, 231.8459109858703)]</t>
         </is>
       </c>
     </row>
@@ -2757,7 +2757,7 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 233.0), (-0.3, 232.87), (-6.598, 233.07055554636707), (-6.598, 232.94055554636708), (-6.598, 233.07055554636707), (-6.598, 232.96055554636706), (-10.064, 233.10938462285299), (-10.064, 232.99938462285297), (-0.3, 232.87), (-0.3, 232.75), (-6.598, 232.94055554636708), (-6.598, 232.82055554636707), (-6.598, 232.96055554636706), (-6.598, 232.82055554636707), (-10.064, 232.99938462285297), (-10.064, 232.759384622853)]</t>
         </is>
       </c>
     </row>
@@ -2767,7 +2767,7 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 234.0), (-0.3, 233.87), (-6.694, 233.8737827975527), (-6.694, 233.7437827975527), (-6.694, 233.8737827975527), (-6.694, 233.7437827975527), (-10.232, 233.80394287539778), (-10.232, 233.67394287539778), (-0.3, 233.87), (-0.3, 233.75), (-6.694, 233.7437827975527), (-6.694, 233.6237827975527), (-6.694, 233.7437827975527), (-6.694, 233.6237827975527), (-10.232, 233.67394287539778), (-10.232, 233.55394287539778)]</t>
         </is>
       </c>
     </row>
@@ -2777,7 +2777,7 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 235.0), (-0.3, 234.87), (-6.865, 234.72144607427487), (-6.865, 234.59144607427487), (-6.865, 234.72144607427487), (-6.865, 234.59144607427487), (-10.356, 234.57332242542392), (-10.356, 234.44332242542393), (-0.3, 234.87), (-0.3, 234.75), (-6.865, 234.59144607427487), (-6.865, 234.47144607427487), (-6.865, 234.59144607427487), (-6.865, 234.47144607427487), (-10.356, 234.44332242542393), (-10.356, 234.32332242542392)]</t>
         </is>
       </c>
     </row>
@@ -2787,7 +2787,7 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 236.0), (-0.3, 235.87), (-6.433, 235.61098289848098), (-6.433, 235.480982898481), (-6.433, 235.61098289848098), (-6.433, 235.480982898481), (-10.083, 235.3794628559986), (-10.083, 235.24946285599862), (-0.3, 235.87), (-0.3, 235.75), (-6.433, 235.480982898481), (-6.433, 235.36098289848098), (-6.433, 235.480982898481), (-6.433, 235.36098289848098), (-10.083, 235.24946285599862), (-10.083, 235.1294628559986)]</t>
         </is>
       </c>
     </row>
@@ -2797,7 +2797,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 237.0), (-0.3, 236.87), (-5.622, 236.62746), (-5.622, 236.49746000000002), (-5.622, 236.62746), (-5.622, 236.49746000000002), (-9.234, 236.37462), (-9.234, 236.24462), (-0.3, 236.87), (-0.3, 236.75), (-5.622, 236.49746000000002), (-5.622, 236.37746), (-5.622, 236.49746000000002), (-5.622, 236.37746), (-9.234, 236.24462), (-9.234, 236.12462)]</t>
         </is>
       </c>
     </row>
@@ -2807,7 +2807,7 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 238.0), (-0.3, 237.87), (-4.904, 237.67772), (-4.904, 237.54772), (-4.904, 237.67772), (-4.904, 237.54772), (-8.564, 237.42152), (-8.564, 237.29152), (-0.3, 237.87), (-0.3, 237.75), (-4.904, 237.54772), (-4.904, 237.42772), (-4.904, 237.54772), (-4.904, 237.42772), (-8.564, 237.29152), (-8.564, 237.17152)]</t>
         </is>
       </c>
     </row>
@@ -2817,7 +2817,7 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 239.0), (-0.3, 238.87), (-4.102, 238.73386), (-4.102, 238.60386), (-4.102, 238.73386), (-4.102, 238.60386), (-7.913, 238.46709), (-7.913, 238.33709000000002), (-0.3, 238.87), (-0.3, 238.75), (-4.102, 238.60386), (-4.102, 238.48386), (-4.102, 238.60386), (-4.102, 238.48386), (-7.913, 238.33709000000002), (-7.913, 238.21709)]</t>
         </is>
       </c>
     </row>
@@ -2827,7 +2827,7 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 240.0), (-0.3, 239.87), (-3.709, 239.76137), (-3.709, 239.63137), (-3.709, 239.76137), (-3.709, 239.63137), (-7.59, 239.4897), (-7.59, 239.3597), (-0.3, 239.87), (-0.3, 239.75), (-3.709, 239.63137), (-3.709, 239.51137), (-3.709, 239.63137), (-3.709, 239.51137), (-7.59, 239.3597), (-7.59, 239.2397)]</t>
         </is>
       </c>
     </row>
@@ -2837,7 +2837,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 241.0), (-0.3, 240.87), (-3.488, 240.84073776727553), (-3.488, 240.71073776727553), (-3.488, 240.84073776727553), (-3.488, 240.71073776727553), (-7.284, 240.65110180886208), (-7.284, 240.52110180886208), (-0.3, 240.87), (-0.3, 240.75), (-3.488, 240.71073776727553), (-3.488, 240.59073776727553), (-3.488, 240.71073776727553), (-3.488, 240.59073776727553), (-7.284, 240.52110180886208), (-7.284, 240.40110180886208)]</t>
         </is>
       </c>
     </row>
@@ -2847,7 +2847,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 242.0), (-0.3, 241.87), (-3.388, 241.91058144584278), (-3.388, 241.78058144584278), (-3.388, 241.91058144584278), (-3.388, 241.78058144584278), (-7.389, 241.7947253463664), (-7.389, 241.6647253463664), (-0.3, 241.87), (-0.3, 241.75), (-3.388, 241.78058144584278), (-3.388, 241.66058144584278), (-3.388, 241.78058144584278), (-3.388, 241.66058144584278), (-7.389, 241.6647253463664), (-7.389, 241.5447253463664)]</t>
         </is>
       </c>
     </row>
@@ -2907,7 +2907,7 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 248.0), (-0.3, 247.86), (-3.123, 248.19761), (-3.123, 248.05761), (-3.123, 248.19761), (-3.123, 248.08760999999998), (-6.875, 248.46025), (-6.875, 248.35025), (-0.3, 247.86), (-0.3, 247.75), (-3.123, 248.05761), (-3.123, 247.93761), (-3.123, 248.08760999999998), (-3.123, 247.93761), (-6.875, 248.35025), (-6.875, 248.15025)]</t>
         </is>
       </c>
     </row>
@@ -3077,7 +3077,7 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 265.0), (-0.3, 264.85), (-6.557, 264.56201), (-6.557, 264.41201), (-6.557, 264.56201), (-6.557, 264.45201), (-10.352, 264.29636), (-10.352, 264.18636), (-0.3, 264.85), (-0.3, 264.55), (-6.557, 264.41201), (-6.557, 264.25201), (-6.557, 264.45201), (-6.557, 264.25201), (-10.352, 264.18636), (-10.352, 264.04636)]</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 274.0), (-0.3, 273.86), (-5.91, 273.66646702810965), (-5.91, 273.52646702810966), (-0.3, 273.86), (-0.3, 273.74), (-5.91, 273.52646702810966), (-5.91, 273.41646702810965)]</t>
         </is>
       </c>
     </row>
@@ -3347,7 +3347,7 @@
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 292.0), (-0.3, 291.86), (-2.517, 291.84481), (-2.517, 291.70481), (-0.3, 291.86), (-0.3, 291.73), (-2.517, 291.70481), (-2.517, 291.59481)]</t>
         </is>
       </c>
     </row>
@@ -5017,7 +5017,7 @@
       </c>
       <c r="B460" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 459.0), (-0.3, 458.89), (-8.349, 458.91663834317296), (-8.349, 458.80663834317295), (-0.3, 458.89), (-0.3, 458.68), (-8.349, 458.80663834317295), (-8.349, 458.66663834317296)]</t>
         </is>
       </c>
     </row>
@@ -5047,7 +5047,7 @@
       </c>
       <c r="B463" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 462.0), (-0.3, 461.89), (-8.916, 462.3270511115744), (-8.916, 462.2170511115744), (-0.3, 461.89), (-0.3, 461.75), (-8.916, 462.2170511115744), (-8.916, 461.9770511115744)]</t>
         </is>
       </c>
     </row>
@@ -5057,7 +5057,7 @@
       </c>
       <c r="B464" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 463.0), (-0.3, 462.89), (-8.991, 463.4009208569551), (-8.991, 463.2909208569551), (-0.3, 462.89), (-0.3, 462.75), (-8.991, 463.2909208569551), (-8.991, 463.00092085695513)]</t>
         </is>
       </c>
     </row>
@@ -5097,7 +5097,7 @@
       </c>
       <c r="B468" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 467.0), (-0.3, 466.86), (-3.104, 467.19628), (-3.104, 467.05628), (-3.104, 467.19628), (-3.104, 467.08628), (-9.819, 467.66633), (-9.819, 467.55633), (-0.3, 466.86), (-0.3, 466.75), (-3.104, 467.05628), (-3.104, 466.93628), (-3.104, 467.08628), (-3.104, 466.93628), (-9.819, 467.55633), (-9.819, 467.25633)]</t>
         </is>
       </c>
     </row>
@@ -5107,7 +5107,7 @@
       </c>
       <c r="B469" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 468.0), (-0.3, 467.87), (-3.425, 468.21875), (-3.425, 468.08875), (-3.425, 468.21875), (-3.425, 468.10875), (-10.177, 468.69139), (-10.177, 468.58139), (-0.3, 467.87), (-0.3, 467.75), (-3.425, 468.08875), (-3.425, 467.96875), (-3.425, 468.10875), (-3.425, 467.96875), (-10.177, 468.58139), (-10.177, 468.31139)]</t>
         </is>
       </c>
     </row>
@@ -5127,7 +5127,7 @@
       </c>
       <c r="B471" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 470.0), (-0.3, 469.87), (-3.89, 470.2513), (-3.89, 470.1213), (-3.89, 470.2513), (-3.89, 470.1413), (-10.655, 470.72485), (-10.655, 470.61485), (-0.3, 469.87), (-0.3, 469.75), (-3.89, 470.1213), (-3.89, 470.0013), (-3.89, 470.1413), (-3.89, 470.0013), (-10.655, 470.61485), (-10.655, 470.31485)]</t>
         </is>
       </c>
     </row>
@@ -5157,7 +5157,7 @@
       </c>
       <c r="B474" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 473.0), (-0.3, 472.86), (-4.582, 473.29974), (-4.582, 473.15974), (-4.582, 473.29974), (-4.582, 473.18974), (-11.31, 473.7707), (-11.31, 473.66069999999996), (-0.3, 472.86), (-0.3, 472.75), (-4.582, 473.15974), (-4.582, 473.02974), (-4.582, 473.18974), (-4.582, 473.02974), (-11.31, 473.66069999999996), (-11.31, 473.36069999999995)]</t>
         </is>
       </c>
     </row>
@@ -5197,7 +5197,7 @@
       </c>
       <c r="B478" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 477.0), (-0.3, 476.87), (-4.91, 477.3227), (-4.91, 477.1927), (-4.91, 477.3227), (-4.91, 477.2027), (-11.668, 477.79576), (-11.668, 477.67575999999997), (-0.3, 476.87), (-0.3, 476.75), (-4.91, 477.1927), (-4.91, 477.0727), (-4.91, 477.2027), (-4.91, 477.0727), (-11.668, 477.67575999999997), (-11.668, 477.37575999999996)]</t>
         </is>
       </c>
     </row>
@@ -5217,7 +5217,7 @@
       </c>
       <c r="B480" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 479.0), (-0.3, 478.86), (-4.907, 479.32249), (-4.907, 479.18249000000003), (-4.907, 479.32249), (-4.907, 479.20249), (-11.606, 479.79142), (-11.606, 479.67142), (-0.3, 478.86), (-0.3, 478.75), (-4.907, 479.18249000000003), (-4.907, 479.06249), (-4.907, 479.20249), (-4.907, 479.06249), (-11.606, 479.67142), (-11.606, 479.37142)]</t>
         </is>
       </c>
     </row>
@@ -5227,7 +5227,7 @@
       </c>
       <c r="B481" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 480.0), (-0.3, 479.86), (-4.838, 480.31766), (-4.838, 480.17766), (-4.838, 480.31766), (-4.838, 480.17766), (-11.598, 480.79086), (-11.598, 480.65086), (-0.3, 479.86), (-0.3, 479.75), (-4.838, 480.17766), (-4.838, 480.04766), (-4.838, 480.17766), (-4.838, 480.04766), (-11.598, 480.65086), (-11.598, 480.35086)]</t>
         </is>
       </c>
     </row>
@@ -5327,7 +5327,7 @@
       </c>
       <c r="B491" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 490.0), (-0.3, 489.69), (-5.217, 489.877075), (-5.217, 489.687075), (-5.217, 489.877075), (-5.217, 489.767075), (-12.015, 489.707125), (-12.015, 489.597125), (-0.3, 489.69), (-0.3, 489.38), (-5.217, 489.687075), (-5.217, 489.497075), (-5.217, 489.767075), (-5.217, 489.497075), (-12.015, 489.597125), (-12.015, 489.457125)]</t>
         </is>
       </c>
     </row>
@@ -5337,7 +5337,7 @@
       </c>
       <c r="B492" t="inlineStr">
         <is>
-          <t>[(-0.3, 491.0), (-0.3, 490.66), (-5.197, 490.877575), (-5.197, 490.65757499999995), (-5.197, 490.877575), (-5.197, 490.727575), (-12.024, 490.7069), (-12.024, 490.55690000000004), (-0.3, 490.66), (-0.3, 490.32), (-5.197, 490.65757499999995), (-5.197, 490.437575), (-5.197, 490.727575), (-5.197, 490.427575), (-12.024, 490.55690000000004), (-12.024, 490.3869)]</t>
+          <t>[(-0.3, 491.0), (-0.3, 490.68), (-5.197, 490.877575), (-5.197, 490.677575), (-5.197, 490.877575), (-5.197, 490.76757499999997), (-12.024, 490.7069), (-12.024, 490.5969), (-0.3, 490.68), (-0.3, 490.36), (-5.197, 490.677575), (-5.197, 490.477575), (-5.197, 490.76757499999997), (-5.197, 490.487575), (-12.024, 490.5969), (-12.024, 490.43690000000004)]</t>
         </is>
       </c>
     </row>
@@ -5347,7 +5347,7 @@
       </c>
       <c r="B493" t="inlineStr">
         <is>
-          <t>[(-0.3, 492.0), (-0.3, 491.61), (-5.221, 491.876975), (-5.221, 491.59697500000004), (-5.221, 491.876975), (-5.221, 491.59697500000004), (-12.004, 491.7074), (-12.004, 491.42740000000003), (-0.3, 491.61), (-0.3, 491.22), (-5.221, 491.59697500000004), (-5.221, 491.316975), (-5.221, 491.59697500000004), (-5.221, 491.326975), (-12.004, 491.42740000000003), (-12.004, 491.2674)]</t>
+          <t>[(-0.3, 492.0), (-0.3, 491.68), (-5.221, 491.876975), (-5.221, 491.676975), (-5.221, 491.876975), (-5.221, 491.766975), (-12.004, 491.7074), (-12.004, 491.5974), (-0.3, 491.68), (-0.3, 491.36), (-5.221, 491.676975), (-5.221, 491.47697500000004), (-5.221, 491.766975), (-5.221, 491.47697500000004), (-12.004, 491.5974), (-12.004, 491.4074)]</t>
         </is>
       </c>
     </row>
@@ -5357,7 +5357,7 @@
       </c>
       <c r="B494" t="inlineStr">
         <is>
-          <t>[(-0.3, 493.0), (-0.3, 492.55), (-5.159, 492.878525), (-5.159, 492.55852500000003), (-5.159, 492.878525), (-5.159, 492.66852500000005), (-11.984, 492.7079), (-11.984, 492.4979), (-0.3, 492.55), (-0.3, 492.1), (-5.159, 492.55852500000003), (-5.159, 492.23852500000004), (-5.159, 492.66852500000005), (-5.159, 492.458525), (-11.984, 492.4979), (-11.984, 492.2879)]</t>
+          <t>[(-0.3, 493.0), (-0.3, 492.68), (-5.159, 492.878525), (-5.159, 492.67852500000004), (-5.159, 492.878525), (-5.159, 492.768525), (-11.984, 492.7079), (-11.984, 492.5979), (-0.3, 492.68), (-0.3, 492.36), (-5.159, 492.67852500000004), (-5.159, 492.47852500000005), (-5.159, 492.768525), (-5.159, 492.48852500000004), (-11.984, 492.5979), (-11.984, 492.4079)]</t>
         </is>
       </c>
     </row>
@@ -5367,7 +5367,7 @@
       </c>
       <c r="B495" t="inlineStr">
         <is>
-          <t>[(-0.3, 494.0), (-0.3, 493.5), (-5.114, 493.87965), (-5.114, 493.47965000000005), (-5.114, 493.87965), (-5.114, 493.60965000000004), (-11.935, 493.709125), (-11.935, 493.439125), (-0.3, 493.5), (-0.3, 493.0), (-5.114, 493.47965000000005), (-5.114, 493.07965), (-5.114, 493.60965000000004), (-5.114, 493.33965), (-11.935, 493.439125), (-11.935, 493.16912499999995)]</t>
+          <t>[(-0.3, 494.0), (-0.3, 493.65), (-5.114, 493.87965), (-5.114, 493.63965), (-5.114, 493.87965), (-5.114, 493.68965000000003), (-11.935, 493.709125), (-11.935, 493.519125), (-0.3, 493.65), (-0.3, 493.3), (-5.114, 493.63965), (-5.114, 493.39965), (-5.114, 493.68965000000003), (-5.114, 493.38965), (-11.935, 493.519125), (-11.935, 493.369125)]</t>
         </is>
       </c>
     </row>
@@ -5377,7 +5377,7 @@
       </c>
       <c r="B496" t="inlineStr">
         <is>
-          <t>[(-0.3, 495.0), (-0.3, 494.5), (-5.078, 494.88055), (-5.078, 494.46055), (-5.078, 494.88055), (-5.078, 494.67055000000005), (-11.886, 494.71035), (-11.886, 494.50035), (-0.3, 494.5), (-0.3, 494.0), (-5.078, 494.46055), (-5.078, 494.04055000000005), (-5.078, 494.67055000000005), (-5.078, 494.46055), (-11.886, 494.50035), (-11.886, 494.29035)]</t>
+          <t>[(-0.3, 495.0), (-0.3, 494.66), (-5.078, 494.88055), (-5.078, 494.62055000000004), (-5.078, 494.88055), (-5.078, 494.61055000000005), (-11.886, 494.71035), (-11.886, 494.44035), (-0.3, 494.66), (-0.3, 494.32), (-5.078, 494.62055000000004), (-5.078, 494.36055000000005), (-5.078, 494.61055000000005), (-5.078, 494.35055000000006), (-11.886, 494.44035), (-11.886, 494.28035)]</t>
         </is>
       </c>
     </row>
@@ -5387,7 +5387,7 @@
       </c>
       <c r="B497" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 496.0), (-0.3, 495.78), (-5.063, 495.880925), (-5.063, 495.66092499999996), (-5.063, 495.880925), (-5.063, 495.680925), (-11.947, 495.708825), (-11.947, 495.508825), (-0.3, 495.78), (-0.3, 495.56), (-5.063, 495.66092499999996), (-5.063, 495.440925), (-5.063, 495.680925), (-5.063, 495.480925), (-11.947, 495.508825), (-11.947, 495.308825), (-0.3, 495.56), (-0.3, 495.36), (-5.063, 495.440925), (-5.063, 495.300925), (-5.063, 495.480925), (-5.063, 495.300925), (-11.947, 495.308825), (-11.947, 495.16882499999997)]</t>
         </is>
       </c>
     </row>
@@ -5397,7 +5397,7 @@
       </c>
       <c r="B498" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 497.0), (-0.3, 496.79), (-5.088, 496.8522459061705), (-5.088, 496.6422459061705), (-5.088, 496.8522459061705), (-5.088, 496.6622459061705), (-11.96, 496.6401811332389), (-11.96, 496.4501811332389), (-0.3, 496.79), (-0.3, 496.58), (-5.088, 496.6422459061705), (-5.088, 496.43224590617046), (-5.088, 496.6622459061705), (-5.088, 496.4722459061705), (-11.96, 496.4501811332389), (-11.96, 496.2601811332389), (-0.3, 496.58), (-0.3, 496.38), (-5.088, 496.43224590617046), (-5.088, 496.3222459061705), (-5.088, 496.4722459061705), (-5.088, 496.3222459061705), (-11.96, 496.2601811332389), (-11.96, 496.0801811332389)]</t>
         </is>
       </c>
     </row>
@@ -5407,7 +5407,7 @@
       </c>
       <c r="B499" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 498.0), (-0.3, 497.79), (-5.187, 497.80034608329106), (-5.187, 497.5903460832911), (-5.187, 497.80034608329106), (-5.187, 497.61034608329106), (-12.125, 497.51690043685636), (-12.125, 497.32690043685636), (-0.3, 497.79), (-0.3, 497.58), (-5.187, 497.5903460832911), (-5.187, 497.38034608329104), (-5.187, 497.61034608329106), (-5.187, 497.42034608329107), (-12.125, 497.32690043685636), (-12.125, 497.13690043685637), (-0.3, 497.58), (-0.3, 497.38), (-5.187, 497.38034608329104), (-5.187, 497.23034608329107), (-5.187, 497.42034608329107), (-5.187, 497.23034608329107), (-12.125, 497.13690043685637), (-12.125, 496.9869004368564)]</t>
         </is>
       </c>
     </row>
@@ -5417,7 +5417,7 @@
       </c>
       <c r="B500" t="inlineStr">
         <is>
-          <t>[(-0.3, 499.0), (-0.3, 498.71), (-5.357, 498.74285700980244), (-5.357, 498.4528570098024), (-5.357, 498.74285700980244), (-5.357, 498.5028570098024), (-12.301, 498.389762106909), (-12.301, 498.149762106909), (-0.3, 498.71), (-0.3, 498.42), (-5.357, 498.4528570098024), (-5.357, 498.16285700980245), (-5.357, 498.5028570098024), (-5.357, 498.2628570098024), (-12.301, 498.149762106909), (-12.301, 497.909762106909), (-0.3, 498.42), (-0.3, 498.14), (-5.357, 498.16285700980245), (-5.357, 498.0228570098024), (-5.357, 498.2628570098024), (-5.357, 498.0228570098024), (-12.301, 497.909762106909), (-12.301, 497.779762106909)]</t>
+          <t>[(-0.3, 499.0), (-0.3, 498.64), (-5.357, 498.74285700980244), (-5.357, 498.4528570098024), (-5.357, 498.74285700980244), (-5.357, 498.4528570098024), (-12.301, 498.389762106909), (-12.301, 498.099762106909), (-0.3, 498.64), (-0.3, 498.28), (-5.357, 498.4528570098024), (-5.357, 498.16285700980245), (-5.357, 498.4528570098024), (-5.357, 498.16285700980245), (-12.301, 498.099762106909), (-12.301, 497.909762106909)]</t>
         </is>
       </c>
     </row>
@@ -5427,7 +5427,7 @@
       </c>
       <c r="B501" t="inlineStr">
         <is>
-          <t>[(-0.3, 500.0), (-0.3, 499.72), (-5.533, 499.68160462999606), (-5.533, 499.4016046299961), (-5.533, 499.68160462999606), (-5.533, 499.3416046299961), (-12.507, 499.2572802825075), (-12.507, 499.0172802825075), (-0.3, 499.72), (-0.3, 499.44), (-5.533, 499.4016046299961), (-5.533, 499.12160462999606), (-5.533, 499.3416046299961), (-5.533, 499.00160462999605), (-12.507, 499.0172802825075), (-12.507, 498.7772802825075), (-0.3, 499.44), (-0.3, 499.17), (-5.533, 499.12160462999606), (-5.533, 499.01160462999604), (-5.533, 499.00160462999605), (-5.533, 499.00160462999605), (-12.507, 498.7772802825075), (-12.507, 498.7772802825075)]</t>
+          <t>[(-0.3, 500.0), (-0.3, 499.63), (-5.533, 499.68160462999606), (-5.533, 499.4016046299961), (-5.533, 499.68160462999606), (-5.533, 499.4016046299961), (-12.507, 499.2572802825075), (-12.507, 499.0772802825075), (-0.3, 499.63), (-0.3, 499.26), (-5.533, 499.4016046299961), (-5.533, 499.12160462999606), (-5.533, 499.4016046299961), (-5.533, 499.12160462999606), (-12.507, 499.0772802825075), (-12.507, 498.8972802825075)]</t>
         </is>
       </c>
     </row>
@@ -5437,7 +5437,7 @@
       </c>
       <c r="B502" t="inlineStr">
         <is>
-          <t>[(-0.3, 501.0), (-0.3, 500.6), (-5.774, 500.61682), (-5.774, 500.31682), (-5.774, 500.61682), (-5.774, 500.31682), (-12.784, 500.12612), (-12.784, 499.82612), (-0.3, 500.6), (-0.3, 500.2), (-5.774, 500.31682), (-5.774, 500.01682), (-5.774, 500.31682), (-5.774, 500.02682000000004), (-12.784, 499.82612), (-12.784, 499.71612)]</t>
+          <t>[(-0.3, 501.0), (-0.3, 500.62), (-5.774, 500.61682), (-5.774, 500.35682), (-5.774, 500.61682), (-5.774, 500.38682), (-12.784, 500.12612), (-12.784, 499.89612), (-0.3, 500.62), (-0.3, 500.24), (-5.774, 500.35682), (-5.774, 500.09682000000004), (-5.774, 500.38682), (-5.774, 500.08682000000005), (-12.784, 499.89612), (-12.784, 499.76612)]</t>
         </is>
       </c>
     </row>
@@ -5447,7 +5447,7 @@
       </c>
       <c r="B503" t="inlineStr">
         <is>
-          <t>[(-0.3, 502.0), (-0.3, 501.65), (-5.857, 501.61101), (-5.857, 501.38101), (-5.857, 501.61101), (-5.857, 501.38101), (-12.779, 501.12647), (-12.779, 500.99647), (-0.3, 501.65), (-0.3, 501.3), (-5.857, 501.38101), (-5.857, 501.15101000000004), (-5.857, 501.38101), (-5.857, 501.15101000000004), (-12.779, 500.99647), (-12.779, 500.86647)]</t>
+          <t>[(-0.3, 502.0), (-0.3, 501.66), (-5.857, 501.61101), (-5.857, 501.39101), (-5.857, 501.61101), (-5.857, 501.39101), (-12.779, 501.12647), (-12.779, 501.00647), (-0.3, 501.66), (-0.3, 501.32), (-5.857, 501.39101), (-5.857, 501.17101), (-5.857, 501.39101), (-5.857, 501.17101), (-12.779, 501.00647), (-12.779, 500.88647)]</t>
         </is>
       </c>
     </row>
@@ -5457,7 +5457,7 @@
       </c>
       <c r="B504" t="inlineStr">
         <is>
-          <t>[(-0.3, 503.0), (-0.3, 502.68), (-5.904, 502.60772), (-5.904, 502.37771999999995), (-5.904, 502.60772), (-5.904, 502.37771999999995), (-12.805, 502.12465), (-12.805, 501.99465), (-0.3, 502.68), (-0.3, 502.36), (-5.904, 502.37771999999995), (-5.904, 502.14772), (-5.904, 502.37771999999995), (-5.904, 502.14772), (-12.805, 501.99465), (-12.805, 501.86465)]</t>
+          <t>[(-0.3, 503.0), (-0.3, 502.66), (-5.904, 502.60772), (-5.904, 502.35772), (-5.904, 502.60772), (-5.904, 502.35772), (-12.805, 502.12465), (-12.805, 501.98465), (-0.3, 502.66), (-0.3, 502.32), (-5.904, 502.35772), (-5.904, 502.10772), (-5.904, 502.35772), (-5.904, 502.10772), (-12.805, 501.98465), (-12.805, 501.84465)]</t>
         </is>
       </c>
     </row>
@@ -5467,7 +5467,7 @@
       </c>
       <c r="B505" t="inlineStr">
         <is>
-          <t>[(-0.3, 504.0), (-0.3, 503.64), (-5.981, 503.60233), (-5.981, 503.36233), (-5.981, 503.60233), (-5.981, 503.41233), (-12.864, 503.12052), (-12.864, 502.93052), (-0.3, 503.64), (-0.3, 503.28), (-5.981, 503.36233), (-5.981, 503.12233), (-5.981, 503.41233), (-5.981, 503.11233), (-12.864, 502.93052), (-12.864, 502.77052)]</t>
+          <t>[(-0.3, 504.0), (-0.3, 503.6), (-5.981, 503.60233), (-5.981, 503.32233), (-5.981, 503.60233), (-5.981, 503.31233), (-12.864, 503.12052), (-12.864, 502.83052), (-0.3, 503.6), (-0.3, 503.2), (-5.981, 503.32233), (-5.981, 503.04233), (-5.981, 503.31233), (-5.981, 503.03233), (-12.864, 502.83052), (-12.864, 502.70052)]</t>
         </is>
       </c>
     </row>
@@ -5477,7 +5477,7 @@
       </c>
       <c r="B506" t="inlineStr">
         <is>
-          <t>[(-0.3, 505.0), (-0.3, 504.66), (-5.857, 504.61101), (-5.857, 504.35101000000003), (-5.857, 504.61101), (-5.857, 504.35101000000003), (-12.727, 504.13011), (-12.727, 503.97011), (-0.3, 504.66), (-0.3, 504.32), (-5.857, 504.35101000000003), (-5.857, 504.09101000000004), (-5.857, 504.35101000000003), (-5.857, 504.09101000000004), (-12.727, 503.97011), (-12.727, 503.81011)]</t>
+          <t>[(-0.3, 505.0), (-0.3, 504.6), (-5.857, 504.61101), (-5.857, 504.30101), (-5.857, 504.61101), (-5.857, 504.30101), (-12.727, 504.13011), (-12.727, 503.91011), (-0.3, 504.6), (-0.3, 504.2), (-5.857, 504.30101), (-5.857, 503.99101), (-5.857, 504.30101), (-5.857, 503.99101), (-12.727, 503.91011), (-12.727, 503.69011)]</t>
         </is>
       </c>
     </row>
@@ -5487,7 +5487,7 @@
       </c>
       <c r="B507" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 506.0), (-0.3, 505.62), (-5.566, 505.63138), (-5.566, 505.37138), (-5.566, 505.63138), (-5.566, 505.40137999999996), (-12.448, 505.14964), (-12.448, 504.91963999999996), (-0.3, 505.62), (-0.3, 505.24), (-5.566, 505.37138), (-5.566, 505.11138), (-5.566, 505.40137999999996), (-5.566, 505.10138), (-12.448, 504.91963999999996), (-12.448, 504.80964)]</t>
         </is>
       </c>
     </row>
@@ -5497,7 +5497,7 @@
       </c>
       <c r="B508" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 507.0), (-0.3, 506.71), (-5.221, 506.65559939136335), (-5.221, 506.36559939136333), (-5.221, 506.65559939136335), (-5.221, 506.54559939136334), (-12.118, 506.1729066464402), (-12.118, 506.0629066464402), (-0.3, 506.71), (-0.3, 506.42), (-5.221, 506.36559939136333), (-5.221, 506.2555993913634), (-5.221, 506.54559939136334), (-5.221, 506.2555993913634), (-12.118, 506.0629066464402), (-12.118, 505.9229066464402)]</t>
         </is>
       </c>
     </row>
@@ -5507,7 +5507,7 @@
       </c>
       <c r="B509" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 508.0), (-0.3, 507.74), (-4.862, 507.7263207648414), (-4.862, 507.4663207648414), (-4.862, 507.7263207648414), (-4.862, 507.61632076484136), (-11.663, 507.3183215368024), (-11.663, 507.2083215368024), (-0.3, 507.74), (-0.3, 507.48), (-4.862, 507.4663207648414), (-4.862, 507.3263207648414), (-4.862, 507.61632076484136), (-4.862, 507.3263207648414), (-11.663, 507.2083215368024), (-11.663, 507.0683215368024)]</t>
         </is>
       </c>
     </row>
@@ -5517,7 +5517,7 @@
       </c>
       <c r="B510" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 509.0), (-0.3, 508.81), (-4.666, 508.7817164616033), (-4.666, 508.5917164616033), (-4.666, 508.7817164616033), (-4.666, 508.6717164616033), (-11.551, 508.43749242086557), (-11.551, 508.32749242086555), (-0.3, 508.81), (-0.3, 508.51), (-4.666, 508.5917164616033), (-4.666, 508.4317164616033), (-4.666, 508.6717164616033), (-4.666, 508.4317164616033), (-11.551, 508.32749242086555), (-11.551, 508.18749242086557)]</t>
         </is>
       </c>
     </row>
@@ -5527,7 +5527,7 @@
       </c>
       <c r="B511" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 510.0), (-0.3, 509.79), (-4.571, 509.8291540422877), (-4.571, 509.61915404228773), (-4.571, 509.8291540422877), (-4.571, 509.7191540422877), (-11.467, 509.5533044229049), (-11.467, 509.4433044229049), (-0.3, 509.79), (-0.3, 509.58), (-4.571, 509.61915404228773), (-4.571, 509.5091540422877), (-4.571, 509.7191540422877), (-4.571, 509.5091540422877), (-11.467, 509.4433044229049), (-11.467, 509.3033044229049)]</t>
         </is>
       </c>
     </row>
@@ -5537,7 +5537,7 @@
       </c>
       <c r="B512" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 511.0), (-0.3, 510.89), (-4.512, 510.8736123682158), (-4.512, 510.7636123682158), (-4.512, 510.8736123682158), (-4.512, 510.7336123682158), (-11.402, 510.666867168075), (-11.402, 510.526867168075), (-0.3, 510.89), (-0.3, 510.65), (-4.512, 510.7636123682158), (-4.512, 510.6136123682158), (-4.512, 510.7336123682158), (-4.512, 510.6136123682158), (-11.402, 510.526867168075), (-11.402, 510.416867168075)]</t>
         </is>
       </c>
     </row>
@@ -5547,7 +5547,7 @@
       </c>
       <c r="B513" t="inlineStr">
         <is>
-          <t>[(-0.3, 512.0), (-0.3, 511.89), (-4.393, 511.9270935479339), (-4.393, 511.8170935479339), (-4.393, 511.9270935479339), (-4.393, 511.77709354793393), (-11.313, 511.80383123464367), (-11.313, 511.6538312346437), (-0.3, 511.89), (-0.3, 511.63), (-4.393, 511.8170935479339), (-4.393, 511.64709354793393), (-4.393, 511.77709354793393), (-4.393, 511.64709354793393), (-11.313, 511.6538312346437), (-11.313, 511.3538312346437)]</t>
+          <t>[(-0.3, 512.0), (-0.3, 511.8), (-4.393, 511.9270935479339), (-4.393, 511.7270935479339), (-4.393, 511.9270935479339), (-4.393, 511.7470935479339), (-11.313, 511.80383123464367), (-11.313, 511.62383123464366), (-0.3, 511.8), (-0.3, 511.6), (-4.393, 511.7270935479339), (-4.393, 511.6170935479339), (-4.393, 511.7470935479339), (-4.393, 511.6170935479339), (-11.313, 511.62383123464366), (-11.313, 511.32383123464365)]</t>
         </is>
       </c>
     </row>
@@ -5557,7 +5557,7 @@
       </c>
       <c r="B514" t="inlineStr">
         <is>
-          <t>[(-0.3, 513.0), (-0.3, 512.76), (-4.237, 512.9865706123701), (-4.237, 512.7465706123701), (-4.237, 512.9865706123701), (-4.237, 512.77657061237), (-11.169, 512.962925066256), (-11.169, 512.6529250662561), (-0.3, 512.76), (-0.3, 512.52), (-4.237, 512.7465706123701), (-4.237, 512.5665706123701), (-4.237, 512.77657061237), (-4.237, 512.5665706123701), (-11.169, 512.6529250662561), (-11.169, 512.342925066256)]</t>
+          <t>[(-0.3, 513.0), (-0.3, 512.75), (-4.237, 512.9865706123701), (-4.237, 512.7365706123701), (-4.237, 512.9865706123701), (-4.237, 512.7665706123701), (-11.169, 512.962925066256), (-11.169, 512.642925066256), (-0.3, 512.75), (-0.3, 512.5), (-4.237, 512.7365706123701), (-4.237, 512.54657061237), (-4.237, 512.7665706123701), (-4.237, 512.54657061237), (-11.169, 512.642925066256), (-11.169, 512.3229250662561)]</t>
         </is>
       </c>
     </row>
@@ -5567,7 +5567,7 @@
       </c>
       <c r="B515" t="inlineStr">
         <is>
-          <t>[(-0.3, 514.0), (-0.3, 513.73), (-4.16, 514.0424226755699), (-4.16, 513.7724226755699), (-4.16, 514.0424226755699), (-4.16, 513.8124226755699), (-11.078, 514.1184537816821), (-11.078, 513.798453781682), (-0.3, 513.73), (-0.3, 513.47), (-4.16, 513.7724226755699), (-4.16, 513.5824226755699), (-4.16, 513.8124226755699), (-4.16, 513.5824226755699), (-11.078, 513.798453781682), (-11.078, 513.4784537816821)]</t>
+          <t>[(-0.3, 514.0), (-0.3, 513.72), (-4.16, 514.0424226755699), (-4.16, 513.76242267557), (-4.16, 514.0424226755699), (-4.16, 513.8024226755699), (-11.078, 514.1184537816821), (-11.078, 513.788453781682), (-0.3, 513.72), (-0.3, 513.45), (-4.16, 513.76242267557), (-4.16, 513.5624226755699), (-4.16, 513.8024226755699), (-4.16, 513.5624226755699), (-11.078, 513.788453781682), (-11.078, 513.4584537816821)]</t>
         </is>
       </c>
     </row>
@@ -5577,7 +5577,7 @@
       </c>
       <c r="B516" t="inlineStr">
         <is>
-          <t>[(-0.3, 515.0), (-0.3, 514.85), (-4.027, 515.0942611932987), (-4.027, 514.9442611932988), (-4.027, 515.0942611932987), (-4.027, 514.8142611932988), (-10.92, 515.2685950825953), (-10.92, 514.9885950825953), (-0.3, 514.85), (-0.3, 514.7), (-4.027, 514.9442611932988), (-4.027, 514.7942611932988), (-4.027, 514.8142611932988), (-4.027, 514.6642611932988), (-10.92, 514.9885950825953), (-10.92, 514.7185950825954), (-0.3, 514.7), (-0.3, 514.58), (-4.027, 514.7942611932988), (-4.027, 514.6642611932988), (-4.027, 514.6642611932988), (-4.027, 514.6642611932988), (-10.92, 514.7185950825954), (-10.92, 514.7185950825954)]</t>
+          <t>[(-0.3, 515.0), (-0.3, 514.85), (-4.027, 515.0942611932987), (-4.027, 514.9442611932988), (-4.027, 515.0942611932987), (-4.027, 514.8042611932988), (-10.92, 515.2685950825953), (-10.92, 514.9785950825953), (-0.3, 514.85), (-0.3, 514.7), (-4.027, 514.9442611932988), (-4.027, 514.7942611932988), (-4.027, 514.8042611932988), (-4.027, 514.6542611932987), (-10.92, 514.9785950825953), (-10.92, 514.6985950825953), (-0.3, 514.7), (-0.3, 514.57), (-4.027, 514.7942611932988), (-4.027, 514.6542611932987), (-4.027, 514.6542611932987), (-4.027, 514.6542611932987), (-10.92, 514.6985950825953), (-10.92, 514.6985950825953)]</t>
         </is>
       </c>
     </row>
@@ -5587,7 +5587,7 @@
       </c>
       <c r="B517" t="inlineStr">
         <is>
-          <t>[(-0.3, 516.0), (-0.3, 515.86), (-3.916, 516.1301967007082), (-3.916, 515.9901967007082), (-3.916, 516.1301967007082), (-3.916, 515.8701967007082), (-10.782, 516.377412006865), (-10.782, 516.117412006865), (-0.3, 515.86), (-0.3, 515.72), (-3.916, 515.9901967007082), (-3.916, 515.8501967007082), (-3.916, 515.8701967007082), (-3.916, 515.7301967007082), (-10.782, 516.117412006865), (-10.782, 515.857412006865), (-0.3, 515.72), (-0.3, 515.6), (-3.916, 515.8501967007082), (-3.916, 515.7301967007082), (-3.916, 515.7301967007082), (-3.916, 515.7301967007082), (-10.782, 515.857412006865), (-10.782, 515.857412006865)]</t>
+          <t>[(-0.3, 516.0), (-0.3, 515.85), (-3.916, 516.1301967007082), (-3.916, 515.9801967007082), (-3.916, 516.1301967007082), (-3.916, 515.8601967007082), (-10.782, 516.377412006865), (-10.782, 516.107412006865), (-0.3, 515.85), (-0.3, 515.7), (-3.916, 515.9801967007082), (-3.916, 515.8301967007083), (-3.916, 515.8601967007082), (-3.916, 515.7201967007082), (-10.782, 516.107412006865), (-10.782, 515.847412006865), (-0.3, 515.7), (-0.3, 515.58), (-3.916, 515.8301967007083), (-3.916, 515.7201967007082), (-3.916, 515.7201967007082), (-3.916, 515.7201967007082), (-10.782, 515.847412006865), (-10.782, 515.847412006865)]</t>
         </is>
       </c>
     </row>
@@ -5597,7 +5597,7 @@
       </c>
       <c r="B518" t="inlineStr">
         <is>
-          <t>[(-0.3, 517.0), (-0.3, 516.79), (-4.131, 517.1789843601017), (-4.131, 516.9689843601017), (-4.131, 517.1789843601017), (-4.131, 516.9289843601017), (-10.953, 517.4977082715121), (-10.953, 517.2477082715121), (-0.3, 516.79), (-0.3, 516.59), (-4.131, 516.9689843601017), (-4.131, 516.8089843601017), (-4.131, 516.9289843601017), (-4.131, 516.8089843601017), (-10.953, 517.2477082715121), (-10.953, 516.9977082715121)]</t>
+          <t>[(-0.3, 517.0), (-0.3, 516.79), (-4.131, 517.1789843601017), (-4.131, 516.9689843601017), (-4.131, 517.1789843601017), (-4.131, 516.9189843601017), (-10.953, 517.4977082715121), (-10.953, 517.2377082715121), (-0.3, 516.79), (-0.3, 516.58), (-4.131, 516.9689843601017), (-4.131, 516.7989843601017), (-4.131, 516.9189843601017), (-4.131, 516.7989843601017), (-10.953, 517.2377082715121), (-10.953, 516.9877082715121)]</t>
         </is>
       </c>
     </row>
@@ -5607,7 +5607,7 @@
       </c>
       <c r="B519" t="inlineStr">
         <is>
-          <t>[(-0.3, 518.0), (-0.3, 517.77), (-4.733, 518.2546062349746), (-4.733, 518.0246062349746), (-4.733, 518.2546062349746), (-4.733, 518.0246062349746), (-11.574, 518.6475142551554), (-11.574, 518.3275142551554), (-0.3, 517.77), (-0.3, 517.59), (-4.733, 518.0246062349746), (-4.733, 517.7946062349746), (-4.733, 518.0246062349746), (-4.733, 517.7946062349746), (-11.574, 518.3275142551554), (-11.574, 518.0075142551555)]</t>
+          <t>[(-0.3, 518.0), (-0.3, 517.76), (-4.733, 518.2546062349746), (-4.733, 518.0146062349746), (-4.733, 518.2546062349746), (-4.733, 518.0146062349746), (-11.574, 518.6475142551554), (-11.574, 518.3275142551554), (-0.3, 517.76), (-0.3, 517.58), (-4.733, 518.0146062349746), (-4.733, 517.7846062349746), (-4.733, 518.0146062349746), (-4.733, 517.7746062349746), (-11.574, 518.3275142551554), (-11.574, 518.0075142551555)]</t>
         </is>
       </c>
     </row>
@@ -5617,7 +5617,7 @@
       </c>
       <c r="B520" t="inlineStr">
         <is>
-          <t>[(-0.3, 519.0), (-0.3, 518.75), (-5.234, 519.3362451030761), (-5.234, 519.0862451030761), (-5.234, 519.3362451030761), (-5.234, 519.0862451030761), (-12.18, 519.8096051529274), (-12.18, 519.4696051529273), (-0.3, 518.75), (-0.3, 518.6), (-5.234, 519.0862451030761), (-5.234, 518.8362451030761), (-5.234, 519.0862451030761), (-5.234, 518.8362451030761), (-12.18, 519.4696051529273), (-12.18, 519.1296051529274)]</t>
+          <t>[(-0.3, 519.0), (-0.3, 518.74), (-5.234, 519.3362451030761), (-5.234, 519.0762451030761), (-5.234, 519.3362451030761), (-5.234, 519.0762451030761), (-12.18, 519.8096051529274), (-12.18, 519.4596051529273), (-0.3, 518.74), (-0.3, 518.59), (-5.234, 519.0762451030761), (-5.234, 518.8262451030761), (-5.234, 519.0762451030761), (-5.234, 518.8162451030761), (-12.18, 519.4596051529273), (-12.18, 519.1096051529273)]</t>
         </is>
       </c>
     </row>
@@ -5627,7 +5627,7 @@
       </c>
       <c r="B521" t="inlineStr">
         <is>
-          <t>[(-0.3, 520.0), (-0.3, 519.73), (-5.555, 520.36785), (-5.555, 520.09785), (-5.555, 520.36785), (-5.555, 520.10785), (-12.458, 520.85106), (-12.458, 520.5110599999999), (-0.3, 519.73), (-0.3, 519.55), (-5.555, 520.09785), (-5.555, 519.83785), (-5.555, 520.10785), (-5.555, 519.84785), (-12.458, 520.5110599999999), (-12.458, 520.17106)]</t>
+          <t>[(-0.3, 520.0), (-0.3, 519.73), (-5.555, 520.36785), (-5.555, 520.09785), (-5.555, 520.36785), (-5.555, 520.09785), (-12.458, 520.85106), (-12.458, 520.5110599999999), (-0.3, 519.73), (-0.3, 519.55), (-5.555, 520.09785), (-5.555, 519.82785), (-5.555, 520.09785), (-5.555, 519.82785), (-12.458, 520.5110599999999), (-12.458, 520.17106)]</t>
         </is>
       </c>
     </row>
@@ -5637,7 +5637,7 @@
       </c>
       <c r="B522" t="inlineStr">
         <is>
-          <t>[(-0.3, 521.0), (-0.3, 520.75), (-5.537, 521.36659), (-5.537, 521.11659), (-5.537, 521.36659), (-5.537, 521.11659), (-12.466, 521.85162), (-12.466, 521.52162), (-0.3, 520.75), (-0.3, 520.6), (-5.537, 521.11659), (-5.537, 520.86659), (-5.537, 521.11659), (-5.537, 520.86659), (-12.466, 521.52162), (-12.466, 521.1916200000001)]</t>
+          <t>[(-0.3, 521.0), (-0.3, 520.75), (-5.537, 521.36659), (-5.537, 521.11659), (-5.537, 521.36659), (-5.537, 521.11659), (-12.466, 521.85162), (-12.466, 521.51162), (-0.3, 520.75), (-0.3, 520.6), (-5.537, 521.11659), (-5.537, 520.86659), (-5.537, 521.11659), (-5.537, 520.86659), (-12.466, 521.51162), (-12.466, 521.1716200000001)]</t>
         </is>
       </c>
     </row>
@@ -5747,7 +5747,7 @@
       </c>
       <c r="B533" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 532.0), (-0.3, 531.89), (-7.239, 531.8360117809314), (-7.239, 531.7260117809313), (-0.3, 531.89), (-0.3, 531.66), (-7.239, 531.7260117809313), (-7.239, 531.5860117809314)]</t>
         </is>
       </c>
     </row>
@@ -5787,7 +5787,7 @@
       </c>
       <c r="B537" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 536.0), (-0.3, 535.87), (-7.123, 535.829425), (-7.123, 535.699425), (-0.3, 535.87), (-0.3, 535.75), (-7.123, 535.699425), (-7.123, 535.579425)]</t>
         </is>
       </c>
     </row>
@@ -5837,7 +5837,7 @@
       </c>
       <c r="B542" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 541.0), (-0.3, 540.87), (-6.828, 540.8368), (-6.828, 540.7068), (-0.3, 540.87), (-0.3, 540.75), (-6.828, 540.7068), (-6.828, 540.5868)]</t>
         </is>
       </c>
     </row>
@@ -5847,7 +5847,7 @@
       </c>
       <c r="B543" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 542.0), (-0.3, 541.87), (-6.768, 541.8383), (-6.768, 541.7083), (-0.3, 541.87), (-0.3, 541.75), (-6.768, 541.7083), (-6.768, 541.5883)]</t>
         </is>
       </c>
     </row>
@@ -5857,7 +5857,7 @@
       </c>
       <c r="B544" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 543.0), (-0.3, 542.87), (-6.686, 542.84035), (-6.686, 542.71035), (-0.3, 542.87), (-0.3, 542.75), (-6.686, 542.71035), (-6.686, 542.59035)]</t>
         </is>
       </c>
     </row>
@@ -5867,7 +5867,7 @@
       </c>
       <c r="B545" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 544.0), (-0.3, 543.87), (-6.632, 543.8417), (-6.632, 543.7117), (-0.3, 543.87), (-0.3, 543.75), (-6.632, 543.7117), (-6.632, 543.5917)]</t>
         </is>
       </c>
     </row>
@@ -5877,7 +5877,7 @@
       </c>
       <c r="B546" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 545.0), (-0.3, 544.87), (-6.632, 544.8417), (-6.632, 544.7117), (-0.3, 544.87), (-0.3, 544.75), (-6.632, 544.7117), (-6.632, 544.5917)]</t>
         </is>
       </c>
     </row>
@@ -5887,7 +5887,7 @@
       </c>
       <c r="B547" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 546.0), (-0.3, 545.87), (-6.624, 545.8419), (-6.624, 545.7119), (-0.3, 545.87), (-0.3, 545.75), (-6.624, 545.7119), (-6.624, 545.5919)]</t>
         </is>
       </c>
     </row>
@@ -5897,7 +5897,7 @@
       </c>
       <c r="B548" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 547.0), (-0.3, 546.87), (-6.615, 546.842125), (-6.615, 546.712125), (-0.3, 546.87), (-0.3, 546.75), (-6.615, 546.712125), (-6.615, 546.592125)]</t>
         </is>
       </c>
     </row>
@@ -5907,7 +5907,7 @@
       </c>
       <c r="B549" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 548.0), (-0.3, 547.87), (-6.603, 547.842425), (-6.603, 547.712425), (-0.3, 547.87), (-0.3, 547.75), (-6.603, 547.712425), (-6.603, 547.592425)]</t>
         </is>
       </c>
     </row>
@@ -5917,7 +5917,7 @@
       </c>
       <c r="B550" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 549.0), (-0.3, 548.87), (-6.588, 548.8428), (-6.588, 548.7128), (-0.3, 548.87), (-0.3, 548.75), (-6.588, 548.7128), (-6.588, 548.5928)]</t>
         </is>
       </c>
     </row>
@@ -5927,7 +5927,7 @@
       </c>
       <c r="B551" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 550.0), (-0.3, 549.87), (-6.566, 549.84335), (-6.566, 549.71335), (-0.3, 549.87), (-0.3, 549.75), (-6.566, 549.71335), (-6.566, 549.59335)]</t>
         </is>
       </c>
     </row>
@@ -5937,7 +5937,7 @@
       </c>
       <c r="B552" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 551.0), (-0.3, 550.87), (-6.624, 550.8419), (-6.624, 550.7119), (-0.3, 550.87), (-0.3, 550.75), (-6.624, 550.7119), (-6.624, 550.5919)]</t>
         </is>
       </c>
     </row>
@@ -5947,7 +5947,7 @@
       </c>
       <c r="B553" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 552.0), (-0.3, 551.87), (-6.746, 551.83885), (-6.746, 551.70885), (-0.3, 551.87), (-0.3, 551.75), (-6.746, 551.70885), (-6.746, 551.58885)]</t>
         </is>
       </c>
     </row>
@@ -5957,7 +5957,7 @@
       </c>
       <c r="B554" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 553.0), (-0.3, 552.87), (-6.891, 552.835225), (-6.891, 552.705225), (-0.3, 552.87), (-0.3, 552.75), (-6.891, 552.705225), (-6.891, 552.585225)]</t>
         </is>
       </c>
     </row>
@@ -5967,7 +5967,7 @@
       </c>
       <c r="B555" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 554.0), (-0.3, 553.87), (-7.062, 553.83095), (-7.062, 553.70095), (-0.3, 553.87), (-0.3, 553.75), (-7.062, 553.70095), (-7.062, 553.58095)]</t>
         </is>
       </c>
     </row>
@@ -5977,7 +5977,7 @@
       </c>
       <c r="B556" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 555.0), (-0.3, 554.87), (-10.218, 554.75205), (-10.218, 554.6220500000001), (-0.3, 554.87), (-0.3, 554.75), (-10.218, 554.6220500000001), (-10.218, 554.50205)]</t>
         </is>
       </c>
     </row>
@@ -5987,7 +5987,7 @@
       </c>
       <c r="B557" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 556.0), (-0.3, 555.87), (-9.355, 555.773625), (-9.355, 555.643625), (-0.3, 555.87), (-0.3, 555.75), (-9.355, 555.643625), (-9.355, 555.523625)]</t>
         </is>
       </c>
     </row>
@@ -5997,7 +5997,7 @@
       </c>
       <c r="B558" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 557.0), (-0.3, 556.87), (-8.685, 556.790375), (-8.685, 556.660375), (-0.3, 556.87), (-0.3, 556.75), (-8.685, 556.660375), (-8.685, 556.540375)]</t>
         </is>
       </c>
     </row>
@@ -6007,7 +6007,7 @@
       </c>
       <c r="B559" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 558.0), (-0.3, 557.87), (-8.126, 557.80435), (-8.126, 557.67435), (-0.3, 557.87), (-0.3, 557.75), (-8.126, 557.67435), (-8.126, 557.55435)]</t>
         </is>
       </c>
     </row>
@@ -6017,7 +6017,7 @@
       </c>
       <c r="B560" t="inlineStr">
         <is>
-          <t>[(-0.3, 559.0), (-0.3, 558.86), (-7.618, 558.81705), (-7.618, 558.67705), (-0.3, 558.86), (-0.3, 558.73), (-7.618, 558.67705), (-7.618, 558.56705)]</t>
+          <t>[(-0.3, 559.0), (-0.3, 558.87), (-7.618, 558.81705), (-7.618, 558.68705), (-0.3, 558.87), (-0.3, 558.75), (-7.618, 558.68705), (-7.618, 558.56705)]</t>
         </is>
       </c>
     </row>
@@ -6027,7 +6027,7 @@
       </c>
       <c r="B561" t="inlineStr">
         <is>
-          <t>[(-0.3, 560.0), (-0.3, 559.82), (-7.298, 559.82505), (-7.298, 559.6450500000001), (-0.3, 559.82), (-0.3, 559.64), (-7.298, 559.6450500000001), (-7.298, 559.5150500000001)]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6037,7 +6037,7 @@
       </c>
       <c r="B562" t="inlineStr">
         <is>
-          <t>[(-0.3, 561.0), (-0.3, 560.82), (-7.039, 560.831525), (-7.039, 560.6515250000001), (-0.3, 560.82), (-0.3, 560.65), (-7.039, 560.6515250000001), (-7.039, 560.5215250000001)]</t>
+          <t>[(-0.3, 561.0), (-0.3, 560.81), (-7.039, 560.831525), (-7.039, 560.641525), (-0.3, 560.81), (-0.3, 560.63), (-7.039, 560.641525), (-7.039, 560.511525)]</t>
         </is>
       </c>
     </row>
@@ -6047,7 +6047,7 @@
       </c>
       <c r="B563" t="inlineStr">
         <is>
-          <t>[(-0.3, 562.0), (-0.3, 561.89), (-6.683, 561.840425), (-6.683, 561.730425), (-0.3, 561.89), (-0.3, 561.61), (-6.683, 561.730425), (-6.683, 561.560425)]</t>
+          <t>[(-0.3, 562.0), (-0.3, 561.74), (-6.683, 561.840425), (-6.683, 561.580425), (-0.3, 561.74), (-0.3, 561.48), (-6.683, 561.580425), (-6.683, 561.420425)]</t>
         </is>
       </c>
     </row>
@@ -6057,7 +6057,7 @@
       </c>
       <c r="B564" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 563.0), (-0.3, 562.68), (-6.372, 562.852504150004), (-6.372, 562.612504150004), (-0.3, 562.68), (-0.3, 562.36), (-6.372, 562.612504150004), (-6.372, 562.372504150004)]</t>
         </is>
       </c>
     </row>
@@ -6067,7 +6067,7 @@
       </c>
       <c r="B565" t="inlineStr">
         <is>
-          <t>[(-0.3, 564.0), (-0.3, 563.84), (-6.054, 564.0040787350335), (-6.054, 563.8440787350336), (-0.3, 563.84), (-0.3, 563.68), (-6.054, 563.8440787350336), (-6.054, 563.7340787350336)]</t>
+          <t>[(-0.3, 564.0), (-0.3, 563.79), (-6.054, 564.0040787350335), (-6.054, 563.7940787350335), (-0.3, 563.79), (-0.3, 563.58), (-6.054, 563.7940787350335), (-6.054, 563.5840787350336), (-0.3, 563.58), (-0.3, 563.38), (-6.054, 563.5840787350336), (-6.054, 563.4340787350335)]</t>
         </is>
       </c>
     </row>
@@ -6077,7 +6077,7 @@
       </c>
       <c r="B566" t="inlineStr">
         <is>
-          <t>[(-0.3, 565.0), (-0.3, 564.83), (-5.826, 565.1394990070415), (-5.826, 564.9694990070416), (-0.3, 564.83), (-0.3, 564.67), (-5.826, 564.9694990070416), (-5.826, 564.8194990070415)]</t>
+          <t>[(-0.3, 565.0), (-0.3, 564.84), (-5.826, 565.1394990070415), (-5.826, 564.9794990070416), (-0.3, 564.84), (-0.3, 564.68), (-5.826, 564.9794990070416), (-5.826, 564.8194990070415), (-0.3, 564.68), (-0.3, 564.52), (-5.826, 564.8194990070415), (-5.826, 564.6594990070415), (-0.3, 564.52), (-0.3, 564.38), (-5.826, 564.6594990070415), (-5.826, 564.5294990070415)]</t>
         </is>
       </c>
     </row>
@@ -6087,7 +6087,7 @@
       </c>
       <c r="B567" t="inlineStr">
         <is>
-          <t>[(-0.3, 566.0), (-0.3, 565.84), (-5.72, 566.1834876710203), (-5.72, 566.0234876710203), (-0.3, 565.84), (-0.3, 565.73), (-5.72, 566.0234876710203), (-5.72, 565.8734876710204)]</t>
+          <t>[(-0.3, 566.0), (-0.3, 565.8), (-5.72, 566.1834876710203), (-5.72, 565.9834876710203), (-0.3, 565.8), (-0.3, 565.6), (-5.72, 565.9834876710203), (-5.72, 565.7834876710203), (-0.3, 565.6), (-0.3, 565.46), (-5.72, 565.7834876710203), (-5.72, 565.6034876710203)]</t>
         </is>
       </c>
     </row>
@@ -6097,7 +6097,7 @@
       </c>
       <c r="B568" t="inlineStr">
         <is>
-          <t>[(-0.3, 567.0), (-0.3, 566.89), (-5.575, 567.2239950031015), (-5.575, 567.1139950031015), (-0.3, 566.89), (-0.3, 566.72), (-5.575, 567.1139950031015), (-5.575, 566.8739950031015)]</t>
+          <t>[(-0.3, 567.0), (-0.3, 566.8), (-5.575, 567.2239950031015), (-5.575, 567.0239950031015), (-0.3, 566.8), (-0.3, 566.6), (-5.575, 567.0239950031015), (-5.575, 566.8239950031016), (-0.3, 566.6), (-0.3, 566.47), (-5.575, 566.8239950031016), (-5.575, 566.6239950031015)]</t>
         </is>
       </c>
     </row>
@@ -6107,7 +6107,7 @@
       </c>
       <c r="B569" t="inlineStr">
         <is>
-          <t>[(-0.3, 568.0), (-0.3, 567.89), (-5.352, 568.2580218142435), (-5.352, 568.1480218142435), (-0.3, 567.89), (-0.3, 567.72), (-5.352, 568.1480218142435), (-5.352, 567.9080218142435)]</t>
+          <t>[(-0.3, 568.0), (-0.3, 567.8), (-5.352, 568.2580218142435), (-5.352, 568.0580218142435), (-0.3, 567.8), (-0.3, 567.6), (-5.352, 568.0580218142435), (-5.352, 567.8580218142436), (-0.3, 567.6), (-0.3, 567.49), (-5.352, 567.8580218142436), (-5.352, 567.6680218142435)]</t>
         </is>
       </c>
     </row>
@@ -6117,7 +6117,7 @@
       </c>
       <c r="B570" t="inlineStr">
         <is>
-          <t>[(-0.3, 569.0), (-0.3, 568.89), (-5.076, 569.2850455084694), (-5.076, 569.1750455084693), (-0.3, 568.89), (-0.3, 568.75), (-5.076, 569.1750455084693), (-5.076, 568.9050455084694)]</t>
+          <t>[(-0.3, 569.0), (-0.3, 568.7), (-5.076, 569.2850455084694), (-5.076, 568.9850455084694), (-0.3, 568.7), (-0.3, 568.53), (-5.076, 568.9850455084694), (-5.076, 568.6850455084693)]</t>
         </is>
       </c>
     </row>
@@ -6127,7 +6127,7 @@
       </c>
       <c r="B571" t="inlineStr">
         <is>
-          <t>[(-0.3, 570.0), (-0.3, 569.88), (-4.808, 570.3078629924009), (-4.808, 570.1878629924009), (-0.3, 569.88), (-0.3, 569.75), (-4.808, 570.1878629924009), (-4.808, 569.887862992401)]</t>
+          <t>[(-0.3, 570.0), (-0.3, 569.78), (-4.808, 570.3078629924009), (-4.808, 569.997862992401), (-0.3, 569.78), (-0.3, 569.56), (-4.808, 569.997862992401), (-4.808, 569.6878629924009)]</t>
         </is>
       </c>
     </row>
@@ -6137,7 +6137,7 @@
       </c>
       <c r="B572" t="inlineStr">
         <is>
-          <t>[(-0.3, 571.0), (-0.3, 570.87), (-4.475, 571.29225), (-4.475, 571.16225), (-0.3, 570.87), (-0.3, 570.73), (-4.475, 571.16225), (-4.475, 570.86225)]</t>
+          <t>[(-0.3, 571.0), (-0.3, 570.78), (-4.475, 571.29225), (-4.475, 570.99225), (-0.3, 570.78), (-0.3, 570.56), (-4.475, 570.99225), (-4.475, 570.69225)]</t>
         </is>
       </c>
     </row>
@@ -6147,7 +6147,7 @@
       </c>
       <c r="B573" t="inlineStr">
         <is>
-          <t>[(-0.3, 572.0), (-0.3, 571.82), (-4.178, 572.27146), (-4.178, 572.0914600000001), (-0.3, 571.82), (-0.3, 571.68), (-4.178, 572.0914600000001), (-4.178, 571.79146)]</t>
+          <t>[(-0.3, 572.0), (-0.3, 571.76), (-4.178, 572.27146), (-4.178, 571.95146), (-0.3, 571.76), (-0.3, 571.52), (-4.178, 571.95146), (-4.178, 571.6314600000001)]</t>
         </is>
       </c>
     </row>
@@ -6157,7 +6157,7 @@
       </c>
       <c r="B574" t="inlineStr">
         <is>
-          <t>[(-0.3, 573.0), (-0.3, 572.88), (-3.883, 573.25081), (-3.883, 573.13081), (-0.3, 572.88), (-0.3, 572.69), (-3.883, 573.13081), (-3.883, 572.83081)]</t>
+          <t>[(-0.3, 573.0), (-0.3, 572.72), (-3.883, 573.25081), (-3.883, 572.97081), (-0.3, 572.72), (-0.3, 572.55), (-3.883, 572.97081), (-3.883, 572.69081)]</t>
         </is>
       </c>
     </row>
@@ -6167,7 +6167,7 @@
       </c>
       <c r="B575" t="inlineStr">
         <is>
-          <t>[(-0.3, 574.0), (-0.3, 573.89), (-3.535, 574.22645), (-3.535, 574.11645), (-0.3, 573.89), (-0.3, 573.71), (-3.535, 574.11645), (-3.535, 573.84645)]</t>
+          <t>[(-0.3, 574.0), (-0.3, 573.75), (-3.535, 574.22645), (-3.535, 573.97645), (-0.3, 573.75), (-0.3, 573.58), (-3.535, 573.97645), (-3.535, 573.72645)]</t>
         </is>
       </c>
     </row>
@@ -6177,7 +6177,7 @@
       </c>
       <c r="B576" t="inlineStr">
         <is>
-          <t>[(-0.3, 575.0), (-0.3, 574.89), (-3.088, 575.19516), (-3.088, 575.08516), (-0.3, 574.89), (-0.3, 574.74), (-3.088, 575.08516), (-3.088, 574.88516)]</t>
+          <t>[(-0.3, 575.0), (-0.3, 574.79), (-3.088, 575.19516), (-3.088, 574.98516), (-0.3, 574.79), (-0.3, 574.64), (-3.088, 574.98516), (-3.088, 574.77516)]</t>
         </is>
       </c>
     </row>
@@ -6187,7 +6187,7 @@
       </c>
       <c r="B577" t="inlineStr">
         <is>
-          <t>[(-0.3, 576.0), (-0.3, 575.89), (-2.856, 576.17892), (-2.856, 576.0689199999999), (-0.3, 575.89), (-0.3, 575.73), (-2.856, 576.0689199999999), (-2.856, 575.80892)]</t>
+          <t>[(-0.3, 576.0), (-0.3, 575.77), (-2.856, 576.17892), (-2.856, 575.9489199999999), (-0.3, 575.77), (-0.3, 575.64), (-2.856, 575.9489199999999), (-2.856, 575.7289199999999)]</t>
         </is>
       </c>
     </row>
@@ -6197,7 +6197,7 @@
       </c>
       <c r="B578" t="inlineStr">
         <is>
-          <t>[(-0.3, 577.0), (-0.3, 576.79), (-2.574, 577.15918), (-2.574, 576.94918), (-0.3, 576.79), (-0.3, 576.65), (-2.574, 576.94918), (-2.574, 576.74918)]</t>
+          <t>[(-0.3, 577.0), (-0.3, 576.76), (-2.574, 577.15918), (-2.574, 576.91918), (-0.3, 576.76), (-0.3, 576.58), (-2.574, 576.91918), (-2.574, 576.67918)]</t>
         </is>
       </c>
     </row>
@@ -6467,7 +6467,7 @@
       </c>
       <c r="B605" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 604.0), (-0.3, 603.76), (-5.788, 603.8628), (-5.788, 603.7428), (-0.3, 603.76), (-0.3, 603.52), (-5.788, 603.7428), (-5.788, 603.6228)]</t>
         </is>
       </c>
     </row>
@@ -6637,7 +6637,7 @@
       </c>
       <c r="B622" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 621.0), (-0.3, 620.86), (-5.488, 620.8210012365475), (-5.488, 620.6810012365476), (-0.3, 620.86), (-0.3, 620.74), (-5.488, 620.6810012365476), (-5.488, 620.5710012365475)]</t>
         </is>
       </c>
     </row>
@@ -6767,7 +6767,7 @@
       </c>
       <c r="B635" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 634.0), (-0.3, 633.87), (-7.796, 633.73764), (-7.796, 633.6076400000001), (-0.3, 633.87), (-0.3, 633.75), (-7.796, 633.6076400000001), (-7.796, 633.48764)]</t>
         </is>
       </c>
     </row>
@@ -6777,7 +6777,7 @@
       </c>
       <c r="B636" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 635.0), (-0.3, 634.87), (-6.877, 634.769805), (-6.877, 634.639805), (-0.3, 634.87), (-0.3, 634.75), (-6.877, 634.639805), (-6.877, 634.519805)]</t>
         </is>
       </c>
     </row>
@@ -6787,7 +6787,7 @@
       </c>
       <c r="B637" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 636.0), (-0.3, 635.87), (-6.963, 635.766795), (-6.963, 635.636795), (-0.3, 635.87), (-0.3, 635.75), (-6.963, 635.636795), (-6.963, 635.516795)]</t>
         </is>
       </c>
     </row>
@@ -6797,7 +6797,7 @@
       </c>
       <c r="B638" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 637.0), (-0.3, 636.87), (-7.004, 636.76536), (-7.004, 636.63536), (-0.3, 636.87), (-0.3, 636.75), (-7.004, 636.63536), (-7.004, 636.51536)]</t>
         </is>
       </c>
     </row>
@@ -6807,7 +6807,7 @@
       </c>
       <c r="B639" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 638.0), (-0.3, 637.87), (-7.037, 637.764205), (-7.037, 637.634205), (-0.3, 637.87), (-0.3, 637.75), (-7.037, 637.634205), (-7.037, 637.514205)]</t>
         </is>
       </c>
     </row>
@@ -6817,7 +6817,7 @@
       </c>
       <c r="B640" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 639.0), (-0.3, 638.87), (-7.102, 638.76193), (-7.102, 638.63193), (-0.3, 638.87), (-0.3, 638.75), (-7.102, 638.63193), (-7.102, 638.51193)]</t>
         </is>
       </c>
     </row>
@@ -6827,7 +6827,7 @@
       </c>
       <c r="B641" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 640.0), (-0.3, 639.87), (-7.456, 639.77809244), (-7.456, 639.64809244), (-0.3, 639.87), (-0.3, 639.75), (-7.456, 639.64809244), (-7.456, 639.52809244)]</t>
         </is>
       </c>
     </row>
@@ -6837,7 +6837,7 @@
       </c>
       <c r="B642" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 641.0), (-0.3, 640.87), (-7.614, 640.7637578), (-7.614, 640.6337578), (-0.3, 640.87), (-0.3, 640.75), (-7.614, 640.6337578), (-7.614, 640.5137578)]</t>
         </is>
       </c>
     </row>
@@ -6847,7 +6847,7 @@
       </c>
       <c r="B643" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[(-0.3, 641.6355600000002), (-0.3, 641.5055600000002), (-7.624, 641.4084427600002), (-7.624, 641.2784427600002), (-0.3, 641.5055600000002), (-0.3, 641.3855600000002), (-7.624, 641.2784427600002), (-7.624, 641.1584427600002)]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Testing & general review
</commit_message>
<xml_diff>
--- a/output/layerCoordinates_left.xlsx
+++ b/output/layerCoordinates_left.xlsx
@@ -437,7 +437,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[(-1.99999999999412, 1.0), (-1.99999999999412, 0.89), (-14.169, 0.7650108327052388), (-14.169, 0.6550108327052389), (-1.99999999999412, 0.89), (-1.99999999999412, 0.75), (-14.169, 0.6550108327052389), (-14.169, 0.41501083270523886)]</t>
+          <t>[(-1.99999999999412, 1.0), (-1.99999999999412, 0.88), (-13.9555152609054, 0.7691333243701213), (-13.9555152609054, 0.6491333243701214), (-1.99999999999412, 0.88), (-1.99999999999412, 0.75), (-13.9555152609054, 0.6491333243701214), (-13.9555152609054, 0.41913332437012135)]</t>
         </is>
       </c>
     </row>
@@ -447,7 +447,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[(-1.99999999999293, 2.0), (-1.99999999999293, 1.89), (-13.64, 1.7366317044098496), (-13.64, 1.6266317044098497), (-1.99999999999293, 1.89), (-1.99999999999293, 1.75), (-13.64, 1.6266317044098497), (-13.64, 1.4266317044098495)]</t>
+          <t>[(-1.99999999999293, 2.0), (-1.99999999999293, 1.88), (-13.5000000001641, 1.7397993643187313), (-13.5000000001641, 1.6197993643187312), (-1.99999999999293, 1.88), (-1.99999999999293, 1.75), (-13.5000000001641, 1.6197993643187312), (-13.5000000001641, 1.4297993643187312)]</t>
         </is>
       </c>
     </row>
@@ -457,7 +457,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[(-1.99999999999412, 3.0), (-1.99999999999412, 2.89), (-13.653, 2.776587363834314), (-13.653, 2.666587363834314), (-1.99999999999412, 2.89), (-1.99999999999412, 2.75), (-13.653, 2.666587363834314), (-13.653, 2.446587363834314)]</t>
+          <t>[(-1.99999999999412, 3.0), (-1.99999999999412, 2.88), (-13.5000000002424, 2.779520697163), (-13.5000000002424, 2.659520697163), (-1.99999999999412, 2.88), (-1.99999999999412, 2.75), (-13.5000000002424, 2.659520697163), (-13.5000000002424, 2.449520697163)]</t>
         </is>
       </c>
     </row>
@@ -497,7 +497,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[(-1.99999999999293, 7.0), (-1.99999999999293, 6.89), (-10.654, 6.8905574449841875), (-10.654, 6.780557444984187), (-1.99999999999293, 6.89), (-1.99999999999293, 6.75), (-10.654, 6.780557444984187), (-10.654, 6.530557444984187)]</t>
+          <t>[(-1.99999999999293, 7.0), (-1.99999999999293, 6.88), (-10.49999999999692, 6.892505001428925), (-10.49999999999692, 6.772505001428925), (-1.99999999999293, 6.88), (-1.99999999999293, 6.75), (-10.49999999999692, 6.772505001428925), (-10.49999999999692, 6.532505001428925)]</t>
         </is>
       </c>
     </row>
@@ -507,7 +507,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[(-1.99999999999412, 8.0), (-1.99999999999412, 7.89), (-10.673, 7.862074598814413), (-10.673, 7.752074598814413), (-1.99999999999412, 7.89), (-1.99999999999412, 7.75), (-10.673, 7.752074598814413), (-10.673, 7.492074598814413)]</t>
+          <t>[(-1.99999999999412, 8.0), (-1.99999999999412, 7.88), (-10.4999999999981, 7.864825791528048), (-10.4999999999981, 7.744825791528048), (-1.99999999999412, 7.88), (-1.99999999999412, 7.75), (-10.4999999999981, 7.744825791528048), (-10.4999999999981, 7.494825791528048)]</t>
         </is>
       </c>
     </row>
@@ -517,7 +517,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[(-1.99999999999293, 9.0), (-1.99999999999293, 8.88), (-10.704, 8.906585699841033), (-10.704, 8.786585699841034), (-1.99999999999293, 8.88), (-1.99999999999293, 8.75), (-10.704, 8.786585699841034), (-10.704, 8.486585699841033)]</t>
+          <t>[(-1.99999999999293, 9.0), (-1.99999999999293, 8.88), (-10.49999999999692, 8.908775097501039), (-10.49999999999692, 8.78877509750104), (-1.99999999999293, 8.88), (-1.99999999999293, 8.75), (-10.49999999999692, 8.78877509750104), (-10.49999999999692, 8.488775097501039)]</t>
         </is>
       </c>
     </row>
@@ -527,7 +527,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[(-1.99999999999293, 10.0), (-1.99999999999293, 9.89), (-10.767, 9.874775122021147), (-10.767, 9.764775122021147), (-1.99999999999293, 9.89), (-1.99999999999293, 9.75), (-10.767, 9.764775122021147), (-10.767, 9.474775122021146)]</t>
+          <t>[(-1.99999999999293, 10.0), (-1.99999999999293, 9.88), (-10.4999999999981, 9.878588860177935), (-10.4999999999981, 9.758588860177936), (-1.99999999999293, 9.88), (-1.99999999999293, 9.75), (-10.4999999999981, 9.758588860177936), (-10.4999999999981, 9.478588860177934)]</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[(-1.99999999997917, 11.0), (-1.99999999997917, 10.89), (-10.728, 10.876066159367973), (-10.728, 10.766066159367973), (-1.99999999997917, 10.89), (-1.99999999997917, 10.75), (-10.728, 10.766066159367973), (-10.728, 10.516066159367973)]</t>
+          <t>[(-1.99999999997917, 11.0), (-1.99999999997917, 10.88), (-10.49999999999692, 10.879303661162705), (-10.49999999999692, 10.759303661162706), (-1.99999999997917, 10.88), (-1.99999999997917, 10.75), (-10.49999999999692, 10.759303661162706), (-10.49999999999692, 10.519303661162706)]</t>
         </is>
       </c>
     </row>
@@ -547,7 +547,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>[(-1.99999999999293, 12.0), (-1.99999999999293, 11.89), (-10.747, 11.869367069138887), (-10.747, 11.759367069138888), (-1.99999999999293, 11.89), (-1.99999999999293, 11.75), (-10.747, 11.759367069138888), (-10.747, 11.559367069138887)]</t>
+          <t>[(-1.99999999999293, 12.0), (-1.99999999999293, 11.88), (-10.49999999999692, 11.873055914905787), (-10.49999999999692, 11.753055914905788), (-1.99999999999293, 11.88), (-1.99999999999293, 11.75), (-10.49999999999692, 11.753055914905788), (-10.49999999999692, 11.563055914905787)]</t>
         </is>
       </c>
     </row>
@@ -567,7 +567,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[(-1.99999999999293, 14.0), (-1.99999999999293, 13.87), (-10.721, 13.842581227436696), (-10.721, 13.712581227436695), (-1.99999999999293, 13.87), (-1.99999999999293, 13.75), (-10.721, 13.712581227436695), (-10.721, 13.592581227436696)]</t>
+          <t>[(-1.99999999999293, 14.0), (-1.99999999999293, 13.87), (-10.49999999999692, 13.846570397111842), (-10.49999999999692, 13.716570397111841), (-1.99999999999293, 13.87), (-1.99999999999293, 13.75), (-10.49999999999692, 13.716570397111841), (-10.49999999999692, 13.596570397111842)]</t>
         </is>
       </c>
     </row>
@@ -577,7 +577,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>[(-1.99999999999293, 15.0), (-1.99999999999293, 14.87), (-10.711, 14.78319734984859), (-10.711, 14.65319734984859), (-1.99999999999293, 14.87), (-1.99999999999293, 14.75), (-10.711, 14.65319734984859), (-10.711, 14.53319734984859)]</t>
+          <t>[(-1.99999999999293, 15.0), (-1.99999999999293, 14.87), (-10.4999999999981, 14.788448797349718), (-10.4999999999981, 14.658448797349717), (-1.99999999999293, 14.87), (-1.99999999999293, 14.75), (-10.4999999999981, 14.658448797349717), (-10.4999999999981, 14.538448797349718)]</t>
         </is>
       </c>
     </row>
@@ -587,7 +587,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>[(-2.00011422891936, 16.0), (-2.00011422891936, 15.86), (-10.664, 15.830599966920335), (-10.664, 15.690599966920335), (-2.00011422891936, 15.86), (-2.00011422891936, 15.75), (-10.664, 15.690599966920335), (-10.664, 15.570599966920335)]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -597,7 +597,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>[(-1.9996071717933, 17.0), (-1.9996071717933, 16.87), (-10.548, 16.720149909988024), (-10.548, 16.590149909988025), (-1.9996071717933, 16.87), (-1.9996071717933, 16.75), (-10.548, 16.590149909988025), (-10.548, 16.470149909988024)]</t>
+          <t>[(-1.9996071717933, 17.0), (-1.9996071717933, 16.87), (-10.49960717178584, 16.721734153670297), (-10.49960717178584, 16.5917341536703), (-1.9996071717933, 16.87), (-1.9996071717933, 16.75), (-10.49960717178584, 16.5917341536703), (-10.49960717178584, 16.471734153670297)]</t>
         </is>
       </c>
     </row>
@@ -1867,7 +1867,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>[(-0.300000000016708, 144.0), (-0.300000000016708, 143.85), (-4.017, 144.1973619800469), (-4.017, 144.0473619800469), (-0.300000000016708, 143.85), (-0.300000000016708, 143.7), (-4.017, 144.0473619800469), (-4.017, 143.8973619800469), (-0.300000000016708, 143.7), (-0.300000000016708, 143.59), (-4.017, 143.8973619800469), (-4.017, 143.7673619800469)]</t>
+          <t>[(-0.300000000016708, 144.0), (-0.300000000016708, 143.78), (-4.017, 144.1973619800469), (-4.017, 143.9773619800469), (-0.300000000016708, 143.78), (-0.300000000016708, 143.59), (-4.017, 143.9773619800469), (-4.017, 143.7673619800469)]</t>
         </is>
       </c>
     </row>
@@ -1927,7 +1927,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>[(-0.300000000025586, 150.0), (-0.300000000025586, 149.85), (-7.035, 150.19139138072168), (-7.035, 150.04139138072168), (-0.300000000025586, 149.85), (-0.300000000025586, 149.7), (-7.035, 150.04139138072168), (-7.035, 149.89139138072167), (-0.300000000025586, 149.7), (-0.300000000025586, 149.59), (-7.035, 149.89139138072167), (-7.035, 149.75139138072169)]</t>
+          <t>[(-0.300000000025586, 150.0), (-0.300000000025586, 149.78), (-7.035, 150.19139138072168), (-7.035, 149.97139138072168), (-0.300000000025586, 149.78), (-0.300000000025586, 149.59), (-7.035, 149.97139138072168), (-7.035, 149.75139138072169)]</t>
         </is>
       </c>
     </row>
@@ -1977,7 +1977,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>[(-0.300000000004276, 155.0), (-0.300000000004276, 154.86), (-2.846, 154.93635000000012), (-2.846, 154.79635000000013), (-2.846, 154.93635000000012), (-2.846, 154.80635000000012), (-10.83, 154.73675000000011), (-10.83, 154.60675000000012), (-0.300000000004276, 154.86), (-0.300000000004276, 154.73), (-2.846, 154.79635000000013), (-2.846, 154.68635000000012), (-2.846, 154.80635000000012), (-2.846, 154.68635000000012), (-10.83, 154.60675000000012), (-10.83, 154.48675000000011)]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2007,7 +2007,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>[(-0.300000000004276, 158.0), (-0.300000000004276, 157.87), (-3.906, 157.90985000000012), (-3.906, 157.77985000000012), (-3.906, 157.90985000000012), (-3.906, 157.77985000000012), (-13.443, 157.6714250000001), (-13.443, 157.54142500000012), (-0.300000000004276, 157.87), (-0.300000000004276, 157.75), (-3.906, 157.77985000000012), (-3.906, 157.65985000000012), (-3.906, 157.77985000000012), (-3.906, 157.65985000000012), (-13.443, 157.54142500000012), (-13.443, 157.4214250000001)]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2017,7 +2017,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>[(-0.300000000003251, 159.0), (-0.300000000003251, 158.89), (-4.157, 158.90357500000007), (-4.157, 158.79357500000006), (-4.157, 158.90357500000007), (-4.157, 158.77357500000008), (-14.083, 158.6554250000001), (-14.083, 158.5254250000001), (-0.300000000003251, 158.89), (-0.300000000003251, 158.68), (-4.157, 158.79357500000006), (-4.157, 158.65357500000007), (-4.157, 158.77357500000008), (-4.157, 158.65357500000007), (-14.083, 158.5254250000001), (-14.083, 158.4054250000001)]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>[(-0.300000000003251, 160.0), (-0.300000000003251, 159.88), (-4.255, 159.9011250000001), (-4.255, 159.7811250000001), (-4.255, 159.9011250000001), (-4.255, 159.7511250000001), (-15.746, 159.61385000000007), (-15.746, 159.46385000000006), (-0.300000000003251, 159.88), (-0.300000000003251, 159.58), (-4.255, 159.7811250000001), (-4.255, 159.6411250000001), (-4.255, 159.7511250000001), (-4.255, 159.6411250000001), (-15.746, 159.46385000000006), (-15.746, 159.16385000000008)]</t>
+          <t>[(-0.300000000003251, 160.0), (-0.300000000003251, 159.88), (-4.255, 159.9011250000001), (-4.255, 159.7811250000001), (-4.255, 159.9011250000001), (-4.255, 159.7711250000001), (-14.5293427398727, 159.64426643150327), (-14.5293427398727, 159.42426643150327), (-0.300000000003251, 159.88), (-0.300000000003251, 159.58), (-4.255, 159.7811250000001), (-4.255, 159.6411250000001), (-4.255, 159.7711250000001), (-4.255, 159.6411250000001), (-14.5293427398727, 159.42426643150327), (-14.5293427398727, 159.20426643150327)]</t>
         </is>
       </c>
     </row>
@@ -2037,7 +2037,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>[(-0.299999999989289, 161.0), (-0.299999999989289, 160.87), (-4.396, 160.89759999999973), (-4.396, 160.76759999999973), (-4.396, 160.89759999999973), (-4.396, 160.7875999999997), (-10.7999999999866, 160.73750000000007), (-10.7999999999866, 160.62750000000005), (-0.299999999989289, 160.87), (-0.299999999989289, 160.57), (-4.396, 160.76759999999973), (-4.396, 160.61759999999973), (-4.396, 160.7875999999997), (-4.396, 160.61759999999973), (-10.7999999999866, 160.62750000000005), (-10.7999999999866, 160.32750000000007)]</t>
+          <t>[(-0.299999999989289, 161.0), (-0.299999999989289, 160.87), (-4.396, 160.89759999999973), (-4.396, 160.76759999999973), (-4.396, 160.89759999999973), (-4.396, 160.77759999999972), (-8.79999999999042, 160.78749999999997), (-8.79999999999042, 160.66749999999996), (-0.299999999989289, 160.87), (-0.299999999989289, 160.57), (-4.396, 160.76759999999973), (-4.396, 160.61759999999973), (-4.396, 160.77759999999972), (-4.396, 160.61759999999973), (-8.79999999999042, 160.66749999999996), (-8.79999999999042, 160.36749999999998)]</t>
         </is>
       </c>
     </row>
@@ -2047,7 +2047,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>[(-0.300000000004276, 162.0), (-0.300000000004276, 161.89), (-4.481, 161.89547500000012), (-4.481, 161.7854750000001), (-4.481, 161.89547500000012), (-4.481, 161.7854750000001), (-10.8000000000016, 161.73750000000007), (-10.8000000000016, 161.62750000000005), (-0.300000000004276, 161.89), (-0.300000000004276, 161.62), (-4.481, 161.7854750000001), (-4.481, 161.64547500000012), (-4.481, 161.7854750000001), (-4.481, 161.64547500000012), (-10.8000000000016, 161.62750000000005), (-10.8000000000016, 161.33750000000006)]</t>
+          <t>[(-0.300000000004276, 162.0), (-0.300000000004276, 161.88), (-4.481, 161.89547500000012), (-4.481, 161.7754750000001), (-4.481, 161.89547500000012), (-4.481, 161.7754750000001), (-8.80000000000438, 161.7875), (-8.80000000000438, 161.6675), (-0.300000000004276, 161.88), (-0.300000000004276, 161.62), (-4.481, 161.7754750000001), (-4.481, 161.64547500000012), (-4.481, 161.7754750000001), (-4.481, 161.64547500000012), (-8.80000000000438, 161.6675), (-8.80000000000438, 161.3875)]</t>
         </is>
       </c>
     </row>
@@ -2057,7 +2057,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>[(-0.299999999985573, 163.0), (-0.299999999985573, 162.89), (-4.635, 162.89162499999964), (-4.635, 162.78162499999962), (-4.635, 162.89162499999964), (-4.635, 162.78162499999962), (-10.7999999999834, 162.73750000000007), (-10.7999999999834, 162.62750000000005), (-0.299999999985573, 162.89), (-0.299999999985573, 162.62), (-4.635, 162.78162499999962), (-4.635, 162.64162499999964), (-4.635, 162.78162499999962), (-4.635, 162.64162499999964), (-10.7999999999834, 162.62750000000005), (-10.7999999999834, 162.32750000000007)]</t>
+          <t>[(-0.299999999985573, 163.0), (-0.299999999985573, 162.88), (-4.635, 162.89162499999964), (-4.635, 162.77162499999963), (-4.635, 162.89162499999964), (-4.635, 162.77162499999963), (-8.79999999998633, 162.7875), (-8.79999999998633, 162.6675), (-0.299999999985573, 162.88), (-0.299999999985573, 162.62), (-4.635, 162.77162499999963), (-4.635, 162.64162499999964), (-4.635, 162.77162499999963), (-4.635, 162.64162499999964), (-8.79999999998633, 162.6675), (-8.79999999998633, 162.3875)]</t>
         </is>
       </c>
     </row>
@@ -2067,7 +2067,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>[(-0.299999999997345, 164.0), (-0.299999999997345, 163.88), (-4.568, 163.89329999999993), (-4.568, 163.77329999999992), (-4.568, 163.89329999999993), (-4.568, 163.77329999999992), (-10.7999999999924, 163.73750000000013), (-10.7999999999924, 163.61750000000012), (-0.299999999997345, 163.88), (-0.299999999997345, 163.58), (-4.568, 163.77329999999992), (-4.568, 163.64329999999993), (-4.568, 163.77329999999992), (-4.568, 163.64329999999993), (-10.7999999999924, 163.61750000000012), (-10.7999999999924, 163.31750000000014)]</t>
+          <t>[(-0.299999999997345, 164.0), (-0.299999999997345, 163.88), (-4.568, 163.89329999999993), (-4.568, 163.77329999999992), (-4.568, 163.89329999999993), (-4.568, 163.77329999999992), (-8.80000000000263, 163.78749999999988), (-8.80000000000263, 163.66749999999988), (-0.299999999997345, 163.88), (-0.299999999997345, 163.58), (-4.568, 163.77329999999992), (-4.568, 163.64329999999993), (-4.568, 163.77329999999992), (-4.568, 163.64329999999993), (-8.80000000000263, 163.66749999999988), (-8.80000000000263, 163.3674999999999)]</t>
         </is>
       </c>
     </row>
@@ -2077,7 +2077,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>[(-0.299999999999201, 165.0), (-0.299999999999201, 164.88), (-4.461, 164.895975), (-4.461, 164.775975), (-4.461, 164.895975), (-4.461, 164.78597499999998), (-10.7999999999954, 164.7375000000001), (-10.7999999999954, 164.62750000000008), (-0.299999999999201, 164.88), (-0.299999999999201, 164.58), (-4.461, 164.775975), (-4.461, 164.645975), (-4.461, 164.78597499999998), (-4.461, 164.645975), (-10.7999999999954, 164.62750000000008), (-10.7999999999954, 164.3675000000001)]</t>
+          <t>[(-0.299999999999201, 165.0), (-0.299999999999201, 164.88), (-4.461, 164.895975), (-4.461, 164.775975), (-4.461, 164.895975), (-4.461, 164.775975), (-8.80000000000645, 164.78749999999982), (-8.80000000000645, 164.66749999999982), (-0.299999999999201, 164.88), (-0.299999999999201, 164.58), (-4.461, 164.775975), (-4.461, 164.645975), (-4.461, 164.775975), (-4.461, 164.645975), (-8.80000000000645, 164.66749999999982), (-8.80000000000645, 164.41749999999982)]</t>
         </is>
       </c>
     </row>
@@ -2087,7 +2087,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>[(-0.299999999993337, 166.0), (-0.299999999993337, 165.89), (-4.253, 165.90117499999982), (-4.253, 165.7911749999998), (-4.253, 165.90117499999982), (-4.253, 165.77117499999983), (-10.7999999999953, 165.73749999999995), (-10.7999999999953, 165.60749999999996), (-0.299999999993337, 165.89), (-0.299999999993337, 165.68), (-4.253, 165.7911749999998), (-4.253, 165.65117499999982), (-4.253, 165.77117499999983), (-4.253, 165.65117499999982), (-10.7999999999953, 165.60749999999996), (-10.7999999999953, 165.48749999999995)]</t>
+          <t>[(-0.299999999993337, 166.0), (-0.299999999993337, 165.88), (-4.253, 165.90117499999982), (-4.253, 165.78117499999982), (-4.253, 165.90117499999982), (-4.253, 165.77117499999983), (-8.7999999999942, 165.78749999999997), (-8.7999999999942, 165.65749999999997), (-0.299999999993337, 165.88), (-0.299999999993337, 165.68), (-4.253, 165.78117499999982), (-4.253, 165.65117499999982), (-4.253, 165.77117499999983), (-4.253, 165.65117499999982), (-8.7999999999942, 165.65749999999997), (-8.7999999999942, 165.53749999999997)]</t>
         </is>
       </c>
     </row>
@@ -2097,7 +2097,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>[(-0.300000000001455, 167.0), (-0.300000000001455, 166.87), (-4.252, 166.90120000000005), (-4.252, 166.77120000000005), (-4.252, 166.90120000000005), (-4.252, 166.77120000000005), (-10.7999999999977, 166.7375000000001), (-10.7999999999977, 166.6075000000001), (-0.300000000001455, 166.87), (-0.300000000001455, 166.75), (-4.252, 166.77120000000005), (-4.252, 166.65120000000005), (-4.252, 166.77120000000005), (-4.252, 166.65120000000005), (-10.7999999999977, 166.6075000000001), (-10.7999999999977, 166.4875000000001)]</t>
+          <t>[(-0.300000000001455, 167.0), (-0.300000000001455, 166.87), (-4.252, 166.90120000000005), (-4.252, 166.77120000000005), (-4.252, 166.90120000000005), (-4.252, 166.77120000000005), (-8.79999999999453, 166.78750000000016), (-8.79999999999453, 166.65750000000017), (-0.300000000001455, 166.87), (-0.300000000001455, 166.75), (-4.252, 166.77120000000005), (-4.252, 166.65120000000005), (-4.252, 166.77120000000005), (-4.252, 166.65120000000005), (-8.79999999999453, 166.65750000000017), (-8.79999999999453, 166.53750000000016)]</t>
         </is>
       </c>
     </row>
@@ -2107,7 +2107,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>[(-0.299999999995238, 168.0), (-0.299999999995238, 167.86), (-4.164, 167.9033999999999), (-4.164, 167.7633999999999), (-4.164, 167.9033999999999), (-4.164, 167.7733999999999), (-11.148, 167.7287999999999), (-11.148, 167.5987999999999), (-0.299999999995238, 167.86), (-0.299999999995238, 167.73), (-4.164, 167.7633999999999), (-4.164, 167.6533999999999), (-4.164, 167.7733999999999), (-4.164, 167.6533999999999), (-11.148, 167.5987999999999), (-11.148, 167.4787999999999)]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>[(-0.299999999992807, 172.0), (-0.299999999992807, 171.89), (-3.841, 171.91147499999983), (-3.841, 171.8014749999998), (-3.841, 171.91147499999983), (-3.841, 171.78147499999983), (-12.411, 171.69722499999983), (-12.411, 171.56722499999984), (-0.299999999992807, 171.89), (-0.299999999992807, 171.66), (-3.841, 171.8014749999998), (-3.841, 171.66147499999983), (-3.841, 171.78147499999983), (-3.841, 171.66147499999983), (-12.411, 171.56722499999984), (-12.411, 171.44722499999983)]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2167,7 +2167,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>[(-0.300000000054567, 174.0), (-0.300000000054567, 173.86), (-4.002, 173.88920942046872), (-4.002, 173.74920942046873), (-4.002, 173.88920942046872), (-4.002, 173.75920942046872), (-11.644, 173.6605055823297), (-11.644, 173.5305055823297), (-0.300000000054567, 173.86), (-0.300000000054567, 173.73), (-4.002, 173.74920942046873), (-4.002, 173.63920942046872), (-4.002, 173.75920942046872), (-4.002, 173.63920942046872), (-11.644, 173.5305055823297), (-11.644, 173.4105055823297)]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2177,7 +2177,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>[(-0.300000000084013, 175.0), (-0.300000000084013, 174.87), (-4.157, 174.86302894558645), (-4.157, 174.73302894558645), (-4.157, 174.86302894558645), (-4.157, 174.73302894558645), (-11.3029138502153, 174.6092608992205), (-11.3029138502153, 174.4792608992205), (-0.300000000084013, 174.87), (-0.300000000084013, 174.75), (-4.157, 174.73302894558645), (-4.157, 174.61302894558645), (-4.157, 174.73302894558645), (-4.157, 174.61302894558645), (-11.3029138502153, 174.4792608992205), (-11.3029138502153, 174.3592608992205)]</t>
+          <t>[(-0.300000000084013, 175.0), (-0.300000000084013, 174.87), (-4.157, 174.86302894558645), (-4.157, 174.73302894558645), (-4.157, 174.86302894558645), (-4.157, 174.73302894558645), (-9.30042272320688, 174.68037402370223), (-9.30042272320688, 174.55037402370223), (-0.300000000084013, 174.87), (-0.300000000084013, 174.75), (-4.157, 174.73302894558645), (-4.157, 174.61302894558645), (-4.157, 174.73302894558645), (-4.157, 174.61302894558645), (-9.30042272320688, 174.55037402370223), (-9.30042272320688, 174.43037402370223)]</t>
         </is>
       </c>
     </row>
@@ -2217,7 +2217,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>[(-0.299999999996132, 179.0), (-0.299999999996132, 178.89), (-3.955, 178.78854818079876), (-3.955, 178.67854818079874), (-3.955, 178.78854818079876), (-3.955, 178.65854818079876), (-10.7999999999935, 178.39254607343088), (-10.7999999999935, 178.26254607343088), (-0.299999999996132, 178.89), (-0.299999999996132, 178.67), (-3.955, 178.67854818079874), (-3.955, 178.53854818079876), (-3.955, 178.65854818079876), (-3.955, 178.53854818079876), (-10.7999999999935, 178.26254607343088), (-10.7999999999935, 178.14254607343088)]</t>
+          <t>[(-0.299999999996132, 179.0), (-0.299999999996132, 178.88), (-3.955, 178.78854818079876), (-3.955, 178.66854818079875), (-3.955, 178.78854818079876), (-3.955, 178.65854818079876), (-8.79999999998878, 178.50825158325387), (-8.79999999998878, 178.37825158325387), (-0.299999999996132, 178.88), (-0.299999999996132, 178.67), (-3.955, 178.66854818079875), (-3.955, 178.53854818079876), (-3.955, 178.65854818079876), (-3.955, 178.53854818079876), (-8.79999999998878, 178.37825158325387), (-8.79999999998878, 178.25825158325387)]</t>
         </is>
       </c>
     </row>
@@ -2227,7 +2227,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>[(-0.299999999997375, 180.0), (-0.299999999997375, 179.89), (-3.483, 179.80901999999983), (-3.483, 179.69901999999982), (-3.483, 179.80901999999983), (-3.483, 179.67901999999984), (-10.493, 179.38841999999985), (-10.493, 179.25841999999986), (-0.299999999997375, 179.89), (-0.299999999997375, 179.69), (-3.483, 179.69901999999982), (-3.483, 179.55901999999983), (-3.483, 179.67901999999984), (-3.483, 179.55901999999983), (-10.493, 179.25841999999986), (-10.493, 179.13841999999985)]</t>
+          <t>[(-0.299999999997375, 180.0), (-0.299999999997375, 179.88), (-3.483, 179.80901999999983), (-3.483, 179.68901999999983), (-3.483, 179.80901999999983), (-3.483, 179.67901999999984), (-8.80000000000704, 179.4899999999994), (-8.80000000000704, 179.35999999999942), (-0.299999999997375, 179.88), (-0.299999999997375, 179.69), (-3.483, 179.68901999999983), (-3.483, 179.55901999999983), (-3.483, 179.67901999999984), (-3.483, 179.55901999999983), (-8.80000000000704, 179.35999999999942), (-8.80000000000704, 179.2399999999994)]</t>
         </is>
       </c>
     </row>
@@ -2237,7 +2237,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>[(-0.299999999992836, 181.0), (-0.299999999992836, 180.89), (-2.824, 180.84855999999957), (-2.824, 180.73855999999955), (-2.824, 180.84855999999957), (-2.824, 180.71855999999957), (-9.811, 180.42933999999957), (-9.811, 180.29933999999957), (-0.299999999992836, 180.89), (-0.299999999992836, 180.66), (-2.824, 180.73855999999955), (-2.824, 180.59855999999957), (-2.824, 180.71855999999957), (-2.824, 180.59855999999957), (-9.811, 180.29933999999957), (-9.811, 180.17933999999957)]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2247,7 +2247,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>[(-0.30000000000151, 182.0), (-0.30000000000151, 181.83), (-9.17, 181.4678000000001), (-9.17, 181.2978000000001), (-0.30000000000151, 181.83), (-0.30000000000151, 181.67), (-9.17, 181.2978000000001), (-9.17, 181.1778000000001)]</t>
+          <t>[(-0.30000000000151, 182.0), (-0.30000000000151, 181.83), (-8.80000000000596, 181.48999999999972), (-8.80000000000596, 181.31999999999974), (-0.30000000000151, 181.83), (-0.30000000000151, 181.67), (-8.80000000000596, 181.31999999999974), (-8.80000000000596, 181.1899999999997)]</t>
         </is>
       </c>
     </row>
@@ -2267,7 +2267,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>[(-0.299999999999572, 184.0), (-0.299999999999572, 183.89), (-7.857, 183.54657999999998), (-7.857, 183.43657999999996), (-0.299999999999572, 183.89), (-0.299999999999572, 183.61), (-7.857, 183.43657999999996), (-7.857, 183.29657999999998)]</t>
+          <t>[(-0.299999999999572, 184.0), (-0.299999999999572, 183.88), (-7.857, 183.54657999999998), (-7.857, 183.42657999999997), (-0.299999999999572, 183.88), (-0.299999999999572, 183.61), (-7.857, 183.42657999999997), (-7.857, 183.29657999999998)]</t>
         </is>
       </c>
     </row>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>[(-0.299999999993799, 185.0), (-0.299999999993799, 184.89), (-6.888, 184.60471999999962), (-6.888, 184.4947199999996), (-0.299999999993799, 184.89), (-0.299999999993799, 184.63), (-6.888, 184.4947199999996), (-6.888, 184.35471999999962)]</t>
+          <t>[(-0.299999999993799, 185.0), (-0.299999999993799, 184.88), (-6.888, 184.60471999999962), (-6.888, 184.4847199999996), (-0.299999999993799, 184.88), (-0.299999999993799, 184.63), (-6.888, 184.4847199999996), (-6.888, 184.35471999999962)]</t>
         </is>
       </c>
     </row>
@@ -2287,7 +2287,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>[(-0.299999999996377, 186.0), (-0.299999999996377, 185.89), (-5.892, 185.66447999999977), (-5.892, 185.55447999999976), (-0.299999999996377, 185.89), (-0.299999999996377, 185.68), (-5.892, 185.55447999999976), (-5.892, 185.41447999999977)]</t>
+          <t>[(-0.299999999996377, 186.0), (-0.299999999996377, 185.88), (-5.892, 185.66447999999977), (-5.892, 185.54447999999977), (-0.299999999996377, 185.88), (-0.299999999996377, 185.68), (-5.892, 185.54447999999977), (-5.892, 185.41447999999977)]</t>
         </is>
       </c>
     </row>
@@ -2297,7 +2297,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>[(-0.300000000007436, 187.0), (-0.300000000007436, 186.89), (-4.905, 186.72370000000043), (-4.905, 186.61370000000042), (-0.300000000007436, 186.89), (-0.300000000007436, 186.68), (-4.905, 186.61370000000042), (-4.905, 186.47370000000043)]</t>
+          <t>[(-0.300000000007436, 187.0), (-0.300000000007436, 186.88), (-4.905, 186.72370000000043), (-4.905, 186.60370000000043), (-0.300000000007436, 186.88), (-0.300000000007436, 186.68), (-4.905, 186.60370000000043), (-4.905, 186.47370000000043)]</t>
         </is>
       </c>
     </row>
@@ -2307,7 +2307,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>[(-0.300000000000548, 188.0), (-0.300000000000548, 187.89), (-4.146, 187.76924000000002), (-4.146, 187.65924), (-0.300000000000548, 187.89), (-0.300000000000548, 187.67), (-4.146, 187.65924), (-4.146, 187.51924000000002)]</t>
+          <t>[(-0.300000000000548, 188.0), (-0.300000000000548, 187.88), (-4.146, 187.76924000000002), (-4.146, 187.64924000000002), (-0.300000000000548, 187.88), (-0.300000000000548, 187.67), (-4.146, 187.64924000000002), (-4.146, 187.51924000000002)]</t>
         </is>
       </c>
     </row>
@@ -2327,7 +2327,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>[(-0.299999999995328, 190.0), (-0.299999999995328, 189.89), (-3.053, 189.83481999999972), (-3.053, 189.7248199999997), (-0.299999999995328, 189.89), (-0.299999999995328, 189.67), (-3.053, 189.7248199999997), (-3.053, 189.58481999999972)]</t>
+          <t>[(-0.299999999995328, 190.0), (-0.299999999995328, 189.88), (-3.053, 189.83481999999972), (-3.053, 189.71481999999972), (-0.299999999995328, 189.88), (-0.299999999995328, 189.67), (-3.053, 189.71481999999972), (-3.053, 189.58481999999972)]</t>
         </is>
       </c>
     </row>
@@ -2557,7 +2557,7 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>[(-0.300000000037866, 213.0), (-0.300000000037866, 212.89), (-2.761, 213.0726978260564), (-2.761, 212.9626978260564), (-0.300000000037866, 212.89), (-0.300000000037866, 212.75), (-2.761, 212.9626978260564), (-2.761, 212.75269782605642)]</t>
+          <t>[(-0.300000000037866, 213.0), (-0.300000000037866, 212.88), (-2.761, 213.0726978260564), (-2.761, 212.9526978260564), (-0.300000000037866, 212.88), (-0.300000000037866, 212.75), (-2.761, 212.9526978260564), (-2.761, 212.75269782605642)]</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>[(-0.299999999995819, 217.0), (-0.299999999995819, 216.87), (-4.206, 217.23903990672204), (-4.206, 217.10903990672205), (-4.206, 217.23903990672204), (-4.206, 217.12903990672203), (-7.515, 217.44154452816144), (-7.515, 217.33154452816143), (-0.299999999995819, 216.87), (-0.299999999995819, 216.75), (-4.206, 217.10903990672205), (-4.206, 216.98903990672204), (-4.206, 217.12903990672203), (-4.206, 216.98903990672204), (-7.515, 217.33154452816143), (-7.515, 217.11154452816143)]</t>
+          <t>[(-0.299999999995819, 217.0), (-0.299999999995819, 216.87), (-4.206, 217.23903990672204), (-4.206, 217.10903990672205), (-4.206, 217.23903990672204), (-4.206, 217.11903990672204), (-7.515, 217.44154452816144), (-7.515, 217.32154452816144), (-0.299999999995819, 216.87), (-0.299999999995819, 216.75), (-4.206, 217.10903990672205), (-4.206, 216.98903990672204), (-4.206, 217.11903990672204), (-4.206, 216.98903990672204), (-7.515, 217.32154452816144), (-7.515, 217.11154452816143)]</t>
         </is>
       </c>
     </row>
@@ -2607,7 +2607,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>[(-0.300000000000684, 218.0), (-0.300000000000684, 217.89), (-6.083, 218.40480999999994), (-6.083, 218.29480999999993), (-6.083, 218.40480999999994), (-6.083, 218.22480999999993), (-9.456, 218.64091999999997), (-9.456, 218.30091999999996), (-0.300000000000684, 217.89), (-0.300000000000684, 217.73), (-6.083, 218.29480999999993), (-6.083, 218.04480999999993), (-6.083, 218.22480999999993), (-6.083, 218.04480999999993), (-9.456, 218.30091999999996), (-9.456, 217.96091999999996)]</t>
+          <t>[(-0.300000000000684, 218.0), (-0.300000000000684, 217.88), (-6.083, 218.40480999999994), (-6.083, 218.28480999999994), (-6.083, 218.40480999999994), (-6.083, 218.22480999999993), (-8.8000000000025, 218.59500000000014), (-8.8000000000025, 218.26500000000013), (-0.300000000000684, 217.88), (-0.300000000000684, 217.73), (-6.083, 218.28480999999994), (-6.083, 218.04480999999993), (-6.083, 218.22480999999993), (-6.083, 218.04480999999993), (-8.8000000000025, 218.26500000000013), (-8.8000000000025, 217.93500000000014)]</t>
         </is>
       </c>
     </row>
@@ -2617,7 +2617,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>[(-0.300000000001353, 219.0), (-0.300000000001353, 218.89), (-7.801, 219.52506999999991), (-7.801, 219.4150699999999), (-7.801, 219.52506999999991), (-7.801, 219.32506999999993), (-10.7999999999967, 219.73499999999967), (-10.7999999999967, 219.37499999999966), (-0.300000000001353, 218.89), (-0.300000000001353, 218.72), (-7.801, 219.4150699999999), (-7.801, 219.11506999999992), (-7.801, 219.32506999999993), (-7.801, 219.1250699999999), (-10.7999999999967, 219.37499999999966), (-10.7999999999967, 219.01499999999967)]</t>
+          <t>[(-0.300000000001353, 219.0), (-0.300000000001353, 218.88), (-7.801, 219.52506999999991), (-7.801, 219.4050699999999), (-7.801, 219.52506999999991), (-7.801, 219.32506999999993), (-8.80000000000079, 219.59499999999997), (-8.80000000000079, 219.27499999999998), (-0.300000000001353, 218.88), (-0.300000000001353, 218.72), (-7.801, 219.4050699999999), (-7.801, 219.11506999999992), (-7.801, 219.32506999999993), (-7.801, 219.1250699999999), (-8.80000000000079, 219.27499999999998), (-8.80000000000079, 218.95499999999998)]</t>
         </is>
       </c>
     </row>
@@ -2627,7 +2627,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>[(-0.299999999992942, 220.0), (-0.299999999992942, 219.86), (-9.188, 220.6221600000005), (-9.188, 220.4821600000005), (-9.188, 220.6221600000005), (-9.188, 220.4021600000005), (-10.7999999999983, 220.73500000000038), (-10.7999999999983, 220.4150000000004), (-0.299999999992942, 219.86), (-0.299999999992942, 219.69), (-9.188, 220.4821600000005), (-9.188, 220.1821600000005), (-9.188, 220.4021600000005), (-9.188, 220.1821600000005), (-10.7999999999983, 220.4150000000004), (-10.7999999999983, 220.0950000000004)]</t>
+          <t>[(-0.299999999992942, 220.0), (-0.299999999992942, 219.86), (-9.188, 220.6221600000005), (-9.188, 220.4821600000005), (-9.188, 220.6221600000005), (-9.188, 220.4021600000005), (-8.79999999999426, 220.59500000000008), (-8.79999999999426, 220.28500000000008), (-0.299999999992942, 219.86), (-0.299999999992942, 219.69), (-9.188, 220.4821600000005), (-9.188, 220.1821600000005), (-9.188, 220.4021600000005), (-9.188, 220.1821600000005), (-8.79999999999426, 220.28500000000008), (-8.79999999999426, 219.97500000000008)]</t>
         </is>
       </c>
     </row>
@@ -2637,7 +2637,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>[(-0.299999999999579, 221.0), (-0.299999999999579, 220.76), (-10.073, 221.68411000000003), (-10.073, 221.44411000000002), (-10.073, 221.68411000000003), (-10.073, 221.44411000000002), (-10.8000000000013, 221.73500000000013), (-10.8000000000013, 221.49500000000012), (-0.299999999999579, 220.76), (-0.299999999999579, 220.53), (-10.073, 221.44411000000002), (-10.073, 221.32411000000002), (-10.073, 221.44411000000002), (-10.073, 221.32411000000002), (-10.8000000000013, 221.49500000000012), (-10.8000000000013, 221.26500000000013)]</t>
+          <t>[(-0.299999999999579, 221.0), (-0.299999999999579, 220.76), (-10.073, 221.68411000000003), (-10.073, 221.44411000000002), (-10.073, 221.68411000000003), (-10.073, 221.47411000000002), (-8.79999999999261, 221.59499999999952), (-8.79999999999261, 221.3849999999995), (-0.299999999999579, 220.76), (-0.299999999999579, 220.53), (-10.073, 221.44411000000002), (-10.073, 221.32411000000002), (-10.073, 221.47411000000002), (-10.073, 221.32411000000002), (-8.79999999999261, 221.3849999999995), (-8.79999999999261, 221.08499999999952)]</t>
         </is>
       </c>
     </row>
@@ -2647,7 +2647,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>[(-0.300000000000845, 222.0), (-0.300000000000845, 221.89), (-10.766, 222.73261999999994), (-10.766, 222.62261999999993), (-10.766, 222.73261999999994), (-10.766, 222.54261999999994), (-10.8000000000053, 222.7350000000003), (-10.8000000000053, 222.5450000000003), (-0.300000000000845, 221.89), (-0.300000000000845, 221.75), (-10.766, 222.62261999999993), (-10.766, 222.42261999999994), (-10.766, 222.54261999999994), (-10.766, 222.42261999999994), (-10.8000000000053, 222.5450000000003), (-10.8000000000053, 222.3650000000003)]</t>
+          <t>[(-0.300000000000845, 222.0), (-0.300000000000845, 221.88), (-10.766, 222.73261999999994), (-10.766, 222.61261999999994), (-10.766, 222.73261999999994), (-10.766, 222.59261999999995), (-8.7999999999958, 222.59499999999966), (-8.7999999999958, 222.45499999999967), (-0.300000000000845, 221.88), (-0.300000000000845, 221.75), (-10.766, 222.61261999999994), (-10.766, 222.42261999999994), (-10.766, 222.59261999999995), (-10.766, 222.42261999999994), (-8.7999999999958, 222.45499999999967), (-8.7999999999958, 222.15499999999966)]</t>
         </is>
       </c>
     </row>
@@ -2657,7 +2657,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>[(-0.300000000004265, 223.0), (-0.300000000004265, 222.89), (-11.007, 223.7494899999997), (-11.007, 223.63948999999968), (-11.007, 223.7494899999997), (-11.007, 223.5494899999997), (-10.8000000000028, 223.7349999999999), (-10.8000000000028, 223.5349999999999), (-0.300000000004265, 222.89), (-0.300000000004265, 222.75), (-11.007, 223.63948999999968), (-11.007, 223.41948999999968), (-11.007, 223.5494899999997), (-11.007, 223.41948999999968), (-10.8000000000028, 223.5349999999999), (-10.8000000000028, 223.3349999999999)]</t>
+          <t>[(-0.300000000004265, 223.0), (-0.300000000004265, 222.88), (-11.007, 223.7494899999997), (-11.007, 223.6294899999997), (-11.007, 223.7494899999997), (-11.007, 223.6194899999997), (-8.79999999999743, 223.59499999999952), (-8.79999999999743, 223.46499999999952), (-0.300000000004265, 222.88), (-0.300000000004265, 222.75), (-11.007, 223.6294899999997), (-11.007, 223.41948999999968), (-11.007, 223.6194899999997), (-11.007, 223.41948999999968), (-8.79999999999743, 223.46499999999952), (-8.79999999999743, 223.1649999999995)]</t>
         </is>
       </c>
     </row>
@@ -2667,7 +2667,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>[(-0.299999999994225, 224.0), (-0.299999999994225, 223.88), (-11.092, 224.7554400000004), (-11.092, 224.51544000000038), (-11.092, 224.7554400000004), (-11.092, 224.45544000000038), (-10.7999999999966, 224.73500000000016), (-10.7999999999966, 224.43500000000014), (-0.299999999994225, 223.88), (-0.299999999994225, 223.76), (-11.092, 224.51544000000038), (-11.092, 224.2754400000004), (-11.092, 224.45544000000038), (-11.092, 224.2754400000004), (-10.7999999999966, 224.43500000000014), (-10.7999999999966, 224.14500000000015)]</t>
+          <t>[(-0.299999999994225, 224.0), (-0.299999999994225, 223.88), (-11.092, 224.7554400000004), (-11.092, 224.51544000000038), (-11.092, 224.7554400000004), (-11.092, 224.4754400000004), (-8.79999999999597, 224.5950000000001), (-8.79999999999597, 224.3150000000001), (-0.299999999994225, 223.88), (-0.299999999994225, 223.76), (-11.092, 224.51544000000038), (-11.092, 224.2754400000004), (-11.092, 224.4754400000004), (-11.092, 224.2754400000004), (-8.79999999999597, 224.3150000000001), (-8.79999999999597, 224.0450000000001)]</t>
         </is>
       </c>
     </row>
@@ -2677,7 +2677,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>[(-0.300000000005367, 225.0), (-0.300000000005367, 224.88), (-10.831, 225.73716999999962), (-10.831, 225.47716999999963), (-10.831, 225.73716999999962), (-10.831, 225.52716999999961), (-10.8000000000056, 225.735), (-10.8000000000056, 225.525), (-0.300000000005367, 224.88), (-0.300000000005367, 224.76), (-10.831, 225.47716999999963), (-10.831, 225.2171699999996), (-10.831, 225.52716999999961), (-10.831, 225.31716999999963), (-10.8000000000056, 225.525), (-10.8000000000056, 225.31500000000003)]</t>
+          <t>[(-0.300000000005367, 225.0), (-0.300000000005367, 224.88), (-10.831, 225.73716999999962), (-10.831, 225.47716999999963), (-10.831, 225.73716999999962), (-10.831, 225.47716999999963), (-8.79999999999447, 225.59499999999923), (-8.79999999999447, 225.27499999999924), (-0.300000000005367, 224.88), (-0.300000000005367, 224.76), (-10.831, 225.47716999999963), (-10.831, 225.2171699999996), (-10.831, 225.47716999999963), (-10.831, 225.2171699999996), (-8.79999999999447, 225.27499999999924), (-8.79999999999447, 224.95499999999925)]</t>
         </is>
       </c>
     </row>
@@ -2687,7 +2687,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>[(-0.299999999999419, 226.0), (-0.299999999999419, 225.88), (-10.166, 226.69062000000005), (-10.166, 226.43062000000006), (-10.166, 226.69062000000005), (-10.166, 226.43062000000006), (-10.7999999999952, 226.7349999999997), (-10.7999999999952, 226.4049999999997), (-0.299999999999419, 225.88), (-0.299999999999419, 225.76), (-10.166, 226.43062000000006), (-10.166, 226.17062000000004), (-10.166, 226.43062000000006), (-10.166, 226.17062000000004), (-10.7999999999952, 226.4049999999997), (-10.7999999999952, 226.0749999999997)]</t>
+          <t>[(-0.299999999999419, 226.0), (-0.299999999999419, 225.88), (-10.166, 226.69062000000005), (-10.166, 226.43062000000006), (-10.166, 226.69062000000005), (-10.166, 226.43062000000006), (-8.80000000000446, 226.59500000000034), (-8.80000000000446, 226.27500000000035), (-0.299999999999419, 225.88), (-0.299999999999419, 225.76), (-10.166, 226.43062000000006), (-10.166, 226.17062000000004), (-10.166, 226.43062000000006), (-10.166, 226.17062000000004), (-8.80000000000446, 226.27500000000035), (-8.80000000000446, 225.95500000000035)]</t>
         </is>
       </c>
     </row>
@@ -2697,7 +2697,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>[(-0.300000000001498, 227.0), (-0.300000000001498, 226.88), (-9.205, 227.6233499999999), (-9.205, 227.3833499999999), (-9.205, 227.6233499999999), (-9.205, 227.3833499999999), (-10.8000000000021, 227.73500000000004), (-10.8000000000021, 227.35500000000005), (-0.300000000001498, 226.88), (-0.300000000001498, 226.76), (-9.205, 227.3833499999999), (-9.205, 227.1433499999999), (-9.205, 227.3833499999999), (-9.205, 227.1433499999999), (-10.8000000000021, 227.35500000000005), (-10.8000000000021, 226.97500000000005)]</t>
+          <t>[(-0.300000000001498, 227.0), (-0.300000000001498, 226.88), (-9.205, 227.6233499999999), (-9.205, 227.3833499999999), (-9.205, 227.6233499999999), (-9.205, 227.3833499999999), (-8.80000000000615, 227.5950000000003), (-8.80000000000615, 227.27500000000032), (-0.300000000001498, 226.88), (-0.300000000001498, 226.76), (-9.205, 227.3833499999999), (-9.205, 227.1433499999999), (-9.205, 227.3833499999999), (-9.205, 227.1433499999999), (-8.80000000000615, 227.27500000000032), (-8.80000000000615, 226.95500000000033)]</t>
         </is>
       </c>
     </row>
@@ -2707,7 +2707,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>[(-0.300000000038602, 228.0), (-0.300000000038602, 227.89), (-8.19, 228.4920039533552), (-8.19, 228.3820039533552), (-8.19, 228.4920039533552), (-8.19, 228.3320039533552), (-10.7999999999988, 228.65475811283082), (-10.7999999999988, 228.34475811283082), (-0.300000000038602, 227.89), (-0.300000000038602, 227.75), (-8.19, 228.3820039533552), (-8.19, 228.1820039533552), (-8.19, 228.3320039533552), (-8.19, 228.17200395335522), (-10.7999999999988, 228.34475811283082), (-10.7999999999988, 228.03475811283081)]</t>
+          <t>[(-0.300000000038602, 228.0), (-0.300000000038602, 227.88), (-8.19, 228.4920039533552), (-8.19, 228.3720039533552), (-8.19, 228.4920039533552), (-8.19, 228.3320039533552), (-8.80000000000219, 228.53004228181518), (-8.80000000000219, 228.2700422818152), (-0.300000000038602, 227.88), (-0.300000000038602, 227.75), (-8.19, 228.3720039533552), (-8.19, 228.1820039533552), (-8.19, 228.3320039533552), (-8.19, 228.17200395335522), (-8.80000000000219, 228.2700422818152), (-8.80000000000219, 228.01004228181517)]</t>
         </is>
       </c>
     </row>
@@ -2717,7 +2717,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>[(-0.299999999993343, 229.0), (-0.299999999993343, 228.87), (-7.184, 229.372801577857), (-7.184, 229.242801577857), (-7.184, 229.372801577857), (-7.184, 229.25280157785699), (-10.707, 229.56358890481644), (-10.707, 229.24358890481645), (-0.299999999993343, 228.87), (-0.299999999993343, 228.75), (-7.184, 229.242801577857), (-7.184, 229.122801577857), (-7.184, 229.25280157785699), (-7.184, 229.13280157785698), (-10.707, 229.24358890481645), (-10.707, 228.92358890481646)]</t>
+          <t>[(-0.299999999993343, 229.0), (-0.299999999993343, 228.87), (-7.184, 229.372801577857), (-7.184, 229.242801577857), (-7.184, 229.372801577857), (-7.184, 229.25280157785699), (-8.80000000000548, 229.46031571931812), (-8.80000000000548, 229.20031571931813), (-0.299999999993343, 228.87), (-0.299999999993343, 228.75), (-7.184, 229.242801577857), (-7.184, 229.122801577857), (-7.184, 229.25280157785699), (-7.184, 229.13280157785698), (-8.80000000000548, 229.20031571931813), (-8.80000000000548, 228.9403157193181)]</t>
         </is>
       </c>
     </row>
@@ -2747,7 +2747,7 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>[(-0.300000000016519, 232.0), (-0.300000000016519, 231.87), (-6.473, 232.18238384993), (-6.473, 232.05238384993), (-6.473, 232.18238384993), (-6.473, 232.06238384993), (-9.977, 232.2859109858698), (-9.977, 231.9659109858698), (-0.300000000016519, 231.87), (-0.300000000016519, 231.75), (-6.473, 232.05238384993), (-6.473, 231.93238384993), (-6.473, 232.06238384993), (-6.473, 231.94238384993), (-9.977, 231.9659109858698), (-9.977, 231.64591098586982)]</t>
+          <t>[(-0.300000000016519, 232.0), (-0.300000000016519, 231.87), (-6.473, 232.18238384993), (-6.473, 232.05238384993), (-6.473, 232.18238384993), (-6.473, 232.06238384993), (-8.80000000000638, 232.25113603181717), (-8.80000000000638, 231.97113603181717), (-0.300000000016519, 231.87), (-0.300000000016519, 231.75), (-6.473, 232.05238384993), (-6.473, 231.93238384993), (-6.473, 232.06238384993), (-6.473, 231.94238384993), (-8.80000000000638, 231.97113603181717), (-8.80000000000638, 231.69113603181717)]</t>
         </is>
       </c>
     </row>
@@ -2757,7 +2757,7 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>[(-0.300000000004104, 233.0), (-0.300000000004104, 232.87), (-6.598, 233.07055554636702), (-6.598, 232.94055554636702), (-6.598, 233.07055554636702), (-6.598, 232.950555546367), (-10.064, 233.10938462285293), (-10.064, 232.83938462285292), (-0.300000000004104, 232.87), (-0.300000000004104, 232.75), (-6.598, 232.94055554636702), (-6.598, 232.82055554636702), (-6.598, 232.950555546367), (-6.598, 232.830555546367), (-10.064, 232.83938462285292), (-10.064, 232.56938462285294)]</t>
+          <t>[(-0.300000000004104, 233.0), (-0.300000000004104, 232.87), (-6.598, 233.07055554636702), (-6.598, 232.94055554636702), (-6.598, 233.07055554636702), (-6.598, 232.950555546367), (-8.80000000000538, 233.09522422104163), (-8.80000000000538, 232.85522422104162), (-0.300000000004104, 232.87), (-0.300000000004104, 232.75), (-6.598, 232.94055554636702), (-6.598, 232.82055554636702), (-6.598, 232.950555546367), (-6.598, 232.830555546367), (-8.80000000000538, 232.85522422104162), (-8.80000000000538, 232.61522422104164)]</t>
         </is>
       </c>
     </row>
@@ -2767,7 +2767,7 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>[(-0.300000000002969, 234.0), (-0.300000000002969, 233.87), (-6.694, 233.87378279755276), (-6.694, 233.74378279755277), (-6.694, 233.87378279755276), (-6.694, 233.74378279755277), (-10.232, 233.80394287539784), (-10.232, 233.67394287539784), (-0.300000000002969, 233.87), (-0.300000000002969, 233.75), (-6.694, 233.74378279755277), (-6.694, 233.62378279755276), (-6.694, 233.74378279755277), (-6.694, 233.62378279755276), (-10.232, 233.67394287539784), (-10.232, 233.55394287539784)]</t>
+          <t>[(-0.300000000002969, 234.0), (-0.300000000002969, 233.87), (-6.694, 233.87378279755276), (-6.694, 233.74378279755277), (-6.694, 233.87378279755276), (-6.694, 233.74378279755277), (-8.80000000000424, 233.83221047532027), (-8.80000000000424, 233.70221047532027), (-0.300000000002969, 233.87), (-0.300000000002969, 233.75), (-6.694, 233.74378279755277), (-6.694, 233.62378279755276), (-6.694, 233.74378279755277), (-6.694, 233.62378279755276), (-8.80000000000424, 233.70221047532027), (-8.80000000000424, 233.58221047532027)]</t>
         </is>
       </c>
     </row>
@@ -2777,7 +2777,7 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>[(-0.300000000074902, 235.0), (-0.300000000074902, 234.87), (-6.865, 234.72144607427805), (-6.865, 234.59144607427805), (-6.865, 234.72144607427805), (-6.865, 234.59144607427805), (-10.356, 234.57332242542708), (-10.356, 234.44332242542708), (-0.300000000074902, 234.87), (-0.300000000074902, 234.75), (-6.865, 234.59144607427805), (-6.865, 234.47144607427805), (-6.865, 234.59144607427805), (-6.865, 234.47144607427805), (-10.356, 234.44332242542708), (-10.356, 234.32332242542708)]</t>
+          <t>[(-0.300000000074902, 235.0), (-0.300000000074902, 234.87), (-6.865, 234.72144607427805), (-6.865, 234.59144607427805), (-6.865, 234.72144607427805), (-6.865, 234.59144607427805), (-8.80000000002093, 234.63934373668718), (-8.80000000002093, 234.50934373668719), (-0.300000000074902, 234.87), (-0.300000000074902, 234.75), (-6.865, 234.59144607427805), (-6.865, 234.47144607427805), (-6.865, 234.59144607427805), (-6.865, 234.47144607427805), (-8.80000000002093, 234.50934373668719), (-8.80000000002093, 234.38934373668718)]</t>
         </is>
       </c>
     </row>
@@ -2787,7 +2787,7 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>[(-0.300000000114203, 236.0), (-0.300000000114203, 235.87), (-6.433, 235.61098289848823), (-6.433, 235.48098289848824), (-6.433, 235.61098289848823), (-6.433, 235.48098289848824), (-10.083, 235.37946285600586), (-10.083, 235.24946285600586), (-0.300000000114203, 235.87), (-0.300000000114203, 235.75), (-6.433, 235.48098289848824), (-6.433, 235.36098289848823), (-6.433, 235.48098289848824), (-6.433, 235.36098289848823), (-10.083, 235.24946285600586), (-10.083, 235.12946285600586)]</t>
+          <t>[(-0.300000000114203, 236.0), (-0.300000000114203, 235.87), (-6.433, 235.61098289848823), (-6.433, 235.48098289848824), (-6.433, 235.61098289848823), (-6.433, 235.48098289848824), (-8.8000000000206, 235.46084373669083), (-8.8000000000206, 235.33084373669084), (-0.300000000114203, 235.87), (-0.300000000114203, 235.75), (-6.433, 235.48098289848824), (-6.433, 235.36098289848823), (-6.433, 235.48098289848824), (-6.433, 235.36098289848823), (-8.8000000000206, 235.33084373669084), (-8.8000000000206, 235.21084373669083)]</t>
         </is>
       </c>
     </row>
@@ -2797,7 +2797,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>[(-0.300000000005366, 237.0), (-0.300000000005366, 236.87), (-5.622, 236.62746000000038), (-5.622, 236.4974600000004), (-5.622, 236.62746000000038), (-5.622, 236.4974600000004), (-9.234, 236.37462000000036), (-9.234, 236.24462000000037), (-0.300000000005366, 236.87), (-0.300000000005366, 236.75), (-5.622, 236.4974600000004), (-5.622, 236.37746000000038), (-5.622, 236.4974600000004), (-5.622, 236.37746000000038), (-9.234, 236.24462000000037), (-9.234, 236.12462000000036)]</t>
+          <t>[(-0.300000000005366, 237.0), (-0.300000000005366, 236.87), (-5.622, 236.62746000000038), (-5.622, 236.4974600000004), (-5.622, 236.62746000000038), (-5.622, 236.4974600000004), (-8.79999999999814, 236.4050000000005), (-8.79999999999814, 236.27500000000052), (-0.300000000005366, 236.87), (-0.300000000005366, 236.75), (-5.622, 236.4974600000004), (-5.622, 236.37746000000038), (-5.622, 236.4974600000004), (-5.622, 236.37746000000038), (-8.79999999999814, 236.27500000000052), (-8.79999999999814, 236.1550000000005)]</t>
         </is>
       </c>
     </row>
@@ -2857,7 +2857,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>[(-0.29999999999459, 243.0), (-0.29999999999459, 242.85), (-3.224, 242.97603312978833), (-3.224, 242.82603312978833), (-3.224, 242.97603312978833), (-3.224, 242.82603312978833), (-9.022, 242.92850921956702), (-9.022, 242.66850921956703), (-0.29999999999459, 242.85), (-0.29999999999459, 242.71), (-3.224, 242.82603312978833), (-3.224, 242.67603312978832), (-3.224, 242.82603312978833), (-3.224, 242.67603312978832), (-9.022, 242.66850921956703), (-9.022, 242.408509219567)]</t>
+          <t>[(-0.29999999999459, 243.0), (-0.29999999999459, 242.85), (-3.224, 242.97603312978833), (-3.224, 242.82603312978833), (-3.224, 242.97603312978833), (-3.224, 242.82603312978833), (-8.79999999999426, 242.93032886566385), (-8.79999999999426, 242.67032886566386), (-0.29999999999459, 242.85), (-0.29999999999459, 242.71), (-3.224, 242.82603312978833), (-3.224, 242.67603312978832), (-3.224, 242.82603312978833), (-3.224, 242.67603312978832), (-8.79999999999426, 242.67032886566386), (-8.79999999999426, 242.41032886566384)]</t>
         </is>
       </c>
     </row>
@@ -2867,7 +2867,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>[(-0.299999999994472, 244.0), (-0.299999999994472, 243.83), (-3.053, 244.03443425116868), (-3.053, 243.8644342511687), (-3.053, 244.03443425116868), (-3.053, 243.8644342511687), (-9.943, 244.12061368834688), (-9.943, 243.76061368834687), (-0.299999999994472, 243.83), (-0.299999999994472, 243.67), (-3.053, 243.8644342511687), (-3.053, 243.69443425116867), (-3.053, 243.8644342511687), (-3.053, 243.69443425116867), (-9.943, 243.76061368834687), (-9.943, 243.40061368834688)]</t>
+          <t>[(-0.299999999994472, 244.0), (-0.299999999994472, 243.83), (-3.053, 244.03443425116868), (-3.053, 243.8644342511687), (-3.053, 244.03443425116868), (-3.053, 243.8644342511687), (-8.79999999999426, 244.1063171576219), (-8.79999999999426, 243.7663171576219), (-0.299999999994472, 243.83), (-0.299999999994472, 243.67), (-3.053, 243.8644342511687), (-3.053, 243.69443425116867), (-3.053, 243.8644342511687), (-3.053, 243.69443425116867), (-8.79999999999426, 243.7663171576219), (-8.79999999999426, 243.4263171576219)]</t>
         </is>
       </c>
     </row>
@@ -2877,7 +2877,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>[(-0.299999999987999, 245.0), (-0.299999999987999, 244.83), (-2.817, 245.07782404970587), (-2.817, 244.90782404970588), (-2.817, 245.07782404970587), (-2.817, 244.90782404970588), (-9.696, 245.29051838340638), (-9.696, 244.93051838340637), (-0.299999999987999, 244.83), (-0.299999999987999, 244.69), (-2.817, 244.90782404970588), (-2.817, 244.73782404970586), (-2.817, 244.90782404970588), (-2.817, 244.73782404970586), (-9.696, 244.93051838340637), (-9.696, 244.57051838340638)]</t>
+          <t>[(-0.299999999987999, 245.0), (-0.299999999987999, 244.83), (-2.817, 245.07782404970587), (-2.817, 244.90782404970588), (-2.817, 245.07782404970587), (-2.817, 244.90782404970588), (-8.79999999998336, 245.26281462951783), (-8.79999999998336, 244.91281462951784), (-0.299999999987999, 244.83), (-0.299999999987999, 244.69), (-2.817, 244.90782404970588), (-2.817, 244.73782404970586), (-2.817, 244.90782404970588), (-2.817, 244.73782404970586), (-8.79999999998336, 244.91281462951784), (-8.79999999998336, 244.56281462951785)]</t>
         </is>
       </c>
     </row>
@@ -2887,7 +2887,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>[(-0.300000000015845, 246.0), (-0.300000000015845, 245.84), (-2.868, 246.11772440706517), (-2.868, 245.95772440706517), (-2.868, 246.11772440706517), (-2.868, 245.95772440706517), (-9.652, 246.42872221763176), (-9.652, 246.08872221763176), (-0.300000000015845, 245.84), (-0.300000000015845, 245.73), (-2.868, 245.95772440706517), (-2.868, 245.79772440706518), (-2.868, 245.95772440706517), (-2.868, 245.79772440706518), (-9.652, 246.08872221763176), (-9.652, 245.74872221763175)]</t>
+          <t>[(-0.300000000015845, 246.0), (-0.300000000015845, 245.88), (-2.868, 246.11772440706517), (-2.868, 245.99772440706516), (-2.868, 246.11772440706517), (-2.868, 245.95772440706517), (-8.8000000000035, 246.38966411996054), (-8.8000000000035, 246.05966411996053), (-0.300000000015845, 245.88), (-0.300000000015845, 245.73), (-2.868, 245.99772440706516), (-2.868, 245.79772440706518), (-2.868, 245.95772440706517), (-2.868, 245.79772440706518), (-8.8000000000035, 246.05966411996053), (-8.8000000000035, 245.72966411996055)]</t>
         </is>
       </c>
     </row>
@@ -2907,7 +2907,7 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>[(-0.30000000000184, 248.0), (-0.30000000000184, 247.86), (-3.123, 248.19760999999988), (-3.123, 248.0576099999999), (-3.123, 248.19760999999988), (-3.123, 248.08760999999987), (-6.875, 248.46024999999986), (-6.875, 248.35024999999985), (-0.30000000000184, 247.86), (-0.30000000000184, 247.75), (-3.123, 248.0576099999999), (-3.123, 247.9376099999999), (-3.123, 248.08760999999987), (-3.123, 247.9376099999999), (-6.875, 248.35024999999985), (-6.875, 248.15024999999986)]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2927,7 +2927,7 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>[(-0.29999999999852, 250.0), (-0.29999999999852, 249.89), (-3.599, 250.23093000000011), (-3.599, 250.1209300000001), (-3.599, 250.23093000000011), (-3.599, 250.0209300000001), (-7.357, 250.4939900000001), (-7.357, 250.2839900000001), (-0.29999999999852, 249.89), (-0.29999999999852, 249.74), (-3.599, 250.1209300000001), (-3.599, 249.9009300000001), (-3.599, 250.0209300000001), (-3.599, 249.9009300000001), (-7.357, 250.2839900000001), (-7.357, 250.0839900000001)]</t>
+          <t>[(-0.29999999999852, 250.0), (-0.29999999999852, 249.88), (-3.599, 250.23093000000011), (-3.599, 250.1109300000001), (-3.599, 250.23093000000011), (-3.599, 250.0209300000001), (-7.357, 250.4939900000001), (-7.357, 250.2839900000001), (-0.29999999999852, 249.88), (-0.29999999999852, 249.74), (-3.599, 250.1109300000001), (-3.599, 249.9009300000001), (-3.599, 250.0209300000001), (-3.599, 249.9009300000001), (-7.357, 250.2839900000001), (-7.357, 250.0839900000001)]</t>
         </is>
       </c>
     </row>
@@ -2937,7 +2937,7 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>[(-0.299999999993185, 251.0), (-0.299999999993185, 250.79), (-3.931, 251.25417000000047), (-3.931, 251.04417000000046), (-3.931, 251.25417000000047), (-3.931, 251.04417000000046), (-10.8000000000009, 251.73500000000055), (-10.8000000000009, 251.37500000000054), (-0.299999999993185, 250.79), (-0.299999999993185, 250.63), (-3.931, 251.04417000000046), (-3.931, 250.83417000000048), (-3.931, 251.04417000000046), (-3.931, 250.83417000000048), (-10.8000000000009, 251.37500000000054), (-10.8000000000009, 251.01500000000055)]</t>
+          <t>[(-0.299999999993185, 251.0), (-0.299999999993185, 250.79), (-3.931, 251.25417000000047), (-3.931, 251.04417000000046), (-3.931, 251.25417000000047), (-3.931, 251.04417000000046), (-8.80000000000373, 251.59500000000074), (-8.80000000000373, 251.23500000000072), (-0.299999999993185, 250.79), (-0.299999999993185, 250.63), (-3.931, 251.04417000000046), (-3.931, 250.83417000000048), (-3.931, 251.04417000000046), (-3.931, 250.83417000000048), (-8.80000000000373, 251.23500000000072), (-8.80000000000373, 250.87500000000074)]</t>
         </is>
       </c>
     </row>
@@ -2957,7 +2957,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>[(-0.300000000150335, 253.0), (-0.300000000150335, 252.83), (-5.084, 253.15003449125732), (-5.084, 252.98003449125733), (-5.084, 253.15003449125732), (-5.084, 252.93003449125732), (-8.801, 253.26660602219815), (-8.801, 252.94660602219815), (-0.300000000150335, 252.83), (-0.300000000150335, 252.66), (-5.084, 252.98003449125733), (-5.084, 252.8100344912573), (-5.084, 252.93003449125732), (-5.084, 252.71003449125732), (-8.801, 252.94660602219815), (-8.801, 252.62660602219816), (-0.300000000150335, 252.66), (-0.300000000150335, 252.51), (-5.084, 252.8100344912573), (-5.084, 252.70003449125733), (-5.084, 252.71003449125732), (-5.084, 252.71003449125732), (-8.801, 252.62660602219816), (-8.801, 252.62660602219816)]</t>
+          <t>[(-0.300000000150335, 253.0), (-0.300000000150335, 252.75), (-5.084, 253.15003449125732), (-5.084, 252.90003449125732), (-5.084, 253.15003449125732), (-5.084, 252.93003449125732), (-8.80000000000522, 253.26657466047354), (-8.80000000000522, 252.94657466047354), (-0.300000000150335, 252.75), (-0.300000000150335, 252.51), (-5.084, 252.90003449125732), (-5.084, 252.70003449125733), (-5.084, 252.93003449125732), (-5.084, 252.71003449125732), (-8.80000000000522, 252.94657466047354), (-8.80000000000522, 252.62657466047355)]</t>
         </is>
       </c>
     </row>
@@ -2967,7 +2967,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>[(-0.300000000068302, 254.0), (-0.300000000068302, 253.79), (-5.837, 254.0601004496114), (-5.837, 253.8501004496114), (-5.837, 254.0601004496114), (-5.837, 253.8201004496114), (-9.608, 254.1010321446606), (-9.608, 253.86103214466058), (-0.300000000068302, 253.79), (-0.300000000068302, 253.59), (-5.837, 253.8501004496114), (-5.837, 253.7001004496114), (-5.837, 253.8201004496114), (-5.837, 253.7001004496114), (-9.608, 253.86103214466058), (-9.608, 253.5610321446606)]</t>
+          <t>[(-0.300000000068302, 254.0), (-0.300000000068302, 253.79), (-5.837, 254.0601004496114), (-5.837, 253.8501004496114), (-5.837, 254.0601004496114), (-5.837, 253.8201004496114), (-8.80000000000395, 254.09226184245972), (-8.80000000000395, 253.8522618424597), (-0.300000000068302, 253.79), (-0.300000000068302, 253.59), (-5.837, 253.8501004496114), (-5.837, 253.7001004496114), (-5.837, 253.8201004496114), (-5.837, 253.7001004496114), (-8.80000000000395, 253.8522618424597), (-8.80000000000395, 253.55226184245973)]</t>
         </is>
       </c>
     </row>
@@ -2977,7 +2977,7 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>[(-0.300000000038982, 255.0), (-0.300000000038982, 254.84), (-6.327, 254.9715525250222), (-6.327, 254.8115525250222), (-6.327, 254.9715525250222), (-6.327, 254.82155252502218), (-10.119, 254.95365426301515), (-10.119, 254.80365426301515), (-0.300000000038982, 254.84), (-0.300000000038982, 254.69), (-6.327, 254.8115525250222), (-6.327, 254.6915525250222), (-6.327, 254.82155252502218), (-6.327, 254.6915525250222), (-10.119, 254.80365426301515), (-10.119, 254.50365426301516)]</t>
+          <t>[(-0.300000000038982, 255.0), (-0.300000000038982, 254.84), (-6.327, 254.9715525250222), (-6.327, 254.8115525250222), (-6.327, 254.9715525250222), (-6.327, 254.8115525250222), (-8.79999999999696, 254.95987995067003), (-8.79999999999696, 254.79987995067003), (-0.300000000038982, 254.84), (-0.300000000038982, 254.69), (-6.327, 254.8115525250222), (-6.327, 254.6915525250222), (-6.327, 254.8115525250222), (-6.327, 254.6915525250222), (-8.79999999999696, 254.79987995067003), (-8.79999999999696, 254.49987995067002)]</t>
         </is>
       </c>
     </row>
@@ -2987,7 +2987,7 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>[(-0.300000000096326, 256.0), (-0.300000000096326, 255.84), (-6.895, 255.9027408940629), (-6.895, 255.7427408940629), (-6.895, 255.9027408940629), (-6.895, 255.7527408940629), (-10.601, 255.84808702801163), (-10.601, 255.59808702801163), (-0.300000000096326, 255.84), (-0.300000000096326, 255.69), (-6.895, 255.7427408940629), (-6.895, 255.6027408940629), (-6.895, 255.7527408940629), (-6.895, 255.6027408940629), (-10.601, 255.59808702801163), (-10.601, 255.34808702801163)]</t>
+          <t>[(-0.300000000096326, 256.0), (-0.300000000096326, 255.84), (-6.895, 255.9027408940629), (-6.895, 255.7427408940629), (-6.895, 255.9027408940629), (-6.895, 255.7527408940629), (-8.80000000001001, 255.87464709621395), (-8.80000000001001, 255.63464709621394), (-0.300000000096326, 255.84), (-0.300000000096326, 255.69), (-6.895, 255.7427408940629), (-6.895, 255.6027408940629), (-6.895, 255.7527408940629), (-6.895, 255.6027408940629), (-8.80000000001001, 255.63464709621394), (-8.80000000001001, 255.39464709621396)]</t>
         </is>
       </c>
     </row>
@@ -2997,7 +2997,7 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>[(-0.300000000165304, 257.0), (-0.300000000165304, 256.79), (-7.551, 256.82035796082397), (-7.551, 256.610357960824), (-7.551, 256.82035796082397), (-7.551, 256.63035796082397), (-10.8000000000084, 256.7398646515842), (-10.8000000000084, 256.4398646515842), (-0.300000000165304, 256.79), (-0.300000000165304, 256.59), (-7.551, 256.610357960824), (-7.551, 256.440357960824), (-7.551, 256.63035796082397), (-7.551, 256.440357960824), (-10.8000000000084, 256.4398646515842), (-10.8000000000084, 256.13986465158416)]</t>
+          <t>[(-0.300000000165304, 257.0), (-0.300000000165304, 256.79), (-7.551, 256.82035796082397), (-7.551, 256.610357960824), (-7.551, 256.82035796082397), (-7.551, 256.63035796082397), (-8.80000000001827, 256.7894142417591), (-8.80000000001827, 256.4994142417591), (-0.300000000165304, 256.79), (-0.300000000165304, 256.59), (-7.551, 256.610357960824), (-7.551, 256.440357960824), (-7.551, 256.63035796082397), (-7.551, 256.440357960824), (-8.80000000001827, 256.4994142417591), (-8.80000000001827, 256.20941424175913)]</t>
         </is>
       </c>
     </row>
@@ -3007,7 +3007,7 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>[(-0.300000000095095, 258.0), (-0.300000000095095, 257.78), (-8.147, 257.72690721719505), (-8.147, 257.506907217195), (-8.147, 257.72690721719505), (-8.147, 257.48690721719504), (-10.7999999999937, 257.63457700784255), (-10.7999999999937, 257.39457700784254), (-0.300000000095095, 257.78), (-0.300000000095095, 257.57), (-8.147, 257.506907217195), (-8.147, 257.376907217195), (-8.147, 257.48690721719504), (-8.147, 257.376907217195), (-10.7999999999937, 257.39457700784254), (-10.7999999999937, 257.09457700784253)]</t>
+          <t>[(-0.300000000095095, 258.0), (-0.300000000095095, 257.78), (-8.147, 257.72690721719505), (-8.147, 257.506907217195), (-8.147, 257.72690721719505), (-8.147, 257.54690721719504), (-8.8000000000018, 257.7041813873015), (-8.8000000000018, 257.4341813873015), (-0.300000000095095, 257.78), (-0.300000000095095, 257.57), (-8.147, 257.506907217195), (-8.147, 257.376907217195), (-8.147, 257.54690721719504), (-8.147, 257.36690721719503), (-8.8000000000018, 257.4341813873015), (-8.8000000000018, 257.1641813873015)]</t>
         </is>
       </c>
     </row>
@@ -3017,7 +3017,7 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>[(-0.300000000045387, 259.0), (-0.300000000045387, 258.8), (-8.681, 258.6242832533834), (-8.681, 258.4242832533834), (-8.681, 258.6242832533834), (-8.681, 258.46428325338337), (-10.8000000000029, 258.5292893640997), (-10.8000000000029, 258.26928936409973), (-0.300000000045387, 258.8), (-0.300000000045387, 258.6), (-8.681, 258.4242832533834), (-8.681, 258.3142832533834), (-8.681, 258.46428325338337), (-8.681, 258.3042832533834), (-10.8000000000029, 258.26928936409973), (-10.8000000000029, 258.00928936409974)]</t>
+          <t>[(-0.300000000045387, 259.0), (-0.300000000045387, 258.88), (-8.681, 258.6242832533834), (-8.681, 258.5042832533834), (-8.681, 258.6242832533834), (-8.681, 258.46428325338337), (-8.80000000000685, 258.61894853284286), (-8.80000000000685, 258.36894853284286), (-0.300000000045387, 258.88), (-0.300000000045387, 258.6), (-8.681, 258.5042832533834), (-8.681, 258.3142832533834), (-8.681, 258.46428325338337), (-8.681, 258.3042832533834), (-8.80000000000685, 258.36894853284286), (-8.80000000000685, 258.11894853284286)]</t>
         </is>
       </c>
     </row>
@@ -3027,7 +3027,7 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>[(-0.300000000020933, 260.0), (-0.300000000020933, 259.76), (-8.606, 259.5443579323137), (-8.606, 259.3043579323137), (-8.606, 259.5443579323137), (-8.606, 259.3643579323137), (-10.8000000000045, 259.4240017203575), (-10.8000000000045, 259.14400172035755), (-0.300000000020933, 259.76), (-0.300000000020933, 259.53), (-8.606, 259.3043579323137), (-8.606, 259.19435793231366), (-8.606, 259.3643579323137), (-8.606, 259.1843579323137), (-10.8000000000045, 259.14400172035755), (-10.8000000000045, 258.8640017203575)]</t>
+          <t>[(-0.300000000020933, 260.0), (-0.300000000020933, 259.83), (-8.606, 259.5443579323137), (-8.606, 259.37435793231367), (-8.606, 259.5443579323137), (-8.606, 259.3643579323137), (-8.80000000000537, 259.5337156783848), (-8.80000000000537, 259.2637156783848), (-0.300000000020933, 259.83), (-0.300000000020933, 259.53), (-8.606, 259.37435793231367), (-8.606, 259.19435793231366), (-8.606, 259.3643579323137), (-8.606, 259.1843579323137), (-8.80000000000537, 259.2637156783848), (-8.80000000000537, 258.9937156783848)]</t>
         </is>
       </c>
     </row>
@@ -3037,7 +3037,7 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>[(-0.300000000013218, 261.0), (-0.300000000013218, 260.71), (-8.556, 260.46431461109955), (-8.556, 260.17431461109953), (-8.556, 260.46431461109955), (-8.556, 260.26431461109956), (-10.8000000000085, 260.31871407661566), (-10.8000000000085, 259.99871407661567), (-0.300000000013218, 260.71), (-0.300000000013218, 260.42), (-8.556, 260.17431461109953), (-8.556, 260.0643146110996), (-8.556, 260.26431461109956), (-8.556, 260.0643146110996), (-10.8000000000085, 259.99871407661567), (-10.8000000000085, 259.6787140766157)]</t>
+          <t>[(-0.300000000013218, 261.0), (-0.300000000013218, 260.72), (-8.556, 260.46431461109955), (-8.556, 260.1843146110996), (-8.556, 260.46431461109955), (-8.556, 260.26431461109956), (-8.80000000000589, 260.4484828239272), (-8.80000000000589, 260.14848282392717), (-0.300000000013218, 260.72), (-0.300000000013218, 260.42), (-8.556, 260.1843146110996), (-8.556, 260.0643146110996), (-8.556, 260.26431461109956), (-8.556, 260.0643146110996), (-8.80000000000589, 260.14848282392717), (-8.80000000000589, 259.84848282392716)]</t>
         </is>
       </c>
     </row>
@@ -3047,7 +3047,7 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>[(-0.300000000003449, 262.0), (-0.300000000003449, 261.67), (-8.125, 261.4522500000002), (-8.125, 261.19225000000023), (-8.125, 261.4522500000002), (-8.125, 261.19225000000023), (-10.7999999999931, 261.2650000000007), (-10.7999999999931, 260.8950000000007), (-0.300000000003449, 261.67), (-0.300000000003449, 261.34), (-8.125, 261.19225000000023), (-8.125, 260.93225000000024), (-8.125, 261.19225000000023), (-8.125, 260.93225000000024), (-10.7999999999931, 260.8950000000007), (-10.7999999999931, 260.5250000000007)]</t>
+          <t>[(-0.300000000003449, 262.0), (-0.300000000003449, 261.67), (-8.125, 261.4522500000002), (-8.125, 261.19225000000023), (-8.125, 261.4522500000002), (-8.125, 261.19225000000023), (-8.79999999999307, 261.4050000000007), (-8.79999999999307, 261.0550000000007), (-0.300000000003449, 261.67), (-0.300000000003449, 261.34), (-8.125, 261.19225000000023), (-8.125, 260.93225000000024), (-8.125, 261.19225000000023), (-8.125, 260.93225000000024), (-8.79999999999307, 261.0550000000007), (-8.79999999999307, 260.7050000000007)]</t>
         </is>
       </c>
     </row>
@@ -3057,7 +3057,7 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>[(-0.300000000002442, 263.0), (-0.300000000002442, 262.66), (-7.604, 262.48872000000017), (-7.604, 262.2087200000002), (-7.604, 262.48872000000017), (-7.604, 262.2087200000002), (-10.8000000000025, 262.265), (-10.8000000000025, 261.865), (-0.300000000002442, 262.66), (-0.300000000002442, 262.32), (-7.604, 262.2087200000002), (-7.604, 261.92872000000017), (-7.604, 262.2087200000002), (-7.604, 261.92872000000017), (-10.8000000000025, 261.865), (-10.8000000000025, 261.465)]</t>
+          <t>[(-0.300000000002442, 263.0), (-0.300000000002442, 262.66), (-7.604, 262.48872000000017), (-7.604, 262.2087200000002), (-7.604, 262.48872000000017), (-7.604, 262.2087200000002), (-8.80000000000119, 262.4050000000001), (-8.80000000000119, 262.0250000000001), (-0.300000000002442, 262.66), (-0.300000000002442, 262.32), (-7.604, 262.2087200000002), (-7.604, 261.92872000000017), (-7.604, 262.2087200000002), (-7.604, 261.92872000000017), (-8.80000000000119, 262.0250000000001), (-8.80000000000119, 261.6450000000001)]</t>
         </is>
       </c>
     </row>
@@ -3067,7 +3067,7 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>[(-0.300000000000919, 264.0), (-0.300000000000919, 263.7), (-6.979, 263.53247000000005), (-6.979, 263.23247000000003), (-6.979, 263.53247000000005), (-6.979, 263.29247000000004), (-10.8000000000038, 263.2649999999998), (-10.8000000000038, 262.9449999999998), (-0.300000000000919, 263.7), (-0.300000000000919, 263.41), (-6.979, 263.23247000000003), (-6.979, 263.05247), (-6.979, 263.29247000000004), (-6.979, 263.05247), (-10.8000000000038, 262.9449999999998), (-10.8000000000038, 262.62499999999983)]</t>
+          <t>[(-0.300000000000919, 264.0), (-0.300000000000919, 263.7), (-6.979, 263.53247000000005), (-6.979, 263.23247000000003), (-6.979, 263.53247000000005), (-6.979, 263.29247000000004), (-8.80000000000047, 263.40500000000003), (-8.80000000000047, 263.08500000000004), (-0.300000000000919, 263.7), (-0.300000000000919, 263.41), (-6.979, 263.23247000000003), (-6.979, 263.05247), (-6.979, 263.29247000000004), (-6.979, 263.05247), (-8.80000000000047, 263.08500000000004), (-8.80000000000047, 262.76500000000004)]</t>
         </is>
       </c>
     </row>
@@ -3077,7 +3077,7 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>[(-0.300000000007065, 265.0), (-0.300000000007065, 264.85), (-6.557, 264.5620100000005), (-6.557, 264.4120100000005), (-6.557, 264.5620100000005), (-6.557, 264.4420100000005), (-10.352, 264.2963600000005), (-10.352, 264.1763600000005), (-0.300000000007065, 264.85), (-0.300000000007065, 264.55), (-6.557, 264.4120100000005), (-6.557, 264.2520100000005), (-6.557, 264.4420100000005), (-6.557, 264.2520100000005), (-10.352, 264.1763600000005), (-10.352, 263.8763600000005)]</t>
+          <t>[(-0.300000000007065, 265.0), (-0.300000000007065, 264.85), (-6.557, 264.5620100000005), (-6.557, 264.4120100000005), (-6.557, 264.5620100000005), (-6.557, 264.4120100000005), (-8.80000000000492, 264.40500000000014), (-8.80000000000492, 264.25500000000017), (-0.300000000007065, 264.85), (-0.300000000007065, 264.55), (-6.557, 264.4120100000005), (-6.557, 264.2520100000005), (-6.557, 264.4120100000005), (-6.557, 264.2520100000005), (-8.80000000000492, 264.25500000000017), (-8.80000000000492, 263.95500000000015)]</t>
         </is>
       </c>
     </row>
@@ -3087,7 +3087,7 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>[(-0.299999999999714, 266.0), (-0.299999999999714, 265.75), (-6.725, 265.55025), (-6.725, 265.30025), (-6.725, 265.55025), (-6.725, 265.30025), (-10.403, 265.29278999999997), (-10.403, 265.04278999999997), (-0.299999999999714, 265.75), (-0.299999999999714, 265.5), (-6.725, 265.30025), (-6.725, 265.19025), (-6.725, 265.30025), (-6.725, 265.19025), (-10.403, 265.04278999999997), (-10.403, 264.80278999999996)]</t>
+          <t>[(-0.299999999999714, 266.0), (-0.299999999999714, 265.8), (-6.725, 265.55025), (-6.725, 265.35025), (-6.725, 265.55025), (-6.725, 265.33025), (-8.79999999999297, 265.4050000000005), (-8.79999999999297, 265.18500000000046), (-0.299999999999714, 265.8), (-0.299999999999714, 265.5), (-6.725, 265.35025), (-6.725, 265.19025), (-6.725, 265.33025), (-6.725, 265.19025), (-8.79999999999297, 265.18500000000046), (-8.79999999999297, 264.8850000000005)]</t>
         </is>
       </c>
     </row>
@@ -3097,7 +3097,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>[(-0.300000000004976, 267.0), (-0.300000000004976, 266.71), (-6.746, 266.54878000000036), (-6.746, 266.25878000000034), (-6.746, 266.54878000000036), (-6.746, 266.29878000000036), (-10.553, 266.28229000000033), (-10.553, 265.96229000000034), (-0.300000000004976, 266.71), (-0.300000000004976, 266.42), (-6.746, 266.25878000000034), (-6.746, 266.04878000000036), (-6.746, 266.29878000000036), (-6.746, 266.04878000000036), (-10.553, 265.96229000000034), (-10.553, 265.64229000000034)]</t>
+          <t>[(-0.300000000004976, 267.0), (-0.300000000004976, 266.71), (-6.746, 266.54878000000036), (-6.746, 266.25878000000034), (-6.746, 266.54878000000036), (-6.746, 266.29878000000036), (-8.80000000000022, 266.4050000000003), (-8.80000000000022, 266.0850000000003), (-0.300000000004976, 266.71), (-0.300000000004976, 266.42), (-6.746, 266.25878000000034), (-6.746, 266.04878000000036), (-6.746, 266.29878000000036), (-6.746, 266.04878000000036), (-8.80000000000022, 266.0850000000003), (-8.80000000000022, 265.7650000000003)]</t>
         </is>
       </c>
     </row>
@@ -3107,7 +3107,7 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>[(-0.299999999999178, 268.0), (-0.299999999999178, 267.8), (-6.694, 267.5524199999999), (-6.694, 267.35241999999994), (-6.694, 267.5524199999999), (-6.694, 267.29241999999994), (-10.486, 267.2869799999999), (-10.486, 266.9669799999999), (-0.299999999999178, 267.8), (-0.299999999999178, 267.6), (-6.694, 267.35241999999994), (-6.694, 267.15241999999995), (-6.694, 267.29241999999994), (-6.694, 267.03241999999995), (-10.486, 266.9669799999999), (-10.486, 266.6469799999999), (-0.299999999999178, 267.6), (-0.299999999999178, 267.4), (-6.694, 267.15241999999995), (-6.694, 267.04241999999994), (-6.694, 267.03241999999995), (-6.694, 267.03241999999995), (-10.486, 266.6469799999999), (-10.486, 266.6469799999999)]</t>
+          <t>[(-0.299999999999178, 268.0), (-0.299999999999178, 267.7), (-6.694, 267.5524199999999), (-6.694, 267.2524199999999), (-6.694, 267.5524199999999), (-6.694, 267.29241999999994), (-8.80000000000594, 267.4049999999995), (-8.80000000000594, 267.06499999999954), (-0.299999999999178, 267.7), (-0.299999999999178, 267.4), (-6.694, 267.2524199999999), (-6.694, 267.04241999999994), (-6.694, 267.29241999999994), (-6.694, 267.03241999999995), (-8.80000000000594, 267.06499999999954), (-8.80000000000594, 266.7249999999995)]</t>
         </is>
       </c>
     </row>
@@ -3117,7 +3117,7 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>[(-0.299999999996696, 269.0), (-0.299999999996696, 268.82), (-6.61, 268.55829999999975), (-6.61, 268.37829999999974), (-6.61, 268.55829999999975), (-6.61, 268.31829999999974), (-10.361, 268.29572999999976), (-10.361, 267.99572999999975), (-0.299999999996696, 268.82), (-0.299999999996696, 268.64), (-6.61, 268.37829999999974), (-6.61, 268.19829999999973), (-6.61, 268.31829999999974), (-6.61, 268.07829999999973), (-10.361, 267.99572999999975), (-10.361, 267.69572999999974), (-0.299999999996696, 268.64), (-0.299999999996696, 268.46), (-6.61, 268.19829999999973), (-6.61, 268.07829999999973), (-6.61, 268.07829999999973), (-6.61, 268.07829999999973), (-10.361, 267.69572999999974), (-10.361, 267.69572999999974)]</t>
+          <t>[(-0.299999999996696, 269.0), (-0.299999999996696, 268.82), (-6.61, 268.55829999999975), (-6.61, 268.37829999999974), (-6.61, 268.55829999999975), (-6.61, 268.31829999999974), (-8.80000000000356, 268.4049999999995), (-8.80000000000356, 268.0849999999995), (-0.299999999996696, 268.82), (-0.299999999996696, 268.64), (-6.61, 268.37829999999974), (-6.61, 268.19829999999973), (-6.61, 268.31829999999974), (-6.61, 268.07829999999973), (-8.80000000000356, 268.0849999999995), (-8.80000000000356, 267.76499999999953), (-0.299999999996696, 268.64), (-0.299999999996696, 268.46), (-6.61, 268.19829999999973), (-6.61, 268.07829999999973), (-6.61, 268.07829999999973), (-6.61, 268.07829999999973), (-8.80000000000356, 267.76499999999953), (-8.80000000000356, 267.76499999999953)]</t>
         </is>
       </c>
     </row>
@@ -3127,7 +3127,7 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>[(-0.300000000003499, 270.0), (-0.300000000003499, 269.77), (-5.972, 269.6029600000002), (-5.972, 269.3729600000002), (-5.972, 269.6029600000002), (-5.972, 269.34296000000023), (-9.945, 269.32485000000025), (-9.945, 269.06485000000026), (-0.300000000003499, 269.77), (-0.300000000003499, 269.55), (-5.972, 269.3729600000002), (-5.972, 269.21296000000024), (-5.972, 269.34296000000023), (-5.972, 269.21296000000024), (-9.945, 269.06485000000026), (-9.945, 268.8048500000003)]</t>
+          <t>[(-0.300000000003499, 270.0), (-0.300000000003499, 269.77), (-5.972, 269.6029600000002), (-5.972, 269.3729600000002), (-5.972, 269.6029600000002), (-5.972, 269.33296000000024), (-8.80000000000085, 269.4050000000002), (-8.80000000000085, 269.1350000000002), (-0.300000000003499, 269.77), (-0.300000000003499, 269.55), (-5.972, 269.3729600000002), (-5.972, 269.21296000000024), (-5.972, 269.33296000000024), (-5.972, 269.21296000000024), (-8.80000000000085, 269.1350000000002), (-8.80000000000085, 268.8650000000002)]</t>
         </is>
       </c>
     </row>
@@ -3137,7 +3137,7 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>[(-0.29999999999453, 271.0), (-0.29999999999453, 270.8), (-5.101, 270.6639299999996), (-5.101, 270.4639299999996), (-5.101, 270.6639299999996), (-5.101, 270.4239299999996), (-8.92, 270.39659999999964), (-8.92, 270.1565999999996), (-0.29999999999453, 270.8), (-0.29999999999453, 270.6), (-5.101, 270.4639299999996), (-5.101, 270.3139299999996), (-5.101, 270.4239299999996), (-5.101, 270.3139299999996), (-8.92, 270.1565999999996), (-8.92, 269.9165999999996)]</t>
+          <t>[(-0.29999999999453, 271.0), (-0.29999999999453, 270.8), (-5.101, 270.6639299999996), (-5.101, 270.4639299999996), (-5.101, 270.6639299999996), (-5.101, 270.4839299999996), (-8.79999999999673, 270.40499999999986), (-8.79999999999673, 270.22499999999985), (-0.29999999999453, 270.8), (-0.29999999999453, 270.6), (-5.101, 270.4639299999996), (-5.101, 270.3139299999996), (-5.101, 270.4839299999996), (-5.101, 270.3139299999996), (-8.79999999999673, 270.22499999999985), (-8.79999999999673, 269.92499999999984)]</t>
         </is>
       </c>
     </row>
@@ -3147,7 +3147,7 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>[(-0.299999999979226, 272.0), (-0.299999999979226, 271.8), (-4.282, 271.72125999999855), (-4.282, 271.52125999999856), (-4.282, 271.72125999999855), (-4.282, 271.61125999999854), (-7.976, 271.46267999999856), (-7.976, 271.35267999999854), (-0.299999999979226, 271.8), (-0.299999999979226, 271.61), (-4.282, 271.52125999999856), (-4.282, 271.40125999999856), (-4.282, 271.61125999999854), (-4.282, 271.40125999999856), (-7.976, 271.35267999999854), (-7.976, 271.20267999999857)]</t>
+          <t>[(-0.299999999979226, 272.0), (-0.299999999979226, 271.8), (-4.282, 271.72125999999855), (-4.282, 271.52125999999856), (-4.282, 271.72125999999855), (-4.282, 271.60125999999855), (-7.976, 271.46267999999856), (-7.976, 271.34267999999855), (-0.299999999979226, 271.8), (-0.299999999979226, 271.61), (-4.282, 271.52125999999856), (-4.282, 271.40125999999856), (-4.282, 271.60125999999855), (-4.282, 271.40125999999856), (-7.976, 271.34267999999855), (-7.976, 271.20267999999857)]</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>[(-0.300000000058636, 274.0), (-0.300000000058636, 273.86), (-5.91, 273.6664670281131), (-5.91, 273.52646702811313), (-0.300000000058636, 273.86), (-0.300000000058636, 273.74), (-5.91, 273.52646702811313), (-5.91, 273.4164670281131)]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3177,7 +3177,7 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>[(-0.300000000024012, 275.0), (-0.300000000024012, 274.87), (-4.864, 274.7598543909959), (-4.864, 274.6298543909959), (-0.300000000024012, 274.87), (-0.300000000024012, 274.74), (-4.864, 274.6298543909959), (-4.864, 274.4998543909959), (-0.300000000024012, 274.74), (-0.300000000024012, 274.63), (-4.864, 274.4998543909959), (-4.864, 274.3898543909959)]</t>
+          <t>[(-0.300000000024012, 275.0), (-0.300000000024012, 274.81), (-4.864, 274.7598543909959), (-4.864, 274.5698543909959), (-0.300000000024012, 274.81), (-0.300000000024012, 274.63), (-4.864, 274.5698543909959), (-4.864, 274.3898543909959)]</t>
         </is>
       </c>
     </row>
@@ -3257,7 +3257,7 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>[(-0.30000000002085, 283.0), (-0.30000000002085, 282.8), (-3.153, 283.16102375221243), (-3.153, 282.96102375221244), (-0.30000000002085, 282.8), (-0.30000000002085, 282.6), (-3.153, 282.96102375221244), (-3.153, 282.76102375221245), (-0.30000000002085, 282.6), (-0.30000000002085, 282.4), (-3.153, 282.76102375221245), (-3.153, 282.5610237522124), (-0.30000000002085, 282.4), (-0.30000000002085, 282.29), (-3.153, 282.5610237522124), (-3.153, 282.39102375221245)]</t>
+          <t>[(-0.30000000002085, 283.0), (-0.30000000002085, 282.74), (-3.153, 283.16102375221243), (-3.153, 282.90102375221244), (-0.30000000002085, 282.74), (-0.30000000002085, 282.48), (-3.153, 282.90102375221244), (-3.153, 282.64102375221245), (-0.30000000002085, 282.48), (-0.30000000002085, 282.29), (-3.153, 282.64102375221245), (-3.153, 282.39102375221245)]</t>
         </is>
       </c>
     </row>
@@ -3347,7 +3347,7 @@
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>[(-0.300000000006342, 292.0), (-0.300000000006342, 291.86), (-2.517, 291.84481000000045), (-2.517, 291.70481000000046), (-0.300000000006342, 291.86), (-0.300000000006342, 291.73), (-2.517, 291.70481000000046), (-2.517, 291.59481000000045)]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4867,7 +4867,7 @@
       </c>
       <c r="B445" t="inlineStr">
         <is>
-          <t>[(-0.300000000006756, 444.0), (-0.300000000006756, 443.86), (-2.622, 443.9419500000002), (-2.622, 443.8019500000002), (-0.300000000006756, 443.86), (-0.300000000006756, 443.72), (-2.622, 443.8019500000002), (-2.622, 443.6619500000002), (-0.300000000006756, 443.72), (-0.300000000006756, 443.61), (-2.622, 443.6619500000002), (-2.622, 443.5519500000002)]</t>
+          <t>[(-0.300000000006756, 444.0), (-0.300000000006756, 443.8), (-2.622, 443.9419500000002), (-2.622, 443.7419500000002), (-0.300000000006756, 443.8), (-0.300000000006756, 443.61), (-2.622, 443.7419500000002), (-2.622, 443.5519500000002)]</t>
         </is>
       </c>
     </row>
@@ -4877,7 +4877,7 @@
       </c>
       <c r="B446" t="inlineStr">
         <is>
-          <t>[(-0.300000000006756, 445.0), (-0.300000000006756, 444.87), (-3.713, 444.91467500000016), (-3.713, 444.78467500000016), (-0.300000000006756, 444.87), (-0.300000000006756, 444.74), (-3.713, 444.78467500000016), (-3.713, 444.65467500000017), (-0.300000000006756, 444.74), (-0.300000000006756, 444.63), (-3.713, 444.65467500000017), (-3.713, 444.53467500000016)]</t>
+          <t>[(-0.300000000006756, 445.0), (-0.300000000006756, 444.81), (-3.713, 444.91467500000016), (-3.713, 444.72467500000016), (-0.300000000006756, 444.81), (-0.300000000006756, 444.63), (-3.713, 444.72467500000016), (-3.713, 444.53467500000016)]</t>
         </is>
       </c>
     </row>
@@ -5007,7 +5007,7 @@
       </c>
       <c r="B459" t="inlineStr">
         <is>
-          <t>[(-0.300000000006756, 458.0), (-0.300000000006756, 457.89), (-8.13, 457.8042500000002), (-8.13, 457.6942500000002), (-0.300000000006756, 457.89), (-0.300000000006756, 457.62), (-8.13, 457.6942500000002), (-8.13, 457.5142500000002)]</t>
+          <t>[(-0.300000000006756, 458.0), (-0.300000000006756, 457.88), (-8.13, 457.8042500000002), (-8.13, 457.6842500000002), (-0.300000000006756, 457.88), (-0.300000000006756, 457.62), (-8.13, 457.6842500000002), (-8.13, 457.5142500000002)]</t>
         </is>
       </c>
     </row>
@@ -5047,7 +5047,7 @@
       </c>
       <c r="B463" t="inlineStr">
         <is>
-          <t>[(-0.300000000000589, 462.0), (-0.300000000000589, 461.88), (-8.916, 462.3270511115744), (-8.916, 462.0570511115744), (-0.300000000000589, 461.88), (-0.300000000000589, 461.76), (-8.916, 462.0570511115744), (-8.916, 461.7870511115744)]</t>
+          <t>[(-0.300000000000589, 462.0), (-0.300000000000589, 461.88), (-8.79999999999889, 462.3226479164789), (-8.79999999999889, 462.0526479164789), (-0.300000000000589, 461.88), (-0.300000000000589, 461.76), (-8.79999999999889, 462.0526479164789), (-8.79999999999889, 461.7826479164789)]</t>
         </is>
       </c>
     </row>
@@ -5057,7 +5057,7 @@
       </c>
       <c r="B464" t="inlineStr">
         <is>
-          <t>[(-0.3000000000414, 463.0), (-0.3000000000414, 462.88), (-8.991, 463.4009208569532), (-8.991, 463.10092085695317), (-0.3000000000414, 462.88), (-0.3000000000414, 462.76), (-8.991, 463.10092085695317), (-8.991, 462.80092085695316)]</t>
+          <t>[(-0.3000000000414, 463.0), (-0.3000000000414, 462.88), (-8.80000000001008, 463.39210991647747), (-8.80000000001008, 463.09210991647745), (-0.3000000000414, 462.88), (-0.3000000000414, 462.76), (-8.80000000001008, 463.09210991647745), (-8.80000000001008, 462.79210991647744)]</t>
         </is>
       </c>
     </row>
@@ -5067,7 +5067,7 @@
       </c>
       <c r="B465" t="inlineStr">
         <is>
-          <t>[(-0.30000000008908, 464.0), (-0.30000000008908, 463.85), (-2.353, 464.11148319346944), (-2.353, 463.96148319346946), (-2.353, 464.11148319346944), (-2.353, 463.97148319346945), (-9.118, 464.4788401364083), (-9.118, 464.1988401364083), (-0.30000000008908, 463.85), (-0.30000000008908, 463.74), (-2.353, 463.96148319346946), (-2.353, 463.83148319346947), (-2.353, 463.97148319346945), (-2.353, 463.83148319346947), (-9.118, 464.1988401364083), (-9.118, 463.9188401364083)]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5077,7 +5077,7 @@
       </c>
       <c r="B466" t="inlineStr">
         <is>
-          <t>[(-0.300000000030209, 465.0), (-0.300000000030209, 464.85), (-2.525, 465.13900593695877), (-2.525, 464.9890059369588), (-2.525, 465.13900593695877), (-2.525, 464.9990059369588), (-9.207, 465.5564610698896), (-9.207, 465.2464610698896), (-0.300000000030209, 464.85), (-0.300000000030209, 464.74), (-2.525, 464.9890059369588), (-2.525, 464.8590059369588), (-2.525, 464.9990059369588), (-2.525, 464.8590059369588), (-9.207, 465.2464610698896), (-9.207, 464.9364610698896)]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5097,7 +5097,7 @@
       </c>
       <c r="B468" t="inlineStr">
         <is>
-          <t>[(-0.300000000003487, 467.0), (-0.300000000003487, 466.86), (-3.104, 467.1962799999998), (-3.104, 467.0562799999998), (-3.104, 467.1962799999998), (-3.104, 467.0662799999998), (-9.819, 467.66632999999973), (-9.819, 467.3663299999997), (-0.300000000003487, 466.86), (-0.300000000003487, 466.75), (-3.104, 467.0562799999998), (-3.104, 466.9362799999998), (-3.104, 467.0662799999998), (-3.104, 466.9362799999998), (-9.819, 467.3663299999997), (-9.819, 467.0663299999997)]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5107,7 +5107,7 @@
       </c>
       <c r="B469" t="inlineStr">
         <is>
-          <t>[(-0.300000000001038, 468.0), (-0.300000000001038, 467.87), (-3.425, 468.21874999999994), (-3.425, 468.08874999999995), (-3.425, 468.21874999999994), (-3.425, 468.09874999999994), (-10.177, 468.69138999999996), (-10.177, 468.41139), (-0.300000000001038, 467.87), (-0.300000000001038, 467.75), (-3.425, 468.08874999999995), (-3.425, 467.96874999999994), (-3.425, 468.09874999999994), (-3.425, 467.97874999999993), (-10.177, 468.41139), (-10.177, 468.1313899999999)]</t>
+          <t>[(-0.300000000001038, 468.0), (-0.300000000001038, 467.87), (-3.425, 468.21874999999994), (-3.425, 468.08874999999995), (-3.425, 468.21874999999994), (-3.425, 468.09874999999994), (-8.80000000000329, 468.59500000000014), (-8.80000000000329, 468.32500000000016), (-0.300000000001038, 467.87), (-0.300000000001038, 467.75), (-3.425, 468.08874999999995), (-3.425, 467.96874999999994), (-3.425, 468.09874999999994), (-3.425, 467.97874999999993), (-8.80000000000329, 468.32500000000016), (-8.80000000000329, 468.0550000000001)]</t>
         </is>
       </c>
     </row>
@@ -5117,7 +5117,7 @@
       </c>
       <c r="B470" t="inlineStr">
         <is>
-          <t>[(-0.300000000022424, 469.0), (-0.300000000022424, 468.84), (-3.597, 469.2307899999984), (-3.597, 469.0707899999984), (-3.597, 469.2307899999984), (-3.597, 469.0707899999984), (-10.382, 469.70573999999846), (-10.382, 469.38573999999846), (-0.300000000022424, 468.84), (-0.300000000022424, 468.72), (-3.597, 469.0707899999984), (-3.597, 468.9107899999984), (-3.597, 469.0707899999984), (-3.597, 468.9107899999984), (-10.382, 469.38573999999846), (-10.382, 469.06573999999847)]</t>
+          <t>[(-0.300000000022424, 469.0), (-0.300000000022424, 468.84), (-3.597, 469.2307899999984), (-3.597, 469.0707899999984), (-3.597, 469.2307899999984), (-3.597, 469.0707899999984), (-8.80000000001358, 469.5949999999994), (-8.80000000001358, 469.2949999999994), (-0.300000000022424, 468.84), (-0.300000000022424, 468.72), (-3.597, 469.0707899999984), (-3.597, 468.9107899999984), (-3.597, 469.0707899999984), (-3.597, 468.9107899999984), (-8.80000000001358, 469.2949999999994), (-8.80000000001358, 468.9949999999994)]</t>
         </is>
       </c>
     </row>
@@ -5127,7 +5127,7 @@
       </c>
       <c r="B471" t="inlineStr">
         <is>
-          <t>[(-0.300000000006231, 470.0), (-0.300000000006231, 469.87), (-3.89, 470.25129999999956), (-3.89, 470.12129999999956), (-3.89, 470.25129999999956), (-3.89, 470.13129999999956), (-10.655, 470.72484999999955), (-10.655, 470.42484999999954), (-0.300000000006231, 469.87), (-0.300000000006231, 469.75), (-3.89, 470.12129999999956), (-3.89, 470.00129999999956), (-3.89, 470.13129999999956), (-3.89, 470.01129999999955), (-10.655, 470.42484999999954), (-10.655, 470.1248499999995)]</t>
+          <t>[(-0.300000000006231, 470.0), (-0.300000000006231, 469.87), (-3.89, 470.25129999999956), (-3.89, 470.12129999999956), (-3.89, 470.25129999999956), (-3.89, 470.13129999999956), (-8.80000000000392, 470.59499999999986), (-8.80000000000392, 470.3149999999999), (-0.300000000006231, 469.87), (-0.300000000006231, 469.75), (-3.89, 470.12129999999956), (-3.89, 470.00129999999956), (-3.89, 470.13129999999956), (-3.89, 470.01129999999955), (-8.80000000000392, 470.3149999999999), (-8.80000000000392, 470.03499999999985)]</t>
         </is>
       </c>
     </row>
@@ -5137,7 +5137,7 @@
       </c>
       <c r="B472" t="inlineStr">
         <is>
-          <t>[(-0.300000000005409, 471.0), (-0.300000000005409, 470.84), (-4.191, 471.2723699999996), (-4.191, 471.1123699999996), (-4.191, 471.2723699999996), (-4.191, 471.1123699999996), (-10.7999999999981, 471.7349999999995), (-10.7999999999981, 471.4149999999995), (-0.300000000005409, 470.84), (-0.300000000005409, 470.72), (-4.191, 471.1123699999996), (-4.191, 470.9623699999996), (-4.191, 471.1123699999996), (-4.191, 470.95236999999963), (-10.7999999999981, 471.4149999999995), (-10.7999999999981, 471.0949999999995)]</t>
+          <t>[(-0.300000000005409, 471.0), (-0.300000000005409, 470.84), (-4.191, 471.2723699999996), (-4.191, 471.1123699999996), (-4.191, 471.2723699999996), (-4.191, 471.1123699999996), (-8.79999999999882, 471.5949999999995), (-8.79999999999882, 471.2949999999995), (-0.300000000005409, 470.84), (-0.300000000005409, 470.72), (-4.191, 471.1123699999996), (-4.191, 470.9623699999996), (-4.191, 471.1123699999996), (-4.191, 470.95236999999963), (-8.79999999999882, 471.2949999999995), (-8.79999999999882, 470.9949999999995)]</t>
         </is>
       </c>
     </row>
@@ -5147,7 +5147,7 @@
       </c>
       <c r="B473" t="inlineStr">
         <is>
-          <t>[(-0.300000000001446, 472.0), (-0.300000000001446, 471.86), (-4.416, 472.2881199999999), (-4.416, 472.1481199999999), (-4.416, 472.2881199999999), (-4.416, 472.1481199999999), (-10.799999999994, 472.7349999999995), (-10.799999999994, 472.4249999999995), (-0.300000000001446, 471.86), (-0.300000000001446, 471.74), (-4.416, 472.1481199999999), (-4.416, 472.0181199999999), (-4.416, 472.1481199999999), (-4.416, 472.0081199999999), (-10.799999999994, 472.4249999999995), (-10.799999999994, 472.1149999999995)]</t>
+          <t>[(-0.300000000001446, 472.0), (-0.300000000001446, 471.86), (-4.416, 472.2881199999999), (-4.416, 472.1481199999999), (-4.416, 472.2881199999999), (-4.416, 472.1481199999999), (-8.79999999999802, 472.59499999999974), (-8.79999999999802, 472.3049999999997), (-0.300000000001446, 471.86), (-0.300000000001446, 471.74), (-4.416, 472.1481199999999), (-4.416, 472.0181199999999), (-4.416, 472.1481199999999), (-4.416, 472.0081199999999), (-8.79999999999802, 472.3049999999997), (-8.79999999999802, 472.01499999999976)]</t>
         </is>
       </c>
     </row>
@@ -5157,7 +5157,7 @@
       </c>
       <c r="B474" t="inlineStr">
         <is>
-          <t>[(-0.300000000005773, 473.0), (-0.300000000005773, 472.86), (-4.582, 473.2997399999996), (-4.582, 473.1597399999996), (-4.582, 473.2997399999996), (-4.582, 473.1597399999996), (-10.7999999999967, 473.7349999999994), (-10.7999999999967, 473.4549999999994), (-0.300000000005773, 472.86), (-0.300000000005773, 472.75), (-4.582, 473.1597399999996), (-4.582, 473.0297399999996), (-4.582, 473.1597399999996), (-4.582, 473.0197399999996), (-10.7999999999967, 473.4549999999994), (-10.7999999999967, 473.1749999999994)]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5177,7 +5177,7 @@
       </c>
       <c r="B476" t="inlineStr">
         <is>
-          <t>[(-0.30000000000354, 475.0), (-0.30000000000354, 474.85), (-4.821, 475.31646999999975), (-4.821, 475.1664699999998), (-4.821, 475.31646999999975), (-4.821, 475.17646999999977), (-10.7999999999972, 475.73499999999956), (-10.7999999999972, 475.44499999999954), (-0.30000000000354, 474.85), (-0.30000000000354, 474.74), (-4.821, 475.1664699999998), (-4.821, 475.02646999999973), (-4.821, 475.17646999999977), (-4.821, 475.0364699999998), (-10.7999999999972, 475.44499999999954), (-10.7999999999972, 475.1549999999996)]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5187,7 +5187,7 @@
       </c>
       <c r="B477" t="inlineStr">
         <is>
-          <t>[(-0.300000000006208, 476.0), (-0.300000000006208, 475.85), (-4.916, 476.32311999999956), (-4.916, 476.1731199999996), (-4.916, 476.32311999999956), (-4.916, 476.1831199999996), (-10.8000000000071, 476.73500000000007), (-10.8000000000071, 476.4650000000001), (-0.300000000006208, 475.85), (-0.300000000006208, 475.74), (-4.916, 476.1731199999996), (-4.916, 476.03311999999954), (-4.916, 476.1831199999996), (-4.916, 476.0431199999996), (-10.8000000000071, 476.4650000000001), (-10.8000000000071, 476.19500000000005)]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5197,7 +5197,7 @@
       </c>
       <c r="B478" t="inlineStr">
         <is>
-          <t>[(-0.299999999994854, 477.0), (-0.299999999994854, 476.87), (-4.91, 477.32270000000034), (-4.91, 477.19270000000034), (-4.91, 477.32270000000034), (-4.91, 477.20270000000033), (-10.8000000000055, 477.73500000000075), (-10.8000000000055, 477.4550000000008), (-0.299999999994854, 476.87), (-0.299999999994854, 476.75), (-4.91, 477.19270000000034), (-4.91, 477.07270000000034), (-4.91, 477.20270000000033), (-4.91, 477.08270000000033), (-10.8000000000055, 477.4550000000008), (-10.8000000000055, 477.17500000000075)]</t>
+          <t>[(-0.299999999994854, 477.0), (-0.299999999994854, 476.87), (-4.91, 477.32270000000034), (-4.91, 477.19270000000034), (-4.91, 477.32270000000034), (-4.91, 477.20270000000033), (-8.79999999999481, 477.59499999999997), (-8.79999999999481, 477.325), (-0.299999999994854, 476.87), (-0.299999999994854, 476.75), (-4.91, 477.19270000000034), (-4.91, 477.07270000000034), (-4.91, 477.20270000000033), (-4.91, 477.08270000000033), (-8.79999999999481, 477.325), (-8.79999999999481, 477.05499999999995)]</t>
         </is>
       </c>
     </row>
@@ -5217,7 +5217,7 @@
       </c>
       <c r="B480" t="inlineStr">
         <is>
-          <t>[(-0.299999999998833, 479.0), (-0.299999999998833, 478.86), (-4.907, 479.3224900000001), (-4.907, 479.1824900000001), (-4.907, 479.3224900000001), (-4.907, 479.1924900000001), (-10.8000000000022, 479.73500000000024), (-10.8000000000022, 479.45500000000027), (-0.299999999998833, 478.86), (-0.299999999998833, 478.75), (-4.907, 479.1824900000001), (-4.907, 479.0624900000001), (-4.907, 479.1924900000001), (-4.907, 479.0624900000001), (-10.8000000000022, 479.45500000000027), (-10.8000000000022, 479.17500000000024)]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5227,7 +5227,7 @@
       </c>
       <c r="B481" t="inlineStr">
         <is>
-          <t>[(-0.299999999998704, 480.0), (-0.299999999998704, 479.86), (-4.838, 480.3176600000001), (-4.838, 480.1776600000001), (-4.838, 480.3176600000001), (-4.838, 480.1776600000001), (-10.7999999999974, 480.7349999999999), (-10.7999999999974, 480.4549999999999), (-0.299999999998704, 479.86), (-0.299999999998704, 479.75), (-4.838, 480.1776600000001), (-4.838, 480.0476600000001), (-4.838, 480.1776600000001), (-4.838, 480.03766000000013), (-10.7999999999974, 480.4549999999999), (-10.7999999999974, 480.1749999999999)]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5247,7 +5247,7 @@
       </c>
       <c r="B483" t="inlineStr">
         <is>
-          <t>[(-0.300000000032176, 482.0), (-0.300000000032176, 481.84), (-4.711, 482.3017570240261), (-4.711, 482.14175702402605), (-4.711, 482.3017570240261), (-4.711, 482.14175702402605), (-10.7999999999906, 482.71830622359647), (-10.7999999999906, 482.3983062235965), (-0.300000000032176, 481.84), (-0.300000000032176, 481.73), (-4.711, 482.14175702402605), (-4.711, 481.99175702402607), (-4.711, 482.14175702402605), (-4.711, 481.9817570240261), (-10.7999999999906, 482.3983062235965), (-10.7999999999906, 482.0783062235965)]</t>
+          <t>[(-0.300000000032176, 482.0), (-0.300000000032176, 481.88), (-4.711, 482.3017570240261), (-4.711, 482.18175702402607), (-4.711, 482.3017570240261), (-4.711, 482.14175702402605), (-8.79999999998781, 482.58148599052976), (-8.79999999998781, 482.28148599052975), (-0.300000000032176, 481.88), (-0.300000000032176, 481.73), (-4.711, 482.18175702402607), (-4.711, 481.99175702402607), (-4.711, 482.14175702402605), (-4.711, 481.9817570240261), (-8.79999999998781, 482.28148599052975), (-8.79999999998781, 481.98148599052973)]</t>
         </is>
       </c>
     </row>
@@ -5257,7 +5257,7 @@
       </c>
       <c r="B484" t="inlineStr">
         <is>
-          <t>[(-0.300000000018094, 483.0), (-0.300000000018094, 482.83), (-4.708, 483.26552961767754), (-4.708, 483.0955296176775), (-4.708, 483.26552961767754), (-4.708, 483.1055296176775), (-10.8000000000099, 483.6325002235988), (-10.8000000000099, 483.3125002235988), (-0.300000000018094, 482.83), (-0.300000000018094, 482.71), (-4.708, 483.0955296176775), (-4.708, 482.93552961767756), (-4.708, 483.1055296176775), (-4.708, 482.94552961767755), (-10.8000000000099, 483.3125002235988), (-10.8000000000099, 482.9925002235988)]</t>
+          <t>[(-0.300000000018094, 483.0), (-0.300000000018094, 482.83), (-4.708, 483.26552961767754), (-4.708, 483.0955296176775), (-4.708, 483.26552961767754), (-4.708, 483.1055296176775), (-8.80000000001151, 483.5120239905324), (-8.80000000001151, 483.2020239905324), (-0.300000000018094, 482.83), (-0.300000000018094, 482.71), (-4.708, 483.0955296176775), (-4.708, 482.93552961767756), (-4.708, 483.1055296176775), (-4.708, 482.94552961767755), (-8.80000000001151, 483.2020239905324), (-8.80000000001151, 482.8920239905324)]</t>
         </is>
       </c>
     </row>
@@ -5267,7 +5267,7 @@
       </c>
       <c r="B485" t="inlineStr">
         <is>
-          <t>[(-0.299999999992888, 484.0), (-0.299999999992888, 483.82), (-4.827, 484.23570330954647), (-4.827, 484.05570330954646), (-4.827, 484.23570330954647), (-4.827, 484.05570330954646), (-10.799999999982, 484.54669422359876), (-10.799999999982, 484.22669422359877), (-0.299999999992888, 483.82), (-0.299999999992888, 483.69), (-4.827, 484.05570330954646), (-4.827, 483.87570330954645), (-4.827, 484.05570330954646), (-4.827, 483.87570330954645), (-10.799999999982, 484.22669422359877), (-10.799999999982, 483.9066942235988)]</t>
+          <t>[(-0.299999999992888, 484.0), (-0.299999999992888, 483.82), (-4.827, 484.23570330954647), (-4.827, 484.05570330954646), (-4.827, 484.23570330954647), (-4.827, 484.05570330954646), (-8.79999999998665, 484.44256199053245), (-8.79999999998665, 484.13256199053245), (-0.299999999992888, 483.82), (-0.299999999992888, 483.69), (-4.827, 484.05570330954646), (-4.827, 483.87570330954645), (-4.827, 484.05570330954646), (-4.827, 483.87570330954645), (-8.79999999998665, 484.13256199053245), (-8.79999999998665, 483.82256199053245)]</t>
         </is>
       </c>
     </row>
@@ -5277,7 +5277,7 @@
       </c>
       <c r="B486" t="inlineStr">
         <is>
-          <t>[(-0.300000000049893, 485.0), (-0.300000000049893, 484.82), (-5.008, 485.20665350063643), (-5.008, 485.0266535006364), (-5.008, 485.20665350063643), (-5.008, 485.0266535006364), (-10.7999999999908, 485.4608882235967), (-10.7999999999908, 485.1708882235967), (-0.300000000049893, 484.82), (-0.300000000049893, 484.67), (-5.008, 485.0266535006364), (-5.008, 484.8566535006364), (-5.008, 485.0266535006364), (-5.008, 484.8466535006364), (-10.7999999999908, 485.1708882235967), (-10.7999999999908, 484.88088822359674)]</t>
+          <t>[(-0.300000000049893, 485.0), (-0.300000000049893, 484.82), (-5.008, 485.20665350063643), (-5.008, 485.0266535006364), (-5.008, 485.20665350063643), (-5.008, 485.0266535006364), (-8.79999999999442, 485.3730999905303), (-8.79999999999442, 485.0730999905303), (-0.300000000049893, 484.82), (-0.300000000049893, 484.67), (-5.008, 485.0266535006364), (-5.008, 484.8566535006364), (-5.008, 485.0266535006364), (-5.008, 484.8466535006364), (-8.79999999999442, 485.0730999905303), (-8.79999999999442, 484.7730999905303)]</t>
         </is>
       </c>
     </row>
@@ -5287,7 +5287,7 @@
       </c>
       <c r="B487" t="inlineStr">
         <is>
-          <t>[(-0.30000000013227, 486.0), (-0.30000000013227, 485.85), (-5.129, 486.17250210073445), (-5.129, 486.02250210073447), (-5.129, 486.17250210073445), (-5.129, 485.96250210073447), (-10.8000000000016, 486.37508222359463), (-10.8000000000016, 486.03508222359466), (-0.30000000013227, 485.85), (-0.30000000013227, 485.7), (-5.129, 486.02250210073447), (-5.129, 485.87250210073444), (-5.129, 485.96250210073447), (-5.129, 485.75250210073443), (-10.8000000000016, 486.03508222359466), (-10.8000000000016, 485.6950822235946), (-0.30000000013227, 485.7), (-0.30000000013227, 485.58), (-5.129, 485.87250210073444), (-5.129, 485.75250210073443), (-5.129, 485.75250210073443), (-5.129, 485.75250210073443), (-10.8000000000016, 485.6950822235946), (-10.8000000000016, 485.6950822235946)]</t>
+          <t>[(-0.30000000013227, 486.0), (-0.30000000013227, 485.85), (-5.129, 486.17250210073445), (-5.129, 486.02250210073447), (-5.129, 486.17250210073445), (-5.129, 485.96250210073447), (-8.79999999999924, 486.30363799052805), (-8.79999999999924, 485.96363799052807), (-0.30000000013227, 485.85), (-0.30000000013227, 485.7), (-5.129, 486.02250210073447), (-5.129, 485.87250210073444), (-5.129, 485.96250210073447), (-5.129, 485.75250210073443), (-8.79999999999924, 485.96363799052807), (-8.79999999999924, 485.62363799052804), (-0.30000000013227, 485.7), (-0.30000000013227, 485.58), (-5.129, 485.87250210073444), (-5.129, 485.75250210073443), (-5.129, 485.75250210073443), (-5.129, 485.75250210073443), (-8.79999999999924, 485.62363799052804), (-8.79999999999924, 485.62363799052804)]</t>
         </is>
       </c>
     </row>
@@ -5297,7 +5297,7 @@
       </c>
       <c r="B488" t="inlineStr">
         <is>
-          <t>[(-0.300000000002996, 487.0), (-0.300000000002996, 486.82), (-5.221, 487.1355741234601), (-5.221, 486.9555741234601), (-5.221, 487.1355741234601), (-5.221, 486.8855741234601), (-10.7999999999821, 487.28927622359873), (-10.7999999999821, 486.9392762235987), (-0.300000000002996, 486.82), (-0.300000000002996, 486.64), (-5.221, 486.9555741234601), (-5.221, 486.7755741234601), (-5.221, 486.8855741234601), (-5.221, 486.6355741234601), (-10.7999999999821, 486.9392762235987), (-10.7999999999821, 486.58927622359874), (-0.300000000002996, 486.64), (-0.300000000002996, 486.48), (-5.221, 486.7755741234601), (-5.221, 486.6355741234601), (-5.221, 486.6355741234601), (-5.221, 486.6355741234601), (-10.7999999999821, 486.58927622359874), (-10.7999999999821, 486.58927622359874)]</t>
+          <t>[(-0.300000000002996, 487.0), (-0.300000000002996, 486.82), (-5.221, 487.1355741234601), (-5.221, 486.9555741234601), (-5.221, 487.1355741234601), (-5.221, 486.8855741234601), (-8.79999999998253, 487.2341759905322), (-8.79999999998253, 486.8741759905322), (-0.300000000002996, 486.82), (-0.300000000002996, 486.64), (-5.221, 486.9555741234601), (-5.221, 486.7755741234601), (-5.221, 486.8855741234601), (-5.221, 486.6355741234601), (-8.79999999998253, 486.8741759905322), (-8.79999999998253, 486.5141759905322), (-0.300000000002996, 486.64), (-0.300000000002996, 486.48), (-5.221, 486.7755741234601), (-5.221, 486.6355741234601), (-5.221, 486.6355741234601), (-5.221, 486.6355741234601), (-8.79999999998253, 486.5141759905322), (-8.79999999998253, 486.5141759905322)]</t>
         </is>
       </c>
     </row>
@@ -5307,7 +5307,7 @@
       </c>
       <c r="B489" t="inlineStr">
         <is>
-          <t>[(-0.299999999994406, 488.0), (-0.299999999994406, 487.7), (-5.246, 488.0385856472514), (-5.246, 487.7385856472514), (-5.246, 488.0385856472514), (-5.246, 487.7985856472514), (-10.799999999983, 488.0819145362189), (-10.799999999983, 487.7419145362189), (-0.299999999994406, 487.7), (-0.299999999994406, 487.41), (-5.246, 487.7385856472514), (-5.246, 487.5585856472514), (-5.246, 487.7985856472514), (-5.246, 487.5585856472514), (-10.799999999983, 487.7419145362189), (-10.799999999983, 487.4019145362189)]</t>
+          <t>[(-0.299999999994406, 488.0), (-0.299999999994406, 487.7), (-5.246, 488.0385856472514), (-5.246, 487.7385856472514), (-5.246, 488.0385856472514), (-5.246, 487.7985856472514), (-8.79999999999288, 488.06631176741536), (-8.79999999999288, 487.7263117674154), (-0.299999999994406, 487.7), (-0.299999999994406, 487.41), (-5.246, 487.7385856472514), (-5.246, 487.5585856472514), (-5.246, 487.7985856472514), (-5.246, 487.5585856472514), (-8.79999999999288, 487.7263117674154), (-8.79999999999288, 487.38631176741535)]</t>
         </is>
       </c>
     </row>
@@ -5317,7 +5317,7 @@
       </c>
       <c r="B490" t="inlineStr">
         <is>
-          <t>[(-0.299999999994406, 489.0), (-0.299999999994406, 488.73), (-5.258, 488.9147292638641), (-5.258, 488.6447292638641), (-5.258, 488.9147292638641), (-5.258, 488.6747292638641), (-10.7999999999993, 488.8194145362189), (-10.7999999999993, 488.5794145362189), (-0.299999999994406, 488.73), (-0.299999999994406, 488.43), (-5.258, 488.6447292638641), (-5.258, 488.5247292638641), (-5.258, 488.6747292638641), (-5.258, 488.5247292638641), (-10.7999999999993, 488.5794145362189), (-10.7999999999993, 488.3494145362189)]</t>
+          <t>[(-0.299999999994406, 489.0), (-0.299999999994406, 488.73), (-5.258, 488.9147292638641), (-5.258, 488.6447292638641), (-5.258, 488.9147292638641), (-5.258, 488.6547292638641), (-8.79999999999288, 488.85381176741544), (-8.79999999999288, 488.59381176741545), (-0.299999999994406, 488.73), (-0.299999999994406, 488.43), (-5.258, 488.6447292638641), (-5.258, 488.5247292638641), (-5.258, 488.6547292638641), (-5.258, 488.5247292638641), (-8.79999999999288, 488.59381176741545), (-8.79999999999288, 488.34381176741545)]</t>
         </is>
       </c>
     </row>
@@ -5327,7 +5327,7 @@
       </c>
       <c r="B491" t="inlineStr">
         <is>
-          <t>[(-0.299999999994406, 490.0), (-0.299999999994406, 489.69), (-5.217, 489.8770749999999), (-5.217, 489.6870749999999), (-5.217, 489.8770749999999), (-5.217, 489.64707499999986), (-10.7999999999993, 489.7374999999999), (-10.7999999999993, 489.5074999999999), (-0.299999999994406, 489.69), (-0.299999999994406, 489.38), (-5.217, 489.6870749999999), (-5.217, 489.4970749999999), (-5.217, 489.64707499999986), (-5.217, 489.4970749999999), (-10.7999999999993, 489.5074999999999), (-10.7999999999993, 489.2874999999999)]</t>
+          <t>[(-0.299999999994406, 490.0), (-0.299999999994406, 489.69), (-5.217, 489.8770749999999), (-5.217, 489.6870749999999), (-5.217, 489.8770749999999), (-5.217, 489.6270749999999), (-8.79999999999288, 489.7875), (-8.79999999999288, 489.5375), (-0.299999999994406, 489.69), (-0.299999999994406, 489.38), (-5.217, 489.6870749999999), (-5.217, 489.4970749999999), (-5.217, 489.6270749999999), (-5.217, 489.4970749999999), (-8.79999999999288, 489.5375), (-8.79999999999288, 489.2975)]</t>
         </is>
       </c>
     </row>
@@ -5337,7 +5337,7 @@
       </c>
       <c r="B492" t="inlineStr">
         <is>
-          <t>[(-0.299999999992618, 491.0), (-0.299999999992618, 490.68), (-5.197, 490.8775749999998), (-5.197, 490.6775749999998), (-5.197, 490.8775749999998), (-5.197, 490.6275749999998), (-10.7999999999975, 490.7374999999999), (-10.7999999999975, 490.4874999999999), (-0.299999999992618, 490.68), (-0.299999999992618, 490.36), (-5.197, 490.6775749999998), (-5.197, 490.47757499999983), (-5.197, 490.6275749999998), (-5.197, 490.4875749999998), (-10.7999999999975, 490.4874999999999), (-10.7999999999975, 490.2474999999999)]</t>
+          <t>[(-0.299999999992618, 491.0), (-0.299999999992618, 490.68), (-5.197, 490.8775749999998), (-5.197, 490.6775749999998), (-5.197, 490.8775749999998), (-5.197, 490.6175749999998), (-8.79999999999109, 490.7875), (-8.79999999999109, 490.52750000000003), (-0.299999999992618, 490.68), (-0.299999999992618, 490.36), (-5.197, 490.6775749999998), (-5.197, 490.47757499999983), (-5.197, 490.6175749999998), (-5.197, 490.4875749999998), (-8.79999999999109, 490.52750000000003), (-8.79999999999109, 490.26750000000004)]</t>
         </is>
       </c>
     </row>
@@ -5347,7 +5347,7 @@
       </c>
       <c r="B493" t="inlineStr">
         <is>
-          <t>[(-0.299999999994406, 492.0), (-0.299999999994406, 491.68), (-5.221, 491.87697499999985), (-5.221, 491.67697499999986), (-5.221, 491.87697499999985), (-5.221, 491.61697499999985), (-10.7999999999975, 491.7374999999999), (-10.7999999999975, 491.4774999999999), (-0.299999999994406, 491.68), (-0.299999999994406, 491.36), (-5.221, 491.67697499999986), (-5.221, 491.47697499999987), (-5.221, 491.61697499999985), (-5.221, 491.47697499999987), (-10.7999999999975, 491.4774999999999), (-10.7999999999975, 491.2174999999999)]</t>
+          <t>[(-0.299999999994406, 492.0), (-0.299999999994406, 491.68), (-5.221, 491.87697499999985), (-5.221, 491.67697499999986), (-5.221, 491.87697499999985), (-5.221, 491.60697499999986), (-8.79999999999288, 491.7875), (-8.79999999999288, 491.51750000000004), (-0.299999999994406, 491.68), (-0.299999999994406, 491.36), (-5.221, 491.67697499999986), (-5.221, 491.47697499999987), (-5.221, 491.60697499999986), (-5.221, 491.47697499999987), (-8.79999999999288, 491.51750000000004), (-8.79999999999288, 491.2475)]</t>
         </is>
       </c>
     </row>
@@ -5357,7 +5357,7 @@
       </c>
       <c r="B494" t="inlineStr">
         <is>
-          <t>[(-0.299999999994406, 493.0), (-0.299999999994406, 492.68), (-5.159, 492.87852499999985), (-5.159, 492.67852499999987), (-5.159, 492.87852499999985), (-5.159, 492.61852499999986), (-10.7999999999993, 492.7374999999999), (-10.7999999999993, 492.4774999999999), (-0.299999999994406, 492.68), (-0.299999999994406, 492.36), (-5.159, 492.67852499999987), (-5.159, 492.4785249999999), (-5.159, 492.61852499999986), (-5.159, 492.48852499999987), (-10.7999999999993, 492.4774999999999), (-10.7999999999993, 492.2174999999999)]</t>
+          <t>[(-0.299999999994406, 493.0), (-0.299999999994406, 492.68), (-5.159, 492.87852499999985), (-5.159, 492.67852499999987), (-5.159, 492.87852499999985), (-5.159, 492.6085249999999), (-8.79999999999288, 492.7875), (-8.79999999999288, 492.51750000000004), (-0.299999999994406, 492.68), (-0.299999999994406, 492.36), (-5.159, 492.67852499999987), (-5.159, 492.4785249999999), (-5.159, 492.6085249999999), (-5.159, 492.48852499999987), (-8.79999999999288, 492.51750000000004), (-8.79999999999288, 492.25750000000005)]</t>
         </is>
       </c>
     </row>
@@ -5367,7 +5367,7 @@
       </c>
       <c r="B495" t="inlineStr">
         <is>
-          <t>[(-0.299999999994406, 494.0), (-0.299999999994406, 493.65), (-5.114, 493.87964999999986), (-5.114, 493.63964999999985), (-5.114, 493.87964999999986), (-5.114, 493.68964999999986), (-10.7999999999993, 493.7374999999999), (-10.7999999999993, 493.5474999999999), (-0.299999999994406, 493.65), (-0.299999999994406, 493.3), (-5.114, 493.63964999999985), (-5.114, 493.39964999999984), (-5.114, 493.68964999999986), (-5.114, 493.49964999999986), (-10.7999999999993, 493.5474999999999), (-10.7999999999993, 493.3574999999999)]</t>
+          <t>[(-0.299999999994406, 494.0), (-0.299999999994406, 493.65), (-5.114, 493.87964999999986), (-5.114, 493.63964999999985), (-5.114, 493.87964999999986), (-5.114, 493.57964999999984), (-8.79999999999288, 493.7875), (-8.79999999999288, 493.4875), (-0.299999999994406, 493.65), (-0.299999999994406, 493.3), (-5.114, 493.63964999999985), (-5.114, 493.39964999999984), (-5.114, 493.57964999999984), (-5.114, 493.38964999999985), (-8.79999999999288, 493.4875), (-8.79999999999288, 493.1875)]</t>
         </is>
       </c>
     </row>
@@ -5377,7 +5377,7 @@
       </c>
       <c r="B496" t="inlineStr">
         <is>
-          <t>[(-0.299999999992618, 495.0), (-0.299999999992618, 494.66), (-5.078, 494.8805499999998), (-5.078, 494.6205499999998), (-5.078, 494.8805499999998), (-5.078, 494.6205499999998), (-10.7999999999975, 494.7374999999999), (-10.7999999999975, 494.4174999999999), (-0.299999999992618, 494.66), (-0.299999999992618, 494.32), (-5.078, 494.6205499999998), (-5.078, 494.3605499999998), (-5.078, 494.6205499999998), (-5.078, 494.3605499999998), (-10.7999999999975, 494.4174999999999), (-10.7999999999975, 494.0974999999999)]</t>
+          <t>[(-0.299999999992618, 495.0), (-0.299999999992618, 494.66), (-5.078, 494.8805499999998), (-5.078, 494.6205499999998), (-5.078, 494.8805499999998), (-5.078, 494.6205499999998), (-8.79999999999109, 494.7875), (-8.79999999999109, 494.44750000000005), (-0.299999999992618, 494.66), (-0.299999999992618, 494.32), (-5.078, 494.6205499999998), (-5.078, 494.3605499999998), (-5.078, 494.6205499999998), (-5.078, 494.3605499999998), (-8.79999999999109, 494.44750000000005), (-8.79999999999109, 494.1075)]</t>
         </is>
       </c>
     </row>
@@ -5387,7 +5387,7 @@
       </c>
       <c r="B497" t="inlineStr">
         <is>
-          <t>[(-0.299999999992618, 496.0), (-0.299999999992618, 495.78), (-5.063, 495.8809249999998), (-5.063, 495.6609249999998), (-5.063, 495.8809249999998), (-5.063, 495.5909249999998), (-10.7999999999975, 495.7374999999999), (-10.7999999999975, 495.3574999999999), (-0.299999999992618, 495.78), (-0.299999999992618, 495.56), (-5.063, 495.6609249999998), (-5.063, 495.4409249999998), (-5.063, 495.5909249999998), (-5.063, 495.30092499999984), (-10.7999999999975, 495.3574999999999), (-10.7999999999975, 494.9774999999999), (-0.299999999992618, 495.56), (-0.299999999992618, 495.36), (-5.063, 495.4409249999998), (-5.063, 495.30092499999984), (-5.063, 495.30092499999984), (-5.063, 495.30092499999984), (-10.7999999999975, 494.9774999999999), (-10.7999999999975, 494.9774999999999)]</t>
+          <t>[(-0.299999999992618, 496.0), (-0.299999999992618, 495.78), (-5.063, 495.8809249999998), (-5.063, 495.6609249999998), (-5.063, 495.8809249999998), (-5.063, 495.5909249999998), (-8.79999999999109, 495.7875), (-8.79999999999109, 495.4075), (-0.299999999992618, 495.78), (-0.299999999992618, 495.56), (-5.063, 495.6609249999998), (-5.063, 495.4409249999998), (-5.063, 495.5909249999998), (-5.063, 495.30092499999984), (-8.79999999999109, 495.4075), (-8.79999999999109, 495.02750000000003), (-0.299999999992618, 495.56), (-0.299999999992618, 495.36), (-5.063, 495.4409249999998), (-5.063, 495.30092499999984), (-5.063, 495.30092499999984), (-5.063, 495.30092499999984), (-8.79999999999109, 495.02750000000003), (-8.79999999999109, 495.02750000000003)]</t>
         </is>
       </c>
     </row>
@@ -5397,7 +5397,7 @@
       </c>
       <c r="B498" t="inlineStr">
         <is>
-          <t>[(-0.300000000075493, 497.0), (-0.300000000075493, 496.79), (-5.088, 496.8522459061728), (-5.088, 496.64224590617283), (-5.088, 496.8522459061728), (-5.088, 496.5922459061728), (-10.7999999999958, 496.67597786441144), (-10.7999999999958, 496.28597786441145), (-0.300000000075493, 496.79), (-0.300000000075493, 496.58), (-5.088, 496.64224590617283), (-5.088, 496.4322459061728), (-5.088, 496.5922459061728), (-5.088, 496.33224590617283), (-10.7999999999958, 496.28597786441145), (-10.7999999999958, 495.89597786441146), (-0.300000000075493, 496.58), (-0.300000000075493, 496.38), (-5.088, 496.4322459061728), (-5.088, 496.32224590617284), (-5.088, 496.33224590617283), (-5.088, 496.33224590617283), (-10.7999999999958, 495.89597786441146), (-10.7999999999958, 495.89597786441146)]</t>
+          <t>[(-0.300000000075493, 497.0), (-0.300000000075493, 496.69), (-5.088, 496.8522459061728), (-5.088, 496.5922459061728), (-5.088, 496.8522459061728), (-5.088, 496.5922459061728), (-8.79999999998839, 496.737696366429), (-8.79999999998839, 496.377696366429), (-0.300000000075493, 496.69), (-0.300000000075493, 496.38), (-5.088, 496.5922459061728), (-5.088, 496.33224590617283), (-5.088, 496.5922459061728), (-5.088, 496.33224590617283), (-8.79999999998839, 496.377696366429), (-8.79999999998839, 496.017696366429)]</t>
         </is>
       </c>
     </row>
@@ -5407,7 +5407,7 @@
       </c>
       <c r="B499" t="inlineStr">
         <is>
-          <t>[(-0.300000000029171, 498.0), (-0.300000000029171, 497.79), (-5.187, 497.80034608329225), (-5.187, 497.5903460832923), (-5.187, 497.80034608329225), (-5.187, 497.5203460832923), (-10.7999999999952, 497.5710321003812), (-10.7999999999952, 497.18103210038123), (-0.300000000029171, 497.79), (-0.300000000029171, 497.58), (-5.187, 497.5903460832923), (-5.187, 497.38034608329224), (-5.187, 497.5203460832923), (-5.187, 497.24034608329225), (-10.7999999999952, 497.18103210038123), (-10.7999999999952, 496.79103210038124), (-0.300000000029171, 497.58), (-0.300000000029171, 497.37), (-5.187, 497.38034608329224), (-5.187, 497.23034608329226), (-5.187, 497.24034608329225), (-5.187, 497.24034608329225), (-10.7999999999952, 496.79103210038124), (-10.7999999999952, 496.79103210038124)]</t>
+          <t>[(-0.300000000029171, 498.0), (-0.300000000029171, 497.79), (-5.187, 497.80034608329225), (-5.187, 497.5903460832923), (-5.187, 497.80034608329225), (-5.187, 497.5203460832923), (-8.79999999999721, 497.6527402717374), (-8.79999999999721, 497.2827402717374), (-0.300000000029171, 497.79), (-0.300000000029171, 497.58), (-5.187, 497.5903460832923), (-5.187, 497.38034608329224), (-5.187, 497.5203460832923), (-5.187, 497.24034608329225), (-8.79999999999721, 497.2827402717374), (-8.79999999999721, 496.9127402717374), (-0.300000000029171, 497.58), (-0.300000000029171, 497.37), (-5.187, 497.38034608329224), (-5.187, 497.23034608329226), (-5.187, 497.24034608329225), (-5.187, 497.24034608329225), (-8.79999999999721, 496.9127402717374), (-8.79999999999721, 496.9127402717374)]</t>
         </is>
       </c>
     </row>
@@ -5417,7 +5417,7 @@
       </c>
       <c r="B500" t="inlineStr">
         <is>
-          <t>[(-0.299999999990458, 499.0), (-0.299999999990458, 498.64), (-5.357, 498.7428570098019), (-5.357, 498.4528570098019), (-5.357, 498.7428570098019), (-5.357, 498.4528570098019), (-10.7999999999927, 498.4660863363506), (-10.7999999999927, 498.0960863363506), (-0.299999999990458, 498.64), (-0.299999999990458, 498.28), (-5.357, 498.4528570098019), (-5.357, 498.16285700980194), (-5.357, 498.4528570098019), (-5.357, 498.16285700980194), (-10.7999999999927, 498.0960863363506), (-10.7999999999927, 497.7260863363506)]</t>
+          <t>[(-0.299999999990458, 499.0), (-0.299999999990458, 498.64), (-5.357, 498.7428570098019), (-5.357, 498.4528570098019), (-5.357, 498.7428570098019), (-5.357, 498.4528570098019), (-8.79999999998244, 498.56778417704624), (-8.79999999998244, 498.2077841770462), (-0.299999999990458, 498.64), (-0.299999999990458, 498.28), (-5.357, 498.4528570098019), (-5.357, 498.16285700980194), (-5.357, 498.4528570098019), (-5.357, 498.16285700980194), (-8.79999999998244, 498.2077841770462), (-8.79999999998244, 497.8477841770462)]</t>
         </is>
       </c>
     </row>
@@ -5427,7 +5427,7 @@
       </c>
       <c r="B501" t="inlineStr">
         <is>
-          <t>[(-0.299999999991877, 500.0), (-0.299999999991877, 499.63), (-5.533, 499.68160462999555), (-5.533, 499.4016046299956), (-5.533, 499.68160462999555), (-5.533, 499.45160462999553), (-10.7999999999893, 499.3611405723217), (-10.7999999999893, 499.13114057232167), (-0.299999999991877, 499.63), (-0.299999999991877, 499.26), (-5.533, 499.4016046299956), (-5.533, 499.12160462999555), (-5.533, 499.45160462999553), (-5.533, 499.22160462999557), (-10.7999999999893, 499.13114057232167), (-10.7999999999893, 498.9011405723217)]</t>
+          <t>[(-0.299999999991877, 500.0), (-0.299999999991877, 499.63), (-5.533, 499.68160462999555), (-5.533, 499.4016046299956), (-5.533, 499.68160462999555), (-5.533, 499.4016046299956), (-8.79999999999738, 499.4828280823552), (-8.79999999999738, 499.1428280823552), (-0.299999999991877, 499.63), (-0.299999999991877, 499.26), (-5.533, 499.4016046299956), (-5.533, 499.12160462999555), (-5.533, 499.4016046299956), (-5.533, 499.12160462999555), (-8.79999999999738, 499.1428280823552), (-8.79999999999738, 498.8028280823552)]</t>
         </is>
       </c>
     </row>
@@ -5437,7 +5437,7 @@
       </c>
       <c r="B502" t="inlineStr">
         <is>
-          <t>[(-0.299999999993062, 501.0), (-0.299999999993062, 500.62), (-5.774, 500.6168199999995), (-5.774, 500.3568199999995), (-5.774, 500.6168199999995), (-5.774, 500.3568199999995), (-10.799999999996, 500.2649999999998), (-10.799999999996, 499.92499999999984), (-0.299999999993062, 500.62), (-0.299999999993062, 500.24), (-5.774, 500.3568199999995), (-5.774, 500.0968199999995), (-5.774, 500.3568199999995), (-5.774, 500.0968199999995), (-10.799999999996, 499.92499999999984), (-10.799999999996, 499.5849999999998)]</t>
+          <t>[(-0.299999999993062, 501.0), (-0.299999999993062, 500.62), (-5.774, 500.6168199999995), (-5.774, 500.3568199999995), (-5.774, 500.6168199999995), (-5.774, 500.3568199999995), (-8.79999999999353, 500.405), (-8.79999999999353, 500.085), (-0.299999999993062, 500.62), (-0.299999999993062, 500.24), (-5.774, 500.3568199999995), (-5.774, 500.0968199999995), (-5.774, 500.3568199999995), (-5.774, 500.0968199999995), (-8.79999999999353, 500.085), (-8.79999999999353, 499.765)]</t>
         </is>
       </c>
     </row>
@@ -5447,7 +5447,7 @@
       </c>
       <c r="B503" t="inlineStr">
         <is>
-          <t>[(-0.299999999985769, 502.0), (-0.299999999985769, 501.66), (-5.857, 501.611009999999), (-5.857, 501.39100999999897), (-5.857, 501.611009999999), (-5.857, 501.321009999999), (-10.7999999999779, 501.26500000000055), (-10.7999999999779, 500.97500000000053), (-0.299999999985769, 501.66), (-0.299999999985769, 501.32), (-5.857, 501.39100999999897), (-5.857, 501.171009999999), (-5.857, 501.321009999999), (-5.857, 501.161009999999), (-10.7999999999779, 500.97500000000053), (-10.7999999999779, 500.69500000000056)]</t>
+          <t>[(-0.299999999985769, 502.0), (-0.299999999985769, 501.66), (-5.857, 501.611009999999), (-5.857, 501.39100999999897), (-5.857, 501.611009999999), (-5.857, 501.331009999999), (-8.79999999998793, 501.40499999999986), (-8.79999999998793, 501.1249999999999), (-0.299999999985769, 501.66), (-0.299999999985769, 501.32), (-5.857, 501.39100999999897), (-5.857, 501.171009999999), (-5.857, 501.331009999999), (-5.857, 501.161009999999), (-8.79999999998793, 501.1249999999999), (-8.79999999998793, 500.85499999999985)]</t>
         </is>
       </c>
     </row>
@@ -5457,7 +5457,7 @@
       </c>
       <c r="B504" t="inlineStr">
         <is>
-          <t>[(-0.299999999982385, 503.0), (-0.299999999982385, 502.66), (-5.904, 502.6077199999988), (-5.904, 502.3577199999988), (-5.904, 502.6077199999988), (-5.904, 502.3577199999988), (-10.7999999999891, 502.26499999999953), (-10.7999999999891, 501.95499999999953), (-0.299999999982385, 502.66), (-0.299999999982385, 502.32), (-5.904, 502.3577199999988), (-5.904, 502.1077199999988), (-5.904, 502.3577199999988), (-5.904, 502.1077199999988), (-10.7999999999891, 501.95499999999953), (-10.7999999999891, 501.6449999999995)]</t>
+          <t>[(-0.299999999982385, 503.0), (-0.299999999982385, 502.66), (-5.904, 502.6077199999988), (-5.904, 502.3577199999988), (-5.904, 502.6077199999988), (-5.904, 502.30771999999877), (-8.79999999998564, 502.40499999999975), (-8.79999999998564, 502.10499999999973), (-0.299999999982385, 502.66), (-0.299999999982385, 502.32), (-5.904, 502.3577199999988), (-5.904, 502.1077199999988), (-5.904, 502.30771999999877), (-5.904, 502.1077199999988), (-8.79999999998564, 502.10499999999973), (-8.79999999998564, 501.8049999999997)]</t>
         </is>
       </c>
     </row>
@@ -5467,7 +5467,7 @@
       </c>
       <c r="B505" t="inlineStr">
         <is>
-          <t>[(-0.299999999992593, 504.0), (-0.299999999992593, 503.6), (-5.981, 503.6023299999995), (-5.981, 503.3223299999995), (-5.981, 503.6023299999995), (-5.981, 503.3223299999995), (-10.8000000000002, 503.2649999999995), (-10.8000000000002, 502.8849999999995), (-0.299999999992593, 503.6), (-0.299999999992593, 503.2), (-5.981, 503.3223299999995), (-5.981, 503.0423299999995), (-5.981, 503.3223299999995), (-5.981, 503.0423299999995), (-10.8000000000002, 502.8849999999995), (-10.8000000000002, 502.5049999999995)]</t>
+          <t>[(-0.299999999992593, 504.0), (-0.299999999992593, 503.6), (-5.981, 503.6023299999995), (-5.981, 503.3223299999995), (-5.981, 503.6023299999995), (-5.981, 503.3223299999995), (-8.80000000000243, 503.4049999999993), (-8.80000000000243, 503.05499999999927), (-0.299999999992593, 503.6), (-0.299999999992593, 503.2), (-5.981, 503.3223299999995), (-5.981, 503.0423299999995), (-5.981, 503.3223299999995), (-5.981, 503.0423299999995), (-8.80000000000243, 503.05499999999927), (-8.80000000000243, 502.7049999999993)]</t>
         </is>
       </c>
     </row>
@@ -5477,7 +5477,7 @@
       </c>
       <c r="B506" t="inlineStr">
         <is>
-          <t>[(-0.300000000005262, 505.0), (-0.300000000005262, 504.6), (-5.857, 504.61101000000036), (-5.857, 504.30101000000036), (-5.857, 504.61101000000036), (-5.857, 504.36101000000036), (-10.7999999999928, 504.2650000000009), (-10.7999999999928, 504.0150000000009), (-0.300000000005262, 504.6), (-0.300000000005262, 504.2), (-5.857, 504.30101000000036), (-5.857, 503.99101000000036), (-5.857, 504.36101000000036), (-5.857, 504.11101000000036), (-10.7999999999928, 504.0150000000009), (-10.7999999999928, 503.7650000000009)]</t>
+          <t>[(-0.300000000005262, 505.0), (-0.300000000005262, 504.6), (-5.857, 504.61101000000036), (-5.857, 504.30101000000036), (-5.857, 504.61101000000036), (-5.857, 504.36101000000036), (-8.79999999999439, 504.40500000000077), (-8.79999999999439, 504.15500000000077), (-0.300000000005262, 504.6), (-0.300000000005262, 504.2), (-5.857, 504.30101000000036), (-5.857, 503.99101000000036), (-5.857, 504.36101000000036), (-5.857, 504.11101000000036), (-8.79999999999439, 504.15500000000077), (-8.79999999999439, 503.90500000000077)]</t>
         </is>
       </c>
     </row>
@@ -5487,7 +5487,7 @@
       </c>
       <c r="B507" t="inlineStr">
         <is>
-          <t>[(-0.300000000002308, 506.0), (-0.300000000002308, 505.62), (-5.566, 505.63138000000015), (-5.566, 505.37138000000016), (-5.566, 505.63138000000015), (-5.566, 505.37138000000016), (-10.7999999999977, 505.2650000000003), (-10.7999999999977, 504.94500000000033), (-0.300000000002308, 505.62), (-0.300000000002308, 505.24), (-5.566, 505.37138000000016), (-5.566, 505.11138000000017), (-5.566, 505.37138000000016), (-5.566, 505.11138000000017), (-10.7999999999977, 504.94500000000033), (-10.7999999999977, 504.62500000000034)]</t>
+          <t>[(-0.300000000002308, 506.0), (-0.300000000002308, 505.62), (-5.566, 505.63138000000015), (-5.566, 505.37138000000016), (-5.566, 505.63138000000015), (-5.566, 505.37138000000016), (-8.80000000000209, 505.40500000000003), (-8.80000000000209, 505.08500000000004), (-0.300000000002308, 505.62), (-0.300000000002308, 505.24), (-5.566, 505.37138000000016), (-5.566, 505.11138000000017), (-5.566, 505.37138000000016), (-5.566, 505.11138000000017), (-8.80000000000209, 505.08500000000004), (-8.80000000000209, 504.76500000000004)]</t>
         </is>
       </c>
     </row>
@@ -5497,7 +5497,7 @@
       </c>
       <c r="B508" t="inlineStr">
         <is>
-          <t>[(-0.300000000084319, 507.0), (-0.300000000084319, 506.71), (-5.221, 506.65559939136926), (-5.221, 506.36559939136924), (-5.221, 506.65559939136926), (-5.221, 506.41559939136926), (-10.8000000000065, 506.26514806123595), (-10.8000000000065, 506.02514806123594), (-0.300000000084319, 506.71), (-0.300000000084319, 506.42), (-5.221, 506.36559939136924), (-5.221, 506.2555993913693), (-5.221, 506.41559939136926), (-5.221, 506.2555993913693), (-10.8000000000065, 506.02514806123594), (-10.8000000000065, 505.78514806123593)]</t>
+          <t>[(-0.300000000084319, 507.0), (-0.300000000084319, 506.72), (-5.221, 506.65559939136926), (-5.221, 506.3755993913693), (-5.221, 506.65559939136926), (-5.221, 506.41559939136926), (-8.80000000000457, 506.40511985909694), (-8.80000000000457, 506.16511985909693), (-0.300000000084319, 506.72), (-0.300000000084319, 506.42), (-5.221, 506.3755993913693), (-5.221, 506.2555993913693), (-5.221, 506.41559939136926), (-5.221, 506.2555993913693), (-8.80000000000457, 506.16511985909693), (-8.80000000000457, 505.9251198590969)]</t>
         </is>
       </c>
     </row>
@@ -5507,7 +5507,7 @@
       </c>
       <c r="B509" t="inlineStr">
         <is>
-          <t>[(-0.300000000036697, 508.0), (-0.300000000036697, 507.74), (-4.862, 507.7263207648436), (-4.862, 507.4663207648436), (-4.862, 507.7263207648436), (-4.862, 507.4963207648436), (-10.8000000000254, 507.3700938252603), (-10.8000000000254, 507.1400938252603), (-0.300000000036697, 507.74), (-0.300000000036697, 507.48), (-4.862, 507.4663207648436), (-4.862, 507.3263207648436), (-4.862, 507.4963207648436), (-4.862, 507.3263207648436), (-10.8000000000254, 507.1400938252603), (-10.8000000000254, 506.91009382526033)]</t>
+          <t>[(-0.300000000036697, 508.0), (-0.300000000036697, 507.74), (-4.862, 507.7263207648436), (-4.862, 507.4663207648436), (-4.862, 507.7263207648436), (-4.862, 507.4863207648436), (-8.80000000001613, 507.4900759537828), (-8.80000000001613, 507.2500759537828), (-0.300000000036697, 507.74), (-0.300000000036697, 507.48), (-4.862, 507.4663207648436), (-4.862, 507.3263207648436), (-4.862, 507.4863207648436), (-4.862, 507.3263207648436), (-8.80000000001613, 507.2500759537828), (-8.80000000001613, 507.0100759537828)]</t>
         </is>
       </c>
     </row>
@@ -5517,7 +5517,7 @@
       </c>
       <c r="B510" t="inlineStr">
         <is>
-          <t>[(-0.299999999991776, 509.0), (-0.299999999991776, 508.81), (-4.666, 508.7817164616029), (-4.666, 508.5917164616029), (-4.666, 508.7817164616029), (-4.666, 508.5417164616029), (-10.8000000000003, 508.4750395892884), (-10.8000000000003, 508.23503958928836), (-0.299999999991776, 508.81), (-0.299999999991776, 508.51), (-4.666, 508.5917164616029), (-4.666, 508.4317164616029), (-4.666, 508.5417164616029), (-4.666, 508.4317164616029), (-10.8000000000003, 508.23503958928836), (-10.8000000000003, 508.00503958928834)]</t>
+          <t>[(-0.299999999991776, 509.0), (-0.299999999991776, 508.81), (-4.666, 508.7817164616029), (-4.666, 508.5917164616029), (-4.666, 508.7817164616029), (-4.666, 508.6017164616029), (-8.80000000000376, 508.5750320484713), (-8.80000000000376, 508.3950320484713), (-0.299999999991776, 508.81), (-0.299999999991776, 508.51), (-4.666, 508.5917164616029), (-4.666, 508.4317164616029), (-4.666, 508.6017164616029), (-4.666, 508.4317164616029), (-8.80000000000376, 508.3950320484713), (-8.80000000000376, 508.0950320484713)]</t>
         </is>
       </c>
     </row>
@@ -5527,7 +5527,7 @@
       </c>
       <c r="B511" t="inlineStr">
         <is>
-          <t>[(-0.300000000034003, 510.0), (-0.300000000034003, 509.79), (-4.571, 509.8291540422891), (-4.571, 509.6191540422891), (-4.571, 509.8291540422891), (-4.571, 509.66915404228905), (-10.8000000000176, 509.5799853533186), (-10.8000000000176, 509.41998535331857), (-0.300000000034003, 509.79), (-0.300000000034003, 509.58), (-4.571, 509.6191540422891), (-4.571, 509.5091540422891), (-4.571, 509.66915404228905), (-4.571, 509.5091540422891), (-10.8000000000176, 509.41998535331857), (-10.8000000000176, 509.1199853533186)]</t>
+          <t>[(-0.300000000034003, 510.0), (-0.300000000034003, 509.88), (-4.571, 509.8291540422891), (-4.571, 509.7091540422891), (-4.571, 509.8291540422891), (-4.571, 509.66915404228905), (-8.8000000000224, 509.6599881431626), (-8.8000000000224, 509.49998814316257), (-0.300000000034003, 509.88), (-0.300000000034003, 509.58), (-4.571, 509.7091540422891), (-4.571, 509.5091540422891), (-4.571, 509.66915404228905), (-4.571, 509.5091540422891), (-8.8000000000224, 509.49998814316257), (-8.8000000000224, 509.1999881431626)]</t>
         </is>
       </c>
     </row>
@@ -5537,7 +5537,7 @@
       </c>
       <c r="B512" t="inlineStr">
         <is>
-          <t>[(-0.300000000101255, 511.0), (-0.300000000101255, 510.89), (-4.512, 510.87361236821886), (-4.512, 510.76361236821884), (-4.512, 510.87361236821886), (-4.512, 510.7236123682189), (-10.8000000000086, 510.6849311173499), (-10.8000000000086, 510.5349311173499), (-0.300000000101255, 510.89), (-0.300000000101255, 510.65), (-4.512, 510.76361236821884), (-4.512, 510.61361236821887), (-4.512, 510.7236123682189), (-4.512, 510.61361236821887), (-10.8000000000086, 510.5349311173499), (-10.8000000000086, 510.2349311173499)]</t>
+          <t>[(-0.300000000101255, 511.0), (-0.300000000101255, 510.88), (-4.512, 510.87361236821886), (-4.512, 510.75361236821885), (-4.512, 510.87361236821886), (-4.512, 510.73361236821887), (-8.80000000000119, 510.7449442378554), (-8.80000000000119, 510.6049442378554), (-0.300000000101255, 510.88), (-0.300000000101255, 510.65), (-4.512, 510.75361236821885), (-4.512, 510.61361236821887), (-4.512, 510.73361236821887), (-4.512, 510.61361236821887), (-8.80000000000119, 510.6049442378554), (-8.80000000000119, 510.3049442378554)]</t>
         </is>
       </c>
     </row>
@@ -5547,7 +5547,7 @@
       </c>
       <c r="B513" t="inlineStr">
         <is>
-          <t>[(-0.300000000005213, 512.0), (-0.300000000005213, 511.8), (-4.393, 511.927093547934), (-4.393, 511.72709354793403), (-4.393, 511.927093547934), (-4.393, 511.767093547934), (-10.7999999999928, 511.8129690333025), (-10.7999999999928, 511.47296903330255), (-0.300000000005213, 511.8), (-0.300000000005213, 511.6), (-4.393, 511.72709354793403), (-4.393, 511.617093547934), (-4.393, 511.767093547934), (-4.393, 511.607093547934), (-10.7999999999928, 511.47296903330255), (-10.7999999999928, 511.1329690333025)]</t>
+          <t>[(-0.300000000005213, 512.0), (-0.300000000005213, 511.88), (-4.393, 511.927093547934), (-4.393, 511.807093547934), (-4.393, 511.927093547934), (-4.393, 511.767093547934), (-8.79999999999452, 511.84859397934014), (-8.79999999999452, 511.5485939793401), (-0.300000000005213, 511.88), (-0.300000000005213, 511.6), (-4.393, 511.807093547934), (-4.393, 511.617093547934), (-4.393, 511.767093547934), (-4.393, 511.607093547934), (-8.79999999999452, 511.5485939793401), (-8.79999999999452, 511.2485939793401)]</t>
         </is>
       </c>
     </row>
@@ -5557,7 +5557,7 @@
       </c>
       <c r="B514" t="inlineStr">
         <is>
-          <t>[(-0.300000000005213, 513.0), (-0.300000000005213, 512.75), (-4.237, 512.9865706123701), (-4.237, 512.7365706123701), (-4.237, 512.9865706123701), (-4.237, 512.7665706123701), (-10.7999999999932, 512.9641837515585), (-10.7999999999932, 512.5441837515585), (-0.300000000005213, 512.75), (-0.300000000005213, 512.5), (-4.237, 512.7365706123701), (-4.237, 512.54657061237), (-4.237, 512.7665706123701), (-4.237, 512.54657061237), (-10.7999999999932, 512.5441837515585), (-10.7999999999932, 512.1241837515585)]</t>
+          <t>[(-0.300000000005213, 513.0), (-0.300000000005213, 512.75), (-4.237, 512.9865706123701), (-4.237, 512.7365706123701), (-4.237, 512.9865706123701), (-4.237, 512.7665706123701), (-8.79999999999452, 512.9710058941188), (-8.79999999999452, 512.5910058941188), (-0.300000000005213, 512.75), (-0.300000000005213, 512.5), (-4.237, 512.7365706123701), (-4.237, 512.54657061237), (-4.237, 512.7665706123701), (-4.237, 512.54657061237), (-8.79999999999452, 512.5910058941188), (-8.79999999999452, 512.2110058941188)]</t>
         </is>
       </c>
     </row>
@@ -5567,7 +5567,7 @@
       </c>
       <c r="B515" t="inlineStr">
         <is>
-          <t>[(-0.300000000005213, 514.0), (-0.300000000005213, 513.72), (-4.16, 514.0424226755699), (-4.16, 513.76242267557), (-4.16, 514.0424226755699), (-4.16, 513.8024226755699), (-10.7999999999932, 514.1153984698144), (-10.7999999999932, 513.6953984698144), (-0.300000000005213, 513.72), (-0.300000000005213, 513.45), (-4.16, 513.76242267557), (-4.16, 513.5624226755699), (-4.16, 513.8024226755699), (-4.16, 513.5624226755699), (-10.7999999999932, 513.6953984698144), (-10.7999999999932, 513.2753984698144)]</t>
+          <t>[(-0.300000000005213, 514.0), (-0.300000000005213, 513.72), (-4.16, 514.0424226755699), (-4.16, 513.76242267557), (-4.16, 514.0424226755699), (-4.16, 513.8024226755699), (-8.79999999999452, 514.0934178088974), (-8.79999999999452, 513.6934178088974), (-0.300000000005213, 513.72), (-0.300000000005213, 513.45), (-4.16, 513.76242267557), (-4.16, 513.5624226755699), (-4.16, 513.8024226755699), (-4.16, 513.5624226755699), (-8.79999999999452, 513.6934178088974), (-8.79999999999452, 513.2934178088974)]</t>
         </is>
       </c>
     </row>
@@ -5577,7 +5577,7 @@
       </c>
       <c r="B516" t="inlineStr">
         <is>
-          <t>[(-0.300000000004548, 515.0), (-0.300000000004548, 514.85), (-4.027, 515.0942611932986), (-4.027, 514.9442611932986), (-4.027, 515.0942611932986), (-4.027, 514.8742611932986), (-10.8000000000125, 515.2655601099108), (-10.8000000000125, 514.8855601099108), (-0.300000000004548, 514.85), (-0.300000000004548, 514.7), (-4.027, 514.9442611932986), (-4.027, 514.7942611932987), (-4.027, 514.8742611932986), (-4.027, 514.6542611932986), (-10.8000000000125, 514.8855601099108), (-10.8000000000125, 514.5055601099108), (-0.300000000004548, 514.7), (-0.300000000004548, 514.57), (-4.027, 514.7942611932987), (-4.027, 514.6542611932986), (-4.027, 514.6542611932986), (-4.027, 514.6542611932986), (-10.8000000000125, 514.5055601099108), (-10.8000000000125, 514.5055601099108)]</t>
+          <t>[(-0.300000000004548, 515.0), (-0.300000000004548, 514.85), (-4.027, 515.0942611932986), (-4.027, 514.9442611932986), (-4.027, 515.0942611932986), (-4.027, 514.8742611932986), (-8.80000000001436, 515.2149772318326), (-8.80000000001436, 514.8549772318325), (-0.300000000004548, 514.85), (-0.300000000004548, 514.7), (-4.027, 514.9442611932986), (-4.027, 514.7942611932987), (-4.027, 514.8742611932986), (-4.027, 514.6542611932986), (-8.80000000001436, 514.8549772318325), (-8.80000000001436, 514.4949772318325), (-0.300000000004548, 514.7), (-0.300000000004548, 514.57), (-4.027, 514.7942611932987), (-4.027, 514.6542611932986), (-4.027, 514.6542611932986), (-4.027, 514.6542611932986), (-8.80000000001436, 514.4949772318325), (-8.80000000001436, 514.4949772318325)]</t>
         </is>
       </c>
     </row>
@@ -5587,7 +5587,7 @@
       </c>
       <c r="B517" t="inlineStr">
         <is>
-          <t>[(-0.300000000028711, 516.0), (-0.300000000028711, 515.85), (-3.916, 516.1301967007072), (-3.916, 515.9801967007072), (-3.916, 516.1301967007072), (-3.916, 515.9301967007071), (-10.782, 516.377412006864), (-10.782, 516.017412006864), (-0.300000000028711, 515.85), (-0.300000000028711, 515.7), (-3.916, 515.9801967007072), (-3.916, 515.8301967007072), (-3.916, 515.9301967007071), (-3.916, 515.7301967007072), (-10.782, 516.017412006864), (-10.782, 515.657412006864), (-0.300000000028711, 515.7), (-0.300000000028711, 515.58), (-3.916, 515.8301967007072), (-3.916, 515.7201967007072), (-3.916, 515.7301967007072), (-3.916, 515.7301967007072), (-10.782, 515.657412006864), (-10.782, 515.657412006864)]</t>
+          <t>[(-0.300000000028711, 516.0), (-0.300000000028711, 515.79), (-3.916, 516.1301967007072), (-3.916, 515.9201967007072), (-3.916, 516.1301967007072), (-3.916, 515.9301967007071), (-8.80000000001792, 516.3060486604033), (-8.80000000001792, 515.9660486604033), (-0.300000000028711, 515.79), (-0.300000000028711, 515.58), (-3.916, 515.9201967007072), (-3.916, 515.7201967007072), (-3.916, 515.9301967007071), (-3.916, 515.7301967007072), (-8.80000000001792, 515.9660486604033), (-8.80000000001792, 515.6260486604034)]</t>
         </is>
       </c>
     </row>
@@ -5597,7 +5597,7 @@
       </c>
       <c r="B518" t="inlineStr">
         <is>
-          <t>[(-0.300000000119848, 517.0), (-0.300000000119848, 516.79), (-4.131, 517.178984360096), (-4.131, 516.968984360096), (-4.131, 517.178984360096), (-4.131, 516.988984360096), (-10.8000000000056, 517.4905601099052), (-10.8000000000056, 517.1405601099052), (-0.300000000119848, 516.79), (-0.300000000119848, 516.58), (-4.131, 516.968984360096), (-4.131, 516.798984360096), (-4.131, 516.988984360096), (-4.131, 516.798984360096), (-10.8000000000056, 517.1405601099052), (-10.8000000000056, 516.7905601099052)]</t>
+          <t>[(-0.300000000119848, 517.0), (-0.300000000119848, 516.79), (-4.131, 517.178984360096), (-4.131, 516.968984360096), (-4.131, 517.178984360096), (-4.131, 516.988984360096), (-8.80000000000311, 517.3971200889698), (-8.80000000000311, 517.0671200889698), (-0.300000000119848, 516.79), (-0.300000000119848, 516.58), (-4.131, 516.968984360096), (-4.131, 516.798984360096), (-4.131, 516.988984360096), (-4.131, 516.798984360096), (-8.80000000000311, 517.0671200889698), (-8.80000000000311, 516.7371200889698)]</t>
         </is>
       </c>
     </row>
@@ -5607,7 +5607,7 @@
       </c>
       <c r="B519" t="inlineStr">
         <is>
-          <t>[(-0.300000000010955, 518.0), (-0.300000000010955, 517.76), (-4.733, 518.254606234974), (-4.733, 518.0146062349739), (-4.733, 518.254606234974), (-4.733, 518.0146062349739), (-10.8000000000107, 518.6030601099105), (-10.8000000000107, 518.2030601099106), (-0.300000000010955, 517.76), (-0.300000000010955, 517.58), (-4.733, 518.0146062349739), (-4.733, 517.7846062349739), (-4.733, 518.0146062349739), (-4.733, 517.7746062349739), (-10.8000000000107, 518.2030601099106), (-10.8000000000107, 517.8030601099106)]</t>
+          <t>[(-0.300000000010955, 518.0), (-0.300000000010955, 517.76), (-4.733, 518.254606234974), (-4.733, 518.0146062349739), (-4.733, 518.254606234974), (-4.733, 518.0146062349739), (-8.80000000001207, 518.4881915175467), (-8.80000000001207, 518.1081915175467), (-0.300000000010955, 517.76), (-0.300000000010955, 517.58), (-4.733, 518.0146062349739), (-4.733, 517.7846062349739), (-4.733, 518.0146062349739), (-4.733, 517.7746062349739), (-8.80000000001207, 518.1081915175467), (-8.80000000001207, 517.7281915175467)]</t>
         </is>
       </c>
     </row>
@@ -5617,7 +5617,7 @@
       </c>
       <c r="B520" t="inlineStr">
         <is>
-          <t>[(-0.300000000071549, 519.0), (-0.300000000071549, 518.74), (-5.234, 519.3362451030712), (-5.234, 519.0762451030712), (-5.234, 519.3362451030712), (-5.234, 519.0762451030712), (-10.7999999999972, 519.7155601099055), (-10.7999999999972, 519.3155601099055), (-0.300000000071549, 518.74), (-0.300000000071549, 518.59), (-5.234, 519.0762451030712), (-5.234, 518.8262451030712), (-5.234, 519.0762451030712), (-5.234, 518.8162451030712), (-10.7999999999972, 519.3155601099055), (-10.7999999999972, 518.9155601099055)]</t>
+          <t>[(-0.300000000071549, 519.0), (-0.300000000071549, 518.74), (-5.234, 519.3362451030712), (-5.234, 519.0762451030712), (-5.234, 519.3362451030712), (-5.234, 519.0762451030712), (-8.79999999999608, 519.579262946113), (-8.79999999999608, 519.179262946113), (-0.300000000071549, 518.74), (-0.300000000071549, 518.59), (-5.234, 519.0762451030712), (-5.234, 518.8262451030712), (-5.234, 519.0762451030712), (-5.234, 518.8162451030712), (-8.79999999999608, 519.179262946113), (-8.79999999999608, 518.779262946113)]</t>
         </is>
       </c>
     </row>
@@ -5627,7 +5627,7 @@
       </c>
       <c r="B521" t="inlineStr">
         <is>
-          <t>[(-0.299999999998654, 520.0), (-0.299999999998654, 519.73), (-5.555, 520.3678500000001), (-5.555, 520.0978500000001), (-5.555, 520.3678500000001), (-5.555, 520.0978500000001), (-10.7999999999963, 520.7349999999998), (-10.7999999999963, 520.3549999999998), (-0.299999999998654, 519.73), (-0.299999999998654, 519.55), (-5.555, 520.0978500000001), (-5.555, 519.8278500000001), (-5.555, 520.0978500000001), (-5.555, 519.8278500000001), (-10.7999999999963, 520.3549999999998), (-10.7999999999963, 519.9749999999998)]</t>
+          <t>[(-0.299999999998654, 520.0), (-0.299999999998654, 519.73), (-5.555, 520.3678500000001), (-5.555, 520.0978500000001), (-5.555, 520.3678500000001), (-5.555, 520.0978500000001), (-8.79999999999749, 520.5949999999999), (-8.79999999999749, 520.1949999999999), (-0.299999999998654, 519.73), (-0.299999999998654, 519.55), (-5.555, 520.0978500000001), (-5.555, 519.8278500000001), (-5.555, 520.0978500000001), (-5.555, 519.8278500000001), (-8.79999999999749, 520.1949999999999), (-8.79999999999749, 519.795)]</t>
         </is>
       </c>
     </row>
@@ -5637,7 +5637,7 @@
       </c>
       <c r="B522" t="inlineStr">
         <is>
-          <t>[(-0.299999999994848, 521.0), (-0.299999999994848, 520.75), (-5.537, 521.3665900000003), (-5.537, 521.1165900000003), (-5.537, 521.3665900000003), (-5.537, 521.1165900000003), (-10.800000000003, 521.7350000000006), (-10.800000000003, 521.3650000000006), (-0.299999999994848, 520.75), (-0.299999999994848, 520.6), (-5.537, 521.1165900000003), (-5.537, 520.8665900000003), (-5.537, 521.1165900000003), (-5.537, 520.8665900000003), (-10.800000000003, 521.3650000000006), (-10.800000000003, 520.9950000000006)]</t>
+          <t>[(-0.299999999994848, 521.0), (-0.299999999994848, 520.75), (-5.537, 521.3665900000003), (-5.537, 521.1165900000003), (-5.537, 521.3665900000003), (-5.537, 521.1165900000003), (-8.79999999999258, 521.5949999999998), (-8.79999999999258, 521.2149999999998), (-0.299999999994848, 520.75), (-0.299999999994848, 520.6), (-5.537, 521.1165900000003), (-5.537, 520.8665900000003), (-5.537, 521.1165900000003), (-5.537, 520.8665900000003), (-8.79999999999258, 521.2149999999998), (-8.79999999999258, 520.8349999999998)]</t>
         </is>
       </c>
     </row>
@@ -5647,7 +5647,7 @@
       </c>
       <c r="B523" t="inlineStr">
         <is>
-          <t>[(-0.299999999994134, 522.0), (-0.299999999994134, 521.77), (-5.217, 522.3441900000004), (-5.217, 522.1141900000003), (-5.217, 522.3441900000004), (-5.217, 522.1141900000003), (-10.799999999994, 522.735), (-10.799999999994, 522.355), (-0.299999999994134, 521.77), (-0.299999999994134, 521.61), (-5.217, 522.1141900000003), (-5.217, 521.8841900000003), (-5.217, 522.1141900000003), (-5.217, 521.8841900000003), (-10.799999999994, 522.355), (-10.799999999994, 521.975)]</t>
+          <t>[(-0.299999999994134, 522.0), (-0.299999999994134, 521.77), (-5.217, 522.3441900000004), (-5.217, 522.1141900000003), (-5.217, 522.3441900000004), (-5.217, 522.1141900000003), (-8.80000000000401, 522.5950000000007), (-8.80000000000401, 522.2150000000007), (-0.299999999994134, 521.77), (-0.299999999994134, 521.61), (-5.217, 522.1141900000003), (-5.217, 521.8841900000003), (-5.217, 522.1141900000003), (-5.217, 521.8841900000003), (-8.80000000000401, 522.2150000000007), (-8.80000000000401, 521.8350000000007)]</t>
         </is>
       </c>
     </row>
@@ -5657,7 +5657,7 @@
       </c>
       <c r="B524" t="inlineStr">
         <is>
-          <t>[(-0.299999999979054, 523.0), (-0.299999999979054, 522.81), (-4.758, 523.3120600000015), (-4.758, 523.1220600000014), (-4.758, 523.3120600000015), (-4.758, 523.1220600000014), (-10.7999999999846, 523.7350000000004), (-10.7999999999846, 523.3750000000003), (-0.299999999979054, 522.81), (-0.299999999979054, 522.66), (-4.758, 523.1220600000014), (-4.758, 522.9320600000015), (-4.758, 523.1220600000014), (-4.758, 522.9320600000015), (-10.7999999999846, 523.3750000000003), (-10.7999999999846, 523.0150000000003)]</t>
+          <t>[(-0.299999999979054, 523.0), (-0.299999999979054, 522.81), (-4.758, 523.3120600000015), (-4.758, 523.1220600000014), (-4.758, 523.3120600000015), (-4.758, 523.1220600000014), (-8.79999999999188, 523.5950000000009), (-8.79999999999188, 523.2550000000009), (-0.299999999979054, 522.81), (-0.299999999979054, 522.66), (-4.758, 523.1220600000014), (-4.758, 522.9320600000015), (-4.758, 523.1220600000014), (-4.758, 522.9320600000015), (-8.79999999999188, 523.2550000000009), (-8.79999999999188, 522.915000000001)]</t>
         </is>
       </c>
     </row>
@@ -5667,7 +5667,7 @@
       </c>
       <c r="B525" t="inlineStr">
         <is>
-          <t>[(-0.299999999999697, 524.0), (-0.299999999999697, 523.83), (-3.886, 524.25102), (-3.886, 524.0810200000001), (-3.886, 524.25102), (-3.886, 524.0910200000001), (-10.769, 524.73283), (-10.769, 524.1928300000001), (-0.299999999999697, 523.83), (-0.299999999999697, 523.7), (-3.886, 524.0810200000001), (-3.886, 523.92102), (-3.886, 524.0910200000001), (-3.886, 523.93102), (-10.769, 524.1928300000001), (-10.769, 523.65283)]</t>
+          <t>[(-0.299999999999697, 524.0), (-0.299999999999697, 523.83), (-3.886, 524.25102), (-3.886, 524.0810200000001), (-3.886, 524.25102), (-3.886, 524.0910200000001), (-8.79999999999566, 524.5949999999997), (-8.79999999999566, 524.1349999999996), (-0.299999999999697, 523.83), (-0.299999999999697, 523.7), (-3.886, 524.0810200000001), (-3.886, 523.92102), (-3.886, 524.0910200000001), (-3.886, 523.93102), (-8.79999999999566, 524.1349999999996), (-8.79999999999566, 523.6749999999997)]</t>
         </is>
       </c>
     </row>
@@ -5677,7 +5677,7 @@
       </c>
       <c r="B526" t="inlineStr">
         <is>
-          <t>[(-0.300000000004062, 525.0), (-0.300000000004062, 524.82), (-2.604, 525.1612799999997), (-2.604, 524.9812799999997), (-2.604, 525.1612799999997), (-2.604, 525.0012799999997), (-9.407, 525.6374899999997), (-9.407, 525.0874899999998), (-0.300000000004062, 524.82), (-0.300000000004062, 524.64), (-2.604, 524.9812799999997), (-2.604, 524.8312799999997), (-2.604, 525.0012799999997), (-2.604, 524.8412799999996), (-9.407, 525.0874899999998), (-9.407, 524.5374899999997)]</t>
+          <t>[(-0.300000000004062, 525.0), (-0.300000000004062, 524.82), (-2.604, 525.1612799999997), (-2.604, 524.9812799999997), (-2.604, 525.1612799999997), (-2.604, 525.0012799999997), (-9.00078263048913, 525.609054784134), (-9.00078263048913, 525.089054784134), (-0.300000000004062, 524.82), (-0.300000000004062, 524.64), (-2.604, 524.9812799999997), (-2.604, 524.8312799999997), (-2.604, 525.0012799999997), (-2.604, 524.8412799999996), (-9.00078263048913, 525.089054784134), (-9.00078263048913, 524.569054784134)]</t>
         </is>
       </c>
     </row>
@@ -5717,7 +5717,7 @@
       </c>
       <c r="B530" t="inlineStr">
         <is>
-          <t>[(-0.300000000004344, 529.0), (-0.300000000004344, 528.89), (-6.439, 529.2228470198341), (-6.439, 529.1128470198341), (-0.300000000004344, 528.89), (-0.300000000004344, 528.69), (-6.439, 529.1128470198341), (-6.439, 528.8128470198342)]</t>
+          <t>[(-0.300000000004344, 529.0), (-0.300000000004344, 528.88), (-6.439, 529.2228470198341), (-6.439, 529.1028470198341), (-0.300000000004344, 528.88), (-0.300000000004344, 528.69), (-6.439, 529.1028470198341), (-6.439, 528.8128470198342)]</t>
         </is>
       </c>
     </row>
@@ -5747,7 +5747,7 @@
       </c>
       <c r="B533" t="inlineStr">
         <is>
-          <t>[(-0.300000000008061, 532.0), (-0.300000000008061, 531.89), (-7.239, 531.8360117809315), (-7.239, 531.7260117809315), (-0.300000000008061, 531.89), (-0.300000000008061, 531.66), (-7.239, 531.7260117809315), (-7.239, 531.5860117809315)]</t>
+          <t>[(-0.300000000008061, 532.0), (-0.300000000008061, 531.88), (-7.239, 531.8360117809315), (-7.239, 531.7160117809315), (-0.300000000008061, 531.88), (-0.300000000008061, 531.66), (-7.239, 531.7160117809315), (-7.239, 531.5860117809315)]</t>
         </is>
       </c>
     </row>
@@ -5777,7 +5777,7 @@
       </c>
       <c r="B536" t="inlineStr">
         <is>
-          <t>[(-0.300000000007116, 535.0), (-0.300000000007116, 534.85), (-9.776, 534.7631000000001), (-9.776, 534.6131000000001), (-0.300000000007116, 534.85), (-0.300000000007116, 534.74), (-9.776, 534.6131000000001), (-9.776, 534.4631000000002)]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5827,7 +5827,7 @@
       </c>
       <c r="B541" t="inlineStr">
         <is>
-          <t>[(-0.300000000007116, 540.0), (-0.300000000007116, 539.85), (-6.919, 539.8345250000002), (-6.919, 539.6845250000002), (-0.300000000007116, 539.85), (-0.300000000007116, 539.74), (-6.919, 539.6845250000002), (-6.919, 539.5345250000003)]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6107,7 +6107,7 @@
       </c>
       <c r="B569" t="inlineStr">
         <is>
-          <t>[(-0.300000000012235, 568.0), (-0.300000000012235, 567.8), (-5.352, 568.2580218142429), (-5.352, 568.0580218142428), (-0.300000000012235, 567.8), (-0.300000000012235, 567.6), (-5.352, 568.0580218142428), (-5.352, 567.8580218142429), (-0.300000000012235, 567.6), (-0.300000000012235, 567.49), (-5.352, 567.8580218142429), (-5.352, 567.6680218142428)]</t>
+          <t>[(-0.300000000012235, 568.0), (-0.300000000012235, 567.7), (-5.352, 568.2580218142429), (-5.352, 567.9580218142429), (-0.300000000012235, 567.7), (-0.300000000012235, 567.49), (-5.352, 567.9580218142429), (-5.352, 567.6680218142428)]</t>
         </is>
       </c>
     </row>
@@ -6317,7 +6317,7 @@
       </c>
       <c r="B590" t="inlineStr">
         <is>
-          <t>[(-0.299999999999168, 589.0), (-0.299999999999168, 588.84), (-6.002, 588.85745), (-6.002, 588.69745), (-0.299999999999168, 588.84), (-0.299999999999168, 588.68), (-6.002, 588.69745), (-6.002, 588.5374499999999), (-0.299999999999168, 588.68), (-0.299999999999168, 588.57), (-6.002, 588.5374499999999), (-6.002, 588.38745)]</t>
+          <t>[(-0.299999999999168, 589.0), (-0.299999999999168, 588.76), (-6.002, 588.85745), (-6.002, 588.61745), (-0.299999999999168, 588.76), (-0.299999999999168, 588.57), (-6.002, 588.61745), (-6.002, 588.38745)]</t>
         </is>
       </c>
     </row>
@@ -6417,7 +6417,7 @@
       </c>
       <c r="B600" t="inlineStr">
         <is>
-          <t>[(-0.299999999990689, 599.0), (-0.299999999990689, 598.82), (-6.221, 598.8519749999998), (-6.221, 598.6719749999999), (-0.299999999990689, 598.82), (-0.299999999990689, 598.64), (-6.221, 598.6719749999999), (-6.221, 598.4919749999998), (-0.299999999990689, 598.64), (-0.299999999990689, 598.48), (-6.221, 598.4919749999998), (-6.221, 598.3819749999998)]</t>
+          <t>[(-0.299999999990689, 599.0), (-0.299999999990689, 598.74), (-6.221, 598.8519749999998), (-6.221, 598.5919749999998), (-0.299999999990689, 598.74), (-0.299999999990689, 598.48), (-6.221, 598.5919749999998), (-6.221, 598.3819749999998)]</t>
         </is>
       </c>
     </row>
@@ -6507,7 +6507,7 @@
       </c>
       <c r="B609" t="inlineStr">
         <is>
-          <t>[(-0.30000000000848, 608.0), (-0.30000000000848, 607.77), (-5.416, 607.8721000000002), (-5.416, 607.6421000000001), (-0.30000000000848, 607.77), (-0.30000000000848, 607.47), (-5.416, 607.6421000000001), (-5.416, 607.5321000000001)]</t>
+          <t>[(-0.30000000000848, 608.0), (-0.30000000000848, 607.74), (-5.416, 607.8721000000002), (-5.416, 607.7021000000002), (-0.30000000000848, 607.74), (-0.30000000000848, 607.48), (-5.416, 607.7021000000002), (-5.416, 607.5321000000001)]</t>
         </is>
       </c>
     </row>
@@ -6587,7 +6587,7 @@
       </c>
       <c r="B617" t="inlineStr">
         <is>
-          <t>[(-0.299999999997719, 616.0), (-0.299999999997719, 615.83), (-5.754, 615.8636499999999), (-5.754, 615.6936499999999), (-0.299999999997719, 615.83), (-0.299999999997719, 615.72), (-5.754, 615.6936499999999), (-5.754, 615.5336499999999)]</t>
+          <t>[(-0.299999999997719, 616.0), (-0.299999999997719, 615.88), (-5.754, 615.8636499999999), (-5.754, 615.7436499999999), (-0.299999999997719, 615.88), (-0.299999999997719, 615.72), (-5.754, 615.7436499999999), (-5.754, 615.5336499999999)]</t>
         </is>
       </c>
     </row>
@@ -6637,7 +6637,7 @@
       </c>
       <c r="B622" t="inlineStr">
         <is>
-          <t>[(-0.300000000027977, 621.0), (-0.300000000027977, 620.86), (-5.488, 620.8210012365486), (-5.488, 620.6810012365486), (-0.300000000027977, 620.86), (-0.300000000027977, 620.74), (-5.488, 620.6810012365486), (-5.488, 620.5710012365486)]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6647,7 +6647,7 @@
       </c>
       <c r="B623" t="inlineStr">
         <is>
-          <t>[(-0.299999999993878, 622.0), (-0.299999999993878, 621.84), (-5.574, 621.8154099999998), (-5.574, 621.6554099999998), (-0.299999999993878, 621.84), (-0.299999999993878, 621.68), (-5.574, 621.6554099999998), (-5.574, 621.5454099999998)]</t>
+          <t>[(-0.299999999993878, 622.0), (-0.299999999993878, 621.88), (-5.574, 621.8154099999998), (-5.574, 621.6954099999998), (-0.299999999993878, 621.88), (-0.299999999993878, 621.68), (-5.574, 621.6954099999998), (-5.574, 621.5454099999998)]</t>
         </is>
       </c>
     </row>
@@ -6657,7 +6657,7 @@
       </c>
       <c r="B624" t="inlineStr">
         <is>
-          <t>[(-0.300000000000493, 623.0), (-0.300000000000493, 622.89), (-5.733, 622.809845), (-5.733, 622.699845), (-0.300000000000493, 622.89), (-0.300000000000493, 622.67), (-5.733, 622.699845), (-5.733, 622.539845)]</t>
+          <t>[(-0.300000000000493, 623.0), (-0.300000000000493, 622.88), (-5.733, 622.809845), (-5.733, 622.689845), (-0.300000000000493, 622.88), (-0.300000000000493, 622.67), (-5.733, 622.689845), (-5.733, 622.539845)]</t>
         </is>
       </c>
     </row>
@@ -6747,7 +6747,7 @@
       </c>
       <c r="B633" t="inlineStr">
         <is>
-          <t>[(-0.299999999997191, 632.0), (-0.299999999997191, 631.83), (-7.345, 631.7534249999999), (-7.345, 631.5834249999999), (-0.299999999997191, 631.83), (-0.299999999997191, 631.67), (-7.345, 631.5834249999999), (-7.345, 631.4734249999999)]</t>
+          <t>[(-0.299999999997191, 632.0), (-0.299999999997191, 631.88), (-7.345, 631.7534249999999), (-7.345, 631.6334249999999), (-0.299999999997191, 631.88), (-0.299999999997191, 631.67), (-7.345, 631.6334249999999), (-7.345, 631.4734249999999)]</t>
         </is>
       </c>
     </row>
@@ -6767,7 +6767,7 @@
       </c>
       <c r="B635" t="inlineStr">
         <is>
-          <t>[(-0.299999999999378, 634.0), (-0.299999999999378, 633.89), (-7.796, 633.7376399999999), (-7.796, 633.6276399999999), (-0.299999999999378, 633.89), (-0.299999999999378, 633.75), (-7.796, 633.6276399999999), (-7.796, 633.3676399999999)]</t>
+          <t>[(-0.299999999999378, 634.0), (-0.299999999999378, 633.88), (-7.796, 633.7376399999999), (-7.796, 633.6176399999999), (-0.299999999999378, 633.88), (-0.299999999999378, 633.75), (-7.796, 633.6176399999999), (-7.796, 633.3676399999999)]</t>
         </is>
       </c>
     </row>
@@ -6827,7 +6827,7 @@
       </c>
       <c r="B641" t="inlineStr">
         <is>
-          <t>[(-0.299999999994159, 640.0), (-0.299999999994159, 639.86), (-7.456, 639.7780924399998), (-7.456, 639.6380924399998), (-0.299999999994159, 639.86), (-0.299999999994159, 639.75), (-7.456, 639.6380924399998), (-7.456, 639.5080924399998)]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6837,7 +6837,7 @@
       </c>
       <c r="B642" t="inlineStr">
         <is>
-          <t>[(-0.300000000005129, 641.0), (-0.300000000005129, 640.86), (-7.614, 640.7637578000001), (-7.614, 640.6237578000001), (-0.300000000005129, 640.86), (-0.300000000005129, 640.75), (-7.614, 640.6237578000001), (-7.614, 640.4937578000001)]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6847,7 +6847,7 @@
       </c>
       <c r="B643" t="inlineStr">
         <is>
-          <t>[(-0.3, 641.6355600000002), (-0.3, 641.4955600000002), (-6.0, 641.4588030000002), (-6.0, 641.3188030000002), (-0.3, 641.4955600000002), (-0.3, 641.3855600000002), (-6.0, 641.3188030000002), (-6.0, 641.1988030000002)]</t>
+          <t>[(-0.3, 641.6355600000002), (-0.3, 641.5055600000002), (-4.0, 641.5208230000002), (-4.0, 641.3908230000002), (-0.3, 641.5055600000002), (-0.3, 641.3855600000002), (-4.0, 641.3908230000002), (-4.0, 641.2708230000002)]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
coordinates.py review. M and P coordinates of section views added
</commit_message>
<xml_diff>
--- a/output/layerCoordinates_left.xlsx
+++ b/output/layerCoordinates_left.xlsx
@@ -427,7 +427,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>[(-1.99999999999293, 0.0), (-1.99999999999293, -0.13), (-13.452, -0.27247505270572203), (-13.452, -0.40247505270572204), (-1.99999999999293, -0.13), (-1.99999999999293, -0.25), (-13.452, -0.40247505270572204), (-13.452, -0.522475052705722)]</t>
+          <t>[(-26287.359385937594, 66786.9607237198), (-26287.359385937594, 66786.8307237198), (-26298.811385937603, 66786.6882486671), (-26298.811385937603, 66786.55824866709), (-26287.359385937594, 66786.8307237198), (-26287.359385937594, 66786.7107237198), (-26298.811385937603, 66786.55824866709), (-26298.811385937603, 66786.4382486671)]</t>
         </is>
       </c>
     </row>
@@ -437,7 +437,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[(-1.99999999999412, 1.0), (-1.99999999999412, 0.88), (-13.9555152609054, 0.7691333243701213), (-13.9555152609054, 0.6491333243701214), (-1.99999999999412, 0.88), (-1.99999999999412, 0.75), (-13.9555152609054, 0.6491333243701214), (-13.9555152609054, 0.41913332437012135)]</t>
+          <t>[(-26282.359385937594, 66832.3328180164), (-26282.359385937594, 66832.2128180164), (-26294.314901198508, 66832.10195134077), (-26294.314901198508, 66831.98195134077), (-26282.359385937594, 66832.2128180164), (-26282.359385937594, 66832.0828180164), (-26294.314901198508, 66831.98195134077), (-26294.314901198508, 66831.75195134076)]</t>
         </is>
       </c>
     </row>
@@ -447,7 +447,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[(-1.99999999999293, 2.0), (-1.99999999999293, 1.88), (-13.5000000001641, 1.7397993643187313), (-13.5000000001641, 1.6197993643187312), (-1.99999999999293, 1.88), (-1.99999999999293, 1.75), (-13.5000000001641, 1.6197993643187312), (-13.5000000001641, 1.4297993643187312)]</t>
+          <t>[(-26222.359385937594, 66793.704912313), (-26222.359385937594, 66793.584912313), (-26233.859385937765, 66793.44471167732), (-26233.859385937765, 66793.32471167733), (-26222.359385937594, 66793.584912313), (-26222.359385937594, 66793.454912313), (-26233.859385937765, 66793.32471167733), (-26233.859385937765, 66793.13471167732)]</t>
         </is>
       </c>
     </row>
@@ -457,7 +457,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[(-1.99999999999412, 3.0), (-1.99999999999412, 2.88), (-13.5000000002424, 2.779520697163), (-13.5000000002424, 2.659520697163), (-1.99999999999412, 2.88), (-1.99999999999412, 2.75), (-13.5000000002424, 2.659520697163), (-13.5000000002424, 2.449520697163)]</t>
+          <t>[(-26222.359385937594, 66835.0431078244), (-26222.359385937594, 66834.9231078244), (-26233.859385937845, 66834.82262852156), (-26233.859385937845, 66834.70262852157), (-26222.359385937594, 66834.9231078244), (-26222.359385937594, 66834.7931078244), (-26233.859385937845, 66834.70262852157), (-26233.859385937845, 66834.49262852156)]</t>
         </is>
       </c>
     </row>
@@ -487,7 +487,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[(-1.99999999999412, 6.0), (-1.99999999999412, 5.87), (-10.541, 5.84420606104222), (-10.541, 5.71420606104222), (-1.99999999999412, 5.87), (-1.99999999999412, 5.75), (-10.541, 5.71420606104222), (-10.541, 5.59420606104222)]</t>
+          <t>[(-26094.159385937593, 66861.0951197353), (-26094.159385937593, 66860.9651197353), (-26102.700385937602, 66860.93932579634), (-26102.700385937602, 66860.80932579633), (-26094.159385937593, 66860.9651197353), (-26094.159385937593, 66860.8451197353), (-26102.700385937602, 66860.80932579633), (-26102.700385937602, 66860.68932579634)]</t>
         </is>
       </c>
     </row>
@@ -497,7 +497,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[(-1.99999999999293, 7.0), (-1.99999999999293, 6.88), (-10.49999999999692, 6.892505001428925), (-10.49999999999692, 6.772505001428925), (-1.99999999999293, 6.88), (-1.99999999999293, 6.75), (-10.49999999999692, 6.772505001428925), (-10.49999999999692, 6.532505001428925)]</t>
+          <t>[(-26034.159385937593, 66786.4450960486), (-26034.159385937593, 66786.3250960486), (-26042.659385937597, 66786.33760105002), (-26042.659385937597, 66786.21760105003), (-26034.159385937593, 66786.3250960486), (-26034.159385937593, 66786.1950960486), (-26042.659385937597, 66786.21760105003), (-26042.659385937597, 66785.97760105002)]</t>
         </is>
       </c>
     </row>
@@ -507,7 +507,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[(-1.99999999999412, 8.0), (-1.99999999999412, 7.88), (-10.4999999999981, 7.864825791528048), (-10.4999999999981, 7.744825791528048), (-1.99999999999412, 7.88), (-1.99999999999412, 7.75), (-10.4999999999981, 7.744825791528048), (-10.4999999999981, 7.494825791528048)]</t>
+          <t>[(-26034.159385937593, 66821.7085864941), (-26034.159385937593, 66821.58858649411), (-26042.659385937597, 66821.57341228564), (-26042.659385937597, 66821.45341228564), (-26034.159385937593, 66821.58858649411), (-26034.159385937593, 66821.4585864941), (-26042.659385937597, 66821.45341228564), (-26042.659385937597, 66821.20341228564)]</t>
         </is>
       </c>
     </row>
@@ -517,7 +517,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[(-1.99999999999293, 9.0), (-1.99999999999293, 8.88), (-10.49999999999692, 8.908775097501039), (-10.49999999999692, 8.78877509750104), (-1.99999999999293, 8.88), (-1.99999999999293, 8.75), (-10.49999999999692, 8.78877509750104), (-10.49999999999692, 8.488775097501039)]</t>
+          <t>[(-25905.959385937593, 66786.8827912253), (-25905.959385937593, 66786.76279122531), (-25914.459385937596, 66786.7915663228), (-25914.459385937596, 66786.67156632281), (-25905.959385937593, 66786.76279122531), (-25905.959385937593, 66786.6327912253), (-25914.459385937596, 66786.67156632281), (-25914.459385937596, 66786.3715663228)]</t>
         </is>
       </c>
     </row>
@@ -527,7 +527,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[(-1.99999999999293, 10.0), (-1.99999999999293, 9.88), (-10.4999999999981, 9.878588860177935), (-10.4999999999981, 9.758588860177936), (-1.99999999999293, 9.88), (-1.99999999999293, 9.75), (-10.4999999999981, 9.758588860177936), (-10.4999999999981, 9.478588860177934)]</t>
+          <t>[(-25905.959385937593, 66823.9677102422), (-25905.959385937593, 66823.8477102422), (-25914.459385937596, 66823.84629910238), (-25914.459385937596, 66823.72629910239), (-25905.959385937593, 66823.8477102422), (-25905.959385937593, 66823.7177102422), (-25914.459385937596, 66823.72629910239), (-25914.459385937596, 66823.44629910239)]</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[(-1.99999999997917, 11.0), (-1.99999999997917, 10.88), (-10.49999999999692, 10.879303661162705), (-10.49999999999692, 10.759303661162706), (-1.99999999997917, 10.88), (-1.99999999997917, 10.75), (-10.49999999999692, 10.759303661162706), (-10.49999999999692, 10.519303661162706)]</t>
+          <t>[(-25845.95938593758, 66786.9633435448), (-25845.95938593758, 66786.84334354481), (-25854.459385937596, 66786.84264720597), (-25854.459385937596, 66786.72264720597), (-25845.95938593758, 66786.84334354481), (-25845.95938593758, 66786.7133435448), (-25854.459385937596, 66786.72264720597), (-25854.459385937596, 66786.48264720596)]</t>
         </is>
       </c>
     </row>
@@ -547,7 +547,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>[(-1.99999999999293, 12.0), (-1.99999999999293, 11.88), (-10.49999999999692, 11.873055914905787), (-10.49999999999692, 11.753055914905788), (-1.99999999999293, 11.88), (-1.99999999999293, 11.75), (-10.49999999999692, 11.753055914905788), (-10.49999999999692, 11.563055914905787)]</t>
+          <t>[(-25845.959385937593, 66823.86969113321), (-25845.959385937593, 66823.74969113321), (-25854.459385937596, 66823.74274704812), (-25854.459385937596, 66823.62274704812), (-25845.959385937593, 66823.74969113321), (-25845.959385937593, 66823.61969113321), (-25854.459385937596, 66823.62274704812), (-25854.459385937596, 66823.43274704812)]</t>
         </is>
       </c>
     </row>
@@ -567,7 +567,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[(-1.99999999999293, 14.0), (-1.99999999999293, 13.87), (-10.49999999999692, 13.846570397111842), (-10.49999999999692, 13.716570397111841), (-1.99999999999293, 13.87), (-1.99999999999293, 13.75), (-10.49999999999692, 13.716570397111841), (-10.49999999999692, 13.596570397111842)]</t>
+          <t>[(-25717.759385937592, 66829.4427724655), (-25717.759385937592, 66829.31277246549), (-25726.259385937596, 66829.28934286261), (-25726.259385937596, 66829.15934286261), (-25717.759385937592, 66829.31277246549), (-25717.759385937592, 66829.1927724655), (-25726.259385937596, 66829.15934286261), (-25726.259385937596, 66829.03934286261)]</t>
         </is>
       </c>
     </row>
@@ -577,7 +577,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>[(-1.99999999999293, 15.0), (-1.99999999999293, 14.87), (-10.4999999999981, 14.788448797349718), (-10.4999999999981, 14.658448797349717), (-1.99999999999293, 14.87), (-1.99999999999293, 14.75), (-10.4999999999981, 14.658448797349717), (-10.4999999999981, 14.538448797349718)]</t>
+          <t>[(-25657.759385937592, 66790.1969229925), (-25657.759385937592, 66790.0669229925), (-25666.259385937596, 66789.98537178985), (-25666.259385937596, 66789.85537178985), (-25657.759385937592, 66790.0669229925), (-25657.759385937592, 66789.9469229925), (-25666.259385937596, 66789.85537178985), (-25666.259385937596, 66789.73537178985)]</t>
         </is>
       </c>
     </row>
@@ -597,7 +597,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>[(-1.9996071717933, 17.0), (-1.9996071717933, 16.87), (-10.49960717178584, 16.721734153670297), (-10.49960717178584, 16.5917341536703), (-1.9996071717933, 16.87), (-1.9996071717933, 16.75), (-10.49960717178584, 16.5917341536703), (-10.49960717178584, 16.471734153670297)]</t>
+          <t>[(-25529.558993109593, 66793.7860360079), (-25529.558993109593, 66793.6560360079), (-25538.058993109586, 66793.50777016158), (-25538.058993109586, 66793.37777016158), (-25529.558993109593, 66793.6560360079), (-25529.558993109593, 66793.5360360079), (-25538.058993109586, 66793.37777016158), (-25538.058993109586, 66793.25777016158)]</t>
         </is>
       </c>
     </row>
@@ -627,7 +627,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>[(-1.99955414938177, 20.0), (-1.99955414938177, 19.87), (-9.792, 19.616670841692454), (-9.792, 19.486670841692455), (-1.99955414938177, 19.87), (-1.99955414938177, 19.75), (-9.792, 19.486670841692455), (-9.792, 19.366670841692454)]</t>
+          <t>[(-25469.55894008708, 66829.0368619369), (-25469.55894008708, 66828.90686193689), (-25477.3513859377, 66828.65353277858), (-25477.3513859377, 66828.52353277858), (-25469.55894008708, 66828.90686193689), (-25469.55894008708, 66828.7868619369), (-25477.3513859377, 66828.52353277858), (-25477.3513859377, 66828.40353277858)]</t>
         </is>
       </c>
     </row>
@@ -637,7 +637,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>[(-2.00000000000298, 21.0), (-2.00000000000298, 20.87), (-9.625, 20.58140736428484), (-9.625, 20.45140736428484), (-2.00000000000298, 20.87), (-2.00000000000298, 20.75), (-9.625, 20.45140736428484), (-9.625, 20.33140736428484)]</t>
+          <t>[(-26282.359385937605, 66486.3937195079), (-26282.359385937605, 66486.2637195079), (-26289.9843859376, 66485.97512687219), (-26289.9843859376, 66485.84512687218), (-26282.359385937605, 66486.2637195079), (-26282.359385937605, 66486.1437195079), (-26289.9843859376, 66485.84512687218), (-26289.9843859376, 66485.72512687219)]</t>
         </is>
       </c>
     </row>
@@ -647,7 +647,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>[(-1.71700374471454, 22.0), (-1.71700374471454, 21.87), (-9.685, 21.522717024308403), (-9.685, 21.392717024308403), (-1.71700374471454, 21.87), (-1.71700374471454, 21.75), (-9.685, 21.392717024308403), (-9.685, 21.272717024308403)]</t>
+          <t>[(-26282.076389682315, 66527.884985681), (-26282.076389682315, 66527.754985681), (-26290.044385937603, 66527.4077027053), (-26290.044385937603, 66527.2777027053), (-26282.076389682315, 66527.754985681), (-26282.076389682315, 66527.634985681), (-26290.044385937603, 66527.2777027053), (-26290.044385937603, 66527.1577027053)]</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>[(-1.43350342575671, 23.0), (-1.43350342575671, 22.87), (-12.241, 22.297512722674185), (-12.241, 22.167512722674186), (-1.43350342575671, 22.87), (-1.43350342575671, 22.75), (-12.241, 22.167512722674186), (-12.241, 22.047512722674185)]</t>
+          <t>[(-26221.792889363358, 66489.5106604563), (-26221.792889363358, 66489.3806604563), (-26232.600385937603, 66488.80817317897), (-26232.600385937603, 66488.67817317897), (-26221.792889363358, 66489.3806604563), (-26221.792889363358, 66489.2606604563), (-26232.600385937603, 66488.67817317897), (-26232.600385937603, 66488.55817317897)]</t>
         </is>
       </c>
     </row>
@@ -667,7 +667,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>[(-1.15000309491454, 24.0), (-1.15000309491454, 23.87), (-10.958, 23.313440216644018), (-10.958, 23.18344021664402), (-1.15000309491454, 23.87), (-1.15000309491454, 23.75), (-10.958, 23.18344021664402), (-10.958, 23.063440216644018)]</t>
+          <t>[(-26221.509389032515, 66527.2707438337), (-26221.509389032515, 66527.14074383369), (-26231.3173859376, 66526.58418405034), (-26231.3173859376, 66526.45418405034), (-26221.509389032515, 66527.14074383369), (-26221.509389032515, 66527.0207438337), (-26231.3173859376, 66526.45418405034), (-26231.3173859376, 66526.33418405034)]</t>
         </is>
       </c>
     </row>
@@ -677,7 +677,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>[(-0.866502753446838, 25.0), (-0.866502753446838, 24.87), (-9.651, 24.38508519274128), (-9.651, 24.25508519274128), (-0.866502753446838, 24.87), (-0.866502753446838, 24.75), (-9.651, 24.25508519274128), (-9.651, 24.13508519274128)]</t>
+          <t>[(-26093.02588869105, 66489.1652358133), (-26093.02588869105, 66489.0352358133), (-26101.810385937602, 66488.55032100604), (-26101.810385937602, 66488.42032100604), (-26093.02588869105, 66489.0352358133), (-26093.02588869105, 66488.9152358133), (-26101.810385937602, 66488.42032100604), (-26101.810385937602, 66488.30032100604)]</t>
         </is>
       </c>
     </row>
@@ -687,7 +687,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>[(-0.58350240243138, 26.0), (-0.58350240243138, 25.87), (-8.446, 25.449625168170197), (-8.446, 25.319625168170198), (-0.58350240243138, 25.87), (-0.58350240243138, 25.75), (-8.446, 25.319625168170198), (-8.446, 25.199625168170197)]</t>
+          <t>[(-26092.74288833993, 66525.194136395), (-26092.74288833993, 66525.064136395), (-26100.6053859375, 66524.64376156317), (-26100.6053859375, 66524.51376156317), (-26092.74288833993, 66525.064136395), (-26092.74288833993, 66524.944136395), (-26100.6053859375, 66524.51376156317), (-26100.6053859375, 66524.39376156317)]</t>
         </is>
       </c>
     </row>
@@ -697,7 +697,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>[(-0.300002027915957, 27.0), (-0.300002027915957, 26.87), (-6.71, 26.551300141954115), (-6.71, 26.421300141954116), (-0.300002027915957, 26.87), (-0.300002027915957, 26.75), (-6.71, 26.421300141954116), (-6.71, 26.301300141954115)]</t>
+          <t>[(-26092.459387965515, 66561.3574455789), (-26092.459387965515, 66561.2274455789), (-26098.8693859376, 66560.90874572087), (-26098.8693859376, 66560.77874572086), (-26092.459387965515, 66561.2274455789), (-26092.459387965515, 66561.1074455789), (-26098.8693859376, 66560.77874572086), (-26098.8693859376, 66560.65874572087)]</t>
         </is>
       </c>
     </row>
@@ -707,7 +707,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>[(-0.300000000004172, 28.0), (-0.300000000004172, 27.87), (-6.105, 27.59365000000029), (-6.105, 27.463650000000293), (-0.300000000004172, 27.87), (-0.300000000004172, 27.75), (-6.105, 27.463650000000293), (-6.105, 27.34365000000029)]</t>
+          <t>[(-26032.4593859375, 66487.6551633649), (-26032.4593859375, 66487.5251633649), (-26038.2643859375, 66487.2488133649), (-26038.2643859375, 66487.1188133649), (-26032.4593859375, 66487.5251633649), (-26032.4593859375, 66487.4051633649), (-26038.2643859375, 66487.1188133649), (-26038.2643859375, 66486.9988133649)]</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>[(-0.300000000004281, 29.0), (-0.300000000004281, 28.87), (-5.902, 28.6078600000003), (-5.902, 28.4778600000003), (-0.300000000004281, 28.87), (-0.300000000004281, 28.75), (-5.902, 28.4778600000003), (-5.902, 28.3578600000003)]</t>
+          <t>[(-25896.259385937603, 66486.08728975311), (-25896.259385937603, 66485.9572897531), (-25901.8613859376, 66485.69514975311), (-25901.8613859376, 66485.5651497531), (-25896.259385937603, 66485.9572897531), (-25896.259385937603, 66485.83728975311), (-25901.8613859376, 66485.5651497531), (-25901.8613859376, 66485.44514975311)]</t>
         </is>
       </c>
     </row>
@@ -727,7 +727,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>[(-0.300000000018342, 30.0), (-0.300000000018342, 29.86), (-5.672, 29.65939784293226), (-5.672, 29.51939784293226), (-0.300000000018342, 29.86), (-0.300000000018342, 29.74), (-5.672, 29.51939784293226), (-5.672, 29.39939784293226)]</t>
+          <t>[(-25886.259385937617, 66534.65382474341), (-25886.259385937617, 66534.51382474341), (-25891.6313859376, 66534.31322258634), (-25891.6313859376, 66534.17322258634), (-25886.259385937617, 66534.51382474341), (-25886.259385937617, 66534.39382474341), (-25891.6313859376, 66534.17322258634), (-25891.6313859376, 66534.05322258634)]</t>
         </is>
       </c>
     </row>
@@ -737,7 +737,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>[(-0.300000000094395, 31.0), (-0.300000000094395, 30.85), (-5.585, 30.699984140085057), (-5.585, 30.54998414008506), (-0.300000000094395, 30.85), (-0.300000000094395, 30.73), (-5.585, 30.54998414008506), (-5.585, 30.419984140085056)]</t>
+          <t>[(-25806.259385937694, 66487.3547683359), (-25806.259385937694, 66487.20476833591), (-25811.5443859376, 66487.05475247599), (-25811.5443859376, 66486.904752476), (-25806.259385937694, 66487.20476833591), (-25806.259385937694, 66487.0847683359), (-25811.5443859376, 66486.904752476), (-25811.5443859376, 66486.77475247599)]</t>
         </is>
       </c>
     </row>
@@ -747,7 +747,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>[(-0.300000000100046, 32.0), (-0.300000000100046, 31.8), (-5.304, 31.74914134306461), (-5.304, 31.549141343064612), (-0.300000000100046, 31.8), (-0.300000000100046, 31.68), (-5.304, 31.549141343064612), (-5.304, 31.35914134306461)]</t>
+          <t>[(-25816.259385937603, 66534.1424051721), (-25816.259385937603, 66533.9424051721), (-25821.263385937502, 66533.89154651517), (-25821.263385937502, 66533.69154651517), (-25816.259385937603, 66533.9424051721), (-25816.259385937603, 66533.82240517209), (-25821.263385937502, 66533.69154651517), (-25821.263385937502, 66533.50154651517)]</t>
         </is>
       </c>
     </row>
@@ -757,7 +757,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>[(-0.300000000007544, 33.0), (-0.300000000007544, 32.78), (-4.806, 32.80400781877728), (-4.806, 32.58400781877728), (-0.300000000007544, 32.78), (-0.300000000007544, 32.63), (-4.806, 32.58400781877728), (-4.806, 32.37400781877728)]</t>
+          <t>[(-25716.059385937708, 66488.9317066049), (-25716.059385937708, 66488.7117066049), (-25720.5653859377, 66488.73571442367), (-25720.5653859377, 66488.51571442367), (-25716.059385937708, 66488.7117066049), (-25716.059385937708, 66488.5617066049), (-25720.5653859377, 66488.51571442367), (-25720.5653859377, 66488.30571442368)]</t>
         </is>
       </c>
     </row>
@@ -767,7 +767,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>[(-0.300000000005614, 34.0), (-0.300000000005614, 33.8), (-3.873, 33.86829914443505), (-3.873, 33.668299144435046), (-0.300000000005614, 33.8), (-0.300000000005614, 33.62), (-3.873, 33.668299144435046), (-3.873, 33.47829914443505)]</t>
+          <t>[(-25716.059385937606, 66529.7210080376), (-25716.059385937606, 66529.5210080376), (-25719.6323859376, 66529.58930718203), (-25719.6323859376, 66529.38930718203), (-25716.059385937606, 66529.5210080376), (-25716.059385937606, 66529.34100803759), (-25719.6323859376, 66529.38930718203), (-25719.6323859376, 66529.19930718203)]</t>
         </is>
       </c>
     </row>
@@ -777,7 +777,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>[(-0.300000000073654, 35.0), (-0.300000000073654, 34.85), (-2.676, 34.928187256419015), (-2.676, 34.77818725641902), (-0.300000000073654, 34.85), (-0.300000000073654, 34.7), (-2.676, 34.77818725641902), (-2.676, 34.62818725641902), (-0.300000000073654, 34.7), (-0.300000000073654, 34.57), (-2.676, 34.62818725641902), (-2.676, 34.498187256419016)]</t>
+          <t>[(-25656.059385937573, 66490.5103094704), (-25656.059385937573, 66490.3603094704), (-25658.4353859375, 66490.43849672681), (-25658.4353859375, 66490.28849672682), (-25656.059385937573, 66490.3603094704), (-25656.059385937573, 66490.21030947039), (-25658.4353859375, 66490.28849672682), (-25658.4353859375, 66490.13849672681), (-25656.059385937573, 66490.21030947039), (-25656.059385937573, 66490.0803094704), (-25658.4353859375, 66490.13849672681), (-25658.4353859375, 66490.00849672682)]</t>
         </is>
       </c>
     </row>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>[(-0.299999999997444, 95.0), (-0.299999999997444, 94.87), (-2.48, 94.86919999999985), (-2.48, 94.73919999999985), (-0.299999999997444, 94.87), (-0.299999999997444, 94.75), (-2.48, 94.73919999999985), (-2.48, 94.61919999999985)]</t>
+          <t>[(-22260.459385937495, 66490.6405937467), (-22260.459385937495, 66490.5105937467), (-22262.6393859375, 66490.5097937467), (-22262.6393859375, 66490.3797937467), (-22260.459385937495, 66490.5105937467), (-22260.459385937495, 66490.3905937467), (-22262.6393859375, 66490.3797937467), (-22262.6393859375, 66490.2597937467)]</t>
         </is>
       </c>
     </row>
@@ -1837,7 +1837,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>[(-0.300000000073797, 141.0), (-0.300000000073797, 140.74), (-2.69, 141.1563943337178), (-2.69, 140.8963943337178), (-0.300000000073797, 140.74), (-0.300000000073797, 140.54), (-2.69, 140.8963943337178), (-2.69, 140.6363943337178)]</t>
+          <t>[(-20190.259385937574, 66489.3476710649), (-20190.259385937574, 66489.0876710649), (-20192.6493859375, 66489.50406539862), (-20192.6493859375, 66489.24406539863), (-20190.259385937574, 66489.0876710649), (-20190.259385937574, 66488.88767106489), (-20192.6493859375, 66489.24406539863), (-20192.6493859375, 66488.98406539862)]</t>
         </is>
       </c>
     </row>
@@ -1847,7 +1847,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>[(-0.29999999997969, 142.0), (-0.29999999997969, 141.73), (-3.261, 142.1815794119408), (-3.261, 141.91157941194078), (-0.29999999997969, 141.73), (-0.29999999997969, 141.54), (-3.261, 141.91157941194078), (-3.261, 141.6415794119408)]</t>
+          <t>[(-20190.25938593758, 66530.1613111599), (-20190.25938593758, 66529.8913111599), (-20193.2203859376, 66530.34289057185), (-20193.2203859376, 66530.07289057184), (-20190.25938593758, 66529.8913111599), (-20190.25938593758, 66529.7013111599), (-20193.2203859376, 66530.07289057184), (-20193.2203859376, 66529.80289057185)]</t>
         </is>
       </c>
     </row>
@@ -1857,7 +1857,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>[(-0.300000000119558, 143.0), (-0.300000000119558, 142.74), (-3.659, 143.19216972424366), (-3.659, 142.93216972424366), (-0.300000000119558, 142.74), (-0.300000000119558, 142.55), (-3.659, 142.93216972424366), (-3.659, 142.67216972424364)]</t>
+          <t>[(-20070.05938593762, 66488.9749512549), (-20070.05938593762, 66488.71495125491), (-20073.4183859375, 66489.16712097915), (-20073.4183859375, 66488.90712097916), (-20070.05938593762, 66488.71495125491), (-20070.05938593762, 66488.5249512549), (-20073.4183859375, 66488.90712097916), (-20073.4183859375, 66488.64712097915)]</t>
         </is>
       </c>
     </row>
@@ -1867,7 +1867,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>[(-0.300000000016708, 144.0), (-0.300000000016708, 143.78), (-4.017, 144.1973619800469), (-4.017, 143.9773619800469), (-0.300000000016708, 143.78), (-0.300000000016708, 143.59), (-4.017, 143.9773619800469), (-4.017, 143.7673619800469)]</t>
+          <t>[(-20070.059385937617, 66525.7885913499), (-20070.059385937617, 66525.5685913499), (-20073.7763859376, 66525.98595332995), (-20073.7763859376, 66525.76595332994), (-20070.059385937617, 66525.5685913499), (-20070.059385937617, 66525.3785913499), (-20073.7763859376, 66525.76595332994), (-20073.7763859376, 66525.55595332995)]</t>
         </is>
       </c>
     </row>
@@ -1877,7 +1877,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>[(-0.30000000003092, 145.0), (-0.30000000003092, 144.81), (-4.438, 145.2026951080557), (-4.438, 145.0126951080557), (-0.30000000003092, 144.81), (-0.30000000003092, 144.64), (-4.438, 145.0126951080557), (-4.438, 144.8226951080557)]</t>
+          <t>[(-20010.059385937533, 66488.60223144491), (-20010.059385937533, 66488.4122314449), (-20014.1973859375, 66488.80492655297), (-20014.1973859375, 66488.61492655297), (-20010.059385937533, 66488.4122314449), (-20010.059385937533, 66488.2422314449), (-20014.1973859375, 66488.61492655297), (-20014.1973859375, 66488.42492655297)]</t>
         </is>
       </c>
     </row>
@@ -1887,7 +1887,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>[(-0.300000000050472, 146.0), (-0.300000000050472, 145.81), (-4.773, 146.20070598565374), (-4.773, 146.01070598565374), (-0.300000000050472, 145.81), (-0.300000000050472, 145.65), (-4.773, 146.01070598565374), (-4.773, 145.82070598565375)]</t>
+          <t>[(-20010.05938593755, 66525.41554088), (-20010.05938593755, 66525.22554088), (-20014.532385937502, 66525.61624686565), (-20014.532385937502, 66525.42624686565), (-20010.05938593755, 66525.22554088), (-20010.05938593755, 66525.06554088), (-20014.532385937502, 66525.42624686565), (-20014.532385937502, 66525.23624686565)]</t>
         </is>
       </c>
     </row>
@@ -1897,7 +1897,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>[(-0.300000000001596, 147.0), (-0.300000000001596, 146.79), (-5.091, 147.19526809118958), (-5.091, 146.98526809118957), (-0.300000000001596, 146.79), (-0.300000000001596, 146.61), (-5.091, 146.98526809118957), (-5.091, 146.7752680911896)]</t>
+          <t>[(-19881.859385937703, 66486.1613877525), (-19881.859385937703, 66485.95138775249), (-19886.6503859377, 66486.35665584369), (-19886.6503859377, 66486.14665584368), (-19881.859385937703, 66485.95138775249), (-19881.859385937703, 66485.7713877525), (-19886.6503859377, 66486.14665584368), (-19886.6503859377, 66485.93665584369)]</t>
         </is>
       </c>
     </row>
@@ -1907,7 +1907,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>[(-0.300000000142978, 148.0), (-0.300000000142978, 147.85), (-5.595, 148.1940299321628), (-5.595, 148.0440299321628), (-0.300000000142978, 147.85), (-0.300000000142978, 147.7), (-5.595, 148.0440299321628), (-5.595, 147.8940299321628), (-0.300000000142978, 147.7), (-0.300000000142978, 147.58), (-5.595, 147.8940299321628), (-5.595, 147.7540299321628)]</t>
+          <t>[(-19881.859385937645, 66526.7893100966), (-19881.859385937645, 66526.63931009661), (-19887.1543859375, 66526.98334002876), (-19887.1543859375, 66526.83334002877), (-19881.859385937645, 66526.63931009661), (-19881.859385937645, 66526.4893100966), (-19887.1543859375, 66526.83334002877), (-19887.1543859375, 66526.68334002876), (-19881.859385937645, 66526.4893100966), (-19881.859385937645, 66526.3693100966), (-19887.1543859375, 66526.68334002876), (-19887.1543859375, 66526.54334002876)]</t>
         </is>
       </c>
     </row>
@@ -1917,7 +1917,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>[(-0.300000000011696, 149.0), (-0.300000000011696, 148.85), (-6.265, 149.19404568345902), (-6.265, 149.04404568345902), (-0.300000000011696, 148.85), (-0.300000000011696, 148.7), (-6.265, 149.04404568345902), (-6.265, 148.894045683459), (-0.300000000011696, 148.7), (-0.300000000011696, 148.57), (-6.265, 148.894045683459), (-6.265, 148.74404568345903)]</t>
+          <t>[(-19821.85938593751, 66487.2993079125), (-19821.85938593751, 66487.1493079125), (-19827.8243859375, 66487.49335359596), (-19827.8243859375, 66487.34335359596), (-19821.85938593751, 66487.1493079125), (-19821.85938593751, 66486.9993079125), (-19827.8243859375, 66487.34335359596), (-19827.8243859375, 66487.19335359595), (-19821.85938593751, 66486.9993079125), (-19821.85938593751, 66486.86930791251), (-19827.8243859375, 66487.19335359595), (-19827.8243859375, 66487.04335359596)]</t>
         </is>
       </c>
     </row>
@@ -1927,7 +1927,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>[(-0.300000000025586, 150.0), (-0.300000000025586, 149.78), (-7.035, 150.19139138072168), (-7.035, 149.97139138072168), (-0.300000000025586, 149.78), (-0.300000000025586, 149.59), (-7.035, 149.97139138072168), (-7.035, 149.75139138072169)]</t>
+          <t>[(-19821.859385937623, 66525.6913812001), (-19821.859385937623, 66525.4713812001), (-19828.5943859376, 66525.88277258082), (-19828.5943859376, 66525.66277258082), (-19821.859385937623, 66525.4713812001), (-19821.859385937623, 66525.2813812001), (-19828.5943859376, 66525.66277258082), (-19828.5943859376, 66525.44277258082)]</t>
         </is>
       </c>
     </row>
@@ -1937,7 +1937,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>[(-0.300000000004276, 151.0), (-0.300000000004276, 150.79), (-7.802, 151.15582175639136), (-7.802, 150.94582175639135), (-0.300000000004276, 150.79), (-0.300000000004276, 150.61), (-7.802, 150.94582175639135), (-7.802, 150.73582175639137)]</t>
+          <t>[(-19693.659385937503, 66487.9655299594), (-19693.659385937503, 66487.7555299594), (-19701.1613859375, 66488.12135171579), (-19701.1613859375, 66487.91135171578), (-19693.659385937503, 66487.7555299594), (-19693.659385937503, 66487.5755299594), (-19701.1613859375, 66487.91135171578), (-19701.1613859375, 66487.70135171579)]</t>
         </is>
       </c>
     </row>
@@ -1947,7 +1947,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>[(-0.300000000004276, 152.0), (-0.300000000004276, 151.82), (-8.397, 151.96575532011482), (-8.397, 151.78575532011482), (-0.300000000004276, 151.82), (-0.300000000004276, 151.65), (-8.397, 151.78575532011482), (-8.397, 151.6357553201148)]</t>
+          <t>[(-19693.659385937503, 66530.1217541904), (-19693.659385937503, 66529.94175419041), (-19701.7563859375, 66530.08750951051), (-19701.7563859375, 66529.90750951052), (-19693.659385937503, 66529.94175419041), (-19693.659385937503, 66529.7717541904), (-19701.7563859375, 66529.90750951052), (-19701.7563859375, 66529.75750951051)]</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>[(-0.300000000003251, 160.0), (-0.300000000003251, 159.88), (-4.255, 159.9011250000001), (-4.255, 159.7811250000001), (-4.255, 159.9011250000001), (-4.255, 159.7711250000001), (-14.5293427398727, 159.64426643150327), (-14.5293427398727, 159.42426643150327), (-0.300000000003251, 159.88), (-0.300000000003251, 159.58), (-4.255, 159.7811250000001), (-4.255, 159.6411250000001), (-4.255, 159.7711250000001), (-4.255, 159.6411250000001), (-14.5293427398727, 159.42426643150327), (-14.5293427398727, 159.20426643150327)]</t>
+          <t>[(-19319.259385937505, 66545.37958786241), (-19319.259385937505, 66545.25958786241), (-19323.214385937503, 66545.28071286241), (-19323.214385937503, 66545.16071286242), (-19323.214385937503, 66545.28071286241), (-19323.214385937503, 66545.1507128624), (-19333.488728677374, 66545.0238542939), (-19333.488728677374, 66544.8038542939), (-19319.259385937505, 66545.25958786241), (-19319.259385937505, 66544.95958786241), (-19323.214385937503, 66545.16071286242), (-19323.214385937503, 66545.02071286242), (-19323.214385937503, 66545.1507128624), (-19323.214385937503, 66545.02071286242), (-19333.488728677374, 66544.8038542939), (-19333.488728677374, 66544.5838542939)]</t>
         </is>
       </c>
     </row>
@@ -2037,7 +2037,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>[(-0.299999999989289, 161.0), (-0.299999999989289, 160.87), (-4.396, 160.89759999999973), (-4.396, 160.76759999999973), (-4.396, 160.89759999999973), (-4.396, 160.77759999999972), (-8.79999999999042, 160.78749999999997), (-8.79999999999042, 160.66749999999996), (-0.299999999989289, 160.87), (-0.299999999989289, 160.57), (-4.396, 160.76759999999973), (-4.396, 160.61759999999973), (-4.396, 160.77759999999972), (-4.396, 160.61759999999973), (-8.79999999999042, 160.66749999999996), (-8.79999999999042, 160.36749999999998)]</t>
+          <t>[(-19239.25938593749, 66498.6853193004), (-19239.25938593749, 66498.5553193004), (-19243.355385937502, 66498.5829193004), (-19243.355385937502, 66498.4529193004), (-19243.355385937502, 66498.5829193004), (-19243.355385937502, 66498.46291930041), (-19247.759385937494, 66498.47281930041), (-19247.759385937494, 66498.35281930042), (-19239.25938593749, 66498.5553193004), (-19239.25938593749, 66498.25531930041), (-19243.355385937502, 66498.4529193004), (-19243.355385937502, 66498.3029193004), (-19243.355385937502, 66498.46291930041), (-19243.355385937502, 66498.3029193004), (-19247.759385937494, 66498.35281930042), (-19247.759385937494, 66498.05281930041)]</t>
         </is>
       </c>
     </row>
@@ -2047,7 +2047,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>[(-0.300000000004276, 162.0), (-0.300000000004276, 161.88), (-4.481, 161.89547500000012), (-4.481, 161.7754750000001), (-4.481, 161.89547500000012), (-4.481, 161.7754750000001), (-8.80000000000438, 161.7875), (-8.80000000000438, 161.6675), (-0.300000000004276, 161.88), (-0.300000000004276, 161.62), (-4.481, 161.7754750000001), (-4.481, 161.64547500000012), (-4.481, 161.7754750000001), (-4.481, 161.64547500000012), (-8.80000000000438, 161.6675), (-8.80000000000438, 161.3875)]</t>
+          <t>[(-19239.259385937505, 66545.935247167), (-19239.259385937505, 66545.815247167), (-19243.4403859375, 66545.830722167), (-19243.4403859375, 66545.710722167), (-19243.4403859375, 66545.830722167), (-19243.4403859375, 66545.710722167), (-19247.759385937505, 66545.722747167), (-19247.759385937505, 66545.60274716701), (-19239.259385937505, 66545.815247167), (-19239.259385937505, 66545.555247167), (-19243.4403859375, 66545.710722167), (-19243.4403859375, 66545.580722167), (-19243.4403859375, 66545.710722167), (-19243.4403859375, 66545.580722167), (-19247.759385937505, 66545.60274716701), (-19247.759385937505, 66545.32274716701)]</t>
         </is>
       </c>
     </row>
@@ -2057,7 +2057,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>[(-0.299999999985573, 163.0), (-0.299999999985573, 162.88), (-4.635, 162.89162499999964), (-4.635, 162.77162499999963), (-4.635, 162.89162499999964), (-4.635, 162.77162499999963), (-8.79999999998633, 162.7875), (-8.79999999998633, 162.6675), (-0.299999999985573, 162.88), (-0.299999999985573, 162.62), (-4.635, 162.77162499999963), (-4.635, 162.64162499999964), (-4.635, 162.77162499999963), (-4.635, 162.64162499999964), (-8.79999999998633, 162.6675), (-8.79999999998633, 162.3875)]</t>
+          <t>[(-19128.059385937486, 66499.1293714622), (-19128.059385937486, 66499.0093714622), (-19132.3943859375, 66499.0209964622), (-19132.3943859375, 66498.90099646221), (-19132.3943859375, 66499.0209964622), (-19132.3943859375, 66498.90099646221), (-19136.559385937486, 66498.9168714622), (-19136.559385937486, 66498.79687146221), (-19128.059385937486, 66499.0093714622), (-19128.059385937486, 66498.7493714622), (-19132.3943859375, 66498.90099646221), (-19132.3943859375, 66498.7709964622), (-19132.3943859375, 66498.90099646221), (-19132.3943859375, 66498.7709964622), (-19136.559385937486, 66498.79687146221), (-19136.559385937486, 66498.51687146221)]</t>
         </is>
       </c>
     </row>
@@ -2067,7 +2067,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>[(-0.299999999997345, 164.0), (-0.299999999997345, 163.88), (-4.568, 163.89329999999993), (-4.568, 163.77329999999992), (-4.568, 163.89329999999993), (-4.568, 163.77329999999992), (-8.80000000000263, 163.78749999999988), (-8.80000000000263, 163.66749999999988), (-0.299999999997345, 163.88), (-0.299999999997345, 163.58), (-4.568, 163.77329999999992), (-4.568, 163.64329999999993), (-4.568, 163.77329999999992), (-4.568, 163.64329999999993), (-8.80000000000263, 163.66749999999988), (-8.80000000000263, 163.3674999999999)]</t>
+          <t>[(-19133.059385937497, 66538.2676921859), (-19133.059385937497, 66538.1476921859), (-19137.3273859375, 66538.16099218589), (-19137.3273859375, 66538.0409921859), (-19137.3273859375, 66538.16099218589), (-19137.3273859375, 66538.0409921859), (-19141.559385937504, 66538.0551921859), (-19141.559385937504, 66537.9351921859), (-19133.059385937497, 66538.1476921859), (-19133.059385937497, 66537.8476921859), (-19137.3273859375, 66538.0409921859), (-19137.3273859375, 66537.91099218589), (-19137.3273859375, 66538.0409921859), (-19137.3273859375, 66537.91099218589), (-19141.559385937504, 66537.9351921859), (-19141.559385937504, 66537.6351921859)]</t>
         </is>
       </c>
     </row>
@@ -2077,7 +2077,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>[(-0.299999999999201, 165.0), (-0.299999999999201, 164.88), (-4.461, 164.895975), (-4.461, 164.775975), (-4.461, 164.895975), (-4.461, 164.775975), (-8.80000000000645, 164.78749999999982), (-8.80000000000645, 164.66749999999982), (-0.299999999999201, 164.88), (-0.299999999999201, 164.58), (-4.461, 164.775975), (-4.461, 164.645975), (-4.461, 164.775975), (-4.461, 164.645975), (-8.80000000000645, 164.66749999999982), (-8.80000000000645, 164.41749999999982)]</t>
+          <t>[(-19045.0593859376, 66491.3502093382), (-19045.0593859376, 66491.2302093382), (-19049.2203859376, 66491.2461843382), (-19049.2203859376, 66491.12618433821), (-19049.2203859376, 66491.2461843382), (-19049.2203859376, 66491.12618433821), (-19053.559385937606, 66491.1377093382), (-19053.559385937606, 66491.01770933821), (-19045.0593859376, 66491.2302093382), (-19045.0593859376, 66490.9302093382), (-19049.2203859376, 66491.12618433821), (-19049.2203859376, 66490.9961843382), (-19049.2203859376, 66491.12618433821), (-19049.2203859376, 66490.9961843382), (-19053.559385937606, 66491.01770933821), (-19053.559385937606, 66490.76770933821)]</t>
         </is>
       </c>
     </row>
@@ -2087,7 +2087,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>[(-0.299999999993337, 166.0), (-0.299999999993337, 165.88), (-4.253, 165.90117499999982), (-4.253, 165.78117499999982), (-4.253, 165.90117499999982), (-4.253, 165.77117499999983), (-8.7999999999942, 165.78749999999997), (-8.7999999999942, 165.65749999999997), (-0.299999999993337, 165.88), (-0.299999999993337, 165.68), (-4.253, 165.78117499999982), (-4.253, 165.65117499999982), (-4.253, 165.77117499999983), (-4.253, 165.65117499999982), (-8.7999999999942, 165.65749999999997), (-8.7999999999942, 165.53749999999997)]</t>
+          <t>[(-19045.059385937493, 66538.397876596), (-19045.059385937493, 66538.27787659601), (-19049.0123859375, 66538.29905159601), (-19049.0123859375, 66538.17905159602), (-19049.0123859375, 66538.29905159601), (-19049.0123859375, 66538.169051596), (-19053.559385937497, 66538.18537659601), (-19053.559385937497, 66538.055376596), (-19045.059385937493, 66538.27787659601), (-19045.059385937493, 66538.077876596), (-19049.0123859375, 66538.17905159602), (-19049.0123859375, 66538.04905159601), (-19049.0123859375, 66538.169051596), (-19049.0123859375, 66538.04905159601), (-19053.559385937497, 66538.055376596), (-19053.559385937497, 66537.93537659601)]</t>
         </is>
       </c>
     </row>
@@ -2097,7 +2097,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>[(-0.300000000001455, 167.0), (-0.300000000001455, 166.87), (-4.252, 166.90120000000005), (-4.252, 166.77120000000005), (-4.252, 166.90120000000005), (-4.252, 166.77120000000005), (-8.79999999999453, 166.78750000000016), (-8.79999999999453, 166.65750000000017), (-0.300000000001455, 166.87), (-0.300000000001455, 166.75), (-4.252, 166.77120000000005), (-4.252, 166.65120000000005), (-4.252, 166.77120000000005), (-4.252, 166.65120000000005), (-8.79999999999453, 166.65750000000017), (-8.79999999999453, 166.53750000000016)]</t>
+          <t>[(-18946.859385937503, 66491.4450472582), (-18946.859385937503, 66491.31504725819), (-18950.8113859375, 66491.34624725819), (-18950.8113859375, 66491.21624725818), (-18950.8113859375, 66491.34624725819), (-18950.8113859375, 66491.21624725818), (-18955.359385937496, 66491.2325472582), (-18955.359385937496, 66491.1025472582), (-18946.859385937503, 66491.31504725819), (-18946.859385937503, 66491.1950472582), (-18950.8113859375, 66491.21624725818), (-18950.8113859375, 66491.09624725819), (-18950.8113859375, 66491.21624725818), (-18950.8113859375, 66491.09624725819), (-18955.359385937496, 66491.1025472582), (-18955.359385937496, 66490.9825472582)]</t>
         </is>
       </c>
     </row>
@@ -2177,7 +2177,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>[(-0.300000000084013, 175.0), (-0.300000000084013, 174.87), (-4.157, 174.86302894558645), (-4.157, 174.73302894558645), (-4.157, 174.86302894558645), (-4.157, 174.73302894558645), (-9.30042272320688, 174.68037402370223), (-9.30042272320688, 174.55037402370223), (-0.300000000084013, 174.87), (-0.300000000084013, 174.75), (-4.157, 174.73302894558645), (-4.157, 174.61302894558645), (-4.157, 174.73302894558645), (-4.157, 174.61302894558645), (-9.30042272320688, 174.55037402370223), (-9.30042272320688, 174.43037402370223)]</t>
+          <t>[(-18652.659385937583, 66488.313942537), (-18652.659385937583, 66488.183942537), (-18656.5163859375, 66488.1769714826), (-18656.5163859375, 66488.04697148259), (-18656.5163859375, 66488.1769714826), (-18656.5163859375, 66488.04697148259), (-18661.65980866071, 66487.99431656071), (-18661.65980866071, 66487.8643165607), (-18652.659385937583, 66488.183942537), (-18652.659385937583, 66488.063942537), (-18656.5163859375, 66488.04697148259), (-18656.5163859375, 66487.9269714826), (-18656.5163859375, 66488.04697148259), (-18656.5163859375, 66487.9269714826), (-18661.65980866071, 66487.8643165607), (-18661.65980866071, 66487.74431656071)]</t>
         </is>
       </c>
     </row>
@@ -2217,7 +2217,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>[(-0.299999999996132, 179.0), (-0.299999999996132, 178.88), (-3.955, 178.78854818079876), (-3.955, 178.66854818079875), (-3.955, 178.78854818079876), (-3.955, 178.65854818079876), (-8.79999999998878, 178.50825158325387), (-8.79999999998878, 178.37825158325387), (-0.299999999996132, 178.88), (-0.299999999996132, 178.67), (-3.955, 178.66854818079875), (-3.955, 178.53854818079876), (-3.955, 178.65854818079876), (-3.955, 178.53854818079876), (-8.79999999998878, 178.37825158325387), (-8.79999999998878, 178.25825158325387)]</t>
+          <t>[(-18497.459385937495, 66534.2818878893), (-18497.459385937495, 66534.1618878893), (-18501.1143859375, 66534.0704360701), (-18501.1143859375, 66533.95043607011), (-18501.1143859375, 66534.0704360701), (-18501.1143859375, 66533.9404360701), (-18505.959385937487, 66533.79013947255), (-18505.959385937487, 66533.66013947254), (-18497.459385937495, 66534.1618878893), (-18497.459385937495, 66533.9518878893), (-18501.1143859375, 66533.95043607011), (-18501.1143859375, 66533.8204360701), (-18501.1143859375, 66533.9404360701), (-18501.1143859375, 66533.8204360701), (-18505.959385937487, 66533.66013947254), (-18505.959385937487, 66533.54013947255)]</t>
         </is>
       </c>
     </row>
@@ -2227,7 +2227,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>[(-0.299999999997375, 180.0), (-0.299999999997375, 179.88), (-3.483, 179.80901999999983), (-3.483, 179.68901999999983), (-3.483, 179.80901999999983), (-3.483, 179.67901999999984), (-8.80000000000704, 179.4899999999994), (-8.80000000000704, 179.35999999999942), (-0.299999999997375, 179.88), (-0.299999999997375, 179.69), (-3.483, 179.68901999999983), (-3.483, 179.55901999999983), (-3.483, 179.67901999999984), (-3.483, 179.55901999999983), (-8.80000000000704, 179.35999999999942), (-8.80000000000704, 179.2399999999994)]</t>
+          <t>[(-18377.259385937497, 66491.9767963053), (-18377.259385937497, 66491.8567963053), (-18380.442385937502, 66491.7858163053), (-18380.442385937502, 66491.6658163053), (-18380.442385937502, 66491.7858163053), (-18380.442385937502, 66491.6558163053), (-18385.75938593751, 66491.4667963053), (-18385.75938593751, 66491.3367963053), (-18377.259385937497, 66491.8567963053), (-18377.259385937497, 66491.6667963053), (-18380.442385937502, 66491.6658163053), (-18380.442385937502, 66491.5358163053), (-18380.442385937502, 66491.6558163053), (-18380.442385937502, 66491.5358163053), (-18385.75938593751, 66491.3367963053), (-18385.75938593751, 66491.2167963053)]</t>
         </is>
       </c>
     </row>
@@ -2247,7 +2247,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>[(-0.30000000000151, 182.0), (-0.30000000000151, 181.83), (-8.80000000000596, 181.48999999999972), (-8.80000000000596, 181.31999999999974), (-0.30000000000151, 181.83), (-0.30000000000151, 181.67), (-8.80000000000596, 181.31999999999974), (-8.80000000000596, 181.1899999999997)]</t>
+          <t>[(-18309.259385937505, 66489.6101196308), (-18309.259385937505, 66489.4401196308), (-18317.75938593751, 66489.1001196308), (-18317.75938593751, 66488.93011963081), (-18309.259385937505, 66489.4401196308), (-18309.259385937505, 66489.2801196308), (-18317.75938593751, 66488.93011963081), (-18317.75938593751, 66488.8001196308)]</t>
         </is>
       </c>
     </row>
@@ -2257,7 +2257,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>[(-0.299999999993821, 183.0), (-0.299999999993821, 182.81), (-8.644, 182.49935999999963), (-8.644, 182.30935999999963), (-0.299999999993821, 182.81), (-0.299999999993821, 182.63), (-8.644, 182.30935999999963), (-8.644, 182.18935999999962)]</t>
+          <t>[(-18309.259385937497, 66533.5485345403), (-18309.259385937497, 66533.3585345403), (-18317.603385937502, 66533.0478945403), (-18317.603385937502, 66532.8578945403), (-18309.259385937497, 66533.3585345403), (-18309.259385937497, 66533.1785345403), (-18317.603385937502, 66532.8578945403), (-18317.603385937502, 66532.7378945403)]</t>
         </is>
       </c>
     </row>
@@ -2267,7 +2267,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>[(-0.299999999999572, 184.0), (-0.299999999999572, 183.88), (-7.857, 183.54657999999998), (-7.857, 183.42657999999997), (-0.299999999999572, 183.88), (-0.299999999999572, 183.61), (-7.857, 183.42657999999997), (-7.857, 183.29657999999998)]</t>
+          <t>[(-18189.0593859375, 66489.56811828101), (-18189.0593859375, 66489.44811828101), (-18196.6163859375, 66489.114698281), (-18196.6163859375, 66488.994698281), (-18189.0593859375, 66489.44811828101), (-18189.0593859375, 66489.17811828101), (-18196.6163859375, 66488.994698281), (-18196.6163859375, 66488.864698281)]</t>
         </is>
       </c>
     </row>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>[(-0.299999999993799, 185.0), (-0.299999999993799, 184.88), (-6.888, 184.60471999999962), (-6.888, 184.4847199999996), (-0.299999999993799, 184.88), (-0.299999999993799, 184.63), (-6.888, 184.4847199999996), (-6.888, 184.35471999999962)]</t>
+          <t>[(-18189.059385937493, 66529.6688708529), (-18189.059385937493, 66529.5488708529), (-18195.6473859375, 66529.2735908529), (-18195.6473859375, 66529.1535908529), (-18189.059385937493, 66529.5488708529), (-18189.059385937493, 66529.2988708529), (-18195.6473859375, 66529.1535908529), (-18195.6473859375, 66529.0235908529)]</t>
         </is>
       </c>
     </row>
@@ -2287,7 +2287,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>[(-0.299999999996377, 186.0), (-0.299999999996377, 185.88), (-5.892, 185.66447999999977), (-5.892, 185.54447999999977), (-0.299999999996377, 185.88), (-0.299999999996377, 185.68), (-5.892, 185.54447999999977), (-5.892, 185.41447999999977)]</t>
+          <t>[(-18120.059385937497, 66489.85079225591), (-18120.059385937497, 66489.73079225591), (-18125.6513859375, 66489.51527225591), (-18125.6513859375, 66489.39527225592), (-18120.059385937497, 66489.73079225591), (-18120.059385937497, 66489.5307922559), (-18125.6513859375, 66489.39527225592), (-18125.6513859375, 66489.26527225591)]</t>
         </is>
       </c>
     </row>
@@ -2297,7 +2297,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>[(-0.300000000007436, 187.0), (-0.300000000007436, 186.88), (-4.905, 186.72370000000043), (-4.905, 186.60370000000043), (-0.300000000007436, 186.88), (-0.300000000007436, 186.68), (-4.905, 186.60370000000043), (-4.905, 186.47370000000043)]</t>
+          <t>[(-18120.059385937508, 66530.1138824901), (-18120.059385937508, 66529.9938824901), (-18124.6643859375, 66529.8375824901), (-18124.6643859375, 66529.7175824901), (-18120.059385937508, 66529.9938824901), (-18120.059385937508, 66529.79388249009), (-18124.6643859375, 66529.7175824901), (-18124.6643859375, 66529.5875824901)]</t>
         </is>
       </c>
     </row>
@@ -2307,7 +2307,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>[(-0.300000000000548, 188.0), (-0.300000000000548, 187.88), (-4.146, 187.76924000000002), (-4.146, 187.64924000000002), (-0.300000000000548, 187.88), (-0.300000000000548, 187.67), (-4.146, 187.64924000000002), (-4.146, 187.51924000000002)]</t>
+          <t>[(-17999.8593859375, 66488.4581415554), (-17999.8593859375, 66488.3381415554), (-18003.7053859375, 66488.22738155539), (-18003.7053859375, 66488.1073815554), (-17999.8593859375, 66488.3381415554), (-17999.8593859375, 66488.1281415554), (-18003.7053859375, 66488.1073815554), (-18003.7053859375, 66487.97738155539)]</t>
         </is>
       </c>
     </row>
@@ -2317,7 +2317,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>[(-0.300000000001171, 189.0), (-0.300000000001171, 188.81), (-3.637, 188.79978000000008), (-3.637, 188.6097800000001), (-0.300000000001171, 188.81), (-0.300000000001171, 188.62), (-3.637, 188.6097800000001), (-3.637, 188.48978000000008)]</t>
+          <t>[(-17999.859385937503, 66528.883569452), (-17999.859385937503, 66528.69356945199), (-18003.1963859375, 66528.683349452), (-18003.1963859375, 66528.493349452), (-17999.859385937503, 66528.69356945199), (-17999.859385937503, 66528.50356945199), (-18003.1963859375, 66528.493349452), (-18003.1963859375, 66528.373349452)]</t>
         </is>
       </c>
     </row>
@@ -2327,7 +2327,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>[(-0.299999999995328, 190.0), (-0.299999999995328, 189.88), (-3.053, 189.83481999999972), (-3.053, 189.71481999999972), (-0.299999999995328, 189.88), (-0.299999999995328, 189.67), (-3.053, 189.71481999999972), (-3.053, 189.58481999999972)]</t>
+          <t>[(-17939.859385937594, 66489.3901661796), (-17939.859385937594, 66489.2701661796), (-17942.6123859376, 66489.2249861796), (-17942.6123859376, 66489.1049861796), (-17939.859385937594, 66489.2701661796), (-17939.859385937594, 66489.0601661796), (-17942.6123859376, 66489.1049861796), (-17942.6123859376, 66488.9749861796)]</t>
         </is>
       </c>
     </row>
@@ -2337,7 +2337,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>[(-0.300000000021018, 191.0), (-0.300000000021018, 190.82), (-2.361, 190.8818044998709), (-2.361, 190.7018044998709), (-0.300000000021018, 190.82), (-0.300000000021018, 190.64), (-2.361, 190.7018044998709), (-2.361, 190.5618044998709)]</t>
+          <t>[(-17939.85938593752, 66527.9779317385), (-17939.85938593752, 66527.7979317385), (-17941.9203859375, 66527.85973623837), (-17941.9203859375, 66527.67973623838), (-17939.85938593752, 66527.7979317385), (-17939.85938593752, 66527.6179317385), (-17941.9203859375, 66527.67973623838), (-17941.9203859375, 66527.53973623837)]</t>
         </is>
       </c>
     </row>
@@ -2557,7 +2557,7 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>[(-0.300000000037866, 213.0), (-0.300000000037866, 212.88), (-2.761, 213.0726978260564), (-2.761, 212.9526978260564), (-0.300000000037866, 212.88), (-0.300000000037866, 212.75), (-2.761, 212.9526978260564), (-2.761, 212.75269782605642)]</t>
+          <t>[(-26194.65938593754, 66187.0509243367), (-26194.65938593754, 66186.9309243367), (-26197.1203859375, 66187.12362216275), (-26197.1203859375, 66187.00362216275), (-26194.65938593754, 66186.9309243367), (-26194.65938593754, 66186.8009243367), (-26197.1203859375, 66187.00362216275), (-26197.1203859375, 66186.80362216274)]</t>
         </is>
       </c>
     </row>
@@ -2567,7 +2567,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>[(-0.300000000010389, 214.0), (-0.300000000010389, 213.87), (-3.359, 214.0994181172989), (-3.359, 213.96941811729891), (-0.300000000010389, 213.87), (-0.300000000010389, 213.75), (-3.359, 213.96941811729891), (-3.359, 213.8494181172989)]</t>
+          <t>[(-26204.65938593741, 66237.44199903701), (-26204.65938593741, 66237.311999037), (-26207.7183859374, 66237.54141715431), (-26207.7183859374, 66237.4114171543), (-26204.65938593741, 66237.311999037), (-26204.65938593741, 66237.19199903701), (-26207.7183859374, 66237.4114171543), (-26207.7183859374, 66237.29141715431)]</t>
         </is>
       </c>
     </row>
@@ -2577,7 +2577,7 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>[(-0.300000000052873, 215.0), (-0.300000000052873, 214.87), (-4.285, 215.14130989282856), (-4.285, 215.01130989282856), (-0.300000000052873, 214.87), (-0.300000000052873, 214.75), (-4.285, 215.01130989282856), (-4.285, 214.89130989282856)]</t>
+          <t>[(-26095.641365578053, 66185.7914070706), (-26095.641365578053, 66185.6614070706), (-26099.626365578, 66185.93271696343), (-26099.626365578, 66185.80271696343), (-26095.641365578053, 66185.6614070706), (-26095.641365578053, 66185.5414070706), (-26099.626365578, 66185.80271696343), (-26099.626365578, 66185.68271696343)]</t>
         </is>
       </c>
     </row>
@@ -2587,7 +2587,7 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>[(-0.300000000056731, 216.0), (-0.300000000056731, 215.87), (-2.315, 216.07642026067023), (-2.315, 215.94642026067024), (-2.315, 216.07642026067023), (-2.315, 215.94642026067024), (-5.644, 216.2026748749523), (-5.644, 216.0726748749523), (-0.300000000056731, 215.87), (-0.300000000056731, 215.75), (-2.315, 215.94642026067024), (-2.315, 215.82642026067023), (-2.315, 215.94642026067024), (-2.315, 215.82642026067023), (-5.644, 216.0726748749523), (-5.644, 215.9526748749523)]</t>
+          <t>[(-26097.27740629736, 66236.1078680389), (-26097.27740629736, 66235.9778680389), (-26099.2924062973, 66236.18428829957), (-26099.2924062973, 66236.05428829957), (-26099.2924062973, 66236.18428829957), (-26099.2924062973, 66236.05428829957), (-26102.6214062973, 66236.31054291385), (-26102.6214062973, 66236.18054291385), (-26097.27740629736, 66235.9778680389), (-26097.27740629736, 66235.8578680389), (-26099.2924062973, 66236.05428829957), (-26099.2924062973, 66235.93428829957), (-26099.2924062973, 66236.05428829957), (-26099.2924062973, 66235.93428829957), (-26102.6214062973, 66236.18054291385), (-26102.6214062973, 66236.06054291385)]</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>[(-0.299999999995819, 217.0), (-0.299999999995819, 216.87), (-4.206, 217.23903990672204), (-4.206, 217.10903990672205), (-4.206, 217.23903990672204), (-4.206, 217.11903990672204), (-7.515, 217.44154452816144), (-7.515, 217.32154452816144), (-0.299999999995819, 216.87), (-0.299999999995819, 216.75), (-4.206, 217.10903990672205), (-4.206, 216.98903990672204), (-4.206, 217.11903990672204), (-4.206, 216.98903990672204), (-7.515, 217.32154452816144), (-7.515, 217.11154452816143)]</t>
+          <t>[(-26031.459385937596, 66194.4034809633), (-26031.459385937596, 66194.2734809633), (-26035.3653859376, 66194.64252087002), (-26035.3653859376, 66194.51252087002), (-26035.3653859376, 66194.64252087002), (-26035.3653859376, 66194.52252087003), (-26038.6743859376, 66194.84502549146), (-26038.6743859376, 66194.72502549147), (-26031.459385937596, 66194.2734809633), (-26031.459385937596, 66194.1534809633), (-26035.3653859376, 66194.51252087002), (-26035.3653859376, 66194.39252087002), (-26035.3653859376, 66194.52252087003), (-26035.3653859376, 66194.39252087002), (-26038.6743859376, 66194.72502549147), (-26038.6743859376, 66194.51502549146)]</t>
         </is>
       </c>
     </row>
@@ -2607,7 +2607,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>[(-0.300000000000684, 218.0), (-0.300000000000684, 217.88), (-6.083, 218.40480999999994), (-6.083, 218.28480999999994), (-6.083, 218.40480999999994), (-6.083, 218.22480999999993), (-8.8000000000025, 218.59500000000014), (-8.8000000000025, 218.26500000000013), (-0.300000000000684, 217.88), (-0.300000000000684, 217.73), (-6.083, 218.28480999999994), (-6.083, 218.04480999999993), (-6.083, 218.22480999999993), (-6.083, 218.04480999999993), (-8.8000000000025, 218.26500000000013), (-8.8000000000025, 217.93500000000014)]</t>
+          <t>[(-26041.4593859376, 66236.6643716655), (-26041.4593859376, 66236.5443716655), (-26047.2423859376, 66237.06918166549), (-26047.2423859376, 66236.94918166549), (-26047.2423859376, 66237.06918166549), (-26047.2423859376, 66236.8891816655), (-26049.959385937604, 66237.2593716655), (-26049.959385937604, 66236.9293716655), (-26041.4593859376, 66236.5443716655), (-26041.4593859376, 66236.39437166549), (-26047.2423859376, 66236.94918166549), (-26047.2423859376, 66236.70918166549), (-26047.2423859376, 66236.8891816655), (-26047.2423859376, 66236.70918166549), (-26049.959385937604, 66236.9293716655), (-26049.959385937604, 66236.59937166549)]</t>
         </is>
       </c>
     </row>
@@ -2617,7 +2617,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>[(-0.300000000001353, 219.0), (-0.300000000001353, 218.88), (-6.091, 219.4053699999999), (-6.091, 219.2853699999999), (-6.091, 219.4053699999999), (-6.091, 219.19536999999988), (-8.80000000000079, 219.59499999999997), (-8.80000000000079, 219.27499999999998), (-0.300000000001353, 218.88), (-0.300000000001353, 218.72), (-6.091, 219.2853699999999), (-6.091, 218.9853699999999), (-6.091, 219.19536999999988), (-6.091, 218.9853699999999), (-8.80000000000079, 219.27499999999998), (-8.80000000000079, 218.95499999999998)]</t>
+          <t>[(-25904.259385937603, 66190.8905401455), (-25904.259385937603, 66190.7705401455), (-25910.0503859376, 66191.29591014549), (-25910.0503859376, 66191.1759101455), (-25910.0503859376, 66191.29591014549), (-25910.0503859376, 66191.08591014548), (-25912.7593859376, 66191.4855401455), (-25912.7593859376, 66191.16554014549), (-25904.259385937603, 66190.7705401455), (-25904.259385937603, 66190.6105401455), (-25910.0503859376, 66191.1759101455), (-25910.0503859376, 66190.87591014549), (-25910.0503859376, 66191.08591014548), (-25910.0503859376, 66190.87591014549), (-25912.7593859376, 66191.16554014549), (-25912.7593859376, 66190.8455401455)]</t>
         </is>
       </c>
     </row>
@@ -2627,7 +2627,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>[(-0.299999999992942, 220.0), (-0.299999999992942, 219.88), (-7.41, 220.4977000000005), (-7.41, 220.3777000000005), (-7.41, 220.4977000000005), (-7.41, 220.28770000000048), (-8.79999999999426, 220.59500000000008), (-8.79999999999426, 220.28500000000008), (-0.299999999992942, 219.88), (-0.299999999992942, 219.69), (-7.41, 220.3777000000005), (-7.41, 220.0777000000005), (-7.41, 220.28770000000048), (-7.41, 220.0777000000005), (-8.79999999999426, 220.28500000000008), (-8.79999999999426, 219.97500000000008)]</t>
+          <t>[(-25904.259385937592, 66233.0819864032), (-25904.259385937592, 66232.9619864032), (-25911.3693859376, 66233.5796864032), (-25911.3693859376, 66233.4596864032), (-25911.3693859376, 66233.5796864032), (-25911.3693859376, 66233.3696864032), (-25912.759385937596, 66233.6769864032), (-25912.759385937596, 66233.3669864032), (-25904.259385937592, 66232.9619864032), (-25904.259385937592, 66232.7719864032), (-25911.3693859376, 66233.4596864032), (-25911.3693859376, 66233.1596864032), (-25911.3693859376, 66233.3696864032), (-25911.3693859376, 66233.1596864032), (-25912.759385937596, 66233.3669864032), (-25912.759385937596, 66233.0569864032)]</t>
         </is>
       </c>
     </row>
@@ -2637,7 +2637,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>[(-0.299999999999579, 221.0), (-0.299999999999579, 220.83), (-8.461, 221.57127000000003), (-8.461, 221.40127000000004), (-8.461, 221.57127000000003), (-8.461, 221.41127000000003), (-8.79999999999261, 221.59499999999952), (-8.79999999999261, 221.33499999999952), (-0.299999999999579, 220.83), (-0.299999999999579, 220.53), (-8.461, 221.40127000000004), (-8.461, 221.26127000000002), (-8.461, 221.41127000000003), (-8.461, 221.25127000000003), (-8.79999999999261, 221.33499999999952), (-8.79999999999261, 221.0749999999995)]</t>
+          <t>[(-25845.2593859376, 66187.2487934222), (-25845.2593859376, 66187.0787934222), (-25853.4203859376, 66187.8200634222), (-25853.4203859376, 66187.6500634222), (-25853.4203859376, 66187.8200634222), (-25853.4203859376, 66187.6600634222), (-25853.759385937592, 66187.8437934222), (-25853.759385937592, 66187.5837934222), (-25845.2593859376, 66187.0787934222), (-25845.2593859376, 66186.7787934222), (-25853.4203859376, 66187.6500634222), (-25853.4203859376, 66187.5100634222), (-25853.4203859376, 66187.6600634222), (-25853.4203859376, 66187.5000634222), (-25853.759385937592, 66187.5837934222), (-25853.759385937592, 66187.3237934222)]</t>
         </is>
       </c>
     </row>
@@ -2657,7 +2657,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>[(-0.300000000004265, 223.0), (-0.300000000004265, 222.88), (-11.007, 223.7494899999997), (-11.007, 223.6294899999997), (-11.007, 223.7494899999997), (-11.007, 223.6194899999997), (-8.79999999999743, 223.59499999999952), (-8.79999999999743, 223.46499999999952), (-0.300000000004265, 222.88), (-0.300000000004265, 222.75), (-11.007, 223.6294899999997), (-11.007, 223.41948999999968), (-11.007, 223.6194899999997), (-11.007, 223.41948999999968), (-8.79999999999743, 223.46499999999952), (-8.79999999999743, 223.1649999999995)]</t>
+          <t>[(-25718.059385937504, 66187.58044212741), (-25718.059385937504, 66187.46044212741), (-25728.766385937502, 66188.32993212741), (-25728.766385937502, 66188.20993212741), (-25728.766385937502, 66188.32993212741), (-25728.766385937502, 66188.1999321274), (-25726.559385937497, 66188.17544212741), (-25726.559385937497, 66188.0454421274), (-25718.059385937504, 66187.46044212741), (-25718.059385937504, 66187.33044212741), (-25728.766385937502, 66188.20993212741), (-25728.766385937502, 66187.99993212741), (-25728.766385937502, 66188.1999321274), (-25728.766385937502, 66187.99993212741), (-25726.559385937497, 66188.0454421274), (-25726.559385937497, 66187.74544212742)]</t>
         </is>
       </c>
     </row>
@@ -2667,7 +2667,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>[(-0.299999999994225, 224.0), (-0.299999999994225, 223.88), (-11.092, 224.7554400000004), (-11.092, 224.51544000000038), (-11.092, 224.7554400000004), (-11.092, 224.4754400000004), (-8.79999999999597, 224.5950000000001), (-8.79999999999597, 224.3150000000001), (-0.299999999994225, 223.88), (-0.299999999994225, 223.76), (-11.092, 224.51544000000038), (-11.092, 224.2754400000004), (-11.092, 224.4754400000004), (-11.092, 224.2754400000004), (-8.79999999999597, 224.3150000000001), (-8.79999999999597, 224.0450000000001)]</t>
+          <t>[(-25527.859385937496, 66187.7462664801), (-25527.859385937496, 66187.6262664801), (-25538.6513859375, 66188.50170648009), (-25538.6513859375, 66188.26170648009), (-25538.6513859375, 66188.50170648009), (-25538.6513859375, 66188.2217064801), (-25536.359385937496, 66188.3412664801), (-25536.359385937496, 66188.0612664801), (-25527.859385937496, 66187.6262664801), (-25527.859385937496, 66187.5062664801), (-25538.6513859375, 66188.26170648009), (-25538.6513859375, 66188.0217064801), (-25538.6513859375, 66188.2217064801), (-25538.6513859375, 66188.0217064801), (-25536.359385937496, 66188.0612664801), (-25536.359385937496, 66187.7912664801)]</t>
         </is>
       </c>
     </row>
@@ -2677,7 +2677,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>[(-0.300000000005367, 225.0), (-0.300000000005367, 224.88), (-10.831, 225.73716999999962), (-10.831, 225.47716999999963), (-10.831, 225.73716999999962), (-10.831, 225.47716999999963), (-8.79999999999447, 225.59499999999923), (-8.79999999999447, 225.27499999999924), (-0.300000000005367, 224.88), (-0.300000000005367, 224.76), (-10.831, 225.47716999999963), (-10.831, 225.2171699999996), (-10.831, 225.47716999999963), (-10.831, 225.2171699999996), (-8.79999999999447, 225.27499999999924), (-8.79999999999447, 224.95499999999925)]</t>
+          <t>[(-25340.659385937506, 66187.9120908327), (-25340.659385937506, 66187.7920908327), (-25351.190385937498, 66188.6492608327), (-25351.190385937498, 66188.3892608327), (-25351.190385937498, 66188.6492608327), (-25351.190385937498, 66188.3892608327), (-25349.159385937495, 66188.5070908327), (-25349.159385937495, 66188.1870908327), (-25340.659385937506, 66187.7920908327), (-25340.659385937506, 66187.6720908327), (-25351.190385937498, 66188.3892608327), (-25351.190385937498, 66188.12926083269), (-25351.190385937498, 66188.3892608327), (-25351.190385937498, 66188.12926083269), (-25349.159385937495, 66188.1870908327), (-25349.159385937495, 66187.8670908327)]</t>
         </is>
       </c>
     </row>
@@ -2687,7 +2687,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>[(-0.299999999999419, 226.0), (-0.299999999999419, 225.88), (-8.479, 226.57253000000003), (-8.479, 226.45253000000002), (-8.479, 226.57253000000003), (-8.479, 226.36253000000002), (-8.80000000000446, 226.59500000000034), (-8.80000000000446, 226.27500000000035), (-0.299999999999419, 225.88), (-0.299999999999419, 225.75), (-8.479, 226.45253000000002), (-8.479, 226.15253000000004), (-8.479, 226.36253000000002), (-8.479, 226.15253000000004), (-8.80000000000446, 226.27500000000035), (-8.80000000000446, 225.95500000000035)]</t>
+          <t>[(-25272.6593859375, 66188.0779151853), (-25272.6593859375, 66187.95791518531), (-25280.8383859375, 66188.65044518531), (-25280.8383859375, 66188.53044518532), (-25280.8383859375, 66188.65044518531), (-25280.8383859375, 66188.4404451853), (-25281.159385937503, 66188.6729151853), (-25281.159385937503, 66188.3529151853), (-25272.6593859375, 66187.95791518531), (-25272.6593859375, 66187.8279151853), (-25280.8383859375, 66188.53044518532), (-25280.8383859375, 66188.23044518531), (-25280.8383859375, 66188.4404451853), (-25280.8383859375, 66188.23044518531), (-25281.159385937503, 66188.3529151853), (-25281.159385937503, 66188.03291518531)]</t>
         </is>
       </c>
     </row>
@@ -2697,7 +2697,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>[(-0.300000000001498, 227.0), (-0.300000000001498, 226.88), (-7.374, 227.4951799999999), (-7.374, 227.3751799999999), (-7.374, 227.4951799999999), (-7.374, 227.31517999999988), (-8.80000000000615, 227.5950000000003), (-8.80000000000615, 227.27500000000032), (-0.300000000001498, 226.88), (-0.300000000001498, 226.75), (-7.374, 227.3751799999999), (-7.374, 227.1251799999999), (-7.374, 227.31517999999988), (-7.374, 227.13517999999988), (-8.80000000000615, 227.27500000000032), (-8.80000000000615, 226.95500000000033)]</t>
+          <t>[(-25152.459385937604, 66188.243739538), (-25152.459385937604, 66188.123739538), (-25159.5333859376, 66188.738919538), (-25159.5333859376, 66188.618919538), (-25159.5333859376, 66188.738919538), (-25159.5333859376, 66188.558919538), (-25160.959385937607, 66188.838739538), (-25160.959385937607, 66188.51873953799), (-25152.459385937604, 66188.123739538), (-25152.459385937604, 66187.993739538), (-25159.5333859376, 66188.618919538), (-25159.5333859376, 66188.368919538), (-25159.5333859376, 66188.558919538), (-25159.5333859376, 66188.378919538), (-25160.959385937607, 66188.51873953799), (-25160.959385937607, 66188.198739538)]</t>
         </is>
       </c>
     </row>
@@ -2717,7 +2717,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>[(-0.299999999993343, 229.0), (-0.299999999993343, 228.87), (-5.372, 229.2746730974566), (-5.372, 229.1446730974566), (-5.372, 229.2746730974566), (-5.372, 229.1546730974566), (-8.80000000000548, 229.46031571931812), (-8.80000000000548, 229.20031571931813), (-0.299999999993343, 228.87), (-0.299999999993343, 228.75), (-5.372, 229.1446730974566), (-5.372, 229.0246730974566), (-5.372, 229.1546730974566), (-5.372, 229.0346730974566), (-8.80000000000548, 229.20031571931813), (-8.80000000000548, 228.9403157193181)]</t>
+          <t>[(-24965.25938593769, 66188.5753882432), (-24965.25938593769, 66188.4453882432), (-24970.331385937698, 66188.85006134066), (-24970.331385937698, 66188.72006134066), (-24970.331385937698, 66188.85006134066), (-24970.331385937698, 66188.73006134067), (-24973.759385937705, 66189.03570396252), (-24973.759385937705, 66188.77570396253), (-24965.25938593769, 66188.4453882432), (-24965.25938593769, 66188.3253882432), (-24970.331385937698, 66188.72006134066), (-24970.331385937698, 66188.60006134066), (-24970.331385937698, 66188.73006134067), (-24970.331385937698, 66188.61006134066), (-24973.759385937705, 66188.77570396253), (-24973.759385937705, 66188.51570396252)]</t>
         </is>
       </c>
     </row>
@@ -2747,7 +2747,7 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>[(-0.300000000016519, 232.0), (-0.300000000016519, 231.87), (-6.473, 232.18238384993), (-6.473, 232.05238384993), (-6.473, 232.18238384993), (-6.473, 232.06238384993), (-8.80000000000638, 232.25113603181717), (-8.80000000000638, 231.97113603181717), (-0.300000000016519, 231.87), (-0.300000000016519, 231.75), (-6.473, 232.05238384993), (-6.473, 231.93238384993), (-6.473, 232.06238384993), (-6.473, 231.94238384993), (-8.80000000000638, 231.97113603181717), (-8.80000000000638, 231.69113603181717)]</t>
+          <t>[(-24699.05938593752, 66193.0728613011), (-24699.05938593752, 66192.9428613011), (-24705.232385937503, 66193.25524515103), (-24705.232385937503, 66193.12524515102), (-24705.232385937503, 66193.25524515103), (-24705.232385937503, 66193.13524515103), (-24707.559385937508, 66193.32399733292), (-24707.559385937508, 66193.04399733292), (-24699.05938593752, 66192.9428613011), (-24699.05938593752, 66192.8228613011), (-24705.232385937503, 66193.12524515102), (-24705.232385937503, 66193.00524515103), (-24705.232385937503, 66193.13524515103), (-24705.232385937503, 66193.01524515102), (-24707.559385937508, 66193.04399733292), (-24707.559385937508, 66192.76399733292)]</t>
         </is>
       </c>
     </row>
@@ -2757,7 +2757,7 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>[(-0.300000000004104, 233.0), (-0.300000000004104, 232.87), (-6.598, 233.07055554636702), (-6.598, 232.94055554636702), (-6.598, 233.07055554636702), (-6.598, 232.950555546367), (-8.80000000000538, 233.09522422104163), (-8.80000000000538, 232.85522422104162), (-0.300000000004104, 232.87), (-0.300000000004104, 232.75), (-6.598, 232.94055554636702), (-6.598, 232.82055554636702), (-6.598, 232.950555546367), (-6.598, 232.830555546367), (-8.80000000000538, 232.85522422104162), (-8.80000000000538, 232.61522422104164)]</t>
+          <t>[(-24587.859385937503, 66191.2386856537), (-24587.859385937503, 66191.1086856537), (-24594.157385937502, 66191.30924120007), (-24594.157385937502, 66191.17924120007), (-24594.157385937502, 66191.30924120007), (-24594.157385937502, 66191.18924120007), (-24596.359385937507, 66191.33390987475), (-24596.359385937507, 66191.09390987475), (-24587.859385937503, 66191.1086856537), (-24587.859385937503, 66190.9886856537), (-24594.157385937502, 66191.17924120007), (-24594.157385937502, 66191.05924120007), (-24594.157385937502, 66191.18924120007), (-24594.157385937502, 66191.06924120006), (-24596.359385937507, 66191.09390987475), (-24596.359385937507, 66190.85390987476)]</t>
         </is>
       </c>
     </row>
@@ -2767,7 +2767,7 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>[(-0.300000000002969, 234.0), (-0.300000000002969, 233.87), (-6.694, 233.87378279755276), (-6.694, 233.74378279755277), (-6.694, 233.87378279755276), (-6.694, 233.74378279755277), (-8.80000000000424, 233.83221047532027), (-8.80000000000424, 233.70221047532027), (-0.300000000002969, 233.87), (-0.300000000002969, 233.75), (-6.694, 233.74378279755277), (-6.694, 233.62378279755276), (-6.694, 233.74378279755277), (-6.694, 233.62378279755276), (-8.80000000000424, 233.70221047532027), (-8.80000000000424, 233.58221047532027)]</t>
+          <t>[(-24587.8593859376, 66235.4045100064), (-24587.8593859376, 66235.27451000639), (-24594.253385937598, 66235.27829280395), (-24594.253385937598, 66235.14829280395), (-24594.253385937598, 66235.27829280395), (-24594.253385937598, 66235.14829280395), (-24596.3593859376, 66235.23672048171), (-24596.3593859376, 66235.10672048171), (-24587.8593859376, 66235.27451000639), (-24587.8593859376, 66235.1545100064), (-24594.253385937598, 66235.14829280395), (-24594.253385937598, 66235.02829280395), (-24594.253385937598, 66235.14829280395), (-24594.253385937598, 66235.02829280395), (-24596.3593859376, 66235.10672048171), (-24596.3593859376, 66234.98672048171)]</t>
         </is>
       </c>
     </row>
@@ -2777,7 +2777,7 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>[(-0.300000000074902, 235.0), (-0.300000000074902, 234.87), (-5.066, 234.79777791165498), (-5.066, 234.66777791165498), (-5.066, 234.79777791165498), (-5.066, 234.66777791165498), (-8.80000000002093, 234.63934373668718), (-8.80000000002093, 234.50934373668719), (-0.300000000074902, 234.87), (-0.300000000074902, 234.75), (-5.066, 234.66777791165498), (-5.066, 234.54777791165498), (-5.066, 234.66777791165498), (-5.066, 234.54777791165498), (-8.80000000002093, 234.50934373668719), (-8.80000000002093, 234.38934373668718)]</t>
+          <t>[(-24400.659385937575, 66189.570334359), (-24400.659385937575, 66189.440334359), (-24405.4253859375, 66189.36811227065), (-24405.4253859375, 66189.23811227064), (-24405.4253859375, 66189.36811227065), (-24405.4253859375, 66189.23811227064), (-24409.15938593752, 66189.20967809569), (-24409.15938593752, 66189.07967809569), (-24400.659385937575, 66189.440334359), (-24400.659385937575, 66189.320334359), (-24405.4253859375, 66189.23811227064), (-24405.4253859375, 66189.11811227065), (-24405.4253859375, 66189.23811227064), (-24405.4253859375, 66189.11811227065), (-24409.15938593752, 66189.07967809569), (-24409.15938593752, 66188.95967809569)]</t>
         </is>
       </c>
     </row>
@@ -2787,7 +2787,7 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>[(-0.300000000114203, 236.0), (-0.300000000114203, 235.87), (-6.433, 235.61098289848823), (-6.433, 235.48098289848824), (-6.433, 235.61098289848823), (-6.433, 235.48098289848824), (-8.8000000000206, 235.46084373669083), (-8.8000000000206, 235.33084373669084), (-0.300000000114203, 235.87), (-0.300000000114203, 235.75), (-6.433, 235.48098289848824), (-6.433, 235.36098289848823), (-6.433, 235.48098289848824), (-6.433, 235.36098289848823), (-8.8000000000206, 235.33084373669084), (-8.8000000000206, 235.21084373669083)]</t>
+          <t>[(-24400.659385937615, 66249.7361587116), (-24400.659385937615, 66249.6061587116), (-24406.7923859375, 66249.3471416101), (-24406.7923859375, 66249.21714161009), (-24406.7923859375, 66249.3471416101), (-24406.7923859375, 66249.21714161009), (-24409.15938593752, 66249.19700244829), (-24409.15938593752, 66249.06700244828), (-24400.659385937615, 66249.6061587116), (-24400.659385937615, 66249.4861587116), (-24406.7923859375, 66249.21714161009), (-24406.7923859375, 66249.0971416101), (-24406.7923859375, 66249.21714161009), (-24406.7923859375, 66249.0971416101), (-24409.15938593752, 66249.06700244828), (-24409.15938593752, 66248.94700244829)]</t>
         </is>
       </c>
     </row>
@@ -2797,7 +2797,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>[(-0.300000000005366, 237.0), (-0.300000000005366, 236.87), (-5.622, 236.62746000000038), (-5.622, 236.4974600000004), (-5.622, 236.62746000000038), (-5.622, 236.4974600000004), (-8.79999999999814, 236.4050000000005), (-8.79999999999814, 236.27500000000052), (-0.300000000005366, 236.87), (-0.300000000005366, 236.75), (-5.622, 236.4974600000004), (-5.622, 236.37746000000038), (-5.622, 236.4974600000004), (-5.622, 236.37746000000038), (-8.79999999999814, 236.27500000000052), (-8.79999999999814, 236.1550000000005)]</t>
+          <t>[(-24322.659385937608, 66189.90198306431), (-24322.659385937608, 66189.7719830643), (-24327.9813859376, 66189.52944306431), (-24327.9813859376, 66189.3994430643), (-24327.9813859376, 66189.52944306431), (-24327.9813859376, 66189.3994430643), (-24331.1593859376, 66189.3069830643), (-24331.1593859376, 66189.1769830643), (-24322.659385937608, 66189.7719830643), (-24322.659385937608, 66189.65198306431), (-24327.9813859376, 66189.3994430643), (-24327.9813859376, 66189.27944306431), (-24327.9813859376, 66189.3994430643), (-24327.9813859376, 66189.27944306431), (-24331.1593859376, 66189.1769830643), (-24331.1593859376, 66189.0569830643)]</t>
         </is>
       </c>
     </row>
@@ -2807,7 +2807,7 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>[(-0.299999999999214, 238.0), (-0.299999999999214, 237.87), (-4.904, 237.67771999999994), (-4.904, 237.54771999999994), (-4.904, 237.67771999999994), (-4.904, 237.54771999999994), (-8.564, 237.42151999999996), (-8.564, 237.29151999999996), (-0.299999999999214, 237.87), (-0.299999999999214, 237.75), (-4.904, 237.54771999999994), (-4.904, 237.42771999999994), (-4.904, 237.54771999999994), (-4.904, 237.42771999999994), (-8.564, 237.29151999999996), (-8.564, 237.17151999999996)]</t>
+          <t>[(-24322.6593859376, 66250.0678074169), (-24322.6593859376, 66249.93780741689), (-24327.2633859376, 66249.7455274169), (-24327.2633859376, 66249.6155274169), (-24327.2633859376, 66249.7455274169), (-24327.2633859376, 66249.6155274169), (-24330.9233859376, 66249.4893274169), (-24330.9233859376, 66249.3593274169), (-24322.6593859376, 66249.93780741689), (-24322.6593859376, 66249.8178074169), (-24327.2633859376, 66249.6155274169), (-24327.2633859376, 66249.4955274169), (-24327.2633859376, 66249.6155274169), (-24327.2633859376, 66249.4955274169), (-24330.9233859376, 66249.3593274169), (-24330.9233859376, 66249.2393274169)]</t>
         </is>
       </c>
     </row>
@@ -2817,7 +2817,7 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>[(-0.300000000003921, 239.0), (-0.300000000003921, 238.87), (-4.102, 238.73386000000028), (-4.102, 238.60386000000028), (-4.102, 238.73386000000028), (-4.102, 238.60386000000028), (-7.913, 238.46709000000027), (-7.913, 238.33709000000027), (-0.300000000003921, 238.87), (-0.300000000003921, 238.75), (-4.102, 238.60386000000028), (-4.102, 238.48386000000028), (-4.102, 238.60386000000028), (-4.102, 238.48386000000028), (-7.913, 238.33709000000027), (-7.913, 238.21709000000027)]</t>
+          <t>[(-24212.459385937604, 66190.2336317695), (-24212.459385937604, 66190.1036317695), (-24216.2613859376, 66189.9674917695), (-24216.2613859376, 66189.83749176949), (-24216.2613859376, 66189.9674917695), (-24216.2613859376, 66189.83749176949), (-24220.0723859376, 66189.7007217695), (-24220.0723859376, 66189.5707217695), (-24212.459385937604, 66190.1036317695), (-24212.459385937604, 66189.9836317695), (-24216.2613859376, 66189.83749176949), (-24216.2613859376, 66189.7174917695), (-24216.2613859376, 66189.83749176949), (-24216.2613859376, 66189.7174917695), (-24220.0723859376, 66189.5707217695), (-24220.0723859376, 66189.4507217695)]</t>
         </is>
       </c>
     </row>
@@ -2827,7 +2827,7 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>[(-0.2999999999998, 240.0), (-0.2999999999998, 239.87), (-3.709, 239.76137), (-3.709, 239.63137), (-3.709, 239.76137), (-3.709, 239.63137), (-7.59, 239.4897), (-7.59, 239.3597), (-0.2999999999998, 239.87), (-0.2999999999998, 239.75), (-3.709, 239.63137), (-3.709, 239.51137), (-3.709, 239.63137), (-3.709, 239.51137), (-7.59, 239.3597), (-7.59, 239.2397)]</t>
+          <t>[(-24212.4593859376, 66240.3994561221), (-24212.4593859376, 66240.2694561221), (-24215.8683859376, 66240.1608261221), (-24215.8683859376, 66240.03082612209), (-24215.8683859376, 66240.1608261221), (-24215.8683859376, 66240.03082612209), (-24219.7493859376, 66239.88915612211), (-24219.7493859376, 66239.7591561221), (-24212.4593859376, 66240.2694561221), (-24212.4593859376, 66240.1494561221), (-24215.8683859376, 66240.03082612209), (-24215.8683859376, 66239.9108261221), (-24215.8683859376, 66240.03082612209), (-24215.8683859376, 66239.9108261221), (-24219.7493859376, 66239.7591561221), (-24219.7493859376, 66239.63915612211)]</t>
         </is>
       </c>
     </row>
@@ -2837,7 +2837,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>[(-0.299999999990775, 241.0), (-0.299999999990775, 240.87), (-3.488, 240.84073776727507), (-3.488, 240.71073776727508), (-3.488, 240.84073776727507), (-3.488, 240.71073776727508), (-7.284, 240.65110180886163), (-7.284, 240.52110180886163), (-0.299999999990775, 240.87), (-0.299999999990775, 240.75), (-3.488, 240.71073776727508), (-3.488, 240.59073776727507), (-3.488, 240.71073776727508), (-3.488, 240.59073776727507), (-7.284, 240.52110180886163), (-7.284, 240.40110180886163)]</t>
+          <t>[(-24023.259385937494, 66192.5652804748), (-24023.259385937494, 66192.43528047479), (-24026.447385937503, 66192.40601824207), (-24026.447385937503, 66192.27601824206), (-24026.447385937503, 66192.40601824207), (-24026.447385937503, 66192.27601824206), (-24030.2433859375, 66192.21638228366), (-24030.2433859375, 66192.08638228365), (-24023.259385937494, 66192.43528047479), (-24023.259385937494, 66192.3152804748), (-24026.447385937503, 66192.27601824206), (-24026.447385937503, 66192.15601824207), (-24026.447385937503, 66192.27601824206), (-24026.447385937503, 66192.15601824207), (-24030.2433859375, 66192.08638228365), (-24030.2433859375, 66191.96638228366)]</t>
         </is>
       </c>
     </row>
@@ -2847,7 +2847,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>[(-0.300000000139077, 242.0), (-0.300000000139077, 241.87), (-3.388, 241.91058144584682), (-3.388, 241.78058144584682), (-3.388, 241.91058144584682), (-3.388, 241.78058144584682), (-7.389, 241.79472534637043), (-7.389, 241.66472534637043), (-0.300000000139077, 241.87), (-0.300000000139077, 241.75), (-3.388, 241.78058144584682), (-3.388, 241.66058144584682), (-3.388, 241.78058144584682), (-3.388, 241.66058144584682), (-7.389, 241.66472534637043), (-7.389, 241.54472534637043)]</t>
+          <t>[(-24023.259385937738, 66246.7311048274), (-24023.259385937738, 66246.6011048274), (-24026.3473859376, 66246.64168627324), (-24026.3473859376, 66246.51168627324), (-24026.3473859376, 66246.64168627324), (-24026.3473859376, 66246.51168627324), (-24030.3483859376, 66246.52583017376), (-24030.3483859376, 66246.39583017376), (-24023.259385937738, 66246.6011048274), (-24023.259385937738, 66246.4811048274), (-24026.3473859376, 66246.51168627324), (-24026.3473859376, 66246.39168627324), (-24026.3473859376, 66246.51168627324), (-24026.3473859376, 66246.39168627324), (-24030.3483859376, 66246.39583017376), (-24030.3483859376, 66246.27583017376)]</t>
         </is>
       </c>
     </row>
@@ -2857,7 +2857,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>[(-0.29999999999459, 243.0), (-0.29999999999459, 242.85), (-3.224, 242.97603312978833), (-3.224, 242.82603312978833), (-3.224, 242.97603312978833), (-3.224, 242.82603312978833), (-8.79999999999426, 242.93032886566385), (-8.79999999999426, 242.67032886566386), (-0.29999999999459, 242.85), (-0.29999999999459, 242.71), (-3.224, 242.82603312978833), (-3.224, 242.67603312978832), (-3.224, 242.82603312978833), (-3.224, 242.67603312978832), (-8.79999999999426, 242.67032886566386), (-8.79999999999426, 242.41032886566384)]</t>
+          <t>[(-23954.259385937497, 66192.89692918), (-23954.259385937497, 66192.74692918001), (-23957.1833859375, 66192.87296230979), (-23957.1833859375, 66192.7229623098), (-23957.1833859375, 66192.87296230979), (-23957.1833859375, 66192.7229623098), (-23962.759385937497, 66192.82725804567), (-23962.759385937497, 66192.56725804567), (-23954.259385937497, 66192.74692918001), (-23954.259385937497, 66192.60692918001), (-23957.1833859375, 66192.7229623098), (-23957.1833859375, 66192.57296230979), (-23957.1833859375, 66192.7229623098), (-23957.1833859375, 66192.57296230979), (-23962.759385937497, 66192.56725804567), (-23962.759385937497, 66192.30725804566)]</t>
         </is>
       </c>
     </row>
@@ -2867,7 +2867,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>[(-0.299999999994472, 244.0), (-0.299999999994472, 243.83), (-3.053, 244.03443425116868), (-3.053, 243.8644342511687), (-3.053, 244.03443425116868), (-3.053, 243.8644342511687), (-8.79999999999426, 244.1063171576219), (-8.79999999999426, 243.7663171576219), (-0.299999999994472, 243.83), (-0.299999999994472, 243.67), (-3.053, 243.8644342511687), (-3.053, 243.69443425116867), (-3.053, 243.8644342511687), (-3.053, 243.69443425116867), (-8.79999999999426, 243.7663171576219), (-8.79999999999426, 243.4263171576219)]</t>
+          <t>[(-23954.259385937596, 66245.06275353271), (-23954.259385937596, 66244.89275353271), (-23957.0123859376, 66245.09718778387), (-23957.0123859376, 66244.92718778388), (-23957.0123859376, 66245.09718778387), (-23957.0123859376, 66244.92718778388), (-23962.759385937596, 66245.16907069033), (-23962.759385937596, 66244.82907069034), (-23954.259385937596, 66244.89275353271), (-23954.259385937596, 66244.7327535327), (-23957.0123859376, 66244.92718778388), (-23957.0123859376, 66244.75718778388), (-23957.0123859376, 66244.92718778388), (-23957.0123859376, 66244.75718778388), (-23962.759385937596, 66244.82907069034), (-23962.759385937596, 66244.48907069034)]</t>
         </is>
       </c>
     </row>
@@ -2877,7 +2877,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>[(-0.299999999987999, 245.0), (-0.299999999987999, 244.83), (-2.817, 245.07782404970587), (-2.817, 244.90782404970588), (-2.817, 245.07782404970587), (-2.817, 244.90782404970588), (-8.79999999998336, 245.26281462951783), (-8.79999999998336, 244.91281462951784), (-0.299999999987999, 244.83), (-0.299999999987999, 244.69), (-2.817, 244.90782404970588), (-2.817, 244.73782404970586), (-2.817, 244.90782404970588), (-2.817, 244.73782404970586), (-8.79999999998336, 244.91281462951784), (-8.79999999998336, 244.56281462951785)]</t>
+          <t>[(-23834.05938593769, 66191.2285778853), (-23834.05938593769, 66191.0585778853), (-23836.5763859377, 66191.306401935), (-23836.5763859377, 66191.136401935), (-23836.5763859377, 66191.306401935), (-23836.5763859377, 66191.136401935), (-23842.559385937686, 66191.49139251481), (-23842.559385937686, 66191.14139251481), (-23834.05938593769, 66191.0585778853), (-23834.05938593769, 66190.9185778853), (-23836.5763859377, 66191.136401935), (-23836.5763859377, 66190.966401935), (-23836.5763859377, 66191.136401935), (-23836.5763859377, 66190.966401935), (-23842.559385937686, 66191.14139251481), (-23842.559385937686, 66190.79139251482)]</t>
         </is>
       </c>
     </row>
@@ -2887,7 +2887,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>[(-0.300000000015845, 246.0), (-0.300000000015845, 245.88), (-2.868, 246.11772440706517), (-2.868, 245.99772440706516), (-2.868, 246.11772440706517), (-2.868, 245.95772440706517), (-8.8000000000035, 246.38966411996054), (-8.8000000000035, 246.05966411996053), (-0.300000000015845, 245.88), (-0.300000000015845, 245.73), (-2.868, 245.99772440706516), (-2.868, 245.79772440706518), (-2.868, 245.95772440706517), (-2.868, 245.79772440706518), (-8.8000000000035, 246.05966411996053), (-8.8000000000035, 245.72966411996055)]</t>
+          <t>[(-23834.05938593752, 66247.3944022379), (-23834.05938593752, 66247.2744022379), (-23836.6273859375, 66247.51212664497), (-23836.6273859375, 66247.39212664498), (-23836.6273859375, 66247.51212664497), (-23836.6273859375, 66247.35212664497), (-23842.559385937504, 66247.78406635785), (-23842.559385937504, 66247.45406635785), (-23834.05938593752, 66247.2744022379), (-23834.05938593752, 66247.1244022379), (-23836.6273859375, 66247.39212664498), (-23836.6273859375, 66247.19212664496), (-23836.6273859375, 66247.35212664497), (-23836.6273859375, 66247.19212664496), (-23842.559385937504, 66247.45406635785), (-23842.559385937504, 66247.12406635785)]</t>
         </is>
       </c>
     </row>
@@ -2927,7 +2927,7 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>[(-0.29999999999852, 250.0), (-0.29999999999852, 249.88), (-3.599, 250.23093000000011), (-3.599, 250.1109300000001), (-3.599, 250.23093000000011), (-3.599, 250.0209300000001), (-7.357, 250.4939900000001), (-7.357, 250.2839900000001), (-0.29999999999852, 249.88), (-0.29999999999852, 249.74), (-3.599, 250.1109300000001), (-3.599, 249.9009300000001), (-3.599, 250.0209300000001), (-3.599, 249.9009300000001), (-7.357, 250.2839900000001), (-7.357, 250.0839900000001)]</t>
+          <t>[(-23645.8593859375, 66236.1161689523), (-23645.8593859375, 66235.9961689523), (-23649.1583859375, 66236.3470989523), (-23649.1583859375, 66236.22709895231), (-23649.1583859375, 66236.3470989523), (-23649.1583859375, 66236.1370989523), (-23652.9163859375, 66236.6101589523), (-23652.9163859375, 66236.4001589523), (-23645.8593859375, 66235.9961689523), (-23645.8593859375, 66235.8561689523), (-23649.1583859375, 66236.22709895231), (-23649.1583859375, 66236.0170989523), (-23649.1583859375, 66236.1370989523), (-23649.1583859375, 66236.0170989523), (-23652.9163859375, 66236.4001589523), (-23652.9163859375, 66236.2001589523)]</t>
         </is>
       </c>
     </row>
@@ -2937,7 +2937,7 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>[(-0.299999999993185, 251.0), (-0.299999999993185, 250.79), (-3.931, 251.25417000000047), (-3.931, 251.04417000000046), (-3.931, 251.25417000000047), (-3.931, 251.04417000000046), (-8.80000000000373, 251.59500000000074), (-8.80000000000373, 251.23500000000072), (-0.299999999993185, 250.79), (-0.299999999993185, 250.63), (-3.931, 251.04417000000046), (-3.931, 250.83417000000048), (-3.931, 251.04417000000046), (-3.931, 250.83417000000048), (-8.80000000000373, 251.23500000000072), (-8.80000000000373, 250.87500000000074)]</t>
+          <t>[(-23585.859385937492, 66186.4818981399), (-23585.859385937492, 66186.2718981399), (-23589.4903859375, 66186.7360681399), (-23589.4903859375, 66186.5260681399), (-23589.4903859375, 66186.7360681399), (-23589.4903859375, 66186.5260681399), (-23594.359385937503, 66187.0768981399), (-23594.359385937503, 66186.7168981399), (-23585.859385937492, 66186.2718981399), (-23585.859385937492, 66186.1118981399), (-23589.4903859375, 66186.5260681399), (-23589.4903859375, 66186.3160681399), (-23589.4903859375, 66186.5260681399), (-23589.4903859375, 66186.3160681399), (-23594.359385937503, 66186.7168981399), (-23594.359385937503, 66186.3568981399)]</t>
         </is>
       </c>
     </row>
@@ -2947,7 +2947,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>[(-0.300000000064306, 252.0), (-0.300000000064306, 251.85), (-4.19, 252.2017708578024), (-4.19, 252.05177085780238), (-4.19, 252.2017708578024), (-4.19, 252.05177085780238), (-7.959, 252.3972655526789), (-7.959, 252.2472655526789), (-0.300000000064306, 251.85), (-0.300000000064306, 251.7), (-4.19, 252.05177085780238), (-4.19, 251.90177085780238), (-4.19, 252.05177085780238), (-4.19, 251.90177085780238), (-7.959, 252.2472655526789), (-7.959, 252.0972655526789), (-0.300000000064306, 251.7), (-0.300000000064306, 251.55), (-4.19, 251.90177085780238), (-4.19, 251.7617708578024), (-4.19, 251.90177085780238), (-4.19, 251.7617708578024), (-7.959, 252.0972655526789), (-7.959, 251.9572655526789)]</t>
+          <t>[(-23590.859385937663, 66236.989672782), (-23590.859385937663, 66236.839672782), (-23594.749385937597, 66237.19144363981), (-23594.749385937597, 66237.04144363981), (-23594.749385937597, 66237.19144363981), (-23594.749385937597, 66237.04144363981), (-23598.518385937597, 66237.38693833468), (-23598.518385937597, 66237.23693833468), (-23590.859385937663, 66236.839672782), (-23590.859385937663, 66236.689672782), (-23594.749385937597, 66237.04144363981), (-23594.749385937597, 66236.8914436398), (-23594.749385937597, 66237.04144363981), (-23594.749385937597, 66236.8914436398), (-23598.518385937597, 66237.23693833468), (-23598.518385937597, 66237.08693833467), (-23590.859385937663, 66236.689672782), (-23590.859385937663, 66236.539672782), (-23594.749385937597, 66236.8914436398), (-23594.749385937597, 66236.7514436398), (-23594.749385937597, 66236.8914436398), (-23594.749385937597, 66236.7514436398), (-23598.518385937597, 66237.08693833467), (-23598.518385937597, 66236.94693833467)]</t>
         </is>
       </c>
     </row>
@@ -2957,7 +2957,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>[(-0.300000000150335, 253.0), (-0.300000000150335, 252.75), (-5.084, 253.15003449125732), (-5.084, 252.90003449125732), (-5.084, 253.15003449125732), (-5.084, 252.93003449125732), (-8.80000000000522, 253.26657466047354), (-8.80000000000522, 252.94657466047354), (-0.300000000150335, 252.75), (-0.300000000150335, 252.51), (-5.084, 252.90003449125732), (-5.084, 252.70003449125733), (-5.084, 252.93003449125732), (-5.084, 252.71003449125732), (-8.80000000000522, 252.94657466047354), (-8.80000000000522, 252.62657466047355)]</t>
+          <t>[(-23459.159385937754, 66187.6394928787), (-23459.159385937754, 66187.3894928787), (-23463.9433859376, 66187.78952736997), (-23463.9433859376, 66187.53952736997), (-23463.9433859376, 66187.78952736997), (-23463.9433859376, 66187.56952736997), (-23467.659385937608, 66187.90606753918), (-23467.659385937608, 66187.58606753917), (-23459.159385937754, 66187.3894928787), (-23459.159385937754, 66187.1494928787), (-23463.9433859376, 66187.53952736997), (-23463.9433859376, 66187.33952736997), (-23463.9433859376, 66187.56952736997), (-23463.9433859376, 66187.34952736997), (-23467.659385937608, 66187.58606753917), (-23467.659385937608, 66187.26606753918)]</t>
         </is>
       </c>
     </row>
@@ -2967,7 +2967,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>[(-0.300000000068302, 254.0), (-0.300000000068302, 253.79), (-5.837, 254.0601004496114), (-5.837, 253.8501004496114), (-5.837, 254.0601004496114), (-5.837, 253.8201004496114), (-8.80000000000395, 254.09226184245972), (-8.80000000000395, 253.8522618424597), (-0.300000000068302, 253.79), (-0.300000000068302, 253.59), (-5.837, 253.8501004496114), (-5.837, 253.7001004496114), (-5.837, 253.8201004496114), (-5.837, 253.7001004496114), (-8.80000000000395, 253.8522618424597), (-8.80000000000395, 253.55226184245973)]</t>
+          <t>[(-23459.15938593767, 66226.4313584299), (-23459.15938593767, 66226.22135842989), (-23464.6963859376, 66226.4914588795), (-23464.6963859376, 66226.2814588795), (-23464.6963859376, 66226.4914588795), (-23464.6963859376, 66226.2514588795), (-23467.659385937604, 66226.52362027236), (-23467.659385937604, 66226.28362027236), (-23459.15938593767, 66226.22135842989), (-23459.15938593767, 66226.02135842989), (-23464.6963859376, 66226.2814588795), (-23464.6963859376, 66226.1314588795), (-23464.6963859376, 66226.2514588795), (-23464.6963859376, 66226.1314588795), (-23467.659385937604, 66226.28362027236), (-23467.659385937604, 66225.98362027237)]</t>
         </is>
       </c>
     </row>
@@ -2977,7 +2977,7 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>[(-0.300000000038982, 255.0), (-0.300000000038982, 254.84), (-6.327, 254.9715525250222), (-6.327, 254.8115525250222), (-6.327, 254.9715525250222), (-6.327, 254.8115525250222), (-8.79999999999696, 254.95987995067003), (-8.79999999999696, 254.79987995067003), (-0.300000000038982, 254.84), (-0.300000000038982, 254.69), (-6.327, 254.8115525250222), (-6.327, 254.6915525250222), (-6.327, 254.8115525250222), (-6.327, 254.6915525250222), (-8.79999999999696, 254.79987995067003), (-8.79999999999696, 254.49987995067002)]</t>
+          <t>[(-23271.459385937538, 66195.3652694357), (-23271.459385937538, 66195.2052694357), (-23277.4863859375, 66195.33682196072), (-23277.4863859375, 66195.17682196072), (-23277.4863859375, 66195.33682196072), (-23277.4863859375, 66195.17682196072), (-23279.959385937495, 66195.32514938636), (-23279.959385937495, 66195.16514938636), (-23271.459385937538, 66195.2052694357), (-23271.459385937538, 66195.0552694357), (-23277.4863859375, 66195.17682196072), (-23277.4863859375, 66195.05682196072), (-23277.4863859375, 66195.17682196072), (-23277.4863859375, 66195.05682196072), (-23279.959385937495, 66195.16514938636), (-23279.959385937495, 66194.86514938636)]</t>
         </is>
       </c>
     </row>
@@ -2987,7 +2987,7 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>[(-0.300000000096326, 256.0), (-0.300000000096326, 255.84), (-3.081, 255.9589874793623), (-3.081, 255.7989874793623), (-3.081, 255.9589874793623), (-3.081, 255.7689874793623), (-8.80000000001001, 255.87464709621395), (-8.80000000001001, 255.68464709621395), (-0.300000000096326, 255.84), (-0.300000000096326, 255.69), (-3.081, 255.7989874793623), (-3.081, 255.6389874793623), (-3.081, 255.7689874793623), (-3.081, 255.6389874793623), (-8.80000000001001, 255.68464709621395), (-8.80000000001001, 255.38464709621394)]</t>
+          <t>[(-23271.459385937596, 66242.44122589601), (-23271.459385937596, 66242.281225896), (-23274.240385937497, 66242.40021337537), (-23274.240385937497, 66242.24021337536), (-23274.240385937497, 66242.40021337537), (-23274.240385937497, 66242.21021337537), (-23279.95938593751, 66242.31587299221), (-23279.95938593751, 66242.12587299221), (-23271.459385937596, 66242.281225896), (-23271.459385937596, 66242.13122589601), (-23274.240385937497, 66242.24021337536), (-23274.240385937497, 66242.08021337536), (-23274.240385937497, 66242.21021337537), (-23274.240385937497, 66242.08021337536), (-23279.95938593751, 66242.12587299221), (-23279.95938593751, 66241.82587299221)]</t>
         </is>
       </c>
     </row>
@@ -2997,7 +2997,7 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>[(-0.300000000165304, 257.0), (-0.300000000165304, 256.86), (-3.301, 256.92565083994623), (-3.301, 256.78565083994624), (-3.301, 256.92565083994623), (-3.301, 256.6356508399462), (-8.80000000001827, 256.7894142417591), (-8.80000000001827, 256.4994142417591), (-0.300000000165304, 256.86), (-0.300000000165304, 256.72), (-3.301, 256.78565083994624), (-3.301, 256.64565083994626), (-3.301, 256.6356508399462), (-3.301, 256.5156508399462), (-8.80000000001827, 256.4994142417591), (-8.80000000001827, 256.20941424175913), (-0.300000000165304, 256.72), (-0.300000000165304, 256.59), (-3.301, 256.64565083994626), (-3.301, 256.5156508399462), (-3.301, 256.5156508399462), (-3.301, 256.5156508399462), (-8.80000000001827, 256.20941424175913), (-8.80000000001827, 256.20941424175913)]</t>
+          <t>[(-23191.459385937767, 66197.6592278109), (-23191.459385937767, 66197.5192278109), (-23194.4603859376, 66197.58487865084), (-23194.4603859376, 66197.44487865084), (-23194.4603859376, 66197.58487865084), (-23194.4603859376, 66197.29487865085), (-23199.95938593762, 66197.44864205267), (-23199.95938593762, 66197.15864205267), (-23191.459385937767, 66197.5192278109), (-23191.459385937767, 66197.3792278109), (-23194.4603859376, 66197.44487865084), (-23194.4603859376, 66197.30487865084), (-23194.4603859376, 66197.29487865085), (-23194.4603859376, 66197.17487865084), (-23199.95938593762, 66197.15864205267), (-23199.95938593762, 66196.86864205266), (-23191.459385937767, 66197.3792278109), (-23191.459385937767, 66197.2492278109), (-23194.4603859376, 66197.30487865084), (-23194.4603859376, 66197.17487865084), (-23194.4603859376, 66197.17487865084), (-23194.4603859376, 66197.17487865084), (-23199.95938593762, 66196.86864205266), (-23199.95938593762, 66196.86864205266)]</t>
         </is>
       </c>
     </row>
@@ -3007,7 +3007,7 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>[(-0.300000000095095, 258.0), (-0.300000000095095, 257.78), (-3.53, 257.88758892717664), (-3.53, 257.6675889271766), (-3.53, 257.88758892717664), (-3.53, 257.61758892717666), (-8.8000000000018, 257.7041813873015), (-8.8000000000018, 257.4341813873015), (-0.300000000095095, 257.78), (-0.300000000095095, 257.57), (-3.53, 257.6675889271766), (-3.53, 257.49758892717665), (-3.53, 257.61758892717666), (-3.53, 257.49758892717665), (-8.8000000000018, 257.4341813873015), (-8.8000000000018, 257.1641813873015)]</t>
+          <t>[(-23191.459385937593, 66245.0192751803), (-23191.459385937593, 66244.7992751803), (-23194.689385937498, 66244.90686410747), (-23194.689385937498, 66244.68686410747), (-23194.689385937498, 66244.90686410747), (-23194.689385937498, 66244.63686410747), (-23199.9593859375, 66244.7234565676), (-23199.9593859375, 66244.4534565676), (-23191.459385937593, 66244.7992751803), (-23191.459385937593, 66244.5892751803), (-23194.689385937498, 66244.68686410747), (-23194.689385937498, 66244.51686410747), (-23194.689385937498, 66244.63686410747), (-23194.689385937498, 66244.51686410747), (-23199.9593859375, 66244.4534565676), (-23199.9593859375, 66244.18345656761)]</t>
         </is>
       </c>
     </row>
@@ -3017,7 +3017,7 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>[(-0.300000000045387, 259.0), (-0.300000000045387, 258.8), (-3.934, 258.8370892903955), (-3.934, 258.6370892903955), (-3.934, 258.8370892903955), (-3.934, 258.5870892903955), (-8.80000000000685, 258.61894853284286), (-8.80000000000685, 258.36894853284286), (-0.300000000045387, 258.8), (-0.300000000045387, 258.6), (-3.934, 258.6370892903955), (-3.934, 258.4670892903955), (-3.934, 258.5870892903955), (-3.934, 258.4670892903955), (-8.80000000000685, 258.36894853284286), (-8.80000000000685, 258.11894853284286)]</t>
+          <t>[(-23081.259385937446, 66202.5213680042), (-23081.259385937446, 66202.32136800421), (-23084.8933859374, 66202.3584572946), (-23084.8933859374, 66202.1584572946), (-23084.8933859374, 66202.3584572946), (-23084.8933859374, 66202.1084572946), (-23089.759385937406, 66202.14031653704), (-23089.759385937406, 66201.89031653704), (-23081.259385937446, 66202.32136800421), (-23081.259385937446, 66202.12136800421), (-23084.8933859374, 66202.1584572946), (-23084.8933859374, 66201.9884572946), (-23084.8933859374, 66202.1084572946), (-23084.8933859374, 66201.9884572946), (-23089.759385937406, 66201.89031653704), (-23089.759385937406, 66201.64031653704)]</t>
         </is>
       </c>
     </row>
@@ -3027,7 +3027,7 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>[(-0.300000000020933, 260.0), (-0.300000000020933, 259.76), (-3.986, 259.79779717535683), (-3.986, 259.5577971753568), (-3.986, 259.79779717535683), (-3.986, 259.52779717535685), (-8.80000000000537, 259.5337156783848), (-8.80000000000537, 259.2637156783848), (-0.300000000020933, 259.76), (-0.300000000020933, 259.53), (-3.986, 259.5577971753568), (-3.986, 259.3777971753568), (-3.986, 259.52779717535685), (-3.986, 259.3777971753568), (-8.80000000000537, 259.2637156783848), (-8.80000000000537, 258.9937156783848)]</t>
+          <t>[(-23081.259385937523, 66254.1655062827), (-23081.259385937523, 66253.9255062827), (-23084.945385937503, 66253.96330345806), (-23084.945385937503, 66253.72330345806), (-23084.945385937503, 66253.96330345806), (-23084.945385937503, 66253.69330345806), (-23089.75938593751, 66253.69922196108), (-23089.75938593751, 66253.42922196108), (-23081.259385937523, 66253.9255062827), (-23081.259385937523, 66253.6955062827), (-23084.945385937503, 66253.72330345806), (-23084.945385937503, 66253.54330345806), (-23084.945385937503, 66253.69330345806), (-23084.945385937503, 66253.54330345806), (-23089.75938593751, 66253.42922196108), (-23089.75938593751, 66253.15922196109)]</t>
         </is>
       </c>
     </row>
@@ -3037,7 +3037,7 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>[(-0.300000000013218, 261.0), (-0.300000000013218, 260.71), (-3.802, 260.77277492345866), (-3.802, 260.48277492345863), (-3.802, 260.77277492345866), (-3.802, 260.47277492345864), (-8.80000000000589, 260.4484828239272), (-8.80000000000589, 260.14848282392717), (-0.300000000013218, 260.71), (-0.300000000013218, 260.42), (-3.802, 260.48277492345863), (-3.802, 260.26277492345866), (-3.802, 260.47277492345864), (-3.802, 260.26277492345866), (-8.80000000000589, 260.14848282392717), (-8.80000000000589, 259.8584828239272)]</t>
+          <t>[(-22893.059385937515, 66199.9516900158), (-22893.059385937515, 66199.66169001581), (-22896.5613859375, 66199.72446493927), (-22896.5613859375, 66199.43446493927), (-22896.5613859375, 66199.72446493927), (-22896.5613859375, 66199.42446493926), (-22901.559385937508, 66199.40017283973), (-22901.559385937508, 66199.10017283972), (-22893.059385937515, 66199.66169001581), (-22893.059385937515, 66199.3716900158), (-22896.5613859375, 66199.43446493927), (-22896.5613859375, 66199.21446493927), (-22896.5613859375, 66199.42446493926), (-22896.5613859375, 66199.21446493927), (-22901.559385937508, 66199.10017283972), (-22901.559385937508, 66198.81017283973)]</t>
         </is>
       </c>
     </row>
@@ -3047,7 +3047,7 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>[(-0.300000000003449, 262.0), (-0.300000000003449, 261.78), (-3.285, 261.79105000000027), (-3.285, 261.57105000000024), (-3.285, 261.79105000000027), (-3.285, 261.49105000000026), (-8.79999999999307, 261.4050000000007), (-8.79999999999307, 261.0550000000007), (-0.300000000003449, 261.78), (-0.300000000003449, 261.56), (-3.285, 261.57105000000024), (-3.285, 261.35105000000027), (-3.285, 261.49105000000026), (-3.285, 261.19105000000025), (-8.79999999999307, 261.0550000000007), (-8.79999999999307, 260.7050000000007), (-0.300000000003449, 261.56), (-0.300000000003449, 261.34), (-3.285, 261.35105000000027), (-3.285, 261.2010500000003), (-3.285, 261.19105000000025), (-3.285, 261.19105000000025), (-8.79999999999307, 260.7050000000007), (-8.79999999999307, 260.7050000000007)]</t>
+          <t>[(-22893.059385937602, 66251.8363156126), (-22893.059385937602, 66251.6163156126), (-22896.0443859376, 66251.6273656126), (-22896.0443859376, 66251.4073656126), (-22896.0443859376, 66251.6273656126), (-22896.0443859376, 66251.3273656126), (-22901.55938593759, 66251.2413156126), (-22901.55938593759, 66250.8913156126), (-22893.059385937602, 66251.6163156126), (-22893.059385937602, 66251.3963156126), (-22896.0443859376, 66251.4073656126), (-22896.0443859376, 66251.1873656126), (-22896.0443859376, 66251.3273656126), (-22896.0443859376, 66251.0273656126), (-22901.55938593759, 66250.8913156126), (-22901.55938593759, 66250.5413156126), (-22893.059385937602, 66251.3963156126), (-22893.059385937602, 66251.1763156126), (-22896.0443859376, 66251.1873656126), (-22896.0443859376, 66251.0373656126), (-22896.0443859376, 66251.0273656126), (-22896.0443859376, 66251.0273656126), (-22901.55938593759, 66250.5413156126), (-22901.55938593759, 66250.5413156126)]</t>
         </is>
       </c>
     </row>
@@ -3057,7 +3057,7 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>[(-0.300000000002442, 263.0), (-0.300000000002442, 262.83), (-2.798, 262.82514000000015), (-2.798, 262.65514000000013), (-2.798, 262.82514000000015), (-2.798, 262.57514000000015), (-8.80000000000119, 262.4050000000001), (-8.80000000000119, 262.1550000000001), (-0.300000000002442, 262.83), (-0.300000000002442, 262.66), (-2.798, 262.65514000000013), (-2.798, 262.4851400000002), (-2.798, 262.57514000000015), (-2.798, 262.32514000000015), (-8.80000000000119, 262.1550000000001), (-8.80000000000119, 261.9050000000001), (-0.300000000002442, 262.66), (-0.300000000002442, 262.49), (-2.798, 262.4851400000002), (-2.798, 262.31514000000016), (-2.798, 262.32514000000015), (-2.798, 262.19514000000015), (-8.80000000000119, 261.9050000000001), (-8.80000000000119, 261.6550000000001), (-0.300000000002442, 262.49), (-0.300000000002442, 262.33), (-2.798, 262.31514000000016), (-2.798, 262.19514000000015), (-2.798, 262.19514000000015), (-2.798, 262.19514000000015), (-8.80000000000119, 261.6550000000001), (-8.80000000000119, 261.6550000000001)]</t>
+          <t>[(-22703.859385937503, 66195.7242689034), (-22703.859385937503, 66195.5542689034), (-22706.3573859375, 66195.5494089034), (-22706.3573859375, 66195.3794089034), (-22706.3573859375, 66195.5494089034), (-22706.3573859375, 66195.2994089034), (-22712.359385937503, 66195.1292689034), (-22712.359385937503, 66194.8792689034), (-22703.859385937503, 66195.5542689034), (-22703.859385937503, 66195.3842689034), (-22706.3573859375, 66195.3794089034), (-22706.3573859375, 66195.2094089034), (-22706.3573859375, 66195.2994089034), (-22706.3573859375, 66195.0494089034), (-22712.359385937503, 66194.8792689034), (-22712.359385937503, 66194.6292689034), (-22703.859385937503, 66195.3842689034), (-22703.859385937503, 66195.21426890341), (-22706.3573859375, 66195.2094089034), (-22706.3573859375, 66195.03940890341), (-22706.3573859375, 66195.0494089034), (-22706.3573859375, 66194.9194089034), (-22712.359385937503, 66194.6292689034), (-22712.359385937503, 66194.3792689034), (-22703.859385937503, 66195.21426890341), (-22703.859385937503, 66195.0542689034), (-22706.3573859375, 66195.03940890341), (-22706.3573859375, 66194.9194089034), (-22706.3573859375, 66194.9194089034), (-22706.3573859375, 66194.9194089034), (-22712.359385937503, 66194.3792689034), (-22712.359385937503, 66194.3792689034)]</t>
         </is>
       </c>
     </row>
@@ -3067,7 +3067,7 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>[(-0.300000000000919, 264.0), (-0.300000000000919, 263.78), (-8.80000000000047, 263.40500000000003), (-8.80000000000047, 263.185), (-0.300000000000919, 263.78), (-0.300000000000919, 263.56), (-8.80000000000047, 263.185), (-8.80000000000047, 262.96500000000003), (-0.300000000000919, 263.56), (-0.300000000000919, 263.41), (-8.80000000000047, 262.96500000000003), (-8.80000000000047, 262.75500000000005)]</t>
+          <t>[(-22703.859385937598, 66239.6122221941), (-22703.859385937598, 66239.3922221941), (-22712.359385937598, 66239.0172221941), (-22712.359385937598, 66238.7972221941), (-22703.859385937598, 66239.3922221941), (-22703.859385937598, 66239.1722221941), (-22712.359385937598, 66238.7972221941), (-22712.359385937598, 66238.5772221941), (-22703.859385937598, 66239.1722221941), (-22703.859385937598, 66239.02222219411), (-22712.359385937598, 66238.5772221941), (-22712.359385937598, 66238.36722219411)]</t>
         </is>
       </c>
     </row>
@@ -3077,7 +3077,7 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>[(-0.300000000007065, 265.0), (-0.300000000007065, 264.85), (-6.557, 264.5620100000005), (-6.557, 264.4120100000005), (-6.557, 264.5620100000005), (-6.557, 264.4120100000005), (-8.80000000000492, 264.40500000000014), (-8.80000000000492, 264.25500000000017), (-0.300000000007065, 264.85), (-0.300000000007065, 264.55), (-6.557, 264.4120100000005), (-6.557, 264.2520100000005), (-6.557, 264.4120100000005), (-6.557, 264.2520100000005), (-8.80000000000492, 264.25500000000017), (-8.80000000000492, 263.95500000000015)]</t>
+          <t>[(-22518.659385937506, 66195.5001754849), (-22518.659385937506, 66195.35017548491), (-22524.9163859375, 66195.0621854849), (-22524.9163859375, 66194.9121854849), (-22524.9163859375, 66195.0621854849), (-22524.9163859375, 66194.9121854849), (-22527.159385937506, 66194.9051754849), (-22527.159385937506, 66194.75517548491), (-22518.659385937506, 66195.35017548491), (-22518.659385937506, 66195.05017548491), (-22524.9163859375, 66194.9121854849), (-22524.9163859375, 66194.7521854849), (-22524.9163859375, 66194.9121854849), (-22524.9163859375, 66194.7521854849), (-22527.159385937506, 66194.75517548491), (-22527.159385937506, 66194.45517548491)]</t>
         </is>
       </c>
     </row>
@@ -3087,7 +3087,7 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>[(-0.299999999999714, 266.0), (-0.299999999999714, 265.8), (-6.725, 265.55025), (-6.725, 265.35025), (-6.725, 265.55025), (-6.725, 265.33025), (-8.79999999999297, 265.4050000000005), (-8.79999999999297, 265.18500000000046), (-0.299999999999714, 265.8), (-0.299999999999714, 265.5), (-6.725, 265.35025), (-6.725, 265.19025), (-6.725, 265.33025), (-6.725, 265.19025), (-8.79999999999297, 265.18500000000046), (-8.79999999999297, 264.8850000000005)]</t>
+          <t>[(-22518.6593859376, 66237.3455648563), (-22518.6593859376, 66237.1455648563), (-22525.0843859376, 66236.8958148563), (-22525.0843859376, 66236.6958148563), (-22525.0843859376, 66236.8958148563), (-22525.0843859376, 66236.6758148563), (-22527.159385937593, 66236.7505648563), (-22527.159385937593, 66236.5305648563), (-22518.6593859376, 66237.1455648563), (-22518.6593859376, 66236.8455648563), (-22525.0843859376, 66236.6958148563), (-22525.0843859376, 66236.5358148563), (-22525.0843859376, 66236.6758148563), (-22525.0843859376, 66236.5358148563), (-22527.159385937593, 66236.5305648563), (-22527.159385937593, 66236.23056485629)]</t>
         </is>
       </c>
     </row>
@@ -3097,7 +3097,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>[(-0.300000000004976, 267.0), (-0.300000000004976, 266.71), (-6.746, 266.54878000000036), (-6.746, 266.25878000000034), (-6.746, 266.54878000000036), (-6.746, 266.29878000000036), (-8.80000000000022, 266.4050000000003), (-8.80000000000022, 266.0850000000003), (-0.300000000004976, 266.71), (-0.300000000004976, 266.42), (-6.746, 266.25878000000034), (-6.746, 266.04878000000036), (-6.746, 266.29878000000036), (-6.746, 266.04878000000036), (-8.80000000000022, 266.0850000000003), (-8.80000000000022, 265.7650000000003)]</t>
+          <t>[(-22441.659385937506, 66191.1909542276), (-22441.659385937506, 66190.9009542276), (-22448.1053859375, 66190.7397342276), (-22448.1053859375, 66190.4497342276), (-22448.1053859375, 66190.7397342276), (-22448.1053859375, 66190.4897342276), (-22450.1593859375, 66190.5959542276), (-22450.1593859375, 66190.27595422759), (-22441.659385937506, 66190.9009542276), (-22441.659385937506, 66190.6109542276), (-22448.1053859375, 66190.4497342276), (-22448.1053859375, 66190.2397342276), (-22448.1053859375, 66190.4897342276), (-22448.1053859375, 66190.2397342276), (-22450.1593859375, 66190.27595422759), (-22450.1593859375, 66189.9559542276)]</t>
         </is>
       </c>
     </row>
@@ -3107,7 +3107,7 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>[(-0.299999999999178, 268.0), (-0.299999999999178, 267.7), (-6.694, 267.5524199999999), (-6.694, 267.2524199999999), (-6.694, 267.5524199999999), (-6.694, 267.29241999999994), (-8.80000000000594, 267.4049999999995), (-8.80000000000594, 267.06499999999954), (-0.299999999999178, 267.7), (-0.299999999999178, 267.4), (-6.694, 267.2524199999999), (-6.694, 267.04241999999994), (-6.694, 267.29241999999994), (-6.694, 267.03241999999995), (-8.80000000000594, 267.06499999999954), (-8.80000000000594, 266.7249999999995)]</t>
+          <t>[(-22441.6593859375, 66237.036343599), (-22441.6593859375, 66236.736343599), (-22448.0533859375, 66236.588763599), (-22448.0533859375, 66236.28876359899), (-22448.0533859375, 66236.588763599), (-22448.0533859375, 66236.328763599), (-22450.159385937506, 66236.441343599), (-22450.159385937506, 66236.101343599), (-22441.6593859375, 66236.736343599), (-22441.6593859375, 66236.436343599), (-22448.0533859375, 66236.28876359899), (-22448.0533859375, 66236.078763599), (-22448.0533859375, 66236.328763599), (-22448.0533859375, 66236.06876359899), (-22450.159385937506, 66236.101343599), (-22450.159385937506, 66235.761343599)]</t>
         </is>
       </c>
     </row>
@@ -3117,7 +3117,7 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>[(-0.299999999996696, 269.0), (-0.299999999996696, 268.82), (-6.61, 268.55829999999975), (-6.61, 268.37829999999974), (-6.61, 268.55829999999975), (-6.61, 268.31829999999974), (-8.80000000000356, 268.4049999999995), (-8.80000000000356, 268.0849999999995), (-0.299999999996696, 268.82), (-0.299999999996696, 268.64), (-6.61, 268.37829999999974), (-6.61, 268.19829999999973), (-6.61, 268.31829999999974), (-6.61, 268.07829999999973), (-8.80000000000356, 268.0849999999995), (-8.80000000000356, 267.76499999999953), (-0.299999999996696, 268.64), (-0.299999999996696, 268.46), (-6.61, 268.19829999999973), (-6.61, 268.07829999999973), (-6.61, 268.07829999999973), (-6.61, 268.07829999999973), (-8.80000000000356, 267.76499999999953), (-8.80000000000356, 267.76499999999953)]</t>
+          <t>[(-22329.459385937495, 66192.8817329704), (-22329.459385937495, 66192.70173297041), (-22335.7693859375, 66192.44003297041), (-22335.7693859375, 66192.26003297041), (-22335.7693859375, 66192.44003297041), (-22335.7693859375, 66192.2000329704), (-22337.9593859375, 66192.2867329704), (-22337.9593859375, 66191.9667329704), (-22329.459385937495, 66192.70173297041), (-22329.459385937495, 66192.5217329704), (-22335.7693859375, 66192.26003297041), (-22335.7693859375, 66192.0800329704), (-22335.7693859375, 66192.2000329704), (-22335.7693859375, 66191.96003297041), (-22337.9593859375, 66191.9667329704), (-22337.9593859375, 66191.6467329704), (-22329.459385937495, 66192.5217329704), (-22329.459385937495, 66192.34173297041), (-22335.7693859375, 66192.0800329704), (-22335.7693859375, 66191.96003297041), (-22335.7693859375, 66191.96003297041), (-22335.7693859375, 66191.96003297041), (-22337.9593859375, 66191.6467329704), (-22337.9593859375, 66191.6467329704)]</t>
         </is>
       </c>
     </row>
@@ -3127,7 +3127,7 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>[(-0.300000000003499, 270.0), (-0.300000000003499, 269.77), (-5.972, 269.6029600000002), (-5.972, 269.3729600000002), (-5.972, 269.6029600000002), (-5.972, 269.33296000000024), (-8.80000000000085, 269.4050000000002), (-8.80000000000085, 269.1350000000002), (-0.300000000003499, 269.77), (-0.300000000003499, 269.55), (-5.972, 269.3729600000002), (-5.972, 269.21296000000024), (-5.972, 269.33296000000024), (-5.972, 269.21296000000024), (-8.80000000000085, 269.1350000000002), (-8.80000000000085, 268.8650000000002)]</t>
+          <t>[(-22329.4593859375, 66232.7271223417), (-22329.4593859375, 66232.49712234171), (-22335.1313859375, 66232.33008234171), (-22335.1313859375, 66232.10008234171), (-22335.1313859375, 66232.33008234171), (-22335.1313859375, 66232.0600823417), (-22337.959385937498, 66232.1321223417), (-22337.959385937498, 66231.8621223417), (-22329.4593859375, 66232.49712234171), (-22329.4593859375, 66232.27712234171), (-22335.1313859375, 66232.10008234171), (-22335.1313859375, 66231.94008234171), (-22335.1313859375, 66232.0600823417), (-22335.1313859375, 66231.94008234171), (-22337.959385937498, 66231.8621223417), (-22337.959385937498, 66231.59212234171)]</t>
         </is>
       </c>
     </row>
@@ -3137,7 +3137,7 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>[(-0.29999999999453, 271.0), (-0.29999999999453, 270.8), (-5.101, 270.6639299999996), (-5.101, 270.4639299999996), (-5.101, 270.6639299999996), (-5.101, 270.4839299999996), (-8.79999999999673, 270.40499999999986), (-8.79999999999673, 270.22499999999985), (-0.29999999999453, 270.8), (-0.29999999999453, 270.6), (-5.101, 270.4639299999996), (-5.101, 270.3139299999996), (-5.101, 270.4839299999996), (-5.101, 270.3139299999996), (-8.79999999999673, 270.22499999999985), (-8.79999999999673, 269.92499999999984)]</t>
+          <t>[(-22261.459385937495, 66190.57251171311), (-22261.459385937495, 66190.37251171311), (-22266.260385937498, 66190.2364417131), (-22266.260385937498, 66190.0364417131), (-22266.260385937498, 66190.2364417131), (-22266.260385937498, 66190.05644171311), (-22269.959385937495, 66189.9775117131), (-22269.959385937495, 66189.79751171311), (-22261.459385937495, 66190.37251171311), (-22261.459385937495, 66190.17251171311), (-22266.260385937498, 66190.0364417131), (-22266.260385937498, 66189.8864417131), (-22266.260385937498, 66190.05644171311), (-22266.260385937498, 66189.8864417131), (-22269.959385937495, 66189.79751171311), (-22269.959385937495, 66189.49751171311)]</t>
         </is>
       </c>
     </row>
@@ -3147,7 +3147,7 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>[(-0.299999999979226, 272.0), (-0.299999999979226, 271.8), (-4.282, 271.72125999999855), (-4.282, 271.52125999999856), (-4.282, 271.72125999999855), (-4.282, 271.60125999999855), (-7.976, 271.46267999999856), (-7.976, 271.34267999999855), (-0.299999999979226, 271.8), (-0.299999999979226, 271.61), (-4.282, 271.52125999999856), (-4.282, 271.40125999999856), (-4.282, 271.60125999999855), (-4.282, 271.40125999999856), (-7.976, 271.34267999999855), (-7.976, 271.20267999999857)]</t>
+          <t>[(-22261.459385937476, 66232.4179010845), (-22261.459385937476, 66232.2179010845), (-22265.441385937498, 66232.1391610845), (-22265.441385937498, 66231.9391610845), (-22265.441385937498, 66232.1391610845), (-22265.441385937498, 66232.0191610845), (-22269.135385937498, 66231.8805810845), (-22269.135385937498, 66231.7605810845), (-22261.459385937476, 66232.2179010845), (-22261.459385937476, 66232.0279010845), (-22265.441385937498, 66231.9391610845), (-22265.441385937498, 66231.8191610845), (-22265.441385937498, 66232.0191610845), (-22265.441385937498, 66231.8191610845), (-22269.135385937498, 66231.7605810845), (-22269.135385937498, 66231.6205810845)]</t>
         </is>
       </c>
     </row>
@@ -3157,7 +3157,7 @@
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>[(-0.300000000124842, 273.0), (-0.300000000124842, 272.83), (-3.183, 272.80888814942216), (-3.183, 272.63888814942214), (-3.183, 272.80888814942216), (-3.183, 272.6588881494222), (-6.948, 272.5593091978243), (-6.948, 272.4093091978243), (-0.300000000124842, 272.83), (-0.300000000124842, 272.66), (-3.183, 272.63888814942214), (-3.183, 272.50888814942215), (-3.183, 272.6588881494222), (-3.183, 272.50888814942215), (-6.948, 272.4093091978243), (-6.948, 272.2893091978243)]</t>
+          <t>[(-22141.25938593763, 66190.2632904559), (-22141.25938593763, 66190.0932904559), (-22144.142385937503, 66190.07217860532), (-22144.142385937503, 66189.90217860532), (-22144.142385937503, 66190.07217860532), (-22144.142385937503, 66189.92217860532), (-22147.907385937502, 66189.82259965372), (-22147.907385937502, 66189.67259965373), (-22141.25938593763, 66190.0932904559), (-22141.25938593763, 66189.9232904559), (-22144.142385937503, 66189.90217860532), (-22144.142385937503, 66189.77217860532), (-22144.142385937503, 66189.92217860532), (-22144.142385937503, 66189.77217860532), (-22147.907385937502, 66189.67259965373), (-22147.907385937502, 66189.55259965372)]</t>
         </is>
       </c>
     </row>
@@ -3177,7 +3177,7 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>[(-0.300000000024012, 275.0), (-0.300000000024012, 274.81), (-4.864, 274.7598543909959), (-4.864, 274.5698543909959), (-0.300000000024012, 274.81), (-0.300000000024012, 274.63), (-4.864, 274.5698543909959), (-4.864, 274.3898543909959)]</t>
+          <t>[(-22072.259385937625, 66188.0774126936), (-22072.259385937625, 66187.8874126936), (-22076.8233859376, 66187.8372670846), (-22076.8233859376, 66187.6472670846), (-22072.259385937625, 66187.8874126936), (-22072.259385937625, 66187.7074126936), (-22076.8233859376, 66187.6472670846), (-22076.8233859376, 66187.4672670846)]</t>
         </is>
       </c>
     </row>
@@ -3187,7 +3187,7 @@
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>[(-0.300000000004446, 276.0), (-0.300000000004446, 275.8), (-4.198, 275.82154403391445), (-4.198, 275.62154403391446), (-0.300000000004446, 275.8), (-0.300000000004446, 275.62), (-4.198, 275.62154403391446), (-4.198, 275.4215440339145)]</t>
+          <t>[(-22072.259385937505, 66226.04614556), (-22072.259385937505, 66225.84614556), (-22076.157385937502, 66225.86768959391), (-22076.157385937502, 66225.66768959392), (-22072.259385937505, 66225.84614556), (-22072.259385937505, 66225.66614556), (-22076.157385937502, 66225.66768959392), (-22076.157385937502, 66225.46768959392)]</t>
         </is>
       </c>
     </row>
@@ -3197,7 +3197,7 @@
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>[(-0.299999999988337, 277.0), (-0.299999999988337, 276.84), (-3.617, 276.87081784226876), (-3.617, 276.71081784226874), (-0.299999999988337, 276.84), (-0.299999999988337, 276.68), (-3.617, 276.71081784226874), (-3.617, 276.55081784226877), (-0.299999999988337, 276.68), (-0.299999999988337, 276.55), (-3.617, 276.55081784226877), (-3.617, 276.40081784226874)]</t>
+          <t>[(-21951.059385937588, 66186.0148784264), (-21951.059385937588, 66185.8548784264), (-21954.376385937598, 66185.88569626867), (-21954.376385937598, 66185.72569626867), (-21951.059385937588, 66185.8548784264), (-21951.059385937588, 66185.6948784264), (-21954.376385937598, 66185.72569626867), (-21954.376385937598, 66185.56569626866), (-21951.059385937588, 66185.6948784264), (-21951.059385937588, 66185.5648784264), (-21954.376385937598, 66185.56569626866), (-21954.376385937598, 66185.41569626867)]</t>
         </is>
       </c>
     </row>
@@ -3207,7 +3207,7 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>[(-0.300000000013571, 278.0), (-0.300000000013571, 277.82), (-3.264, 277.9048273155204), (-3.264, 277.7248273155204), (-0.300000000013571, 277.82), (-0.300000000013571, 277.64), (-3.264, 277.7248273155204), (-3.264, 277.54482731552037), (-0.300000000013571, 277.64), (-0.300000000013571, 277.5), (-3.264, 277.54482731552037), (-3.264, 277.36482731552036)]</t>
+          <t>[(-21921.059385937613, 66221.9836112928), (-21921.059385937613, 66221.80361129281), (-21924.0233859376, 66221.88843860832), (-21924.0233859376, 66221.70843860833), (-21921.059385937613, 66221.80361129281), (-21921.059385937613, 66221.6236112928), (-21924.0233859376, 66221.70843860833), (-21924.0233859376, 66221.52843860832), (-21921.059385937613, 66221.6236112928), (-21921.059385937613, 66221.4836112928), (-21924.0233859376, 66221.52843860832), (-21924.0233859376, 66221.34843860833)]</t>
         </is>
       </c>
     </row>
@@ -3217,7 +3217,7 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>[(-0.300000000028603, 279.0), (-0.300000000028603, 278.79), (-3.209, 278.92647908255515), (-3.209, 278.71647908255517), (-0.300000000028603, 278.79), (-0.300000000028603, 278.58), (-3.209, 278.71647908255517), (-3.209, 278.50647908255513), (-0.300000000028603, 278.58), (-0.300000000028603, 278.43), (-3.209, 278.50647908255513), (-3.209, 278.31647908255513)]</t>
+          <t>[(-21742.859385937427, 66185.9523441593), (-21742.859385937427, 66185.7423441593), (-21745.768385937397, 66185.87882324186), (-21745.768385937397, 66185.66882324185), (-21742.859385937427, 66185.7423441593), (-21742.859385937427, 66185.5323441593), (-21745.768385937397, 66185.66882324185), (-21745.768385937397, 66185.45882324186), (-21742.859385937427, 66185.5323441593), (-21742.859385937427, 66185.3823441593), (-21745.768385937397, 66185.45882324186), (-21745.768385937397, 66185.26882324186)]</t>
         </is>
       </c>
     </row>
@@ -3227,7 +3227,7 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>[(-0.29999999999737, 280.0), (-0.29999999999737, 279.76), (-3.332, 279.9755752535416), (-3.332, 279.7355752535416), (-0.29999999999737, 279.76), (-0.29999999999737, 279.52), (-3.332, 279.7355752535416), (-3.332, 279.4955752535416), (-0.29999999999737, 279.52), (-0.29999999999737, 279.36), (-3.332, 279.4955752535416), (-3.332, 279.2655752535416)]</t>
+          <t>[(-21742.859385937496, 66235.9210770257), (-21742.859385937496, 66235.6810770257), (-21745.8913859375, 66235.89665227925), (-21745.8913859375, 66235.65665227924), (-21742.859385937496, 66235.6810770257), (-21742.859385937496, 66235.44107702571), (-21745.8913859375, 66235.65665227924), (-21745.8913859375, 66235.41665227925), (-21742.859385937496, 66235.44107702571), (-21742.859385937496, 66235.2810770257), (-21745.8913859375, 66235.41665227925), (-21745.8913859375, 66235.18665227924)]</t>
         </is>
       </c>
     </row>
@@ -3237,7 +3237,7 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>[(-0.29999999999737, 281.0), (-0.29999999999737, 280.75), (-3.387, 281.02962024354105), (-3.387, 280.77962024354105), (-0.29999999999737, 280.75), (-0.29999999999737, 280.5), (-3.387, 280.77962024354105), (-3.387, 280.52962024354105), (-0.29999999999737, 280.5), (-0.29999999999737, 280.34), (-3.387, 280.52962024354105), (-3.387, 280.28962024354104)]</t>
+          <t>[(-21555.659385937597, 66185.8898098921), (-21555.659385937597, 66185.6398098921), (-21558.7463859376, 66185.91943013565), (-21558.7463859376, 66185.66943013565), (-21555.659385937597, 66185.6398098921), (-21555.659385937597, 66185.3898098921), (-21558.7463859376, 66185.66943013565), (-21558.7463859376, 66185.41943013565), (-21555.659385937597, 66185.3898098921), (-21555.659385937597, 66185.2298098921), (-21558.7463859376, 66185.41943013565), (-21558.7463859376, 66185.17943013564)]</t>
         </is>
       </c>
     </row>
@@ -3247,7 +3247,7 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>[(-0.300000000087842, 282.0), (-0.300000000087842, 281.75), (-3.34, 282.0867889340731), (-3.34, 281.8367889340731), (-0.300000000087842, 281.75), (-0.300000000087842, 281.5), (-3.34, 281.8367889340731), (-3.34, 281.5867889340731), (-0.300000000087842, 281.5), (-0.300000000087842, 281.36), (-3.34, 281.5867889340731), (-3.34, 281.3567889340731)]</t>
+          <t>[(-21545.659385937586, 66237.8585427585), (-21545.659385937586, 66237.6085427585), (-21548.6993859375, 66237.94533169258), (-21548.6993859375, 66237.69533169258), (-21545.659385937586, 66237.6085427585), (-21545.659385937586, 66237.3585427585), (-21548.6993859375, 66237.69533169258), (-21548.6993859375, 66237.44533169258), (-21545.659385937586, 66237.3585427585), (-21545.659385937586, 66237.2185427585), (-21548.6993859375, 66237.44533169258), (-21548.6993859375, 66237.21533169258)]</t>
         </is>
       </c>
     </row>
@@ -3257,7 +3257,7 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>[(-0.30000000002085, 283.0), (-0.30000000002085, 282.74), (-3.153, 283.16102375221243), (-3.153, 282.90102375221244), (-0.30000000002085, 282.74), (-0.30000000002085, 282.48), (-3.153, 282.90102375221244), (-3.153, 282.64102375221245), (-0.30000000002085, 282.48), (-0.30000000002085, 282.29), (-3.153, 282.64102375221245), (-3.153, 282.39102375221245)]</t>
+          <t>[(-21356.45938593752, 66187.7949616644), (-21356.45938593752, 66187.53496166441), (-21359.312385937497, 66187.95598541661), (-21359.312385937497, 66187.69598541662), (-21356.45938593752, 66187.53496166441), (-21356.45938593752, 66187.2749616644), (-21359.312385937497, 66187.69598541662), (-21359.312385937497, 66187.43598541661), (-21356.45938593752, 66187.2749616644), (-21356.45938593752, 66187.0849616644), (-21359.312385937497, 66187.43598541661), (-21359.312385937497, 66187.18598541661)]</t>
         </is>
       </c>
     </row>
@@ -3267,7 +3267,7 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>[(-0.299999999993575, 284.0), (-0.299999999993575, 283.75), (-2.809, 284.17563000000047), (-2.809, 283.92563000000047), (-0.299999999993575, 283.75), (-0.299999999993575, 283.5), (-2.809, 283.92563000000047), (-2.809, 283.67563000000047), (-0.299999999993575, 283.5), (-0.299999999993575, 283.36), (-2.809, 283.67563000000047), (-2.809, 283.44563000000045)]</t>
+          <t>[(-21159.259385937494, 66191.7043655305), (-21159.259385937494, 66191.4543655305), (-21161.768385937503, 66191.8799955305), (-21161.768385937503, 66191.6299955305), (-21159.259385937494, 66191.4543655305), (-21159.259385937494, 66191.2043655305), (-21161.768385937503, 66191.6299955305), (-21161.768385937503, 66191.3799955305), (-21159.259385937494, 66191.2043655305), (-21159.259385937494, 66191.0643655305), (-21161.768385937503, 66191.3799955305), (-21161.768385937503, 66191.1499955305)]</t>
         </is>
       </c>
     </row>
@@ -3277,7 +3277,7 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>[(-0.299999999993456, 285.0), (-0.299999999993456, 284.77), (-2.587, 285.1600900000005), (-2.587, 284.93009000000046), (-0.299999999993456, 284.77), (-0.299999999993456, 284.54), (-2.587, 284.93009000000046), (-2.587, 284.7000900000005), (-0.299999999993456, 284.54), (-0.299999999993456, 284.4), (-2.587, 284.7000900000005), (-2.587, 284.49009000000046)]</t>
+          <t>[(-20963.059385937493, 66195.6137693966), (-20963.059385937493, 66195.3837693966), (-20965.3463859375, 66195.7738593966), (-20965.3463859375, 66195.54385939661), (-20963.059385937493, 66195.3837693966), (-20963.059385937493, 66195.1537693966), (-20965.3463859375, 66195.54385939661), (-20965.3463859375, 66195.3138593966), (-20963.059385937493, 66195.1537693966), (-20963.059385937493, 66195.0137693966), (-20965.3463859375, 66195.3138593966), (-20965.3463859375, 66195.10385939661)]</t>
         </is>
       </c>
     </row>
@@ -3287,7 +3287,7 @@
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>[(-0.300000000003352, 286.0), (-0.300000000003352, 285.77), (-2.332, 286.1422399999998), (-2.332, 285.91223999999977), (-0.300000000003352, 285.77), (-0.300000000003352, 285.54), (-2.332, 285.91223999999977), (-2.332, 285.6822399999998), (-0.300000000003352, 285.54), (-0.300000000003352, 285.4), (-2.332, 285.6822399999998), (-2.332, 285.4722399999998)]</t>
+          <t>[(-20782.859385937503, 66191.5231732628), (-20782.859385937503, 66191.2931732628), (-20784.8913859375, 66191.6654132628), (-20784.8913859375, 66191.4354132628), (-20782.859385937503, 66191.2931732628), (-20782.859385937503, 66191.0631732628), (-20784.8913859375, 66191.4354132628), (-20784.8913859375, 66191.2054132628), (-20782.859385937503, 66191.0631732628), (-20782.859385937503, 66190.9231732628), (-20784.8913859375, 66191.2054132628), (-20784.8913859375, 66190.9954132628)]</t>
         </is>
       </c>
     </row>
@@ -3337,7 +3337,7 @@
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>[(-0.300000000091564, 291.0), (-0.300000000091564, 290.8), (-2.383, 290.86865527140577), (-2.383, 290.6686552714058), (-0.300000000091564, 290.8), (-0.300000000091564, 290.61), (-2.383, 290.6686552714058), (-2.383, 290.5286552714058)]</t>
+          <t>[(-20218.25938593769, 66190.8059989966), (-20218.25938593769, 66190.6059989966), (-20220.3423859376, 66190.674654268), (-20220.3423859376, 66190.47465426801), (-20218.25938593769, 66190.6059989966), (-20218.25938593769, 66190.4159989966), (-20220.3423859376, 66190.47465426801), (-20220.3423859376, 66190.33465426801)]</t>
         </is>
       </c>
     </row>
@@ -3357,7 +3357,7 @@
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>[(-0.299999999991311, 293.0), (-0.299999999991311, 292.84), (-2.637, 292.8364099999994), (-2.637, 292.67640999999935), (-0.299999999991311, 292.84), (-0.299999999991311, 292.69), (-2.637, 292.67640999999935), (-2.637, 292.54640999999936)]</t>
+          <t>[(-19842.859385937492, 66190.6136978306), (-19842.859385937492, 66190.4536978306), (-19845.1963859375, 66190.4501078306), (-19845.1963859375, 66190.2901078306), (-19842.859385937492, 66190.4536978306), (-19842.859385937492, 66190.3036978306), (-19845.1963859375, 66190.2901078306), (-19845.1963859375, 66190.16010783061)]</t>
         </is>
       </c>
     </row>
@@ -3367,7 +3367,7 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>[(-0.29999999999791, 294.0), (-0.29999999999791, 293.84), (-2.775, 293.82674999999983), (-2.775, 293.6667499999998), (-0.29999999999791, 293.84), (-0.29999999999791, 293.68), (-2.775, 293.6667499999998), (-2.775, 293.5367499999998)]</t>
+          <t>[(-19653.6593859375, 66188.5780411977), (-19653.6593859375, 66188.4180411977), (-19656.1343859375, 66188.4047911977), (-19656.1343859375, 66188.24479119769), (-19653.6593859375, 66188.4180411977), (-19653.6593859375, 66188.2580411977), (-19656.1343859375, 66188.24479119769), (-19656.1343859375, 66188.1147911977)]</t>
         </is>
       </c>
     </row>
@@ -3377,7 +3377,7 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>[(-0.300000000005656, 295.0), (-0.300000000005656, 294.82), (-2.84, 294.8222000000004), (-2.84, 294.6422000000004), (-0.300000000005656, 294.82), (-0.300000000005656, 294.65), (-2.84, 294.6422000000004), (-2.84, 294.4922000000004)]</t>
+          <t>[(-19456.459385937505, 66186.5423845648), (-19456.459385937505, 66186.36238456481), (-19458.9993859375, 66186.3645845648), (-19458.9993859375, 66186.1845845648), (-19456.459385937505, 66186.36238456481), (-19456.459385937505, 66186.1923845648), (-19458.9993859375, 66186.1845845648), (-19458.9993859375, 66186.0345845648)]</t>
         </is>
       </c>
     </row>
@@ -3387,7 +3387,7 @@
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>[(-0.300000000105499, 296.0), (-0.300000000105499, 295.8), (-2.912, 295.8424308753117), (-2.912, 295.64243087531173), (-0.300000000105499, 295.8), (-0.300000000105499, 295.6), (-2.912, 295.64243087531173), (-2.912, 295.4824308753117)]</t>
+          <t>[(-19277.259385937705, 66188.5067279319), (-19277.259385937705, 66188.30672793191), (-19279.8713859376, 66188.34915880722), (-19279.8713859376, 66188.14915880722), (-19277.259385937705, 66188.30672793191), (-19277.259385937705, 66188.10672793191), (-19279.8713859376, 66188.14915880722), (-19279.8713859376, 66187.98915880722)]</t>
         </is>
       </c>
     </row>
@@ -3397,7 +3397,7 @@
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>[(-0.300000000016048, 297.0), (-0.300000000016048, 296.85), (-3.01, 296.9053266548742), (-3.01, 296.75532665487424), (-0.300000000016048, 296.85), (-0.300000000016048, 296.7), (-3.01, 296.75532665487424), (-3.01, 296.6053266548742), (-0.300000000016048, 296.7), (-0.300000000016048, 296.57), (-3.01, 296.6053266548742), (-3.01, 296.4853266548742)]</t>
+          <t>[(-19111.05938593752, 66190.471071299), (-19111.05938593752, 66190.32107129901), (-19113.7693859375, 66190.37639795388), (-19113.7693859375, 66190.22639795388), (-19111.05938593752, 66190.32107129901), (-19111.05938593752, 66190.171071299), (-19113.7693859375, 66190.22639795388), (-19113.7693859375, 66190.07639795388), (-19111.05938593752, 66190.171071299), (-19111.05938593752, 66190.04107129901), (-19113.7693859375, 66190.07639795388), (-19113.7693859375, 66189.95639795388)]</t>
         </is>
       </c>
     </row>
@@ -3407,7 +3407,7 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>[(-0.300000000014052, 298.0), (-0.300000000014052, 297.82), (-2.908, 297.9751078360928), (-2.908, 297.79510783609277), (-0.300000000014052, 297.82), (-0.300000000014052, 297.64), (-2.908, 297.79510783609277), (-2.908, 297.61510783609276), (-0.300000000014052, 297.64), (-0.300000000014052, 297.5), (-2.908, 297.61510783609276), (-2.908, 297.4551078360928)]</t>
+          <t>[(-19044.059385937515, 66192.4494424183), (-19044.059385937515, 66192.26944241831), (-19046.6673859375, 66192.42455025439), (-19046.6673859375, 66192.2445502544), (-19044.059385937515, 66192.26944241831), (-19044.059385937515, 66192.0894424183), (-19046.6673859375, 66192.2445502544), (-19046.6673859375, 66192.06455025439), (-19044.059385937515, 66192.0894424183), (-19044.059385937515, 66191.9494424183), (-19046.6673859375, 66192.06455025439), (-19046.6673859375, 66191.90455025439)]</t>
         </is>
       </c>
     </row>
@@ -3417,7 +3417,7 @@
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>[(-0.300000000149659, 299.0), (-0.300000000149659, 298.83), (-2.859, 299.02169509896214), (-2.859, 298.8516950989621), (-0.300000000149659, 298.83), (-0.300000000149659, 298.66), (-2.859, 298.8516950989621), (-2.859, 298.68169509896217), (-0.300000000149659, 298.66), (-0.300000000149659, 298.53), (-2.859, 298.68169509896217), (-2.859, 298.52169509896214)]</t>
+          <t>[(-18909.85938593765, 66186.42781353761), (-18909.85938593765, 66186.25781353761), (-18912.4183859375, 66186.44950863656), (-18912.4183859375, 66186.27950863657), (-18909.85938593765, 66186.25781353761), (-18909.85938593765, 66186.08781353761), (-18912.4183859375, 66186.27950863657), (-18912.4183859375, 66186.10950863657), (-18909.85938593765, 66186.08781353761), (-18909.85938593765, 66185.9578135376), (-18912.4183859375, 66186.10950863657), (-18912.4183859375, 66185.94950863656)]</t>
         </is>
       </c>
     </row>
@@ -3427,7 +3427,7 @@
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>[(-0.300000000006431, 300.0), (-0.300000000006431, 299.82), (-2.716, 300.0533031122712), (-2.716, 299.8733031122712), (-0.300000000006431, 299.82), (-0.300000000006431, 299.64), (-2.716, 299.8733031122712), (-2.716, 299.69330311227117), (-0.300000000006431, 299.64), (-0.300000000006431, 299.51), (-2.716, 299.69330311227117), (-2.716, 299.51330311227116)]</t>
+          <t>[(-18732.541326985207, 66186.4061846569), (-18732.541326985207, 66186.2261846569), (-18734.9573269852, 66186.45948776917), (-18734.9573269852, 66186.27948776918), (-18732.541326985207, 66186.2261846569), (-18732.541326985207, 66186.0461846569), (-18734.9573269852, 66186.27948776918), (-18734.9573269852, 66186.09948776917), (-18732.541326985207, 66186.0461846569), (-18732.541326985207, 66185.91618465689), (-18734.9573269852, 66186.09948776917), (-18734.9573269852, 66185.91948776918)]</t>
         </is>
       </c>
     </row>
@@ -3437,7 +3437,7 @@
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>[(-0.30000000012637, 301.0), (-0.30000000012637, 300.82), (-2.574, 301.08106158090186), (-2.574, 300.90106158090185), (-0.30000000012637, 300.82), (-0.30000000012637, 300.64), (-2.574, 300.90106158090185), (-2.574, 300.72106158090185), (-0.30000000012637, 300.64), (-0.30000000012637, 300.5), (-2.574, 300.72106158090185), (-2.574, 300.54106158090184)]</t>
+          <t>[(-18742.541326985825, 66244.3845557763), (-18742.541326985825, 66244.2045557763), (-18744.8153269857, 66244.4656173572), (-18744.8153269857, 66244.2856173572), (-18742.541326985825, 66244.2045557763), (-18742.541326985825, 66244.0245557763), (-18744.8153269857, 66244.2856173572), (-18744.8153269857, 66244.1056173572), (-18742.541326985825, 66244.0245557763), (-18742.541326985825, 66243.8845557763), (-18744.8153269857, 66244.1056173572), (-18744.8153269857, 66243.9256173572)]</t>
         </is>
       </c>
     </row>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>[(-0.300000000019455, 302.0), (-0.300000000019455, 301.78), (-2.465, 302.1065866736659), (-2.465, 301.8865866736659), (-0.300000000019455, 301.78), (-0.300000000019455, 301.56), (-2.465, 301.8865866736659), (-2.465, 301.6665866736659), (-0.300000000019455, 301.56), (-0.300000000019455, 301.42), (-2.465, 301.6665866736659), (-2.465, 301.4665866736659)]</t>
+          <t>[(-18670.659385937623, 66190.3629268956), (-18670.659385937623, 66190.1429268956), (-18672.8243859376, 66190.46951356926), (-18672.8243859376, 66190.24951356926), (-18670.659385937623, 66190.1429268956), (-18670.659385937623, 66189.9229268956), (-18672.8243859376, 66190.24951356926), (-18672.8243859376, 66190.02951356926), (-18670.659385937623, 66189.9229268956), (-18670.659385937623, 66189.7829268956), (-18672.8243859376, 66190.02951356926), (-18672.8243859376, 66189.82951356926)]</t>
         </is>
       </c>
     </row>
@@ -4247,7 +4247,7 @@
       </c>
       <c r="B383" t="inlineStr">
         <is>
-          <t>[(-0.300000000002373, 382.0), (-0.300000000002373, 381.87), (-2.403, 381.8582759393319), (-2.403, 381.7282759393319), (-0.300000000002373, 381.87), (-0.300000000002373, 381.75), (-2.403, 381.7282759393319), (-2.403, 381.6082759393319)]</t>
+          <t>[(-14553.259385937403, 66187.4527333416), (-14553.259385937403, 66187.3227333416), (-14555.3623859374, 66187.31100928094), (-14555.3623859374, 66187.18100928093), (-14553.259385937403, 66187.3227333416), (-14553.259385937403, 66187.2027333416), (-14555.3623859374, 66187.18100928093), (-14555.3623859374, 66187.06100928094)]</t>
         </is>
       </c>
     </row>
@@ -4257,7 +4257,7 @@
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>[(-0.300000000153819, 383.0), (-0.300000000153819, 382.87), (-2.438, 382.8770834411638), (-2.438, 382.7470834411638), (-0.300000000153819, 382.87), (-0.300000000153819, 382.75), (-2.438, 382.7470834411638), (-2.438, 382.6270834411638)]</t>
+          <t>[(-14543.259385937654, 66226.0121075804), (-14543.259385937654, 66225.8821075804), (-14545.3973859375, 66225.88919102158), (-14545.3973859375, 66225.75919102157), (-14543.259385937654, 66225.8821075804), (-14543.259385937654, 66225.7621075804), (-14545.3973859375, 66225.75919102157), (-14545.3973859375, 66225.63919102158)]</t>
         </is>
       </c>
     </row>
@@ -4817,7 +4817,7 @@
       </c>
       <c r="B440" t="inlineStr">
         <is>
-          <t>[(-0.300000000037907, 439.0), (-0.300000000037907, 438.83), (-4.836, 438.8098424565949), (-4.836, 438.63984245659486), (-0.300000000037907, 438.83), (-0.300000000037907, 438.69), (-4.836, 438.63984245659486), (-4.836, 438.4698424565949)]</t>
+          <t>[(-24389.65938593754, 65886.1838577571), (-24389.65938593754, 65886.0138577571), (-24394.1953859375, 65885.9937002137), (-24394.1953859375, 65885.8237002137), (-24389.65938593754, 65886.0138577571), (-24389.65938593754, 65885.8738577571), (-24394.1953859375, 65885.8237002137), (-24394.1953859375, 65885.6537002137)]</t>
         </is>
       </c>
     </row>
@@ -4827,7 +4827,7 @@
       </c>
       <c r="B441" t="inlineStr">
         <is>
-          <t>[(-0.300000000108372, 440.0), (-0.300000000108372, 439.83), (-2.75, 439.9107914503244), (-2.75, 439.74079145032437), (-0.300000000108372, 439.83), (-0.300000000108372, 439.68), (-2.75, 439.74079145032437), (-2.75, 439.5707914503244)]</t>
+          <t>[(-24389.65938593771, 65930.7972276573), (-24389.65938593771, 65930.6272276573), (-24392.1093859376, 65930.70801910762), (-24392.1093859376, 65930.53801910763), (-24389.65938593771, 65930.6272276573), (-24389.65938593771, 65930.47722765729), (-24392.1093859376, 65930.53801910763), (-24392.1093859376, 65930.36801910763)]</t>
         </is>
       </c>
     </row>
@@ -4837,7 +4837,7 @@
       </c>
       <c r="B442" t="inlineStr">
         <is>
-          <t>[(-0.30000000004277, 441.0), (-0.30000000004277, 440.83), (-4.523, 440.86950318151287), (-4.523, 440.69950318151285), (-0.30000000004277, 440.83), (-0.30000000004277, 440.69), (-4.523, 440.69950318151285), (-4.523, 440.5395031815129)]</t>
+          <t>[(-24321.659385937644, 65887.355287823), (-24321.659385937644, 65887.185287823), (-24325.882385937603, 65887.22479100451), (-24325.882385937603, 65887.05479100451), (-24321.659385937644, 65887.185287823), (-24321.659385937644, 65887.045287823), (-24325.882385937603, 65887.05479100451), (-24325.882385937603, 65886.89479100451)]</t>
         </is>
       </c>
     </row>
@@ -4847,7 +4847,7 @@
       </c>
       <c r="B443" t="inlineStr">
         <is>
-          <t>[(-0.30000000013396, 442.0), (-0.30000000013396, 441.83), (-5.604, 441.86532483775835), (-5.604, 441.69532483775833), (-0.30000000013396, 441.83), (-0.30000000013396, 441.67), (-5.604, 441.69532483775833), (-5.604, 441.53532483775837)]</t>
+          <t>[(-24321.659385937735, 65929.8580382542), (-24321.659385937735, 65929.6880382542), (-24326.9633859376, 65929.72336309195), (-24326.9633859376, 65929.55336309195), (-24321.659385937735, 65929.6880382542), (-24321.659385937735, 65929.5280382542), (-24326.9633859376, 65929.55336309195), (-24326.9633859376, 65929.39336309195)]</t>
         </is>
       </c>
     </row>
@@ -4857,7 +4857,7 @@
       </c>
       <c r="B444" t="inlineStr">
         <is>
-          <t>[(-0.300000000008999, 443.0), (-0.300000000008999, 442.81), (-6.634, 442.84165000000024), (-6.634, 442.65165000000025), (-0.300000000008999, 442.81), (-0.300000000008999, 442.64), (-6.634, 442.65165000000025), (-6.634, 442.47165000000024)]</t>
+          <t>[(-24210.45938593751, 65886.3054789509), (-24210.45938593751, 65886.1154789509), (-24216.793385937497, 65886.1471289509), (-24216.793385937497, 65885.9571289509), (-24210.45938593751, 65886.1154789509), (-24210.45938593751, 65885.9454789509), (-24216.793385937497, 65885.9571289509), (-24216.793385937497, 65885.77712895091)]</t>
         </is>
       </c>
     </row>
@@ -4867,7 +4867,7 @@
       </c>
       <c r="B445" t="inlineStr">
         <is>
-          <t>[(-0.300000000006756, 444.0), (-0.300000000006756, 443.8), (-2.622, 443.9419500000002), (-2.622, 443.7419500000002), (-0.300000000006756, 443.8), (-0.300000000006756, 443.61), (-2.622, 443.7419500000002), (-2.622, 443.5519500000002)]</t>
+          <t>[(-24210.459385937607, 65924.6986083218), (-24210.459385937607, 65924.49860832181), (-24212.7813859376, 65924.6405583218), (-24212.7813859376, 65924.4405583218), (-24210.459385937607, 65924.49860832181), (-24210.459385937607, 65924.30860832181), (-24212.7813859376, 65924.4405583218), (-24212.7813859376, 65924.2505583218)]</t>
         </is>
       </c>
     </row>
@@ -4877,7 +4877,7 @@
       </c>
       <c r="B446" t="inlineStr">
         <is>
-          <t>[(-0.300000000006756, 445.0), (-0.300000000006756, 444.81), (-3.713, 444.91467500000016), (-3.713, 444.72467500000016), (-0.300000000006756, 444.81), (-0.300000000006756, 444.63), (-3.713, 444.72467500000016), (-3.713, 444.53467500000016)]</t>
+          <t>[(-24150.459385937607, 65887.0735936243), (-24150.459385937607, 65886.8835936243), (-24153.8723859376, 65886.9882686243), (-24153.8723859376, 65886.7982686243), (-24150.459385937607, 65886.8835936243), (-24150.459385937607, 65886.7035936243), (-24153.8723859376, 65886.7982686243), (-24153.8723859376, 65886.6082686243)]</t>
         </is>
       </c>
     </row>
@@ -4887,7 +4887,7 @@
       </c>
       <c r="B447" t="inlineStr">
         <is>
-          <t>[(-0.300000000008999, 446.0), (-0.300000000008999, 445.83), (-5.03, 445.88175000000024), (-5.03, 445.7117500000002), (-0.300000000008999, 445.83), (-0.300000000008999, 445.66), (-5.03, 445.7117500000002), (-5.03, 445.54175000000026)]</t>
+          <t>[(-24150.45938593751, 65925.4485789267), (-24150.45938593751, 65925.2785789267), (-24155.189385937498, 65925.3303289267), (-24155.189385937498, 65925.16032892671), (-24150.45938593751, 65925.2785789267), (-24150.45938593751, 65925.10857892671), (-24155.189385937498, 65925.16032892671), (-24155.189385937498, 65924.99032892671)]</t>
         </is>
       </c>
     </row>
@@ -4897,7 +4897,7 @@
       </c>
       <c r="B448" t="inlineStr">
         <is>
-          <t>[(-0.300000000006756, 447.0), (-0.300000000006756, 446.8), (-5.47, 446.87075000000016), (-5.47, 446.67075000000017), (-0.300000000006756, 446.8), (-0.300000000006756, 446.61), (-5.47, 446.67075000000017), (-5.47, 446.50075000000015)]</t>
+          <t>[(-24022.259385937607, 65889.8235642291), (-24022.259385937607, 65889.6235642291), (-24027.4293859376, 65889.6943142291), (-24027.4293859376, 65889.4943142291), (-24022.259385937607, 65889.6235642291), (-24022.259385937607, 65889.4335642291), (-24027.4293859376, 65889.4943142291), (-24027.4293859376, 65889.3243142291)]</t>
         </is>
       </c>
     </row>
@@ -4907,7 +4907,7 @@
       </c>
       <c r="B449" t="inlineStr">
         <is>
-          <t>[(-0.300000000006756, 448.0), (-0.300000000006756, 447.86), (-5.501, 447.8699750000002), (-5.501, 447.7299750000002), (-0.300000000006756, 447.86), (-0.300000000006756, 447.56), (-5.501, 447.7299750000002), (-5.501, 447.56997500000017)]</t>
+          <t>[(-24022.259385937607, 65930.1985495315), (-24022.259385937607, 65930.0585495315), (-24027.4603859376, 65930.0685245315), (-24027.4603859376, 65929.9285245315), (-24022.259385937607, 65930.0585495315), (-24022.259385937607, 65929.7585495315), (-24027.4603859376, 65929.9285245315), (-24027.4603859376, 65929.7685245315)]</t>
         </is>
       </c>
     </row>
@@ -4917,7 +4917,7 @@
       </c>
       <c r="B450" t="inlineStr">
         <is>
-          <t>[(-0.300000000008999, 449.0), (-0.300000000008999, 448.85), (-8.746, 448.78885000000025), (-8.746, 448.6388500000003), (-0.300000000008999, 448.85), (-0.300000000008999, 448.7), (-8.746, 448.6388500000003), (-8.746, 448.48885000000024), (-0.300000000008999, 448.7), (-0.300000000008999, 448.55), (-8.746, 448.48885000000024), (-8.746, 448.34885000000025)]</t>
+          <t>[(-23962.259385937512, 65890.573534834), (-23962.259385937512, 65890.423534834), (-23970.7053859375, 65890.36238483399), (-23970.7053859375, 65890.212384834), (-23962.259385937512, 65890.423534834), (-23962.259385937512, 65890.27353483399), (-23970.7053859375, 65890.212384834), (-23970.7053859375, 65890.06238483399), (-23962.259385937512, 65890.27353483399), (-23962.259385937512, 65890.123534834), (-23970.7053859375, 65890.06238483399), (-23970.7053859375, 65889.92238483399)]</t>
         </is>
       </c>
     </row>
@@ -4927,7 +4927,7 @@
       </c>
       <c r="B451" t="inlineStr">
         <is>
-          <t>[(-0.300000000006756, 450.0), (-0.300000000006756, 449.79), (-7.23, 449.8267500000002), (-7.23, 449.6167500000002), (-0.300000000006756, 449.79), (-0.300000000006756, 449.58), (-7.23, 449.6167500000002), (-7.23, 449.46675000000016)]</t>
+          <t>[(-23962.25938593751, 65928.9485201364), (-23962.25938593751, 65928.7385201364), (-23969.1893859375, 65928.7752701364), (-23969.1893859375, 65928.56527013639), (-23962.25938593751, 65928.7385201364), (-23962.25938593751, 65928.5285201364), (-23969.1893859375, 65928.56527013639), (-23969.1893859375, 65928.4152701364)]</t>
         </is>
       </c>
     </row>
@@ -4937,7 +4937,7 @@
       </c>
       <c r="B452" t="inlineStr">
         <is>
-          <t>[(-0.300000000006756, 451.0), (-0.300000000006756, 450.81), (-6.067, 450.85582500000015), (-6.067, 450.66582500000015), (-0.300000000006756, 450.81), (-0.300000000006756, 450.62), (-6.067, 450.66582500000015), (-6.067, 450.50582500000013)]</t>
+          <t>[(-23834.059385937508, 65889.3235054388), (-23834.059385937508, 65889.1335054388), (-23839.8263859375, 65889.17933043881), (-23839.8263859375, 65888.98933043881), (-23834.059385937508, 65889.1335054388), (-23834.059385937508, 65888.9435054388), (-23839.8263859375, 65888.98933043881), (-23839.8263859375, 65888.8293304388)]</t>
         </is>
       </c>
     </row>
@@ -4947,7 +4947,7 @@
       </c>
       <c r="B453" t="inlineStr">
         <is>
-          <t>[(-0.300000000008999, 452.0), (-0.300000000008999, 451.82), (-6.353, 451.84867500000024), (-6.353, 451.66867500000023), (-0.300000000008999, 451.82), (-0.300000000008999, 451.65), (-6.353, 451.66867500000023), (-6.353, 451.53867500000024)]</t>
+          <t>[(-23834.05938593761, 65927.6984907412), (-23834.05938593761, 65927.5184907412), (-23840.1123859376, 65927.5471657412), (-23840.1123859376, 65927.3671657412), (-23834.05938593761, 65927.5184907412), (-23834.05938593761, 65927.34849074119), (-23840.1123859376, 65927.3671657412), (-23840.1123859376, 65927.2371657412)]</t>
         </is>
       </c>
     </row>
@@ -4957,7 +4957,7 @@
       </c>
       <c r="B454" t="inlineStr">
         <is>
-          <t>[(-0.300000000006756, 453.0), (-0.300000000006756, 452.84), (-6.671, 452.8407250000002), (-6.671, 452.68072500000017), (-0.300000000006756, 452.84), (-0.300000000006756, 452.68), (-6.671, 452.68072500000017), (-6.671, 452.55072500000017)]</t>
+          <t>[(-23774.059385937606, 65888.0734760437), (-23774.059385937606, 65887.9134760437), (-23780.430385937598, 65887.9142010437), (-23780.430385937598, 65887.7542010437), (-23774.059385937606, 65887.9134760437), (-23774.059385937606, 65887.7534760437), (-23780.430385937598, 65887.7542010437), (-23780.430385937598, 65887.62420104371)]</t>
         </is>
       </c>
     </row>
@@ -4967,7 +4967,7 @@
       </c>
       <c r="B455" t="inlineStr">
         <is>
-          <t>[(-0.300000000008999, 454.0), (-0.300000000008999, 453.84), (-6.993, 453.8326750000002), (-6.993, 453.6726750000002), (-0.300000000008999, 453.84), (-0.300000000008999, 453.68), (-6.993, 453.6726750000002), (-6.993, 453.5426750000002)]</t>
+          <t>[(-23774.05938593751, 65928.4484613461), (-23774.05938593751, 65928.28846134609), (-23780.7523859375, 65928.2811363461), (-23780.7523859375, 65928.12113634609), (-23774.05938593751, 65928.28846134609), (-23774.05938593751, 65928.12846134609), (-23780.7523859375, 65928.12113634609), (-23780.7523859375, 65927.9911363461)]</t>
         </is>
       </c>
     </row>
@@ -4977,7 +4977,7 @@
       </c>
       <c r="B456" t="inlineStr">
         <is>
-          <t>[(-0.300000000006756, 455.0), (-0.300000000006756, 454.82), (-7.248, 454.8263000000002), (-7.248, 454.64630000000017), (-0.300000000006756, 454.82), (-0.300000000006756, 454.64), (-7.248, 454.64630000000017), (-7.248, 454.5063000000002)]</t>
+          <t>[(-23645.859385937605, 65890.8234466485), (-23645.859385937605, 65890.64344664851), (-23652.807385937598, 65890.6497466485), (-23652.807385937598, 65890.46974664851), (-23645.859385937605, 65890.64344664851), (-23645.859385937605, 65890.4634466485), (-23652.807385937598, 65890.46974664851), (-23652.807385937598, 65890.3297466485)]</t>
         </is>
       </c>
     </row>
@@ -4987,7 +4987,7 @@
       </c>
       <c r="B457" t="inlineStr">
         <is>
-          <t>[(-0.300000000008999, 456.0), (-0.300000000008999, 455.83), (-7.525, 455.8193750000002), (-7.525, 455.6493750000002), (-0.300000000008999, 455.83), (-0.300000000008999, 455.66), (-7.525, 455.6493750000002), (-7.525, 455.5293750000002)]</t>
+          <t>[(-23645.85938593761, 65929.1984319509), (-23645.85938593761, 65929.02843195091), (-23653.0843859376, 65929.01780695091), (-23653.0843859376, 65928.84780695091), (-23645.85938593761, 65929.02843195091), (-23645.85938593761, 65928.85843195091), (-23653.0843859376, 65928.84780695091), (-23653.0843859376, 65928.72780695092)]</t>
         </is>
       </c>
     </row>
@@ -4997,7 +4997,7 @@
       </c>
       <c r="B458" t="inlineStr">
         <is>
-          <t>[(-0.300000000008999, 457.0), (-0.300000000008999, 456.8), (-7.834, 456.8116500000002), (-7.834, 456.6116500000002), (-0.300000000008999, 456.8), (-0.300000000008999, 456.6), (-7.834, 456.6116500000002), (-7.834, 456.48165000000023)]</t>
+          <t>[(-23586.85938593751, 65891.5734172534), (-23586.85938593751, 65891.3734172534), (-23594.3933859375, 65891.3850672534), (-23594.3933859375, 65891.1850672534), (-23586.85938593751, 65891.3734172534), (-23586.85938593751, 65891.1734172534), (-23594.3933859375, 65891.1850672534), (-23594.3933859375, 65891.0550672534)]</t>
         </is>
       </c>
     </row>
@@ -5007,7 +5007,7 @@
       </c>
       <c r="B459" t="inlineStr">
         <is>
-          <t>[(-0.300000000006756, 458.0), (-0.300000000006756, 457.88), (-8.13, 457.8042500000002), (-8.13, 457.6842500000002), (-0.300000000006756, 457.88), (-0.300000000006756, 457.62), (-8.13, 457.6842500000002), (-8.13, 457.5142500000002)]</t>
+          <t>[(-23586.859385937605, 65931.9484025558), (-23586.859385937605, 65931.82840255581), (-23594.6893859376, 65931.7526525558), (-23594.6893859376, 65931.63265255581), (-23586.859385937605, 65931.82840255581), (-23586.859385937605, 65931.5684025558), (-23594.6893859376, 65931.63265255581), (-23594.6893859376, 65931.46265255581)]</t>
         </is>
       </c>
     </row>
@@ -5017,7 +5017,7 @@
       </c>
       <c r="B460" t="inlineStr">
         <is>
-          <t>[(-0.300000000006756, 459.0), (-0.300000000006756, 458.79), (-8.349, 458.916638343173), (-8.349, 458.70663834317304), (-0.300000000006756, 458.79), (-0.300000000006756, 458.67), (-8.349, 458.70663834317304), (-8.349, 458.496638343173)]</t>
+          <t>[(-23457.659385937608, 65890.3233878582), (-23457.659385937608, 65890.11338785819), (-23465.7083859376, 65890.24002620137), (-23465.7083859376, 65890.03002620136), (-23457.659385937608, 65890.11338785819), (-23457.659385937608, 65889.9933878582), (-23465.7083859376, 65890.03002620136), (-23465.7083859376, 65889.82002620137)]</t>
         </is>
       </c>
     </row>
@@ -5027,7 +5027,7 @@
       </c>
       <c r="B461" t="inlineStr">
         <is>
-          <t>[(-0.300000000008999, 460.0), (-0.300000000008999, 459.82), (-8.559, 460.1209384210789), (-8.559, 459.9409384210789), (-0.300000000008999, 459.82), (-0.300000000008999, 459.68), (-8.559, 459.9409384210789), (-8.559, 459.6409384210789)]</t>
+          <t>[(-23457.65938593751, 65930.6852388993), (-23457.65938593751, 65930.5052388993), (-23465.9183859375, 65930.80617732038), (-23465.9183859375, 65930.62617732039), (-23457.65938593751, 65930.5052388993), (-23457.65938593751, 65930.36523889929), (-23465.9183859375, 65930.62617732039), (-23465.9183859375, 65930.32617732038)]</t>
         </is>
       </c>
     </row>
@@ -5037,7 +5037,7 @@
       </c>
       <c r="B462" t="inlineStr">
         <is>
-          <t>[(-0.300000000022718, 461.0), (-0.300000000022718, 460.84), (-8.777, 461.2525008251748), (-8.777, 460.97250082517485), (-0.300000000022718, 460.84), (-0.300000000022718, 460.68), (-8.777, 460.97250082517485), (-8.777, 460.6925008251748)]</t>
+          <t>[(-23397.659385937623, 65891.0470899404), (-23397.659385937623, 65890.8870899404), (-23406.1363859376, 65891.29959076557), (-23406.1363859376, 65891.01959076557), (-23397.659385937623, 65890.8870899404), (-23397.659385937623, 65890.7270899404), (-23406.1363859376, 65891.01959076557), (-23406.1363859376, 65890.73959076557)]</t>
         </is>
       </c>
     </row>
@@ -5047,7 +5047,7 @@
       </c>
       <c r="B463" t="inlineStr">
         <is>
-          <t>[(-0.300000000000589, 462.0), (-0.300000000000589, 461.88), (-8.79999999999889, 462.3226479164789), (-8.79999999999889, 462.0526479164789), (-0.300000000000589, 461.88), (-0.300000000000589, 461.76), (-8.79999999999889, 462.0526479164789), (-8.79999999999889, 461.7826479164789)]</t>
+          <t>[(-23397.6593859375, 65931.4089409815), (-23397.6593859375, 65931.28894098151), (-23406.1593859375, 65931.73158889798), (-23406.1593859375, 65931.46158889798), (-23397.6593859375, 65931.28894098151), (-23397.6593859375, 65931.1689409815), (-23406.1593859375, 65931.46158889798), (-23406.1593859375, 65931.19158889799)]</t>
         </is>
       </c>
     </row>
@@ -5057,7 +5057,7 @@
       </c>
       <c r="B464" t="inlineStr">
         <is>
-          <t>[(-0.3000000000414, 463.0), (-0.3000000000414, 462.88), (-8.80000000001008, 463.39210991647747), (-8.80000000001008, 463.09210991647745), (-0.3000000000414, 462.88), (-0.3000000000414, 462.76), (-8.80000000001008, 463.09210991647745), (-8.80000000001008, 462.79210991647744)]</t>
+          <t>[(-23269.459385937644, 65891.7707920227), (-23269.459385937644, 65891.6507920227), (-23277.95938593761, 65892.16290193917), (-23277.95938593761, 65891.86290193917), (-23269.459385937644, 65891.6507920227), (-23269.459385937644, 65891.53079202269), (-23277.95938593761, 65891.86290193917), (-23277.95938593761, 65891.56290193916)]</t>
         </is>
       </c>
     </row>
@@ -5107,7 +5107,7 @@
       </c>
       <c r="B469" t="inlineStr">
         <is>
-          <t>[(-0.300000000001038, 468.0), (-0.300000000001038, 467.87), (-3.425, 468.21874999999994), (-3.425, 468.08874999999995), (-3.425, 468.21874999999994), (-3.425, 468.09874999999994), (-8.80000000000329, 468.59500000000014), (-8.80000000000329, 468.32500000000016), (-0.300000000001038, 467.87), (-0.300000000001038, 467.75), (-3.425, 468.08874999999995), (-3.425, 467.96874999999994), (-3.425, 468.09874999999994), (-3.425, 467.97874999999993), (-8.80000000000329, 468.32500000000016), (-8.80000000000329, 468.0550000000001)]</t>
+          <t>[(-23081.2593859376, 65927.5800472282), (-23081.2593859376, 65927.4500472282), (-23084.3843859376, 65927.7987972282), (-23084.3843859376, 65927.6687972282), (-23084.3843859376, 65927.7987972282), (-23084.3843859376, 65927.6787972282), (-23089.759385937603, 65928.1750472282), (-23089.759385937603, 65927.9050472282), (-23081.2593859376, 65927.4500472282), (-23081.2593859376, 65927.3300472282), (-23084.3843859376, 65927.6687972282), (-23084.3843859376, 65927.5487972282), (-23084.3843859376, 65927.6787972282), (-23084.3843859376, 65927.5587972282), (-23089.759385937603, 65927.9050472282), (-23089.759385937603, 65927.6350472282)]</t>
         </is>
       </c>
     </row>
@@ -5117,7 +5117,7 @@
       </c>
       <c r="B470" t="inlineStr">
         <is>
-          <t>[(-0.300000000022424, 469.0), (-0.300000000022424, 468.84), (-3.597, 469.2307899999984), (-3.597, 469.0707899999984), (-3.597, 469.2307899999984), (-3.597, 469.0707899999984), (-8.80000000001358, 469.5949999999994), (-8.80000000001358, 469.2949999999994), (-0.300000000022424, 468.84), (-0.300000000022424, 468.72), (-3.597, 469.0707899999984), (-3.597, 468.9107899999984), (-3.597, 469.0707899999984), (-3.597, 468.9107899999984), (-8.80000000001358, 469.2949999999994), (-8.80000000001358, 468.9949999999994)]</t>
+          <t>[(-23022.259385937523, 65885.9418982693), (-23022.259385937523, 65885.7818982693), (-23025.556385937503, 65886.1726882693), (-23025.556385937503, 65886.0126882693), (-23025.556385937503, 65886.1726882693), (-23025.556385937503, 65886.0126882693), (-23030.759385937516, 65886.5368982693), (-23030.759385937516, 65886.2368982693), (-23022.259385937523, 65885.7818982693), (-23022.259385937523, 65885.6618982693), (-23025.556385937503, 65886.0126882693), (-23025.556385937503, 65885.8526882693), (-23025.556385937503, 65886.0126882693), (-23025.556385937503, 65885.8526882693), (-23030.759385937516, 65886.2368982693), (-23030.759385937516, 65885.9368982693)]</t>
         </is>
       </c>
     </row>
@@ -5127,7 +5127,7 @@
       </c>
       <c r="B471" t="inlineStr">
         <is>
-          <t>[(-0.300000000006231, 470.0), (-0.300000000006231, 469.87), (-3.89, 470.25129999999956), (-3.89, 470.12129999999956), (-3.89, 470.25129999999956), (-3.89, 470.13129999999956), (-8.80000000000392, 470.59499999999986), (-8.80000000000392, 470.3149999999999), (-0.300000000006231, 469.87), (-0.300000000006231, 469.75), (-3.89, 470.12129999999956), (-3.89, 470.00129999999956), (-3.89, 470.13129999999956), (-3.89, 470.01129999999955), (-8.80000000000392, 470.3149999999999), (-8.80000000000392, 470.03499999999985)]</t>
+          <t>[(-23022.25938593751, 65926.3037493104), (-23022.25938593751, 65926.1737493104), (-23025.8493859375, 65926.55504931041), (-23025.8493859375, 65926.4250493104), (-23025.8493859375, 65926.55504931041), (-23025.8493859375, 65926.43504931041), (-23030.759385937505, 65926.8987493104), (-23030.759385937505, 65926.61874931041), (-23022.25938593751, 65926.1737493104), (-23022.25938593751, 65926.0537493104), (-23025.8493859375, 65926.4250493104), (-23025.8493859375, 65926.30504931041), (-23025.8493859375, 65926.43504931041), (-23025.8493859375, 65926.3150493104), (-23030.759385937505, 65926.61874931041), (-23030.759385937505, 65926.33874931041)]</t>
         </is>
       </c>
     </row>
@@ -5137,7 +5137,7 @@
       </c>
       <c r="B472" t="inlineStr">
         <is>
-          <t>[(-0.300000000005409, 471.0), (-0.300000000005409, 470.84), (-4.191, 471.2723699999996), (-4.191, 471.1123699999996), (-4.191, 471.2723699999996), (-4.191, 471.1123699999996), (-8.79999999999882, 471.5949999999995), (-8.79999999999882, 471.2949999999995), (-0.300000000005409, 470.84), (-0.300000000005409, 470.72), (-4.191, 471.1123699999996), (-4.191, 470.9623699999996), (-4.191, 471.1123699999996), (-4.191, 470.95236999999963), (-8.79999999999882, 471.2949999999995), (-8.79999999999882, 470.9949999999995)]</t>
+          <t>[(-22895.059385937508, 65886.6656003515), (-22895.059385937508, 65886.50560035149), (-22898.9503859375, 65886.9379703515), (-22898.9503859375, 65886.7779703515), (-22898.9503859375, 65886.9379703515), (-22898.9503859375, 65886.7779703515), (-22903.5593859375, 65887.2606003515), (-22903.5593859375, 65886.9606003515), (-22895.059385937508, 65886.50560035149), (-22895.059385937508, 65886.3856003515), (-22898.9503859375, 65886.7779703515), (-22898.9503859375, 65886.6279703515), (-22898.9503859375, 65886.7779703515), (-22898.9503859375, 65886.6179703515), (-22903.5593859375, 65886.9606003515), (-22903.5593859375, 65886.66060035149)]</t>
         </is>
       </c>
     </row>
@@ -5147,7 +5147,7 @@
       </c>
       <c r="B473" t="inlineStr">
         <is>
-          <t>[(-0.300000000001446, 472.0), (-0.300000000001446, 471.86), (-4.416, 472.2881199999999), (-4.416, 472.1481199999999), (-4.416, 472.2881199999999), (-4.416, 472.1481199999999), (-8.79999999999802, 472.59499999999974), (-8.79999999999802, 472.3049999999997), (-0.300000000001446, 471.86), (-0.300000000001446, 471.74), (-4.416, 472.1481199999999), (-4.416, 472.0181199999999), (-4.416, 472.1481199999999), (-4.416, 472.0081199999999), (-8.79999999999802, 472.3049999999997), (-8.79999999999802, 472.01499999999976)]</t>
+          <t>[(-22895.059385937602, 65937.0274513926), (-22895.059385937602, 65936.8874513926), (-22899.1753859376, 65937.3155713926), (-22899.1753859376, 65937.1755713926), (-22899.1753859376, 65937.3155713926), (-22899.1753859376, 65937.1755713926), (-22903.5593859376, 65937.6224513926), (-22903.5593859376, 65937.3324513926), (-22895.059385937602, 65936.8874513926), (-22895.059385937602, 65936.7674513926), (-22899.1753859376, 65937.1755713926), (-22899.1753859376, 65937.04557139259), (-22899.1753859376, 65937.1755713926), (-22899.1753859376, 65937.0355713926), (-22903.5593859376, 65937.3324513926), (-22903.5593859376, 65937.0424513926)]</t>
         </is>
       </c>
     </row>
@@ -5197,7 +5197,7 @@
       </c>
       <c r="B478" t="inlineStr">
         <is>
-          <t>[(-0.299999999994854, 477.0), (-0.299999999994854, 476.87), (-4.91, 477.32270000000034), (-4.91, 477.19270000000034), (-4.91, 477.32270000000034), (-4.91, 477.20270000000033), (-8.79999999999481, 477.59499999999997), (-8.79999999999481, 477.325), (-0.299999999994854, 476.87), (-0.299999999994854, 476.75), (-4.91, 477.19270000000034), (-4.91, 477.07270000000034), (-4.91, 477.20270000000033), (-4.91, 477.08270000000033), (-8.79999999999481, 477.325), (-8.79999999999481, 477.05499999999995)]</t>
+          <t>[(-22328.459385937495, 65888.9026280038), (-22328.459385937495, 65888.77262800379), (-22333.0693859375, 65889.2253280038), (-22333.0693859375, 65889.0953280038), (-22333.0693859375, 65889.2253280038), (-22333.0693859375, 65889.1053280038), (-22336.959385937495, 65889.4976280038), (-22336.959385937495, 65889.22762800379), (-22328.459385937495, 65888.77262800379), (-22328.459385937495, 65888.6526280038), (-22333.0693859375, 65889.0953280038), (-22333.0693859375, 65888.9753280038), (-22333.0693859375, 65889.1053280038), (-22333.0693859375, 65888.9853280038), (-22336.959385937495, 65889.22762800379), (-22336.959385937495, 65888.9576280038)]</t>
         </is>
       </c>
     </row>
@@ -5247,7 +5247,7 @@
       </c>
       <c r="B483" t="inlineStr">
         <is>
-          <t>[(-0.300000000032176, 482.0), (-0.300000000032176, 481.88), (-4.711, 482.3017570240261), (-4.711, 482.18175702402607), (-4.711, 482.3017570240261), (-4.711, 482.14175702402605), (-8.79999999998781, 482.58148599052976), (-8.79999999998781, 482.28148599052975), (-0.300000000032176, 481.88), (-0.300000000032176, 481.73), (-4.711, 482.18175702402607), (-4.711, 481.99175702402607), (-4.711, 482.14175702402605), (-4.711, 481.9817570240261), (-8.79999999998781, 482.28148599052975), (-8.79999999998781, 481.98148599052973)]</t>
+          <t>[(-21386.45938593753, 65888.8766867233), (-21386.45938593753, 65888.75668672331), (-21390.8703859375, 65889.17844374733), (-21390.8703859375, 65889.05844374733), (-21390.8703859375, 65889.17844374733), (-21390.8703859375, 65889.01844374732), (-21394.959385937487, 65889.45817271384), (-21394.959385937487, 65889.15817271384), (-21386.45938593753, 65888.75668672331), (-21386.45938593753, 65888.6066867233), (-21390.8703859375, 65889.05844374733), (-21390.8703859375, 65888.86844374733), (-21390.8703859375, 65889.01844374732), (-21390.8703859375, 65888.85844374732), (-21394.959385937487, 65889.15817271384), (-21394.959385937487, 65888.85817271384)]</t>
         </is>
       </c>
     </row>
@@ -5257,7 +5257,7 @@
       </c>
       <c r="B484" t="inlineStr">
         <is>
-          <t>[(-0.300000000018094, 483.0), (-0.300000000018094, 482.83), (-4.708, 483.26552961767754), (-4.708, 483.0955296176775), (-4.708, 483.26552961767754), (-4.708, 483.1055296176775), (-8.80000000001151, 483.5120239905324), (-8.80000000001151, 483.2020239905324), (-0.300000000018094, 482.83), (-0.300000000018094, 482.71), (-4.708, 483.0955296176775), (-4.708, 482.93552961767756), (-4.708, 483.1055296176775), (-4.708, 482.94552961767755), (-8.80000000001151, 483.2020239905324), (-8.80000000001151, 482.8920239905324)]</t>
+          <t>[(-21198.25938593752, 65889.27149846731), (-21198.25938593752, 65889.10149846731), (-21202.6673859375, 65889.53702808499), (-21202.6673859375, 65889.36702808499), (-21202.6673859375, 65889.53702808499), (-21202.6673859375, 65889.37702808499), (-21206.759385937512, 65889.78352245784), (-21206.759385937512, 65889.47352245785), (-21198.25938593752, 65889.10149846731), (-21198.25938593752, 65888.98149846731), (-21202.6673859375, 65889.36702808499), (-21202.6673859375, 65889.20702808499), (-21202.6673859375, 65889.37702808499), (-21202.6673859375, 65889.21702808498), (-21206.759385937512, 65889.47352245785), (-21206.759385937512, 65889.16352245785)]</t>
         </is>
       </c>
     </row>
@@ -5267,7 +5267,7 @@
       </c>
       <c r="B485" t="inlineStr">
         <is>
-          <t>[(-0.299999999992888, 484.0), (-0.299999999992888, 483.82), (-4.827, 484.23570330954647), (-4.827, 484.05570330954646), (-4.827, 484.23570330954647), (-4.827, 484.05570330954646), (-8.79999999998665, 484.44256199053245), (-8.79999999998665, 484.13256199053245), (-0.299999999992888, 483.82), (-0.299999999992888, 483.69), (-4.827, 484.05570330954646), (-4.827, 483.87570330954645), (-4.827, 484.05570330954646), (-4.827, 483.87570330954645), (-8.79999999998665, 484.13256199053245), (-8.79999999998665, 483.82256199053245)]</t>
+          <t>[(-21011.059385937493, 65889.6977255177), (-21011.059385937493, 65889.51772551771), (-21015.586385937502, 65889.93342882725), (-21015.586385937502, 65889.75342882726), (-21015.586385937502, 65889.93342882725), (-21015.586385937502, 65889.75342882726), (-21019.55938593749, 65890.14028750824), (-21019.55938593749, 65889.83028750824), (-21011.059385937493, 65889.51772551771), (-21011.059385937493, 65889.3877255177), (-21015.586385937502, 65889.75342882726), (-21015.586385937502, 65889.57342882725), (-21015.586385937502, 65889.75342882726), (-21015.586385937502, 65889.57342882725), (-21019.55938593749, 65889.83028750824), (-21019.55938593749, 65889.52028750825)]</t>
         </is>
       </c>
     </row>
@@ -5277,7 +5277,7 @@
       </c>
       <c r="B486" t="inlineStr">
         <is>
-          <t>[(-0.300000000049893, 485.0), (-0.300000000049893, 484.82), (-5.008, 485.20665350063643), (-5.008, 485.0266535006364), (-5.008, 485.20665350063643), (-5.008, 485.0266535006364), (-8.79999999999442, 485.3730999905303), (-8.79999999999442, 485.0730999905303), (-0.300000000049893, 484.82), (-0.300000000049893, 484.67), (-5.008, 485.0266535006364), (-5.008, 484.8566535006364), (-5.008, 485.0266535006364), (-5.008, 484.8466535006364), (-8.79999999999442, 485.0730999905303), (-8.79999999999442, 484.7730999905303)]</t>
+          <t>[(-20824.85938593765, 65890.1239525681), (-20824.85938593765, 65889.94395256811), (-20829.5673859376, 65890.33060606873), (-20829.5673859376, 65890.15060606874), (-20829.5673859376, 65890.33060606873), (-20829.5673859376, 65890.15060606874), (-20833.359385937594, 65890.49705255863), (-20833.359385937594, 65890.19705255862), (-20824.85938593765, 65889.94395256811), (-20824.85938593765, 65889.7939525681), (-20829.5673859376, 65890.15060606874), (-20829.5673859376, 65889.98060606873), (-20829.5673859376, 65890.15060606874), (-20829.5673859376, 65889.97060606873), (-20833.359385937594, 65890.19705255862), (-20833.359385937594, 65889.89705255862)]</t>
         </is>
       </c>
     </row>
@@ -5287,7 +5287,7 @@
       </c>
       <c r="B487" t="inlineStr">
         <is>
-          <t>[(-0.30000000013227, 486.0), (-0.30000000013227, 485.85), (-5.129, 486.17250210073445), (-5.129, 486.02250210073447), (-5.129, 486.17250210073445), (-5.129, 485.96250210073447), (-8.79999999999924, 486.30363799052805), (-8.79999999999924, 485.96363799052807), (-0.30000000013227, 485.85), (-0.30000000013227, 485.7), (-5.129, 486.02250210073447), (-5.129, 485.87250210073444), (-5.129, 485.96250210073447), (-5.129, 485.75250210073443), (-8.79999999999924, 485.96363799052807), (-8.79999999999924, 485.62363799052804), (-0.30000000013227, 485.7), (-0.30000000013227, 485.58), (-5.129, 485.87250210073444), (-5.129, 485.75250210073443), (-5.129, 485.75250210073443), (-5.129, 485.75250210073443), (-8.79999999999924, 485.62363799052804), (-8.79999999999924, 485.62363799052804)]</t>
+          <t>[(-20824.859385937634, 65942.5501796186), (-20824.859385937634, 65942.4001796186), (-20829.6883859375, 65942.72268171933), (-20829.6883859375, 65942.57268171934), (-20829.6883859375, 65942.72268171933), (-20829.6883859375, 65942.51268171932), (-20833.3593859375, 65942.85381760912), (-20833.3593859375, 65942.51381760913), (-20824.859385937634, 65942.4001796186), (-20824.859385937634, 65942.2501796186), (-20829.6883859375, 65942.57268171934), (-20829.6883859375, 65942.42268171933), (-20829.6883859375, 65942.51268171932), (-20829.6883859375, 65942.30268171933), (-20833.3593859375, 65942.51381760913), (-20833.3593859375, 65942.17381760913), (-20824.859385937634, 65942.2501796186), (-20824.859385937634, 65942.1301796186), (-20829.6883859375, 65942.42268171933), (-20829.6883859375, 65942.30268171933), (-20829.6883859375, 65942.30268171933), (-20829.6883859375, 65942.30268171933), (-20833.3593859375, 65942.17381760913), (-20833.3593859375, 65942.17381760913)]</t>
         </is>
       </c>
     </row>
@@ -5297,7 +5297,7 @@
       </c>
       <c r="B488" t="inlineStr">
         <is>
-          <t>[(-0.300000000002996, 487.0), (-0.300000000002996, 486.82), (-5.221, 487.1355741234601), (-5.221, 486.9555741234601), (-5.221, 487.1355741234601), (-5.221, 486.8855741234601), (-8.79999999998253, 487.2341759905322), (-8.79999999998253, 486.8741759905322), (-0.300000000002996, 486.82), (-0.300000000002996, 486.64), (-5.221, 486.9555741234601), (-5.221, 486.7755741234601), (-5.221, 486.8855741234601), (-5.221, 486.6355741234601), (-8.79999999998253, 486.8741759905322), (-8.79999999998253, 486.5141759905322), (-0.300000000002996, 486.64), (-0.300000000002996, 486.48), (-5.221, 486.7755741234601), (-5.221, 486.6355741234601), (-5.221, 486.6355741234601), (-5.221, 486.6355741234601), (-8.79999999998253, 486.5141759905322), (-8.79999999998253, 486.5141759905322)]</t>
+          <t>[(-20744.859385937503, 65888.976406669), (-20744.859385937503, 65888.796406669), (-20749.7803859375, 65889.11198079246), (-20749.7803859375, 65888.93198079246), (-20749.7803859375, 65889.11198079246), (-20749.7803859375, 65888.86198079246), (-20753.35938593748, 65889.21058265954), (-20753.35938593748, 65888.85058265954), (-20744.859385937503, 65888.796406669), (-20744.859385937503, 65888.616406669), (-20749.7803859375, 65888.93198079246), (-20749.7803859375, 65888.75198079245), (-20749.7803859375, 65888.86198079246), (-20749.7803859375, 65888.61198079246), (-20753.35938593748, 65888.85058265954), (-20753.35938593748, 65888.49058265953), (-20744.859385937503, 65888.616406669), (-20744.859385937503, 65888.45640666899), (-20749.7803859375, 65888.75198079245), (-20749.7803859375, 65888.61198079246), (-20749.7803859375, 65888.61198079246), (-20749.7803859375, 65888.61198079246), (-20753.35938593748, 65888.49058265953), (-20753.35938593748, 65888.49058265953)]</t>
         </is>
       </c>
     </row>
@@ -5307,7 +5307,7 @@
       </c>
       <c r="B489" t="inlineStr">
         <is>
-          <t>[(-0.299999999994406, 488.0), (-0.299999999994406, 487.7), (-5.246, 488.0385856472514), (-5.246, 487.7385856472514), (-5.246, 488.0385856472514), (-5.246, 487.7985856472514), (-8.79999999999288, 488.06631176741536), (-8.79999999999288, 487.7263117674154), (-0.299999999994406, 487.7), (-0.299999999994406, 487.41), (-5.246, 487.7385856472514), (-5.246, 487.5585856472514), (-5.246, 487.7985856472514), (-5.246, 487.5585856472514), (-8.79999999999288, 487.7263117674154), (-8.79999999999288, 487.38631176741535)]</t>
+          <t>[(-20744.859385937496, 65941.4026337195), (-20744.859385937496, 65941.10263371949), (-20749.8053859375, 65941.44121936675), (-20749.8053859375, 65941.14121936675), (-20749.8053859375, 65941.44121936675), (-20749.8053859375, 65941.20121936675), (-20753.359385937492, 65941.46894548691), (-20753.359385937492, 65941.12894548691), (-20744.859385937496, 65941.10263371949), (-20744.859385937496, 65940.8126337195), (-20749.8053859375, 65941.14121936675), (-20749.8053859375, 65940.96121936676), (-20749.8053859375, 65941.20121936675), (-20749.8053859375, 65940.96121936676), (-20753.359385937492, 65941.12894548691), (-20753.359385937492, 65940.78894548691)]</t>
         </is>
       </c>
     </row>
@@ -5317,7 +5317,7 @@
       </c>
       <c r="B490" t="inlineStr">
         <is>
-          <t>[(-0.299999999994406, 489.0), (-0.299999999994406, 488.73), (-5.258, 488.9147292638641), (-5.258, 488.6447292638641), (-5.258, 488.9147292638641), (-5.258, 488.6547292638641), (-8.79999999999288, 488.85381176741544), (-8.79999999999288, 488.59381176741545), (-0.299999999994406, 488.73), (-0.299999999994406, 488.43), (-5.258, 488.6447292638641), (-5.258, 488.5247292638641), (-5.258, 488.6547292638641), (-5.258, 488.5247292638641), (-8.79999999999288, 488.59381176741545), (-8.79999999999288, 488.34381176741545)]</t>
+          <t>[(-20633.659385937495, 65889.8288607699), (-20633.659385937495, 65889.5588607699), (-20638.6173859375, 65889.74359003377), (-20638.6173859375, 65889.47359003377), (-20638.6173859375, 65889.74359003377), (-20638.6173859375, 65889.48359003378), (-20642.15938593749, 65889.68267253732), (-20642.15938593749, 65889.42267253733), (-20633.659385937495, 65889.5588607699), (-20633.659385937495, 65889.2588607699), (-20638.6173859375, 65889.47359003377), (-20638.6173859375, 65889.35359003377), (-20638.6173859375, 65889.48359003378), (-20638.6173859375, 65889.35359003377), (-20642.15938593749, 65889.42267253733), (-20642.15938593749, 65889.17267253733)]</t>
         </is>
       </c>
     </row>
@@ -5327,7 +5327,7 @@
       </c>
       <c r="B491" t="inlineStr">
         <is>
-          <t>[(-0.299999999994406, 490.0), (-0.299999999994406, 489.69), (-5.217, 489.8770749999999), (-5.217, 489.6870749999999), (-5.217, 489.8770749999999), (-5.217, 489.6270749999999), (-8.79999999999288, 489.7875), (-8.79999999999288, 489.5375), (-0.299999999994406, 489.69), (-0.299999999994406, 489.38), (-5.217, 489.6870749999999), (-5.217, 489.4970749999999), (-5.217, 489.6270749999999), (-5.217, 489.4970749999999), (-8.79999999999288, 489.5375), (-8.79999999999288, 489.2975)]</t>
+          <t>[(-20633.659385937495, 65942.2550878203), (-20633.659385937495, 65941.9450878203), (-20638.5763859375, 65942.1321628203), (-20638.5763859375, 65941.9421628203), (-20638.5763859375, 65942.1321628203), (-20638.5763859375, 65941.8821628203), (-20642.15938593749, 65942.04258782031), (-20642.15938593749, 65941.79258782031), (-20633.659385937495, 65941.9450878203), (-20633.659385937495, 65941.63508782031), (-20638.5763859375, 65941.9421628203), (-20638.5763859375, 65941.7521628203), (-20638.5763859375, 65941.8821628203), (-20638.5763859375, 65941.7521628203), (-20642.15938593749, 65941.79258782031), (-20642.15938593749, 65941.5525878203)]</t>
         </is>
       </c>
     </row>
@@ -5337,7 +5337,7 @@
       </c>
       <c r="B492" t="inlineStr">
         <is>
-          <t>[(-0.299999999992618, 491.0), (-0.299999999992618, 490.68), (-5.197, 490.8775749999998), (-5.197, 490.6775749999998), (-5.197, 490.8775749999998), (-5.197, 490.6175749999998), (-8.79999999999109, 490.7875), (-8.79999999999109, 490.52750000000003), (-0.299999999992618, 490.68), (-0.299999999992618, 490.36), (-5.197, 490.6775749999998), (-5.197, 490.47757499999983), (-5.197, 490.6175749999998), (-5.197, 490.4875749999998), (-8.79999999999109, 490.52750000000003), (-8.79999999999109, 490.26750000000004)]</t>
+          <t>[(-20448.45938593749, 65888.6292296054), (-20448.45938593749, 65888.3092296054), (-20453.3563859375, 65888.50680460541), (-20453.3563859375, 65888.30680460541), (-20453.3563859375, 65888.50680460541), (-20453.3563859375, 65888.24680460541), (-20456.95938593749, 65888.41672960541), (-20456.95938593749, 65888.15672960541), (-20448.45938593749, 65888.3092296054), (-20448.45938593749, 65887.9892296054), (-20453.3563859375, 65888.30680460541), (-20453.3563859375, 65888.10680460541), (-20453.3563859375, 65888.24680460541), (-20453.3563859375, 65888.11680460541), (-20456.95938593749, 65888.15672960541), (-20456.95938593749, 65887.8967296054)]</t>
         </is>
       </c>
     </row>
@@ -5347,7 +5347,7 @@
       </c>
       <c r="B493" t="inlineStr">
         <is>
-          <t>[(-0.299999999994406, 492.0), (-0.299999999994406, 491.68), (-5.221, 491.87697499999985), (-5.221, 491.67697499999986), (-5.221, 491.87697499999985), (-5.221, 491.60697499999986), (-8.79999999999288, 491.7875), (-8.79999999999288, 491.51750000000004), (-0.299999999994406, 491.68), (-0.299999999994406, 491.36), (-5.221, 491.67697499999986), (-5.221, 491.47697499999987), (-5.221, 491.60697499999986), (-5.221, 491.47697499999987), (-8.79999999999288, 491.51750000000004), (-8.79999999999288, 491.2475)]</t>
+          <t>[(-20448.459385937495, 65940.9602899508), (-20448.459385937495, 65940.6402899508), (-20453.3803859375, 65940.83726495081), (-20453.3803859375, 65940.63726495081), (-20453.3803859375, 65940.83726495081), (-20453.3803859375, 65940.5672649508), (-20456.95938593749, 65940.74778995081), (-20456.95938593749, 65940.4777899508), (-20448.459385937495, 65940.6402899508), (-20448.459385937495, 65940.3202899508), (-20453.3803859375, 65940.63726495081), (-20453.3803859375, 65940.43726495082), (-20453.3803859375, 65940.5672649508), (-20453.3803859375, 65940.43726495082), (-20456.95938593749, 65940.4777899508), (-20456.95938593749, 65940.20778995081)]</t>
         </is>
       </c>
     </row>
@@ -5357,7 +5357,7 @@
       </c>
       <c r="B494" t="inlineStr">
         <is>
-          <t>[(-0.299999999994406, 493.0), (-0.299999999994406, 492.68), (-5.159, 492.87852499999985), (-5.159, 492.67852499999987), (-5.159, 492.87852499999985), (-5.159, 492.6085249999999), (-8.79999999999288, 492.7875), (-8.79999999999288, 492.51750000000004), (-0.299999999994406, 492.68), (-0.299999999994406, 492.36), (-5.159, 492.67852499999987), (-5.159, 492.4785249999999), (-5.159, 492.6085249999999), (-5.159, 492.48852499999987), (-8.79999999999288, 492.51750000000004), (-8.79999999999288, 492.25750000000005)]</t>
+          <t>[(-20368.459385937495, 65887.2913502961), (-20368.459385937495, 65886.9713502961), (-20373.3183859375, 65887.1698752961), (-20373.3183859375, 65886.9698752961), (-20373.3183859375, 65887.1698752961), (-20373.3183859375, 65886.89987529609), (-20376.95938593749, 65887.07885029611), (-20376.95938593749, 65886.8088502961), (-20368.459385937495, 65886.9713502961), (-20368.459385937495, 65886.6513502961), (-20373.3183859375, 65886.9698752961), (-20373.3183859375, 65886.7698752961), (-20373.3183859375, 65886.89987529609), (-20373.3183859375, 65886.7798752961), (-20376.95938593749, 65886.8088502961), (-20376.95938593749, 65886.54885029611)]</t>
         </is>
       </c>
     </row>
@@ -5367,7 +5367,7 @@
       </c>
       <c r="B495" t="inlineStr">
         <is>
-          <t>[(-0.299999999994406, 494.0), (-0.299999999994406, 493.65), (-5.114, 493.87964999999986), (-5.114, 493.63964999999985), (-5.114, 493.87964999999986), (-5.114, 493.57964999999984), (-8.79999999999288, 493.7875), (-8.79999999999288, 493.4875), (-0.299999999994406, 493.65), (-0.299999999994406, 493.3), (-5.114, 493.63964999999985), (-5.114, 493.39964999999984), (-5.114, 493.57964999999984), (-5.114, 493.38964999999985), (-8.79999999999288, 493.4875), (-8.79999999999288, 493.1875)]</t>
+          <t>[(-20368.459385937495, 65939.6224106415), (-20368.459385937495, 65939.2724106415), (-20373.2733859375, 65939.5020606415), (-20373.2733859375, 65939.2620606415), (-20373.2733859375, 65939.5020606415), (-20373.2733859375, 65939.2020606415), (-20376.95938593749, 65939.40991064151), (-20376.95938593749, 65939.1099106415), (-20368.459385937495, 65939.2724106415), (-20368.459385937495, 65938.9224106415), (-20373.2733859375, 65939.2620606415), (-20373.2733859375, 65939.02206064151), (-20373.2733859375, 65939.2020606415), (-20373.2733859375, 65939.0120606415), (-20376.95938593749, 65939.1099106415), (-20376.95938593749, 65938.8099106415)]</t>
         </is>
       </c>
     </row>
@@ -5377,7 +5377,7 @@
       </c>
       <c r="B496" t="inlineStr">
         <is>
-          <t>[(-0.299999999992618, 495.0), (-0.299999999992618, 494.66), (-5.078, 494.8805499999998), (-5.078, 494.6205499999998), (-5.078, 494.8805499999998), (-5.078, 494.6205499999998), (-8.79999999999109, 494.7875), (-8.79999999999109, 494.44750000000005), (-0.299999999992618, 494.66), (-0.299999999992618, 494.32), (-5.078, 494.6205499999998), (-5.078, 494.3605499999998), (-5.078, 494.6205499999998), (-5.078, 494.3605499999998), (-8.79999999999109, 494.44750000000005), (-8.79999999999109, 494.1075)]</t>
+          <t>[(-20260.259385937494, 65887.9534709868), (-20260.259385937494, 65887.6134709868), (-20265.037385937503, 65887.8340209868), (-20265.037385937503, 65887.57402098681), (-20265.037385937503, 65887.8340209868), (-20265.037385937503, 65887.57402098681), (-20268.759385937494, 65887.74097098681), (-20268.759385937494, 65887.40097098681), (-20260.259385937494, 65887.6134709868), (-20260.259385937494, 65887.27347098681), (-20265.037385937503, 65887.57402098681), (-20265.037385937503, 65887.3140209868), (-20265.037385937503, 65887.57402098681), (-20265.037385937503, 65887.3140209868), (-20268.759385937494, 65887.40097098681), (-20268.759385937494, 65887.06097098681)]</t>
         </is>
       </c>
     </row>
@@ -5387,7 +5387,7 @@
       </c>
       <c r="B497" t="inlineStr">
         <is>
-          <t>[(-0.299999999992618, 496.0), (-0.299999999992618, 495.78), (-5.063, 495.8809249999998), (-5.063, 495.6609249999998), (-5.063, 495.8809249999998), (-5.063, 495.5909249999998), (-8.79999999999109, 495.7875), (-8.79999999999109, 495.4075), (-0.299999999992618, 495.78), (-0.299999999992618, 495.56), (-5.063, 495.6609249999998), (-5.063, 495.4409249999998), (-5.063, 495.5909249999998), (-5.063, 495.30092499999984), (-8.79999999999109, 495.4075), (-8.79999999999109, 495.02750000000003), (-0.299999999992618, 495.56), (-0.299999999992618, 495.36), (-5.063, 495.4409249999998), (-5.063, 495.30092499999984), (-5.063, 495.30092499999984), (-5.063, 495.30092499999984), (-8.79999999999109, 495.02750000000003), (-8.79999999999109, 495.02750000000003)]</t>
+          <t>[(-20260.259385937494, 65936.2649848334), (-20260.259385937494, 65936.0449848334), (-20265.0223859375, 65936.1459098334), (-20265.0223859375, 65935.9259098334), (-20265.0223859375, 65936.1459098334), (-20265.0223859375, 65935.85590983341), (-20268.759385937494, 65936.0524848334), (-20268.759385937494, 65935.6724848334), (-20260.259385937494, 65936.0449848334), (-20260.259385937494, 65935.8249848334), (-20265.0223859375, 65935.9259098334), (-20265.0223859375, 65935.7059098334), (-20265.0223859375, 65935.85590983341), (-20265.0223859375, 65935.5659098334), (-20268.759385937494, 65935.6724848334), (-20268.759385937494, 65935.29248483341), (-20260.259385937494, 65935.8249848334), (-20260.259385937494, 65935.6249848334), (-20265.0223859375, 65935.7059098334), (-20265.0223859375, 65935.5659098334), (-20265.0223859375, 65935.5659098334), (-20265.0223859375, 65935.5659098334), (-20268.759385937494, 65935.29248483341), (-20268.759385937494, 65935.29248483341)]</t>
         </is>
       </c>
     </row>
@@ -5397,7 +5397,7 @@
       </c>
       <c r="B498" t="inlineStr">
         <is>
-          <t>[(-0.300000000075493, 497.0), (-0.300000000075493, 496.69), (-5.088, 496.8522459061728), (-5.088, 496.5922459061728), (-5.088, 496.8522459061728), (-5.088, 496.5922459061728), (-8.79999999998839, 496.737696366429), (-8.79999999998839, 496.377696366429), (-0.300000000075493, 496.69), (-0.300000000075493, 496.38), (-5.088, 496.5922459061728), (-5.088, 496.33224590617283), (-5.088, 496.5922459061728), (-5.088, 496.33224590617283), (-8.79999999998839, 496.377696366429), (-8.79999999998839, 496.017696366429)]</t>
+          <t>[(-20070.059385937577, 65886.5153653057), (-20070.059385937577, 65886.20536530571), (-20074.8473859375, 65886.36761121188), (-20074.8473859375, 65886.10761121189), (-20074.8473859375, 65886.36761121188), (-20074.8473859375, 65886.10761121189), (-20078.55938593749, 65886.25306167213), (-20078.55938593749, 65885.89306167213), (-20070.059385937577, 65886.20536530571), (-20070.059385937577, 65885.89536530571), (-20074.8473859375, 65886.10761121189), (-20074.8473859375, 65885.84761121188), (-20074.8473859375, 65886.10761121189), (-20074.8473859375, 65885.84761121188), (-20078.55938593749, 65885.89306167213), (-20078.55938593749, 65885.53306167213)]</t>
         </is>
       </c>
     </row>
@@ -5407,7 +5407,7 @@
       </c>
       <c r="B499" t="inlineStr">
         <is>
-          <t>[(-0.300000000029171, 498.0), (-0.300000000029171, 497.79), (-5.187, 497.80034608329225), (-5.187, 497.5903460832923), (-5.187, 497.80034608329225), (-5.187, 497.5203460832923), (-8.79999999999721, 497.6527402717374), (-8.79999999999721, 497.2827402717374), (-0.300000000029171, 497.79), (-0.300000000029171, 497.58), (-5.187, 497.5903460832923), (-5.187, 497.38034608329224), (-5.187, 497.5203460832923), (-5.187, 497.24034608329225), (-8.79999999999721, 497.2827402717374), (-8.79999999999721, 496.9127402717374), (-0.300000000029171, 497.58), (-0.300000000029171, 497.37), (-5.187, 497.38034608329224), (-5.187, 497.23034608329226), (-5.187, 497.24034608329225), (-5.187, 497.24034608329225), (-8.79999999999721, 496.9127402717374), (-8.79999999999721, 496.9127402717374)]</t>
+          <t>[(-20070.05938593753, 65938.703245778), (-20070.05938593753, 65938.493245778), (-20074.946385937503, 65938.5035918613), (-20074.946385937503, 65938.2935918613), (-20074.946385937503, 65938.5035918613), (-20074.946385937503, 65938.2235918613), (-20078.559385937497, 65938.35598604973), (-20078.559385937497, 65937.98598604974), (-20070.05938593753, 65938.493245778), (-20070.05938593753, 65938.283245778), (-20074.946385937503, 65938.2935918613), (-20074.946385937503, 65938.0835918613), (-20074.946385937503, 65938.2235918613), (-20074.946385937503, 65937.9435918613), (-20078.559385937497, 65937.98598604974), (-20078.559385937497, 65937.61598604973), (-20070.05938593753, 65938.283245778), (-20070.05938593753, 65938.073245778), (-20074.946385937503, 65938.0835918613), (-20074.946385937503, 65937.93359186129), (-20074.946385937503, 65937.9435918613), (-20074.946385937503, 65937.9435918613), (-20078.559385937497, 65937.61598604973), (-20078.559385937497, 65937.61598604973)]</t>
         </is>
       </c>
     </row>
@@ -5417,7 +5417,7 @@
       </c>
       <c r="B500" t="inlineStr">
         <is>
-          <t>[(-0.299999999990458, 499.0), (-0.299999999990458, 498.64), (-5.357, 498.7428570098019), (-5.357, 498.4528570098019), (-5.357, 498.7428570098019), (-5.357, 498.4528570098019), (-8.79999999998244, 498.56778417704624), (-8.79999999998244, 498.2077841770462), (-0.299999999990458, 498.64), (-0.299999999990458, 498.28), (-5.357, 498.4528570098019), (-5.357, 498.16285700980194), (-5.357, 498.4528570098019), (-5.357, 498.16285700980194), (-8.79999999998244, 498.2077841770462), (-8.79999999998244, 497.8477841770462)]</t>
+          <t>[(-19883.859385937492, 65886.8286262503), (-19883.859385937492, 65886.4686262503), (-19888.9163859375, 65886.5714832601), (-19888.9163859375, 65886.2814832601), (-19888.9163859375, 65886.5714832601), (-19888.9163859375, 65886.2814832601), (-19892.35938593748, 65886.39641042735), (-19892.35938593748, 65886.03641042735), (-19883.859385937492, 65886.4686262503), (-19883.859385937492, 65886.1086262503), (-19888.9163859375, 65886.2814832601), (-19888.9163859375, 65885.99148326009), (-19888.9163859375, 65886.2814832601), (-19888.9163859375, 65885.99148326009), (-19892.35938593748, 65886.03641042735), (-19892.35938593748, 65885.67641042735)]</t>
         </is>
       </c>
     </row>
@@ -5427,7 +5427,7 @@
       </c>
       <c r="B501" t="inlineStr">
         <is>
-          <t>[(-0.299999999991877, 500.0), (-0.299999999991877, 499.63), (-5.533, 499.68160462999555), (-5.533, 499.4016046299956), (-5.533, 499.68160462999555), (-5.533, 499.4016046299956), (-8.79999999999738, 499.4828280823552), (-8.79999999999738, 499.1428280823552), (-0.299999999991877, 499.63), (-0.299999999991877, 499.26), (-5.533, 499.4016046299956), (-5.533, 499.12160462999555), (-5.533, 499.4016046299956), (-5.533, 499.12160462999555), (-8.79999999999738, 499.1428280823552), (-8.79999999999738, 498.8028280823552)]</t>
+          <t>[(-19883.85938593759, 65940.8915067226), (-19883.85938593759, 65940.52150672261), (-19889.092385937598, 65940.5731113526), (-19889.092385937598, 65940.2931113526), (-19889.092385937598, 65940.5731113526), (-19889.092385937598, 65940.2931113526), (-19892.359385937594, 65940.37433480496), (-19892.359385937594, 65940.03433480496), (-19883.85938593759, 65940.52150672261), (-19883.85938593759, 65940.1515067226), (-19889.092385937598, 65940.2931113526), (-19889.092385937598, 65940.0131113526), (-19889.092385937598, 65940.2931113526), (-19889.092385937598, 65940.0131113526), (-19892.359385937594, 65940.03433480496), (-19892.359385937594, 65939.69433480497)]</t>
         </is>
       </c>
     </row>
@@ -5437,7 +5437,7 @@
       </c>
       <c r="B502" t="inlineStr">
         <is>
-          <t>[(-0.299999999993062, 501.0), (-0.299999999993062, 500.62), (-5.774, 500.6168199999995), (-5.774, 500.3568199999995), (-5.774, 500.6168199999995), (-5.774, 500.3568199999995), (-8.79999999999353, 500.405), (-8.79999999999353, 500.085), (-0.299999999993062, 500.62), (-0.299999999993062, 500.24), (-5.774, 500.3568199999995), (-5.774, 500.0968199999995), (-5.774, 500.3568199999995), (-5.774, 500.0968199999995), (-8.79999999999353, 500.085), (-8.79999999999353, 499.765)]</t>
+          <t>[(-19806.859385937492, 65890.8918871949), (-19806.859385937492, 65890.5118871949), (-19812.3333859375, 65890.5087071949), (-19812.3333859375, 65890.2487071949), (-19812.3333859375, 65890.5087071949), (-19812.3333859375, 65890.2487071949), (-19815.359385937492, 65890.2968871949), (-19815.359385937492, 65889.97688719489), (-19806.859385937492, 65890.5118871949), (-19806.859385937492, 65890.1318871949), (-19812.3333859375, 65890.2487071949), (-19812.3333859375, 65889.98870719489), (-19812.3333859375, 65890.2487071949), (-19812.3333859375, 65889.98870719489), (-19815.359385937492, 65889.97688719489), (-19815.359385937492, 65889.6568871949)]</t>
         </is>
       </c>
     </row>
@@ -5447,7 +5447,7 @@
       </c>
       <c r="B503" t="inlineStr">
         <is>
-          <t>[(-0.299999999985769, 502.0), (-0.299999999985769, 501.66), (-5.857, 501.611009999999), (-5.857, 501.39100999999897), (-5.857, 501.611009999999), (-5.857, 501.331009999999), (-8.79999999998793, 501.40499999999986), (-8.79999999998793, 501.1249999999999), (-0.299999999985769, 501.66), (-0.299999999985769, 501.32), (-5.857, 501.39100999999897), (-5.857, 501.171009999999), (-5.857, 501.331009999999), (-5.857, 501.161009999999), (-8.79999999998793, 501.1249999999999), (-8.79999999998793, 500.85499999999985)]</t>
+          <t>[(-19806.859385937485, 65938.82976766721), (-19806.859385937485, 65938.48976766721), (-19812.4163859375, 65938.4407776672), (-19812.4163859375, 65938.2207776672), (-19812.4163859375, 65938.4407776672), (-19812.4163859375, 65938.1607776672), (-19815.35938593749, 65938.2347676672), (-19815.35938593749, 65937.95476766721), (-19806.859385937485, 65938.48976766721), (-19806.859385937485, 65938.14976766722), (-19812.4163859375, 65938.2207776672), (-19812.4163859375, 65938.0007776672), (-19812.4163859375, 65938.1607776672), (-19812.4163859375, 65937.9907776672), (-19815.35938593749, 65937.95476766721), (-19815.35938593749, 65937.6847676672)]</t>
         </is>
       </c>
     </row>
@@ -5457,7 +5457,7 @@
       </c>
       <c r="B504" t="inlineStr">
         <is>
-          <t>[(-0.299999999982385, 503.0), (-0.299999999982385, 502.66), (-5.904, 502.6077199999988), (-5.904, 502.3577199999988), (-5.904, 502.6077199999988), (-5.904, 502.30771999999877), (-8.79999999998564, 502.40499999999975), (-8.79999999998564, 502.10499999999973), (-0.299999999982385, 502.66), (-0.299999999982385, 502.32), (-5.904, 502.3577199999988), (-5.904, 502.1077199999988), (-5.904, 502.30771999999877), (-5.904, 502.1077199999988), (-8.79999999998564, 502.10499999999973), (-8.79999999998564, 501.8049999999997)]</t>
+          <t>[(-19693.65938593748, 65890.7051481395), (-19693.65938593748, 65890.3651481395), (-19699.2633859375, 65890.3128681395), (-19699.2633859375, 65890.0628681395), (-19699.2633859375, 65890.3128681395), (-19699.2633859375, 65890.0128681395), (-19702.159385937484, 65890.1101481395), (-19702.159385937484, 65889.8101481395), (-19693.65938593748, 65890.3651481395), (-19693.65938593748, 65890.02514813951), (-19699.2633859375, 65890.0628681395), (-19699.2633859375, 65889.8128681395), (-19699.2633859375, 65890.0128681395), (-19699.2633859375, 65889.8128681395), (-19702.159385937484, 65889.8101481395), (-19702.159385937484, 65889.5101481395)]</t>
         </is>
       </c>
     </row>
@@ -5467,7 +5467,7 @@
       </c>
       <c r="B505" t="inlineStr">
         <is>
-          <t>[(-0.299999999992593, 504.0), (-0.299999999992593, 503.6), (-5.981, 503.6023299999995), (-5.981, 503.3223299999995), (-5.981, 503.6023299999995), (-5.981, 503.3223299999995), (-8.80000000000243, 503.4049999999993), (-8.80000000000243, 503.05499999999927), (-0.299999999992593, 503.6), (-0.299999999992593, 503.2), (-5.981, 503.3223299999995), (-5.981, 503.0423299999995), (-5.981, 503.3223299999995), (-5.981, 503.0423299999995), (-8.80000000000243, 503.05499999999927), (-8.80000000000243, 502.7049999999993)]</t>
+          <t>[(-19693.65938593749, 65936.5180286118), (-19693.65938593749, 65936.1180286118), (-19699.3403859375, 65936.12035861179), (-19699.3403859375, 65935.8403586118), (-19699.3403859375, 65936.12035861179), (-19699.3403859375, 65935.8403586118), (-19702.159385937503, 65935.9230286118), (-19702.159385937503, 65935.57302861179), (-19693.65938593749, 65936.1180286118), (-19693.65938593749, 65935.7180286118), (-19699.3403859375, 65935.8403586118), (-19699.3403859375, 65935.5603586118), (-19699.3403859375, 65935.8403586118), (-19699.3403859375, 65935.5603586118), (-19702.159385937503, 65935.57302861179), (-19702.159385937503, 65935.2230286118)]</t>
         </is>
       </c>
     </row>
@@ -5477,7 +5477,7 @@
       </c>
       <c r="B506" t="inlineStr">
         <is>
-          <t>[(-0.300000000005262, 505.0), (-0.300000000005262, 504.6), (-5.857, 504.61101000000036), (-5.857, 504.30101000000036), (-5.857, 504.61101000000036), (-5.857, 504.36101000000036), (-8.79999999999439, 504.40500000000077), (-8.79999999999439, 504.15500000000077), (-0.300000000005262, 504.6), (-0.300000000005262, 504.2), (-5.857, 504.30101000000036), (-5.857, 503.99101000000036), (-5.857, 504.36101000000036), (-5.857, 504.11101000000036), (-8.79999999999439, 504.15500000000077), (-8.79999999999439, 503.90500000000077)]</t>
+          <t>[(-19634.659385937506, 65894.2684090841), (-19634.659385937506, 65893.86840908411), (-19640.2163859375, 65893.8794190841), (-19640.2163859375, 65893.5694190841), (-19640.2163859375, 65893.8794190841), (-19640.2163859375, 65893.6294190841), (-19643.159385937495, 65893.6734090841), (-19643.159385937495, 65893.4234090841), (-19634.659385937506, 65893.86840908411), (-19634.659385937506, 65893.4684090841), (-19640.2163859375, 65893.5694190841), (-19640.2163859375, 65893.2594190841), (-19640.2163859375, 65893.6294190841), (-19640.2163859375, 65893.3794190841), (-19643.159385937495, 65893.4234090841), (-19643.159385937495, 65893.1734090841)]</t>
         </is>
       </c>
     </row>
@@ -5487,7 +5487,7 @@
       </c>
       <c r="B507" t="inlineStr">
         <is>
-          <t>[(-0.300000000002308, 506.0), (-0.300000000002308, 505.62), (-5.566, 505.63138000000015), (-5.566, 505.37138000000016), (-5.566, 505.63138000000015), (-5.566, 505.37138000000016), (-8.80000000000209, 505.40500000000003), (-8.80000000000209, 505.08500000000004), (-0.300000000002308, 505.62), (-0.300000000002308, 505.24), (-5.566, 505.37138000000016), (-5.566, 505.11138000000017), (-5.566, 505.37138000000016), (-5.566, 505.11138000000017), (-8.80000000000209, 505.08500000000004), (-8.80000000000209, 504.76500000000004)]</t>
+          <t>[(-19634.659385937503, 65937.9562895564), (-19634.659385937503, 65937.5762895564), (-19639.9253859375, 65937.58766955641), (-19639.9253859375, 65937.32766955641), (-19639.9253859375, 65937.58766955641), (-19639.9253859375, 65937.32766955641), (-19643.159385937503, 65937.3612895564), (-19643.159385937503, 65937.0412895564), (-19634.659385937503, 65937.5762895564), (-19634.659385937503, 65937.1962895564), (-19639.9253859375, 65937.32766955641), (-19639.9253859375, 65937.0676695564), (-19639.9253859375, 65937.32766955641), (-19639.9253859375, 65937.0676695564), (-19643.159385937503, 65937.0412895564), (-19643.159385937503, 65936.7212895564)]</t>
         </is>
       </c>
     </row>
@@ -5497,7 +5497,7 @@
       </c>
       <c r="B508" t="inlineStr">
         <is>
-          <t>[(-0.300000000084319, 507.0), (-0.300000000084319, 506.72), (-5.221, 506.65559939136926), (-5.221, 506.3755993913693), (-5.221, 506.65559939136926), (-5.221, 506.41559939136926), (-8.80000000000457, 506.40511985909694), (-8.80000000000457, 506.16511985909693), (-0.300000000084319, 506.72), (-0.300000000084319, 506.42), (-5.221, 506.3755993913693), (-5.221, 506.2555993913693), (-5.221, 506.41559939136926), (-5.221, 506.2555993913693), (-8.80000000000457, 506.16511985909693), (-8.80000000000457, 505.9251198590969)]</t>
+          <t>[(-19508.959385937982, 65887.5816700287), (-19508.959385937982, 65887.3016700287), (-19513.8803859379, 65887.23726942006), (-19513.8803859379, 65886.95726942006), (-19513.8803859379, 65887.23726942006), (-19513.8803859379, 65886.99726942006), (-19517.459385937902, 65886.9867898878), (-19517.459385937902, 65886.7467898878), (-19508.959385937982, 65887.3016700287), (-19508.959385937982, 65887.0016700287), (-19513.8803859379, 65886.95726942006), (-19513.8803859379, 65886.83726942007), (-19513.8803859379, 65886.99726942006), (-19513.8803859379, 65886.83726942007), (-19517.459385937902, 65886.7467898878), (-19517.459385937902, 65886.5067898878)]</t>
         </is>
       </c>
     </row>
@@ -5507,7 +5507,7 @@
       </c>
       <c r="B509" t="inlineStr">
         <is>
-          <t>[(-0.300000000036697, 508.0), (-0.300000000036697, 507.74), (-4.862, 507.7263207648436), (-4.862, 507.4663207648436), (-4.862, 507.7263207648436), (-4.862, 507.4863207648436), (-8.80000000001613, 507.4900759537828), (-8.80000000001613, 507.2500759537828), (-0.300000000036697, 507.74), (-0.300000000036697, 507.48), (-4.862, 507.4663207648436), (-4.862, 507.3263207648436), (-4.862, 507.4863207648436), (-4.862, 507.3263207648436), (-8.80000000001613, 507.2500759537828), (-8.80000000001613, 507.0100759537828)]</t>
+          <t>[(-19508.959385937735, 65941.144550501), (-19508.959385937735, 65940.88455050101), (-19513.5213859377, 65940.87087126586), (-19513.5213859377, 65940.61087126586), (-19513.5213859377, 65940.87087126586), (-19513.5213859377, 65940.63087126585), (-19517.459385937716, 65940.63462645479), (-19517.459385937716, 65940.39462645478), (-19508.959385937735, 65940.88455050101), (-19508.959385937735, 65940.624550501), (-19513.5213859377, 65940.61087126586), (-19513.5213859377, 65940.47087126586), (-19513.5213859377, 65940.63087126585), (-19513.5213859377, 65940.47087126586), (-19517.459385937716, 65940.39462645478), (-19517.459385937716, 65940.1546264548)]</t>
         </is>
       </c>
     </row>
@@ -5517,7 +5517,7 @@
       </c>
       <c r="B510" t="inlineStr">
         <is>
-          <t>[(-0.299999999991776, 509.0), (-0.299999999991776, 508.81), (-4.666, 508.7817164616029), (-4.666, 508.5917164616029), (-4.666, 508.7817164616029), (-4.666, 508.6017164616029), (-8.80000000000376, 508.5750320484713), (-8.80000000000376, 508.3950320484713), (-0.299999999991776, 508.81), (-0.299999999991776, 508.51), (-4.666, 508.5917164616029), (-4.666, 508.4317164616029), (-4.666, 508.6017164616029), (-4.666, 508.4317164616029), (-8.80000000000376, 508.3950320484713), (-8.80000000000376, 508.0950320484713)]</t>
+          <t>[(-19445.45938593749, 65886.6449309733), (-19445.45938593749, 65886.4549309733), (-19449.8253859375, 65886.4266474349), (-19449.8253859375, 65886.2366474349), (-19449.8253859375, 65886.4266474349), (-19449.8253859375, 65886.2466474349), (-19453.9593859375, 65886.21996302177), (-19453.9593859375, 65886.03996302177), (-19445.45938593749, 65886.4549309733), (-19445.45938593749, 65886.1549309733), (-19449.8253859375, 65886.2366474349), (-19449.8253859375, 65886.0766474349), (-19449.8253859375, 65886.2466474349), (-19449.8253859375, 65886.0766474349), (-19453.9593859375, 65886.03996302177), (-19453.9593859375, 65885.73996302177)]</t>
         </is>
       </c>
     </row>
@@ -5527,7 +5527,7 @@
       </c>
       <c r="B511" t="inlineStr">
         <is>
-          <t>[(-0.300000000034003, 510.0), (-0.300000000034003, 509.88), (-4.571, 509.8291540422891), (-4.571, 509.7091540422891), (-4.571, 509.8291540422891), (-4.571, 509.66915404228905), (-8.8000000000224, 509.6599881431626), (-8.8000000000224, 509.49998814316257), (-0.300000000034003, 509.88), (-0.300000000034003, 509.58), (-4.571, 509.7091540422891), (-4.571, 509.5091540422891), (-4.571, 509.66915404228905), (-4.571, 509.5091540422891), (-8.8000000000224, 509.49998814316257), (-8.8000000000224, 509.1999881431626)]</t>
+          <t>[(-19440.459385937535, 65940.0828114456), (-19440.459385937535, 65939.9628114456), (-19444.7303859375, 65939.91196548789), (-19444.7303859375, 65939.7919654879), (-19444.7303859375, 65939.91196548789), (-19444.7303859375, 65939.75196548789), (-19448.95938593752, 65939.74279958876), (-19448.95938593752, 65939.58279958875), (-19440.459385937535, 65939.9628114456), (-19440.459385937535, 65939.6628114456), (-19444.7303859375, 65939.7919654879), (-19444.7303859375, 65939.59196548788), (-19444.7303859375, 65939.75196548789), (-19444.7303859375, 65939.59196548788), (-19448.95938593752, 65939.58279958875), (-19448.95938593752, 65939.28279958875)]</t>
         </is>
       </c>
     </row>
@@ -5537,7 +5537,7 @@
       </c>
       <c r="B512" t="inlineStr">
         <is>
-          <t>[(-0.300000000101255, 511.0), (-0.300000000101255, 510.88), (-4.512, 510.87361236821886), (-4.512, 510.75361236821885), (-4.512, 510.87361236821886), (-4.512, 510.73361236821887), (-8.80000000000119, 510.7449442378554), (-8.80000000000119, 510.6049442378554), (-0.300000000101255, 510.88), (-0.300000000101255, 510.65), (-4.512, 510.75361236821885), (-4.512, 510.61361236821887), (-4.512, 510.73361236821887), (-4.512, 510.61361236821887), (-8.80000000000119, 510.6049442378554), (-8.80000000000119, 510.3049442378554)]</t>
+          <t>[(-19319.259385937603, 65887.477102374), (-19319.259385937603, 65887.35710237401), (-19323.4713859375, 65887.35071474222), (-19323.4713859375, 65887.23071474223), (-19323.4713859375, 65887.35071474222), (-19323.4713859375, 65887.21071474222), (-19327.759385937505, 65887.22204661186), (-19327.759385937505, 65887.08204661186), (-19319.259385937603, 65887.35710237401), (-19319.259385937603, 65887.127102374), (-19323.4713859375, 65887.23071474223), (-19323.4713859375, 65887.09071474223), (-19323.4713859375, 65887.21071474222), (-19323.4713859375, 65887.09071474223), (-19327.759385937505, 65887.08204661186), (-19327.759385937505, 65886.78204661186)]</t>
         </is>
       </c>
     </row>
@@ -5547,7 +5547,7 @@
       </c>
       <c r="B513" t="inlineStr">
         <is>
-          <t>[(-0.300000000005213, 512.0), (-0.300000000005213, 511.88), (-4.393, 511.927093547934), (-4.393, 511.807093547934), (-4.393, 511.927093547934), (-4.393, 511.767093547934), (-8.79999999999452, 511.84859397934014), (-8.79999999999452, 511.5485939793401), (-0.300000000005213, 511.88), (-0.300000000005213, 511.6), (-4.393, 511.807093547934), (-4.393, 511.617093547934), (-4.393, 511.767093547934), (-4.393, 511.607093547934), (-8.79999999999452, 511.5485939793401), (-8.79999999999452, 511.2485939793401)]</t>
+          <t>[(-19319.259385937607, 65938.8698518447), (-19319.259385937607, 65938.74985184471), (-19323.3523859376, 65938.79694539263), (-19323.3523859376, 65938.67694539264), (-19323.3523859376, 65938.79694539263), (-19323.3523859376, 65938.63694539263), (-19327.759385937596, 65938.71844582405), (-19327.759385937596, 65938.41844582405), (-19319.259385937607, 65938.74985184471), (-19319.259385937607, 65938.46985184471), (-19323.3523859376, 65938.67694539264), (-19323.3523859376, 65938.48694539264), (-19323.3523859376, 65938.63694539263), (-19323.3523859376, 65938.47694539263), (-19327.759385937596, 65938.41844582405), (-19327.759385937596, 65938.11844582405)]</t>
         </is>
       </c>
     </row>
@@ -5557,7 +5557,7 @@
       </c>
       <c r="B514" t="inlineStr">
         <is>
-          <t>[(-0.300000000005213, 513.0), (-0.300000000005213, 512.75), (-4.237, 512.9865706123701), (-4.237, 512.7365706123701), (-4.237, 512.9865706123701), (-4.237, 512.7665706123701), (-8.79999999999452, 512.9710058941188), (-8.79999999999452, 512.5910058941188), (-0.300000000005213, 512.75), (-0.300000000005213, 512.5), (-4.237, 512.7365706123701), (-4.237, 512.54657061237), (-4.237, 512.7665706123701), (-4.237, 512.54657061237), (-8.79999999999452, 512.5910058941188), (-8.79999999999452, 512.2110058941188)]</t>
+          <t>[(-19242.25938593751, 65890.2524289631), (-19242.25938593751, 65890.0024289631), (-19246.196385937503, 65890.23899957546), (-19246.196385937503, 65889.98899957546), (-19246.196385937503, 65890.23899957546), (-19246.196385937503, 65890.01899957546), (-19250.759385937497, 65890.22343485721), (-19250.759385937497, 65889.8434348572), (-19242.25938593751, 65890.0024289631), (-19242.25938593751, 65889.7524289631), (-19246.196385937503, 65889.98899957546), (-19246.196385937503, 65889.79899957546), (-19246.196385937503, 65890.01899957546), (-19246.196385937503, 65889.79899957546), (-19250.759385937497, 65889.8434348572), (-19250.759385937497, 65889.46343485721)]</t>
         </is>
       </c>
     </row>
@@ -5567,7 +5567,7 @@
       </c>
       <c r="B515" t="inlineStr">
         <is>
-          <t>[(-0.300000000005213, 514.0), (-0.300000000005213, 513.72), (-4.16, 514.0424226755699), (-4.16, 513.76242267557), (-4.16, 514.0424226755699), (-4.16, 513.8024226755699), (-8.79999999999452, 514.0934178088974), (-8.79999999999452, 513.6934178088974), (-0.300000000005213, 513.72), (-0.300000000005213, 513.45), (-4.16, 513.76242267557), (-4.16, 513.5624226755699), (-4.16, 513.8024226755699), (-4.16, 513.5624226755699), (-8.79999999999452, 513.6934178088974), (-8.79999999999452, 513.2934178088974)]</t>
+          <t>[(-19242.25938593751, 65935.58475259651), (-19242.25938593751, 65935.30475259651), (-19246.1193859375, 65935.62717527208), (-19246.1193859375, 65935.34717527208), (-19246.1193859375, 65935.62717527208), (-19246.1193859375, 65935.38717527207), (-19250.759385937497, 65935.6781704054), (-19250.759385937497, 65935.2781704054), (-19242.25938593751, 65935.30475259651), (-19242.25938593751, 65935.0347525965), (-19246.1193859375, 65935.34717527208), (-19246.1193859375, 65935.14717527208), (-19246.1193859375, 65935.38717527207), (-19246.1193859375, 65935.14717527208), (-19250.759385937497, 65935.2781704054), (-19250.759385937497, 65934.8781704054)]</t>
         </is>
       </c>
     </row>
@@ -5577,7 +5577,7 @@
       </c>
       <c r="B516" t="inlineStr">
         <is>
-          <t>[(-0.300000000004548, 515.0), (-0.300000000004548, 514.85), (-4.027, 515.0942611932986), (-4.027, 514.9442611932986), (-4.027, 515.0942611932986), (-4.027, 514.8742611932986), (-8.80000000001436, 515.2149772318326), (-8.80000000001436, 514.8549772318325), (-0.300000000004548, 514.85), (-0.300000000004548, 514.7), (-4.027, 514.9442611932986), (-4.027, 514.7942611932987), (-4.027, 514.8742611932986), (-4.027, 514.6542611932986), (-8.80000000001436, 514.8549772318325), (-8.80000000001436, 514.4949772318325), (-0.300000000004548, 514.7), (-0.300000000004548, 514.57), (-4.027, 514.7942611932987), (-4.027, 514.6542611932986), (-4.027, 514.6542611932986), (-4.027, 514.6542611932986), (-8.80000000001436, 514.4949772318325), (-8.80000000001436, 514.4949772318325)]</t>
+          <t>[(-19129.059385937504, 65888.8627284039), (-19129.059385937504, 65888.7127284039), (-19132.7863859375, 65888.9569895972), (-19132.7863859375, 65888.8069895972), (-19132.7863859375, 65888.9569895972), (-19132.7863859375, 65888.7369895972), (-19137.559385937515, 65889.07770563573), (-19137.559385937515, 65888.71770563573), (-19129.059385937504, 65888.7127284039), (-19129.059385937504, 65888.5627284039), (-19132.7863859375, 65888.8069895972), (-19132.7863859375, 65888.65698959719), (-19132.7863859375, 65888.7369895972), (-19132.7863859375, 65888.51698959719), (-19137.559385937515, 65888.71770563573), (-19137.559385937515, 65888.35770563573), (-19129.059385937504, 65888.5627284039), (-19129.059385937504, 65888.4327284039), (-19132.7863859375, 65888.65698959719), (-19132.7863859375, 65888.51698959719), (-19132.7863859375, 65888.51698959719), (-19132.7863859375, 65888.51698959719), (-19137.559385937515, 65888.35770563573), (-19137.559385937515, 65888.35770563573)]</t>
         </is>
       </c>
     </row>
@@ -5587,7 +5587,7 @@
       </c>
       <c r="B517" t="inlineStr">
         <is>
-          <t>[(-0.300000000028711, 516.0), (-0.300000000028711, 515.79), (-3.916, 516.1301967007072), (-3.916, 515.9201967007072), (-3.916, 516.1301967007072), (-3.916, 515.9301967007071), (-8.80000000001792, 516.3060486604033), (-8.80000000001792, 515.9660486604033), (-0.300000000028711, 515.79), (-0.300000000028711, 515.58), (-3.916, 515.9201967007072), (-3.916, 515.7201967007072), (-3.916, 515.9301967007071), (-3.916, 515.7301967007072), (-8.80000000001792, 515.9660486604033), (-8.80000000001792, 515.6260486604034)]</t>
+          <t>[(-19129.05938593753, 65934.0863563851), (-19129.05938593753, 65933.8763563851), (-19132.675385937502, 65934.2165530858), (-19132.675385937502, 65934.0065530858), (-19132.675385937502, 65934.2165530858), (-19132.675385937502, 65934.0165530858), (-19137.55938593752, 65934.39240504551), (-19137.55938593752, 65934.05240504551), (-19129.05938593753, 65933.8763563851), (-19129.05938593753, 65933.6663563851), (-19132.675385937502, 65934.0065530858), (-19132.675385937502, 65933.8065530858), (-19132.675385937502, 65934.0165530858), (-19132.675385937502, 65933.81655308581), (-19137.55938593752, 65934.05240504551), (-19137.55938593752, 65933.71240504552)]</t>
         </is>
       </c>
     </row>
@@ -5597,7 +5597,7 @@
       </c>
       <c r="B518" t="inlineStr">
         <is>
-          <t>[(-0.300000000119848, 517.0), (-0.300000000119848, 516.79), (-4.131, 517.178984360096), (-4.131, 516.968984360096), (-4.131, 517.178984360096), (-4.131, 516.988984360096), (-8.80000000000311, 517.3971200889698), (-8.80000000000311, 517.0671200889698), (-0.300000000119848, 516.79), (-0.300000000119848, 516.58), (-4.131, 516.968984360096), (-4.131, 516.798984360096), (-4.131, 516.988984360096), (-4.131, 516.798984360096), (-8.80000000000311, 517.0671200889698), (-8.80000000000311, 516.7371200889698)]</t>
+          <t>[(-19069.05938593762, 65887.2556365403), (-19069.05938593762, 65887.0456365403), (-19072.890385937502, 65887.4346209004), (-19072.890385937502, 65887.2246209004), (-19072.890385937502, 65887.4346209004), (-19072.890385937502, 65887.2446209004), (-19077.559385937504, 65887.65275662926), (-19077.559385937504, 65887.32275662926), (-19069.05938593762, 65887.0456365403), (-19069.05938593762, 65886.8356365403), (-19072.890385937502, 65887.2246209004), (-19072.890385937502, 65887.0546209004), (-19072.890385937502, 65887.2446209004), (-19072.890385937502, 65887.0546209004), (-19077.559385937504, 65887.32275662926), (-19077.559385937504, 65886.99275662926)]</t>
         </is>
       </c>
     </row>
@@ -5607,7 +5607,7 @@
       </c>
       <c r="B519" t="inlineStr">
         <is>
-          <t>[(-0.300000000010955, 518.0), (-0.300000000010955, 517.76), (-4.733, 518.254606234974), (-4.733, 518.0146062349739), (-4.733, 518.254606234974), (-4.733, 518.0146062349739), (-8.80000000001207, 518.4881915175467), (-8.80000000001207, 518.1081915175467), (-0.300000000010955, 517.76), (-0.300000000010955, 517.58), (-4.733, 518.0146062349739), (-4.733, 517.7846062349739), (-4.733, 518.0146062349739), (-4.733, 517.7746062349739), (-8.80000000001207, 518.1081915175467), (-8.80000000001207, 517.7281915175467)]</t>
+          <t>[(-19069.05938593761, 65934.3705688694), (-19069.05938593761, 65934.1305688694), (-19073.4923859376, 65934.62517510437), (-19073.4923859376, 65934.38517510437), (-19073.4923859376, 65934.62517510437), (-19073.4923859376, 65934.38517510437), (-19077.559385937613, 65934.85876038695), (-19077.559385937613, 65934.47876038695), (-19069.05938593761, 65934.1305688694), (-19069.05938593761, 65933.9505688694), (-19073.4923859376, 65934.38517510437), (-19073.4923859376, 65934.15517510437), (-19073.4923859376, 65934.38517510437), (-19073.4923859376, 65934.14517510438), (-19077.559385937613, 65934.47876038695), (-19077.559385937613, 65934.09876038696)]</t>
         </is>
       </c>
     </row>
@@ -5617,7 +5617,7 @@
       </c>
       <c r="B520" t="inlineStr">
         <is>
-          <t>[(-0.300000000071549, 519.0), (-0.300000000071549, 518.74), (-5.234, 519.3362451030712), (-5.234, 519.0762451030712), (-5.234, 519.3362451030712), (-5.234, 519.0762451030712), (-8.79999999999608, 519.579262946113), (-8.79999999999608, 519.179262946113), (-0.300000000071549, 518.74), (-0.300000000071549, 518.59), (-5.234, 519.0762451030712), (-5.234, 518.8262451030712), (-5.234, 519.0762451030712), (-5.234, 518.8162451030712), (-8.79999999999608, 519.179262946113), (-8.79999999999608, 518.779262946113)]</t>
+          <t>[(-18940.85938593767, 65887.4311533724), (-18940.85938593767, 65887.1711533724), (-18945.7933859376, 65887.76739847547), (-18945.7933859376, 65887.50739847547), (-18945.7933859376, 65887.76739847547), (-18945.7933859376, 65887.50739847547), (-18949.359385937594, 65888.0104163185), (-18949.359385937594, 65887.61041631851), (-18940.85938593767, 65887.1711533724), (-18940.85938593767, 65887.02115337239), (-18945.7933859376, 65887.50739847547), (-18945.7933859376, 65887.25739847547), (-18945.7933859376, 65887.50739847547), (-18945.7933859376, 65887.24739847546), (-18949.359385937594, 65887.61041631851), (-18949.359385937594, 65887.2104163185)]</t>
         </is>
       </c>
     </row>
@@ -5627,7 +5627,7 @@
       </c>
       <c r="B521" t="inlineStr">
         <is>
-          <t>[(-0.299999999998654, 520.0), (-0.299999999998654, 519.73), (-5.555, 520.3678500000001), (-5.555, 520.0978500000001), (-5.555, 520.3678500000001), (-5.555, 520.0978500000001), (-8.79999999999749, 520.5949999999999), (-8.79999999999749, 520.1949999999999), (-0.299999999998654, 519.73), (-0.299999999998654, 519.55), (-5.555, 520.0978500000001), (-5.555, 519.8278500000001), (-5.555, 520.0978500000001), (-5.555, 519.8278500000001), (-8.79999999999749, 520.1949999999999), (-8.79999999999749, 519.795)]</t>
+          <t>[(-18940.8593859377, 65930.43739004931), (-18940.8593859377, 65930.1673900493), (-18946.1143859377, 65930.8052400493), (-18946.1143859377, 65930.5352400493), (-18946.1143859377, 65930.8052400493), (-18946.1143859377, 65930.5352400493), (-18949.3593859377, 65931.03239004931), (-18949.3593859377, 65930.63239004932), (-18940.8593859377, 65930.1673900493), (-18940.8593859377, 65929.98739004931), (-18946.1143859377, 65930.5352400493), (-18946.1143859377, 65930.26524004931), (-18946.1143859377, 65930.5352400493), (-18946.1143859377, 65930.26524004931), (-18949.3593859377, 65930.63239004932), (-18949.3593859377, 65930.2323900493)]</t>
         </is>
       </c>
     </row>
@@ -5637,7 +5637,7 @@
       </c>
       <c r="B522" t="inlineStr">
         <is>
-          <t>[(-0.299999999994848, 521.0), (-0.299999999994848, 520.75), (-5.537, 521.3665900000003), (-5.537, 521.1165900000003), (-5.537, 521.3665900000003), (-5.537, 521.1165900000003), (-8.79999999999258, 521.5949999999998), (-8.79999999999258, 521.2149999999998), (-0.299999999994848, 520.75), (-0.299999999994848, 520.6), (-5.537, 521.1165900000003), (-5.537, 520.8665900000003), (-5.537, 521.1165900000003), (-5.537, 520.8665900000003), (-8.79999999999258, 521.2149999999998), (-8.79999999999258, 520.8349999999998)]</t>
+          <t>[(-26280.659385937597, 65587.3892789001), (-26280.659385937597, 65587.1392789001), (-26285.8963859376, 65587.7558689001), (-26285.8963859376, 65587.5058689001), (-26285.8963859376, 65587.7558689001), (-26285.8963859376, 65587.5058689001), (-26289.159385937593, 65587.9842789001), (-26289.159385937593, 65587.6042789001), (-26280.659385937597, 65587.1392789001), (-26280.659385937597, 65586.9892789001), (-26285.8963859376, 65587.5058689001), (-26285.8963859376, 65587.2558689001), (-26285.8963859376, 65587.5058689001), (-26285.8963859376, 65587.2558689001), (-26289.159385937593, 65587.6042789001), (-26289.159385937593, 65587.2242789001)]</t>
         </is>
       </c>
     </row>
@@ -5647,7 +5647,7 @@
       </c>
       <c r="B523" t="inlineStr">
         <is>
-          <t>[(-0.299999999994134, 522.0), (-0.299999999994134, 521.77), (-5.217, 522.3441900000004), (-5.217, 522.1141900000003), (-5.217, 522.3441900000004), (-5.217, 522.1141900000003), (-8.80000000000401, 522.5950000000007), (-8.80000000000401, 522.2150000000007), (-0.299999999994134, 521.77), (-0.299999999994134, 521.61), (-5.217, 522.1141900000003), (-5.217, 521.8841900000003), (-5.217, 522.1141900000003), (-5.217, 521.8841900000003), (-8.80000000000401, 522.2150000000007), (-8.80000000000401, 521.8350000000007)]</t>
+          <t>[(-26280.659385937597, 65630.2996130788), (-26280.659385937597, 65630.0696130788), (-26285.576385937602, 65630.6438030788), (-26285.576385937602, 65630.4138030788), (-26285.576385937602, 65630.6438030788), (-26285.576385937602, 65630.4138030788), (-26289.159385937604, 65630.8946130788), (-26289.159385937604, 65630.51461307879), (-26280.659385937597, 65630.0696130788), (-26280.659385937597, 65629.9096130788), (-26285.576385937602, 65630.4138030788), (-26285.576385937602, 65630.18380307879), (-26285.576385937602, 65630.4138030788), (-26285.576385937602, 65630.18380307879), (-26289.159385937604, 65630.51461307879), (-26289.159385937604, 65630.1346130788)]</t>
         </is>
       </c>
     </row>
@@ -5657,7 +5657,7 @@
       </c>
       <c r="B524" t="inlineStr">
         <is>
-          <t>[(-0.299999999979054, 523.0), (-0.299999999979054, 522.81), (-4.758, 523.3120600000015), (-4.758, 523.1220600000014), (-4.758, 523.3120600000015), (-4.758, 523.1220600000014), (-8.79999999999188, 523.5950000000009), (-8.79999999999188, 523.2550000000009), (-0.299999999979054, 522.81), (-0.299999999979054, 522.66), (-4.758, 523.1220600000014), (-4.758, 522.9320600000015), (-4.758, 523.1220600000014), (-4.758, 522.9320600000015), (-8.79999999999188, 523.2550000000009), (-8.79999999999188, 522.915000000001)]</t>
+          <t>[(-26220.65938593758, 65587.2072704065), (-26220.65938593758, 65587.0172704065), (-26225.117385937603, 65587.5193304065), (-26225.117385937603, 65587.3293304065), (-26225.117385937603, 65587.5193304065), (-26225.117385937603, 65587.3293304065), (-26229.159385937593, 65587.80227040651), (-26229.159385937593, 65587.46227040651), (-26220.65938593758, 65587.0172704065), (-26220.65938593758, 65586.86727040651), (-26225.117385937603, 65587.3293304065), (-26225.117385937603, 65587.1393304065), (-26225.117385937603, 65587.3293304065), (-26225.117385937603, 65587.1393304065), (-26229.159385937593, 65587.46227040651), (-26229.159385937593, 65587.12227040651)]</t>
         </is>
       </c>
     </row>
@@ -5667,7 +5667,7 @@
       </c>
       <c r="B525" t="inlineStr">
         <is>
-          <t>[(-0.299999999999697, 524.0), (-0.299999999999697, 523.83), (-3.886, 524.25102), (-3.886, 524.0810200000001), (-3.886, 524.25102), (-3.886, 524.0910200000001), (-8.79999999999566, 524.5949999999997), (-8.79999999999566, 524.1349999999996), (-0.299999999999697, 523.83), (-0.299999999999697, 523.7), (-3.886, 524.0810200000001), (-3.886, 523.92102), (-3.886, 524.0910200000001), (-3.886, 523.93102), (-8.79999999999566, 524.1349999999996), (-8.79999999999566, 523.6749999999997)]</t>
+          <t>[(-26220.6593859375, 65630.1118298462), (-26220.6593859375, 65629.9418298462), (-26224.2453859375, 65630.36284984619), (-26224.2453859375, 65630.1928498462), (-26224.2453859375, 65630.36284984619), (-26224.2453859375, 65630.20284984619), (-26229.159385937495, 65630.7068298462), (-26229.159385937495, 65630.24682984619), (-26220.6593859375, 65629.9418298462), (-26220.6593859375, 65629.81182984619), (-26224.2453859375, 65630.1928498462), (-26224.2453859375, 65630.03284984619), (-26224.2453859375, 65630.20284984619), (-26224.2453859375, 65630.04284984618), (-26229.159385937495, 65630.24682984619), (-26229.159385937495, 65629.7868298462)]</t>
         </is>
       </c>
     </row>
@@ -5677,7 +5677,7 @@
       </c>
       <c r="B526" t="inlineStr">
         <is>
-          <t>[(-0.300000000004062, 525.0), (-0.300000000004062, 524.82), (-2.604, 525.1612799999997), (-2.604, 524.9812799999997), (-2.604, 525.1612799999997), (-2.604, 525.0012799999997), (-9.00078263048913, 525.609054784134), (-9.00078263048913, 525.089054784134), (-0.300000000004062, 524.82), (-0.300000000004062, 524.64), (-2.604, 524.9812799999997), (-2.604, 524.8312799999997), (-2.604, 525.0012799999997), (-2.604, 524.8412799999996), (-9.00078263048913, 525.089054784134), (-9.00078263048913, 524.569054784134)]</t>
+          <t>[(-26096.459385937604, 65586.9739631394), (-26096.459385937604, 65586.79396313941), (-26098.7633859376, 65587.1352431394), (-26098.7633859376, 65586.95524313941), (-26098.7633859376, 65587.1352431394), (-26098.7633859376, 65586.9752431394), (-26105.16016856809, 65587.58301792353), (-26105.16016856809, 65587.06301792353), (-26096.459385937604, 65586.79396313941), (-26096.459385937604, 65586.6139631394), (-26098.7633859376, 65586.95524313941), (-26098.7633859376, 65586.8052431394), (-26098.7633859376, 65586.9752431394), (-26098.7633859376, 65586.8152431394), (-26105.16016856809, 65587.06301792353), (-26105.16016856809, 65586.54301792354)]</t>
         </is>
       </c>
     </row>
@@ -5687,7 +5687,7 @@
       </c>
       <c r="B527" t="inlineStr">
         <is>
-          <t>[(-0.300000000025313, 526.0), (-0.300000000025313, 525.82), (-8.305, 526.5478867924357), (-8.305, 526.1078867924357), (-0.300000000025313, 525.82), (-0.300000000025313, 525.64), (-8.305, 526.1078867924357), (-8.305, 525.6678867924358)]</t>
+          <t>[(-26096.459385937625, 65625.7817486065), (-26096.459385937625, 65625.60174860651), (-26104.4643859376, 65626.32963539894), (-26104.4643859376, 65625.88963539894), (-26096.459385937625, 65625.60174860651), (-26096.459385937625, 65625.4217486065), (-26104.4643859376, 65625.88963539894), (-26104.4643859376, 65625.44963539894)]</t>
         </is>
       </c>
     </row>
@@ -5697,7 +5697,7 @@
       </c>
       <c r="B528" t="inlineStr">
         <is>
-          <t>[(-0.299999999982753, 527.0), (-0.299999999982753, 526.82), (-7.338, 527.4062951988271), (-7.338, 527.1162951988272), (-0.299999999982753, 526.82), (-0.299999999982753, 526.64), (-7.338, 527.1162951988272), (-7.338, 526.8262951988271)]</t>
+          <t>[(-26048.45938593748, 65588.5351862475), (-26048.45938593748, 65588.35518624751), (-26055.4973859375, 65588.94148144634), (-26055.4973859375, 65588.65148144634), (-26048.45938593748, 65588.35518624751), (-26048.45938593748, 65588.1751862475), (-26055.4973859375, 65588.65148144634), (-26055.4973859375, 65588.36148144634)]</t>
         </is>
       </c>
     </row>
@@ -5707,7 +5707,7 @@
       </c>
       <c r="B529" t="inlineStr">
         <is>
-          <t>[(-0.30000000005047, 528.0), (-0.30000000005047, 527.81), (-6.61, 528.2966614994526), (-6.61, 528.1066614994526), (-0.30000000005047, 527.81), (-0.30000000005047, 527.67), (-6.61, 528.1066614994526), (-6.61, 527.8066614994526)]</t>
+          <t>[(-26048.45938593755, 65627.2342760624), (-26048.45938593755, 65627.0442760624), (-26054.7693859375, 65627.53093756185), (-26054.7693859375, 65627.34093756185), (-26048.45938593755, 65627.0442760624), (-26048.45938593755, 65626.9042760624), (-26054.7693859375, 65627.34093756185), (-26054.7693859375, 65627.04093756185)]</t>
         </is>
       </c>
     </row>
@@ -5717,7 +5717,7 @@
       </c>
       <c r="B530" t="inlineStr">
         <is>
-          <t>[(-0.300000000004344, 529.0), (-0.300000000004344, 528.88), (-6.439, 529.2228470198341), (-6.439, 529.1028470198341), (-0.300000000004344, 528.88), (-0.300000000004344, 528.69), (-6.439, 529.1028470198341), (-6.439, 528.8128470198342)]</t>
+          <t>[(-26000.4593859375, 65587.8790180512), (-26000.4593859375, 65587.7590180512), (-26006.598385937497, 65588.10186507103), (-26006.598385937497, 65587.98186507104), (-26000.4593859375, 65587.7590180512), (-26000.4593859375, 65587.5690180512), (-26006.598385937497, 65587.98186507104), (-26006.598385937497, 65587.69186507103)]</t>
         </is>
       </c>
     </row>
@@ -5727,7 +5727,7 @@
       </c>
       <c r="B531" t="inlineStr">
         <is>
-          <t>[(-0.30000000015198, 530.0), (-0.30000000015198, 529.78), (-6.65, 530.162470650908), (-6.65, 529.9424706509079), (-0.30000000015198, 529.78), (-0.30000000015198, 529.61), (-6.65, 529.9424706509079), (-6.65, 529.732470650908)]</t>
+          <t>[(-25895.259385937752, 65590.4694122139), (-25895.259385937752, 65590.2494122139), (-25901.6093859376, 65590.6318828648), (-25901.6093859376, 65590.4118828648), (-25895.259385937752, 65590.2494122139), (-25895.259385937752, 65590.0794122139), (-25901.6093859376, 65590.4118828648), (-25901.6093859376, 65590.20188286481)]</t>
         </is>
       </c>
     </row>
@@ -5737,7 +5737,7 @@
       </c>
       <c r="B532" t="inlineStr">
         <is>
-          <t>[(-0.300000000007116, 531.0), (-0.300000000007116, 530.8), (-6.883, 531.0090000690116), (-6.883, 530.8090000690115), (-0.300000000007116, 530.8), (-0.300000000007116, 530.61), (-6.883, 530.8090000690115), (-6.883, 530.6890000690115)]</t>
+          <t>[(-25905.259385937705, 65631.0054585506), (-25905.259385937705, 65630.8054585506), (-25911.8423859377, 65631.01445861961), (-25911.8423859377, 65630.81445861961), (-25905.259385937705, 65630.8054585506), (-25905.259385937705, 65630.6154585506), (-25911.8423859377, 65630.81445861961), (-25911.8423859377, 65630.6944586196)]</t>
         </is>
       </c>
     </row>
@@ -5747,7 +5747,7 @@
       </c>
       <c r="B533" t="inlineStr">
         <is>
-          <t>[(-0.300000000008061, 532.0), (-0.300000000008061, 531.88), (-7.239, 531.8360117809315), (-7.239, 531.7160117809315), (-0.300000000008061, 531.88), (-0.300000000008061, 531.66), (-7.239, 531.7160117809315), (-7.239, 531.5860117809315)]</t>
+          <t>[(-25837.259385937607, 65587.48814090231), (-25837.259385937607, 65587.36814090231), (-25844.1983859376, 65587.32415268324), (-25844.1983859376, 65587.20415268325), (-25837.259385937607, 65587.36814090231), (-25837.259385937607, 65587.14814090231), (-25844.1983859376, 65587.20415268325), (-25844.1983859376, 65587.07415268324)]</t>
         </is>
       </c>
     </row>
@@ -5757,7 +5757,7 @@
       </c>
       <c r="B534" t="inlineStr">
         <is>
-          <t>[(-0.300000000007116, 533.0), (-0.300000000007116, 532.84), (-8.053, 532.8061750000002), (-8.053, 532.6461750000002), (-0.300000000007116, 532.84), (-0.300000000007116, 532.68), (-8.053, 532.6461750000002), (-8.053, 532.5261750000002)]</t>
+          <t>[(-25837.25938593751, 65629.9530066435), (-25837.25938593751, 65629.7930066435), (-25845.0123859375, 65629.7591816435), (-25845.0123859375, 65629.5991816435), (-25837.25938593751, 65629.7930066435), (-25837.25938593751, 65629.63300664349), (-25845.0123859375, 65629.5991816435), (-25845.0123859375, 65629.4791816435)]</t>
         </is>
       </c>
     </row>
@@ -5767,7 +5767,7 @@
       </c>
       <c r="B535" t="inlineStr">
         <is>
-          <t>[(-0.300000000007116, 534.0), (-0.300000000007116, 533.85), (-8.848, 533.7863000000002), (-8.848, 533.6363000000002), (-0.300000000007116, 533.85), (-0.300000000007116, 533.73), (-8.848, 533.6363000000002), (-8.848, 533.5063000000002)]</t>
+          <t>[(-25717.059385937508, 65586.4178723847), (-25717.059385937508, 65586.2678723847), (-25725.607385937503, 65586.2041723847), (-25725.607385937503, 65586.05417238471), (-25717.059385937508, 65586.2678723847), (-25717.059385937508, 65586.1478723847), (-25725.607385937503, 65586.05417238471), (-25725.607385937503, 65585.92417238471)]</t>
         </is>
       </c>
     </row>
@@ -5787,7 +5787,7 @@
       </c>
       <c r="B537" t="inlineStr">
         <is>
-          <t>[(-0.300000000008061, 536.0), (-0.300000000008061, 535.87), (-7.123, 535.8294250000002), (-7.123, 535.6994250000002), (-0.300000000008061, 535.87), (-0.300000000008061, 535.75), (-7.123, 535.6994250000002), (-7.123, 535.5794250000002)]</t>
+          <t>[(-25639.059385937606, 65591.3476038672), (-25639.059385937606, 65591.21760386719), (-25645.8823859376, 65591.1770288672), (-25645.8823859376, 65591.0470288672), (-25639.059385937606, 65591.21760386719), (-25639.059385937606, 65591.0976038672), (-25645.8823859376, 65591.0470288672), (-25645.8823859376, 65590.9270288672)]</t>
         </is>
       </c>
     </row>
@@ -5797,7 +5797,7 @@
       </c>
       <c r="B538" t="inlineStr">
         <is>
-          <t>[(-0.300000000009005, 537.0), (-0.300000000009005, 536.86), (-7.109, 536.8297750000003), (-7.109, 536.6897750000003), (-0.300000000009005, 536.86), (-0.300000000009005, 536.74), (-7.109, 536.6897750000003), (-7.109, 536.5597750000003)]</t>
+          <t>[(-25639.05938593751, 65631.8124696084), (-25639.05938593751, 65631.6724696084), (-25645.8683859375, 65631.6422446084), (-25645.8683859375, 65631.5022446084), (-25639.05938593751, 65631.6724696084), (-25639.05938593751, 65631.5524696084), (-25645.8683859375, 65631.5022446084), (-25645.8683859375, 65631.3722446084)]</t>
         </is>
       </c>
     </row>
@@ -5817,7 +5817,7 @@
       </c>
       <c r="B540" t="inlineStr">
         <is>
-          <t>[(-0.300000000008061, 539.0), (-0.300000000008061, 538.85), (-6.982, 538.8329500000002), (-6.982, 538.6829500000002), (-0.300000000008061, 538.85), (-0.300000000008061, 538.71), (-6.982, 538.6829500000002), (-6.982, 538.5329500000003)]</t>
+          <t>[(-25528.859385937507, 65630.7422010908), (-25528.859385937507, 65630.59220109081), (-25535.5413859375, 65630.5751510908), (-25535.5413859375, 65630.4251510908), (-25528.859385937507, 65630.59220109081), (-25528.859385937507, 65630.45220109081), (-25535.5413859375, 65630.4251510908), (-25535.5413859375, 65630.2751510908)]</t>
         </is>
       </c>
     </row>
@@ -5837,7 +5837,7 @@
       </c>
       <c r="B542" t="inlineStr">
         <is>
-          <t>[(-0.300000000008061, 541.0), (-0.300000000008061, 540.87), (-6.828, 540.8368000000002), (-6.828, 540.7068000000002), (-0.300000000008061, 540.87), (-0.300000000008061, 540.75), (-6.828, 540.7068000000002), (-6.828, 540.5868000000002)]</t>
+          <t>[(-25459.859385937507, 65631.6719325733), (-25459.859385937507, 65631.5419325733), (-25466.3873859375, 65631.5087325733), (-25466.3873859375, 65631.3787325733), (-25459.859385937507, 65631.5419325733), (-25459.859385937507, 65631.4219325733), (-25466.3873859375, 65631.3787325733), (-25466.3873859375, 65631.2587325733)]</t>
         </is>
       </c>
     </row>
@@ -5847,7 +5847,7 @@
       </c>
       <c r="B543" t="inlineStr">
         <is>
-          <t>[(-0.300000000007116, 542.0), (-0.300000000007116, 541.87), (-6.768, 541.8383000000002), (-6.768, 541.7083000000002), (-0.300000000007116, 541.87), (-0.300000000007116, 541.75), (-6.768, 541.7083000000002), (-6.768, 541.5883000000002)]</t>
+          <t>[(-25339.659385937608, 65590.1847629142), (-25339.659385937608, 65590.0547629142), (-25346.1273859376, 65590.0230629142), (-25346.1273859376, 65589.8930629142), (-25339.659385937608, 65590.0547629142), (-25339.659385937608, 65589.9347629142), (-25346.1273859376, 65589.8930629142), (-25346.1273859376, 65589.7730629142)]</t>
         </is>
       </c>
     </row>
@@ -5857,7 +5857,7 @@
       </c>
       <c r="B544" t="inlineStr">
         <is>
-          <t>[(-0.300000000007116, 543.0), (-0.300000000007116, 542.87), (-6.686, 542.8403500000002), (-6.686, 542.7103500000002), (-0.300000000007116, 542.87), (-0.300000000007116, 542.75), (-6.686, 542.7103500000002), (-6.686, 542.5903500000002)]</t>
+          <t>[(-25339.659385937608, 65630.8613840561), (-25339.659385937608, 65630.7313840561), (-25346.045385937603, 65630.7017340561), (-25346.045385937603, 65630.5717340561), (-25339.659385937608, 65630.7313840561), (-25339.659385937608, 65630.6113840561), (-25346.045385937603, 65630.5717340561), (-25346.045385937603, 65630.4517340561)]</t>
         </is>
       </c>
     </row>
@@ -5867,7 +5867,7 @@
       </c>
       <c r="B545" t="inlineStr">
         <is>
-          <t>[(-0.300000000009005, 544.0), (-0.300000000009005, 543.87), (-6.632, 543.8417000000002), (-6.632, 543.7117000000002), (-0.300000000009005, 543.87), (-0.300000000009005, 543.75), (-6.632, 543.7117000000002), (-6.632, 543.5917000000002)]</t>
+          <t>[(-25270.65938593751, 65591.706924117), (-25270.65938593751, 65591.57692411699), (-25276.9913859375, 65591.548624117), (-25276.9913859375, 65591.418624117), (-25270.65938593751, 65591.57692411699), (-25270.65938593751, 65591.456924117), (-25276.9913859375, 65591.418624117), (-25276.9913859375, 65591.298624117)]</t>
         </is>
       </c>
     </row>
@@ -5877,7 +5877,7 @@
       </c>
       <c r="B546" t="inlineStr">
         <is>
-          <t>[(-0.300000000008061, 545.0), (-0.300000000008061, 544.87), (-6.632, 544.8417000000002), (-6.632, 544.7117000000002), (-0.300000000008061, 544.87), (-0.300000000008061, 544.75), (-6.632, 544.7117000000002), (-6.632, 544.5917000000002)]</t>
+          <t>[(-25270.659385937506, 65632.7213830968), (-25270.659385937506, 65632.59138309679), (-25276.9913859375, 65632.5630830968), (-25276.9913859375, 65632.4330830968), (-25270.659385937506, 65632.59138309679), (-25270.659385937506, 65632.4713830968), (-25276.9913859375, 65632.4330830968), (-25276.9913859375, 65632.3130830968)]</t>
         </is>
       </c>
     </row>
@@ -5887,7 +5887,7 @@
       </c>
       <c r="B547" t="inlineStr">
         <is>
-          <t>[(-0.300000000008061, 546.0), (-0.300000000008061, 545.87), (-6.624, 545.8419000000002), (-6.624, 545.7119000000002), (-0.300000000008061, 545.87), (-0.300000000008061, 545.75), (-6.624, 545.7119000000002), (-6.624, 545.5919000000002)]</t>
+          <t>[(-25143.459385937505, 65591.8896260396), (-25143.459385937505, 65591.7596260396), (-25149.7833859375, 65591.7315260396), (-25149.7833859375, 65591.6015260396), (-25143.459385937505, 65591.7596260396), (-25143.459385937505, 65591.6396260396), (-25149.7833859375, 65591.6015260396), (-25149.7833859375, 65591.4815260396)]</t>
         </is>
       </c>
     </row>
@@ -5897,7 +5897,7 @@
       </c>
       <c r="B548" t="inlineStr">
         <is>
-          <t>[(-0.300000000007116, 547.0), (-0.300000000007116, 546.87), (-6.615, 546.8421250000001), (-6.615, 546.7121250000001), (-0.300000000007116, 546.87), (-0.300000000007116, 546.75), (-6.615, 546.7121250000001), (-6.615, 546.5921250000001)]</t>
+          <t>[(-25153.459385937505, 65633.1483575866), (-25153.459385937505, 65633.0183575866), (-25159.7743859375, 65632.9904825866), (-25159.7743859375, 65632.86048258659), (-25153.459385937505, 65633.0183575866), (-25153.459385937505, 65632.8983575866), (-25159.7743859375, 65632.86048258659), (-25159.7743859375, 65632.7404825866)]</t>
         </is>
       </c>
     </row>
@@ -5907,7 +5907,7 @@
       </c>
       <c r="B549" t="inlineStr">
         <is>
-          <t>[(-0.300000000008061, 548.0), (-0.300000000008061, 547.87), (-6.603, 547.8424250000002), (-6.603, 547.7124250000002), (-0.300000000008061, 547.87), (-0.300000000008061, 547.75), (-6.603, 547.7124250000002), (-6.603, 547.5924250000002)]</t>
+          <t>[(-25075.459385937505, 65590.4987268538), (-25075.459385937505, 65590.36872685379), (-25081.762385937498, 65590.34115185379), (-25081.762385937498, 65590.21115185379), (-25075.459385937505, 65590.36872685379), (-25075.459385937505, 65590.2487268538), (-25081.762385937498, 65590.21115185379), (-25081.762385937498, 65590.09115185379)]</t>
         </is>
       </c>
     </row>
@@ -5917,7 +5917,7 @@
       </c>
       <c r="B550" t="inlineStr">
         <is>
-          <t>[(-0.300000000007116, 549.0), (-0.300000000007116, 548.87), (-6.588, 548.8428000000001), (-6.588, 548.7128000000001), (-0.300000000007116, 548.87), (-0.300000000007116, 548.75), (-6.588, 548.7128000000001), (-6.588, 548.5928000000001)]</t>
+          <t>[(-25075.459385937505, 65629.9625390672), (-25075.459385937505, 65629.8325390672), (-25081.7473859375, 65629.8053390672), (-25081.7473859375, 65629.6753390672), (-25075.459385937505, 65629.8325390672), (-25075.459385937505, 65629.7125390672), (-25081.7473859375, 65629.6753390672), (-25081.7473859375, 65629.5553390672)]</t>
         </is>
       </c>
     </row>
@@ -5927,7 +5927,7 @@
       </c>
       <c r="B551" t="inlineStr">
         <is>
-          <t>[(-0.300000000007116, 550.0), (-0.300000000007116, 549.87), (-6.566, 549.8433500000002), (-6.566, 549.7133500000002), (-0.300000000007116, 549.87), (-0.300000000007116, 549.75), (-6.566, 549.7133500000002), (-6.566, 549.5933500000002)]</t>
+          <t>[(-24963.25938593751, 65589.5513512806), (-24963.25938593751, 65589.4213512806), (-24969.5253859375, 65589.3947012806), (-24969.5253859375, 65589.2647012806), (-24963.25938593751, 65589.4213512806), (-24963.25938593751, 65589.3013512806), (-24969.5253859375, 65589.2647012806), (-24969.5253859375, 65589.1447012806)]</t>
         </is>
       </c>
     </row>
@@ -5937,7 +5937,7 @@
       </c>
       <c r="B552" t="inlineStr">
         <is>
-          <t>[(-0.300000000009005, 551.0), (-0.300000000009005, 550.87), (-6.624, 550.8419000000002), (-6.624, 550.7119000000002), (-0.300000000009005, 550.87), (-0.300000000009005, 550.75), (-6.624, 550.7119000000002), (-6.624, 550.5919000000002)]</t>
+          <t>[(-24963.259385937512, 65629.2651634939), (-24963.259385937512, 65629.13516349389), (-24969.5833859375, 65629.1070634939), (-24969.5833859375, 65628.97706349389), (-24963.259385937512, 65629.13516349389), (-24963.259385937512, 65629.0151634939), (-24969.5833859375, 65628.97706349389), (-24969.5833859375, 65628.8570634939)]</t>
         </is>
       </c>
     </row>
@@ -5947,7 +5947,7 @@
       </c>
       <c r="B553" t="inlineStr">
         <is>
-          <t>[(-0.300000000007116, 552.0), (-0.300000000007116, 551.87), (-6.746, 551.8388500000002), (-6.746, 551.7088500000002), (-0.300000000007116, 551.87), (-0.300000000007116, 551.75), (-6.746, 551.7088500000002), (-6.746, 551.5888500000002)]</t>
+          <t>[(-24904.25938593751, 65591.1039757073), (-24904.25938593751, 65590.9739757073), (-24910.7053859375, 65590.9428257073), (-24910.7053859375, 65590.8128257073), (-24904.25938593751, 65590.9739757073), (-24904.25938593751, 65590.8539757073), (-24910.7053859375, 65590.8128257073), (-24910.7053859375, 65590.6928257073)]</t>
         </is>
       </c>
     </row>
@@ -5957,7 +5957,7 @@
       </c>
       <c r="B554" t="inlineStr">
         <is>
-          <t>[(-0.300000000008061, 553.0), (-0.300000000008061, 552.87), (-6.891, 552.8352250000002), (-6.891, 552.7052250000002), (-0.300000000008061, 552.87), (-0.300000000008061, 552.75), (-6.891, 552.7052250000002), (-6.891, 552.5852250000002)]</t>
+          <t>[(-24904.25938593751, 65629.0677879207), (-24904.25938593751, 65628.9377879207), (-24910.8503859375, 65628.90301292071), (-24910.8503859375, 65628.7730129207), (-24904.25938593751, 65628.9377879207), (-24904.25938593751, 65628.8177879207), (-24910.8503859375, 65628.7730129207), (-24910.8503859375, 65628.65301292071)]</t>
         </is>
       </c>
     </row>
@@ -5967,7 +5967,7 @@
       </c>
       <c r="B555" t="inlineStr">
         <is>
-          <t>[(-0.300000000007116, 554.0), (-0.300000000007116, 553.87), (-7.062, 553.8309500000001), (-7.062, 553.7009500000001), (-0.300000000007116, 553.87), (-0.300000000007116, 553.75), (-7.062, 553.7009500000001), (-7.062, 553.5809500000001)]</t>
+          <t>[(-24775.059385937606, 65589.1566001341), (-24775.059385937606, 65589.0266001341), (-24781.8213859376, 65588.9875501341), (-24781.8213859376, 65588.8575501341), (-24775.059385937606, 65589.0266001341), (-24775.059385937606, 65588.9066001341), (-24781.8213859376, 65588.8575501341), (-24781.8213859376, 65588.7375501341)]</t>
         </is>
       </c>
     </row>
@@ -5977,7 +5977,7 @@
       </c>
       <c r="B556" t="inlineStr">
         <is>
-          <t>[(-0.300000000008061, 555.0), (-0.300000000008061, 554.87), (-10.218, 554.7520500000002), (-10.218, 554.6220500000002), (-0.300000000008061, 554.87), (-0.300000000008061, 554.75), (-10.218, 554.6220500000002), (-10.218, 554.5020500000002)]</t>
+          <t>[(-24775.059385937508, 65627.3704123474), (-24775.059385937508, 65627.2404123474), (-24784.977385937502, 65627.1224623474), (-24784.977385937502, 65626.99246234739), (-24775.059385937508, 65627.2404123474), (-24775.059385937508, 65627.1204123474), (-24784.977385937502, 65626.99246234739), (-24784.977385937502, 65626.8724623474)]</t>
         </is>
       </c>
     </row>
@@ -5987,7 +5987,7 @@
       </c>
       <c r="B557" t="inlineStr">
         <is>
-          <t>[(-0.300000000006172, 556.0), (-0.300000000006172, 555.87), (-9.355, 555.7736250000002), (-9.355, 555.6436250000002), (-0.300000000006172, 555.87), (-0.300000000006172, 555.75), (-9.355, 555.6436250000002), (-9.355, 555.5236250000002)]</t>
+          <t>[(-24716.059385937508, 65589.70922456081), (-24716.059385937508, 65589.5792245608), (-24725.1143859375, 65589.48284956081), (-24725.1143859375, 65589.3528495608), (-24716.059385937508, 65589.5792245608), (-24716.059385937508, 65589.45922456081), (-24725.1143859375, 65589.3528495608), (-24725.1143859375, 65589.23284956081)]</t>
         </is>
       </c>
     </row>
@@ -5997,7 +5997,7 @@
       </c>
       <c r="B558" t="inlineStr">
         <is>
-          <t>[(-0.300000000007116, 557.0), (-0.300000000007116, 556.87), (-8.685, 556.7903750000002), (-8.685, 556.6603750000002), (-0.300000000007116, 556.87), (-0.300000000007116, 556.75), (-8.685, 556.6603750000002), (-8.685, 556.5403750000002)]</t>
+          <t>[(-24716.059385937508, 65632.1730367742), (-24716.059385937508, 65632.0430367742), (-24724.444385937502, 65631.9634117742), (-24724.444385937502, 65631.83341177419), (-24716.059385937508, 65632.0430367742), (-24716.059385937508, 65631.9230367742), (-24724.444385937502, 65631.83341177419), (-24724.444385937502, 65631.7134117742)]</t>
         </is>
       </c>
     </row>
@@ -6007,7 +6007,7 @@
       </c>
       <c r="B559" t="inlineStr">
         <is>
-          <t>[(-0.300000000009005, 558.0), (-0.300000000009005, 557.87), (-8.126, 557.8043500000002), (-8.126, 557.6743500000002), (-0.300000000009005, 557.87), (-0.300000000009005, 557.75), (-8.126, 557.6743500000002), (-8.126, 557.5543500000002)]</t>
+          <t>[(-24587.85938593751, 65592.7618489876), (-24587.85938593751, 65592.6318489876), (-24595.6853859375, 65592.56619898761), (-24595.6853859375, 65592.4361989876), (-24587.85938593751, 65592.6318489876), (-24587.85938593751, 65592.5118489876), (-24595.6853859375, 65592.4361989876), (-24595.6853859375, 65592.31619898761)]</t>
         </is>
       </c>
     </row>
@@ -6017,7 +6017,7 @@
       </c>
       <c r="B560" t="inlineStr">
         <is>
-          <t>[(-0.300000000007116, 559.0), (-0.300000000007116, 558.87), (-7.618, 558.8170500000002), (-7.618, 558.6870500000002), (-0.300000000007116, 558.87), (-0.300000000007116, 558.75), (-7.618, 558.6870500000002), (-7.618, 558.5670500000002)]</t>
+          <t>[(-24587.859385937507, 65631.47566120091), (-24587.859385937507, 65631.3456612009), (-24595.1773859375, 65631.2927112009), (-24595.1773859375, 65631.1627112009), (-24587.859385937507, 65631.3456612009), (-24587.859385937507, 65631.22566120091), (-24595.1773859375, 65631.1627112009), (-24595.1773859375, 65631.0427112009)]</t>
         </is>
       </c>
     </row>
@@ -6037,7 +6037,7 @@
       </c>
       <c r="B562" t="inlineStr">
         <is>
-          <t>[(-0.300000000007116, 561.0), (-0.300000000007116, 560.81), (-7.039, 560.8315250000002), (-7.039, 560.6415250000001), (-0.300000000007116, 560.81), (-0.300000000007116, 560.63), (-7.039, 560.6415250000001), (-7.039, 560.5115250000001)]</t>
+          <t>[(-24518.859385937507, 65629.2757199607), (-24518.859385937507, 65629.0857199607), (-24525.5983859375, 65629.1072449607), (-24525.5983859375, 65628.9172449607), (-24518.859385937507, 65629.0857199607), (-24518.859385937507, 65628.9057199607), (-24525.5983859375, 65628.9172449607), (-24525.5983859375, 65628.7872449607)]</t>
         </is>
       </c>
     </row>
@@ -6047,7 +6047,7 @@
       </c>
       <c r="B563" t="inlineStr">
         <is>
-          <t>[(-0.300000000008061, 562.0), (-0.300000000008061, 561.74), (-6.683, 561.8404250000002), (-6.683, 561.5804250000002), (-0.300000000008061, 561.74), (-0.300000000008061, 561.48), (-6.683, 561.5804250000002), (-6.683, 561.4204250000003)]</t>
+          <t>[(-24390.659385937506, 65586.2767059671), (-24390.659385937506, 65586.01670596711), (-24397.0423859375, 65586.1171309671), (-24397.0423859375, 65585.85713096711), (-24390.659385937506, 65586.01670596711), (-24390.659385937506, 65585.7567059671), (-24397.0423859375, 65585.85713096711), (-24397.0423859375, 65585.6971309671)]</t>
         </is>
       </c>
     </row>
@@ -6057,7 +6057,7 @@
       </c>
       <c r="B564" t="inlineStr">
         <is>
-          <t>[(-0.300000000007116, 563.0), (-0.300000000007116, 562.68), (-6.372, 562.8525041500043), (-6.372, 562.6125041500043), (-0.300000000007116, 562.68), (-0.300000000007116, 562.36), (-6.372, 562.6125041500043), (-6.372, 562.3725041500043)]</t>
+          <t>[(-24380.659385937506, 65631.2711045127), (-24380.659385937506, 65630.9511045127), (-24386.7313859375, 65631.12360866272), (-24386.7313859375, 65630.88360866271), (-24380.659385937506, 65630.9511045127), (-24380.659385937506, 65630.63110451271), (-24386.7313859375, 65630.88360866271), (-24386.7313859375, 65630.64360866272)]</t>
         </is>
       </c>
     </row>
@@ -6067,7 +6067,7 @@
       </c>
       <c r="B565" t="inlineStr">
         <is>
-          <t>[(-0.300000000007116, 564.0), (-0.300000000007116, 563.79), (-6.054, 564.0040787350335), (-6.054, 563.7940787350335), (-0.300000000007116, 563.79), (-0.300000000007116, 563.58), (-6.054, 563.7940787350335), (-6.054, 563.5840787350336), (-0.300000000007116, 563.58), (-0.300000000007116, 563.38), (-6.054, 563.5840787350336), (-6.054, 563.4340787350335)]</t>
+          <t>[(-24179.459385937505, 65586.2071205681), (-24179.459385937505, 65585.99712056809), (-24185.2133859375, 65586.21119930313), (-24185.2133859375, 65586.00119930312), (-24179.459385937505, 65585.99712056809), (-24179.459385937505, 65585.7871205681), (-24185.2133859375, 65586.00119930312), (-24185.2133859375, 65585.79119930313), (-24179.459385937505, 65585.7871205681), (-24179.459385937505, 65585.5871205681), (-24185.2133859375, 65585.79119930313), (-24185.2133859375, 65585.64119930312)]</t>
         </is>
       </c>
     </row>
@@ -6077,7 +6077,7 @@
       </c>
       <c r="B566" t="inlineStr">
         <is>
-          <t>[(-0.300000757202311, 565.0), (-0.300000757202311, 564.84), (-5.826, 565.1394989879266), (-5.826, 564.9794989879266), (-0.300000757202311, 564.84), (-0.300000757202311, 564.68), (-5.826, 564.9794989879266), (-5.826, 564.8194989879265), (-0.300000757202311, 564.68), (-0.300000757202311, 564.52), (-5.826, 564.8194989879265), (-5.826, 564.6594989879266), (-0.300000757202311, 564.52), (-0.300000757202311, 564.38), (-5.826, 564.6594989879266), (-5.826, 564.5294989879266)]</t>
+          <t>[(-23982.2593866948, 65587.073692179), (-23982.2593866948, 65586.91369217899), (-23987.7853859376, 65587.21319116693), (-23987.7853859376, 65587.05319116692), (-23982.2593866948, 65586.91369217899), (-23982.2593866948, 65586.75369217899), (-23987.7853859376, 65587.05319116692), (-23987.7853859376, 65586.89319116692), (-23982.2593866948, 65586.75369217899), (-23982.2593866948, 65586.593692179), (-23987.7853859376, 65586.89319116692), (-23987.7853859376, 65586.73319116693), (-23982.2593866948, 65586.593692179), (-23982.2593866948, 65586.453692179), (-23987.7853859376, 65586.73319116693), (-23987.7853859376, 65586.60319116693)]</t>
         </is>
       </c>
     </row>
@@ -6087,7 +6087,7 @@
       </c>
       <c r="B567" t="inlineStr">
         <is>
-          <t>[(-0.300000000075906, 566.0), (-0.300000000075906, 565.8), (-5.72, 566.1834876710177), (-5.72, 565.9834876710177), (-0.300000000075906, 565.8), (-0.300000000075906, 565.6), (-5.72, 565.9834876710177), (-5.72, 565.7834876710177), (-0.300000000075906, 565.6), (-0.300000000075906, 565.46), (-5.72, 565.7834876710177), (-5.72, 565.6034876710177)]</t>
+          <t>[(-23804.059385937675, 65587.8708193455), (-23804.059385937675, 65587.6708193455), (-23809.4793859376, 65588.05430701651), (-23809.4793859376, 65587.85430701652), (-23804.059385937675, 65587.6708193455), (-23804.059385937675, 65587.4708193455), (-23809.4793859376, 65587.85430701652), (-23809.4793859376, 65587.65430701652), (-23804.059385937675, 65587.4708193455), (-23804.059385937675, 65587.3308193455), (-23809.4793859376, 65587.65430701652), (-23809.4793859376, 65587.47430701651)]</t>
         </is>
       </c>
     </row>
@@ -6097,7 +6097,7 @@
       </c>
       <c r="B568" t="inlineStr">
         <is>
-          <t>[(-0.300000000025587, 567.0), (-0.300000000025587, 566.8), (-5.575, 567.2239950031004), (-5.575, 567.0239950031004), (-0.300000000025587, 566.8), (-0.300000000025587, 566.6), (-5.575, 567.0239950031004), (-5.575, 566.8239950031004), (-0.300000000025587, 566.6), (-0.300000000025587, 566.47), (-5.575, 566.8239950031004), (-5.575, 566.6239950031004)]</t>
+          <t>[(-23616.859385937525, 65586.5985020675), (-23616.859385937525, 65586.3985020675), (-23622.1343859375, 65586.8224970706), (-23622.1343859375, 65586.62249707061), (-23616.859385937525, 65586.3985020675), (-23616.859385937525, 65586.1985020675), (-23622.1343859375, 65586.62249707061), (-23622.1343859375, 65586.42249707061), (-23616.859385937525, 65586.1985020675), (-23616.859385937525, 65586.0685020675), (-23622.1343859375, 65586.42249707061), (-23622.1343859375, 65586.2224970706)]</t>
         </is>
       </c>
     </row>
@@ -6107,7 +6107,7 @@
       </c>
       <c r="B569" t="inlineStr">
         <is>
-          <t>[(-0.300000000012235, 568.0), (-0.300000000012235, 567.7), (-5.352, 568.2580218142429), (-5.352, 567.9580218142429), (-0.300000000012235, 567.7), (-0.300000000012235, 567.49), (-5.352, 567.9580218142429), (-5.352, 567.6680218142428)]</t>
+          <t>[(-23616.859385937612, 65643.2567403451), (-23616.859385937612, 65642.9567403451), (-23621.911385937598, 65643.51476215934), (-23621.911385937598, 65643.21476215933), (-23616.859385937612, 65642.9567403451), (-23616.859385937612, 65642.7467403451), (-23621.911385937598, 65643.21476215933), (-23621.911385937598, 65642.92476215934)]</t>
         </is>
       </c>
     </row>
@@ -6117,7 +6117,7 @@
       </c>
       <c r="B570" t="inlineStr">
         <is>
-          <t>[(-0.300000000024299, 569.0), (-0.300000000024299, 568.7), (-5.076, 569.2850455084679), (-5.076, 568.9850455084679), (-0.300000000024299, 568.7), (-0.300000000024299, 568.53), (-5.076, 568.9850455084679), (-5.076, 568.6850455084679)]</t>
+          <t>[(-23436.659385937524, 65587.8455341783), (-23436.659385937524, 65587.5455341783), (-23441.4353859375, 65588.13057968677), (-23441.4353859375, 65587.83057968676), (-23436.659385937524, 65587.5455341783), (-23436.659385937524, 65587.3755341783), (-23441.4353859375, 65587.83057968676), (-23441.4353859375, 65587.53057968676)]</t>
         </is>
       </c>
     </row>
@@ -6127,7 +6127,7 @@
       </c>
       <c r="B571" t="inlineStr">
         <is>
-          <t>[(-0.300000000096395, 570.0), (-0.300000000096395, 569.78), (-4.808, 570.3078629923943), (-4.808, 569.9978629923944), (-0.300000000096395, 569.78), (-0.300000000096395, 569.56), (-4.808, 569.9978629923944), (-4.808, 569.6878629923943)]</t>
+          <t>[(-23446.659385937597, 65638.364883567), (-23446.659385937597, 65638.144883567), (-23451.1673859375, 65638.6727465594), (-23451.1673859375, 65638.3627465594), (-23446.659385937597, 65638.144883567), (-23446.659385937597, 65637.924883567), (-23451.1673859375, 65638.3627465594), (-23451.1673859375, 65638.0527465594)]</t>
         </is>
       </c>
     </row>
@@ -6137,7 +6137,7 @@
       </c>
       <c r="B572" t="inlineStr">
         <is>
-          <t>[(-0.300000000000165, 571.0), (-0.300000000000165, 570.78), (-4.475, 571.29225), (-4.475, 570.99225), (-0.300000000000165, 570.78), (-0.300000000000165, 570.56), (-4.475, 570.99225), (-4.475, 570.69225)]</t>
+          <t>[(-23369.6593859375, 65588.8147885112), (-23369.6593859375, 65588.5947885112), (-23373.834385937498, 65589.1070385112), (-23373.834385937498, 65588.8070385112), (-23369.6593859375, 65588.5947885112), (-23369.6593859375, 65588.3747885112), (-23373.834385937498, 65588.8070385112), (-23373.834385937498, 65588.50703851119)]</t>
         </is>
       </c>
     </row>
@@ -6147,7 +6147,7 @@
       </c>
       <c r="B573" t="inlineStr">
         <is>
-          <t>[(-0.300000000004786, 572.0), (-0.300000000004786, 571.76), (-4.178, 572.2714599999997), (-4.178, 571.9514599999997), (-0.300000000004786, 571.76), (-0.300000000004786, 571.52), (-4.178, 571.9514599999997), (-4.178, 571.6314599999997)]</t>
+          <t>[(-23374.659385937506, 65639.195249011), (-23374.659385937506, 65638.95524901099), (-23378.5373859375, 65639.466709011), (-23378.5373859375, 65639.146709011), (-23374.659385937506, 65638.95524901099), (-23374.659385937506, 65638.715249011), (-23378.5373859375, 65639.146709011), (-23378.5373859375, 65638.826709011)]</t>
         </is>
       </c>
     </row>
@@ -6157,7 +6157,7 @@
       </c>
       <c r="B574" t="inlineStr">
         <is>
-          <t>[(-0.299999999990177, 573.0), (-0.299999999990177, 572.72), (-3.883, 573.2508100000007), (-3.883, 572.9708100000007), (-0.299999999990177, 572.72), (-0.299999999990177, 572.55), (-3.883, 572.9708100000007), (-3.883, 572.6908100000007)]</t>
+          <t>[(-23269.459385937487, 65587.5062650664), (-23269.459385937487, 65587.2262650664), (-23273.0423859375, 65587.7570750664), (-23273.0423859375, 65587.4770750664), (-23269.459385937487, 65587.2262650664), (-23269.459385937487, 65587.0562650664), (-23273.0423859375, 65587.4770750664), (-23273.0423859375, 65587.1970750664)]</t>
         </is>
       </c>
     </row>
@@ -6167,7 +6167,7 @@
       </c>
       <c r="B575" t="inlineStr">
         <is>
-          <t>[(-0.300000000002488, 574.0), (-0.300000000002488, 573.75), (-3.535, 574.2264499999998), (-3.535, 573.9764499999998), (-0.300000000002488, 573.75), (-0.300000000002488, 573.58), (-3.535, 573.9764499999998), (-3.535, 573.7264499999998)]</t>
+          <t>[(-23269.4593859375, 65629.7478366773), (-23269.4593859375, 65629.4978366773), (-23272.6943859375, 65629.9742866773), (-23272.6943859375, 65629.7242866773), (-23269.4593859375, 65629.4978366773), (-23269.4593859375, 65629.3278366773), (-23272.6943859375, 65629.7242866773), (-23272.6943859375, 65629.4742866773)]</t>
         </is>
       </c>
     </row>
@@ -6177,7 +6177,7 @@
       </c>
       <c r="B576" t="inlineStr">
         <is>
-          <t>[(-0.299999999991817, 575.0), (-0.299999999991817, 574.79), (-3.088, 575.1951600000006), (-3.088, 574.9851600000005), (-0.299999999991817, 574.79), (-0.299999999991817, 574.64), (-3.088, 574.9851600000005), (-3.088, 574.7751600000006)]</t>
+          <t>[(-23210.45938593749, 65585.9199638438), (-23210.45938593749, 65585.7099638438), (-23213.2473859375, 65586.1151238438), (-23213.2473859375, 65585.9051238438), (-23210.45938593749, 65585.7099638438), (-23210.45938593749, 65585.5599638438), (-23213.2473859375, 65585.9051238438), (-23213.2473859375, 65585.6951238438)]</t>
         </is>
       </c>
     </row>
@@ -6187,7 +6187,7 @@
       </c>
       <c r="B577" t="inlineStr">
         <is>
-          <t>[(-0.300000000006434, 576.0), (-0.300000000006434, 575.77), (-2.856, 576.1789199999995), (-2.856, 575.9489199999995), (-0.300000000006434, 575.77), (-0.300000000006434, 575.64), (-2.856, 575.9489199999995), (-2.856, 575.7289199999994)]</t>
+          <t>[(-23210.459385937505, 65628.0226465658), (-23210.459385937505, 65627.79264656581), (-23213.0153859375, 65628.20156656581), (-23213.0153859375, 65627.97156656582), (-23210.459385937505, 65627.79264656581), (-23210.459385937505, 65627.6626465658), (-23213.0153859375, 65627.97156656582), (-23213.0153859375, 65627.75156656581)]</t>
         </is>
       </c>
     </row>
@@ -6197,7 +6197,7 @@
       </c>
       <c r="B578" t="inlineStr">
         <is>
-          <t>[(-0.30000000000059, 577.0), (-0.30000000000059, 576.76), (-2.574, 577.15918), (-2.574, 576.91918), (-0.30000000000059, 576.76), (-0.30000000000059, 576.58), (-2.574, 576.91918), (-2.574, 576.67918)]</t>
+          <t>[(-23072.2593859375, 65586.0558848434), (-23072.2593859375, 65585.8158848434), (-23074.533385937502, 65586.2150648434), (-23074.533385937502, 65585.9750648434), (-23072.2593859375, 65585.8158848434), (-23072.2593859375, 65585.6358848434), (-23074.533385937502, 65585.9750648434), (-23074.533385937502, 65585.73506484341)]</t>
         </is>
       </c>
     </row>
@@ -6257,7 +6257,7 @@
       </c>
       <c r="B584" t="inlineStr">
         <is>
-          <t>[(-0.300000000087704, 583.0), (-0.300000000087704, 582.82), (-2.817, 583.0832250563453), (-2.817, 582.9032250563454), (-0.300000000087704, 582.82), (-0.300000000087704, 582.64), (-2.817, 582.9032250563454), (-2.817, 582.7232250563453), (-0.300000000087704, 582.64), (-0.300000000087704, 582.51), (-2.817, 582.7232250563453), (-2.817, 582.5532250563454)]</t>
+          <t>[(-22825.059385937588, 65593.0185068088), (-22825.059385937588, 65592.83850680881), (-22827.5763859375, 65593.10173186514), (-22827.5763859375, 65592.92173186515), (-22825.059385937588, 65592.83850680881), (-22825.059385937588, 65592.6585068088), (-22827.5763859375, 65592.92173186515), (-22827.5763859375, 65592.74173186514), (-22825.059385937588, 65592.6585068088), (-22825.059385937588, 65592.5285068088), (-22827.5763859375, 65592.74173186514), (-22827.5763859375, 65592.57173186514)]</t>
         </is>
       </c>
     </row>
@@ -6267,7 +6267,7 @@
       </c>
       <c r="B585" t="inlineStr">
         <is>
-          <t>[(-0.30000000000313, 584.0), (-0.30000000000313, 583.8), (-3.503, 584.0750107082638), (-3.503, 583.8750107082637), (-0.30000000000313, 583.8), (-0.30000000000313, 583.6), (-3.503, 583.8750107082637), (-3.503, 583.6750107082638), (-0.30000000000313, 583.6), (-0.30000000000313, 583.48), (-3.503, 583.6750107082638), (-3.503, 583.4950107082637)]</t>
+          <t>[(-22835.059385937602, 65642.7757627227), (-22835.059385937602, 65642.5757627227), (-22838.2623859376, 65642.85077343095), (-22838.2623859376, 65642.65077343096), (-22835.059385937602, 65642.5757627227), (-22835.059385937602, 65642.3757627227), (-22838.2623859376, 65642.65077343096), (-22838.2623859376, 65642.45077343096), (-22835.059385937602, 65642.3757627227), (-22835.059385937602, 65642.25576272269), (-22838.2623859376, 65642.45077343096), (-22838.2623859376, 65642.27077343095)]</t>
         </is>
       </c>
     </row>
@@ -6277,7 +6277,7 @@
       </c>
       <c r="B586" t="inlineStr">
         <is>
-          <t>[(-0.30000000000313, 585.0), (-0.30000000000313, 584.81), (-4.21, 584.9938178642872), (-4.21, 584.8038178642871), (-0.30000000000313, 584.81), (-0.30000000000313, 584.62), (-4.21, 584.8038178642871), (-4.21, 584.6138178642872), (-0.30000000000313, 584.62), (-0.30000000000313, 584.49), (-4.21, 584.6138178642872), (-4.21, 584.4338178642872)]</t>
+          <t>[(-22704.859385937503, 65590.5330186365), (-22704.859385937503, 65590.3430186365), (-22708.7693859375, 65590.5268365008), (-22708.7693859375, 65590.33683650079), (-22704.859385937503, 65590.3430186365), (-22704.859385937503, 65590.1530186365), (-22708.7693859375, 65590.33683650079), (-22708.7693859375, 65590.14683650079), (-22704.859385937503, 65590.1530186365), (-22704.859385937503, 65590.02301863651), (-22708.7693859375, 65590.14683650079), (-22708.7693859375, 65589.9668365008)]</t>
         </is>
       </c>
     </row>
@@ -6287,7 +6287,7 @@
       </c>
       <c r="B587" t="inlineStr">
         <is>
-          <t>[(-0.300000000004766, 586.0), (-0.300000000004766, 585.86), (-4.773, 585.8881750000002), (-4.773, 585.7481750000002), (-0.300000000004766, 585.86), (-0.300000000004766, 585.72), (-4.773, 585.7481750000002), (-4.773, 585.6081750000002), (-0.300000000004766, 585.72), (-0.300000000004766, 585.58), (-4.773, 585.6081750000002), (-4.773, 585.4681750000002), (-0.300000000004766, 585.58), (-0.300000000004766, 585.45), (-4.773, 585.4681750000002), (-4.773, 585.3381750000002)]</t>
+          <t>[(-22704.859385937507, 65634.2902745504), (-22704.859385937507, 65634.1502745504), (-22709.3323859375, 65634.1784495504), (-22709.3323859375, 65634.0384495504), (-22704.859385937507, 65634.1502745504), (-22704.859385937507, 65634.0102745504), (-22709.3323859375, 65634.0384495504), (-22709.3323859375, 65633.8984495504), (-22704.859385937507, 65634.0102745504), (-22704.859385937507, 65633.8702745504), (-22709.3323859375, 65633.8984495504), (-22709.3323859375, 65633.7584495504), (-22704.859385937507, 65633.8702745504), (-22704.859385937507, 65633.7402745504), (-22709.3323859375, 65633.7584495504), (-22709.3323859375, 65633.6284495504)]</t>
         </is>
       </c>
     </row>
@@ -6297,7 +6297,7 @@
       </c>
       <c r="B588" t="inlineStr">
         <is>
-          <t>[(-0.30000000000313, 587.0), (-0.30000000000313, 586.81), (-5.262, 586.8759500000001), (-5.262, 586.68595), (-0.30000000000313, 586.81), (-0.30000000000313, 586.62), (-5.262, 586.68595), (-5.262, 586.4959500000001), (-0.30000000000313, 586.62), (-0.30000000000313, 586.46), (-5.262, 586.4959500000001), (-5.262, 586.3159500000002)]</t>
+          <t>[(-22645.859385937503, 65590.0475304642), (-22645.859385937503, 65589.8575304642), (-22650.8213859375, 65589.9234804642), (-22650.8213859375, 65589.7334804642), (-22645.859385937503, 65589.8575304642), (-22645.859385937503, 65589.6675304642), (-22650.8213859375, 65589.7334804642), (-22650.8213859375, 65589.5434804642), (-22645.859385937503, 65589.6675304642), (-22645.859385937503, 65589.50753046421), (-22650.8213859375, 65589.5434804642), (-22650.8213859375, 65589.3634804642)]</t>
         </is>
       </c>
     </row>
@@ -6307,7 +6307,7 @@
       </c>
       <c r="B589" t="inlineStr">
         <is>
-          <t>[(-0.30000000000313, 588.0), (-0.30000000000313, 587.83), (-5.703, 587.8649250000001), (-5.703, 587.6949250000001), (-0.30000000000313, 587.83), (-0.30000000000313, 587.66), (-5.703, 587.6949250000001), (-5.703, 587.524925), (-0.30000000000313, 587.66), (-0.30000000000313, 587.52), (-5.703, 587.524925), (-5.703, 587.3649250000001)]</t>
+          <t>[(-22635.859385937503, 65631.8047863781), (-22635.859385937503, 65631.6347863781), (-22641.2623859375, 65631.6697113781), (-22641.2623859375, 65631.4997113781), (-22635.859385937503, 65631.6347863781), (-22635.859385937503, 65631.4647863781), (-22641.2623859375, 65631.4997113781), (-22641.2623859375, 65631.3297113781), (-22635.859385937503, 65631.4647863781), (-22635.859385937503, 65631.3247863781), (-22641.2623859375, 65631.3297113781), (-22641.2623859375, 65631.1697113781)]</t>
         </is>
       </c>
     </row>
@@ -6317,7 +6317,7 @@
       </c>
       <c r="B590" t="inlineStr">
         <is>
-          <t>[(-0.299999999999168, 589.0), (-0.299999999999168, 588.76), (-6.002, 588.85745), (-6.002, 588.61745), (-0.299999999999168, 588.76), (-0.299999999999168, 588.57), (-6.002, 588.61745), (-6.002, 588.38745)]</t>
+          <t>[(-22507.6593859376, 65589.5620422919), (-22507.6593859376, 65589.3220422919), (-22513.361385937602, 65589.4194922919), (-22513.361385937602, 65589.17949229189), (-22507.6593859376, 65589.3220422919), (-22507.6593859376, 65589.13204229191), (-22513.361385937602, 65589.17949229189), (-22513.361385937602, 65588.9494922919)]</t>
         </is>
       </c>
     </row>
@@ -6327,7 +6327,7 @@
       </c>
       <c r="B591" t="inlineStr">
         <is>
-          <t>[(-0.300000000004184, 590.0), (-0.300000000004184, 589.85), (-6.096, 589.8551000000001), (-6.096, 589.7051000000001), (-0.300000000004184, 589.85), (-0.300000000004184, 589.7), (-6.096, 589.7051000000001), (-6.096, 589.5551000000002), (-0.300000000004184, 589.7), (-0.300000000004184, 589.56), (-6.096, 589.5551000000002), (-6.096, 589.4251000000002)]</t>
+          <t>[(-22507.659385937503, 65633.3192982058), (-22507.659385937503, 65633.1692982058), (-22513.4553859375, 65633.1743982058), (-22513.4553859375, 65633.0243982058), (-22507.659385937503, 65633.1692982058), (-22507.659385937503, 65633.01929820579), (-22513.4553859375, 65633.0243982058), (-22513.4553859375, 65632.8743982058), (-22507.659385937503, 65633.01929820579), (-22507.659385937503, 65632.8792982058), (-22513.4553859375, 65632.8743982058), (-22513.4553859375, 65632.7443982058)]</t>
         </is>
       </c>
     </row>
@@ -6337,7 +6337,7 @@
       </c>
       <c r="B592" t="inlineStr">
         <is>
-          <t>[(-0.299999999996994, 591.0), (-0.299999999996994, 590.8), (-6.187, 590.8528249999999), (-6.187, 590.6528249999999), (-0.299999999996994, 590.8), (-0.299999999996994, 590.61), (-6.187, 590.6528249999999), (-6.187, 590.4828249999999)]</t>
+          <t>[(-22439.659385937495, 65589.0765541196), (-22439.659385937495, 65588.8765541196), (-22445.5463859375, 65588.9293791196), (-22445.5463859375, 65588.7293791196), (-22439.659385937495, 65588.8765541196), (-22439.659385937495, 65588.6865541196), (-22445.5463859375, 65588.7293791196), (-22445.5463859375, 65588.5593791196)]</t>
         </is>
       </c>
     </row>
@@ -6347,7 +6347,7 @@
       </c>
       <c r="B593" t="inlineStr">
         <is>
-          <t>[(-0.300000000003808, 592.0), (-0.300000000003808, 591.8), (-6.289, 591.8502750000001), (-6.289, 591.6502750000001), (-0.300000000003808, 591.8), (-0.300000000003808, 591.62), (-6.289, 591.6502750000001), (-6.289, 591.4602750000001)]</t>
+          <t>[(-22449.659385937503, 65634.8338100335), (-22449.659385937503, 65634.6338100335), (-22455.6483859375, 65634.6840850335), (-22455.6483859375, 65634.4840850335), (-22449.659385937503, 65634.6338100335), (-22449.659385937503, 65634.45381003349), (-22455.6483859375, 65634.4840850335), (-22455.6483859375, 65634.2940850335)]</t>
         </is>
       </c>
     </row>
@@ -6357,7 +6357,7 @@
       </c>
       <c r="B594" t="inlineStr">
         <is>
-          <t>[(-0.300000000004488, 593.0), (-0.300000000004488, 592.85), (-6.402, 592.8474500000001), (-6.402, 592.6974500000001), (-0.300000000004488, 592.85), (-0.300000000004488, 592.7), (-6.402, 592.6974500000001), (-6.402, 592.5474500000001), (-0.300000000004488, 592.7), (-0.300000000004488, 592.56), (-6.402, 592.5474500000001), (-6.402, 592.39745)]</t>
+          <t>[(-22328.4593859375, 65588.5905334043), (-22328.4593859375, 65588.44053340431), (-22334.561385937497, 65588.4379834043), (-22334.561385937497, 65588.28798340431), (-22328.4593859375, 65588.44053340431), (-22328.4593859375, 65588.2905334043), (-22334.561385937497, 65588.28798340431), (-22334.561385937497, 65588.1379834043), (-22328.4593859375, 65588.2905334043), (-22328.4593859375, 65588.1505334043), (-22334.561385937497, 65588.1379834043), (-22334.561385937497, 65587.98798340431)]</t>
         </is>
       </c>
     </row>
@@ -6367,7 +6367,7 @@
       </c>
       <c r="B595" t="inlineStr">
         <is>
-          <t>[(-0.299999999990689, 594.0), (-0.299999999990689, 593.84), (-6.422, 593.8469499999998), (-6.422, 593.6869499999998), (-0.299999999990689, 593.84), (-0.299999999990689, 593.68), (-6.422, 593.6869499999998), (-6.422, 593.5269499999997), (-0.299999999990689, 593.68), (-0.299999999990689, 593.54), (-6.422, 593.5269499999997), (-6.422, 593.3669499999997)]</t>
+          <t>[(-22328.45938593749, 65628.3044668459), (-22328.45938593749, 65628.1444668459), (-22334.581385937498, 65628.15141684591), (-22334.581385937498, 65627.9914168459), (-22328.45938593749, 65628.1444668459), (-22328.45938593749, 65627.9844668459), (-22334.581385937498, 65627.9914168459), (-22334.581385937498, 65627.8314168459), (-22328.45938593749, 65627.9844668459), (-22328.45938593749, 65627.8444668459), (-22334.581385937498, 65627.8314168459), (-22334.581385937498, 65627.67141684591)]</t>
         </is>
       </c>
     </row>
@@ -6377,7 +6377,7 @@
       </c>
       <c r="B596" t="inlineStr">
         <is>
-          <t>[(-0.299999999990689, 595.0), (-0.299999999990689, 594.83), (-6.296, 594.8500999999998), (-6.296, 594.6800999999998), (-0.299999999990689, 594.83), (-0.299999999990689, 594.66), (-6.296, 594.6800999999998), (-6.296, 594.5100999999997), (-0.299999999990689, 594.66), (-0.299999999990689, 594.51), (-6.296, 594.5100999999997), (-6.296, 594.3400999999998)]</t>
+          <t>[(-22269.45938593749, 65587.948955843), (-22269.45938593749, 65587.77895584301), (-22275.455385937497, 65587.799055843), (-22275.455385937497, 65587.629055843), (-22269.45938593749, 65587.77895584301), (-22269.45938593749, 65587.60895584301), (-22275.455385937497, 65587.629055843), (-22275.455385937497, 65587.459055843), (-22269.45938593749, 65587.60895584301), (-22269.45938593749, 65587.458955843), (-22275.455385937497, 65587.459055843), (-22275.455385937497, 65587.28905584301)]</t>
         </is>
       </c>
     </row>
@@ -6387,7 +6387,7 @@
       </c>
       <c r="B597" t="inlineStr">
         <is>
-          <t>[(-0.299999999990689, 596.0), (-0.299999999990689, 595.78), (-6.131, 595.8542249999998), (-6.131, 595.6342249999998), (-0.299999999990689, 595.78), (-0.299999999990689, 595.61), (-6.131, 595.6342249999998), (-6.131, 595.4142249999998)]</t>
+          <t>[(-22259.45938593749, 65627.5240003957), (-22259.45938593749, 65627.3040003957), (-22265.2903859375, 65627.3782253957), (-22265.2903859375, 65627.1582253957), (-22259.45938593749, 65627.3040003957), (-22259.45938593749, 65627.1340003957), (-22265.2903859375, 65627.1582253957), (-22265.2903859375, 65626.9382253957)]</t>
         </is>
       </c>
     </row>
@@ -6397,7 +6397,7 @@
       </c>
       <c r="B598" t="inlineStr">
         <is>
-          <t>[(-0.299999999990689, 597.0), (-0.299999999990689, 596.8), (-6.058, 596.8560499999998), (-6.058, 596.6560499999997), (-0.299999999990689, 596.8), (-0.299999999990689, 596.61), (-6.058, 596.6560499999997), (-6.058, 596.4960499999997)]</t>
+          <t>[(-22131.259385937494, 65587.0296005039), (-22131.259385937494, 65586.8296005039), (-22137.017385937503, 65586.8856505039), (-22137.017385937503, 65586.6856505039), (-22131.259385937494, 65586.8296005039), (-22131.259385937494, 65586.6396005039), (-22137.017385937503, 65586.6856505039), (-22137.017385937503, 65586.5256505039)]</t>
         </is>
       </c>
     </row>
@@ -6407,7 +6407,7 @@
       </c>
       <c r="B599" t="inlineStr">
         <is>
-          <t>[(-0.299999999993936, 598.0), (-0.299999999993936, 597.83), (-6.146, 597.8538499999999), (-6.146, 597.6838499999999), (-0.299999999993936, 597.83), (-0.299999999993936, 597.53), (-6.146, 597.6838499999999), (-6.146, 597.5638499999999)]</t>
+          <t>[(-22131.259385937497, 65632.4657561677), (-22131.259385937497, 65632.2957561677), (-22137.105385937502, 65632.3196061677), (-22137.105385937502, 65632.1496061677), (-22131.259385937497, 65632.2957561677), (-22131.259385937497, 65631.9957561677), (-22137.105385937502, 65632.1496061677), (-22137.105385937502, 65632.0296061677)]</t>
         </is>
       </c>
     </row>
@@ -6417,7 +6417,7 @@
       </c>
       <c r="B600" t="inlineStr">
         <is>
-          <t>[(-0.299999999990689, 599.0), (-0.299999999990689, 598.74), (-6.221, 598.8519749999998), (-6.221, 598.5919749999998), (-0.299999999990689, 598.74), (-0.299999999990689, 598.48), (-6.221, 598.5919749999998), (-6.221, 598.3819749999998)]</t>
+          <t>[(-22063.259385937494, 65587.83246738701), (-22063.259385937494, 65587.57246738701), (-22069.180385937503, 65587.684442387), (-22069.180385937503, 65587.42444238701), (-22063.259385937494, 65587.57246738701), (-22063.259385937494, 65587.312467387), (-22069.180385937503, 65587.42444238701), (-22069.180385937503, 65587.214442387)]</t>
         </is>
       </c>
     </row>
@@ -6427,7 +6427,7 @@
       </c>
       <c r="B601" t="inlineStr">
         <is>
-          <t>[(-0.299999999992312, 600.0), (-0.299999999992312, 599.72), (-6.222, 599.8519499999998), (-6.222, 599.5719499999998), (-0.299999999992312, 599.72), (-0.299999999992312, 599.45), (-6.222, 599.5719499999998), (-6.222, 599.4219499999998)]</t>
+          <t>[(-22063.259385937494, 65633.1297341619), (-22063.259385937494, 65632.84973416191), (-22069.181385937503, 65632.9816841619), (-22069.181385937503, 65632.7016841619), (-22063.259385937494, 65632.84973416191), (-22063.259385937494, 65632.5797341619), (-22069.181385937503, 65632.7016841619), (-22069.181385937503, 65632.55168416191)]</t>
         </is>
       </c>
     </row>
@@ -6437,7 +6437,7 @@
       </c>
       <c r="B602" t="inlineStr">
         <is>
-          <t>[(-0.299999999990689, 601.0), (-0.299999999990689, 600.76), (-6.155, 600.8536249999997), (-6.155, 600.6136249999997), (-0.299999999990689, 600.76), (-0.299999999990689, 600.46), (-6.155, 600.6136249999997), (-6.155, 600.4836249999997)]</t>
+          <t>[(-21943.059385937493, 65590.3575564923), (-21943.059385937493, 65590.11755649229), (-21948.9143859375, 65590.2111814923), (-21948.9143859375, 65589.97118149229), (-21943.059385937493, 65590.11755649229), (-21943.059385937493, 65589.8175564923), (-21948.9143859375, 65589.97118149229), (-21948.9143859375, 65589.8411814923)]</t>
         </is>
       </c>
     </row>
@@ -6447,7 +6447,7 @@
       </c>
       <c r="B603" t="inlineStr">
         <is>
-          <t>[(-0.29999999999556, 602.0), (-0.29999999999556, 601.74), (-6.006, 601.8573499999999), (-6.006, 601.7173499999999), (-0.29999999999556, 601.74), (-0.29999999999556, 601.48), (-6.006, 601.7173499999999), (-6.006, 601.5773499999999)]</t>
+          <t>[(-21953.059385937497, 65637.5159343783), (-21953.059385937497, 65637.2559343783), (-21958.765385937502, 65637.37328437831), (-21958.765385937502, 65637.23328437831), (-21953.059385937497, 65637.2559343783), (-21953.059385937497, 65636.9959343783), (-21958.765385937502, 65637.23328437831), (-21958.765385937502, 65637.09328437831)]</t>
         </is>
       </c>
     </row>
@@ -6457,7 +6457,7 @@
       </c>
       <c r="B604" t="inlineStr">
         <is>
-          <t>[(-0.300000000002968, 603.0), (-0.300000000002968, 602.76), (-5.889, 602.8602750000001), (-5.889, 602.7402750000001), (-0.300000000002968, 602.76), (-0.300000000002968, 602.52), (-5.889, 602.7402750000001), (-5.889, 602.6202750000001)]</t>
+          <t>[(-21884.059385937504, 65590.6048768857), (-21884.059385937504, 65590.3648768857), (-21889.6483859375, 65590.4651518857), (-21889.6483859375, 65590.3451518857), (-21884.059385937504, 65590.3648768857), (-21884.059385937504, 65590.1248768857), (-21889.6483859375, 65590.3451518857), (-21889.6483859375, 65590.2251518857)]</t>
         </is>
       </c>
     </row>
@@ -6467,7 +6467,7 @@
       </c>
       <c r="B605" t="inlineStr">
         <is>
-          <t>[(-0.299999999994839, 604.0), (-0.299999999994839, 603.76), (-5.788, 603.8627999999999), (-5.788, 603.7427999999999), (-0.299999999994839, 603.76), (-0.299999999994839, 603.52), (-5.788, 603.7427999999999), (-5.788, 603.6227999999999)]</t>
+          <t>[(-21884.059385937497, 65637.66021021901), (-21884.059385937497, 65637.420210219), (-21889.5473859375, 65637.52301021901), (-21889.5473859375, 65637.40301021902), (-21884.059385937497, 65637.420210219), (-21884.059385937497, 65637.18021021901), (-21889.5473859375, 65637.40301021902), (-21889.5473859375, 65637.283010219)]</t>
         </is>
       </c>
     </row>
@@ -6477,7 +6477,7 @@
       </c>
       <c r="B606" t="inlineStr">
         <is>
-          <t>[(-0.300000000000944, 605.0), (-0.300000000000944, 604.76), (-5.663, 604.8659250000001), (-5.663, 604.7359250000001), (-0.300000000000944, 604.76), (-0.300000000000944, 604.52), (-5.663, 604.7359250000001), (-5.663, 604.6059250000001)]</t>
+          <t>[(-21763.8593859375, 65590.7155435523), (-21763.8593859375, 65590.4755435523), (-21769.2223859375, 65590.58146855231), (-21769.2223859375, 65590.4514685523), (-21763.8593859375, 65590.4755435523), (-21763.8593859375, 65590.2355435523), (-21769.2223859375, 65590.4514685523), (-21769.2223859375, 65590.32146855231)]</t>
         </is>
       </c>
     </row>
@@ -6487,7 +6487,7 @@
       </c>
       <c r="B607" t="inlineStr">
         <is>
-          <t>[(-0.300000000001999, 606.0), (-0.300000000001999, 605.74), (-5.511, 605.869725), (-5.511, 605.719725), (-0.300000000001999, 605.74), (-0.300000000001999, 605.48), (-5.511, 605.719725), (-5.511, 605.5697250000001)]</t>
+          <t>[(-21763.859385937503, 65633.7708768857), (-21763.859385937503, 65633.5108768857), (-21769.0703859375, 65633.6406018857), (-21769.0703859375, 65633.4906018857), (-21763.859385937503, 65633.5108768857), (-21763.859385937503, 65633.2508768857), (-21769.0703859375, 65633.4906018857), (-21769.0703859375, 65633.34060188569)]</t>
         </is>
       </c>
     </row>
@@ -6497,7 +6497,7 @@
       </c>
       <c r="B608" t="inlineStr">
         <is>
-          <t>[(-0.300000000003967, 607.0), (-0.300000000003967, 606.74), (-5.47, 606.87075), (-5.47, 606.7207500000001), (-0.300000000003967, 606.74), (-0.300000000003967, 606.48), (-5.47, 606.7207500000001), (-5.47, 606.5707500000001)]</t>
+          <t>[(-21703.859385937503, 65590.826210219), (-21703.859385937503, 65590.56621021901), (-21709.0293859375, 65590.69696021901), (-21709.0293859375, 65590.54696021901), (-21703.859385937503, 65590.56621021901), (-21703.859385937503, 65590.306210219), (-21709.0293859375, 65590.54696021901), (-21709.0293859375, 65590.396960219)]</t>
         </is>
       </c>
     </row>
@@ -6507,7 +6507,7 @@
       </c>
       <c r="B609" t="inlineStr">
         <is>
-          <t>[(-0.30000000000848, 608.0), (-0.30000000000848, 607.74), (-5.416, 607.8721000000002), (-5.416, 607.7021000000002), (-0.30000000000848, 607.74), (-0.30000000000848, 607.48), (-5.416, 607.7021000000002), (-5.416, 607.5321000000001)]</t>
+          <t>[(-21703.85938593751, 65631.8815435523), (-21703.85938593751, 65631.6215435523), (-21708.9753859375, 65631.75364355229), (-21708.9753859375, 65631.5836435523), (-21703.85938593751, 65631.6215435523), (-21703.85938593751, 65631.3615435523), (-21708.9753859375, 65631.5836435523), (-21708.9753859375, 65631.4136435523)]</t>
         </is>
       </c>
     </row>
@@ -6517,7 +6517,7 @@
       </c>
       <c r="B610" t="inlineStr">
         <is>
-          <t>[(-0.300000000001001, 609.0), (-0.300000000001001, 608.81), (-5.474, 608.8706500000001), (-5.474, 608.68065), (-0.300000000001001, 608.81), (-0.300000000001001, 608.51), (-5.474, 608.68065), (-5.474, 608.54065)]</t>
+          <t>[(-21576.6593859375, 65588.93687688561), (-21576.6593859375, 65588.7468768856), (-21581.833385937498, 65588.8075268856), (-21581.833385937498, 65588.6175268856), (-21576.6593859375, 65588.7468768856), (-21576.6593859375, 65588.4468768856), (-21581.833385937498, 65588.6175268856), (-21581.833385937498, 65588.4775268856)]</t>
         </is>
       </c>
     </row>
@@ -6527,7 +6527,7 @@
       </c>
       <c r="B611" t="inlineStr">
         <is>
-          <t>[(-0.299999999997719, 610.0), (-0.299999999997719, 609.82), (-5.528, 609.8693), (-5.528, 609.6893), (-0.299999999997719, 609.82), (-0.299999999997719, 609.52), (-5.528, 609.6893), (-5.528, 609.5492999999999)]</t>
+          <t>[(-21566.6593859375, 65631.992210219), (-21566.6593859375, 65631.81221021901), (-21571.887385937498, 65631.86151021901), (-21571.887385937498, 65631.68151021902), (-21566.6593859375, 65631.81221021901), (-21566.6593859375, 65631.512210219), (-21571.887385937498, 65631.68151021902), (-21571.887385937498, 65631.541510219)]</t>
         </is>
       </c>
     </row>
@@ -6537,7 +6537,7 @@
       </c>
       <c r="B612" t="inlineStr">
         <is>
-          <t>[(-0.29999999999936, 611.0), (-0.29999999999936, 610.78), (-5.578, 610.86805), (-5.578, 610.64805), (-0.29999999999936, 610.78), (-0.29999999999936, 610.56), (-5.578, 610.64805), (-5.578, 610.51805)]</t>
+          <t>[(-21498.6593859375, 65587.04760303251), (-21498.6593859375, 65586.8276030325), (-21503.9373859375, 65586.91565303251), (-21503.9373859375, 65586.69565303251), (-21498.6593859375, 65586.8276030325), (-21498.6593859375, 65586.6076030325), (-21503.9373859375, 65586.69565303251), (-21503.9373859375, 65586.5656530325)]</t>
         </is>
       </c>
     </row>
@@ -6547,7 +6547,7 @@
       </c>
       <c r="B613" t="inlineStr">
         <is>
-          <t>[(-0.299999999996078, 612.0), (-0.299999999996078, 611.84), (-5.642, 611.8664499999999), (-5.642, 611.7064499999999), (-0.299999999996078, 611.84), (-0.299999999996078, 611.68), (-5.642, 611.7064499999999), (-5.642, 611.5464499999998), (-0.299999999996078, 611.68), (-0.299999999996078, 611.55), (-5.642, 611.5464499999998), (-5.642, 611.3864499999999)]</t>
+          <t>[(-21508.659385937495, 65634.1259960596), (-21508.659385937495, 65633.9659960596), (-21514.0013859375, 65633.99244605961), (-21514.0013859375, 65633.8324460596), (-21508.659385937495, 65633.9659960596), (-21508.659385937495, 65633.8059960596), (-21514.0013859375, 65633.8324460596), (-21514.0013859375, 65633.6724460596), (-21508.659385937495, 65633.8059960596), (-21508.659385937495, 65633.67599605961), (-21514.0013859375, 65633.6724460596), (-21514.0013859375, 65633.51244605961)]</t>
         </is>
       </c>
     </row>
@@ -6557,7 +6557,7 @@
       </c>
       <c r="B614" t="inlineStr">
         <is>
-          <t>[(-0.29999999999936, 613.0), (-0.29999999999936, 612.76), (-5.707, 612.864825), (-5.707, 612.624825), (-0.29999999999936, 612.76), (-0.29999999999936, 612.59), (-5.707, 612.624825), (-5.707, 612.394825)]</t>
+          <t>[(-21387.459385937498, 65591.2460557534), (-21387.459385937498, 65591.0060557534), (-21392.866385937497, 65591.1108807534), (-21392.866385937497, 65590.8708807534), (-21387.459385937498, 65591.0060557534), (-21387.459385937498, 65590.8360557534), (-21392.866385937497, 65590.8708807534), (-21392.866385937497, 65590.6408807534)]</t>
         </is>
       </c>
     </row>
@@ -6567,7 +6567,7 @@
       </c>
       <c r="B615" t="inlineStr">
         <is>
-          <t>[(-0.29999999999936, 614.0), (-0.29999999999936, 613.78), (-5.693, 613.865175), (-5.693, 613.645175), (-0.29999999999936, 613.78), (-0.29999999999936, 613.61), (-5.693, 613.645175), (-5.693, 613.4351750000001)]</t>
+          <t>[(-21387.459385937498, 65634.4077821139), (-21387.459385937498, 65634.1877821139), (-21392.8523859375, 65634.2729571139), (-21392.8523859375, 65634.0529571139), (-21387.459385937498, 65634.1877821139), (-21387.459385937498, 65634.01778211391), (-21392.8523859375, 65634.0529571139), (-21392.8523859375, 65633.84295711391)]</t>
         </is>
       </c>
     </row>
@@ -6577,7 +6577,7 @@
       </c>
       <c r="B616" t="inlineStr">
         <is>
-          <t>[(-0.29999999999936, 615.0), (-0.29999999999936, 614.82), (-5.737, 614.864075), (-5.737, 614.684075), (-0.29999999999936, 614.82), (-0.29999999999936, 614.65), (-5.737, 614.684075), (-5.737, 614.504075)]</t>
+          <t>[(-21327.459385937498, 65591.611175141), (-21327.459385937498, 65591.43117514101), (-21332.8963859375, 65591.47525014101), (-21332.8963859375, 65591.29525014102), (-21327.459385937498, 65591.43117514101), (-21327.459385937498, 65591.261175141), (-21332.8963859375, 65591.29525014102), (-21332.8963859375, 65591.11525014101)]</t>
         </is>
       </c>
     </row>
@@ -6587,7 +6587,7 @@
       </c>
       <c r="B617" t="inlineStr">
         <is>
-          <t>[(-0.299999999997719, 616.0), (-0.299999999997719, 615.88), (-5.754, 615.8636499999999), (-5.754, 615.7436499999999), (-0.299999999997719, 615.88), (-0.299999999997719, 615.72), (-5.754, 615.7436499999999), (-5.754, 615.5336499999999)]</t>
+          <t>[(-21327.459385937498, 65634.8562348348), (-21327.459385937498, 65634.73623483481), (-21332.9133859375, 65634.7198848348), (-21332.9133859375, 65634.59988483481), (-21327.459385937498, 65634.73623483481), (-21327.459385937498, 65634.5762348348), (-21332.9133859375, 65634.59988483481), (-21332.9133859375, 65634.3898848348)]</t>
         </is>
       </c>
     </row>
@@ -6597,7 +6597,7 @@
       </c>
       <c r="B618" t="inlineStr">
         <is>
-          <t>[(-0.300000000034916, 617.0), (-0.300000000034916, 616.82), (-5.745, 616.856482134722), (-5.745, 616.676482134722), (-0.300000000034916, 616.82), (-0.300000000034916, 616.69), (-5.745, 616.676482134722), (-5.745, 616.496482134722)]</t>
+          <t>[(-21199.259385937537, 65590.1429611952), (-21199.259385937537, 65589.96296119521), (-21204.7043859375, 65589.99944332993), (-21204.7043859375, 65589.81944332994), (-21199.259385937537, 65589.96296119521), (-21199.259385937537, 65589.8329611952), (-21204.7043859375, 65589.81944332994), (-21204.7043859375, 65589.63944332993)]</t>
         </is>
       </c>
     </row>
@@ -6607,7 +6607,7 @@
       </c>
       <c r="B619" t="inlineStr">
         <is>
-          <t>[(-0.299999999997212, 618.0), (-0.299999999997212, 617.85), (-5.566, 617.8504776380835), (-5.566, 617.7004776380835), (-0.299999999997212, 617.85), (-0.299999999997212, 617.72), (-5.566, 617.7004776380835), (-5.566, 617.5504776380835)]</t>
+          <t>[(-21199.259385937694, 65635.4713542224), (-21199.259385937694, 65635.32135422241), (-21204.525385937697, 65635.32183186049), (-21204.525385937697, 65635.1718318605), (-21199.259385937694, 65635.32135422241), (-21199.259385937694, 65635.1913542224), (-21204.525385937697, 65635.1718318605), (-21204.525385937697, 65635.02183186049)]</t>
         </is>
       </c>
     </row>
@@ -6627,7 +6627,7 @@
       </c>
       <c r="B621" t="inlineStr">
         <is>
-          <t>[(-0.300000000106398, 620.0), (-0.300000000106398, 619.85), (-5.379, 619.8351037699371), (-5.379, 619.6851037699371), (-0.300000000106398, 619.85), (-0.300000000106398, 619.72), (-5.379, 619.6851037699371), (-5.379, 619.5551037699371)]</t>
+          <t>[(-21140.259385937607, 65636.2531402766), (-21140.259385937607, 65636.10314027661), (-21145.338385937503, 65636.08824404654), (-21145.338385937503, 65635.93824404654), (-21140.259385937607, 65636.10314027661), (-21140.259385937607, 65635.9731402766), (-21145.338385937503, 65635.93824404654), (-21145.338385937503, 65635.80824404654)]</t>
         </is>
       </c>
     </row>
@@ -6647,7 +6647,7 @@
       </c>
       <c r="B623" t="inlineStr">
         <is>
-          <t>[(-0.299999999993878, 622.0), (-0.299999999993878, 621.88), (-5.574, 621.8154099999998), (-5.574, 621.6954099999998), (-0.299999999993878, 621.88), (-0.299999999993878, 621.68), (-5.574, 621.6954099999998), (-5.574, 621.5454099999998)]</t>
+          <t>[(-21002.059385937497, 65633.2015929975), (-21002.059385937497, 65633.0815929975), (-21007.3333859375, 65633.0170029975), (-21007.3333859375, 65632.8970029975), (-21002.059385937497, 65633.0815929975), (-21002.059385937497, 65632.8815929975), (-21007.3333859375, 65632.8970029975), (-21007.3333859375, 65632.7470029975)]</t>
         </is>
       </c>
     </row>
@@ -6657,7 +6657,7 @@
       </c>
       <c r="B624" t="inlineStr">
         <is>
-          <t>[(-0.300000000000493, 623.0), (-0.300000000000493, 622.88), (-5.733, 622.809845), (-5.733, 622.689845), (-0.300000000000493, 622.88), (-0.300000000000493, 622.67), (-5.733, 622.689845), (-5.733, 622.539845)]</t>
+          <t>[(-20934.0593859375, 65586.738319358), (-20934.0593859375, 65586.61831935801), (-20939.4923859375, 65586.548164358), (-20939.4923859375, 65586.428164358), (-20934.0593859375, 65586.61831935801), (-20934.0593859375, 65586.408319358), (-20939.4923859375, 65586.428164358), (-20939.4923859375, 65586.278164358)]</t>
         </is>
       </c>
     </row>
@@ -6667,7 +6667,7 @@
       </c>
       <c r="B625" t="inlineStr">
         <is>
-          <t>[(-0.299999999992329, 624.0), (-0.299999999992329, 623.82), (-5.937, 623.8027049999997), (-5.937, 623.6227049999998), (-0.299999999992329, 623.82), (-0.299999999992329, 623.65), (-5.937, 623.6227049999998), (-5.937, 623.4827049999997)]</t>
+          <t>[(-20934.059385937493, 65632.3167123851), (-20934.059385937493, 65632.13671238511), (-20939.696385937503, 65632.1194173851), (-20939.696385937503, 65631.9394173851), (-20934.059385937493, 65632.13671238511), (-20934.059385937493, 65631.9667123851), (-20939.696385937503, 65631.9394173851), (-20939.696385937503, 65631.79941738509)]</t>
         </is>
       </c>
     </row>
@@ -6677,7 +6677,7 @@
       </c>
       <c r="B626" t="inlineStr">
         <is>
-          <t>[(-0.300000000002759, 625.0), (-0.300000000002759, 624.8), (-6.034, 624.7993100000001), (-6.034, 624.5993100000001), (-0.300000000002759, 624.8), (-0.300000000002759, 624.61), (-6.034, 624.5993100000001), (-6.034, 624.4393100000001)]</t>
+          <t>[(-20804.859385937503, 65587.931011957), (-20804.859385937503, 65587.731011957), (-20810.5933859375, 65587.730321957), (-20810.5933859375, 65587.530321957), (-20804.859385937503, 65587.731011957), (-20804.859385937503, 65587.541011957), (-20810.5933859375, 65587.530321957), (-20810.5933859375, 65587.370321957)]</t>
         </is>
       </c>
     </row>
@@ -6687,7 +6687,7 @@
       </c>
       <c r="B627" t="inlineStr">
         <is>
-          <t>[(-0.300000000002964, 626.0), (-0.300000000002964, 625.78), (-6.25, 625.7917500000001), (-6.25, 625.5717500000001), (-0.300000000002964, 625.78), (-0.300000000002964, 625.57), (-6.25, 625.5717500000001), (-6.25, 625.3917500000001)]</t>
+          <t>[(-20804.859385937503, 65639.54999585), (-20804.859385937503, 65639.32999585), (-20810.8093859375, 65639.34174585), (-20810.8093859375, 65639.12174585), (-20804.859385937503, 65639.32999585), (-20804.859385937503, 65639.11999585001), (-20810.8093859375, 65639.12174585), (-20810.8093859375, 65638.94174585001)]</t>
         </is>
       </c>
     </row>
@@ -6697,7 +6697,7 @@
       </c>
       <c r="B628" t="inlineStr">
         <is>
-          <t>[(-0.299999999998948, 627.0), (-0.299999999998948, 626.78), (-6.434, 626.78531), (-6.434, 626.56531), (-0.299999999998948, 626.78), (-0.299999999998948, 626.56), (-6.434, 626.56531), (-6.434, 626.38531)]</t>
+          <t>[(-20737.8593859375, 65589.168979743), (-20737.8593859375, 65588.948979743), (-20743.9933859375, 65588.95428974301), (-20743.9933859375, 65588.734289743), (-20737.8593859375, 65588.948979743), (-20737.8593859375, 65588.728979743), (-20743.9933859375, 65588.734289743), (-20743.9933859375, 65588.55428974301)]</t>
         </is>
       </c>
     </row>
@@ -6707,7 +6707,7 @@
       </c>
       <c r="B629" t="inlineStr">
         <is>
-          <t>[(-0.300000000007299, 628.0), (-0.300000000007299, 627.78), (-6.611, 627.7791150000003), (-6.611, 627.5591150000002), (-0.300000000007299, 627.78), (-0.300000000007299, 627.57), (-6.611, 627.5591150000002), (-6.611, 627.3891150000003)]</t>
+          <t>[(-20747.859385937507, 65640.787963636), (-20747.859385937507, 65640.567963636), (-20754.1703859375, 65640.567078636), (-20754.1703859375, 65640.347078636), (-20747.859385937507, 65640.567963636), (-20747.859385937507, 65640.35796363601), (-20754.1703859375, 65640.347078636), (-20754.1703859375, 65640.177078636)]</t>
         </is>
       </c>
     </row>
@@ -6717,7 +6717,7 @@
       </c>
       <c r="B630" t="inlineStr">
         <is>
-          <t>[(-0.300000000005412, 629.0), (-0.300000000005412, 628.79), (-6.849, 628.7707850000002), (-6.849, 628.5607850000001), (-0.300000000005412, 628.79), (-0.300000000005412, 628.58), (-6.849, 628.5607850000001), (-6.849, 628.4107850000001)]</t>
+          <t>[(-20634.659385937506, 65588.406947529), (-20634.659385937506, 65588.196947529), (-20641.208385937498, 65588.177732529), (-20641.208385937498, 65587.967732529), (-20634.659385937506, 65588.196947529), (-20634.659385937506, 65587.986947529), (-20641.208385937498, 65587.967732529), (-20641.208385937498, 65587.817732529)]</t>
         </is>
       </c>
     </row>
@@ -6727,7 +6727,7 @@
       </c>
       <c r="B631" t="inlineStr">
         <is>
-          <t>[(-0.3000000000067, 630.0), (-0.3000000000067, 629.77), (-7.077, 629.7628050000002), (-7.077, 629.5328050000002), (-0.3000000000067, 629.77), (-0.3000000000067, 629.54), (-7.077, 629.5328050000002), (-7.077, 629.3628050000002)]</t>
+          <t>[(-20634.659385937506, 65628.025931422), (-20634.659385937506, 65627.795931422), (-20641.4363859375, 65627.78873642201), (-20641.4363859375, 65627.55873642201), (-20634.659385937506, 65627.795931422), (-20634.659385937506, 65627.565931422), (-20641.4363859375, 65627.55873642201), (-20641.4363859375, 65627.38873642201)]</t>
         </is>
       </c>
     </row>
@@ -6737,7 +6737,7 @@
       </c>
       <c r="B632" t="inlineStr">
         <is>
-          <t>[(-0.300000000009039, 631.0), (-0.300000000009039, 630.81), (-7.33, 630.7539500000004), (-7.33, 630.5639500000003), (-0.300000000009039, 630.81), (-0.300000000009039, 630.62), (-7.33, 630.5639500000003), (-7.33, 630.3939500000004)]</t>
+          <t>[(-20574.65938593751, 65589.6104501498), (-20574.65938593751, 65589.4204501498), (-20581.6893859375, 65589.3644001498), (-20581.6893859375, 65589.1744001498), (-20574.65938593751, 65589.4204501498), (-20574.65938593751, 65589.2304501498), (-20581.6893859375, 65589.1744001498), (-20581.6893859375, 65589.0044001498)]</t>
         </is>
       </c>
     </row>
@@ -6747,7 +6747,7 @@
       </c>
       <c r="B633" t="inlineStr">
         <is>
-          <t>[(-0.299999999997191, 632.0), (-0.299999999997191, 631.88), (-7.345, 631.7534249999999), (-7.345, 631.6334249999999), (-0.299999999997191, 631.88), (-0.299999999997191, 631.67), (-7.345, 631.6334249999999), (-7.345, 631.4734249999999)]</t>
+          <t>[(-20574.659385937495, 65629.109804151), (-20574.659385937495, 65628.989804151), (-20581.7043859375, 65628.863229151), (-20581.7043859375, 65628.743229151), (-20574.659385937495, 65628.989804151), (-20574.659385937495, 65628.779804151), (-20581.7043859375, 65628.743229151), (-20581.7043859375, 65628.583229151)]</t>
         </is>
       </c>
     </row>
@@ -6767,7 +6767,7 @@
       </c>
       <c r="B635" t="inlineStr">
         <is>
-          <t>[(-0.299999999999378, 634.0), (-0.299999999999378, 633.88), (-7.796, 633.7376399999999), (-7.796, 633.6176399999999), (-0.299999999999378, 633.88), (-0.299999999999378, 633.75), (-7.796, 633.6176399999999), (-7.796, 633.3676399999999)]</t>
+          <t>[(-20446.459385937498, 65629.85166283831), (-20446.459385937498, 65629.73166283831), (-20453.955385937497, 65629.58930283831), (-20453.955385937497, 65629.46930283832), (-20446.459385937498, 65629.73166283831), (-20446.459385937498, 65629.60166283831), (-20453.955385937497, 65629.46930283832), (-20453.955385937497, 65629.21930283832)]</t>
         </is>
       </c>
     </row>
@@ -6777,7 +6777,7 @@
       </c>
       <c r="B636" t="inlineStr">
         <is>
-          <t>[(-0.299999999991446, 635.0), (-0.299999999991446, 634.87), (-6.877, 634.7698049999997), (-6.877, 634.6398049999997), (-0.299999999991446, 634.87), (-0.299999999991446, 634.75), (-6.877, 634.6398049999997), (-6.877, 634.5198049999997)]</t>
+          <t>[(-20386.45938593749, 65591.0941675244), (-20386.45938593749, 65590.96416752439), (-20393.0363859375, 65590.8639725244), (-20393.0363859375, 65590.7339725244), (-20386.45938593749, 65590.96416752439), (-20386.45938593749, 65590.8441675244), (-20393.0363859375, 65590.7339725244), (-20393.0363859375, 65590.6139725244)]</t>
         </is>
       </c>
     </row>
@@ -6787,7 +6787,7 @@
       </c>
       <c r="B637" t="inlineStr">
         <is>
-          <t>[(-0.300000000005308, 636.0), (-0.300000000005308, 635.87), (-6.963, 635.7667950000002), (-6.963, 635.6367950000002), (-0.300000000005308, 635.87), (-0.300000000005308, 635.75), (-6.963, 635.6367950000002), (-6.963, 635.5167950000002)]</t>
+          <t>[(-20386.459385937505, 65632.2510557722), (-20386.459385937505, 65632.1210557722), (-20393.1223859375, 65632.0178507722), (-20393.1223859375, 65631.8878507722), (-20386.459385937505, 65632.1210557722), (-20386.459385937505, 65632.0010557722), (-20393.1223859375, 65631.8878507722), (-20393.1223859375, 65631.7678507722)]</t>
         </is>
       </c>
     </row>
@@ -6797,7 +6797,7 @@
       </c>
       <c r="B638" t="inlineStr">
         <is>
-          <t>[(-0.300000000009692, 637.0), (-0.300000000009692, 636.87), (-7.004, 636.7653600000003), (-7.004, 636.6353600000003), (-0.300000000009692, 636.87), (-0.300000000009692, 636.75), (-7.004, 636.6353600000003), (-7.004, 636.5153600000003)]</t>
+          <t>[(-20257.259385937512, 65587.3223275816), (-20257.259385937512, 65587.1923275816), (-20263.963385937503, 65587.0876875816), (-20263.963385937503, 65586.9576875816), (-20257.259385937512, 65587.1923275816), (-20257.259385937512, 65587.0723275816), (-20263.963385937503, 65586.9576875816), (-20263.963385937503, 65586.8376875816)]</t>
         </is>
       </c>
     </row>
@@ -6807,7 +6807,7 @@
       </c>
       <c r="B639" t="inlineStr">
         <is>
-          <t>[(-0.299999999991601, 638.0), (-0.299999999991601, 637.87), (-7.037, 637.7642049999997), (-7.037, 637.6342049999997), (-0.299999999991601, 637.87), (-0.299999999991601, 637.75), (-7.037, 637.6342049999997), (-7.037, 637.5142049999997)]</t>
+          <t>[(-20257.259385937494, 65626.3079829527), (-20257.259385937494, 65626.1779829527), (-20263.996385937502, 65626.0721879527), (-20263.996385937502, 65625.94218795269), (-20257.259385937494, 65626.1779829527), (-20257.259385937494, 65626.0579829527), (-20263.996385937502, 65625.94218795269), (-20263.996385937502, 65625.8221879527)]</t>
         </is>
       </c>
     </row>
@@ -6817,7 +6817,7 @@
       </c>
       <c r="B640" t="inlineStr">
         <is>
-          <t>[(-0.300000000005187, 639.0), (-0.300000000005187, 638.87), (-7.102, 638.7619300000002), (-7.102, 638.6319300000002), (-0.300000000005187, 638.87), (-0.300000000005187, 638.75), (-7.102, 638.6319300000002), (-7.102, 638.5119300000002)]</t>
+          <t>[(-20209.25938593751, 65587.2080218854), (-20209.25938593751, 65587.07802188539), (-20216.0613859375, 65586.96995188539), (-20216.0613859375, 65586.83995188538), (-20209.25938593751, 65587.07802188539), (-20209.25938593751, 65586.9580218854), (-20216.0613859375, 65586.83995188538), (-20216.0613859375, 65586.71995188539)]</t>
         </is>
       </c>
     </row>
@@ -6847,7 +6847,7 @@
       </c>
       <c r="B643" t="inlineStr">
         <is>
-          <t>[(-0.3, 641.6355600000002), (-0.3, 641.5055600000002), (-4.0, 641.5208230000002), (-4.0, 641.3908230000002), (-0.3, 641.5055600000002), (-0.3, 641.3855600000002), (-4.0, 641.3908230000002), (-4.0, 641.2708230000002)]</t>
+          <t>[(-20161.2593859375, 65625.8993674492), (-20161.2593859375, 65625.76936744919), (-20164.9593859375, 65625.7846304492), (-20164.9593859375, 65625.6546304492), (-20161.2593859375, 65625.76936744919), (-20161.2593859375, 65625.6493674492), (-20164.9593859375, 65625.6546304492), (-20164.9593859375, 65625.5346304492)]</t>
         </is>
       </c>
     </row>

</xml_diff>